<commit_message>
assign final unicode for 2 draft icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="579">
   <si>
     <t>name</t>
   </si>
@@ -1739,6 +1739,24 @@
   </si>
   <si>
     <t>used in context menu or toolbar for Delete command, matching Add command.</t>
+  </si>
+  <si>
+    <t>row-child</t>
+  </si>
+  <si>
+    <t>row child sub indent tree</t>
+  </si>
+  <si>
+    <t>Used for creating a child node of the current node in a tree structure.</t>
+  </si>
+  <si>
+    <t>log-remove</t>
+  </si>
+  <si>
+    <t>log activity remove delete</t>
+  </si>
+  <si>
+    <t>Used for removing activity entry on Kanban board.</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1842,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1864,6 +1882,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -14456,6 +14476,82 @@
         <a:xfrm>
           <a:off x="1171575" y="133378575"/>
           <a:ext cx="247685" cy="266737"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409610</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>342935</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="333" name="Picture 332"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId332"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="133797675"/>
+          <a:ext cx="247685" cy="247685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>334</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>428658</xdr:colOff>
+      <xdr:row>334</xdr:row>
+      <xdr:rowOff>323885</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="334" name="Picture 333"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId333"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="134178675"/>
+          <a:ext cx="238158" cy="247685"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14730,11 +14826,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL333"/>
+  <dimension ref="A1:AL410"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A328" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G334" sqref="G334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -25699,7 +25795,7 @@
         <v>234</v>
       </c>
       <c r="L324" t="str">
-        <f t="shared" ref="L324:L333" si="11">CONCATENATE("u",C324,"-",E324,".svg")</f>
+        <f t="shared" ref="L324:L357" si="11">CONCATENATE("u",C324,"-",E324,".svg")</f>
         <v>uEA41-view-list-tree.svg</v>
       </c>
     </row>
@@ -25984,6 +26080,753 @@
       <c r="L333" t="str">
         <f t="shared" si="11"/>
         <v>uEA4A-square.svg</v>
+      </c>
+    </row>
+    <row r="334" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A334" s="2">
+        <v>332</v>
+      </c>
+      <c r="C334" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA4B</v>
+      </c>
+      <c r="D334" s="13">
+        <v>59979</v>
+      </c>
+      <c r="E334" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="F334" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G334" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H334" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="I334" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J334" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K334" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="L334" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA4B-row-child.svg</v>
+      </c>
+    </row>
+    <row r="335" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="2">
+        <v>333</v>
+      </c>
+      <c r="C335" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA4C</v>
+      </c>
+      <c r="D335" s="13">
+        <v>59980</v>
+      </c>
+      <c r="E335" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F335" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G335" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H335" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="I335" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J335" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K335" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="L335" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA4C-log-remove.svg</v>
+      </c>
+    </row>
+    <row r="336" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C336" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA4D</v>
+      </c>
+      <c r="D336" s="13">
+        <v>59981</v>
+      </c>
+      <c r="L336" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA4D-.svg</v>
+      </c>
+    </row>
+    <row r="337" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C337" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA4E</v>
+      </c>
+      <c r="D337" s="13">
+        <v>59982</v>
+      </c>
+      <c r="L337" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA4E-.svg</v>
+      </c>
+    </row>
+    <row r="338" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C338" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA4F</v>
+      </c>
+      <c r="D338" s="13">
+        <v>59983</v>
+      </c>
+      <c r="L338" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA4F-.svg</v>
+      </c>
+    </row>
+    <row r="339" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C339" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA50</v>
+      </c>
+      <c r="D339" s="13">
+        <v>59984</v>
+      </c>
+      <c r="L339" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA50-.svg</v>
+      </c>
+    </row>
+    <row r="340" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C340" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA51</v>
+      </c>
+      <c r="D340" s="13">
+        <v>59985</v>
+      </c>
+      <c r="L340" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA51-.svg</v>
+      </c>
+    </row>
+    <row r="341" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C341" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA52</v>
+      </c>
+      <c r="D341" s="13">
+        <v>59986</v>
+      </c>
+      <c r="L341" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA52-.svg</v>
+      </c>
+    </row>
+    <row r="342" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C342" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA53</v>
+      </c>
+      <c r="D342" s="13">
+        <v>59987</v>
+      </c>
+      <c r="L342" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA53-.svg</v>
+      </c>
+    </row>
+    <row r="343" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C343" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA54</v>
+      </c>
+      <c r="D343" s="13">
+        <v>59988</v>
+      </c>
+      <c r="L343" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA54-.svg</v>
+      </c>
+    </row>
+    <row r="344" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C344" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA55</v>
+      </c>
+      <c r="D344" s="13">
+        <v>59989</v>
+      </c>
+      <c r="L344" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA55-.svg</v>
+      </c>
+    </row>
+    <row r="345" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C345" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA56</v>
+      </c>
+      <c r="D345" s="13">
+        <v>59990</v>
+      </c>
+      <c r="L345" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA56-.svg</v>
+      </c>
+    </row>
+    <row r="346" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C346" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA57</v>
+      </c>
+      <c r="D346" s="13">
+        <v>59991</v>
+      </c>
+      <c r="L346" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA57-.svg</v>
+      </c>
+    </row>
+    <row r="347" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C347" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA58</v>
+      </c>
+      <c r="D347" s="13">
+        <v>59992</v>
+      </c>
+      <c r="L347" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA58-.svg</v>
+      </c>
+    </row>
+    <row r="348" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C348" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA59</v>
+      </c>
+      <c r="D348" s="13">
+        <v>59993</v>
+      </c>
+      <c r="L348" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA59-.svg</v>
+      </c>
+    </row>
+    <row r="349" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C349" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA5A</v>
+      </c>
+      <c r="D349" s="13">
+        <v>59994</v>
+      </c>
+      <c r="L349" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA5A-.svg</v>
+      </c>
+    </row>
+    <row r="350" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C350" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA5B</v>
+      </c>
+      <c r="D350" s="13">
+        <v>59995</v>
+      </c>
+      <c r="L350" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA5B-.svg</v>
+      </c>
+    </row>
+    <row r="351" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C351" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA5C</v>
+      </c>
+      <c r="D351" s="13">
+        <v>59996</v>
+      </c>
+      <c r="L351" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA5C-.svg</v>
+      </c>
+    </row>
+    <row r="352" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C352" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA5D</v>
+      </c>
+      <c r="D352" s="13">
+        <v>59997</v>
+      </c>
+      <c r="L352" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA5D-.svg</v>
+      </c>
+    </row>
+    <row r="353" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C353" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA5E</v>
+      </c>
+      <c r="D353" s="13">
+        <v>59998</v>
+      </c>
+      <c r="L353" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA5E-.svg</v>
+      </c>
+    </row>
+    <row r="354" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C354" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA5F</v>
+      </c>
+      <c r="D354" s="13">
+        <v>59999</v>
+      </c>
+      <c r="L354" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA5F-.svg</v>
+      </c>
+    </row>
+    <row r="355" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C355" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA60</v>
+      </c>
+      <c r="D355" s="13">
+        <v>60000</v>
+      </c>
+      <c r="L355" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA60-.svg</v>
+      </c>
+    </row>
+    <row r="356" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C356" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA61</v>
+      </c>
+      <c r="D356" s="13">
+        <v>60001</v>
+      </c>
+      <c r="L356" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA61-.svg</v>
+      </c>
+    </row>
+    <row r="357" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C357" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA62</v>
+      </c>
+      <c r="D357" s="13">
+        <v>60002</v>
+      </c>
+      <c r="L357" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA62-.svg</v>
+      </c>
+    </row>
+    <row r="358" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C358" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA63</v>
+      </c>
+      <c r="D358" s="13">
+        <v>60003</v>
+      </c>
+    </row>
+    <row r="359" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C359" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA64</v>
+      </c>
+      <c r="D359" s="13">
+        <v>60004</v>
+      </c>
+    </row>
+    <row r="360" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C360" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA65</v>
+      </c>
+      <c r="D360" s="13">
+        <v>60005</v>
+      </c>
+    </row>
+    <row r="361" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C361" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA66</v>
+      </c>
+      <c r="D361" s="13">
+        <v>60006</v>
+      </c>
+    </row>
+    <row r="362" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C362" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA67</v>
+      </c>
+      <c r="D362" s="13">
+        <v>60007</v>
+      </c>
+    </row>
+    <row r="363" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C363" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA68</v>
+      </c>
+      <c r="D363" s="13">
+        <v>60008</v>
+      </c>
+    </row>
+    <row r="364" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C364" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA69</v>
+      </c>
+      <c r="D364" s="13">
+        <v>60009</v>
+      </c>
+    </row>
+    <row r="365" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C365" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA6A</v>
+      </c>
+      <c r="D365" s="13">
+        <v>60010</v>
+      </c>
+    </row>
+    <row r="366" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C366" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA6B</v>
+      </c>
+      <c r="D366" s="13">
+        <v>60011</v>
+      </c>
+    </row>
+    <row r="367" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C367" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA6C</v>
+      </c>
+      <c r="D367" s="13">
+        <v>60012</v>
+      </c>
+    </row>
+    <row r="368" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C368" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA6D</v>
+      </c>
+      <c r="D368" s="13">
+        <v>60013</v>
+      </c>
+    </row>
+    <row r="369" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C369" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA6E</v>
+      </c>
+      <c r="D369" s="13">
+        <v>60014</v>
+      </c>
+    </row>
+    <row r="370" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C370" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA6F</v>
+      </c>
+      <c r="D370" s="13">
+        <v>60015</v>
+      </c>
+    </row>
+    <row r="371" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C371" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA70</v>
+      </c>
+      <c r="D371" s="13">
+        <v>60016</v>
+      </c>
+    </row>
+    <row r="372" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C372" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA71</v>
+      </c>
+      <c r="D372" s="13">
+        <v>60017</v>
+      </c>
+    </row>
+    <row r="373" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C373" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA72</v>
+      </c>
+      <c r="D373" s="13">
+        <v>60018</v>
+      </c>
+    </row>
+    <row r="374" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C374" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA73</v>
+      </c>
+      <c r="D374" s="13">
+        <v>60019</v>
+      </c>
+    </row>
+    <row r="375" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C375" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA74</v>
+      </c>
+      <c r="D375" s="13">
+        <v>60020</v>
+      </c>
+    </row>
+    <row r="376" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C376" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA75</v>
+      </c>
+      <c r="D376" s="13">
+        <v>60021</v>
+      </c>
+    </row>
+    <row r="377" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C377" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA76</v>
+      </c>
+      <c r="D377" s="13">
+        <v>60022</v>
+      </c>
+    </row>
+    <row r="378" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C378" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA77</v>
+      </c>
+      <c r="D378" s="13">
+        <v>60023</v>
+      </c>
+    </row>
+    <row r="379" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C379" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA78</v>
+      </c>
+      <c r="D379" s="13">
+        <v>60024</v>
+      </c>
+    </row>
+    <row r="380" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C380" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>EA79</v>
+      </c>
+      <c r="D380" s="13">
+        <v>60025</v>
+      </c>
+    </row>
+    <row r="381" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C381" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C382" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C383" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C384" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C385" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C386" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C387" s="13" t="str">
+        <f t="shared" ref="C387:C410" si="12">DEC2HEX(D387)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C388" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C389" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C390" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C391" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C392" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C393" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C394" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C395" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C396" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C397" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C398" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C399" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C400" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C401" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C402" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C403" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C404" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C405" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C406" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C407" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C408" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C409" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C410" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -25999,10 +26842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L332"/>
+  <dimension ref="A1:L339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L332"/>
+    <sheetView topLeftCell="A312" workbookViewId="0">
+      <selection activeCell="C333" sqref="C333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42140,7 +42983,7 @@
         <v/>
       </c>
       <c r="K323" t="str">
-        <f t="shared" ref="K323:K334" si="10">IF(NOT(ISBLANK(A323)),CONCATENATE("{'",$A$1,"':",A323,",'",$B$1,"':'",B323,"',","'",$C$1,"':'",C323,"','",$D$1,"':",D323,",'",$E$1,"':'",FIXED(E323,1),"','",$F$1,"':'",F323,"','",$G$1,"':'",G323,"','",$H$1,"':'",H323,"','",$I$1,"':['",SUBSTITUTE(I323," ","','"),"'],'",$J$1,"':'",J323,"'}"))</f>
+        <f t="shared" ref="K323:K332" si="10">IF(NOT(ISBLANK(A323)),CONCATENATE("{'",$A$1,"':",A323,",'",$B$1,"':'",B323,"',","'",$C$1,"':'",C323,"','",$D$1,"':",D323,",'",$E$1,"':'",FIXED(E323,1),"','",$F$1,"':'",F323,"','",$G$1,"':'",G323,"','",$H$1,"':'",H323,"','",$I$1,"':['",SUBSTITUTE(I323," ","','"),"'],'",$J$1,"':'",J323,"'}"))</f>
         <v>{'id':322,'name':'view-list-tree','unicode':'EA41','decimal':59969,'version':'1.0','style':'','subset':'VSTS','group':'work','keywords':[''],'usage':''}</v>
       </c>
       <c r="L323" t="str">
@@ -42596,6 +43439,356 @@
       <c r="L332" t="str">
         <f t="shared" si="11"/>
         <v>{"id":331,"name":"square","unicode":"EA4A","decimal":59978,"version":"1.0","style":"bold","subset":"VSTS","group":"","keywords":["square"],"usage":"check if it is same as stop-fill"}</v>
+      </c>
+    </row>
+    <row r="333" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A333" s="15">
+        <f>'Bowtie v1.0 reorg'!A334</f>
+        <v>332</v>
+      </c>
+      <c r="B333" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!E334</f>
+        <v>row-child</v>
+      </c>
+      <c r="C333" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!C334</f>
+        <v>EA4B</v>
+      </c>
+      <c r="D333" s="15">
+        <f>'Bowtie v1.0 reorg'!D334</f>
+        <v>59979</v>
+      </c>
+      <c r="E333" s="16">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F334),"",'Bowtie v1.0 reorg'!F334)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F333" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G334),"",'Bowtie v1.0 reorg'!G334)</f>
+        <v>light</v>
+      </c>
+      <c r="G333" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I334),"",'Bowtie v1.0 reorg'!I334)</f>
+        <v>VSTS</v>
+      </c>
+      <c r="H333" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J334),"",'Bowtie v1.0 reorg'!J334)</f>
+        <v>common</v>
+      </c>
+      <c r="I333" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H334),"",'Bowtie v1.0 reorg'!H334)</f>
+        <v>row child sub indent tree</v>
+      </c>
+      <c r="J333" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K334),"",'Bowtie v1.0 reorg'!K334)</f>
+        <v>Used for creating a child node of the current node in a tree structure.</v>
+      </c>
+      <c r="K333" s="15" t="str">
+        <f t="shared" ref="K333:K339" si="12">IF(NOT(ISBLANK(A333)),CONCATENATE("{'",$A$1,"':",A333,",'",$B$1,"':'",B333,"',","'",$C$1,"':'",C333,"','",$D$1,"':",D333,",'",$E$1,"':'",FIXED(E333,1),"','",$F$1,"':'",F333,"','",$G$1,"':'",G333,"','",$H$1,"':'",H333,"','",$I$1,"':['",SUBSTITUTE(I333," ","','"),"'],'",$J$1,"':'",J333,"'}"))</f>
+        <v>{'id':332,'name':'row-child','unicode':'EA4B','decimal':59979,'version':'1.1','style':'light','subset':'VSTS','group':'common','keywords':['row','child','sub','indent','tree'],'usage':'Used for creating a child node of the current node in a tree structure.'}</v>
+      </c>
+      <c r="L333" s="15" t="str">
+        <f t="shared" ref="L333:L339" si="13">SUBSTITUTE(K333,"'","""")</f>
+        <v>{"id":332,"name":"row-child","unicode":"EA4B","decimal":59979,"version":"1.1","style":"light","subset":"VSTS","group":"common","keywords":["row","child","sub","indent","tree"],"usage":"Used for creating a child node of the current node in a tree structure."}</v>
+      </c>
+    </row>
+    <row r="334" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A334" s="15">
+        <f>'Bowtie v1.0 reorg'!A335</f>
+        <v>333</v>
+      </c>
+      <c r="B334" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!E335</f>
+        <v>log-remove</v>
+      </c>
+      <c r="C334" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!C335</f>
+        <v>EA4C</v>
+      </c>
+      <c r="D334" s="15">
+        <f>'Bowtie v1.0 reorg'!D335</f>
+        <v>59980</v>
+      </c>
+      <c r="E334" s="16">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F335),"",'Bowtie v1.0 reorg'!F335)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F334" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G335),"",'Bowtie v1.0 reorg'!G335)</f>
+        <v>light</v>
+      </c>
+      <c r="G334" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I335),"",'Bowtie v1.0 reorg'!I335)</f>
+        <v>VSTS</v>
+      </c>
+      <c r="H334" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J335),"",'Bowtie v1.0 reorg'!J335)</f>
+        <v>work</v>
+      </c>
+      <c r="I334" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H335),"",'Bowtie v1.0 reorg'!H335)</f>
+        <v>log activity remove delete</v>
+      </c>
+      <c r="J334" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K335),"",'Bowtie v1.0 reorg'!K335)</f>
+        <v>Used for removing activity entry on Kanban board.</v>
+      </c>
+      <c r="K334" s="15" t="str">
+        <f t="shared" si="12"/>
+        <v>{'id':333,'name':'log-remove','unicode':'EA4C','decimal':59980,'version':'1.1','style':'light','subset':'VSTS','group':'work','keywords':['log','activity','remove','delete'],'usage':'Used for removing activity entry on Kanban board.'}</v>
+      </c>
+      <c r="L334" s="15" t="str">
+        <f t="shared" si="13"/>
+        <v>{"id":333,"name":"log-remove","unicode":"EA4C","decimal":59980,"version":"1.1","style":"light","subset":"VSTS","group":"work","keywords":["log","activity","remove","delete"],"usage":"Used for removing activity entry on Kanban board."}</v>
+      </c>
+    </row>
+    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <f>'Bowtie v1.0 reorg'!A336</f>
+        <v>0</v>
+      </c>
+      <c r="B335">
+        <f>'Bowtie v1.0 reorg'!E336</f>
+        <v>0</v>
+      </c>
+      <c r="C335" t="str">
+        <f>'Bowtie v1.0 reorg'!C336</f>
+        <v>EA4D</v>
+      </c>
+      <c r="D335">
+        <f>'Bowtie v1.0 reorg'!D336</f>
+        <v>59981</v>
+      </c>
+      <c r="E335" s="14" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F336),"",'Bowtie v1.0 reorg'!F336)</f>
+        <v/>
+      </c>
+      <c r="F335" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G336),"",'Bowtie v1.0 reorg'!G336)</f>
+        <v/>
+      </c>
+      <c r="G335" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I336),"",'Bowtie v1.0 reorg'!I336)</f>
+        <v/>
+      </c>
+      <c r="H335" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J336),"",'Bowtie v1.0 reorg'!J336)</f>
+        <v/>
+      </c>
+      <c r="I335" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H336),"",'Bowtie v1.0 reorg'!H336)</f>
+        <v/>
+      </c>
+      <c r="J335" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K336),"",'Bowtie v1.0 reorg'!K336)</f>
+        <v/>
+      </c>
+      <c r="K335" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L335" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <f>'Bowtie v1.0 reorg'!A337</f>
+        <v>0</v>
+      </c>
+      <c r="B336">
+        <f>'Bowtie v1.0 reorg'!E337</f>
+        <v>0</v>
+      </c>
+      <c r="C336" t="str">
+        <f>'Bowtie v1.0 reorg'!C337</f>
+        <v>EA4E</v>
+      </c>
+      <c r="D336">
+        <f>'Bowtie v1.0 reorg'!D337</f>
+        <v>59982</v>
+      </c>
+      <c r="E336" s="14" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F337),"",'Bowtie v1.0 reorg'!F337)</f>
+        <v/>
+      </c>
+      <c r="F336" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G337),"",'Bowtie v1.0 reorg'!G337)</f>
+        <v/>
+      </c>
+      <c r="G336" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I337),"",'Bowtie v1.0 reorg'!I337)</f>
+        <v/>
+      </c>
+      <c r="H336" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J337),"",'Bowtie v1.0 reorg'!J337)</f>
+        <v/>
+      </c>
+      <c r="I336" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H337),"",'Bowtie v1.0 reorg'!H337)</f>
+        <v/>
+      </c>
+      <c r="J336" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K337),"",'Bowtie v1.0 reorg'!K337)</f>
+        <v/>
+      </c>
+      <c r="K336" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L336" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <f>'Bowtie v1.0 reorg'!A338</f>
+        <v>0</v>
+      </c>
+      <c r="B337">
+        <f>'Bowtie v1.0 reorg'!E338</f>
+        <v>0</v>
+      </c>
+      <c r="C337" t="str">
+        <f>'Bowtie v1.0 reorg'!C338</f>
+        <v>EA4F</v>
+      </c>
+      <c r="D337">
+        <f>'Bowtie v1.0 reorg'!D338</f>
+        <v>59983</v>
+      </c>
+      <c r="E337" s="14" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F338),"",'Bowtie v1.0 reorg'!F338)</f>
+        <v/>
+      </c>
+      <c r="F337" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G338),"",'Bowtie v1.0 reorg'!G338)</f>
+        <v/>
+      </c>
+      <c r="G337" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I338),"",'Bowtie v1.0 reorg'!I338)</f>
+        <v/>
+      </c>
+      <c r="H337" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J338),"",'Bowtie v1.0 reorg'!J338)</f>
+        <v/>
+      </c>
+      <c r="I337" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H338),"",'Bowtie v1.0 reorg'!H338)</f>
+        <v/>
+      </c>
+      <c r="J337" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K338),"",'Bowtie v1.0 reorg'!K338)</f>
+        <v/>
+      </c>
+      <c r="K337" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L337" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <f>'Bowtie v1.0 reorg'!A339</f>
+        <v>0</v>
+      </c>
+      <c r="B338">
+        <f>'Bowtie v1.0 reorg'!E339</f>
+        <v>0</v>
+      </c>
+      <c r="C338" t="str">
+        <f>'Bowtie v1.0 reorg'!C339</f>
+        <v>EA50</v>
+      </c>
+      <c r="D338">
+        <f>'Bowtie v1.0 reorg'!D339</f>
+        <v>59984</v>
+      </c>
+      <c r="E338" s="14" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F339),"",'Bowtie v1.0 reorg'!F339)</f>
+        <v/>
+      </c>
+      <c r="F338" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G339),"",'Bowtie v1.0 reorg'!G339)</f>
+        <v/>
+      </c>
+      <c r="G338" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I339),"",'Bowtie v1.0 reorg'!I339)</f>
+        <v/>
+      </c>
+      <c r="H338" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J339),"",'Bowtie v1.0 reorg'!J339)</f>
+        <v/>
+      </c>
+      <c r="I338" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H339),"",'Bowtie v1.0 reorg'!H339)</f>
+        <v/>
+      </c>
+      <c r="J338" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K339),"",'Bowtie v1.0 reorg'!K339)</f>
+        <v/>
+      </c>
+      <c r="K338" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L338" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <f>'Bowtie v1.0 reorg'!A340</f>
+        <v>0</v>
+      </c>
+      <c r="B339">
+        <f>'Bowtie v1.0 reorg'!E340</f>
+        <v>0</v>
+      </c>
+      <c r="C339" t="str">
+        <f>'Bowtie v1.0 reorg'!C340</f>
+        <v>EA51</v>
+      </c>
+      <c r="D339">
+        <f>'Bowtie v1.0 reorg'!D340</f>
+        <v>59985</v>
+      </c>
+      <c r="E339" s="14" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F340),"",'Bowtie v1.0 reorg'!F340)</f>
+        <v/>
+      </c>
+      <c r="F339" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G340),"",'Bowtie v1.0 reorg'!G340)</f>
+        <v/>
+      </c>
+      <c r="G339" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I340),"",'Bowtie v1.0 reorg'!I340)</f>
+        <v/>
+      </c>
+      <c r="H339" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J340),"",'Bowtie v1.0 reorg'!J340)</f>
+        <v/>
+      </c>
+      <c r="I339" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H340),"",'Bowtie v1.0 reorg'!H340)</f>
+        <v/>
+      </c>
+      <c r="J339" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K340),"",'Bowtie v1.0 reorg'!K340)</f>
+        <v/>
+      </c>
+      <c r="K339" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L339" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added live-update-feed-off for Kanban
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="582">
   <si>
     <t>name</t>
   </si>
@@ -1757,6 +1757,15 @@
   </si>
   <si>
     <t>Used for removing activity entry on Kanban board.</t>
+  </si>
+  <si>
+    <t>live-update-feed-off</t>
+  </si>
+  <si>
+    <t>live update feed signal broadcast radar off</t>
+  </si>
+  <si>
+    <t>Used to indicate listen to Kanban board live updates is toggled off. Adding a slash is not the common toggle off pattern. It is only used in this case.</t>
   </si>
 </sst>
 </file>
@@ -14552,6 +14561,44 @@
         <a:xfrm>
           <a:off x="1133475" y="134178675"/>
           <a:ext cx="238158" cy="247685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>335</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>428662</xdr:colOff>
+      <xdr:row>335</xdr:row>
+      <xdr:rowOff>361985</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="335" name="Picture 334"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId334"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="134616825"/>
+          <a:ext cx="266737" cy="247685"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14828,9 +14875,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL410"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A328" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G334" sqref="G334"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A331" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K340" sqref="K340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15309,6 +15356,9 @@
       <c r="F11" s="3">
         <v>1</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="I11" s="2" t="s">
         <v>15</v>
       </c>
@@ -15336,6 +15386,9 @@
       </c>
       <c r="F12" s="3">
         <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>15</v>
@@ -26157,6 +26210,9 @@
       </c>
     </row>
     <row r="336" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="2">
+        <v>334</v>
+      </c>
       <c r="C336" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA4D</v>
@@ -26164,9 +26220,30 @@
       <c r="D336" s="13">
         <v>59981</v>
       </c>
+      <c r="E336" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="F336" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G336" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H336" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="I336" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J336" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K336" s="2" t="s">
+        <v>581</v>
+      </c>
       <c r="L336" t="str">
         <f t="shared" si="11"/>
-        <v>uEA4D-.svg</v>
+        <v>uEA4D-live-update-feed-off.svg</v>
       </c>
     </row>
     <row r="337" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -26844,8 +26921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L339"/>
   <sheetViews>
-    <sheetView topLeftCell="A312" workbookViewId="0">
-      <selection activeCell="C333" sqref="C333"/>
+    <sheetView tabSelected="1" topLeftCell="B312" workbookViewId="0">
+      <selection activeCell="L335" sqref="L335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27314,7 +27391,7 @@
       </c>
       <c r="F10" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G11),"",'Bowtie v1.0 reorg'!G11)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G10" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I11),"",'Bowtie v1.0 reorg'!I11)</f>
@@ -27334,11 +27411,11 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>{'id':9,'name':'arrow-export','unicode':'E908','decimal':59656,'version':'1.0','style':'','subset':'VSTS','group':'arrow','keywords':[''],'usage':''}</v>
+        <v>{'id':9,'name':'arrow-export','unicode':'E908','decimal':59656,'version':'1.0','style':'light','subset':'VSTS','group':'arrow','keywords':[''],'usage':''}</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="1"/>
-        <v>{"id":9,"name":"arrow-export","unicode":"E908","decimal":59656,"version":"1.0","style":"","subset":"VSTS","group":"arrow","keywords":[""],"usage":""}</v>
+        <v>{"id":9,"name":"arrow-export","unicode":"E908","decimal":59656,"version":"1.0","style":"light","subset":"VSTS","group":"arrow","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -27364,7 +27441,7 @@
       </c>
       <c r="F11" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G12),"",'Bowtie v1.0 reorg'!G12)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G11" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I12),"",'Bowtie v1.0 reorg'!I12)</f>
@@ -27384,11 +27461,11 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>{'id':10,'name':'arrow-open','unicode':'E909','decimal':59657,'version':'1.0','style':'','subset':'VSTS','group':'arrow','keywords':[''],'usage':''}</v>
+        <v>{'id':10,'name':'arrow-open','unicode':'E909','decimal':59657,'version':'1.0','style':'light','subset':'VSTS','group':'arrow','keywords':[''],'usage':''}</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="1"/>
-        <v>{"id":10,"name":"arrow-open","unicode":"E909","decimal":59657,"version":"1.0","style":"","subset":"VSTS","group":"arrow","keywords":[""],"usage":""}</v>
+        <v>{"id":10,"name":"arrow-open","unicode":"E909","decimal":59657,"version":"1.0","style":"light","subset":"VSTS","group":"arrow","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -42983,11 +43060,11 @@
         <v/>
       </c>
       <c r="K323" t="str">
-        <f t="shared" ref="K323:K332" si="10">IF(NOT(ISBLANK(A323)),CONCATENATE("{'",$A$1,"':",A323,",'",$B$1,"':'",B323,"',","'",$C$1,"':'",C323,"','",$D$1,"':",D323,",'",$E$1,"':'",FIXED(E323,1),"','",$F$1,"':'",F323,"','",$G$1,"':'",G323,"','",$H$1,"':'",H323,"','",$I$1,"':['",SUBSTITUTE(I323," ","','"),"'],'",$J$1,"':'",J323,"'}"))</f>
+        <f t="shared" ref="K323:K337" si="10">IF(NOT(ISBLANK(A323)),CONCATENATE("{'",$A$1,"':",A323,",'",$B$1,"':'",B323,"',","'",$C$1,"':'",C323,"','",$D$1,"':",D323,",'",$E$1,"':'",FIXED(E323,1),"','",$F$1,"':'",F323,"','",$G$1,"':'",G323,"','",$H$1,"':'",H323,"','",$I$1,"':['",SUBSTITUTE(I323," ","','"),"'],'",$J$1,"':'",J323,"'}"))</f>
         <v>{'id':322,'name':'view-list-tree','unicode':'EA41','decimal':59969,'version':'1.0','style':'','subset':'VSTS','group':'work','keywords':[''],'usage':''}</v>
       </c>
       <c r="L323" t="str">
-        <f t="shared" ref="L323:L332" si="11">SUBSTITUTE(K323,"'","""")</f>
+        <f t="shared" ref="L323:L329" si="11">SUBSTITUTE(K323,"'","""")</f>
         <v>{"id":322,"name":"view-list-tree","unicode":"EA41","decimal":59969,"version":"1.0","style":"","subset":"VSTS","group":"work","keywords":[""],"usage":""}</v>
       </c>
     </row>
@@ -43337,7 +43414,7 @@
         <v>{'id':329,'name':'recycle-bin','unicode':'EA48','decimal':59976,'version':'1.0','style':'light','subset':'VSTS','group':'work','keywords':['recycle','bin'],'usage':''}</v>
       </c>
       <c r="L330" t="str">
-        <f t="shared" si="11"/>
+        <f>SUBSTITUTE(K330,"'","""")</f>
         <v>{"id":329,"name":"recycle-bin","unicode":"EA48","decimal":59976,"version":"1.0","style":"light","subset":"VSTS","group":"work","keywords":["recycle","bin"],"usage":""}</v>
       </c>
     </row>
@@ -43387,7 +43464,7 @@
         <v>{'id':330,'name':'dot','unicode':'EA49','decimal':59977,'version':'1.0','style':'bold','subset':'VSTS','group':'','keywords':['dot','circle'],'usage':'check if it is same as record-fill'}</v>
       </c>
       <c r="L331" t="str">
-        <f t="shared" si="11"/>
+        <f>SUBSTITUTE(K331,"'","""")</f>
         <v>{"id":330,"name":"dot","unicode":"EA49","decimal":59977,"version":"1.0","style":"bold","subset":"VSTS","group":"","keywords":["dot","circle"],"usage":"check if it is same as record-fill"}</v>
       </c>
     </row>
@@ -43437,158 +43514,158 @@
         <v>{'id':331,'name':'square','unicode':'EA4A','decimal':59978,'version':'1.0','style':'bold','subset':'VSTS','group':'','keywords':['square'],'usage':'check if it is same as stop-fill'}</v>
       </c>
       <c r="L332" t="str">
-        <f t="shared" si="11"/>
+        <f>SUBSTITUTE(K332,"'","""")</f>
         <v>{"id":331,"name":"square","unicode":"EA4A","decimal":59978,"version":"1.0","style":"bold","subset":"VSTS","group":"","keywords":["square"],"usage":"check if it is same as stop-fill"}</v>
       </c>
     </row>
-    <row r="333" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A333" s="15">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A333">
         <f>'Bowtie v1.0 reorg'!A334</f>
         <v>332</v>
       </c>
-      <c r="B333" s="15" t="str">
+      <c r="B333" t="str">
         <f>'Bowtie v1.0 reorg'!E334</f>
         <v>row-child</v>
       </c>
-      <c r="C333" s="15" t="str">
+      <c r="C333" t="str">
         <f>'Bowtie v1.0 reorg'!C334</f>
         <v>EA4B</v>
       </c>
-      <c r="D333" s="15">
+      <c r="D333">
         <f>'Bowtie v1.0 reorg'!D334</f>
         <v>59979</v>
       </c>
-      <c r="E333" s="16">
+      <c r="E333">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F334),"",'Bowtie v1.0 reorg'!F334)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F333" s="15" t="str">
+      <c r="F333" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G334),"",'Bowtie v1.0 reorg'!G334)</f>
         <v>light</v>
       </c>
-      <c r="G333" s="15" t="str">
+      <c r="G333" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I334),"",'Bowtie v1.0 reorg'!I334)</f>
         <v>VSTS</v>
       </c>
-      <c r="H333" s="15" t="str">
+      <c r="H333" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J334),"",'Bowtie v1.0 reorg'!J334)</f>
         <v>common</v>
       </c>
-      <c r="I333" s="15" t="str">
+      <c r="I333" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H334),"",'Bowtie v1.0 reorg'!H334)</f>
         <v>row child sub indent tree</v>
       </c>
-      <c r="J333" s="15" t="str">
+      <c r="J333" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K334),"",'Bowtie v1.0 reorg'!K334)</f>
         <v>Used for creating a child node of the current node in a tree structure.</v>
       </c>
-      <c r="K333" s="15" t="str">
+      <c r="K333" t="str">
         <f t="shared" ref="K333:K339" si="12">IF(NOT(ISBLANK(A333)),CONCATENATE("{'",$A$1,"':",A333,",'",$B$1,"':'",B333,"',","'",$C$1,"':'",C333,"','",$D$1,"':",D333,",'",$E$1,"':'",FIXED(E333,1),"','",$F$1,"':'",F333,"','",$G$1,"':'",G333,"','",$H$1,"':'",H333,"','",$I$1,"':['",SUBSTITUTE(I333," ","','"),"'],'",$J$1,"':'",J333,"'}"))</f>
         <v>{'id':332,'name':'row-child','unicode':'EA4B','decimal':59979,'version':'1.1','style':'light','subset':'VSTS','group':'common','keywords':['row','child','sub','indent','tree'],'usage':'Used for creating a child node of the current node in a tree structure.'}</v>
       </c>
-      <c r="L333" s="15" t="str">
-        <f t="shared" ref="L333:L339" si="13">SUBSTITUTE(K333,"'","""")</f>
+      <c r="L333" t="str">
+        <f t="shared" ref="L333:L337" si="13">SUBSTITUTE(K333,"'","""")</f>
         <v>{"id":332,"name":"row-child","unicode":"EA4B","decimal":59979,"version":"1.1","style":"light","subset":"VSTS","group":"common","keywords":["row","child","sub","indent","tree"],"usage":"Used for creating a child node of the current node in a tree structure."}</v>
       </c>
     </row>
-    <row r="334" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A334" s="15">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A334">
         <f>'Bowtie v1.0 reorg'!A335</f>
         <v>333</v>
       </c>
-      <c r="B334" s="15" t="str">
+      <c r="B334" t="str">
         <f>'Bowtie v1.0 reorg'!E335</f>
         <v>log-remove</v>
       </c>
-      <c r="C334" s="15" t="str">
+      <c r="C334" t="str">
         <f>'Bowtie v1.0 reorg'!C335</f>
         <v>EA4C</v>
       </c>
-      <c r="D334" s="15">
+      <c r="D334">
         <f>'Bowtie v1.0 reorg'!D335</f>
         <v>59980</v>
       </c>
-      <c r="E334" s="16">
+      <c r="E334">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F335),"",'Bowtie v1.0 reorg'!F335)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F334" s="15" t="str">
+      <c r="F334" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G335),"",'Bowtie v1.0 reorg'!G335)</f>
         <v>light</v>
       </c>
-      <c r="G334" s="15" t="str">
+      <c r="G334" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I335),"",'Bowtie v1.0 reorg'!I335)</f>
         <v>VSTS</v>
       </c>
-      <c r="H334" s="15" t="str">
+      <c r="H334" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J335),"",'Bowtie v1.0 reorg'!J335)</f>
         <v>work</v>
       </c>
-      <c r="I334" s="15" t="str">
+      <c r="I334" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H335),"",'Bowtie v1.0 reorg'!H335)</f>
         <v>log activity remove delete</v>
       </c>
-      <c r="J334" s="15" t="str">
+      <c r="J334" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K335),"",'Bowtie v1.0 reorg'!K335)</f>
         <v>Used for removing activity entry on Kanban board.</v>
       </c>
-      <c r="K334" s="15" t="str">
-        <f t="shared" si="12"/>
+      <c r="K334" t="str">
+        <f t="shared" si="10"/>
         <v>{'id':333,'name':'log-remove','unicode':'EA4C','decimal':59980,'version':'1.1','style':'light','subset':'VSTS','group':'work','keywords':['log','activity','remove','delete'],'usage':'Used for removing activity entry on Kanban board.'}</v>
       </c>
-      <c r="L334" s="15" t="str">
+      <c r="L334" t="str">
         <f t="shared" si="13"/>
         <v>{"id":333,"name":"log-remove","unicode":"EA4C","decimal":59980,"version":"1.1","style":"light","subset":"VSTS","group":"work","keywords":["log","activity","remove","delete"],"usage":"Used for removing activity entry on Kanban board."}</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A335">
+    <row r="335" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="15">
         <f>'Bowtie v1.0 reorg'!A336</f>
-        <v>0</v>
-      </c>
-      <c r="B335">
+        <v>334</v>
+      </c>
+      <c r="B335" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E336</f>
-        <v>0</v>
-      </c>
-      <c r="C335" t="str">
+        <v>live-update-feed-off</v>
+      </c>
+      <c r="C335" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C336</f>
         <v>EA4D</v>
       </c>
-      <c r="D335">
+      <c r="D335" s="15">
         <f>'Bowtie v1.0 reorg'!D336</f>
         <v>59981</v>
       </c>
-      <c r="E335" s="14" t="str">
+      <c r="E335" s="16">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F336),"",'Bowtie v1.0 reorg'!F336)</f>
-        <v/>
-      </c>
-      <c r="F335" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F335" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G336),"",'Bowtie v1.0 reorg'!G336)</f>
-        <v/>
-      </c>
-      <c r="G335" t="str">
+        <v>light</v>
+      </c>
+      <c r="G335" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I336),"",'Bowtie v1.0 reorg'!I336)</f>
-        <v/>
-      </c>
-      <c r="H335" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H335" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J336),"",'Bowtie v1.0 reorg'!J336)</f>
-        <v/>
-      </c>
-      <c r="I335" t="str">
+        <v>work</v>
+      </c>
+      <c r="I335" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H336),"",'Bowtie v1.0 reorg'!H336)</f>
-        <v/>
-      </c>
-      <c r="J335" t="str">
+        <v>live update feed signal broadcast radar off</v>
+      </c>
+      <c r="J335" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K336),"",'Bowtie v1.0 reorg'!K336)</f>
-        <v/>
-      </c>
-      <c r="K335" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L335" t="e">
+        <v>Used to indicate listen to Kanban board live updates is toggled off. Adding a slash is not the common toggle off pattern. It is only used in this case.</v>
+      </c>
+      <c r="K335" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>{'id':334,'name':'live-update-feed-off','unicode':'EA4D','decimal':59981,'version':'1.1','style':'light','subset':'VSTS','group':'work','keywords':['live','update','feed','signal','broadcast','radar','off'],'usage':'Used to indicate listen to Kanban board live updates is toggled off. Adding a slash is not the common toggle off pattern. It is only used in this case.'}</v>
+      </c>
+      <c r="L335" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+        <v>{"id":334,"name":"live-update-feed-off","unicode":"EA4D","decimal":59981,"version":"1.1","style":"light","subset":"VSTS","group":"work","keywords":["live","update","feed","signal","broadcast","radar","off"],"usage":"Used to indicate listen to Kanban board live updates is toggled off. Adding a slash is not the common toggle off pattern. It is only used in this case."}</v>
       </c>
     </row>
     <row r="336" spans="1:12" x14ac:dyDescent="0.25">
@@ -43633,7 +43710,7 @@
         <v/>
       </c>
       <c r="K336" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
       <c r="L336" t="e">
@@ -43683,7 +43760,7 @@
         <v/>
       </c>
       <c r="K337" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
       <c r="L337" t="e">
@@ -43737,7 +43814,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="L338" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L333:L339" si="14">SUBSTITUTE(K338,"'","""")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -43787,7 +43864,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="L339" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new icons corner-resize and link-remove
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="588">
   <si>
     <t>name</t>
   </si>
@@ -1766,6 +1766,24 @@
   </si>
   <si>
     <t>Used to indicate listen to Kanban board live updates is toggled off. Adding a slash is not the common toggle off pattern. It is only used in this case.</t>
+  </si>
+  <si>
+    <t>corner-resize</t>
+  </si>
+  <si>
+    <t>resize grip handle</t>
+  </si>
+  <si>
+    <t>Used for dialog, modal, or textarea resize handle.</t>
+  </si>
+  <si>
+    <t>link-remove</t>
+  </si>
+  <si>
+    <t>link hyperlink url remove</t>
+  </si>
+  <si>
+    <t>Used for removing hyperlink.</t>
   </si>
 </sst>
 </file>
@@ -14599,6 +14617,82 @@
         <a:xfrm>
           <a:off x="1104900" y="134616825"/>
           <a:ext cx="266737" cy="247685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>336</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361977</xdr:colOff>
+      <xdr:row>336</xdr:row>
+      <xdr:rowOff>342928</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="336" name="Picture 335"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId335"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="135045450"/>
+          <a:ext cx="190527" cy="200053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>337</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390564</xdr:colOff>
+      <xdr:row>337</xdr:row>
+      <xdr:rowOff>361986</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="337" name="Picture 336"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId336"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1057275" y="135407400"/>
+          <a:ext cx="276264" cy="257211"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14875,9 +14969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL410"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A331" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K340" sqref="K340"/>
+      <selection pane="bottomLeft" activeCell="F339" sqref="F339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26254,9 +26348,30 @@
       <c r="D337" s="13">
         <v>59982</v>
       </c>
+      <c r="E337" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="F337" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G337" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H337" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="I337" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J337" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K337" s="2" t="s">
+        <v>584</v>
+      </c>
       <c r="L337" t="str">
         <f t="shared" si="11"/>
-        <v>uEA4E-.svg</v>
+        <v>uEA4E-corner-resize.svg</v>
       </c>
     </row>
     <row r="338" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -26267,9 +26382,30 @@
       <c r="D338" s="13">
         <v>59983</v>
       </c>
+      <c r="E338" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="F338" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G338" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H338" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="I338" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J338" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K338" s="2" t="s">
+        <v>587</v>
+      </c>
       <c r="L338" t="str">
         <f t="shared" si="11"/>
-        <v>uEA4F-.svg</v>
+        <v>uEA4F-link-remove.svg</v>
       </c>
     </row>
     <row r="339" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -26922,7 +27058,7 @@
   <dimension ref="A1:L339"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B312" workbookViewId="0">
-      <selection activeCell="L335" sqref="L335"/>
+      <selection activeCell="M332" sqref="M332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43618,154 +43754,154 @@
         <v>{"id":333,"name":"log-remove","unicode":"EA4C","decimal":59980,"version":"1.1","style":"light","subset":"VSTS","group":"work","keywords":["log","activity","remove","delete"],"usage":"Used for removing activity entry on Kanban board."}</v>
       </c>
     </row>
-    <row r="335" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A335" s="15">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A335">
         <f>'Bowtie v1.0 reorg'!A336</f>
         <v>334</v>
       </c>
-      <c r="B335" s="15" t="str">
+      <c r="B335" t="str">
         <f>'Bowtie v1.0 reorg'!E336</f>
         <v>live-update-feed-off</v>
       </c>
-      <c r="C335" s="15" t="str">
+      <c r="C335" t="str">
         <f>'Bowtie v1.0 reorg'!C336</f>
         <v>EA4D</v>
       </c>
-      <c r="D335" s="15">
+      <c r="D335">
         <f>'Bowtie v1.0 reorg'!D336</f>
         <v>59981</v>
       </c>
-      <c r="E335" s="16">
+      <c r="E335">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F336),"",'Bowtie v1.0 reorg'!F336)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F335" s="15" t="str">
+      <c r="F335" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G336),"",'Bowtie v1.0 reorg'!G336)</f>
         <v>light</v>
       </c>
-      <c r="G335" s="15" t="str">
+      <c r="G335" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I336),"",'Bowtie v1.0 reorg'!I336)</f>
         <v>VSTS</v>
       </c>
-      <c r="H335" s="15" t="str">
+      <c r="H335" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J336),"",'Bowtie v1.0 reorg'!J336)</f>
         <v>work</v>
       </c>
-      <c r="I335" s="15" t="str">
+      <c r="I335" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H336),"",'Bowtie v1.0 reorg'!H336)</f>
         <v>live update feed signal broadcast radar off</v>
       </c>
-      <c r="J335" s="15" t="str">
+      <c r="J335" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K336),"",'Bowtie v1.0 reorg'!K336)</f>
         <v>Used to indicate listen to Kanban board live updates is toggled off. Adding a slash is not the common toggle off pattern. It is only used in this case.</v>
       </c>
-      <c r="K335" s="15" t="str">
+      <c r="K335" t="str">
         <f t="shared" si="10"/>
         <v>{'id':334,'name':'live-update-feed-off','unicode':'EA4D','decimal':59981,'version':'1.1','style':'light','subset':'VSTS','group':'work','keywords':['live','update','feed','signal','broadcast','radar','off'],'usage':'Used to indicate listen to Kanban board live updates is toggled off. Adding a slash is not the common toggle off pattern. It is only used in this case.'}</v>
       </c>
-      <c r="L335" s="15" t="str">
+      <c r="L335" t="str">
         <f t="shared" si="13"/>
         <v>{"id":334,"name":"live-update-feed-off","unicode":"EA4D","decimal":59981,"version":"1.1","style":"light","subset":"VSTS","group":"work","keywords":["live","update","feed","signal","broadcast","radar","off"],"usage":"Used to indicate listen to Kanban board live updates is toggled off. Adding a slash is not the common toggle off pattern. It is only used in this case."}</v>
       </c>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A336">
+    <row r="336" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="15">
         <f>'Bowtie v1.0 reorg'!A337</f>
         <v>0</v>
       </c>
-      <c r="B336">
+      <c r="B336" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E337</f>
-        <v>0</v>
-      </c>
-      <c r="C336" t="str">
+        <v>corner-resize</v>
+      </c>
+      <c r="C336" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C337</f>
         <v>EA4E</v>
       </c>
-      <c r="D336">
+      <c r="D336" s="15">
         <f>'Bowtie v1.0 reorg'!D337</f>
         <v>59982</v>
       </c>
-      <c r="E336" s="14" t="str">
+      <c r="E336" s="16">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F337),"",'Bowtie v1.0 reorg'!F337)</f>
-        <v/>
-      </c>
-      <c r="F336" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F336" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G337),"",'Bowtie v1.0 reorg'!G337)</f>
-        <v/>
-      </c>
-      <c r="G336" t="str">
+        <v>light</v>
+      </c>
+      <c r="G336" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I337),"",'Bowtie v1.0 reorg'!I337)</f>
-        <v/>
-      </c>
-      <c r="H336" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H336" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J337),"",'Bowtie v1.0 reorg'!J337)</f>
-        <v/>
-      </c>
-      <c r="I336" t="str">
+        <v>control</v>
+      </c>
+      <c r="I336" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H337),"",'Bowtie v1.0 reorg'!H337)</f>
-        <v/>
-      </c>
-      <c r="J336" t="str">
+        <v>resize grip handle</v>
+      </c>
+      <c r="J336" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K337),"",'Bowtie v1.0 reorg'!K337)</f>
-        <v/>
-      </c>
-      <c r="K336" t="e">
+        <v>Used for dialog, modal, or textarea resize handle.</v>
+      </c>
+      <c r="K336" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L336" t="e">
+        <v>{'id':0,'name':'corner-resize','unicode':'EA4E','decimal':59982,'version':'1.1','style':'light','subset':'VSTS','group':'control','keywords':['resize','grip','handle'],'usage':'Used for dialog, modal, or textarea resize handle.'}</v>
+      </c>
+      <c r="L336" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A337">
+        <v>{"id":0,"name":"corner-resize","unicode":"EA4E","decimal":59982,"version":"1.1","style":"light","subset":"VSTS","group":"control","keywords":["resize","grip","handle"],"usage":"Used for dialog, modal, or textarea resize handle."}</v>
+      </c>
+    </row>
+    <row r="337" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A337" s="15">
         <f>'Bowtie v1.0 reorg'!A338</f>
         <v>0</v>
       </c>
-      <c r="B337">
+      <c r="B337" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E338</f>
-        <v>0</v>
-      </c>
-      <c r="C337" t="str">
+        <v>link-remove</v>
+      </c>
+      <c r="C337" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C338</f>
         <v>EA4F</v>
       </c>
-      <c r="D337">
+      <c r="D337" s="15">
         <f>'Bowtie v1.0 reorg'!D338</f>
         <v>59983</v>
       </c>
-      <c r="E337" s="14" t="str">
+      <c r="E337" s="16">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F338),"",'Bowtie v1.0 reorg'!F338)</f>
-        <v/>
-      </c>
-      <c r="F337" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F337" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G338),"",'Bowtie v1.0 reorg'!G338)</f>
-        <v/>
-      </c>
-      <c r="G337" t="str">
+        <v>light</v>
+      </c>
+      <c r="G337" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I338),"",'Bowtie v1.0 reorg'!I338)</f>
-        <v/>
-      </c>
-      <c r="H337" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H337" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J338),"",'Bowtie v1.0 reorg'!J338)</f>
-        <v/>
-      </c>
-      <c r="I337" t="str">
+        <v>editor</v>
+      </c>
+      <c r="I337" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H338),"",'Bowtie v1.0 reorg'!H338)</f>
-        <v/>
-      </c>
-      <c r="J337" t="str">
+        <v>link hyperlink url remove</v>
+      </c>
+      <c r="J337" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K338),"",'Bowtie v1.0 reorg'!K338)</f>
-        <v/>
-      </c>
-      <c r="K337" t="e">
+        <v>Used for removing hyperlink.</v>
+      </c>
+      <c r="K337" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L337" t="e">
+        <v>{'id':0,'name':'link-remove','unicode':'EA4F','decimal':59983,'version':'1.1','style':'light','subset':'VSTS','group':'editor','keywords':['link','hyperlink','url','remove'],'usage':'Used for removing hyperlink.'}</v>
+      </c>
+      <c r="L337" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+        <v>{"id":0,"name":"link-remove","unicode":"EA4F","decimal":59983,"version":"1.1","style":"light","subset":"VSTS","group":"editor","keywords":["link","hyperlink","url","remove"],"usage":"Used for removing hyperlink."}</v>
       </c>
     </row>
     <row r="338" spans="1:12" x14ac:dyDescent="0.25">
@@ -43814,7 +43950,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="L338" t="e">
-        <f t="shared" ref="L333:L339" si="14">SUBSTITUTE(K338,"'","""")</f>
+        <f t="shared" ref="L338:L339" si="14">SUBSTITUTE(K338,"'","""")</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix id metadata for last 2 new icons in json
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -14969,9 +14969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL410"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A331" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F339" sqref="F339"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A337" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F336" sqref="F336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26340,7 +26340,10 @@
         <v>uEA4D-live-update-feed-off.svg</v>
       </c>
     </row>
-    <row r="337" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A337" s="2">
+        <v>335</v>
+      </c>
       <c r="C337" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA4E</v>
@@ -26374,7 +26377,10 @@
         <v>uEA4E-corner-resize.svg</v>
       </c>
     </row>
-    <row r="338" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A338" s="2">
+        <v>336</v>
+      </c>
       <c r="C338" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA4F</v>
@@ -26408,7 +26414,10 @@
         <v>uEA4F-link-remove.svg</v>
       </c>
     </row>
-    <row r="339" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="2">
+        <v>337</v>
+      </c>
       <c r="C339" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA50</v>
@@ -26421,7 +26430,10 @@
         <v>uEA50-.svg</v>
       </c>
     </row>
-    <row r="340" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="2">
+        <v>338</v>
+      </c>
       <c r="C340" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA51</v>
@@ -26434,7 +26446,10 @@
         <v>uEA51-.svg</v>
       </c>
     </row>
-    <row r="341" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="2">
+        <v>339</v>
+      </c>
       <c r="C341" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA52</v>
@@ -26447,7 +26462,10 @@
         <v>uEA52-.svg</v>
       </c>
     </row>
-    <row r="342" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="2">
+        <v>340</v>
+      </c>
       <c r="C342" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA53</v>
@@ -26460,7 +26478,10 @@
         <v>uEA53-.svg</v>
       </c>
     </row>
-    <row r="343" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="2">
+        <v>341</v>
+      </c>
       <c r="C343" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA54</v>
@@ -26473,7 +26494,10 @@
         <v>uEA54-.svg</v>
       </c>
     </row>
-    <row r="344" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="2">
+        <v>342</v>
+      </c>
       <c r="C344" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA55</v>
@@ -26486,7 +26510,10 @@
         <v>uEA55-.svg</v>
       </c>
     </row>
-    <row r="345" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A345" s="2">
+        <v>343</v>
+      </c>
       <c r="C345" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA56</v>
@@ -26499,7 +26526,10 @@
         <v>uEA56-.svg</v>
       </c>
     </row>
-    <row r="346" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="2">
+        <v>344</v>
+      </c>
       <c r="C346" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA57</v>
@@ -26512,7 +26542,10 @@
         <v>uEA57-.svg</v>
       </c>
     </row>
-    <row r="347" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="2">
+        <v>345</v>
+      </c>
       <c r="C347" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA58</v>
@@ -26525,7 +26558,10 @@
         <v>uEA58-.svg</v>
       </c>
     </row>
-    <row r="348" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="2">
+        <v>346</v>
+      </c>
       <c r="C348" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA59</v>
@@ -26538,7 +26574,10 @@
         <v>uEA59-.svg</v>
       </c>
     </row>
-    <row r="349" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="2">
+        <v>347</v>
+      </c>
       <c r="C349" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA5A</v>
@@ -26551,7 +26590,10 @@
         <v>uEA5A-.svg</v>
       </c>
     </row>
-    <row r="350" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A350" s="2">
+        <v>348</v>
+      </c>
       <c r="C350" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA5B</v>
@@ -26564,7 +26606,10 @@
         <v>uEA5B-.svg</v>
       </c>
     </row>
-    <row r="351" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A351" s="2">
+        <v>349</v>
+      </c>
       <c r="C351" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA5C</v>
@@ -26577,7 +26622,10 @@
         <v>uEA5C-.svg</v>
       </c>
     </row>
-    <row r="352" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A352" s="2">
+        <v>350</v>
+      </c>
       <c r="C352" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA5D</v>
@@ -26590,7 +26638,10 @@
         <v>uEA5D-.svg</v>
       </c>
     </row>
-    <row r="353" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="2">
+        <v>351</v>
+      </c>
       <c r="C353" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA5E</v>
@@ -26603,7 +26654,10 @@
         <v>uEA5E-.svg</v>
       </c>
     </row>
-    <row r="354" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A354" s="2">
+        <v>352</v>
+      </c>
       <c r="C354" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA5F</v>
@@ -26616,7 +26670,10 @@
         <v>uEA5F-.svg</v>
       </c>
     </row>
-    <row r="355" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A355" s="2">
+        <v>353</v>
+      </c>
       <c r="C355" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA60</v>
@@ -26629,7 +26686,10 @@
         <v>uEA60-.svg</v>
       </c>
     </row>
-    <row r="356" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A356" s="2">
+        <v>354</v>
+      </c>
       <c r="C356" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA61</v>
@@ -26642,7 +26702,10 @@
         <v>uEA61-.svg</v>
       </c>
     </row>
-    <row r="357" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A357" s="2">
+        <v>355</v>
+      </c>
       <c r="C357" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA62</v>
@@ -26655,7 +26718,10 @@
         <v>uEA62-.svg</v>
       </c>
     </row>
-    <row r="358" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A358" s="2">
+        <v>356</v>
+      </c>
       <c r="C358" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA63</v>
@@ -26664,7 +26730,10 @@
         <v>60003</v>
       </c>
     </row>
-    <row r="359" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A359" s="2">
+        <v>357</v>
+      </c>
       <c r="C359" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA64</v>
@@ -26673,7 +26742,10 @@
         <v>60004</v>
       </c>
     </row>
-    <row r="360" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A360" s="2">
+        <v>358</v>
+      </c>
       <c r="C360" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA65</v>
@@ -26682,7 +26754,10 @@
         <v>60005</v>
       </c>
     </row>
-    <row r="361" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A361" s="2">
+        <v>359</v>
+      </c>
       <c r="C361" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA66</v>
@@ -26691,7 +26766,10 @@
         <v>60006</v>
       </c>
     </row>
-    <row r="362" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="2">
+        <v>360</v>
+      </c>
       <c r="C362" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA67</v>
@@ -26700,7 +26778,10 @@
         <v>60007</v>
       </c>
     </row>
-    <row r="363" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A363" s="2">
+        <v>361</v>
+      </c>
       <c r="C363" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA68</v>
@@ -26709,7 +26790,10 @@
         <v>60008</v>
       </c>
     </row>
-    <row r="364" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A364" s="2">
+        <v>362</v>
+      </c>
       <c r="C364" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA69</v>
@@ -26718,7 +26802,10 @@
         <v>60009</v>
       </c>
     </row>
-    <row r="365" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A365" s="2">
+        <v>363</v>
+      </c>
       <c r="C365" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA6A</v>
@@ -26727,7 +26814,10 @@
         <v>60010</v>
       </c>
     </row>
-    <row r="366" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A366" s="2">
+        <v>364</v>
+      </c>
       <c r="C366" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA6B</v>
@@ -26736,7 +26826,10 @@
         <v>60011</v>
       </c>
     </row>
-    <row r="367" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A367" s="2">
+        <v>365</v>
+      </c>
       <c r="C367" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA6C</v>
@@ -26745,7 +26838,10 @@
         <v>60012</v>
       </c>
     </row>
-    <row r="368" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A368" s="2">
+        <v>366</v>
+      </c>
       <c r="C368" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA6D</v>
@@ -26754,7 +26850,10 @@
         <v>60013</v>
       </c>
     </row>
-    <row r="369" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A369" s="2">
+        <v>367</v>
+      </c>
       <c r="C369" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA6E</v>
@@ -26763,7 +26862,10 @@
         <v>60014</v>
       </c>
     </row>
-    <row r="370" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A370" s="2">
+        <v>368</v>
+      </c>
       <c r="C370" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA6F</v>
@@ -26772,7 +26874,10 @@
         <v>60015</v>
       </c>
     </row>
-    <row r="371" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A371" s="2">
+        <v>369</v>
+      </c>
       <c r="C371" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA70</v>
@@ -26781,7 +26886,10 @@
         <v>60016</v>
       </c>
     </row>
-    <row r="372" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A372" s="2">
+        <v>370</v>
+      </c>
       <c r="C372" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA71</v>
@@ -26790,7 +26898,10 @@
         <v>60017</v>
       </c>
     </row>
-    <row r="373" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A373" s="2">
+        <v>371</v>
+      </c>
       <c r="C373" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA72</v>
@@ -26799,7 +26910,10 @@
         <v>60018</v>
       </c>
     </row>
-    <row r="374" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A374" s="2">
+        <v>372</v>
+      </c>
       <c r="C374" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA73</v>
@@ -26808,7 +26922,10 @@
         <v>60019</v>
       </c>
     </row>
-    <row r="375" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A375" s="2">
+        <v>373</v>
+      </c>
       <c r="C375" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA74</v>
@@ -26817,7 +26934,10 @@
         <v>60020</v>
       </c>
     </row>
-    <row r="376" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A376" s="2">
+        <v>374</v>
+      </c>
       <c r="C376" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA75</v>
@@ -26826,7 +26946,10 @@
         <v>60021</v>
       </c>
     </row>
-    <row r="377" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A377" s="2">
+        <v>375</v>
+      </c>
       <c r="C377" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA76</v>
@@ -26835,7 +26958,10 @@
         <v>60022</v>
       </c>
     </row>
-    <row r="378" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A378" s="2">
+        <v>376</v>
+      </c>
       <c r="C378" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA77</v>
@@ -26844,7 +26970,7 @@
         <v>60023</v>
       </c>
     </row>
-    <row r="379" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C379" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA78</v>
@@ -26853,7 +26979,7 @@
         <v>60024</v>
       </c>
     </row>
-    <row r="380" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C380" s="13" t="str">
         <f t="shared" si="10"/>
         <v>EA79</v>
@@ -26862,25 +26988,25 @@
         <v>60025</v>
       </c>
     </row>
-    <row r="381" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C381" s="13" t="str">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C382" s="13" t="str">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C383" s="13" t="str">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="3:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C384" s="13" t="str">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -27057,8 +27183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B312" workbookViewId="0">
-      <selection activeCell="M332" sqref="M332"/>
+    <sheetView tabSelected="1" topLeftCell="B321" workbookViewId="0">
+      <selection activeCell="L336" sqref="L336:L337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43807,7 +43933,7 @@
     <row r="336" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A336" s="15">
         <f>'Bowtie v1.0 reorg'!A337</f>
-        <v>0</v>
+        <v>335</v>
       </c>
       <c r="B336" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E337</f>
@@ -43847,17 +43973,17 @@
       </c>
       <c r="K336" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>{'id':0,'name':'corner-resize','unicode':'EA4E','decimal':59982,'version':'1.1','style':'light','subset':'VSTS','group':'control','keywords':['resize','grip','handle'],'usage':'Used for dialog, modal, or textarea resize handle.'}</v>
+        <v>{'id':335,'name':'corner-resize','unicode':'EA4E','decimal':59982,'version':'1.1','style':'light','subset':'VSTS','group':'control','keywords':['resize','grip','handle'],'usage':'Used for dialog, modal, or textarea resize handle.'}</v>
       </c>
       <c r="L336" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>{"id":0,"name":"corner-resize","unicode":"EA4E","decimal":59982,"version":"1.1","style":"light","subset":"VSTS","group":"control","keywords":["resize","grip","handle"],"usage":"Used for dialog, modal, or textarea resize handle."}</v>
+        <v>{"id":335,"name":"corner-resize","unicode":"EA4E","decimal":59982,"version":"1.1","style":"light","subset":"VSTS","group":"control","keywords":["resize","grip","handle"],"usage":"Used for dialog, modal, or textarea resize handle."}</v>
       </c>
     </row>
     <row r="337" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A337" s="15">
         <f>'Bowtie v1.0 reorg'!A338</f>
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="B337" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E338</f>
@@ -43897,17 +44023,17 @@
       </c>
       <c r="K337" s="15" t="str">
         <f t="shared" si="10"/>
-        <v>{'id':0,'name':'link-remove','unicode':'EA4F','decimal':59983,'version':'1.1','style':'light','subset':'VSTS','group':'editor','keywords':['link','hyperlink','url','remove'],'usage':'Used for removing hyperlink.'}</v>
+        <v>{'id':336,'name':'link-remove','unicode':'EA4F','decimal':59983,'version':'1.1','style':'light','subset':'VSTS','group':'editor','keywords':['link','hyperlink','url','remove'],'usage':'Used for removing hyperlink.'}</v>
       </c>
       <c r="L337" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>{"id":0,"name":"link-remove","unicode":"EA4F","decimal":59983,"version":"1.1","style":"light","subset":"VSTS","group":"editor","keywords":["link","hyperlink","url","remove"],"usage":"Used for removing hyperlink."}</v>
+        <v>{"id":336,"name":"link-remove","unicode":"EA4F","decimal":59983,"version":"1.1","style":"light","subset":"VSTS","group":"editor","keywords":["link","hyperlink","url","remove"],"usage":"Used for removing hyperlink."}</v>
       </c>
     </row>
     <row r="338" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A338">
         <f>'Bowtie v1.0 reorg'!A339</f>
-        <v>0</v>
+        <v>337</v>
       </c>
       <c r="B338">
         <f>'Bowtie v1.0 reorg'!E339</f>
@@ -43957,7 +44083,7 @@
     <row r="339" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A339">
         <f>'Bowtie v1.0 reorg'!A340</f>
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="B339">
         <f>'Bowtie v1.0 reorg'!E340</f>

</xml_diff>

<commit_message>
added personalize icon for Work, revised some icons alignment, added 2 draft query icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="591">
   <si>
     <t>name</t>
   </si>
@@ -1784,6 +1784,15 @@
   </si>
   <si>
     <t>Used for removing hyperlink.</t>
+  </si>
+  <si>
+    <t>personalize</t>
+  </si>
+  <si>
+    <t>personalize customize design edit draw pen brush</t>
+  </si>
+  <si>
+    <t>Used for customizing work item form.</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +1878,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1911,6 +1920,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -14693,6 +14708,44 @@
         <a:xfrm>
           <a:off x="1057275" y="135407400"/>
           <a:ext cx="276264" cy="257211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>338</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419137</xdr:colOff>
+      <xdr:row>338</xdr:row>
+      <xdr:rowOff>342933</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="338" name="Picture 337"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId337"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1095375" y="135807450"/>
+          <a:ext cx="266737" cy="238158"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14969,12 +15022,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL410"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A337" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F336" sqref="F336"/>
+      <selection pane="bottomLeft" activeCell="F342" sqref="F342"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -14986,6 +15039,7 @@
     <col min="8" max="8" width="29.85546875" style="2" customWidth="1"/>
     <col min="9" max="10" width="14.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="28" style="2" customWidth="1"/>
+    <col min="12" max="38" width="9" customWidth="1"/>
     <col min="39" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -26340,7 +26394,7 @@
         <v>uEA4D-live-update-feed-off.svg</v>
       </c>
     </row>
-    <row r="337" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="2">
         <v>335</v>
       </c>
@@ -26377,7 +26431,7 @@
         <v>uEA4E-corner-resize.svg</v>
       </c>
     </row>
-    <row r="338" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="2">
         <v>336</v>
       </c>
@@ -26414,23 +26468,70 @@
         <v>uEA4F-link-remove.svg</v>
       </c>
     </row>
-    <row r="339" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A339" s="2">
+    <row r="339" spans="1:38" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="1">
         <v>337</v>
       </c>
-      <c r="C339" s="13" t="str">
+      <c r="C339" s="17" t="str">
         <f t="shared" si="10"/>
         <v>EA50</v>
       </c>
-      <c r="D339" s="13">
+      <c r="D339" s="17">
         <v>59984</v>
       </c>
-      <c r="L339" t="str">
+      <c r="E339" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="F339" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G339" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H339" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="I339" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J339" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K339" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="L339" s="15" t="str">
         <f t="shared" si="11"/>
-        <v>uEA50-.svg</v>
-      </c>
-    </row>
-    <row r="340" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>uEA50-personalize.svg</v>
+      </c>
+      <c r="M339" s="15"/>
+      <c r="N339" s="15"/>
+      <c r="O339" s="15"/>
+      <c r="P339" s="15"/>
+      <c r="Q339" s="15"/>
+      <c r="R339" s="15"/>
+      <c r="S339" s="15"/>
+      <c r="T339" s="15"/>
+      <c r="U339" s="15"/>
+      <c r="V339" s="15"/>
+      <c r="W339" s="15"/>
+      <c r="X339" s="15"/>
+      <c r="Y339" s="15"/>
+      <c r="Z339" s="15"/>
+      <c r="AA339" s="15"/>
+      <c r="AB339" s="15"/>
+      <c r="AC339" s="15"/>
+      <c r="AD339" s="15"/>
+      <c r="AE339" s="15"/>
+      <c r="AF339" s="15"/>
+      <c r="AG339" s="15"/>
+      <c r="AH339" s="15"/>
+      <c r="AI339" s="15"/>
+      <c r="AJ339" s="15"/>
+      <c r="AK339" s="15"/>
+      <c r="AL339" s="15"/>
+    </row>
+    <row r="340" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="2">
         <v>338</v>
       </c>
@@ -26446,7 +26547,7 @@
         <v>uEA51-.svg</v>
       </c>
     </row>
-    <row r="341" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="2">
         <v>339</v>
       </c>
@@ -26462,7 +26563,7 @@
         <v>uEA52-.svg</v>
       </c>
     </row>
-    <row r="342" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A342" s="2">
         <v>340</v>
       </c>
@@ -26478,7 +26579,7 @@
         <v>uEA53-.svg</v>
       </c>
     </row>
-    <row r="343" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="2">
         <v>341</v>
       </c>
@@ -26494,7 +26595,7 @@
         <v>uEA54-.svg</v>
       </c>
     </row>
-    <row r="344" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="2">
         <v>342</v>
       </c>
@@ -26510,7 +26611,7 @@
         <v>uEA55-.svg</v>
       </c>
     </row>
-    <row r="345" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="2">
         <v>343</v>
       </c>
@@ -26526,7 +26627,7 @@
         <v>uEA56-.svg</v>
       </c>
     </row>
-    <row r="346" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="2">
         <v>344</v>
       </c>
@@ -26542,7 +26643,7 @@
         <v>uEA57-.svg</v>
       </c>
     </row>
-    <row r="347" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="2">
         <v>345</v>
       </c>
@@ -26558,7 +26659,7 @@
         <v>uEA58-.svg</v>
       </c>
     </row>
-    <row r="348" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="2">
         <v>346</v>
       </c>
@@ -26574,7 +26675,7 @@
         <v>uEA59-.svg</v>
       </c>
     </row>
-    <row r="349" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A349" s="2">
         <v>347</v>
       </c>
@@ -26590,7 +26691,7 @@
         <v>uEA5A-.svg</v>
       </c>
     </row>
-    <row r="350" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A350" s="2">
         <v>348</v>
       </c>
@@ -26606,7 +26707,7 @@
         <v>uEA5B-.svg</v>
       </c>
     </row>
-    <row r="351" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="2">
         <v>349</v>
       </c>
@@ -26622,7 +26723,7 @@
         <v>uEA5C-.svg</v>
       </c>
     </row>
-    <row r="352" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="2">
         <v>350</v>
       </c>
@@ -27181,10 +27282,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L339"/>
+  <dimension ref="A1:M362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B321" workbookViewId="0">
-      <selection activeCell="L336" sqref="L336:L337"/>
+    <sheetView topLeftCell="A335" workbookViewId="0">
+      <selection activeCell="L338" sqref="L338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43822,7 +43923,7 @@
         <v>Used for creating a child node of the current node in a tree structure.</v>
       </c>
       <c r="K333" t="str">
-        <f t="shared" ref="K333:K339" si="12">IF(NOT(ISBLANK(A333)),CONCATENATE("{'",$A$1,"':",A333,",'",$B$1,"':'",B333,"',","'",$C$1,"':'",C333,"','",$D$1,"':",D333,",'",$E$1,"':'",FIXED(E333,1),"','",$F$1,"':'",F333,"','",$G$1,"':'",G333,"','",$H$1,"':'",H333,"','",$I$1,"':['",SUBSTITUTE(I333," ","','"),"'],'",$J$1,"':'",J333,"'}"))</f>
+        <f t="shared" ref="K333:K340" si="12">IF(NOT(ISBLANK(A333)),CONCATENATE("{'",$A$1,"':",A333,",'",$B$1,"':'",B333,"',","'",$C$1,"':'",C333,"','",$D$1,"':",D333,",'",$E$1,"':'",FIXED(E333,1),"','",$F$1,"':'",F333,"','",$G$1,"':'",G333,"','",$H$1,"':'",H333,"','",$I$1,"':['",SUBSTITUTE(I333," ","','"),"'],'",$J$1,"':'",J333,"'}"))</f>
         <v>{'id':332,'name':'row-child','unicode':'EA4B','decimal':59979,'version':'1.1','style':'light','subset':'VSTS','group':'common','keywords':['row','child','sub','indent','tree'],'usage':'Used for creating a child node of the current node in a tree structure.'}</v>
       </c>
       <c r="L333" t="str">
@@ -43930,157 +44031,157 @@
         <v>{"id":334,"name":"live-update-feed-off","unicode":"EA4D","decimal":59981,"version":"1.1","style":"light","subset":"VSTS","group":"work","keywords":["live","update","feed","signal","broadcast","radar","off"],"usage":"Used to indicate listen to Kanban board live updates is toggled off. Adding a slash is not the common toggle off pattern. It is only used in this case."}</v>
       </c>
     </row>
-    <row r="336" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A336" s="15">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A336">
         <f>'Bowtie v1.0 reorg'!A337</f>
         <v>335</v>
       </c>
-      <c r="B336" s="15" t="str">
+      <c r="B336" t="str">
         <f>'Bowtie v1.0 reorg'!E337</f>
         <v>corner-resize</v>
       </c>
-      <c r="C336" s="15" t="str">
+      <c r="C336" t="str">
         <f>'Bowtie v1.0 reorg'!C337</f>
         <v>EA4E</v>
       </c>
-      <c r="D336" s="15">
+      <c r="D336">
         <f>'Bowtie v1.0 reorg'!D337</f>
         <v>59982</v>
       </c>
-      <c r="E336" s="16">
+      <c r="E336">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F337),"",'Bowtie v1.0 reorg'!F337)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F336" s="15" t="str">
+      <c r="F336" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G337),"",'Bowtie v1.0 reorg'!G337)</f>
         <v>light</v>
       </c>
-      <c r="G336" s="15" t="str">
+      <c r="G336" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I337),"",'Bowtie v1.0 reorg'!I337)</f>
         <v>VSTS</v>
       </c>
-      <c r="H336" s="15" t="str">
+      <c r="H336" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J337),"",'Bowtie v1.0 reorg'!J337)</f>
         <v>control</v>
       </c>
-      <c r="I336" s="15" t="str">
+      <c r="I336" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H337),"",'Bowtie v1.0 reorg'!H337)</f>
         <v>resize grip handle</v>
       </c>
-      <c r="J336" s="15" t="str">
+      <c r="J336" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K337),"",'Bowtie v1.0 reorg'!K337)</f>
         <v>Used for dialog, modal, or textarea resize handle.</v>
       </c>
-      <c r="K336" s="15" t="str">
+      <c r="K336" t="str">
         <f t="shared" si="10"/>
         <v>{'id':335,'name':'corner-resize','unicode':'EA4E','decimal':59982,'version':'1.1','style':'light','subset':'VSTS','group':'control','keywords':['resize','grip','handle'],'usage':'Used for dialog, modal, or textarea resize handle.'}</v>
       </c>
-      <c r="L336" s="15" t="str">
+      <c r="L336" t="str">
         <f t="shared" si="13"/>
         <v>{"id":335,"name":"corner-resize","unicode":"EA4E","decimal":59982,"version":"1.1","style":"light","subset":"VSTS","group":"control","keywords":["resize","grip","handle"],"usage":"Used for dialog, modal, or textarea resize handle."}</v>
       </c>
     </row>
-    <row r="337" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A337" s="15">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A337">
         <f>'Bowtie v1.0 reorg'!A338</f>
         <v>336</v>
       </c>
-      <c r="B337" s="15" t="str">
+      <c r="B337" t="str">
         <f>'Bowtie v1.0 reorg'!E338</f>
         <v>link-remove</v>
       </c>
-      <c r="C337" s="15" t="str">
+      <c r="C337" t="str">
         <f>'Bowtie v1.0 reorg'!C338</f>
         <v>EA4F</v>
       </c>
-      <c r="D337" s="15">
+      <c r="D337">
         <f>'Bowtie v1.0 reorg'!D338</f>
         <v>59983</v>
       </c>
-      <c r="E337" s="16">
+      <c r="E337">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F338),"",'Bowtie v1.0 reorg'!F338)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F337" s="15" t="str">
+      <c r="F337" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G338),"",'Bowtie v1.0 reorg'!G338)</f>
         <v>light</v>
       </c>
-      <c r="G337" s="15" t="str">
+      <c r="G337" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I338),"",'Bowtie v1.0 reorg'!I338)</f>
         <v>VSTS</v>
       </c>
-      <c r="H337" s="15" t="str">
+      <c r="H337" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J338),"",'Bowtie v1.0 reorg'!J338)</f>
         <v>editor</v>
       </c>
-      <c r="I337" s="15" t="str">
+      <c r="I337" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H338),"",'Bowtie v1.0 reorg'!H338)</f>
         <v>link hyperlink url remove</v>
       </c>
-      <c r="J337" s="15" t="str">
+      <c r="J337" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K338),"",'Bowtie v1.0 reorg'!K338)</f>
         <v>Used for removing hyperlink.</v>
       </c>
-      <c r="K337" s="15" t="str">
+      <c r="K337" t="str">
         <f t="shared" si="10"/>
         <v>{'id':336,'name':'link-remove','unicode':'EA4F','decimal':59983,'version':'1.1','style':'light','subset':'VSTS','group':'editor','keywords':['link','hyperlink','url','remove'],'usage':'Used for removing hyperlink.'}</v>
       </c>
-      <c r="L337" s="15" t="str">
+      <c r="L337" t="str">
         <f t="shared" si="13"/>
         <v>{"id":336,"name":"link-remove","unicode":"EA4F","decimal":59983,"version":"1.1","style":"light","subset":"VSTS","group":"editor","keywords":["link","hyperlink","url","remove"],"usage":"Used for removing hyperlink."}</v>
       </c>
     </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A338">
+    <row r="338" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A338" s="15">
         <f>'Bowtie v1.0 reorg'!A339</f>
         <v>337</v>
       </c>
-      <c r="B338">
+      <c r="B338" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E339</f>
-        <v>0</v>
-      </c>
-      <c r="C338" t="str">
+        <v>personalize</v>
+      </c>
+      <c r="C338" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C339</f>
         <v>EA50</v>
       </c>
-      <c r="D338">
+      <c r="D338" s="15">
         <f>'Bowtie v1.0 reorg'!D339</f>
         <v>59984</v>
       </c>
-      <c r="E338" s="14" t="str">
+      <c r="E338" s="16">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F339),"",'Bowtie v1.0 reorg'!F339)</f>
-        <v/>
-      </c>
-      <c r="F338" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F338" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G339),"",'Bowtie v1.0 reorg'!G339)</f>
-        <v/>
-      </c>
-      <c r="G338" t="str">
+        <v>light</v>
+      </c>
+      <c r="G338" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I339),"",'Bowtie v1.0 reorg'!I339)</f>
-        <v/>
-      </c>
-      <c r="H338" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H338" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J339),"",'Bowtie v1.0 reorg'!J339)</f>
-        <v/>
-      </c>
-      <c r="I338" t="str">
+        <v>work</v>
+      </c>
+      <c r="I338" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H339),"",'Bowtie v1.0 reorg'!H339)</f>
-        <v/>
-      </c>
-      <c r="J338" t="str">
+        <v>personalize customize design edit draw pen brush</v>
+      </c>
+      <c r="J338" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K339),"",'Bowtie v1.0 reorg'!K339)</f>
-        <v/>
-      </c>
-      <c r="K338" t="e">
+        <v>Used for customizing work item form.</v>
+      </c>
+      <c r="K338" s="15" t="str">
         <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L338" t="e">
-        <f t="shared" ref="L338:L339" si="14">SUBSTITUTE(K338,"'","""")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
+        <v>{'id':337,'name':'personalize','unicode':'EA50','decimal':59984,'version':'1.1','style':'light','subset':'VSTS','group':'work','keywords':['personalize','customize','design','edit','draw','pen','brush'],'usage':'Used for customizing work item form.'}</v>
+      </c>
+      <c r="L338" s="15" t="str">
+        <f t="shared" ref="L338:L340" si="14">SUBSTITUTE(K338,"'","""")</f>
+        <v>{"id":337,"name":"personalize","unicode":"EA50","decimal":59984,"version":"1.1","style":"light","subset":"VSTS","group":"work","keywords":["personalize","customize","design","edit","draw","pen","brush"],"usage":"Used for customizing work item form."}</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A339">
         <f>'Bowtie v1.0 reorg'!A340</f>
         <v>338</v>
@@ -44097,7 +44198,7 @@
         <f>'Bowtie v1.0 reorg'!D340</f>
         <v>59985</v>
       </c>
-      <c r="E339" s="14" t="str">
+      <c r="E339" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F340),"",'Bowtie v1.0 reorg'!F340)</f>
         <v/>
       </c>
@@ -44129,6 +44230,1164 @@
         <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
+    </row>
+    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <f>'Bowtie v1.0 reorg'!A341</f>
+        <v>339</v>
+      </c>
+      <c r="B340">
+        <f>'Bowtie v1.0 reorg'!E341</f>
+        <v>0</v>
+      </c>
+      <c r="C340" t="str">
+        <f>'Bowtie v1.0 reorg'!C341</f>
+        <v>EA52</v>
+      </c>
+      <c r="D340">
+        <f>'Bowtie v1.0 reorg'!D341</f>
+        <v>59986</v>
+      </c>
+      <c r="E340" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F341),"",'Bowtie v1.0 reorg'!F341)</f>
+        <v/>
+      </c>
+      <c r="F340" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G341),"",'Bowtie v1.0 reorg'!G341)</f>
+        <v/>
+      </c>
+      <c r="G340" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I341),"",'Bowtie v1.0 reorg'!I341)</f>
+        <v/>
+      </c>
+      <c r="H340" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J341),"",'Bowtie v1.0 reorg'!J341)</f>
+        <v/>
+      </c>
+      <c r="I340" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H341),"",'Bowtie v1.0 reorg'!H341)</f>
+        <v/>
+      </c>
+      <c r="J340" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K341),"",'Bowtie v1.0 reorg'!K341)</f>
+        <v/>
+      </c>
+      <c r="K340" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L340" t="e">
+        <f t="shared" si="14"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A341" s="15">
+        <f>'Bowtie v1.0 reorg'!A342</f>
+        <v>340</v>
+      </c>
+      <c r="B341" s="15">
+        <f>'Bowtie v1.0 reorg'!E342</f>
+        <v>0</v>
+      </c>
+      <c r="C341" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!C342</f>
+        <v>EA53</v>
+      </c>
+      <c r="D341" s="15">
+        <f>'Bowtie v1.0 reorg'!D342</f>
+        <v>59987</v>
+      </c>
+      <c r="E341" s="16" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F342),"",'Bowtie v1.0 reorg'!F342)</f>
+        <v/>
+      </c>
+      <c r="F341" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G342),"",'Bowtie v1.0 reorg'!G342)</f>
+        <v/>
+      </c>
+      <c r="G341" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I342),"",'Bowtie v1.0 reorg'!I342)</f>
+        <v/>
+      </c>
+      <c r="H341" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J342),"",'Bowtie v1.0 reorg'!J342)</f>
+        <v/>
+      </c>
+      <c r="I341" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H342),"",'Bowtie v1.0 reorg'!H342)</f>
+        <v/>
+      </c>
+      <c r="J341" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K342),"",'Bowtie v1.0 reorg'!K342)</f>
+        <v/>
+      </c>
+      <c r="K341" s="15" t="e">
+        <f t="shared" ref="K341:K362" si="15">IF(NOT(ISBLANK(A341)),CONCATENATE("{'",$A$1,"':",A341,",'",$B$1,"':'",B341,"',","'",$C$1,"':'",C341,"','",$D$1,"':",D341,",'",$E$1,"':'",FIXED(E341,1),"','",$F$1,"':'",F341,"','",$G$1,"':'",G341,"','",$H$1,"':'",H341,"','",$I$1,"':['",SUBSTITUTE(I341," ","','"),"'],'",$J$1,"':'",J341,"'}"))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L341" s="15" t="e">
+        <f t="shared" ref="L341:L362" si="16">SUBSTITUTE(K341,"'","""")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M341" s="15"/>
+    </row>
+    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <f>'Bowtie v1.0 reorg'!A343</f>
+        <v>341</v>
+      </c>
+      <c r="B342">
+        <f>'Bowtie v1.0 reorg'!E343</f>
+        <v>0</v>
+      </c>
+      <c r="C342" t="str">
+        <f>'Bowtie v1.0 reorg'!C343</f>
+        <v>EA54</v>
+      </c>
+      <c r="D342">
+        <f>'Bowtie v1.0 reorg'!D343</f>
+        <v>59988</v>
+      </c>
+      <c r="E342" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F343),"",'Bowtie v1.0 reorg'!F343)</f>
+        <v/>
+      </c>
+      <c r="F342" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G343),"",'Bowtie v1.0 reorg'!G343)</f>
+        <v/>
+      </c>
+      <c r="G342" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I343),"",'Bowtie v1.0 reorg'!I343)</f>
+        <v/>
+      </c>
+      <c r="H342" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J343),"",'Bowtie v1.0 reorg'!J343)</f>
+        <v/>
+      </c>
+      <c r="I342" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H343),"",'Bowtie v1.0 reorg'!H343)</f>
+        <v/>
+      </c>
+      <c r="J342" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K343),"",'Bowtie v1.0 reorg'!K343)</f>
+        <v/>
+      </c>
+      <c r="K342" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L342" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <f>'Bowtie v1.0 reorg'!A344</f>
+        <v>342</v>
+      </c>
+      <c r="B343">
+        <f>'Bowtie v1.0 reorg'!E344</f>
+        <v>0</v>
+      </c>
+      <c r="C343" t="str">
+        <f>'Bowtie v1.0 reorg'!C344</f>
+        <v>EA55</v>
+      </c>
+      <c r="D343">
+        <f>'Bowtie v1.0 reorg'!D344</f>
+        <v>59989</v>
+      </c>
+      <c r="E343" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F344),"",'Bowtie v1.0 reorg'!F344)</f>
+        <v/>
+      </c>
+      <c r="F343" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G344),"",'Bowtie v1.0 reorg'!G344)</f>
+        <v/>
+      </c>
+      <c r="G343" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I344),"",'Bowtie v1.0 reorg'!I344)</f>
+        <v/>
+      </c>
+      <c r="H343" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J344),"",'Bowtie v1.0 reorg'!J344)</f>
+        <v/>
+      </c>
+      <c r="I343" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H344),"",'Bowtie v1.0 reorg'!H344)</f>
+        <v/>
+      </c>
+      <c r="J343" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K344),"",'Bowtie v1.0 reorg'!K344)</f>
+        <v/>
+      </c>
+      <c r="K343" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L343" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A344" s="15">
+        <f>'Bowtie v1.0 reorg'!A345</f>
+        <v>343</v>
+      </c>
+      <c r="B344" s="15">
+        <f>'Bowtie v1.0 reorg'!E345</f>
+        <v>0</v>
+      </c>
+      <c r="C344" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!C345</f>
+        <v>EA56</v>
+      </c>
+      <c r="D344" s="15">
+        <f>'Bowtie v1.0 reorg'!D345</f>
+        <v>59990</v>
+      </c>
+      <c r="E344" s="16" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F345),"",'Bowtie v1.0 reorg'!F345)</f>
+        <v/>
+      </c>
+      <c r="F344" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G345),"",'Bowtie v1.0 reorg'!G345)</f>
+        <v/>
+      </c>
+      <c r="G344" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I345),"",'Bowtie v1.0 reorg'!I345)</f>
+        <v/>
+      </c>
+      <c r="H344" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J345),"",'Bowtie v1.0 reorg'!J345)</f>
+        <v/>
+      </c>
+      <c r="I344" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H345),"",'Bowtie v1.0 reorg'!H345)</f>
+        <v/>
+      </c>
+      <c r="J344" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K345),"",'Bowtie v1.0 reorg'!K345)</f>
+        <v/>
+      </c>
+      <c r="K344" s="15" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L344" s="15" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M344" s="15"/>
+    </row>
+    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <f>'Bowtie v1.0 reorg'!A346</f>
+        <v>344</v>
+      </c>
+      <c r="B345">
+        <f>'Bowtie v1.0 reorg'!E346</f>
+        <v>0</v>
+      </c>
+      <c r="C345" t="str">
+        <f>'Bowtie v1.0 reorg'!C346</f>
+        <v>EA57</v>
+      </c>
+      <c r="D345">
+        <f>'Bowtie v1.0 reorg'!D346</f>
+        <v>59991</v>
+      </c>
+      <c r="E345" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F346),"",'Bowtie v1.0 reorg'!F346)</f>
+        <v/>
+      </c>
+      <c r="F345" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G346),"",'Bowtie v1.0 reorg'!G346)</f>
+        <v/>
+      </c>
+      <c r="G345" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I346),"",'Bowtie v1.0 reorg'!I346)</f>
+        <v/>
+      </c>
+      <c r="H345" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J346),"",'Bowtie v1.0 reorg'!J346)</f>
+        <v/>
+      </c>
+      <c r="I345" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H346),"",'Bowtie v1.0 reorg'!H346)</f>
+        <v/>
+      </c>
+      <c r="J345" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K346),"",'Bowtie v1.0 reorg'!K346)</f>
+        <v/>
+      </c>
+      <c r="K345" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L345" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <f>'Bowtie v1.0 reorg'!A347</f>
+        <v>345</v>
+      </c>
+      <c r="B346">
+        <f>'Bowtie v1.0 reorg'!E347</f>
+        <v>0</v>
+      </c>
+      <c r="C346" t="str">
+        <f>'Bowtie v1.0 reorg'!C347</f>
+        <v>EA58</v>
+      </c>
+      <c r="D346">
+        <f>'Bowtie v1.0 reorg'!D347</f>
+        <v>59992</v>
+      </c>
+      <c r="E346" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F347),"",'Bowtie v1.0 reorg'!F347)</f>
+        <v/>
+      </c>
+      <c r="F346" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G347),"",'Bowtie v1.0 reorg'!G347)</f>
+        <v/>
+      </c>
+      <c r="G346" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I347),"",'Bowtie v1.0 reorg'!I347)</f>
+        <v/>
+      </c>
+      <c r="H346" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J347),"",'Bowtie v1.0 reorg'!J347)</f>
+        <v/>
+      </c>
+      <c r="I346" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H347),"",'Bowtie v1.0 reorg'!H347)</f>
+        <v/>
+      </c>
+      <c r="J346" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K347),"",'Bowtie v1.0 reorg'!K347)</f>
+        <v/>
+      </c>
+      <c r="K346" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L346" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A347" s="15">
+        <f>'Bowtie v1.0 reorg'!A348</f>
+        <v>346</v>
+      </c>
+      <c r="B347" s="15">
+        <f>'Bowtie v1.0 reorg'!E348</f>
+        <v>0</v>
+      </c>
+      <c r="C347" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!C348</f>
+        <v>EA59</v>
+      </c>
+      <c r="D347" s="15">
+        <f>'Bowtie v1.0 reorg'!D348</f>
+        <v>59993</v>
+      </c>
+      <c r="E347" s="16" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F348),"",'Bowtie v1.0 reorg'!F348)</f>
+        <v/>
+      </c>
+      <c r="F347" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G348),"",'Bowtie v1.0 reorg'!G348)</f>
+        <v/>
+      </c>
+      <c r="G347" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I348),"",'Bowtie v1.0 reorg'!I348)</f>
+        <v/>
+      </c>
+      <c r="H347" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J348),"",'Bowtie v1.0 reorg'!J348)</f>
+        <v/>
+      </c>
+      <c r="I347" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H348),"",'Bowtie v1.0 reorg'!H348)</f>
+        <v/>
+      </c>
+      <c r="J347" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K348),"",'Bowtie v1.0 reorg'!K348)</f>
+        <v/>
+      </c>
+      <c r="K347" s="15" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L347" s="15" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M347" s="15"/>
+    </row>
+    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <f>'Bowtie v1.0 reorg'!A349</f>
+        <v>347</v>
+      </c>
+      <c r="B348">
+        <f>'Bowtie v1.0 reorg'!E349</f>
+        <v>0</v>
+      </c>
+      <c r="C348" t="str">
+        <f>'Bowtie v1.0 reorg'!C349</f>
+        <v>EA5A</v>
+      </c>
+      <c r="D348">
+        <f>'Bowtie v1.0 reorg'!D349</f>
+        <v>59994</v>
+      </c>
+      <c r="E348" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F349),"",'Bowtie v1.0 reorg'!F349)</f>
+        <v/>
+      </c>
+      <c r="F348" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G349),"",'Bowtie v1.0 reorg'!G349)</f>
+        <v/>
+      </c>
+      <c r="G348" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I349),"",'Bowtie v1.0 reorg'!I349)</f>
+        <v/>
+      </c>
+      <c r="H348" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J349),"",'Bowtie v1.0 reorg'!J349)</f>
+        <v/>
+      </c>
+      <c r="I348" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H349),"",'Bowtie v1.0 reorg'!H349)</f>
+        <v/>
+      </c>
+      <c r="J348" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K349),"",'Bowtie v1.0 reorg'!K349)</f>
+        <v/>
+      </c>
+      <c r="K348" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L348" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <f>'Bowtie v1.0 reorg'!A350</f>
+        <v>348</v>
+      </c>
+      <c r="B349">
+        <f>'Bowtie v1.0 reorg'!E350</f>
+        <v>0</v>
+      </c>
+      <c r="C349" t="str">
+        <f>'Bowtie v1.0 reorg'!C350</f>
+        <v>EA5B</v>
+      </c>
+      <c r="D349">
+        <f>'Bowtie v1.0 reorg'!D350</f>
+        <v>59995</v>
+      </c>
+      <c r="E349" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F350),"",'Bowtie v1.0 reorg'!F350)</f>
+        <v/>
+      </c>
+      <c r="F349" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G350),"",'Bowtie v1.0 reorg'!G350)</f>
+        <v/>
+      </c>
+      <c r="G349" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I350),"",'Bowtie v1.0 reorg'!I350)</f>
+        <v/>
+      </c>
+      <c r="H349" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J350),"",'Bowtie v1.0 reorg'!J350)</f>
+        <v/>
+      </c>
+      <c r="I349" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H350),"",'Bowtie v1.0 reorg'!H350)</f>
+        <v/>
+      </c>
+      <c r="J349" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K350),"",'Bowtie v1.0 reorg'!K350)</f>
+        <v/>
+      </c>
+      <c r="K349" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L349" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A350" s="15">
+        <f>'Bowtie v1.0 reorg'!A351</f>
+        <v>349</v>
+      </c>
+      <c r="B350" s="15">
+        <f>'Bowtie v1.0 reorg'!E351</f>
+        <v>0</v>
+      </c>
+      <c r="C350" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!C351</f>
+        <v>EA5C</v>
+      </c>
+      <c r="D350" s="15">
+        <f>'Bowtie v1.0 reorg'!D351</f>
+        <v>59996</v>
+      </c>
+      <c r="E350" s="16" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F351),"",'Bowtie v1.0 reorg'!F351)</f>
+        <v/>
+      </c>
+      <c r="F350" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G351),"",'Bowtie v1.0 reorg'!G351)</f>
+        <v/>
+      </c>
+      <c r="G350" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I351),"",'Bowtie v1.0 reorg'!I351)</f>
+        <v/>
+      </c>
+      <c r="H350" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J351),"",'Bowtie v1.0 reorg'!J351)</f>
+        <v/>
+      </c>
+      <c r="I350" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H351),"",'Bowtie v1.0 reorg'!H351)</f>
+        <v/>
+      </c>
+      <c r="J350" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K351),"",'Bowtie v1.0 reorg'!K351)</f>
+        <v/>
+      </c>
+      <c r="K350" s="15" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L350" s="15" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M350" s="15"/>
+    </row>
+    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <f>'Bowtie v1.0 reorg'!A352</f>
+        <v>350</v>
+      </c>
+      <c r="B351">
+        <f>'Bowtie v1.0 reorg'!E352</f>
+        <v>0</v>
+      </c>
+      <c r="C351" t="str">
+        <f>'Bowtie v1.0 reorg'!C352</f>
+        <v>EA5D</v>
+      </c>
+      <c r="D351">
+        <f>'Bowtie v1.0 reorg'!D352</f>
+        <v>59997</v>
+      </c>
+      <c r="E351" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F352),"",'Bowtie v1.0 reorg'!F352)</f>
+        <v/>
+      </c>
+      <c r="F351" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G352),"",'Bowtie v1.0 reorg'!G352)</f>
+        <v/>
+      </c>
+      <c r="G351" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I352),"",'Bowtie v1.0 reorg'!I352)</f>
+        <v/>
+      </c>
+      <c r="H351" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J352),"",'Bowtie v1.0 reorg'!J352)</f>
+        <v/>
+      </c>
+      <c r="I351" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H352),"",'Bowtie v1.0 reorg'!H352)</f>
+        <v/>
+      </c>
+      <c r="J351" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K352),"",'Bowtie v1.0 reorg'!K352)</f>
+        <v/>
+      </c>
+      <c r="K351" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L351" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <f>'Bowtie v1.0 reorg'!A353</f>
+        <v>351</v>
+      </c>
+      <c r="B352">
+        <f>'Bowtie v1.0 reorg'!E353</f>
+        <v>0</v>
+      </c>
+      <c r="C352" t="str">
+        <f>'Bowtie v1.0 reorg'!C353</f>
+        <v>EA5E</v>
+      </c>
+      <c r="D352">
+        <f>'Bowtie v1.0 reorg'!D353</f>
+        <v>59998</v>
+      </c>
+      <c r="E352" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F353),"",'Bowtie v1.0 reorg'!F353)</f>
+        <v/>
+      </c>
+      <c r="F352" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G353),"",'Bowtie v1.0 reorg'!G353)</f>
+        <v/>
+      </c>
+      <c r="G352" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I353),"",'Bowtie v1.0 reorg'!I353)</f>
+        <v/>
+      </c>
+      <c r="H352" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J353),"",'Bowtie v1.0 reorg'!J353)</f>
+        <v/>
+      </c>
+      <c r="I352" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H353),"",'Bowtie v1.0 reorg'!H353)</f>
+        <v/>
+      </c>
+      <c r="J352" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K353),"",'Bowtie v1.0 reorg'!K353)</f>
+        <v/>
+      </c>
+      <c r="K352" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L352" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A353" s="15">
+        <f>'Bowtie v1.0 reorg'!A354</f>
+        <v>352</v>
+      </c>
+      <c r="B353" s="15">
+        <f>'Bowtie v1.0 reorg'!E354</f>
+        <v>0</v>
+      </c>
+      <c r="C353" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!C354</f>
+        <v>EA5F</v>
+      </c>
+      <c r="D353" s="15">
+        <f>'Bowtie v1.0 reorg'!D354</f>
+        <v>59999</v>
+      </c>
+      <c r="E353" s="16" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F354),"",'Bowtie v1.0 reorg'!F354)</f>
+        <v/>
+      </c>
+      <c r="F353" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G354),"",'Bowtie v1.0 reorg'!G354)</f>
+        <v/>
+      </c>
+      <c r="G353" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I354),"",'Bowtie v1.0 reorg'!I354)</f>
+        <v/>
+      </c>
+      <c r="H353" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J354),"",'Bowtie v1.0 reorg'!J354)</f>
+        <v/>
+      </c>
+      <c r="I353" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H354),"",'Bowtie v1.0 reorg'!H354)</f>
+        <v/>
+      </c>
+      <c r="J353" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K354),"",'Bowtie v1.0 reorg'!K354)</f>
+        <v/>
+      </c>
+      <c r="K353" s="15" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L353" s="15" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M353" s="15"/>
+    </row>
+    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <f>'Bowtie v1.0 reorg'!A355</f>
+        <v>353</v>
+      </c>
+      <c r="B354">
+        <f>'Bowtie v1.0 reorg'!E355</f>
+        <v>0</v>
+      </c>
+      <c r="C354" t="str">
+        <f>'Bowtie v1.0 reorg'!C355</f>
+        <v>EA60</v>
+      </c>
+      <c r="D354">
+        <f>'Bowtie v1.0 reorg'!D355</f>
+        <v>60000</v>
+      </c>
+      <c r="E354" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F355),"",'Bowtie v1.0 reorg'!F355)</f>
+        <v/>
+      </c>
+      <c r="F354" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G355),"",'Bowtie v1.0 reorg'!G355)</f>
+        <v/>
+      </c>
+      <c r="G354" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I355),"",'Bowtie v1.0 reorg'!I355)</f>
+        <v/>
+      </c>
+      <c r="H354" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J355),"",'Bowtie v1.0 reorg'!J355)</f>
+        <v/>
+      </c>
+      <c r="I354" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H355),"",'Bowtie v1.0 reorg'!H355)</f>
+        <v/>
+      </c>
+      <c r="J354" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K355),"",'Bowtie v1.0 reorg'!K355)</f>
+        <v/>
+      </c>
+      <c r="K354" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L354" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <f>'Bowtie v1.0 reorg'!A356</f>
+        <v>354</v>
+      </c>
+      <c r="B355">
+        <f>'Bowtie v1.0 reorg'!E356</f>
+        <v>0</v>
+      </c>
+      <c r="C355" t="str">
+        <f>'Bowtie v1.0 reorg'!C356</f>
+        <v>EA61</v>
+      </c>
+      <c r="D355">
+        <f>'Bowtie v1.0 reorg'!D356</f>
+        <v>60001</v>
+      </c>
+      <c r="E355" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F356),"",'Bowtie v1.0 reorg'!F356)</f>
+        <v/>
+      </c>
+      <c r="F355" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G356),"",'Bowtie v1.0 reorg'!G356)</f>
+        <v/>
+      </c>
+      <c r="G355" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I356),"",'Bowtie v1.0 reorg'!I356)</f>
+        <v/>
+      </c>
+      <c r="H355" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J356),"",'Bowtie v1.0 reorg'!J356)</f>
+        <v/>
+      </c>
+      <c r="I355" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H356),"",'Bowtie v1.0 reorg'!H356)</f>
+        <v/>
+      </c>
+      <c r="J355" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K356),"",'Bowtie v1.0 reorg'!K356)</f>
+        <v/>
+      </c>
+      <c r="K355" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L355" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A356" s="15">
+        <f>'Bowtie v1.0 reorg'!A357</f>
+        <v>355</v>
+      </c>
+      <c r="B356" s="15">
+        <f>'Bowtie v1.0 reorg'!E357</f>
+        <v>0</v>
+      </c>
+      <c r="C356" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!C357</f>
+        <v>EA62</v>
+      </c>
+      <c r="D356" s="15">
+        <f>'Bowtie v1.0 reorg'!D357</f>
+        <v>60002</v>
+      </c>
+      <c r="E356" s="16" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F357),"",'Bowtie v1.0 reorg'!F357)</f>
+        <v/>
+      </c>
+      <c r="F356" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G357),"",'Bowtie v1.0 reorg'!G357)</f>
+        <v/>
+      </c>
+      <c r="G356" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I357),"",'Bowtie v1.0 reorg'!I357)</f>
+        <v/>
+      </c>
+      <c r="H356" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J357),"",'Bowtie v1.0 reorg'!J357)</f>
+        <v/>
+      </c>
+      <c r="I356" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H357),"",'Bowtie v1.0 reorg'!H357)</f>
+        <v/>
+      </c>
+      <c r="J356" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K357),"",'Bowtie v1.0 reorg'!K357)</f>
+        <v/>
+      </c>
+      <c r="K356" s="15" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L356" s="15" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M356" s="15"/>
+    </row>
+    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <f>'Bowtie v1.0 reorg'!A358</f>
+        <v>356</v>
+      </c>
+      <c r="B357">
+        <f>'Bowtie v1.0 reorg'!E358</f>
+        <v>0</v>
+      </c>
+      <c r="C357" t="str">
+        <f>'Bowtie v1.0 reorg'!C358</f>
+        <v>EA63</v>
+      </c>
+      <c r="D357">
+        <f>'Bowtie v1.0 reorg'!D358</f>
+        <v>60003</v>
+      </c>
+      <c r="E357" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F358),"",'Bowtie v1.0 reorg'!F358)</f>
+        <v/>
+      </c>
+      <c r="F357" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G358),"",'Bowtie v1.0 reorg'!G358)</f>
+        <v/>
+      </c>
+      <c r="G357" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I358),"",'Bowtie v1.0 reorg'!I358)</f>
+        <v/>
+      </c>
+      <c r="H357" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J358),"",'Bowtie v1.0 reorg'!J358)</f>
+        <v/>
+      </c>
+      <c r="I357" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H358),"",'Bowtie v1.0 reorg'!H358)</f>
+        <v/>
+      </c>
+      <c r="J357" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K358),"",'Bowtie v1.0 reorg'!K358)</f>
+        <v/>
+      </c>
+      <c r="K357" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L357" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <f>'Bowtie v1.0 reorg'!A359</f>
+        <v>357</v>
+      </c>
+      <c r="B358">
+        <f>'Bowtie v1.0 reorg'!E359</f>
+        <v>0</v>
+      </c>
+      <c r="C358" t="str">
+        <f>'Bowtie v1.0 reorg'!C359</f>
+        <v>EA64</v>
+      </c>
+      <c r="D358">
+        <f>'Bowtie v1.0 reorg'!D359</f>
+        <v>60004</v>
+      </c>
+      <c r="E358" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F359),"",'Bowtie v1.0 reorg'!F359)</f>
+        <v/>
+      </c>
+      <c r="F358" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G359),"",'Bowtie v1.0 reorg'!G359)</f>
+        <v/>
+      </c>
+      <c r="G358" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I359),"",'Bowtie v1.0 reorg'!I359)</f>
+        <v/>
+      </c>
+      <c r="H358" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J359),"",'Bowtie v1.0 reorg'!J359)</f>
+        <v/>
+      </c>
+      <c r="I358" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H359),"",'Bowtie v1.0 reorg'!H359)</f>
+        <v/>
+      </c>
+      <c r="J358" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K359),"",'Bowtie v1.0 reorg'!K359)</f>
+        <v/>
+      </c>
+      <c r="K358" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L358" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A359" s="15">
+        <f>'Bowtie v1.0 reorg'!A360</f>
+        <v>358</v>
+      </c>
+      <c r="B359" s="15">
+        <f>'Bowtie v1.0 reorg'!E360</f>
+        <v>0</v>
+      </c>
+      <c r="C359" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!C360</f>
+        <v>EA65</v>
+      </c>
+      <c r="D359" s="15">
+        <f>'Bowtie v1.0 reorg'!D360</f>
+        <v>60005</v>
+      </c>
+      <c r="E359" s="16" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F360),"",'Bowtie v1.0 reorg'!F360)</f>
+        <v/>
+      </c>
+      <c r="F359" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G360),"",'Bowtie v1.0 reorg'!G360)</f>
+        <v/>
+      </c>
+      <c r="G359" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I360),"",'Bowtie v1.0 reorg'!I360)</f>
+        <v/>
+      </c>
+      <c r="H359" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J360),"",'Bowtie v1.0 reorg'!J360)</f>
+        <v/>
+      </c>
+      <c r="I359" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H360),"",'Bowtie v1.0 reorg'!H360)</f>
+        <v/>
+      </c>
+      <c r="J359" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K360),"",'Bowtie v1.0 reorg'!K360)</f>
+        <v/>
+      </c>
+      <c r="K359" s="15" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L359" s="15" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M359" s="15"/>
+    </row>
+    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <f>'Bowtie v1.0 reorg'!A361</f>
+        <v>359</v>
+      </c>
+      <c r="B360">
+        <f>'Bowtie v1.0 reorg'!E361</f>
+        <v>0</v>
+      </c>
+      <c r="C360" t="str">
+        <f>'Bowtie v1.0 reorg'!C361</f>
+        <v>EA66</v>
+      </c>
+      <c r="D360">
+        <f>'Bowtie v1.0 reorg'!D361</f>
+        <v>60006</v>
+      </c>
+      <c r="E360" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F361),"",'Bowtie v1.0 reorg'!F361)</f>
+        <v/>
+      </c>
+      <c r="F360" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G361),"",'Bowtie v1.0 reorg'!G361)</f>
+        <v/>
+      </c>
+      <c r="G360" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I361),"",'Bowtie v1.0 reorg'!I361)</f>
+        <v/>
+      </c>
+      <c r="H360" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J361),"",'Bowtie v1.0 reorg'!J361)</f>
+        <v/>
+      </c>
+      <c r="I360" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H361),"",'Bowtie v1.0 reorg'!H361)</f>
+        <v/>
+      </c>
+      <c r="J360" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K361),"",'Bowtie v1.0 reorg'!K361)</f>
+        <v/>
+      </c>
+      <c r="K360" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L360" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <f>'Bowtie v1.0 reorg'!A362</f>
+        <v>360</v>
+      </c>
+      <c r="B361">
+        <f>'Bowtie v1.0 reorg'!E362</f>
+        <v>0</v>
+      </c>
+      <c r="C361" t="str">
+        <f>'Bowtie v1.0 reorg'!C362</f>
+        <v>EA67</v>
+      </c>
+      <c r="D361">
+        <f>'Bowtie v1.0 reorg'!D362</f>
+        <v>60007</v>
+      </c>
+      <c r="E361" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F362),"",'Bowtie v1.0 reorg'!F362)</f>
+        <v/>
+      </c>
+      <c r="F361" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G362),"",'Bowtie v1.0 reorg'!G362)</f>
+        <v/>
+      </c>
+      <c r="G361" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I362),"",'Bowtie v1.0 reorg'!I362)</f>
+        <v/>
+      </c>
+      <c r="H361" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J362),"",'Bowtie v1.0 reorg'!J362)</f>
+        <v/>
+      </c>
+      <c r="I361" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H362),"",'Bowtie v1.0 reorg'!H362)</f>
+        <v/>
+      </c>
+      <c r="J361" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K362),"",'Bowtie v1.0 reorg'!K362)</f>
+        <v/>
+      </c>
+      <c r="K361" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L361" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A362" s="15">
+        <f>'Bowtie v1.0 reorg'!A363</f>
+        <v>361</v>
+      </c>
+      <c r="B362" s="15">
+        <f>'Bowtie v1.0 reorg'!E363</f>
+        <v>0</v>
+      </c>
+      <c r="C362" s="15" t="str">
+        <f>'Bowtie v1.0 reorg'!C363</f>
+        <v>EA68</v>
+      </c>
+      <c r="D362" s="15">
+        <f>'Bowtie v1.0 reorg'!D363</f>
+        <v>60008</v>
+      </c>
+      <c r="E362" s="16" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!F363),"",'Bowtie v1.0 reorg'!F363)</f>
+        <v/>
+      </c>
+      <c r="F362" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G363),"",'Bowtie v1.0 reorg'!G363)</f>
+        <v/>
+      </c>
+      <c r="G362" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!I363),"",'Bowtie v1.0 reorg'!I363)</f>
+        <v/>
+      </c>
+      <c r="H362" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!J363),"",'Bowtie v1.0 reorg'!J363)</f>
+        <v/>
+      </c>
+      <c r="I362" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!H363),"",'Bowtie v1.0 reorg'!H363)</f>
+        <v/>
+      </c>
+      <c r="J362" s="15" t="str">
+        <f>IF(ISBLANK('Bowtie v1.0 reorg'!K363),"",'Bowtie v1.0 reorg'!K363)</f>
+        <v/>
+      </c>
+      <c r="K362" s="15" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L362" s="15" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M362" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
moved some draft icons to final
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="607">
   <si>
     <t>name</t>
   </si>
@@ -1802,6 +1802,45 @@
   </si>
   <si>
     <t>Add bowtie-ani-spin-pulse class for animation.</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>parameter variable argument @ at</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Used in Test hub for adding test step parameters.</t>
+  </si>
+  <si>
+    <t>step-insert</t>
+  </si>
+  <si>
+    <t>step-shared-add</t>
+  </si>
+  <si>
+    <t>step-shared-insert</t>
+  </si>
+  <si>
+    <t>step shared reuse multiple add plus stairs</t>
+  </si>
+  <si>
+    <t>step insert stairs arrow right</t>
+  </si>
+  <si>
+    <t>step shared reuse multiple arrow right stairs</t>
+  </si>
+  <si>
+    <t>Used in Test hub for adding test step.</t>
+  </si>
+  <si>
+    <t>Used in Test hub for creating a new test step as shared step.</t>
+  </si>
+  <si>
+    <t>Used in Test hub for inserting existing shared steps.</t>
   </si>
 </sst>
 </file>
@@ -1887,7 +1926,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1934,6 +1973,7 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -14792,6 +14832,158 @@
         <a:xfrm>
           <a:off x="1095375" y="136207500"/>
           <a:ext cx="257211" cy="190527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>340</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381031</xdr:colOff>
+      <xdr:row>340</xdr:row>
+      <xdr:rowOff>304828</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="340" name="Picture 339"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId339"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="136607550"/>
+          <a:ext cx="219106" cy="200053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>341</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>371503</xdr:colOff>
+      <xdr:row>341</xdr:row>
+      <xdr:rowOff>314356</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="341" name="Picture 340"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId340"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="136998075"/>
+          <a:ext cx="200053" cy="219106"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>342</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390552</xdr:colOff>
+      <xdr:row>342</xdr:row>
+      <xdr:rowOff>314356</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="342" name="Picture 341"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId341"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="137398125"/>
+          <a:ext cx="190527" cy="219106"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>343</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400081</xdr:colOff>
+      <xdr:row>343</xdr:row>
+      <xdr:rowOff>333406</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="343" name="Picture 342"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId342"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1123950" y="137817225"/>
+          <a:ext cx="219106" cy="219106"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15068,9 +15260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL410"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A336" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K340" sqref="K340"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A342" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C343" sqref="C343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26625,9 +26817,30 @@
       <c r="D341" s="13">
         <v>59986</v>
       </c>
+      <c r="E341" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="F341" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G341" t="s">
+        <v>17</v>
+      </c>
+      <c r="H341" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="I341" t="s">
+        <v>15</v>
+      </c>
+      <c r="J341" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="K341" s="2" t="s">
+        <v>597</v>
+      </c>
       <c r="L341" t="str">
         <f t="shared" si="11"/>
-        <v>uEA52-.svg</v>
+        <v>uEA52-parameter.svg</v>
       </c>
     </row>
     <row r="342" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -26641,9 +26854,30 @@
       <c r="D342" s="13">
         <v>59987</v>
       </c>
+      <c r="E342" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="F342">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G342" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H342" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="I342" t="s">
+        <v>15</v>
+      </c>
+      <c r="J342" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="K342" s="2" t="s">
+        <v>604</v>
+      </c>
       <c r="L342" t="str">
         <f t="shared" si="11"/>
-        <v>uEA53-.svg</v>
+        <v>uEA53-step-insert.svg</v>
       </c>
     </row>
     <row r="343" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -26657,9 +26891,30 @@
       <c r="D343" s="13">
         <v>59988</v>
       </c>
+      <c r="E343" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="F343" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G343" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H343" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="I343" t="s">
+        <v>15</v>
+      </c>
+      <c r="J343" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="K343" s="2" t="s">
+        <v>605</v>
+      </c>
       <c r="L343" t="str">
         <f t="shared" si="11"/>
-        <v>uEA54-.svg</v>
+        <v>uEA54-step-shared-add.svg</v>
       </c>
     </row>
     <row r="344" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -26673,9 +26928,30 @@
       <c r="D344" s="13">
         <v>59989</v>
       </c>
+      <c r="E344" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="F344">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G344" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H344" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="I344" t="s">
+        <v>15</v>
+      </c>
+      <c r="J344" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="K344" s="2" t="s">
+        <v>606</v>
+      </c>
       <c r="L344" t="str">
         <f t="shared" si="11"/>
-        <v>uEA55-.svg</v>
+        <v>uEA55-step-shared-insert.svg</v>
       </c>
     </row>
     <row r="345" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -27417,8 +27693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" workbookViewId="0">
-      <selection activeCell="E341" sqref="E341"/>
+    <sheetView topLeftCell="A332" workbookViewId="0">
+      <selection activeCell="L340" sqref="L340:L343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44264,7 +44540,7 @@
         <v>{"id":336,"name":"link-remove","unicode":"EA4F","decimal":59983,"version":"1.1","style":"light","subset":"VSTS","group":"editor","keywords":["link","hyperlink","url","remove"],"usage":"Used for removing hyperlink."}</v>
       </c>
     </row>
-    <row r="338" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A338">
         <f>'Bowtie v1.0 reorg'!A339</f>
         <v>337</v>
@@ -44281,7 +44557,7 @@
         <f>'Bowtie v1.0 reorg'!D339</f>
         <v>59984</v>
       </c>
-      <c r="E338" s="14">
+      <c r="E338">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F339),"",'Bowtie v1.0 reorg'!F339)</f>
         <v>1.1000000000000001</v>
       </c>
@@ -44331,7 +44607,7 @@
         <f>'Bowtie v1.0 reorg'!D340</f>
         <v>59985</v>
       </c>
-      <c r="E339" s="14">
+      <c r="E339">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F340),"",'Bowtie v1.0 reorg'!F340)</f>
         <v>1.1000000000000001</v>
       </c>
@@ -44364,205 +44640,204 @@
         <v>{"id":338,"name":"personalize","unicode":"EA51","decimal":59985,"version":"1.1","style":"light","subset":"VSTS","group":"work","keywords":["personalize","customize","design","edit","draw","pen","brush"],"usage":"Used for customizing work item form."}</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A340">
+    <row r="340" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="15">
         <f>'Bowtie v1.0 reorg'!A341</f>
         <v>339</v>
       </c>
-      <c r="B340">
+      <c r="B340" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E341</f>
-        <v>0</v>
-      </c>
-      <c r="C340" t="str">
+        <v>parameter</v>
+      </c>
+      <c r="C340" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C341</f>
         <v>EA52</v>
       </c>
-      <c r="D340">
+      <c r="D340" s="15">
         <f>'Bowtie v1.0 reorg'!D341</f>
         <v>59986</v>
       </c>
-      <c r="E340" s="14" t="str">
+      <c r="E340" s="18">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F341),"",'Bowtie v1.0 reorg'!F341)</f>
-        <v/>
-      </c>
-      <c r="F340" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F340" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G341),"",'Bowtie v1.0 reorg'!G341)</f>
-        <v/>
-      </c>
-      <c r="G340" t="str">
+        <v>light</v>
+      </c>
+      <c r="G340" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I341),"",'Bowtie v1.0 reorg'!I341)</f>
-        <v/>
-      </c>
-      <c r="H340" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H340" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J341),"",'Bowtie v1.0 reorg'!J341)</f>
-        <v/>
-      </c>
-      <c r="I340" t="str">
+        <v>Test</v>
+      </c>
+      <c r="I340" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H341),"",'Bowtie v1.0 reorg'!H341)</f>
-        <v/>
-      </c>
-      <c r="J340" t="str">
+        <v>parameter variable argument @ at</v>
+      </c>
+      <c r="J340" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K341),"",'Bowtie v1.0 reorg'!K341)</f>
-        <v/>
-      </c>
-      <c r="K340" t="e">
+        <v>Used in Test hub for adding test step parameters.</v>
+      </c>
+      <c r="K340" s="15" t="str">
         <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L340" t="e">
+        <v>{'id':339,'name':'parameter','unicode':'EA52','decimal':59986,'version':'1.1','style':'light','subset':'VSTS','group':'Test','keywords':['parameter','variable','argument','@','at'],'usage':'Used in Test hub for adding test step parameters.'}</v>
+      </c>
+      <c r="L340" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A341">
+        <v>{"id":339,"name":"parameter","unicode":"EA52","decimal":59986,"version":"1.1","style":"light","subset":"VSTS","group":"Test","keywords":["parameter","variable","argument","@","at"],"usage":"Used in Test hub for adding test step parameters."}</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="15">
         <f>'Bowtie v1.0 reorg'!A342</f>
         <v>340</v>
       </c>
-      <c r="B341">
+      <c r="B341" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E342</f>
-        <v>0</v>
-      </c>
-      <c r="C341" t="str">
+        <v>step-insert</v>
+      </c>
+      <c r="C341" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C342</f>
         <v>EA53</v>
       </c>
-      <c r="D341">
+      <c r="D341" s="15">
         <f>'Bowtie v1.0 reorg'!D342</f>
         <v>59987</v>
       </c>
-      <c r="E341" s="14" t="str">
+      <c r="E341" s="18">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F342),"",'Bowtie v1.0 reorg'!F342)</f>
-        <v/>
-      </c>
-      <c r="F341" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F341" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G342),"",'Bowtie v1.0 reorg'!G342)</f>
-        <v/>
-      </c>
-      <c r="G341" t="str">
+        <v>bold</v>
+      </c>
+      <c r="G341" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I342),"",'Bowtie v1.0 reorg'!I342)</f>
-        <v/>
-      </c>
-      <c r="H341" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H341" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J342),"",'Bowtie v1.0 reorg'!J342)</f>
-        <v/>
-      </c>
-      <c r="I341" t="str">
+        <v>Test</v>
+      </c>
+      <c r="I341" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H342),"",'Bowtie v1.0 reorg'!H342)</f>
-        <v/>
-      </c>
-      <c r="J341" t="str">
+        <v>step insert stairs arrow right</v>
+      </c>
+      <c r="J341" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K342),"",'Bowtie v1.0 reorg'!K342)</f>
-        <v/>
-      </c>
-      <c r="K341" t="e">
+        <v>Used in Test hub for adding test step.</v>
+      </c>
+      <c r="K341" s="15" t="str">
         <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L341" t="e">
+        <v>{'id':340,'name':'step-insert','unicode':'EA53','decimal':59987,'version':'1.1','style':'bold','subset':'VSTS','group':'Test','keywords':['step','insert','stairs','arrow','right'],'usage':'Used in Test hub for adding test step.'}</v>
+      </c>
+      <c r="L341" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M341" s="15"/>
-    </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A342">
+        <v>{"id":340,"name":"step-insert","unicode":"EA53","decimal":59987,"version":"1.1","style":"bold","subset":"VSTS","group":"Test","keywords":["step","insert","stairs","arrow","right"],"usage":"Used in Test hub for adding test step."}</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="15">
         <f>'Bowtie v1.0 reorg'!A343</f>
         <v>341</v>
       </c>
-      <c r="B342">
+      <c r="B342" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E343</f>
-        <v>0</v>
-      </c>
-      <c r="C342" t="str">
+        <v>step-shared-add</v>
+      </c>
+      <c r="C342" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C343</f>
         <v>EA54</v>
       </c>
-      <c r="D342">
+      <c r="D342" s="15">
         <f>'Bowtie v1.0 reorg'!D343</f>
         <v>59988</v>
       </c>
-      <c r="E342" s="14" t="str">
+      <c r="E342" s="18">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F343),"",'Bowtie v1.0 reorg'!F343)</f>
-        <v/>
-      </c>
-      <c r="F342" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F342" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G343),"",'Bowtie v1.0 reorg'!G343)</f>
-        <v/>
-      </c>
-      <c r="G342" t="str">
+        <v>bold</v>
+      </c>
+      <c r="G342" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I343),"",'Bowtie v1.0 reorg'!I343)</f>
-        <v/>
-      </c>
-      <c r="H342" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H342" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J343),"",'Bowtie v1.0 reorg'!J343)</f>
-        <v/>
-      </c>
-      <c r="I342" t="str">
+        <v>Test</v>
+      </c>
+      <c r="I342" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H343),"",'Bowtie v1.0 reorg'!H343)</f>
-        <v/>
-      </c>
-      <c r="J342" t="str">
+        <v>step shared reuse multiple add plus stairs</v>
+      </c>
+      <c r="J342" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K343),"",'Bowtie v1.0 reorg'!K343)</f>
-        <v/>
-      </c>
-      <c r="K342" t="e">
+        <v>Used in Test hub for creating a new test step as shared step.</v>
+      </c>
+      <c r="K342" s="15" t="str">
         <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L342" t="e">
+        <v>{'id':341,'name':'step-shared-add','unicode':'EA54','decimal':59988,'version':'1.1','style':'bold','subset':'VSTS','group':'Test','keywords':['step','shared','reuse','multiple','add','plus','stairs'],'usage':'Used in Test hub for creating a new test step as shared step.'}</v>
+      </c>
+      <c r="L342" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A343">
+        <v>{"id":341,"name":"step-shared-add","unicode":"EA54","decimal":59988,"version":"1.1","style":"bold","subset":"VSTS","group":"Test","keywords":["step","shared","reuse","multiple","add","plus","stairs"],"usage":"Used in Test hub for creating a new test step as shared step."}</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="15">
         <f>'Bowtie v1.0 reorg'!A344</f>
         <v>342</v>
       </c>
-      <c r="B343">
+      <c r="B343" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E344</f>
-        <v>0</v>
-      </c>
-      <c r="C343" t="str">
+        <v>step-shared-insert</v>
+      </c>
+      <c r="C343" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C344</f>
         <v>EA55</v>
       </c>
-      <c r="D343">
+      <c r="D343" s="15">
         <f>'Bowtie v1.0 reorg'!D344</f>
         <v>59989</v>
       </c>
-      <c r="E343" s="14" t="str">
+      <c r="E343" s="18">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F344),"",'Bowtie v1.0 reorg'!F344)</f>
-        <v/>
-      </c>
-      <c r="F343" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F343" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G344),"",'Bowtie v1.0 reorg'!G344)</f>
-        <v/>
-      </c>
-      <c r="G343" t="str">
+        <v>bold</v>
+      </c>
+      <c r="G343" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I344),"",'Bowtie v1.0 reorg'!I344)</f>
-        <v/>
-      </c>
-      <c r="H343" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H343" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J344),"",'Bowtie v1.0 reorg'!J344)</f>
-        <v/>
-      </c>
-      <c r="I343" t="str">
+        <v>Test</v>
+      </c>
+      <c r="I343" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H344),"",'Bowtie v1.0 reorg'!H344)</f>
-        <v/>
-      </c>
-      <c r="J343" t="str">
+        <v>step shared reuse multiple arrow right stairs</v>
+      </c>
+      <c r="J343" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K344),"",'Bowtie v1.0 reorg'!K344)</f>
-        <v/>
-      </c>
-      <c r="K343" t="e">
+        <v>Used in Test hub for inserting existing shared steps.</v>
+      </c>
+      <c r="K343" s="15" t="str">
         <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L343" t="e">
+        <v>{'id':342,'name':'step-shared-insert','unicode':'EA55','decimal':59989,'version':'1.1','style':'bold','subset':'VSTS','group':'Test','keywords':['step','shared','reuse','multiple','arrow','right','stairs'],'usage':'Used in Test hub for inserting existing shared steps.'}</v>
+      </c>
+      <c r="L343" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+        <v>{"id":342,"name":"step-shared-insert","unicode":"EA55","decimal":59989,"version":"1.1","style":"bold","subset":"VSTS","group":"Test","keywords":["step","shared","reuse","multiple","arrow","right","stairs"],"usage":"Used in Test hub for inserting existing shared steps."}</v>
       </c>
     </row>
     <row r="344" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added locale icons for user profile page
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="646">
   <si>
     <t>name</t>
   </si>
@@ -1928,6 +1928,36 @@
   </si>
   <si>
     <t>column-option</t>
+  </si>
+  <si>
+    <t>globe</t>
+  </si>
+  <si>
+    <t>locale-timezone</t>
+  </si>
+  <si>
+    <t>locale-language</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>web globe country region world</t>
+  </si>
+  <si>
+    <t>web globe country region world locale language letter character</t>
+  </si>
+  <si>
+    <t>web globe country region world timezone time clock</t>
+  </si>
+  <si>
+    <t>Used for web or website. Also used for region or country on user profile page.</t>
+  </si>
+  <si>
+    <t>Used for language preference on user profile page.</t>
+  </si>
+  <si>
+    <t>Used for timezone preference on user profile page.</t>
   </si>
 </sst>
 </file>
@@ -2013,7 +2043,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2060,7 +2090,6 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -15185,6 +15214,120 @@
         <a:xfrm>
           <a:off x="1123950" y="139045950"/>
           <a:ext cx="200053" cy="190527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>347</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419135</xdr:colOff>
+      <xdr:row>347</xdr:row>
+      <xdr:rowOff>333408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="347" name="Picture 346"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId346"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="139398375"/>
+          <a:ext cx="247685" cy="238158"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>348</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>447710</xdr:colOff>
+      <xdr:row>348</xdr:row>
+      <xdr:rowOff>333407</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="348" name="Picture 347"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId347"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="139807950"/>
+          <a:ext cx="247685" cy="228632"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>349</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438187</xdr:colOff>
+      <xdr:row>349</xdr:row>
+      <xdr:rowOff>361989</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="349" name="Picture 348"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId348"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="140188950"/>
+          <a:ext cx="266737" cy="276264"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15462,8 +15605,8 @@
   <dimension ref="A1:AL410"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A342" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F345" sqref="F345"/>
+      <pane ySplit="2" topLeftCell="A345" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C350" sqref="C350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -27340,9 +27483,30 @@
       <c r="D348" s="13">
         <v>59993</v>
       </c>
+      <c r="E348" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="F348" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G348" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H348" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="I348" t="s">
+        <v>15</v>
+      </c>
+      <c r="J348" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="K348" s="2" t="s">
+        <v>643</v>
+      </c>
       <c r="L348" t="str">
         <f t="shared" si="11"/>
-        <v>uEA59-.svg</v>
+        <v>uEA59-globe.svg</v>
       </c>
     </row>
     <row r="349" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -27356,9 +27520,30 @@
       <c r="D349" s="13">
         <v>59994</v>
       </c>
+      <c r="E349" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="F349" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G349" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H349" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="I349" t="s">
+        <v>15</v>
+      </c>
+      <c r="J349" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K349" s="2" t="s">
+        <v>644</v>
+      </c>
       <c r="L349" t="str">
         <f t="shared" si="11"/>
-        <v>uEA5A-.svg</v>
+        <v>uEA5A-locale-language.svg</v>
       </c>
     </row>
     <row r="350" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -27372,9 +27557,30 @@
       <c r="D350" s="13">
         <v>59995</v>
       </c>
+      <c r="E350" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="F350" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G350" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H350" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="I350" t="s">
+        <v>15</v>
+      </c>
+      <c r="J350" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="K350" s="2" t="s">
+        <v>645</v>
+      </c>
       <c r="L350" t="str">
         <f t="shared" si="11"/>
-        <v>uEA5B-.svg</v>
+        <v>uEA5B-locale-timezone.svg</v>
       </c>
     </row>
     <row r="351" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -28020,8 +28226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M362"/>
   <sheetViews>
-    <sheetView topLeftCell="A301" workbookViewId="0">
-      <selection activeCell="G322" sqref="G322"/>
+    <sheetView topLeftCell="A337" workbookViewId="0">
+      <selection activeCell="F360" sqref="F360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44965,202 +45171,202 @@
         <v>{"id":338,"name":"personalize","unicode":"EA51","decimal":59985,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["personalize","customize","design","edit","draw","pen","brush"],"usage":"Used for customizing work item form."}</v>
       </c>
     </row>
-    <row r="340" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A340" s="15">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A340">
         <f>'Bowtie v1.0 reorg'!A341</f>
         <v>339</v>
       </c>
-      <c r="B340" s="15" t="str">
+      <c r="B340" t="str">
         <f>'Bowtie v1.0 reorg'!E341</f>
         <v>parameter</v>
       </c>
-      <c r="C340" s="15" t="str">
+      <c r="C340" t="str">
         <f>'Bowtie v1.0 reorg'!C341</f>
         <v>EA52</v>
       </c>
-      <c r="D340" s="15">
+      <c r="D340">
         <f>'Bowtie v1.0 reorg'!D341</f>
         <v>59986</v>
       </c>
-      <c r="E340" s="18">
+      <c r="E340">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F341),"",'Bowtie v1.0 reorg'!F341)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F340" s="15" t="str">
+      <c r="F340" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G341),"",'Bowtie v1.0 reorg'!G341)</f>
         <v>light</v>
       </c>
-      <c r="G340" s="15" t="str">
+      <c r="G340" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I341),"",'Bowtie v1.0 reorg'!I341)</f>
         <v>VSTS</v>
       </c>
-      <c r="H340" s="15" t="str">
+      <c r="H340" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J341),"",'Bowtie v1.0 reorg'!J341)</f>
         <v>Test</v>
       </c>
-      <c r="I340" s="15" t="str">
+      <c r="I340" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H341),"",'Bowtie v1.0 reorg'!H341)</f>
         <v>parameter variable argument @ at</v>
       </c>
-      <c r="J340" s="15" t="str">
+      <c r="J340" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K341),"",'Bowtie v1.0 reorg'!K341)</f>
         <v>Used in Test hub for adding test step parameters.</v>
       </c>
-      <c r="K340" s="15" t="str">
+      <c r="K340" t="str">
         <f t="shared" si="12"/>
         <v>{'id':339,'name':'parameter','unicode':'EA52','decimal':59986,'version':'1.1','style':'light','subset':'VSTS','group':'Test','keywords':['parameter','variable','argument','@','at'],'usage':'Used in Test hub for adding test step parameters.'}</v>
       </c>
-      <c r="L340" s="15" t="str">
+      <c r="L340" t="str">
         <f t="shared" si="13"/>
         <v>{"id":339,"name":"parameter","unicode":"EA52","decimal":59986,"version":"1.1","style":"light","subset":"VSTS","group":"Test","keywords":["parameter","variable","argument","@","at"],"usage":"Used in Test hub for adding test step parameters."}</v>
       </c>
     </row>
-    <row r="341" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A341" s="15">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A341">
         <f>'Bowtie v1.0 reorg'!A342</f>
         <v>340</v>
       </c>
-      <c r="B341" s="15" t="str">
+      <c r="B341" t="str">
         <f>'Bowtie v1.0 reorg'!E342</f>
         <v>step-insert</v>
       </c>
-      <c r="C341" s="15" t="str">
+      <c r="C341" t="str">
         <f>'Bowtie v1.0 reorg'!C342</f>
         <v>EA53</v>
       </c>
-      <c r="D341" s="15">
+      <c r="D341">
         <f>'Bowtie v1.0 reorg'!D342</f>
         <v>59987</v>
       </c>
-      <c r="E341" s="18">
+      <c r="E341">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F342),"",'Bowtie v1.0 reorg'!F342)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F341" s="15" t="str">
+      <c r="F341" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G342),"",'Bowtie v1.0 reorg'!G342)</f>
         <v>bold</v>
       </c>
-      <c r="G341" s="15" t="str">
+      <c r="G341" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I342),"",'Bowtie v1.0 reorg'!I342)</f>
         <v>VSTS</v>
       </c>
-      <c r="H341" s="15" t="str">
+      <c r="H341" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J342),"",'Bowtie v1.0 reorg'!J342)</f>
         <v>Test</v>
       </c>
-      <c r="I341" s="15" t="str">
+      <c r="I341" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H342),"",'Bowtie v1.0 reorg'!H342)</f>
         <v>step insert stairs arrow right</v>
       </c>
-      <c r="J341" s="15" t="str">
+      <c r="J341" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K342),"",'Bowtie v1.0 reorg'!K342)</f>
         <v>Used in Test hub for adding test step.</v>
       </c>
-      <c r="K341" s="15" t="str">
+      <c r="K341" t="str">
         <f t="shared" si="12"/>
         <v>{'id':340,'name':'step-insert','unicode':'EA53','decimal':59987,'version':'1.1','style':'bold','subset':'VSTS','group':'Test','keywords':['step','insert','stairs','arrow','right'],'usage':'Used in Test hub for adding test step.'}</v>
       </c>
-      <c r="L341" s="15" t="str">
+      <c r="L341" t="str">
         <f t="shared" si="13"/>
         <v>{"id":340,"name":"step-insert","unicode":"EA53","decimal":59987,"version":"1.1","style":"bold","subset":"VSTS","group":"Test","keywords":["step","insert","stairs","arrow","right"],"usage":"Used in Test hub for adding test step."}</v>
       </c>
     </row>
-    <row r="342" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A342" s="15">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A342">
         <f>'Bowtie v1.0 reorg'!A343</f>
         <v>341</v>
       </c>
-      <c r="B342" s="15" t="str">
+      <c r="B342" t="str">
         <f>'Bowtie v1.0 reorg'!E343</f>
         <v>step-shared-add</v>
       </c>
-      <c r="C342" s="15" t="str">
+      <c r="C342" t="str">
         <f>'Bowtie v1.0 reorg'!C343</f>
         <v>EA54</v>
       </c>
-      <c r="D342" s="15">
+      <c r="D342">
         <f>'Bowtie v1.0 reorg'!D343</f>
         <v>59988</v>
       </c>
-      <c r="E342" s="18">
+      <c r="E342">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F343),"",'Bowtie v1.0 reorg'!F343)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F342" s="15" t="str">
+      <c r="F342" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G343),"",'Bowtie v1.0 reorg'!G343)</f>
         <v>bold</v>
       </c>
-      <c r="G342" s="15" t="str">
+      <c r="G342" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I343),"",'Bowtie v1.0 reorg'!I343)</f>
         <v>VSTS</v>
       </c>
-      <c r="H342" s="15" t="str">
+      <c r="H342" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J343),"",'Bowtie v1.0 reorg'!J343)</f>
         <v>Test</v>
       </c>
-      <c r="I342" s="15" t="str">
+      <c r="I342" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H343),"",'Bowtie v1.0 reorg'!H343)</f>
         <v>step shared reuse multiple add plus stairs</v>
       </c>
-      <c r="J342" s="15" t="str">
+      <c r="J342" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K343),"",'Bowtie v1.0 reorg'!K343)</f>
         <v>Used in Test hub for creating a new test step as shared step.</v>
       </c>
-      <c r="K342" s="15" t="str">
+      <c r="K342" t="str">
         <f t="shared" si="12"/>
         <v>{'id':341,'name':'step-shared-add','unicode':'EA54','decimal':59988,'version':'1.1','style':'bold','subset':'VSTS','group':'Test','keywords':['step','shared','reuse','multiple','add','plus','stairs'],'usage':'Used in Test hub for creating a new test step as shared step.'}</v>
       </c>
-      <c r="L342" s="15" t="str">
+      <c r="L342" t="str">
         <f t="shared" si="13"/>
         <v>{"id":341,"name":"step-shared-add","unicode":"EA54","decimal":59988,"version":"1.1","style":"bold","subset":"VSTS","group":"Test","keywords":["step","shared","reuse","multiple","add","plus","stairs"],"usage":"Used in Test hub for creating a new test step as shared step."}</v>
       </c>
     </row>
-    <row r="343" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="15">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A343">
         <f>'Bowtie v1.0 reorg'!A344</f>
         <v>342</v>
       </c>
-      <c r="B343" s="15" t="str">
+      <c r="B343" t="str">
         <f>'Bowtie v1.0 reorg'!E344</f>
         <v>step-shared-insert</v>
       </c>
-      <c r="C343" s="15" t="str">
+      <c r="C343" t="str">
         <f>'Bowtie v1.0 reorg'!C344</f>
         <v>EA55</v>
       </c>
-      <c r="D343" s="15">
+      <c r="D343">
         <f>'Bowtie v1.0 reorg'!D344</f>
         <v>59989</v>
       </c>
-      <c r="E343" s="18">
+      <c r="E343">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F344),"",'Bowtie v1.0 reorg'!F344)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F343" s="15" t="str">
+      <c r="F343" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G344),"",'Bowtie v1.0 reorg'!G344)</f>
         <v>bold</v>
       </c>
-      <c r="G343" s="15" t="str">
+      <c r="G343" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I344),"",'Bowtie v1.0 reorg'!I344)</f>
         <v>VSTS</v>
       </c>
-      <c r="H343" s="15" t="str">
+      <c r="H343" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J344),"",'Bowtie v1.0 reorg'!J344)</f>
         <v>Test</v>
       </c>
-      <c r="I343" s="15" t="str">
+      <c r="I343" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H344),"",'Bowtie v1.0 reorg'!H344)</f>
         <v>step shared reuse multiple arrow right stairs</v>
       </c>
-      <c r="J343" s="15" t="str">
+      <c r="J343" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K344),"",'Bowtie v1.0 reorg'!K344)</f>
         <v>Used in Test hub for inserting existing shared steps.</v>
       </c>
-      <c r="K343" s="15" t="str">
+      <c r="K343" t="str">
         <f t="shared" si="12"/>
         <v>{'id':342,'name':'step-shared-insert','unicode':'EA55','decimal':59989,'version':'1.1','style':'bold','subset':'VSTS','group':'Test','keywords':['step','shared','reuse','multiple','arrow','right','stairs'],'usage':'Used in Test hub for inserting existing shared steps.'}</v>
       </c>
-      <c r="L343" s="15" t="str">
+      <c r="L343" t="str">
         <f t="shared" si="13"/>
         <v>{"id":342,"name":"step-shared-insert","unicode":"EA55","decimal":59989,"version":"1.1","style":"bold","subset":"VSTS","group":"Test","keywords":["step","shared","reuse","multiple","arrow","right","stairs"],"usage":"Used in Test hub for inserting existing shared steps."}</v>
       </c>
@@ -45283,7 +45489,7 @@
         <f>'Bowtie v1.0 reorg'!D347</f>
         <v>59992</v>
       </c>
-      <c r="E346" s="14">
+      <c r="E346">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F347),"",'Bowtie v1.0 reorg'!F347)</f>
         <v>1.1000000000000001</v>
       </c>
@@ -45308,163 +45514,162 @@
         <v>Used for a group of reusable build, deployment tasks.</v>
       </c>
       <c r="K346" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="K346:K361" si="14">IF(NOT(ISBLANK(A346)),CONCATENATE("{'",$A$1,"':",A346,",'",$B$1,"':'",B346,"',","'",$C$1,"':'",C346,"','",$D$1,"':",D346,",'",$E$1,"':'",FIXED(E346,1),"','",$F$1,"':'",F346,"','",$G$1,"':'",G346,"','",$H$1,"':'",H346,"','",$I$1,"':['",SUBSTITUTE(I346," ","','"),"'],'",$J$1,"':'",J346,"'}"))</f>
         <v>{'id':345,'name':'column-option','unicode':'EA58','decimal':59992,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['column','option','settings','gear'],'usage':'Used for a group of reusable build, deployment tasks.'}</v>
       </c>
       <c r="L346" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L346:L361" si="15">SUBSTITUTE(K346,"'","""")</f>
         <v>{"id":345,"name":"column-option","unicode":"EA58","decimal":59992,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["column","option","settings","gear"],"usage":"Used for a group of reusable build, deployment tasks."}</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A347">
+    <row r="347" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="15">
         <f>'Bowtie v1.0 reorg'!A348</f>
         <v>346</v>
       </c>
-      <c r="B347">
+      <c r="B347" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E348</f>
-        <v>0</v>
-      </c>
-      <c r="C347" t="str">
+        <v>globe</v>
+      </c>
+      <c r="C347" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C348</f>
         <v>EA59</v>
       </c>
-      <c r="D347">
+      <c r="D347" s="15">
         <f>'Bowtie v1.0 reorg'!D348</f>
         <v>59993</v>
       </c>
-      <c r="E347" s="14" t="str">
+      <c r="E347" s="15">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F348),"",'Bowtie v1.0 reorg'!F348)</f>
-        <v/>
-      </c>
-      <c r="F347" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F347" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G348),"",'Bowtie v1.0 reorg'!G348)</f>
-        <v/>
-      </c>
-      <c r="G347" t="str">
+        <v>light</v>
+      </c>
+      <c r="G347" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I348),"",'Bowtie v1.0 reorg'!I348)</f>
-        <v/>
-      </c>
-      <c r="H347" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H347" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J348),"",'Bowtie v1.0 reorg'!J348)</f>
-        <v/>
-      </c>
-      <c r="I347" t="str">
+        <v>Common</v>
+      </c>
+      <c r="I347" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H348),"",'Bowtie v1.0 reorg'!H348)</f>
-        <v/>
-      </c>
-      <c r="J347" t="str">
+        <v>web globe country region world</v>
+      </c>
+      <c r="J347" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K348),"",'Bowtie v1.0 reorg'!K348)</f>
-        <v/>
-      </c>
-      <c r="K347" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L347" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M347" s="15"/>
-    </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A348">
+        <v>Used for web or website. Also used for region or country on user profile page.</v>
+      </c>
+      <c r="K347" s="15" t="str">
+        <f t="shared" si="14"/>
+        <v>{'id':346,'name':'globe','unicode':'EA59','decimal':59993,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['web','globe','country','region','world'],'usage':'Used for web or website. Also used for region or country on user profile page.'}</v>
+      </c>
+      <c r="L347" s="15" t="str">
+        <f t="shared" si="15"/>
+        <v>{"id":346,"name":"globe","unicode":"EA59","decimal":59993,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["web","globe","country","region","world"],"usage":"Used for web or website. Also used for region or country on user profile page."}</v>
+      </c>
+    </row>
+    <row r="348" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="15">
         <f>'Bowtie v1.0 reorg'!A349</f>
         <v>347</v>
       </c>
-      <c r="B348">
+      <c r="B348" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E349</f>
-        <v>0</v>
-      </c>
-      <c r="C348" t="str">
+        <v>locale-language</v>
+      </c>
+      <c r="C348" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C349</f>
         <v>EA5A</v>
       </c>
-      <c r="D348">
+      <c r="D348" s="15">
         <f>'Bowtie v1.0 reorg'!D349</f>
         <v>59994</v>
       </c>
-      <c r="E348" s="14" t="str">
+      <c r="E348" s="15">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F349),"",'Bowtie v1.0 reorg'!F349)</f>
-        <v/>
-      </c>
-      <c r="F348" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F348" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G349),"",'Bowtie v1.0 reorg'!G349)</f>
-        <v/>
-      </c>
-      <c r="G348" t="str">
+        <v>light</v>
+      </c>
+      <c r="G348" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I349),"",'Bowtie v1.0 reorg'!I349)</f>
-        <v/>
-      </c>
-      <c r="H348" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H348" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J349),"",'Bowtie v1.0 reorg'!J349)</f>
-        <v/>
-      </c>
-      <c r="I348" t="str">
+        <v>Profile</v>
+      </c>
+      <c r="I348" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H349),"",'Bowtie v1.0 reorg'!H349)</f>
-        <v/>
-      </c>
-      <c r="J348" t="str">
+        <v>web globe country region world locale language letter character</v>
+      </c>
+      <c r="J348" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K349),"",'Bowtie v1.0 reorg'!K349)</f>
-        <v/>
-      </c>
-      <c r="K348" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L348" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A349">
+        <v>Used for language preference on user profile page.</v>
+      </c>
+      <c r="K348" s="15" t="str">
+        <f t="shared" si="14"/>
+        <v>{'id':347,'name':'locale-language','unicode':'EA5A','decimal':59994,'version':'1.1','style':'light','subset':'VSTS','group':'Profile','keywords':['web','globe','country','region','world','locale','language','letter','character'],'usage':'Used for language preference on user profile page.'}</v>
+      </c>
+      <c r="L348" s="15" t="str">
+        <f t="shared" si="15"/>
+        <v>{"id":347,"name":"locale-language","unicode":"EA5A","decimal":59994,"version":"1.1","style":"light","subset":"VSTS","group":"Profile","keywords":["web","globe","country","region","world","locale","language","letter","character"],"usage":"Used for language preference on user profile page."}</v>
+      </c>
+    </row>
+    <row r="349" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="15">
         <f>'Bowtie v1.0 reorg'!A350</f>
         <v>348</v>
       </c>
-      <c r="B349">
+      <c r="B349" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E350</f>
-        <v>0</v>
-      </c>
-      <c r="C349" t="str">
+        <v>locale-timezone</v>
+      </c>
+      <c r="C349" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C350</f>
         <v>EA5B</v>
       </c>
-      <c r="D349">
+      <c r="D349" s="15">
         <f>'Bowtie v1.0 reorg'!D350</f>
         <v>59995</v>
       </c>
-      <c r="E349" s="14" t="str">
+      <c r="E349" s="15">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F350),"",'Bowtie v1.0 reorg'!F350)</f>
-        <v/>
-      </c>
-      <c r="F349" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F349" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G350),"",'Bowtie v1.0 reorg'!G350)</f>
-        <v/>
-      </c>
-      <c r="G349" t="str">
+        <v>light</v>
+      </c>
+      <c r="G349" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I350),"",'Bowtie v1.0 reorg'!I350)</f>
-        <v/>
-      </c>
-      <c r="H349" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H349" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J350),"",'Bowtie v1.0 reorg'!J350)</f>
-        <v/>
-      </c>
-      <c r="I349" t="str">
+        <v>Profile</v>
+      </c>
+      <c r="I349" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H350),"",'Bowtie v1.0 reorg'!H350)</f>
-        <v/>
-      </c>
-      <c r="J349" t="str">
+        <v>web globe country region world timezone time clock</v>
+      </c>
+      <c r="J349" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K350),"",'Bowtie v1.0 reorg'!K350)</f>
-        <v/>
-      </c>
-      <c r="K349" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L349" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+        <v>Used for timezone preference on user profile page.</v>
+      </c>
+      <c r="K349" s="15" t="str">
+        <f t="shared" si="14"/>
+        <v>{'id':348,'name':'locale-timezone','unicode':'EA5B','decimal':59995,'version':'1.1','style':'light','subset':'VSTS','group':'Profile','keywords':['web','globe','country','region','world','timezone','time','clock'],'usage':'Used for timezone preference on user profile page.'}</v>
+      </c>
+      <c r="L349" s="15" t="str">
+        <f t="shared" si="15"/>
+        <v>{"id":348,"name":"locale-timezone","unicode":"EA5B","decimal":59995,"version":"1.1","style":"light","subset":"VSTS","group":"Profile","keywords":["web","globe","country","region","world","timezone","time","clock"],"usage":"Used for timezone preference on user profile page."}</v>
       </c>
     </row>
     <row r="350" spans="1:13" x14ac:dyDescent="0.25">
@@ -45509,11 +45714,11 @@
         <v/>
       </c>
       <c r="K350" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L350" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="M350" s="15"/>
@@ -45560,11 +45765,11 @@
         <v/>
       </c>
       <c r="K351" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L351" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -45585,7 +45790,7 @@
         <f>'Bowtie v1.0 reorg'!D353</f>
         <v>59998</v>
       </c>
-      <c r="E352" s="14" t="str">
+      <c r="E352" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F353),"",'Bowtie v1.0 reorg'!F353)</f>
         <v/>
       </c>
@@ -45610,11 +45815,11 @@
         <v/>
       </c>
       <c r="K352" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L352" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -45635,7 +45840,7 @@
         <f>'Bowtie v1.0 reorg'!D354</f>
         <v>59999</v>
       </c>
-      <c r="E353" s="14" t="str">
+      <c r="E353" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F354),"",'Bowtie v1.0 reorg'!F354)</f>
         <v/>
       </c>
@@ -45660,11 +45865,11 @@
         <v/>
       </c>
       <c r="K353" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L353" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="M353" s="15"/>
@@ -45686,7 +45891,7 @@
         <f>'Bowtie v1.0 reorg'!D355</f>
         <v>60000</v>
       </c>
-      <c r="E354" s="14" t="str">
+      <c r="E354" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F355),"",'Bowtie v1.0 reorg'!F355)</f>
         <v/>
       </c>
@@ -45711,11 +45916,11 @@
         <v/>
       </c>
       <c r="K354" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L354" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -45736,7 +45941,7 @@
         <f>'Bowtie v1.0 reorg'!D356</f>
         <v>60001</v>
       </c>
-      <c r="E355" s="14" t="str">
+      <c r="E355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F356),"",'Bowtie v1.0 reorg'!F356)</f>
         <v/>
       </c>
@@ -45761,11 +45966,11 @@
         <v/>
       </c>
       <c r="K355" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L355" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -45811,11 +46016,11 @@
         <v/>
       </c>
       <c r="K356" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L356" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="M356" s="15"/>
@@ -45862,11 +46067,11 @@
         <v/>
       </c>
       <c r="K357" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L357" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -45887,7 +46092,7 @@
         <f>'Bowtie v1.0 reorg'!D359</f>
         <v>60004</v>
       </c>
-      <c r="E358" s="14" t="str">
+      <c r="E358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F359),"",'Bowtie v1.0 reorg'!F359)</f>
         <v/>
       </c>
@@ -45912,11 +46117,11 @@
         <v/>
       </c>
       <c r="K358" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L358" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -45937,7 +46142,7 @@
         <f>'Bowtie v1.0 reorg'!D360</f>
         <v>60005</v>
       </c>
-      <c r="E359" s="14" t="str">
+      <c r="E359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F360),"",'Bowtie v1.0 reorg'!F360)</f>
         <v/>
       </c>
@@ -45962,11 +46167,11 @@
         <v/>
       </c>
       <c r="K359" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L359" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="M359" s="15"/>
@@ -45988,7 +46193,7 @@
         <f>'Bowtie v1.0 reorg'!D361</f>
         <v>60006</v>
       </c>
-      <c r="E360" s="14" t="str">
+      <c r="E360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F361),"",'Bowtie v1.0 reorg'!F361)</f>
         <v/>
       </c>
@@ -46013,11 +46218,11 @@
         <v/>
       </c>
       <c r="K360" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L360" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -46038,7 +46243,7 @@
         <f>'Bowtie v1.0 reorg'!D362</f>
         <v>60007</v>
       </c>
-      <c r="E361" s="14" t="str">
+      <c r="E361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F362),"",'Bowtie v1.0 reorg'!F362)</f>
         <v/>
       </c>
@@ -46063,11 +46268,11 @@
         <v/>
       </c>
       <c r="K361" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="L361" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -46116,7 +46321,7 @@
         <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L362" t="e">
+      <c r="L362" s="15" t="e">
         <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>

</xml_diff>

<commit_message>
added outline version feedback smiley icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="651">
   <si>
     <t>name</t>
   </si>
@@ -1958,6 +1958,21 @@
   </si>
   <si>
     <t>Used for timezone preference on user profile page.</t>
+  </si>
+  <si>
+    <t>feedback-negative-outline</t>
+  </si>
+  <si>
+    <t>feedback-positive-outline</t>
+  </si>
+  <si>
+    <t>feedback positive smile</t>
+  </si>
+  <si>
+    <t>feedback negative sad</t>
+  </si>
+  <si>
+    <t>Used in dropdown menu on white background.</t>
   </si>
 </sst>
 </file>
@@ -2043,7 +2058,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2090,6 +2105,7 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -15328,6 +15344,82 @@
         <a:xfrm>
           <a:off x="1114425" y="140188950"/>
           <a:ext cx="266737" cy="276264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>350</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409606</xdr:colOff>
+      <xdr:row>350</xdr:row>
+      <xdr:rowOff>304828</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="350" name="Picture 349"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId349"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="140608050"/>
+          <a:ext cx="219106" cy="200053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>351</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400078</xdr:colOff>
+      <xdr:row>351</xdr:row>
+      <xdr:rowOff>314356</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="351" name="Picture 350"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId350"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="140998575"/>
+          <a:ext cx="200053" cy="219106"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15606,7 +15698,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A345" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C350" sqref="C350"/>
+      <selection pane="bottomLeft" activeCell="G347" sqref="G347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -27594,9 +27686,30 @@
       <c r="D351" s="13">
         <v>59996</v>
       </c>
+      <c r="E351" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="F351" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G351" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H351" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="I351" t="s">
+        <v>15</v>
+      </c>
+      <c r="J351" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="K351" s="2" t="s">
+        <v>650</v>
+      </c>
       <c r="L351" t="str">
         <f t="shared" si="11"/>
-        <v>uEA5C-.svg</v>
+        <v>uEA5C-feedback-positive-outline.svg</v>
       </c>
     </row>
     <row r="352" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -27610,9 +27723,30 @@
       <c r="D352" s="13">
         <v>59997</v>
       </c>
+      <c r="E352" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="F352" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G352" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H352" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="I352" t="s">
+        <v>15</v>
+      </c>
+      <c r="J352" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="K352" s="2" t="s">
+        <v>650</v>
+      </c>
       <c r="L352" t="str">
         <f t="shared" si="11"/>
-        <v>uEA5D-.svg</v>
+        <v>uEA5D-feedback-negative-outline.svg</v>
       </c>
     </row>
     <row r="353" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -28227,7 +28361,7 @@
   <dimension ref="A1:M362"/>
   <sheetViews>
     <sheetView topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="F360" sqref="F360"/>
+      <selection activeCell="C350" sqref="C350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45522,255 +45656,255 @@
         <v>{"id":345,"name":"column-option","unicode":"EA58","decimal":59992,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["column","option","settings","gear"],"usage":"Used for a group of reusable build, deployment tasks."}</v>
       </c>
     </row>
-    <row r="347" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A347" s="15">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A347">
         <f>'Bowtie v1.0 reorg'!A348</f>
         <v>346</v>
       </c>
-      <c r="B347" s="15" t="str">
+      <c r="B347" t="str">
         <f>'Bowtie v1.0 reorg'!E348</f>
         <v>globe</v>
       </c>
-      <c r="C347" s="15" t="str">
+      <c r="C347" t="str">
         <f>'Bowtie v1.0 reorg'!C348</f>
         <v>EA59</v>
       </c>
-      <c r="D347" s="15">
+      <c r="D347">
         <f>'Bowtie v1.0 reorg'!D348</f>
         <v>59993</v>
       </c>
-      <c r="E347" s="15">
+      <c r="E347">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F348),"",'Bowtie v1.0 reorg'!F348)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F347" s="15" t="str">
+      <c r="F347" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G348),"",'Bowtie v1.0 reorg'!G348)</f>
         <v>light</v>
       </c>
-      <c r="G347" s="15" t="str">
+      <c r="G347" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I348),"",'Bowtie v1.0 reorg'!I348)</f>
         <v>VSTS</v>
       </c>
-      <c r="H347" s="15" t="str">
+      <c r="H347" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J348),"",'Bowtie v1.0 reorg'!J348)</f>
         <v>Common</v>
       </c>
-      <c r="I347" s="15" t="str">
+      <c r="I347" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H348),"",'Bowtie v1.0 reorg'!H348)</f>
         <v>web globe country region world</v>
       </c>
-      <c r="J347" s="15" t="str">
+      <c r="J347" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K348),"",'Bowtie v1.0 reorg'!K348)</f>
         <v>Used for web or website. Also used for region or country on user profile page.</v>
       </c>
-      <c r="K347" s="15" t="str">
+      <c r="K347" t="str">
         <f t="shared" si="14"/>
         <v>{'id':346,'name':'globe','unicode':'EA59','decimal':59993,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['web','globe','country','region','world'],'usage':'Used for web or website. Also used for region or country on user profile page.'}</v>
       </c>
-      <c r="L347" s="15" t="str">
+      <c r="L347" t="str">
         <f t="shared" si="15"/>
         <v>{"id":346,"name":"globe","unicode":"EA59","decimal":59993,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["web","globe","country","region","world"],"usage":"Used for web or website. Also used for region or country on user profile page."}</v>
       </c>
-    </row>
-    <row r="348" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A348" s="15">
+      <c r="M347" s="15"/>
+    </row>
+    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A348">
         <f>'Bowtie v1.0 reorg'!A349</f>
         <v>347</v>
       </c>
-      <c r="B348" s="15" t="str">
+      <c r="B348" t="str">
         <f>'Bowtie v1.0 reorg'!E349</f>
         <v>locale-language</v>
       </c>
-      <c r="C348" s="15" t="str">
+      <c r="C348" t="str">
         <f>'Bowtie v1.0 reorg'!C349</f>
         <v>EA5A</v>
       </c>
-      <c r="D348" s="15">
+      <c r="D348">
         <f>'Bowtie v1.0 reorg'!D349</f>
         <v>59994</v>
       </c>
-      <c r="E348" s="15">
+      <c r="E348">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F349),"",'Bowtie v1.0 reorg'!F349)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F348" s="15" t="str">
+      <c r="F348" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G349),"",'Bowtie v1.0 reorg'!G349)</f>
         <v>light</v>
       </c>
-      <c r="G348" s="15" t="str">
+      <c r="G348" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I349),"",'Bowtie v1.0 reorg'!I349)</f>
         <v>VSTS</v>
       </c>
-      <c r="H348" s="15" t="str">
+      <c r="H348" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J349),"",'Bowtie v1.0 reorg'!J349)</f>
         <v>Profile</v>
       </c>
-      <c r="I348" s="15" t="str">
+      <c r="I348" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H349),"",'Bowtie v1.0 reorg'!H349)</f>
         <v>web globe country region world locale language letter character</v>
       </c>
-      <c r="J348" s="15" t="str">
+      <c r="J348" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K349),"",'Bowtie v1.0 reorg'!K349)</f>
         <v>Used for language preference on user profile page.</v>
       </c>
-      <c r="K348" s="15" t="str">
+      <c r="K348" t="str">
         <f t="shared" si="14"/>
         <v>{'id':347,'name':'locale-language','unicode':'EA5A','decimal':59994,'version':'1.1','style':'light','subset':'VSTS','group':'Profile','keywords':['web','globe','country','region','world','locale','language','letter','character'],'usage':'Used for language preference on user profile page.'}</v>
       </c>
-      <c r="L348" s="15" t="str">
+      <c r="L348" t="str">
         <f t="shared" si="15"/>
         <v>{"id":347,"name":"locale-language","unicode":"EA5A","decimal":59994,"version":"1.1","style":"light","subset":"VSTS","group":"Profile","keywords":["web","globe","country","region","world","locale","language","letter","character"],"usage":"Used for language preference on user profile page."}</v>
       </c>
     </row>
-    <row r="349" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A349" s="15">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A349">
         <f>'Bowtie v1.0 reorg'!A350</f>
         <v>348</v>
       </c>
-      <c r="B349" s="15" t="str">
+      <c r="B349" t="str">
         <f>'Bowtie v1.0 reorg'!E350</f>
         <v>locale-timezone</v>
       </c>
-      <c r="C349" s="15" t="str">
+      <c r="C349" t="str">
         <f>'Bowtie v1.0 reorg'!C350</f>
         <v>EA5B</v>
       </c>
-      <c r="D349" s="15">
+      <c r="D349">
         <f>'Bowtie v1.0 reorg'!D350</f>
         <v>59995</v>
       </c>
-      <c r="E349" s="15">
+      <c r="E349">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F350),"",'Bowtie v1.0 reorg'!F350)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F349" s="15" t="str">
+      <c r="F349" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G350),"",'Bowtie v1.0 reorg'!G350)</f>
         <v>light</v>
       </c>
-      <c r="G349" s="15" t="str">
+      <c r="G349" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I350),"",'Bowtie v1.0 reorg'!I350)</f>
         <v>VSTS</v>
       </c>
-      <c r="H349" s="15" t="str">
+      <c r="H349" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J350),"",'Bowtie v1.0 reorg'!J350)</f>
         <v>Profile</v>
       </c>
-      <c r="I349" s="15" t="str">
+      <c r="I349" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H350),"",'Bowtie v1.0 reorg'!H350)</f>
         <v>web globe country region world timezone time clock</v>
       </c>
-      <c r="J349" s="15" t="str">
+      <c r="J349" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K350),"",'Bowtie v1.0 reorg'!K350)</f>
         <v>Used for timezone preference on user profile page.</v>
       </c>
-      <c r="K349" s="15" t="str">
+      <c r="K349" t="str">
         <f t="shared" si="14"/>
         <v>{'id':348,'name':'locale-timezone','unicode':'EA5B','decimal':59995,'version':'1.1','style':'light','subset':'VSTS','group':'Profile','keywords':['web','globe','country','region','world','timezone','time','clock'],'usage':'Used for timezone preference on user profile page.'}</v>
       </c>
-      <c r="L349" s="15" t="str">
+      <c r="L349" t="str">
         <f t="shared" si="15"/>
         <v>{"id":348,"name":"locale-timezone","unicode":"EA5B","decimal":59995,"version":"1.1","style":"light","subset":"VSTS","group":"Profile","keywords":["web","globe","country","region","world","timezone","time","clock"],"usage":"Used for timezone preference on user profile page."}</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A350">
+    <row r="350" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A350" s="15">
         <f>'Bowtie v1.0 reorg'!A351</f>
         <v>349</v>
       </c>
-      <c r="B350">
+      <c r="B350" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E351</f>
-        <v>0</v>
-      </c>
-      <c r="C350" t="str">
+        <v>feedback-positive-outline</v>
+      </c>
+      <c r="C350" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C351</f>
         <v>EA5C</v>
       </c>
-      <c r="D350">
+      <c r="D350" s="15">
         <f>'Bowtie v1.0 reorg'!D351</f>
         <v>59996</v>
       </c>
-      <c r="E350" s="14" t="str">
+      <c r="E350" s="18">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F351),"",'Bowtie v1.0 reorg'!F351)</f>
-        <v/>
-      </c>
-      <c r="F350" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F350" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G351),"",'Bowtie v1.0 reorg'!G351)</f>
-        <v/>
-      </c>
-      <c r="G350" t="str">
+        <v>light</v>
+      </c>
+      <c r="G350" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I351),"",'Bowtie v1.0 reorg'!I351)</f>
-        <v/>
-      </c>
-      <c r="H350" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H350" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J351),"",'Bowtie v1.0 reorg'!J351)</f>
-        <v/>
-      </c>
-      <c r="I350" t="str">
+        <v>Common</v>
+      </c>
+      <c r="I350" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H351),"",'Bowtie v1.0 reorg'!H351)</f>
-        <v/>
-      </c>
-      <c r="J350" t="str">
+        <v>feedback positive smile</v>
+      </c>
+      <c r="J350" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K351),"",'Bowtie v1.0 reorg'!K351)</f>
-        <v/>
-      </c>
-      <c r="K350" t="e">
+        <v>Used in dropdown menu on white background.</v>
+      </c>
+      <c r="K350" s="15" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L350" t="e">
+        <v>{'id':349,'name':'feedback-positive-outline','unicode':'EA5C','decimal':59996,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['feedback','positive','smile'],'usage':'Used in dropdown menu on white background.'}</v>
+      </c>
+      <c r="L350" s="15" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M350" s="15"/>
-    </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A351">
+        <v>{"id":349,"name":"feedback-positive-outline","unicode":"EA5C","decimal":59996,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["feedback","positive","smile"],"usage":"Used in dropdown menu on white background."}</v>
+      </c>
+    </row>
+    <row r="351" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A351" s="15">
         <f>'Bowtie v1.0 reorg'!A352</f>
         <v>350</v>
       </c>
-      <c r="B351">
+      <c r="B351" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!E352</f>
-        <v>0</v>
-      </c>
-      <c r="C351" t="str">
+        <v>feedback-negative-outline</v>
+      </c>
+      <c r="C351" s="15" t="str">
         <f>'Bowtie v1.0 reorg'!C352</f>
         <v>EA5D</v>
       </c>
-      <c r="D351">
+      <c r="D351" s="15">
         <f>'Bowtie v1.0 reorg'!D352</f>
         <v>59997</v>
       </c>
-      <c r="E351" s="14" t="str">
+      <c r="E351" s="18">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F352),"",'Bowtie v1.0 reorg'!F352)</f>
-        <v/>
-      </c>
-      <c r="F351" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F351" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G352),"",'Bowtie v1.0 reorg'!G352)</f>
-        <v/>
-      </c>
-      <c r="G351" t="str">
+        <v>light</v>
+      </c>
+      <c r="G351" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I352),"",'Bowtie v1.0 reorg'!I352)</f>
-        <v/>
-      </c>
-      <c r="H351" t="str">
+        <v>VSTS</v>
+      </c>
+      <c r="H351" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J352),"",'Bowtie v1.0 reorg'!J352)</f>
-        <v/>
-      </c>
-      <c r="I351" t="str">
+        <v>Common</v>
+      </c>
+      <c r="I351" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H352),"",'Bowtie v1.0 reorg'!H352)</f>
-        <v/>
-      </c>
-      <c r="J351" t="str">
+        <v>feedback negative sad</v>
+      </c>
+      <c r="J351" s="15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K352),"",'Bowtie v1.0 reorg'!K352)</f>
-        <v/>
-      </c>
-      <c r="K351" t="e">
+        <v>Used in dropdown menu on white background.</v>
+      </c>
+      <c r="K351" s="15" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L351" t="e">
+        <v>{'id':350,'name':'feedback-negative-outline','unicode':'EA5D','decimal':59997,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['feedback','negative','sad'],'usage':'Used in dropdown menu on white background.'}</v>
+      </c>
+      <c r="L351" s="15" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":350,"name":"feedback-negative-outline","unicode":"EA5D","decimal":59997,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["feedback","negative","sad"],"usage":"Used in dropdown menu on white background."}</v>
       </c>
     </row>
     <row r="352" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added vsts brand icon
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1654" uniqueCount="657">
   <si>
     <t>name</t>
   </si>
@@ -1982,6 +1982,15 @@
   </si>
   <si>
     <t>Used for contact card.</t>
+  </si>
+  <si>
+    <t>brand-vsts</t>
+  </si>
+  <si>
+    <t>vsts brand logo</t>
+  </si>
+  <si>
+    <t>VSTS product icon.</t>
   </si>
 </sst>
 </file>
@@ -15465,6 +15474,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1114425" y="141370050"/>
+          <a:ext cx="209579" cy="228632"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>354</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409604</xdr:colOff>
+      <xdr:row>354</xdr:row>
+      <xdr:rowOff>333407</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="353" name="Picture 352"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId352"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="142208250"/>
           <a:ext cx="209579" cy="228632"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15743,8 +15790,8 @@
   <dimension ref="A1:AL410"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C353" sqref="C353"/>
+      <pane ySplit="2" topLeftCell="A348" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K356" sqref="K356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -27795,44 +27842,70 @@
         <v>uEA5D-feedback-negative-outline.svg</v>
       </c>
     </row>
-    <row r="353" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A353" s="2">
+    <row r="353" spans="1:38" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="1">
         <v>351</v>
       </c>
-      <c r="C353" s="13" t="str">
+      <c r="C353" s="16" t="str">
         <f t="shared" si="10"/>
         <v>EA5E</v>
       </c>
-      <c r="D353" s="13">
+      <c r="D353" s="16">
         <v>59998</v>
       </c>
-      <c r="E353" s="2" t="s">
+      <c r="E353" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="F353" s="3">
+      <c r="F353" s="17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G353" s="2" t="s">
+      <c r="G353" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H353" s="2" t="s">
+      <c r="H353" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="I353" s="2" t="s">
+      <c r="I353" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J353" s="2" t="s">
+      <c r="J353" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="K353" s="2" t="s">
+      <c r="K353" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="L353" t="str">
+      <c r="L353" s="15" t="str">
         <f t="shared" si="11"/>
         <v>uEA5E-contact-card.svg</v>
       </c>
-    </row>
-    <row r="354" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M353" s="15"/>
+      <c r="N353" s="15"/>
+      <c r="O353" s="15"/>
+      <c r="P353" s="15"/>
+      <c r="Q353" s="15"/>
+      <c r="R353" s="15"/>
+      <c r="S353" s="15"/>
+      <c r="T353" s="15"/>
+      <c r="U353" s="15"/>
+      <c r="V353" s="15"/>
+      <c r="W353" s="15"/>
+      <c r="X353" s="15"/>
+      <c r="Y353" s="15"/>
+      <c r="Z353" s="15"/>
+      <c r="AA353" s="15"/>
+      <c r="AB353" s="15"/>
+      <c r="AC353" s="15"/>
+      <c r="AD353" s="15"/>
+      <c r="AE353" s="15"/>
+      <c r="AF353" s="15"/>
+      <c r="AG353" s="15"/>
+      <c r="AH353" s="15"/>
+      <c r="AI353" s="15"/>
+      <c r="AJ353" s="15"/>
+      <c r="AK353" s="15"/>
+      <c r="AL353" s="15"/>
+    </row>
+    <row r="354" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="2">
         <v>352</v>
       </c>
@@ -27848,23 +27921,70 @@
         <v>uEA5F-.svg</v>
       </c>
     </row>
-    <row r="355" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A355" s="2">
+    <row r="355" spans="1:38" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A355" s="1">
         <v>353</v>
       </c>
-      <c r="C355" s="13" t="str">
+      <c r="C355" s="16" t="str">
         <f t="shared" si="10"/>
         <v>EA60</v>
       </c>
-      <c r="D355" s="13">
+      <c r="D355" s="16">
         <v>60000</v>
       </c>
-      <c r="L355" t="str">
+      <c r="E355" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="F355" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G355" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H355" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="I355" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J355" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="K355" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="L355" s="15" t="str">
         <f t="shared" si="11"/>
-        <v>uEA60-.svg</v>
-      </c>
-    </row>
-    <row r="356" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>uEA60-brand-vsts.svg</v>
+      </c>
+      <c r="M355" s="15"/>
+      <c r="N355" s="15"/>
+      <c r="O355" s="15"/>
+      <c r="P355" s="15"/>
+      <c r="Q355" s="15"/>
+      <c r="R355" s="15"/>
+      <c r="S355" s="15"/>
+      <c r="T355" s="15"/>
+      <c r="U355" s="15"/>
+      <c r="V355" s="15"/>
+      <c r="W355" s="15"/>
+      <c r="X355" s="15"/>
+      <c r="Y355" s="15"/>
+      <c r="Z355" s="15"/>
+      <c r="AA355" s="15"/>
+      <c r="AB355" s="15"/>
+      <c r="AC355" s="15"/>
+      <c r="AD355" s="15"/>
+      <c r="AE355" s="15"/>
+      <c r="AF355" s="15"/>
+      <c r="AG355" s="15"/>
+      <c r="AH355" s="15"/>
+      <c r="AI355" s="15"/>
+      <c r="AJ355" s="15"/>
+      <c r="AK355" s="15"/>
+      <c r="AL355" s="15"/>
+    </row>
+    <row r="356" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="2">
         <v>354</v>
       </c>
@@ -27880,7 +28000,7 @@
         <v>uEA61-.svg</v>
       </c>
     </row>
-    <row r="357" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="2">
         <v>355</v>
       </c>
@@ -27896,7 +28016,7 @@
         <v>uEA62-.svg</v>
       </c>
     </row>
-    <row r="358" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="2">
         <v>356</v>
       </c>
@@ -27908,7 +28028,7 @@
         <v>60003</v>
       </c>
     </row>
-    <row r="359" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="2">
         <v>357</v>
       </c>
@@ -27920,7 +28040,7 @@
         <v>60004</v>
       </c>
     </row>
-    <row r="360" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="2">
         <v>358</v>
       </c>
@@ -27932,7 +28052,7 @@
         <v>60005</v>
       </c>
     </row>
-    <row r="361" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="2">
         <v>359</v>
       </c>
@@ -27944,7 +28064,7 @@
         <v>60006</v>
       </c>
     </row>
-    <row r="362" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="2">
         <v>360</v>
       </c>
@@ -27956,7 +28076,7 @@
         <v>60007</v>
       </c>
     </row>
-    <row r="363" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="2">
         <v>361</v>
       </c>
@@ -27968,7 +28088,7 @@
         <v>60008</v>
       </c>
     </row>
-    <row r="364" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="2">
         <v>362</v>
       </c>
@@ -27980,7 +28100,7 @@
         <v>60009</v>
       </c>
     </row>
-    <row r="365" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="2">
         <v>363</v>
       </c>
@@ -27992,7 +28112,7 @@
         <v>60010</v>
       </c>
     </row>
-    <row r="366" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="2">
         <v>364</v>
       </c>
@@ -28004,7 +28124,7 @@
         <v>60011</v>
       </c>
     </row>
-    <row r="367" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="2">
         <v>365</v>
       </c>
@@ -28016,7 +28136,7 @@
         <v>60012</v>
       </c>
     </row>
-    <row r="368" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="2">
         <v>366</v>
       </c>
@@ -28427,8 +28547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="O351" sqref="O351"/>
+    <sheetView topLeftCell="A337" workbookViewId="0">
+      <selection activeCell="L354" sqref="L354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44866,11 +44986,11 @@
         <v>Used in context menu for Auto fill template form command.</v>
       </c>
       <c r="K329" t="str">
-        <f t="shared" ref="K329:K362" si="12">IF(NOT(ISBLANK(A329)),CONCATENATE("{'",$A$1,"':",A329,",'",$B$1,"':'",B329,"',","'",$C$1,"':'",C329,"','",$D$1,"':",D329,",'",$E$1,"':'",FIXED(E329,1),"','",$F$1,"':'",F329,"','",$G$1,"':'",G329,"','",$H$1,"':'",H329,"','",$I$1,"':['",SUBSTITUTE(I329," ","','"),"'],'",$J$1,"':'",J329,"'}"))</f>
+        <f t="shared" ref="K329:K345" si="12">IF(NOT(ISBLANK(A329)),CONCATENATE("{'",$A$1,"':",A329,",'",$B$1,"':'",B329,"',","'",$C$1,"':'",C329,"','",$D$1,"':",D329,",'",$E$1,"':'",FIXED(E329,1),"','",$F$1,"':'",F329,"','",$G$1,"':'",G329,"','",$H$1,"':'",H329,"','",$I$1,"':['",SUBSTITUTE(I329," ","','"),"'],'",$J$1,"':'",J329,"'}"))</f>
         <v>{'id':328,'name':'auto-fill-template','unicode':'EA47','decimal':59975,'version':'1.0','style':'light','subset':'VSTS','group':'Work','keywords':['template','watermark','fill','box','form'],'usage':'Used in context menu for Auto fill template form command.'}</v>
       </c>
       <c r="L329" t="str">
-        <f t="shared" ref="L329:L362" si="13">SUBSTITUTE(K329,"'","""")</f>
+        <f t="shared" ref="L329:L345" si="13">SUBSTITUTE(K329,"'","""")</f>
         <v>{"id":328,"name":"auto-fill-template","unicode":"EA47","decimal":59975,"version":"1.0","style":"light","subset":"VSTS","group":"Work","keywords":["template","watermark","fill","box","form"],"usage":"Used in context menu for Auto fill template form command."}</v>
       </c>
     </row>
@@ -45714,11 +45834,11 @@
         <v>Used for a group of reusable build, deployment tasks.</v>
       </c>
       <c r="K346" t="str">
-        <f t="shared" ref="K346:K361" si="14">IF(NOT(ISBLANK(A346)),CONCATENATE("{'",$A$1,"':",A346,",'",$B$1,"':'",B346,"',","'",$C$1,"':'",C346,"','",$D$1,"':",D346,",'",$E$1,"':'",FIXED(E346,1),"','",$F$1,"':'",F346,"','",$G$1,"':'",G346,"','",$H$1,"':'",H346,"','",$I$1,"':['",SUBSTITUTE(I346," ","','"),"'],'",$J$1,"':'",J346,"'}"))</f>
+        <f t="shared" ref="K346:K352" si="14">IF(NOT(ISBLANK(A346)),CONCATENATE("{'",$A$1,"':",A346,",'",$B$1,"':'",B346,"',","'",$C$1,"':'",C346,"','",$D$1,"':",D346,",'",$E$1,"':'",FIXED(E346,1),"','",$F$1,"':'",F346,"','",$G$1,"':'",G346,"','",$H$1,"':'",H346,"','",$I$1,"':['",SUBSTITUTE(I346," ","','"),"'],'",$J$1,"':'",J346,"'}"))</f>
         <v>{'id':345,'name':'column-option','unicode':'EA58','decimal':59992,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['column','option','settings','gear'],'usage':'Used for a group of reusable build, deployment tasks.'}</v>
       </c>
       <c r="L346" t="str">
-        <f t="shared" ref="L346:L361" si="15">SUBSTITUTE(K346,"'","""")</f>
+        <f t="shared" ref="L346:L352" si="15">SUBSTITUTE(K346,"'","""")</f>
         <v>{"id":345,"name":"column-option","unicode":"EA58","decimal":59992,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["column","option","settings","gear"],"usage":"Used for a group of reusable build, deployment tasks."}</v>
       </c>
     </row>
@@ -46077,9 +46197,9 @@
         <f>'Bowtie v1.0 reorg'!A355</f>
         <v>353</v>
       </c>
-      <c r="B354">
+      <c r="B354" t="str">
         <f>'Bowtie v1.0 reorg'!E355</f>
-        <v>0</v>
+        <v>brand-vsts</v>
       </c>
       <c r="C354" t="str">
         <f>'Bowtie v1.0 reorg'!C355</f>
@@ -46089,37 +46209,37 @@
         <f>'Bowtie v1.0 reorg'!D355</f>
         <v>60000</v>
       </c>
-      <c r="E354" t="str">
+      <c r="E354">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F355),"",'Bowtie v1.0 reorg'!F355)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F354" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G355),"",'Bowtie v1.0 reorg'!G355)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G354" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I355),"",'Bowtie v1.0 reorg'!I355)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H354" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J355),"",'Bowtie v1.0 reorg'!J355)</f>
-        <v/>
+        <v>Brand</v>
       </c>
       <c r="I354" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H355),"",'Bowtie v1.0 reorg'!H355)</f>
-        <v/>
+        <v>vsts brand logo</v>
       </c>
       <c r="J354" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K355),"",'Bowtie v1.0 reorg'!K355)</f>
-        <v/>
-      </c>
-      <c r="K354" t="e">
+        <v>VSTS product icon.</v>
+      </c>
+      <c r="K354" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L354" t="e">
+        <v>{'id':353,'name':'brand-vsts','unicode':'EA60','decimal':60000,'version':'1.1','style':'bold','subset':'VSTS','group':'Brand','keywords':['vsts','brand','logo'],'usage':'VSTS product icon.'}</v>
+      </c>
+      <c r="L354" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":353,"name":"brand-vsts","unicode":"EA60","decimal":60000,"version":"1.1","style":"bold","subset":"VSTS","group":"Brand","keywords":["vsts","brand","logo"],"usage":"VSTS product icon."}</v>
       </c>
     </row>
     <row r="355" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added triangle for status icon stacking as background
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1654" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="657">
   <si>
     <t>name</t>
   </si>
@@ -1699,12 +1699,6 @@
     <t>check if it is same as play-fill</t>
   </si>
   <si>
-    <t>check if it is same as record-fill</t>
-  </si>
-  <si>
-    <t>check if it is same as stop-fill</t>
-  </si>
-  <si>
     <t>used in context menu or toolbar for Delete command, matching Add command.</t>
   </si>
   <si>
@@ -1876,9 +1870,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Misc</t>
-  </si>
-  <si>
     <t>mtm microsoft test manager</t>
   </si>
   <si>
@@ -1991,6 +1982,15 @@
   </si>
   <si>
     <t>VSTS product icon.</t>
+  </si>
+  <si>
+    <t>triangle</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>Used for stacking icons as background.</t>
   </si>
 </sst>
 </file>
@@ -15513,6 +15513,44 @@
         <a:xfrm>
           <a:off x="1143000" y="142208250"/>
           <a:ext cx="209579" cy="228632"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>353</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390554</xdr:colOff>
+      <xdr:row>353</xdr:row>
+      <xdr:rowOff>314354</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="354" name="Picture 353"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId353"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1123950" y="141808200"/>
+          <a:ext cx="209579" cy="209579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15790,8 +15828,8 @@
   <dimension ref="A1:AL410"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A348" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K356" sqref="K356"/>
+      <pane ySplit="2" topLeftCell="A351" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G358" sqref="G358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15959,7 +15997,7 @@
         <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>187</v>
@@ -15996,7 +16034,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>187</v>
@@ -16033,7 +16071,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>187</v>
@@ -16070,7 +16108,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>187</v>
@@ -16107,7 +16145,7 @@
         <v>15</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>186</v>
@@ -16145,7 +16183,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>188</v>
@@ -16207,7 +16245,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>186</v>
@@ -16244,7 +16282,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>185</v>
@@ -16275,13 +16313,13 @@
         <v>17</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="1"/>
@@ -16309,13 +16347,13 @@
         <v>17</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="1"/>
@@ -16350,7 +16388,7 @@
         <v>15</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" t="str">
@@ -16411,7 +16449,7 @@
         <v>15</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>168</v>
@@ -16449,7 +16487,7 @@
         <v>15</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>169</v>
@@ -16477,13 +16515,13 @@
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="1"/>
@@ -16508,16 +16546,16 @@
         <v>1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="1"/>
@@ -16542,16 +16580,16 @@
         <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="1"/>
@@ -16576,16 +16614,16 @@
         <v>1</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="1"/>
@@ -16619,7 +16657,7 @@
         <v>15</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="1"/>
@@ -16653,7 +16691,7 @@
         <v>15</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="1"/>
@@ -16687,7 +16725,7 @@
         <v>15</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>193</v>
@@ -16724,7 +16762,7 @@
         <v>15</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>193</v>
@@ -16761,7 +16799,7 @@
         <v>15</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>193</v>
@@ -16798,7 +16836,7 @@
         <v>15</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>193</v>
@@ -16835,7 +16873,7 @@
         <v>15</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>193</v>
@@ -16863,13 +16901,13 @@
         <v>1</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="1"/>
@@ -16903,7 +16941,7 @@
         <v>15</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>193</v>
@@ -16941,7 +16979,7 @@
         <v>15</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>193</v>
@@ -17003,7 +17041,7 @@
         <v>15</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>194</v>
@@ -17040,7 +17078,7 @@
         <v>15</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>193</v>
@@ -17077,7 +17115,7 @@
         <v>15</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>195</v>
@@ -17114,7 +17152,7 @@
         <v>15</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>196</v>
@@ -17152,7 +17190,7 @@
         <v>15</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>116</v>
@@ -17190,7 +17228,7 @@
         <v>15</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>121</v>
@@ -17224,7 +17262,7 @@
         <v>15</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>224</v>
@@ -17286,7 +17324,7 @@
         <v>15</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>203</v>
@@ -17323,7 +17361,7 @@
         <v>15</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>204</v>
@@ -17360,7 +17398,7 @@
         <v>15</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>205</v>
@@ -17397,7 +17435,7 @@
         <v>15</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>206</v>
@@ -17434,7 +17472,7 @@
         <v>15</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>207</v>
@@ -17471,7 +17509,7 @@
         <v>15</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>208</v>
@@ -17508,7 +17546,7 @@
         <v>15</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>209</v>
@@ -17545,7 +17583,7 @@
         <v>15</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>210</v>
@@ -17577,7 +17615,7 @@
         <v>17</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>15</v>
@@ -17651,7 +17689,7 @@
         <v>17</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>15</v>
@@ -17691,7 +17729,7 @@
         <v>15</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L48" t="str">
         <f t="shared" si="1"/>
@@ -17725,7 +17763,7 @@
         <v>15</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L49" t="str">
         <f t="shared" si="1"/>
@@ -17759,7 +17797,7 @@
         <v>15</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L50" t="str">
         <f t="shared" si="1"/>
@@ -17793,7 +17831,7 @@
         <v>15</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L51" t="str">
         <f t="shared" si="1"/>
@@ -17827,7 +17865,7 @@
         <v>15</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" si="1"/>
@@ -17861,7 +17899,7 @@
         <v>15</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L53" t="str">
         <f t="shared" si="1"/>
@@ -17895,7 +17933,7 @@
         <v>15</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L54" t="str">
         <f t="shared" si="1"/>
@@ -17929,7 +17967,7 @@
         <v>15</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" si="1"/>
@@ -17963,7 +18001,7 @@
         <v>15</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>189</v>
@@ -18001,7 +18039,7 @@
         <v>15</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>190</v>
@@ -18039,7 +18077,7 @@
         <v>15</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K58" s="4" t="s">
         <v>190</v>
@@ -18070,13 +18108,13 @@
         <v>17</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L59" t="str">
         <f t="shared" si="1"/>
@@ -18110,7 +18148,7 @@
         <v>15</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>200</v>
@@ -18141,13 +18179,13 @@
         <v>17</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>198</v>
@@ -18184,7 +18222,7 @@
         <v>15</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>199</v>
@@ -18221,7 +18259,7 @@
         <v>15</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>202</v>
@@ -18258,7 +18296,7 @@
         <v>15</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>201</v>
@@ -18286,13 +18324,13 @@
         <v>1</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L65" t="str">
         <f t="shared" si="1"/>
@@ -18326,7 +18364,7 @@
         <v>15</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>221</v>
@@ -18363,7 +18401,7 @@
         <v>15</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L67" t="str">
         <f t="shared" si="1"/>
@@ -18397,7 +18435,7 @@
         <v>15</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L68" t="str">
         <f t="shared" ref="L68:L131" si="3">CONCATENATE("u",C68,"-",E68,".svg")</f>
@@ -18431,7 +18469,7 @@
         <v>15</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L69" t="str">
         <f t="shared" si="3"/>
@@ -18465,7 +18503,7 @@
         <v>15</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L70" t="str">
         <f t="shared" si="3"/>
@@ -18499,7 +18537,7 @@
         <v>15</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L71" t="str">
         <f t="shared" si="3"/>
@@ -18534,7 +18572,7 @@
         <v>15</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K72" s="2"/>
       <c r="L72" t="str">
@@ -18588,13 +18626,13 @@
         <v>16</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L73" t="str">
         <f t="shared" si="3"/>
@@ -18622,13 +18660,13 @@
         <v>16</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L74" t="str">
         <f t="shared" si="3"/>
@@ -18662,7 +18700,7 @@
         <v>15</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L75" t="str">
         <f t="shared" si="3"/>
@@ -18696,7 +18734,7 @@
         <v>15</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L76" t="str">
         <f t="shared" si="3"/>
@@ -18730,7 +18768,7 @@
         <v>15</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L77" t="str">
         <f t="shared" si="3"/>
@@ -18764,7 +18802,7 @@
         <v>15</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L78" t="str">
         <f t="shared" si="3"/>
@@ -18798,7 +18836,7 @@
         <v>15</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L79" t="str">
         <f t="shared" si="3"/>
@@ -18832,7 +18870,7 @@
         <v>15</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L80" t="str">
         <f t="shared" si="3"/>
@@ -18866,7 +18904,7 @@
         <v>15</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L81" t="str">
         <f t="shared" si="3"/>
@@ -18901,10 +18939,10 @@
         <v>15</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="L82" t="str">
         <f t="shared" si="3"/>
@@ -18964,7 +19002,7 @@
         <v>15</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K83" s="4" t="s">
         <v>90</v>
@@ -19001,7 +19039,7 @@
         <v>15</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L84" t="str">
         <f t="shared" si="3"/>
@@ -19035,7 +19073,7 @@
         <v>15</v>
       </c>
       <c r="J85" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L85" t="str">
         <f t="shared" si="3"/>
@@ -19069,7 +19107,7 @@
         <v>15</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L86" t="str">
         <f t="shared" si="3"/>
@@ -19103,7 +19141,7 @@
         <v>15</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>191</v>
@@ -19140,7 +19178,7 @@
         <v>15</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L88" t="str">
         <f t="shared" si="3"/>
@@ -19168,7 +19206,7 @@
         <v>15</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L89" t="str">
         <f t="shared" si="3"/>
@@ -19196,7 +19234,7 @@
         <v>15</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L90" t="str">
         <f t="shared" si="3"/>
@@ -19224,7 +19262,7 @@
         <v>15</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L91" t="str">
         <f t="shared" si="3"/>
@@ -19258,7 +19296,7 @@
         <v>15</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L92" t="str">
         <f t="shared" si="3"/>
@@ -19292,7 +19330,7 @@
         <v>15</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L93" t="str">
         <f t="shared" si="3"/>
@@ -19326,7 +19364,7 @@
         <v>15</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L94" t="str">
         <f t="shared" si="3"/>
@@ -19360,7 +19398,7 @@
         <v>15</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L95" t="str">
         <f t="shared" si="3"/>
@@ -19395,7 +19433,7 @@
         <v>15</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K96" s="2"/>
       <c r="L96" t="str">
@@ -19455,7 +19493,7 @@
         <v>15</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L97" t="str">
         <f t="shared" si="3"/>
@@ -19489,7 +19527,7 @@
         <v>15</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L98" t="str">
         <f t="shared" si="3"/>
@@ -19523,7 +19561,7 @@
         <v>15</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L99" t="str">
         <f t="shared" si="3"/>
@@ -19557,7 +19595,7 @@
         <v>15</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L100" t="str">
         <f t="shared" si="3"/>
@@ -19591,7 +19629,7 @@
         <v>15</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L101" t="str">
         <f t="shared" si="3"/>
@@ -19625,7 +19663,7 @@
         <v>15</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K102" s="2" t="s">
         <v>124</v>
@@ -19662,7 +19700,7 @@
         <v>15</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K103" s="2" t="s">
         <v>123</v>
@@ -19699,7 +19737,7 @@
         <v>15</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L104" t="str">
         <f t="shared" si="3"/>
@@ -19733,7 +19771,7 @@
         <v>15</v>
       </c>
       <c r="J105" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L105" t="str">
         <f t="shared" si="3"/>
@@ -19767,7 +19805,7 @@
         <v>15</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L106" t="str">
         <f t="shared" si="3"/>
@@ -19801,7 +19839,7 @@
         <v>15</v>
       </c>
       <c r="J107" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L107" t="str">
         <f t="shared" si="3"/>
@@ -19835,7 +19873,7 @@
         <v>15</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L108" t="str">
         <f t="shared" si="3"/>
@@ -19869,7 +19907,7 @@
         <v>15</v>
       </c>
       <c r="J109" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L109" t="str">
         <f t="shared" si="3"/>
@@ -19903,7 +19941,7 @@
         <v>15</v>
       </c>
       <c r="J110" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L110" t="str">
         <f t="shared" si="3"/>
@@ -19937,7 +19975,7 @@
         <v>15</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L111" t="str">
         <f t="shared" si="3"/>
@@ -19971,7 +20009,7 @@
         <v>15</v>
       </c>
       <c r="J112" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L112" t="str">
         <f t="shared" si="3"/>
@@ -20005,7 +20043,7 @@
         <v>15</v>
       </c>
       <c r="J113" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L113" t="str">
         <f t="shared" si="3"/>
@@ -20039,7 +20077,7 @@
         <v>15</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L114" t="str">
         <f t="shared" si="3"/>
@@ -20074,7 +20112,7 @@
         <v>15</v>
       </c>
       <c r="J115" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K115" s="2"/>
       <c r="L115" t="str">
@@ -20134,7 +20172,7 @@
         <v>15</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L116" t="str">
         <f t="shared" si="3"/>
@@ -20168,7 +20206,7 @@
         <v>15</v>
       </c>
       <c r="J117" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L117" t="str">
         <f t="shared" si="3"/>
@@ -20202,7 +20240,7 @@
         <v>15</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L118" t="str">
         <f t="shared" si="3"/>
@@ -20236,7 +20274,7 @@
         <v>15</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L119" t="str">
         <f t="shared" si="3"/>
@@ -20270,7 +20308,7 @@
         <v>15</v>
       </c>
       <c r="J120" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L120" t="str">
         <f t="shared" si="3"/>
@@ -20305,7 +20343,7 @@
         <v>15</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K121" s="4" t="s">
         <v>133</v>
@@ -20342,7 +20380,7 @@
         <v>15</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K122" s="2" t="s">
         <v>556</v>
@@ -20379,7 +20417,7 @@
         <v>15</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K123" s="2" t="s">
         <v>211</v>
@@ -20416,7 +20454,7 @@
         <v>15</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L124" t="str">
         <f t="shared" si="3"/>
@@ -20450,7 +20488,7 @@
         <v>15</v>
       </c>
       <c r="J125" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L125" t="str">
         <f t="shared" si="3"/>
@@ -20518,7 +20556,7 @@
         <v>15</v>
       </c>
       <c r="J127" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L127" t="str">
         <f t="shared" si="3"/>
@@ -20552,7 +20590,7 @@
         <v>15</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L128" t="str">
         <f t="shared" si="3"/>
@@ -20586,7 +20624,7 @@
         <v>15</v>
       </c>
       <c r="J129" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L129" t="str">
         <f t="shared" si="3"/>
@@ -20614,7 +20652,7 @@
         <v>15</v>
       </c>
       <c r="J130" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L130" t="str">
         <f t="shared" si="3"/>
@@ -20648,7 +20686,7 @@
         <v>15</v>
       </c>
       <c r="J131" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L131" t="str">
         <f t="shared" si="3"/>
@@ -20676,7 +20714,7 @@
         <v>15</v>
       </c>
       <c r="J132" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L132" t="str">
         <f t="shared" ref="L132:L195" si="5">CONCATENATE("u",C132,"-",E132,".svg")</f>
@@ -20710,7 +20748,7 @@
         <v>15</v>
       </c>
       <c r="J133" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L133" t="str">
         <f t="shared" si="5"/>
@@ -20738,7 +20776,7 @@
         <v>15</v>
       </c>
       <c r="J134" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L134" t="str">
         <f t="shared" si="5"/>
@@ -20766,7 +20804,7 @@
         <v>15</v>
       </c>
       <c r="J135" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L135" t="str">
         <f t="shared" si="5"/>
@@ -20794,7 +20832,7 @@
         <v>15</v>
       </c>
       <c r="J136" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L136" t="str">
         <f t="shared" si="5"/>
@@ -20828,7 +20866,7 @@
         <v>15</v>
       </c>
       <c r="J137" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L137" t="str">
         <f t="shared" si="5"/>
@@ -20862,7 +20900,7 @@
         <v>15</v>
       </c>
       <c r="J138" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L138" t="str">
         <f t="shared" si="5"/>
@@ -20896,7 +20934,7 @@
         <v>15</v>
       </c>
       <c r="J139" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L139" t="str">
         <f t="shared" si="5"/>
@@ -20930,7 +20968,7 @@
         <v>15</v>
       </c>
       <c r="J140" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L140" t="str">
         <f t="shared" si="5"/>
@@ -20965,7 +21003,7 @@
         <v>15</v>
       </c>
       <c r="J141" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K141" s="2"/>
       <c r="L141" t="str">
@@ -21025,7 +21063,7 @@
         <v>15</v>
       </c>
       <c r="J142" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L142" t="str">
         <f t="shared" si="5"/>
@@ -21059,7 +21097,7 @@
         <v>15</v>
       </c>
       <c r="J143" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L143" t="str">
         <f t="shared" si="5"/>
@@ -21094,7 +21132,7 @@
         <v>15</v>
       </c>
       <c r="J144" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K144" s="2"/>
       <c r="L144" t="str">
@@ -21155,7 +21193,7 @@
         <v>15</v>
       </c>
       <c r="J145" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K145" s="2"/>
       <c r="L145" t="str">
@@ -21215,7 +21253,7 @@
         <v>15</v>
       </c>
       <c r="J146" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L146" t="str">
         <f t="shared" si="5"/>
@@ -21246,7 +21284,7 @@
         <v>15</v>
       </c>
       <c r="J147" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L147" t="str">
         <f t="shared" si="5"/>
@@ -21280,7 +21318,7 @@
         <v>15</v>
       </c>
       <c r="J148" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L148" t="str">
         <f t="shared" si="5"/>
@@ -21308,7 +21346,7 @@
         <v>15</v>
       </c>
       <c r="J149" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L149" t="str">
         <f t="shared" si="5"/>
@@ -21342,7 +21380,7 @@
         <v>15</v>
       </c>
       <c r="J150" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L150" t="str">
         <f t="shared" si="5"/>
@@ -21376,7 +21414,7 @@
         <v>15</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L151" t="str">
         <f t="shared" si="5"/>
@@ -21410,7 +21448,7 @@
         <v>15</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L152" t="str">
         <f t="shared" si="5"/>
@@ -21438,7 +21476,7 @@
         <v>15</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L153" t="str">
         <f t="shared" si="5"/>
@@ -21466,7 +21504,7 @@
         <v>15</v>
       </c>
       <c r="J154" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L154" t="str">
         <f t="shared" si="5"/>
@@ -21494,7 +21532,7 @@
         <v>15</v>
       </c>
       <c r="J155" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L155" t="str">
         <f t="shared" si="5"/>
@@ -21522,7 +21560,7 @@
         <v>15</v>
       </c>
       <c r="J156" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L156" t="str">
         <f t="shared" si="5"/>
@@ -21550,7 +21588,7 @@
         <v>15</v>
       </c>
       <c r="J157" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L157" t="str">
         <f t="shared" si="5"/>
@@ -21578,7 +21616,7 @@
         <v>15</v>
       </c>
       <c r="J158" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L158" t="str">
         <f t="shared" si="5"/>
@@ -21606,7 +21644,7 @@
         <v>15</v>
       </c>
       <c r="J159" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L159" t="str">
         <f t="shared" si="5"/>
@@ -21634,7 +21672,7 @@
         <v>15</v>
       </c>
       <c r="J160" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L160" t="str">
         <f t="shared" si="5"/>
@@ -21662,7 +21700,7 @@
         <v>15</v>
       </c>
       <c r="J161" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L161" t="str">
         <f t="shared" si="5"/>
@@ -21696,7 +21734,7 @@
         <v>15</v>
       </c>
       <c r="J162" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K162" s="2" t="s">
         <v>226</v>
@@ -21733,7 +21771,7 @@
         <v>15</v>
       </c>
       <c r="J163" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K163" s="2" t="s">
         <v>213</v>
@@ -21770,7 +21808,7 @@
         <v>15</v>
       </c>
       <c r="J164" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K164" s="2" t="s">
         <v>212</v>
@@ -21807,7 +21845,7 @@
         <v>15</v>
       </c>
       <c r="J165" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K165" s="2" t="s">
         <v>217</v>
@@ -21844,7 +21882,7 @@
         <v>15</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K166" s="2" t="s">
         <v>217</v>
@@ -21881,7 +21919,7 @@
         <v>15</v>
       </c>
       <c r="J167" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K167" s="2" t="s">
         <v>217</v>
@@ -21918,7 +21956,7 @@
         <v>15</v>
       </c>
       <c r="J168" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K168" s="2" t="s">
         <v>217</v>
@@ -21955,7 +21993,7 @@
         <v>15</v>
       </c>
       <c r="J169" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K169" s="2" t="s">
         <v>219</v>
@@ -21992,7 +22030,7 @@
         <v>15</v>
       </c>
       <c r="J170" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K170" s="2" t="s">
         <v>218</v>
@@ -22029,7 +22067,7 @@
         <v>15</v>
       </c>
       <c r="J171" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K171" s="2" t="s">
         <v>216</v>
@@ -22066,7 +22104,7 @@
         <v>15</v>
       </c>
       <c r="J172" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K172" s="2" t="s">
         <v>218</v>
@@ -22097,7 +22135,7 @@
         <v>15</v>
       </c>
       <c r="J173" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L173" t="str">
         <f t="shared" si="5"/>
@@ -22125,7 +22163,7 @@
         <v>15</v>
       </c>
       <c r="J174" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L174" t="str">
         <f t="shared" si="5"/>
@@ -22153,7 +22191,7 @@
         <v>15</v>
       </c>
       <c r="J175" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L175" t="str">
         <f t="shared" si="5"/>
@@ -22181,7 +22219,7 @@
         <v>15</v>
       </c>
       <c r="J176" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L176" t="str">
         <f t="shared" si="5"/>
@@ -22209,7 +22247,7 @@
         <v>15</v>
       </c>
       <c r="J177" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L177" t="str">
         <f t="shared" si="5"/>
@@ -22237,7 +22275,7 @@
         <v>15</v>
       </c>
       <c r="J178" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L178" t="str">
         <f t="shared" si="5"/>
@@ -22265,7 +22303,7 @@
         <v>15</v>
       </c>
       <c r="J179" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L179" t="str">
         <f t="shared" si="5"/>
@@ -22293,7 +22331,7 @@
         <v>15</v>
       </c>
       <c r="J180" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L180" t="str">
         <f t="shared" si="5"/>
@@ -22327,7 +22365,7 @@
         <v>15</v>
       </c>
       <c r="J181" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L181" t="str">
         <f t="shared" si="5"/>
@@ -22361,7 +22399,7 @@
         <v>15</v>
       </c>
       <c r="J182" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L182" t="str">
         <f t="shared" si="5"/>
@@ -22395,7 +22433,7 @@
         <v>15</v>
       </c>
       <c r="J183" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L183" t="str">
         <f t="shared" si="5"/>
@@ -22429,7 +22467,7 @@
         <v>15</v>
       </c>
       <c r="J184" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L184" t="str">
         <f t="shared" si="5"/>
@@ -22463,7 +22501,7 @@
         <v>15</v>
       </c>
       <c r="J185" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L185" t="str">
         <f t="shared" si="5"/>
@@ -22497,7 +22535,7 @@
         <v>15</v>
       </c>
       <c r="J186" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L186" t="str">
         <f t="shared" si="5"/>
@@ -22531,7 +22569,7 @@
         <v>15</v>
       </c>
       <c r="J187" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L187" t="str">
         <f t="shared" si="5"/>
@@ -22565,7 +22603,7 @@
         <v>15</v>
       </c>
       <c r="J188" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L188" t="str">
         <f t="shared" si="5"/>
@@ -22599,7 +22637,7 @@
         <v>15</v>
       </c>
       <c r="J189" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L189" t="str">
         <f t="shared" si="5"/>
@@ -22633,7 +22671,7 @@
         <v>15</v>
       </c>
       <c r="J190" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L190" t="str">
         <f t="shared" si="5"/>
@@ -22667,7 +22705,7 @@
         <v>15</v>
       </c>
       <c r="J191" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L191" t="str">
         <f t="shared" si="5"/>
@@ -22701,7 +22739,7 @@
         <v>15</v>
       </c>
       <c r="J192" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L192" t="str">
         <f t="shared" si="5"/>
@@ -22736,7 +22774,7 @@
         <v>15</v>
       </c>
       <c r="J193" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K193" s="2"/>
       <c r="L193" t="str">
@@ -22797,7 +22835,7 @@
         <v>15</v>
       </c>
       <c r="J194" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K194" s="2"/>
       <c r="L194" t="str">
@@ -22857,7 +22895,7 @@
         <v>15</v>
       </c>
       <c r="J195" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L195" t="str">
         <f t="shared" si="5"/>
@@ -22888,7 +22926,7 @@
         <v>15</v>
       </c>
       <c r="J196" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K196" s="2"/>
       <c r="L196" t="str">
@@ -22948,7 +22986,7 @@
         <v>15</v>
       </c>
       <c r="J197" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L197" t="str">
         <f t="shared" si="7"/>
@@ -22976,7 +23014,7 @@
         <v>15</v>
       </c>
       <c r="J198" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L198" t="str">
         <f t="shared" si="7"/>
@@ -23004,7 +23042,7 @@
         <v>15</v>
       </c>
       <c r="J199" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L199" t="str">
         <f t="shared" si="7"/>
@@ -23032,7 +23070,7 @@
         <v>15</v>
       </c>
       <c r="J200" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L200" t="str">
         <f t="shared" si="7"/>
@@ -23060,7 +23098,7 @@
         <v>15</v>
       </c>
       <c r="J201" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L201" t="str">
         <f t="shared" si="7"/>
@@ -23088,7 +23126,7 @@
         <v>15</v>
       </c>
       <c r="J202" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L202" t="str">
         <f t="shared" si="7"/>
@@ -23116,7 +23154,7 @@
         <v>15</v>
       </c>
       <c r="J203" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L203" t="str">
         <f t="shared" si="7"/>
@@ -23144,7 +23182,7 @@
         <v>15</v>
       </c>
       <c r="J204" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L204" t="str">
         <f t="shared" si="7"/>
@@ -23172,7 +23210,7 @@
         <v>15</v>
       </c>
       <c r="J205" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L205" t="str">
         <f t="shared" si="7"/>
@@ -23200,7 +23238,7 @@
         <v>15</v>
       </c>
       <c r="J206" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L206" t="str">
         <f t="shared" si="7"/>
@@ -23228,7 +23266,7 @@
         <v>15</v>
       </c>
       <c r="J207" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L207" t="str">
         <f t="shared" si="7"/>
@@ -23256,7 +23294,7 @@
         <v>15</v>
       </c>
       <c r="J208" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L208" t="str">
         <f t="shared" si="7"/>
@@ -23284,7 +23322,7 @@
         <v>15</v>
       </c>
       <c r="J209" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L209" t="str">
         <f t="shared" si="7"/>
@@ -23312,7 +23350,7 @@
         <v>15</v>
       </c>
       <c r="J210" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L210" t="str">
         <f t="shared" si="7"/>
@@ -23346,7 +23384,7 @@
         <v>15</v>
       </c>
       <c r="J211" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L211" t="str">
         <f t="shared" si="7"/>
@@ -23374,7 +23412,7 @@
         <v>15</v>
       </c>
       <c r="J212" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L212" t="str">
         <f t="shared" si="7"/>
@@ -23402,7 +23440,7 @@
         <v>15</v>
       </c>
       <c r="J213" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L213" t="str">
         <f t="shared" si="7"/>
@@ -23436,7 +23474,7 @@
         <v>15</v>
       </c>
       <c r="J214" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L214" t="str">
         <f t="shared" si="7"/>
@@ -23470,7 +23508,7 @@
         <v>15</v>
       </c>
       <c r="J215" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L215" t="str">
         <f t="shared" si="7"/>
@@ -23504,7 +23542,7 @@
         <v>15</v>
       </c>
       <c r="J216" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L216" t="str">
         <f t="shared" si="7"/>
@@ -23538,7 +23576,7 @@
         <v>15</v>
       </c>
       <c r="J217" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L217" t="str">
         <f t="shared" si="7"/>
@@ -23572,7 +23610,7 @@
         <v>15</v>
       </c>
       <c r="J218" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L218" t="str">
         <f t="shared" si="7"/>
@@ -23606,7 +23644,7 @@
         <v>15</v>
       </c>
       <c r="J219" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L219" t="str">
         <f t="shared" si="7"/>
@@ -23640,7 +23678,7 @@
         <v>15</v>
       </c>
       <c r="J220" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L220" t="str">
         <f t="shared" si="7"/>
@@ -23674,7 +23712,7 @@
         <v>15</v>
       </c>
       <c r="J221" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L221" t="str">
         <f t="shared" si="7"/>
@@ -23708,7 +23746,7 @@
         <v>15</v>
       </c>
       <c r="J222" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L222" t="str">
         <f t="shared" si="7"/>
@@ -23742,7 +23780,7 @@
         <v>15</v>
       </c>
       <c r="J223" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="L223" t="str">
         <f t="shared" si="7"/>
@@ -23776,7 +23814,7 @@
         <v>15</v>
       </c>
       <c r="J224" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L224" t="str">
         <f t="shared" si="7"/>
@@ -23804,7 +23842,7 @@
         <v>15</v>
       </c>
       <c r="J225" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L225" t="str">
         <f t="shared" si="7"/>
@@ -23838,7 +23876,7 @@
         <v>15</v>
       </c>
       <c r="J226" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L226" t="str">
         <f t="shared" si="7"/>
@@ -23872,7 +23910,7 @@
         <v>15</v>
       </c>
       <c r="J227" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L227" t="str">
         <f t="shared" si="7"/>
@@ -23906,7 +23944,7 @@
         <v>15</v>
       </c>
       <c r="J228" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L228" t="str">
         <f t="shared" si="7"/>
@@ -23940,7 +23978,7 @@
         <v>15</v>
       </c>
       <c r="J229" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L229" t="str">
         <f t="shared" si="7"/>
@@ -23974,7 +24012,7 @@
         <v>15</v>
       </c>
       <c r="J230" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L230" t="str">
         <f t="shared" si="7"/>
@@ -24008,7 +24046,7 @@
         <v>15</v>
       </c>
       <c r="J231" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L231" t="str">
         <f t="shared" si="7"/>
@@ -24043,7 +24081,7 @@
         <v>15</v>
       </c>
       <c r="J232" s="4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="K232" s="4" t="s">
         <v>557</v>
@@ -24081,7 +24119,7 @@
         <v>15</v>
       </c>
       <c r="J233" s="4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="K233" s="4" t="s">
         <v>558</v>
@@ -24112,7 +24150,7 @@
         <v>15</v>
       </c>
       <c r="J234" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L234" t="str">
         <f t="shared" si="7"/>
@@ -24140,7 +24178,7 @@
         <v>15</v>
       </c>
       <c r="J235" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L235" t="str">
         <f t="shared" si="7"/>
@@ -24168,7 +24206,7 @@
         <v>15</v>
       </c>
       <c r="J236" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L236" t="str">
         <f t="shared" si="7"/>
@@ -24196,7 +24234,7 @@
         <v>15</v>
       </c>
       <c r="J237" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L237" t="str">
         <f t="shared" si="7"/>
@@ -24224,7 +24262,7 @@
         <v>15</v>
       </c>
       <c r="J238" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L238" t="str">
         <f t="shared" si="7"/>
@@ -24252,7 +24290,7 @@
         <v>15</v>
       </c>
       <c r="J239" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L239" t="str">
         <f t="shared" si="7"/>
@@ -24280,7 +24318,7 @@
         <v>15</v>
       </c>
       <c r="J240" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L240" t="str">
         <f t="shared" si="7"/>
@@ -24308,7 +24346,7 @@
         <v>15</v>
       </c>
       <c r="J241" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L241" t="str">
         <f t="shared" si="7"/>
@@ -24336,7 +24374,7 @@
         <v>15</v>
       </c>
       <c r="J242" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L242" t="str">
         <f t="shared" si="7"/>
@@ -24364,7 +24402,7 @@
         <v>15</v>
       </c>
       <c r="J243" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L243" t="str">
         <f t="shared" si="7"/>
@@ -24392,7 +24430,7 @@
         <v>15</v>
       </c>
       <c r="J244" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L244" t="str">
         <f t="shared" si="7"/>
@@ -24420,7 +24458,7 @@
         <v>15</v>
       </c>
       <c r="J245" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L245" t="str">
         <f t="shared" si="7"/>
@@ -24448,7 +24486,7 @@
         <v>15</v>
       </c>
       <c r="J246" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L246" t="str">
         <f t="shared" si="7"/>
@@ -24476,7 +24514,7 @@
         <v>15</v>
       </c>
       <c r="J247" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L247" t="str">
         <f t="shared" si="7"/>
@@ -24504,7 +24542,7 @@
         <v>15</v>
       </c>
       <c r="J248" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L248" t="str">
         <f t="shared" si="7"/>
@@ -24532,7 +24570,7 @@
         <v>15</v>
       </c>
       <c r="J249" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L249" t="str">
         <f t="shared" si="7"/>
@@ -24560,7 +24598,7 @@
         <v>15</v>
       </c>
       <c r="J250" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L250" t="str">
         <f t="shared" si="7"/>
@@ -24588,7 +24626,7 @@
         <v>15</v>
       </c>
       <c r="J251" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L251" t="str">
         <f t="shared" si="7"/>
@@ -24622,7 +24660,7 @@
         <v>15</v>
       </c>
       <c r="J252" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L252" t="str">
         <f t="shared" si="7"/>
@@ -24656,7 +24694,7 @@
         <v>15</v>
       </c>
       <c r="J253" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="K253" s="2" t="s">
         <v>136</v>
@@ -24693,7 +24731,7 @@
         <v>15</v>
       </c>
       <c r="J254" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L254" t="str">
         <f t="shared" si="7"/>
@@ -24727,7 +24765,7 @@
         <v>15</v>
       </c>
       <c r="J255" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L255" t="str">
         <f t="shared" si="7"/>
@@ -24761,7 +24799,7 @@
         <v>15</v>
       </c>
       <c r="J256" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L256" t="str">
         <f t="shared" si="7"/>
@@ -24795,7 +24833,7 @@
         <v>15</v>
       </c>
       <c r="J257" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L257" t="str">
         <f t="shared" si="7"/>
@@ -24829,7 +24867,7 @@
         <v>15</v>
       </c>
       <c r="J258" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L258" t="str">
         <f t="shared" si="7"/>
@@ -24863,7 +24901,7 @@
         <v>15</v>
       </c>
       <c r="J259" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L259" t="str">
         <f t="shared" si="7"/>
@@ -24897,7 +24935,7 @@
         <v>15</v>
       </c>
       <c r="J260" s="4" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="K260" s="4" t="s">
         <v>133</v>
@@ -24959,7 +24997,7 @@
         <v>15</v>
       </c>
       <c r="J261" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L261" t="str">
         <f t="shared" si="9"/>
@@ -24993,7 +25031,7 @@
         <v>15</v>
       </c>
       <c r="J262" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L262" t="str">
         <f t="shared" si="9"/>
@@ -25027,7 +25065,7 @@
         <v>15</v>
       </c>
       <c r="J263" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L263" t="str">
         <f t="shared" si="9"/>
@@ -25061,7 +25099,7 @@
         <v>15</v>
       </c>
       <c r="J264" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L264" t="str">
         <f t="shared" si="9"/>
@@ -25092,7 +25130,7 @@
         <v>15</v>
       </c>
       <c r="J265" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L265" t="str">
         <f t="shared" si="9"/>
@@ -25123,7 +25161,7 @@
         <v>15</v>
       </c>
       <c r="J266" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L266" t="str">
         <f t="shared" si="9"/>
@@ -25154,7 +25192,7 @@
         <v>15</v>
       </c>
       <c r="J267" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L267" t="str">
         <f t="shared" si="9"/>
@@ -25185,7 +25223,7 @@
         <v>15</v>
       </c>
       <c r="J268" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L268" t="str">
         <f t="shared" si="9"/>
@@ -25213,7 +25251,7 @@
         <v>15</v>
       </c>
       <c r="J269" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L269" t="str">
         <f t="shared" si="9"/>
@@ -25241,7 +25279,7 @@
         <v>15</v>
       </c>
       <c r="J270" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L270" t="str">
         <f t="shared" si="9"/>
@@ -25269,7 +25307,7 @@
         <v>15</v>
       </c>
       <c r="J271" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L271" t="str">
         <f t="shared" si="9"/>
@@ -25297,7 +25335,7 @@
         <v>15</v>
       </c>
       <c r="J272" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L272" t="str">
         <f t="shared" si="9"/>
@@ -25325,7 +25363,7 @@
         <v>15</v>
       </c>
       <c r="J273" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L273" t="str">
         <f t="shared" si="9"/>
@@ -25353,7 +25391,7 @@
         <v>15</v>
       </c>
       <c r="J274" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L274" t="str">
         <f t="shared" si="9"/>
@@ -25381,7 +25419,7 @@
         <v>15</v>
       </c>
       <c r="J275" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L275" t="str">
         <f t="shared" si="9"/>
@@ -25409,7 +25447,7 @@
         <v>15</v>
       </c>
       <c r="J276" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L276" t="str">
         <f t="shared" si="9"/>
@@ -25437,7 +25475,7 @@
         <v>15</v>
       </c>
       <c r="J277" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L277" t="str">
         <f t="shared" si="9"/>
@@ -25465,7 +25503,7 @@
         <v>15</v>
       </c>
       <c r="J278" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L278" t="str">
         <f t="shared" si="9"/>
@@ -25493,7 +25531,7 @@
         <v>15</v>
       </c>
       <c r="J279" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L279" t="str">
         <f t="shared" si="9"/>
@@ -25521,7 +25559,7 @@
         <v>15</v>
       </c>
       <c r="J280" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L280" t="str">
         <f t="shared" si="9"/>
@@ -25549,7 +25587,7 @@
         <v>15</v>
       </c>
       <c r="J281" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L281" t="str">
         <f t="shared" si="9"/>
@@ -25577,7 +25615,7 @@
         <v>15</v>
       </c>
       <c r="J282" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L282" t="str">
         <f t="shared" si="9"/>
@@ -25605,7 +25643,7 @@
         <v>15</v>
       </c>
       <c r="J283" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L283" t="str">
         <f t="shared" si="9"/>
@@ -25633,7 +25671,7 @@
         <v>15</v>
       </c>
       <c r="J284" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L284" t="str">
         <f t="shared" si="9"/>
@@ -25661,7 +25699,7 @@
         <v>15</v>
       </c>
       <c r="J285" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L285" t="str">
         <f t="shared" si="9"/>
@@ -25689,7 +25727,7 @@
         <v>15</v>
       </c>
       <c r="J286" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L286" t="str">
         <f t="shared" si="9"/>
@@ -25717,7 +25755,7 @@
         <v>15</v>
       </c>
       <c r="J287" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L287" t="str">
         <f t="shared" si="9"/>
@@ -25745,7 +25783,7 @@
         <v>15</v>
       </c>
       <c r="J288" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L288" t="str">
         <f t="shared" si="9"/>
@@ -25773,7 +25811,7 @@
         <v>15</v>
       </c>
       <c r="J289" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L289" t="str">
         <f t="shared" si="9"/>
@@ -25801,7 +25839,7 @@
         <v>15</v>
       </c>
       <c r="J290" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L290" t="str">
         <f t="shared" si="9"/>
@@ -25829,7 +25867,7 @@
         <v>15</v>
       </c>
       <c r="J291" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L291" t="str">
         <f t="shared" si="9"/>
@@ -25857,7 +25895,7 @@
         <v>15</v>
       </c>
       <c r="J292" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L292" t="str">
         <f t="shared" si="9"/>
@@ -25885,7 +25923,7 @@
         <v>15</v>
       </c>
       <c r="J293" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L293" t="str">
         <f t="shared" si="9"/>
@@ -25913,7 +25951,7 @@
         <v>15</v>
       </c>
       <c r="J294" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L294" t="str">
         <f t="shared" si="9"/>
@@ -25941,7 +25979,7 @@
         <v>15</v>
       </c>
       <c r="J295" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L295" t="str">
         <f t="shared" si="9"/>
@@ -25969,7 +26007,7 @@
         <v>15</v>
       </c>
       <c r="J296" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L296" t="str">
         <f t="shared" si="9"/>
@@ -25997,7 +26035,7 @@
         <v>15</v>
       </c>
       <c r="J297" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L297" t="str">
         <f t="shared" si="9"/>
@@ -26025,7 +26063,7 @@
         <v>15</v>
       </c>
       <c r="J298" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L298" t="str">
         <f t="shared" si="9"/>
@@ -26053,7 +26091,7 @@
         <v>15</v>
       </c>
       <c r="J299" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L299" t="str">
         <f t="shared" si="9"/>
@@ -26087,7 +26125,7 @@
         <v>15</v>
       </c>
       <c r="J300" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L300" t="str">
         <f t="shared" si="9"/>
@@ -26121,7 +26159,7 @@
         <v>15</v>
       </c>
       <c r="J301" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L301" t="str">
         <f t="shared" si="9"/>
@@ -26155,7 +26193,7 @@
         <v>15</v>
       </c>
       <c r="J302" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L302" t="str">
         <f t="shared" si="9"/>
@@ -26189,7 +26227,7 @@
         <v>15</v>
       </c>
       <c r="J303" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L303" t="str">
         <f t="shared" si="9"/>
@@ -26223,7 +26261,7 @@
         <v>15</v>
       </c>
       <c r="J304" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L304" t="str">
         <f t="shared" si="9"/>
@@ -26257,7 +26295,7 @@
         <v>15</v>
       </c>
       <c r="J305" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L305" t="str">
         <f t="shared" si="9"/>
@@ -26291,7 +26329,7 @@
         <v>15</v>
       </c>
       <c r="J306" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L306" t="str">
         <f t="shared" si="9"/>
@@ -26325,7 +26363,7 @@
         <v>15</v>
       </c>
       <c r="J307" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L307" t="str">
         <f t="shared" si="9"/>
@@ -26353,7 +26391,7 @@
         <v>15</v>
       </c>
       <c r="J308" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L308" t="str">
         <f t="shared" si="9"/>
@@ -26387,7 +26425,7 @@
         <v>15</v>
       </c>
       <c r="J309" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L309" t="str">
         <f t="shared" si="9"/>
@@ -26415,7 +26453,7 @@
         <v>15</v>
       </c>
       <c r="J310" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L310" t="str">
         <f t="shared" si="9"/>
@@ -26449,7 +26487,7 @@
         <v>15</v>
       </c>
       <c r="J311" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L311" t="str">
         <f t="shared" si="9"/>
@@ -26477,7 +26515,7 @@
         <v>15</v>
       </c>
       <c r="J312" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L312" t="str">
         <f t="shared" si="9"/>
@@ -26505,7 +26543,7 @@
         <v>15</v>
       </c>
       <c r="J313" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L313" t="str">
         <f t="shared" si="9"/>
@@ -26533,7 +26571,7 @@
         <v>15</v>
       </c>
       <c r="J314" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L314" t="str">
         <f t="shared" si="9"/>
@@ -26561,7 +26599,7 @@
         <v>15</v>
       </c>
       <c r="J315" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L315" t="str">
         <f t="shared" si="9"/>
@@ -26589,7 +26627,7 @@
         <v>15</v>
       </c>
       <c r="J316" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L316" t="str">
         <f t="shared" si="9"/>
@@ -26617,7 +26655,7 @@
         <v>15</v>
       </c>
       <c r="J317" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L317" t="str">
         <f t="shared" si="9"/>
@@ -26645,7 +26683,7 @@
         <v>15</v>
       </c>
       <c r="J318" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L318" t="str">
         <f t="shared" si="9"/>
@@ -26673,7 +26711,7 @@
         <v>15</v>
       </c>
       <c r="J319" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L319" t="str">
         <f t="shared" si="9"/>
@@ -26701,7 +26739,7 @@
         <v>15</v>
       </c>
       <c r="J320" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L320" t="str">
         <f t="shared" si="9"/>
@@ -26735,7 +26773,7 @@
         <v>15</v>
       </c>
       <c r="J321" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L321" t="str">
         <f t="shared" si="9"/>
@@ -26763,7 +26801,7 @@
         <v>15</v>
       </c>
       <c r="J322" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L322" t="str">
         <f t="shared" si="9"/>
@@ -26791,7 +26829,7 @@
         <v>15</v>
       </c>
       <c r="J323" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L323" t="str">
         <f t="shared" si="9"/>
@@ -26819,7 +26857,7 @@
         <v>15</v>
       </c>
       <c r="J324" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L324" t="str">
         <f t="shared" ref="L324:L357" si="11">CONCATENATE("u",C324,"-",E324,".svg")</f>
@@ -26847,7 +26885,7 @@
         <v>15</v>
       </c>
       <c r="J325" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L325" t="str">
         <f t="shared" si="11"/>
@@ -26875,7 +26913,7 @@
         <v>15</v>
       </c>
       <c r="J326" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L326" t="str">
         <f t="shared" si="11"/>
@@ -26903,7 +26941,7 @@
         <v>15</v>
       </c>
       <c r="J327" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L327" t="str">
         <f t="shared" si="11"/>
@@ -26931,7 +26969,7 @@
         <v>15</v>
       </c>
       <c r="J328" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L328" t="str">
         <f t="shared" si="11"/>
@@ -26959,7 +26997,7 @@
         <v>15</v>
       </c>
       <c r="J329" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L329" t="str">
         <f t="shared" si="11"/>
@@ -26993,7 +27031,7 @@
         <v>15</v>
       </c>
       <c r="J330" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="K330" s="2" t="s">
         <v>192</v>
@@ -27030,7 +27068,7 @@
         <v>15</v>
       </c>
       <c r="J331" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L331" t="str">
         <f t="shared" si="11"/>
@@ -27065,10 +27103,10 @@
         <v>15</v>
       </c>
       <c r="J332" s="4" t="s">
-        <v>618</v>
+        <v>655</v>
       </c>
       <c r="K332" s="4" t="s">
-        <v>559</v>
+        <v>656</v>
       </c>
       <c r="L332" t="str">
         <f t="shared" si="11"/>
@@ -27103,10 +27141,10 @@
         <v>15</v>
       </c>
       <c r="J333" s="4" t="s">
-        <v>618</v>
+        <v>655</v>
       </c>
       <c r="K333" s="4" t="s">
-        <v>560</v>
+        <v>656</v>
       </c>
       <c r="L333" t="str">
         <f t="shared" si="11"/>
@@ -27125,7 +27163,7 @@
         <v>59979</v>
       </c>
       <c r="E334" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F334" s="3">
         <v>1.1000000000000001</v>
@@ -27134,16 +27172,16 @@
         <v>17</v>
       </c>
       <c r="H334" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="I334" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J334" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K334" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="L334" t="str">
         <f t="shared" si="11"/>
@@ -27162,7 +27200,7 @@
         <v>59980</v>
       </c>
       <c r="E335" s="2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F335" s="3">
         <v>1.1000000000000001</v>
@@ -27171,16 +27209,16 @@
         <v>17</v>
       </c>
       <c r="H335" s="2" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="I335" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J335" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="K335" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="L335" t="str">
         <f t="shared" si="11"/>
@@ -27199,7 +27237,7 @@
         <v>59981</v>
       </c>
       <c r="E336" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F336" s="3">
         <v>1.1000000000000001</v>
@@ -27208,16 +27246,16 @@
         <v>17</v>
       </c>
       <c r="H336" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="I336" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J336" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="K336" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="L336" t="str">
         <f t="shared" si="11"/>
@@ -27236,7 +27274,7 @@
         <v>59982</v>
       </c>
       <c r="E337" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F337" s="3">
         <v>1.1000000000000001</v>
@@ -27245,16 +27283,16 @@
         <v>17</v>
       </c>
       <c r="H337" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="I337" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J337" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K337" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="L337" t="str">
         <f t="shared" si="11"/>
@@ -27273,7 +27311,7 @@
         <v>59983</v>
       </c>
       <c r="E338" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F338" s="3">
         <v>1.1000000000000001</v>
@@ -27282,16 +27320,16 @@
         <v>17</v>
       </c>
       <c r="H338" s="2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="I338" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J338" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="K338" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="L338" t="str">
         <f t="shared" si="11"/>
@@ -27310,7 +27348,7 @@
         <v>59984</v>
       </c>
       <c r="E339" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="F339" s="17">
         <v>1.1000000000000001</v>
@@ -27319,16 +27357,16 @@
         <v>16</v>
       </c>
       <c r="H339" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="I339" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J339" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="K339" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="L339" s="15" t="str">
         <f>CONCATENATE("u",C339,"-",E339,".svg")</f>
@@ -27373,7 +27411,7 @@
         <v>59985</v>
       </c>
       <c r="E340" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F340">
         <v>1.1000000000000001</v>
@@ -27382,16 +27420,16 @@
         <v>17</v>
       </c>
       <c r="H340" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="I340" t="s">
         <v>15</v>
       </c>
       <c r="J340" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="K340" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="L340" t="str">
         <f t="shared" si="11"/>
@@ -27410,7 +27448,7 @@
         <v>59986</v>
       </c>
       <c r="E341" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F341" s="3">
         <v>1.1000000000000001</v>
@@ -27419,16 +27457,16 @@
         <v>17</v>
       </c>
       <c r="H341" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="I341" t="s">
         <v>15</v>
       </c>
       <c r="J341" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="K341" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="L341" t="str">
         <f t="shared" si="11"/>
@@ -27447,7 +27485,7 @@
         <v>59987</v>
       </c>
       <c r="E342" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F342">
         <v>1.1000000000000001</v>
@@ -27456,16 +27494,16 @@
         <v>16</v>
       </c>
       <c r="H342" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="I342" t="s">
         <v>15</v>
       </c>
       <c r="J342" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="K342" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="L342" t="str">
         <f t="shared" si="11"/>
@@ -27484,7 +27522,7 @@
         <v>59988</v>
       </c>
       <c r="E343" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F343" s="3">
         <v>1.1000000000000001</v>
@@ -27493,16 +27531,16 @@
         <v>16</v>
       </c>
       <c r="H343" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="I343" t="s">
         <v>15</v>
       </c>
       <c r="J343" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="K343" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L343" t="str">
         <f t="shared" si="11"/>
@@ -27521,7 +27559,7 @@
         <v>59989</v>
       </c>
       <c r="E344" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F344">
         <v>1.1000000000000001</v>
@@ -27530,16 +27568,16 @@
         <v>16</v>
       </c>
       <c r="H344" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="I344" t="s">
         <v>15</v>
       </c>
       <c r="J344" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="K344" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L344" t="str">
         <f t="shared" si="11"/>
@@ -27558,7 +27596,7 @@
         <v>59990</v>
       </c>
       <c r="E345" s="2" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F345" s="3">
         <v>1.1000000000000001</v>
@@ -27567,16 +27605,16 @@
         <v>17</v>
       </c>
       <c r="H345" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="I345" t="s">
         <v>15</v>
       </c>
       <c r="J345" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="K345" s="2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L345" t="str">
         <f t="shared" si="11"/>
@@ -27595,7 +27633,7 @@
         <v>59991</v>
       </c>
       <c r="E346" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F346" s="3">
         <v>1.1000000000000001</v>
@@ -27604,16 +27642,16 @@
         <v>17</v>
       </c>
       <c r="H346" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="I346" t="s">
         <v>15</v>
       </c>
       <c r="J346" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="K346" s="2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L346" t="str">
         <f t="shared" si="11"/>
@@ -27632,7 +27670,7 @@
         <v>59992</v>
       </c>
       <c r="E347" s="2" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="F347" s="3">
         <v>1.1000000000000001</v>
@@ -27641,16 +27679,16 @@
         <v>17</v>
       </c>
       <c r="H347" s="2" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="I347" t="s">
         <v>15</v>
       </c>
       <c r="J347" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K347" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L347" t="str">
         <f t="shared" si="11"/>
@@ -27669,7 +27707,7 @@
         <v>59993</v>
       </c>
       <c r="E348" s="2" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="F348" s="3">
         <v>1.1000000000000001</v>
@@ -27678,16 +27716,16 @@
         <v>17</v>
       </c>
       <c r="H348" s="2" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="I348" t="s">
         <v>15</v>
       </c>
       <c r="J348" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K348" s="2" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="L348" t="str">
         <f t="shared" si="11"/>
@@ -27706,7 +27744,7 @@
         <v>59994</v>
       </c>
       <c r="E349" s="2" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="F349" s="3">
         <v>1.1000000000000001</v>
@@ -27715,16 +27753,16 @@
         <v>17</v>
       </c>
       <c r="H349" s="2" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="I349" t="s">
         <v>15</v>
       </c>
       <c r="J349" s="2" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="K349" s="2" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="L349" t="str">
         <f t="shared" si="11"/>
@@ -27743,7 +27781,7 @@
         <v>59995</v>
       </c>
       <c r="E350" s="2" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="F350" s="3">
         <v>1.1000000000000001</v>
@@ -27752,16 +27790,16 @@
         <v>17</v>
       </c>
       <c r="H350" s="2" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="I350" t="s">
         <v>15</v>
       </c>
       <c r="J350" s="2" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="K350" s="2" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="L350" t="str">
         <f t="shared" si="11"/>
@@ -27780,7 +27818,7 @@
         <v>59996</v>
       </c>
       <c r="E351" s="2" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="F351" s="3">
         <v>1.1000000000000001</v>
@@ -27789,16 +27827,16 @@
         <v>17</v>
       </c>
       <c r="H351" s="2" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="I351" t="s">
         <v>15</v>
       </c>
       <c r="J351" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K351" s="2" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="L351" t="str">
         <f t="shared" si="11"/>
@@ -27817,7 +27855,7 @@
         <v>59997</v>
       </c>
       <c r="E352" s="2" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="F352" s="3">
         <v>1.1000000000000001</v>
@@ -27826,163 +27864,158 @@
         <v>17</v>
       </c>
       <c r="H352" s="2" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="I352" t="s">
         <v>15</v>
       </c>
       <c r="J352" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K352" s="2" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="L352" t="str">
         <f t="shared" si="11"/>
         <v>uEA5D-feedback-negative-outline.svg</v>
       </c>
     </row>
-    <row r="353" spans="1:38" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A353" s="1">
+    <row r="353" spans="1:38" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A353">
         <v>351</v>
       </c>
-      <c r="C353" s="16" t="str">
+      <c r="C353" t="str">
         <f t="shared" si="10"/>
         <v>EA5E</v>
       </c>
-      <c r="D353" s="16">
+      <c r="D353">
         <v>59998</v>
       </c>
-      <c r="E353" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="F353" s="17">
+      <c r="E353" t="s">
+        <v>648</v>
+      </c>
+      <c r="F353">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G353" s="1" t="s">
+      <c r="G353" t="s">
         <v>17</v>
       </c>
-      <c r="H353" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="I353" s="1" t="s">
+      <c r="H353" t="s">
+        <v>649</v>
+      </c>
+      <c r="I353" t="s">
         <v>15</v>
       </c>
-      <c r="J353" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="K353" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="L353" s="15" t="str">
+      <c r="J353" t="s">
+        <v>599</v>
+      </c>
+      <c r="K353" t="s">
+        <v>650</v>
+      </c>
+      <c r="L353" t="str">
         <f t="shared" si="11"/>
         <v>uEA5E-contact-card.svg</v>
       </c>
-      <c r="M353" s="15"/>
-      <c r="N353" s="15"/>
-      <c r="O353" s="15"/>
-      <c r="P353" s="15"/>
-      <c r="Q353" s="15"/>
-      <c r="R353" s="15"/>
-      <c r="S353" s="15"/>
-      <c r="T353" s="15"/>
-      <c r="U353" s="15"/>
-      <c r="V353" s="15"/>
-      <c r="W353" s="15"/>
-      <c r="X353" s="15"/>
-      <c r="Y353" s="15"/>
-      <c r="Z353" s="15"/>
-      <c r="AA353" s="15"/>
-      <c r="AB353" s="15"/>
-      <c r="AC353" s="15"/>
-      <c r="AD353" s="15"/>
-      <c r="AE353" s="15"/>
-      <c r="AF353" s="15"/>
-      <c r="AG353" s="15"/>
-      <c r="AH353" s="15"/>
-      <c r="AI353" s="15"/>
-      <c r="AJ353" s="15"/>
-      <c r="AK353" s="15"/>
-      <c r="AL353" s="15"/>
-    </row>
-    <row r="354" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A354" s="2">
+    </row>
+    <row r="354" spans="1:38" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A354" s="1">
         <v>352</v>
       </c>
-      <c r="C354" s="13" t="str">
+      <c r="C354" s="16" t="str">
         <f t="shared" si="10"/>
         <v>EA5F</v>
       </c>
-      <c r="D354" s="13">
+      <c r="D354" s="16">
         <v>59999</v>
       </c>
-      <c r="L354" t="str">
+      <c r="E354" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="F354" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G354" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H354" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="I354" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J354" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="K354" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="L354" s="15" t="str">
         <f t="shared" si="11"/>
-        <v>uEA5F-.svg</v>
-      </c>
-    </row>
-    <row r="355" spans="1:38" s="1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A355" s="1">
+        <v>uEA5F-triangle.svg</v>
+      </c>
+      <c r="M354" s="15"/>
+      <c r="N354" s="15"/>
+      <c r="O354" s="15"/>
+      <c r="P354" s="15"/>
+      <c r="Q354" s="15"/>
+      <c r="R354" s="15"/>
+      <c r="S354" s="15"/>
+      <c r="T354" s="15"/>
+      <c r="U354" s="15"/>
+      <c r="V354" s="15"/>
+      <c r="W354" s="15"/>
+      <c r="X354" s="15"/>
+      <c r="Y354" s="15"/>
+      <c r="Z354" s="15"/>
+      <c r="AA354" s="15"/>
+      <c r="AB354" s="15"/>
+      <c r="AC354" s="15"/>
+      <c r="AD354" s="15"/>
+      <c r="AE354" s="15"/>
+      <c r="AF354" s="15"/>
+      <c r="AG354" s="15"/>
+      <c r="AH354" s="15"/>
+      <c r="AI354" s="15"/>
+      <c r="AJ354" s="15"/>
+      <c r="AK354" s="15"/>
+      <c r="AL354" s="15"/>
+    </row>
+    <row r="355" spans="1:38" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A355">
         <v>353</v>
       </c>
-      <c r="C355" s="16" t="str">
+      <c r="C355" t="str">
         <f t="shared" si="10"/>
         <v>EA60</v>
       </c>
-      <c r="D355" s="16">
+      <c r="D355">
         <v>60000</v>
       </c>
-      <c r="E355" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="F355" s="17">
+      <c r="E355" t="s">
+        <v>651</v>
+      </c>
+      <c r="F355">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G355" s="1" t="s">
+      <c r="G355" t="s">
         <v>16</v>
       </c>
-      <c r="H355" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="I355" s="1" t="s">
+      <c r="H355" t="s">
+        <v>652</v>
+      </c>
+      <c r="I355" t="s">
         <v>15</v>
       </c>
-      <c r="J355" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="K355" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="L355" s="15" t="str">
+      <c r="J355" t="s">
+        <v>612</v>
+      </c>
+      <c r="K355" t="s">
+        <v>653</v>
+      </c>
+      <c r="L355" t="str">
         <f t="shared" si="11"/>
         <v>uEA60-brand-vsts.svg</v>
       </c>
-      <c r="M355" s="15"/>
-      <c r="N355" s="15"/>
-      <c r="O355" s="15"/>
-      <c r="P355" s="15"/>
-      <c r="Q355" s="15"/>
-      <c r="R355" s="15"/>
-      <c r="S355" s="15"/>
-      <c r="T355" s="15"/>
-      <c r="U355" s="15"/>
-      <c r="V355" s="15"/>
-      <c r="W355" s="15"/>
-      <c r="X355" s="15"/>
-      <c r="Y355" s="15"/>
-      <c r="Z355" s="15"/>
-      <c r="AA355" s="15"/>
-      <c r="AB355" s="15"/>
-      <c r="AC355" s="15"/>
-      <c r="AD355" s="15"/>
-      <c r="AE355" s="15"/>
-      <c r="AF355" s="15"/>
-      <c r="AG355" s="15"/>
-      <c r="AH355" s="15"/>
-      <c r="AI355" s="15"/>
-      <c r="AJ355" s="15"/>
-      <c r="AK355" s="15"/>
-      <c r="AL355" s="15"/>
     </row>
     <row r="356" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="2">
@@ -28547,8 +28580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="L354" sqref="L354"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45074,7 +45107,7 @@
         <v>VSTS</v>
       </c>
       <c r="H331" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="I331" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H332),"",'Bowtie v1.0 reorg'!H332)</f>
@@ -45082,15 +45115,15 @@
       </c>
       <c r="J331" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K332),"",'Bowtie v1.0 reorg'!K332)</f>
-        <v>check if it is same as record-fill</v>
+        <v>Used for stacking icons as background.</v>
       </c>
       <c r="K331" t="str">
         <f t="shared" si="12"/>
-        <v>{'id':330,'name':'dot','unicode':'EA49','decimal':59977,'version':'1.0','style':'bold','subset':'VSTS','group':'misc','keywords':['dot','circle'],'usage':'check if it is same as record-fill'}</v>
+        <v>{'id':330,'name':'dot','unicode':'EA49','decimal':59977,'version':'1.0','style':'bold','subset':'VSTS','group':'misc','keywords':['dot','circle'],'usage':'Used for stacking icons as background.'}</v>
       </c>
       <c r="L331" t="str">
         <f t="shared" si="13"/>
-        <v>{"id":330,"name":"dot","unicode":"EA49","decimal":59977,"version":"1.0","style":"bold","subset":"VSTS","group":"misc","keywords":["dot","circle"],"usage":"check if it is same as record-fill"}</v>
+        <v>{"id":330,"name":"dot","unicode":"EA49","decimal":59977,"version":"1.0","style":"bold","subset":"VSTS","group":"misc","keywords":["dot","circle"],"usage":"Used for stacking icons as background."}</v>
       </c>
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.25">
@@ -45123,7 +45156,7 @@
         <v>VSTS</v>
       </c>
       <c r="H332" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="I332" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H333),"",'Bowtie v1.0 reorg'!H333)</f>
@@ -45131,15 +45164,15 @@
       </c>
       <c r="J332" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K333),"",'Bowtie v1.0 reorg'!K333)</f>
-        <v>check if it is same as stop-fill</v>
+        <v>Used for stacking icons as background.</v>
       </c>
       <c r="K332" t="str">
         <f t="shared" si="12"/>
-        <v>{'id':331,'name':'square','unicode':'EA4A','decimal':59978,'version':'1.0','style':'bold','subset':'VSTS','group':'misc','keywords':['square'],'usage':'check if it is same as stop-fill'}</v>
+        <v>{'id':331,'name':'square','unicode':'EA4A','decimal':59978,'version':'1.0','style':'bold','subset':'VSTS','group':'misc','keywords':['square'],'usage':'Used for stacking icons as background.'}</v>
       </c>
       <c r="L332" t="str">
         <f t="shared" si="13"/>
-        <v>{"id":331,"name":"square","unicode":"EA4A","decimal":59978,"version":"1.0","style":"bold","subset":"VSTS","group":"misc","keywords":["square"],"usage":"check if it is same as stop-fill"}</v>
+        <v>{"id":331,"name":"square","unicode":"EA4A","decimal":59978,"version":"1.0","style":"bold","subset":"VSTS","group":"misc","keywords":["square"],"usage":"Used for stacking icons as background."}</v>
       </c>
     </row>
     <row r="333" spans="1:12" x14ac:dyDescent="0.25">
@@ -46147,9 +46180,9 @@
         <f>'Bowtie v1.0 reorg'!A354</f>
         <v>352</v>
       </c>
-      <c r="B353">
+      <c r="B353" t="str">
         <f>'Bowtie v1.0 reorg'!E354</f>
-        <v>0</v>
+        <v>triangle</v>
       </c>
       <c r="C353" t="str">
         <f>'Bowtie v1.0 reorg'!C354</f>
@@ -46159,37 +46192,37 @@
         <f>'Bowtie v1.0 reorg'!D354</f>
         <v>59999</v>
       </c>
-      <c r="E353" t="str">
+      <c r="E353">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F354),"",'Bowtie v1.0 reorg'!F354)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F353" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G354),"",'Bowtie v1.0 reorg'!G354)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G353" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I354),"",'Bowtie v1.0 reorg'!I354)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H353" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J354),"",'Bowtie v1.0 reorg'!J354)</f>
-        <v/>
+        <v>Utility</v>
       </c>
       <c r="I353" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H354),"",'Bowtie v1.0 reorg'!H354)</f>
-        <v/>
+        <v>triangle</v>
       </c>
       <c r="J353" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K354),"",'Bowtie v1.0 reorg'!K354)</f>
-        <v/>
-      </c>
-      <c r="K353" t="e">
+        <v>Used for stacking icons as background.</v>
+      </c>
+      <c r="K353" t="str">
         <f t="shared" ref="K353:K416" si="16">IF(NOT(ISBLANK(A353)),CONCATENATE("{'",$A$1,"':",A353,",'",$B$1,"':'",B353,"',","'",$C$1,"':'",C353,"','",$D$1,"':",D353,",'",$E$1,"':'",FIXED(E353,1),"','",$F$1,"':'",F353,"','",$G$1,"':'",G353,"','",$H$1,"':'",H353,"','",$I$1,"':['",SUBSTITUTE(I353," ","','"),"'],'",$J$1,"':'",J353,"'}"))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L353" t="e">
+        <v>{'id':352,'name':'triangle','unicode':'EA5F','decimal':59999,'version':'1.1','style':'bold','subset':'VSTS','group':'Utility','keywords':['triangle'],'usage':'Used for stacking icons as background.'}</v>
+      </c>
+      <c r="L353" t="str">
         <f t="shared" ref="L353:L416" si="17">SUBSTITUTE(K353,"'","""")</f>
-        <v>#VALUE!</v>
+        <v>{"id":352,"name":"triangle","unicode":"EA5F","decimal":59999,"version":"1.1","style":"bold","subset":"VSTS","group":"Utility","keywords":["triangle"],"usage":"Used for stacking icons as background."}</v>
       </c>
     </row>
     <row r="354" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added smaller version status icons for stacking; updated demo page guideline
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1660" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="688">
   <si>
     <t>name</t>
   </si>
@@ -1991,6 +1991,99 @@
   </si>
   <si>
     <t>Used for stacking icons as background.</t>
+  </si>
+  <si>
+    <t>status-success-sm</t>
+  </si>
+  <si>
+    <t>status-warning-sm</t>
+  </si>
+  <si>
+    <t>status-info-sm</t>
+  </si>
+  <si>
+    <t>status-failure-sm</t>
+  </si>
+  <si>
+    <t>status-error-sm</t>
+  </si>
+  <si>
+    <t>status-run-sm</t>
+  </si>
+  <si>
+    <t>status-help-sm</t>
+  </si>
+  <si>
+    <t>status-stop-sm</t>
+  </si>
+  <si>
+    <t>status-pause-sm</t>
+  </si>
+  <si>
+    <t>This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot.</t>
+  </si>
+  <si>
+    <t>This is a smaller version of bowtie-status-warning. It is used for stacking with bowtie-triangle.</t>
+  </si>
+  <si>
+    <t>This is a smaller version of bowtie-status-info. It is used for stacking with bowtie-dot.</t>
+  </si>
+  <si>
+    <t>This is a smaller version of bowtie-status-failure. It is used for stacking with bowtie-dot.</t>
+  </si>
+  <si>
+    <t>This is a smaller version of bowtie-status-error. It is used for stacking with bowtie-dot.</t>
+  </si>
+  <si>
+    <t>This is a smaller version of bowtie-status-run. It is used for stacking with bowtie-dot.</t>
+  </si>
+  <si>
+    <t>This is a smaller version of bowtie-status-help. It is used for stacking with bowtie-dot.</t>
+  </si>
+  <si>
+    <t>This is a smaller version of bowtie-status-stop. It is used for stacking with bowtie-dot.</t>
+  </si>
+  <si>
+    <t>status success complete ok pass positive good checkmark</t>
+  </si>
+  <si>
+    <t>status warning problem attention exclaimation</t>
+  </si>
+  <si>
+    <t>status information letter i</t>
+  </si>
+  <si>
+    <t>status failure negative critical problem fatal error</t>
+  </si>
+  <si>
+    <t>status run play execute in progress triangle</t>
+  </si>
+  <si>
+    <t>status help question</t>
+  </si>
+  <si>
+    <t>status stop square</t>
+  </si>
+  <si>
+    <t>status pause</t>
+  </si>
+  <si>
+    <t>status waiting clock time pending queue</t>
+  </si>
+  <si>
+    <t>status no block mute unavailable</t>
+  </si>
+  <si>
+    <t>status-waiting-fill-sm</t>
+  </si>
+  <si>
+    <t>This is a smaller version of bowtie-status-waiting-fill. It is used for stacking with bowtie-dot.</t>
+  </si>
+  <si>
+    <t>status-no-fill-sm</t>
+  </si>
+  <si>
+    <t>This is a smaller version of bowtie-status-no-fill. It is used for stacking with bowtie-dot.</t>
   </si>
 </sst>
 </file>
@@ -15551,6 +15644,424 @@
         <a:xfrm>
           <a:off x="1123950" y="141808200"/>
           <a:ext cx="209579" cy="209579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>355</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323877</xdr:colOff>
+      <xdr:row>355</xdr:row>
+      <xdr:rowOff>314352</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="355" name="Picture 354"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId354"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1076325" y="142627350"/>
+          <a:ext cx="190527" cy="190527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>356</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409607</xdr:colOff>
+      <xdr:row>356</xdr:row>
+      <xdr:rowOff>333404</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="357" name="Picture 356"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId355"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1123950" y="143027400"/>
+          <a:ext cx="228632" cy="209579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>357</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381027</xdr:colOff>
+      <xdr:row>357</xdr:row>
+      <xdr:rowOff>314350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="358" name="Picture 357"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId356"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="143436975"/>
+          <a:ext cx="190527" cy="181000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>358</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>371504</xdr:colOff>
+      <xdr:row>358</xdr:row>
+      <xdr:rowOff>323879</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="359" name="Picture 358"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId357"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="143817975"/>
+          <a:ext cx="209579" cy="209579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>359</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381029</xdr:colOff>
+      <xdr:row>359</xdr:row>
+      <xdr:rowOff>333404</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="360" name="Picture 359"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId358"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="144227550"/>
+          <a:ext cx="209579" cy="209579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>360</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381031</xdr:colOff>
+      <xdr:row>360</xdr:row>
+      <xdr:rowOff>352461</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="361" name="Picture 360"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId359"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="144599025"/>
+          <a:ext cx="219106" cy="257211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>361</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361982</xdr:colOff>
+      <xdr:row>361</xdr:row>
+      <xdr:rowOff>342935</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="362" name="Picture 361"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId360"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1076325" y="144999075"/>
+          <a:ext cx="228632" cy="247685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>362</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352452</xdr:colOff>
+      <xdr:row>362</xdr:row>
+      <xdr:rowOff>304827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="363" name="Picture 362"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId361"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="145418175"/>
+          <a:ext cx="190527" cy="190527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>363</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419135</xdr:colOff>
+      <xdr:row>363</xdr:row>
+      <xdr:rowOff>314358</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="364" name="Picture 363"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId362"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="145780125"/>
+          <a:ext cx="247685" cy="238158"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>364</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361981</xdr:colOff>
+      <xdr:row>364</xdr:row>
+      <xdr:rowOff>361982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="365" name="Picture 364"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId363"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1085850" y="146237325"/>
+          <a:ext cx="219106" cy="228632"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>365</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361977</xdr:colOff>
+      <xdr:row>365</xdr:row>
+      <xdr:rowOff>314350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="366" name="Picture 365"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId364"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="146637375"/>
+          <a:ext cx="190527" cy="181000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15828,8 +16339,8 @@
   <dimension ref="A1:AL410"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A351" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G358" sqref="G358"/>
+      <pane ySplit="2" topLeftCell="A358" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N364" sqref="N364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26860,7 +27371,7 @@
         <v>604</v>
       </c>
       <c r="L324" t="str">
-        <f t="shared" ref="L324:L357" si="11">CONCATENATE("u",C324,"-",E324,".svg")</f>
+        <f t="shared" ref="L324:L387" si="11">CONCATENATE("u",C324,"-",E324,".svg")</f>
         <v>uEA41-view-list-tree.svg</v>
       </c>
     </row>
@@ -28028,9 +28539,30 @@
       <c r="D356" s="13">
         <v>60001</v>
       </c>
+      <c r="E356" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="F356" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G356" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H356" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="I356" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J356" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K356" s="2" t="s">
+        <v>666</v>
+      </c>
       <c r="L356" t="str">
         <f t="shared" si="11"/>
-        <v>uEA61-.svg</v>
+        <v>uEA61-status-success-sm.svg</v>
       </c>
     </row>
     <row r="357" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -28044,9 +28576,30 @@
       <c r="D357" s="13">
         <v>60002</v>
       </c>
+      <c r="E357" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="F357">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G357" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H357" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="I357" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J357" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K357" s="2" t="s">
+        <v>667</v>
+      </c>
       <c r="L357" t="str">
         <f t="shared" si="11"/>
-        <v>uEA62-.svg</v>
+        <v>uEA62-status-warning-sm.svg</v>
       </c>
     </row>
     <row r="358" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -28060,6 +28613,31 @@
       <c r="D358" s="13">
         <v>60003</v>
       </c>
+      <c r="E358" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="F358" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G358" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H358" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="I358" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J358" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K358" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="L358" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA63-status-info-sm.svg</v>
+      </c>
     </row>
     <row r="359" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="2">
@@ -28072,6 +28650,31 @@
       <c r="D359" s="13">
         <v>60004</v>
       </c>
+      <c r="E359" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="F359">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G359" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H359" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="I359" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J359" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K359" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="L359" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA64-status-failure-sm.svg</v>
+      </c>
     </row>
     <row r="360" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="2">
@@ -28084,6 +28687,31 @@
       <c r="D360" s="13">
         <v>60005</v>
       </c>
+      <c r="E360" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="F360" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G360" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H360" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I360" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J360" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K360" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="L360" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA65-status-error-sm.svg</v>
+      </c>
     </row>
     <row r="361" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="2">
@@ -28096,6 +28724,31 @@
       <c r="D361" s="13">
         <v>60006</v>
       </c>
+      <c r="E361" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="F361">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G361" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H361" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="I361" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J361" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K361" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="L361" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA66-status-run-sm.svg</v>
+      </c>
     </row>
     <row r="362" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="2">
@@ -28108,6 +28761,31 @@
       <c r="D362" s="13">
         <v>60007</v>
       </c>
+      <c r="E362" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="F362" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G362" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H362" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="I362" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J362" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K362" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="L362" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA67-status-help-sm.svg</v>
+      </c>
     </row>
     <row r="363" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="2">
@@ -28120,6 +28798,31 @@
       <c r="D363" s="13">
         <v>60008</v>
       </c>
+      <c r="E363" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="F363">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G363" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H363" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="I363" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J363" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K363" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="L363" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA68-status-stop-sm.svg</v>
+      </c>
     </row>
     <row r="364" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="2">
@@ -28132,6 +28835,31 @@
       <c r="D364" s="13">
         <v>60009</v>
       </c>
+      <c r="E364" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="F364" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G364" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H364" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="I364" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J364" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K364" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="L364" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA69-status-pause-sm.svg</v>
+      </c>
     </row>
     <row r="365" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="2">
@@ -28144,6 +28872,31 @@
       <c r="D365" s="13">
         <v>60010</v>
       </c>
+      <c r="E365" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="F365">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G365" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H365" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="I365" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J365" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K365" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="L365" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA6A-status-waiting-fill-sm.svg</v>
+      </c>
     </row>
     <row r="366" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="2">
@@ -28156,6 +28909,31 @@
       <c r="D366" s="13">
         <v>60011</v>
       </c>
+      <c r="E366" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="F366" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G366" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H366" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="I366" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J366" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="K366" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="L366" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA6B-status-no-fill-sm.svg</v>
+      </c>
     </row>
     <row r="367" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="2">
@@ -28168,6 +28946,10 @@
       <c r="D367" s="13">
         <v>60012</v>
       </c>
+      <c r="L367" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA6C-.svg</v>
+      </c>
     </row>
     <row r="368" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="2">
@@ -28180,8 +28962,12 @@
       <c r="D368" s="13">
         <v>60013</v>
       </c>
-    </row>
-    <row r="369" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L368" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA6D-.svg</v>
+      </c>
+    </row>
+    <row r="369" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="2">
         <v>367</v>
       </c>
@@ -28192,8 +28978,12 @@
       <c r="D369" s="13">
         <v>60014</v>
       </c>
-    </row>
-    <row r="370" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L369" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA6E-.svg</v>
+      </c>
+    </row>
+    <row r="370" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="2">
         <v>368</v>
       </c>
@@ -28204,8 +28994,12 @@
       <c r="D370" s="13">
         <v>60015</v>
       </c>
-    </row>
-    <row r="371" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L370" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA6F-.svg</v>
+      </c>
+    </row>
+    <row r="371" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="2">
         <v>369</v>
       </c>
@@ -28216,8 +29010,12 @@
       <c r="D371" s="13">
         <v>60016</v>
       </c>
-    </row>
-    <row r="372" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L371" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA70-.svg</v>
+      </c>
+    </row>
+    <row r="372" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="2">
         <v>370</v>
       </c>
@@ -28228,8 +29026,12 @@
       <c r="D372" s="13">
         <v>60017</v>
       </c>
-    </row>
-    <row r="373" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L372" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA71-.svg</v>
+      </c>
+    </row>
+    <row r="373" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="2">
         <v>371</v>
       </c>
@@ -28240,8 +29042,12 @@
       <c r="D373" s="13">
         <v>60018</v>
       </c>
-    </row>
-    <row r="374" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L373" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA72-.svg</v>
+      </c>
+    </row>
+    <row r="374" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="2">
         <v>372</v>
       </c>
@@ -28252,8 +29058,12 @@
       <c r="D374" s="13">
         <v>60019</v>
       </c>
-    </row>
-    <row r="375" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L374" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA73-.svg</v>
+      </c>
+    </row>
+    <row r="375" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="2">
         <v>373</v>
       </c>
@@ -28264,8 +29074,12 @@
       <c r="D375" s="13">
         <v>60020</v>
       </c>
-    </row>
-    <row r="376" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L375" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA74-.svg</v>
+      </c>
+    </row>
+    <row r="376" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="2">
         <v>374</v>
       </c>
@@ -28276,8 +29090,12 @@
       <c r="D376" s="13">
         <v>60021</v>
       </c>
-    </row>
-    <row r="377" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L376" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA75-.svg</v>
+      </c>
+    </row>
+    <row r="377" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A377" s="2">
         <v>375</v>
       </c>
@@ -28288,8 +29106,12 @@
       <c r="D377" s="13">
         <v>60022</v>
       </c>
-    </row>
-    <row r="378" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L377" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA76-.svg</v>
+      </c>
+    </row>
+    <row r="378" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A378" s="2">
         <v>376</v>
       </c>
@@ -28300,8 +29122,12 @@
       <c r="D378" s="13">
         <v>60023</v>
       </c>
-    </row>
-    <row r="379" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L378" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA77-.svg</v>
+      </c>
+    </row>
+    <row r="379" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A379" s="2">
         <v>377</v>
       </c>
@@ -28312,8 +29138,12 @@
       <c r="D379" s="13">
         <v>60024</v>
       </c>
-    </row>
-    <row r="380" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L379" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA78-.svg</v>
+      </c>
+    </row>
+    <row r="380" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A380" s="2">
         <v>378</v>
       </c>
@@ -28324,8 +29154,12 @@
       <c r="D380" s="13">
         <v>60025</v>
       </c>
-    </row>
-    <row r="381" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L380" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA79-.svg</v>
+      </c>
+    </row>
+    <row r="381" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A381" s="2">
         <v>379</v>
       </c>
@@ -28333,8 +29167,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="382" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L381" t="str">
+        <f t="shared" si="11"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="382" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A382" s="2">
         <v>380</v>
       </c>
@@ -28342,8 +29180,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="383" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L382" t="str">
+        <f t="shared" si="11"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="383" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A383" s="2">
         <v>381</v>
       </c>
@@ -28351,8 +29193,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="384" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L383" t="str">
+        <f t="shared" si="11"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="384" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A384" s="2">
         <v>382</v>
       </c>
@@ -28360,8 +29206,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="385" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L384" t="str">
+        <f t="shared" si="11"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="385" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A385" s="2">
         <v>383</v>
       </c>
@@ -28369,8 +29219,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="386" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L385" t="str">
+        <f t="shared" si="11"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="386" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="2">
         <v>384</v>
       </c>
@@ -28378,8 +29232,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="387" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L386" t="str">
+        <f t="shared" si="11"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="387" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="2">
         <v>385</v>
       </c>
@@ -28387,8 +29245,12 @@
         <f t="shared" ref="C387:C410" si="12">DEC2HEX(D387)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="388" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L387" t="str">
+        <f t="shared" si="11"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="388" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A388" s="2">
         <v>386</v>
       </c>
@@ -28396,8 +29258,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="389" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L388" t="str">
+        <f t="shared" ref="L388:L402" si="13">CONCATENATE("u",C388,"-",E388,".svg")</f>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="389" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A389" s="2">
         <v>387</v>
       </c>
@@ -28405,8 +29271,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="390" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L389" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="390" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A390" s="2">
         <v>388</v>
       </c>
@@ -28414,8 +29284,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="391" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L390" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="391" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="2">
         <v>389</v>
       </c>
@@ -28423,8 +29297,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="392" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L391" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="392" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A392" s="2">
         <v>390</v>
       </c>
@@ -28432,8 +29310,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="393" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L392" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="393" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="2">
         <v>391</v>
       </c>
@@ -28441,8 +29323,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="394" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L393" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="394" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="2">
         <v>392</v>
       </c>
@@ -28450,8 +29336,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="395" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L394" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="395" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="2">
         <v>393</v>
       </c>
@@ -28459,8 +29349,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="396" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L395" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="396" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A396" s="2">
         <v>394</v>
       </c>
@@ -28468,8 +29362,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="397" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L396" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="397" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="2">
         <v>395</v>
       </c>
@@ -28477,8 +29375,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="398" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L397" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="398" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A398" s="2">
         <v>396</v>
       </c>
@@ -28486,8 +29388,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="399" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L398" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="399" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A399" s="2">
         <v>397</v>
       </c>
@@ -28495,8 +29401,12 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="400" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L399" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="400" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="2">
         <v>398</v>
       </c>
@@ -28504,62 +29414,74 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="401" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L400" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="401" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C401" s="13" t="str">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="402" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L401" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="402" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C402" s="13" t="str">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="403" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L402" t="str">
+        <f t="shared" si="13"/>
+        <v>u0-.svg</v>
+      </c>
+    </row>
+    <row r="403" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C403" s="13" t="str">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C404" s="13" t="str">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C405" s="13" t="str">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C406" s="13" t="str">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C407" s="13" t="str">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C408" s="13" t="str">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C409" s="13" t="str">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="3:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="3:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C410" s="13" t="str">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -28580,8 +29502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="B365" sqref="B365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46280,9 +47202,9 @@
         <f>'Bowtie v1.0 reorg'!A356</f>
         <v>354</v>
       </c>
-      <c r="B355">
+      <c r="B355" t="str">
         <f>'Bowtie v1.0 reorg'!E356</f>
-        <v>0</v>
+        <v>status-success-sm</v>
       </c>
       <c r="C355" t="str">
         <f>'Bowtie v1.0 reorg'!C356</f>
@@ -46292,37 +47214,37 @@
         <f>'Bowtie v1.0 reorg'!D356</f>
         <v>60001</v>
       </c>
-      <c r="E355" t="str">
+      <c r="E355">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F356),"",'Bowtie v1.0 reorg'!F356)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G356),"",'Bowtie v1.0 reorg'!G356)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I356),"",'Bowtie v1.0 reorg'!I356)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J356),"",'Bowtie v1.0 reorg'!J356)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H356),"",'Bowtie v1.0 reorg'!H356)</f>
-        <v/>
+        <v>status success complete ok pass positive good checkmark</v>
       </c>
       <c r="J355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K356),"",'Bowtie v1.0 reorg'!K356)</f>
-        <v/>
-      </c>
-      <c r="K355" t="e">
+        <v>This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot.</v>
+      </c>
+      <c r="K355" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L355" t="e">
+        <v>{'id':354,'name':'status-success-sm','unicode':'EA61','decimal':60001,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','success','complete','ok','pass','positive','good','checkmark'],'usage':'This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot.'}</v>
+      </c>
+      <c r="L355" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":354,"name":"status-success-sm","unicode":"EA61","decimal":60001,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","success","complete","ok","pass","positive","good","checkmark"],"usage":"This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot."}</v>
       </c>
     </row>
     <row r="356" spans="1:12" x14ac:dyDescent="0.25">
@@ -46330,9 +47252,9 @@
         <f>'Bowtie v1.0 reorg'!A357</f>
         <v>355</v>
       </c>
-      <c r="B356">
+      <c r="B356" t="str">
         <f>'Bowtie v1.0 reorg'!E357</f>
-        <v>0</v>
+        <v>status-warning-sm</v>
       </c>
       <c r="C356" t="str">
         <f>'Bowtie v1.0 reorg'!C357</f>
@@ -46342,37 +47264,37 @@
         <f>'Bowtie v1.0 reorg'!D357</f>
         <v>60002</v>
       </c>
-      <c r="E356" t="str">
+      <c r="E356">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F357),"",'Bowtie v1.0 reorg'!F357)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G357),"",'Bowtie v1.0 reorg'!G357)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I357),"",'Bowtie v1.0 reorg'!I357)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J357),"",'Bowtie v1.0 reorg'!J357)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H357),"",'Bowtie v1.0 reorg'!H357)</f>
-        <v/>
+        <v>status warning problem attention exclaimation</v>
       </c>
       <c r="J356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K357),"",'Bowtie v1.0 reorg'!K357)</f>
-        <v/>
-      </c>
-      <c r="K356" t="e">
+        <v>This is a smaller version of bowtie-status-warning. It is used for stacking with bowtie-triangle.</v>
+      </c>
+      <c r="K356" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L356" t="e">
+        <v>{'id':355,'name':'status-warning-sm','unicode':'EA62','decimal':60002,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','warning','problem','attention','exclaimation'],'usage':'This is a smaller version of bowtie-status-warning. It is used for stacking with bowtie-triangle.'}</v>
+      </c>
+      <c r="L356" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":355,"name":"status-warning-sm","unicode":"EA62","decimal":60002,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","warning","problem","attention","exclaimation"],"usage":"This is a smaller version of bowtie-status-warning. It is used for stacking with bowtie-triangle."}</v>
       </c>
     </row>
     <row r="357" spans="1:12" x14ac:dyDescent="0.25">
@@ -46380,9 +47302,9 @@
         <f>'Bowtie v1.0 reorg'!A358</f>
         <v>356</v>
       </c>
-      <c r="B357">
+      <c r="B357" t="str">
         <f>'Bowtie v1.0 reorg'!E358</f>
-        <v>0</v>
+        <v>status-info-sm</v>
       </c>
       <c r="C357" t="str">
         <f>'Bowtie v1.0 reorg'!C358</f>
@@ -46392,37 +47314,37 @@
         <f>'Bowtie v1.0 reorg'!D358</f>
         <v>60003</v>
       </c>
-      <c r="E357" t="str">
+      <c r="E357">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F358),"",'Bowtie v1.0 reorg'!F358)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G358),"",'Bowtie v1.0 reorg'!G358)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I358),"",'Bowtie v1.0 reorg'!I358)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J358),"",'Bowtie v1.0 reorg'!J358)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H358),"",'Bowtie v1.0 reorg'!H358)</f>
-        <v/>
+        <v>status information letter i</v>
       </c>
       <c r="J357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K358),"",'Bowtie v1.0 reorg'!K358)</f>
-        <v/>
-      </c>
-      <c r="K357" t="e">
+        <v>This is a smaller version of bowtie-status-info. It is used for stacking with bowtie-dot.</v>
+      </c>
+      <c r="K357" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L357" t="e">
+        <v>{'id':356,'name':'status-info-sm','unicode':'EA63','decimal':60003,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','information','letter','i'],'usage':'This is a smaller version of bowtie-status-info. It is used for stacking with bowtie-dot.'}</v>
+      </c>
+      <c r="L357" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":356,"name":"status-info-sm","unicode":"EA63","decimal":60003,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","information","letter","i"],"usage":"This is a smaller version of bowtie-status-info. It is used for stacking with bowtie-dot."}</v>
       </c>
     </row>
     <row r="358" spans="1:12" x14ac:dyDescent="0.25">
@@ -46430,9 +47352,9 @@
         <f>'Bowtie v1.0 reorg'!A359</f>
         <v>357</v>
       </c>
-      <c r="B358">
+      <c r="B358" t="str">
         <f>'Bowtie v1.0 reorg'!E359</f>
-        <v>0</v>
+        <v>status-failure-sm</v>
       </c>
       <c r="C358" t="str">
         <f>'Bowtie v1.0 reorg'!C359</f>
@@ -46442,37 +47364,37 @@
         <f>'Bowtie v1.0 reorg'!D359</f>
         <v>60004</v>
       </c>
-      <c r="E358" t="str">
+      <c r="E358">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F359),"",'Bowtie v1.0 reorg'!F359)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G359),"",'Bowtie v1.0 reorg'!G359)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I359),"",'Bowtie v1.0 reorg'!I359)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J359),"",'Bowtie v1.0 reorg'!J359)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H359),"",'Bowtie v1.0 reorg'!H359)</f>
-        <v/>
+        <v>status failure negative critical problem fatal error</v>
       </c>
       <c r="J358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K359),"",'Bowtie v1.0 reorg'!K359)</f>
-        <v/>
-      </c>
-      <c r="K358" t="e">
+        <v>This is a smaller version of bowtie-status-failure. It is used for stacking with bowtie-dot.</v>
+      </c>
+      <c r="K358" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L358" t="e">
+        <v>{'id':357,'name':'status-failure-sm','unicode':'EA64','decimal':60004,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','failure','negative','critical','problem','fatal','error'],'usage':'This is a smaller version of bowtie-status-failure. It is used for stacking with bowtie-dot.'}</v>
+      </c>
+      <c r="L358" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":357,"name":"status-failure-sm","unicode":"EA64","decimal":60004,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","failure","negative","critical","problem","fatal","error"],"usage":"This is a smaller version of bowtie-status-failure. It is used for stacking with bowtie-dot."}</v>
       </c>
     </row>
     <row r="359" spans="1:12" x14ac:dyDescent="0.25">
@@ -46480,9 +47402,9 @@
         <f>'Bowtie v1.0 reorg'!A360</f>
         <v>358</v>
       </c>
-      <c r="B359">
+      <c r="B359" t="str">
         <f>'Bowtie v1.0 reorg'!E360</f>
-        <v>0</v>
+        <v>status-error-sm</v>
       </c>
       <c r="C359" t="str">
         <f>'Bowtie v1.0 reorg'!C360</f>
@@ -46492,37 +47414,37 @@
         <f>'Bowtie v1.0 reorg'!D360</f>
         <v>60005</v>
       </c>
-      <c r="E359" t="str">
+      <c r="E359">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F360),"",'Bowtie v1.0 reorg'!F360)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G360),"",'Bowtie v1.0 reorg'!G360)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I360),"",'Bowtie v1.0 reorg'!I360)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J360),"",'Bowtie v1.0 reorg'!J360)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H360),"",'Bowtie v1.0 reorg'!H360)</f>
-        <v/>
+        <v>status error alert invalid problem circle exclaimation</v>
       </c>
       <c r="J359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K360),"",'Bowtie v1.0 reorg'!K360)</f>
-        <v/>
-      </c>
-      <c r="K359" t="e">
+        <v>This is a smaller version of bowtie-status-error. It is used for stacking with bowtie-dot.</v>
+      </c>
+      <c r="K359" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L359" t="e">
+        <v>{'id':358,'name':'status-error-sm','unicode':'EA65','decimal':60005,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','error','alert','invalid','problem','circle','exclaimation'],'usage':'This is a smaller version of bowtie-status-error. It is used for stacking with bowtie-dot.'}</v>
+      </c>
+      <c r="L359" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":358,"name":"status-error-sm","unicode":"EA65","decimal":60005,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","error","alert","invalid","problem","circle","exclaimation"],"usage":"This is a smaller version of bowtie-status-error. It is used for stacking with bowtie-dot."}</v>
       </c>
     </row>
     <row r="360" spans="1:12" x14ac:dyDescent="0.25">
@@ -46530,9 +47452,9 @@
         <f>'Bowtie v1.0 reorg'!A361</f>
         <v>359</v>
       </c>
-      <c r="B360">
+      <c r="B360" t="str">
         <f>'Bowtie v1.0 reorg'!E361</f>
-        <v>0</v>
+        <v>status-run-sm</v>
       </c>
       <c r="C360" t="str">
         <f>'Bowtie v1.0 reorg'!C361</f>
@@ -46542,37 +47464,37 @@
         <f>'Bowtie v1.0 reorg'!D361</f>
         <v>60006</v>
       </c>
-      <c r="E360" t="str">
+      <c r="E360">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F361),"",'Bowtie v1.0 reorg'!F361)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G361),"",'Bowtie v1.0 reorg'!G361)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I361),"",'Bowtie v1.0 reorg'!I361)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J361),"",'Bowtie v1.0 reorg'!J361)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H361),"",'Bowtie v1.0 reorg'!H361)</f>
-        <v/>
+        <v>status run play execute in progress triangle</v>
       </c>
       <c r="J360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K361),"",'Bowtie v1.0 reorg'!K361)</f>
-        <v/>
-      </c>
-      <c r="K360" t="e">
+        <v>This is a smaller version of bowtie-status-run. It is used for stacking with bowtie-dot.</v>
+      </c>
+      <c r="K360" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L360" t="e">
+        <v>{'id':359,'name':'status-run-sm','unicode':'EA66','decimal':60006,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','run','play','execute','in','progress','triangle'],'usage':'This is a smaller version of bowtie-status-run. It is used for stacking with bowtie-dot.'}</v>
+      </c>
+      <c r="L360" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":359,"name":"status-run-sm","unicode":"EA66","decimal":60006,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","run","play","execute","in","progress","triangle"],"usage":"This is a smaller version of bowtie-status-run. It is used for stacking with bowtie-dot."}</v>
       </c>
     </row>
     <row r="361" spans="1:12" x14ac:dyDescent="0.25">
@@ -46580,9 +47502,9 @@
         <f>'Bowtie v1.0 reorg'!A362</f>
         <v>360</v>
       </c>
-      <c r="B361">
+      <c r="B361" t="str">
         <f>'Bowtie v1.0 reorg'!E362</f>
-        <v>0</v>
+        <v>status-help-sm</v>
       </c>
       <c r="C361" t="str">
         <f>'Bowtie v1.0 reorg'!C362</f>
@@ -46592,37 +47514,37 @@
         <f>'Bowtie v1.0 reorg'!D362</f>
         <v>60007</v>
       </c>
-      <c r="E361" t="str">
+      <c r="E361">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F362),"",'Bowtie v1.0 reorg'!F362)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G362),"",'Bowtie v1.0 reorg'!G362)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I362),"",'Bowtie v1.0 reorg'!I362)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J362),"",'Bowtie v1.0 reorg'!J362)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H362),"",'Bowtie v1.0 reorg'!H362)</f>
-        <v/>
+        <v>status help question</v>
       </c>
       <c r="J361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K362),"",'Bowtie v1.0 reorg'!K362)</f>
-        <v/>
-      </c>
-      <c r="K361" t="e">
+        <v>This is a smaller version of bowtie-status-help. It is used for stacking with bowtie-dot.</v>
+      </c>
+      <c r="K361" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L361" t="e">
+        <v>{'id':360,'name':'status-help-sm','unicode':'EA67','decimal':60007,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','help','question'],'usage':'This is a smaller version of bowtie-status-help. It is used for stacking with bowtie-dot.'}</v>
+      </c>
+      <c r="L361" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":360,"name":"status-help-sm","unicode":"EA67","decimal":60007,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","help","question"],"usage":"This is a smaller version of bowtie-status-help. It is used for stacking with bowtie-dot."}</v>
       </c>
     </row>
     <row r="362" spans="1:12" x14ac:dyDescent="0.25">
@@ -46630,9 +47552,9 @@
         <f>'Bowtie v1.0 reorg'!A363</f>
         <v>361</v>
       </c>
-      <c r="B362">
+      <c r="B362" t="str">
         <f>'Bowtie v1.0 reorg'!E363</f>
-        <v>0</v>
+        <v>status-stop-sm</v>
       </c>
       <c r="C362" t="str">
         <f>'Bowtie v1.0 reorg'!C363</f>
@@ -46642,37 +47564,37 @@
         <f>'Bowtie v1.0 reorg'!D363</f>
         <v>60008</v>
       </c>
-      <c r="E362" t="str">
+      <c r="E362">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F363),"",'Bowtie v1.0 reorg'!F363)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G363),"",'Bowtie v1.0 reorg'!G363)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I363),"",'Bowtie v1.0 reorg'!I363)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J363),"",'Bowtie v1.0 reorg'!J363)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H363),"",'Bowtie v1.0 reorg'!H363)</f>
-        <v/>
+        <v>status stop square</v>
       </c>
       <c r="J362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K363),"",'Bowtie v1.0 reorg'!K363)</f>
-        <v/>
-      </c>
-      <c r="K362" t="e">
+        <v>This is a smaller version of bowtie-status-stop. It is used for stacking with bowtie-dot.</v>
+      </c>
+      <c r="K362" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L362" t="e">
+        <v>{'id':361,'name':'status-stop-sm','unicode':'EA68','decimal':60008,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','stop','square'],'usage':'This is a smaller version of bowtie-status-stop. It is used for stacking with bowtie-dot.'}</v>
+      </c>
+      <c r="L362" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":361,"name":"status-stop-sm","unicode":"EA68","decimal":60008,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","stop","square"],"usage":"This is a smaller version of bowtie-status-stop. It is used for stacking with bowtie-dot."}</v>
       </c>
     </row>
     <row r="363" spans="1:12" x14ac:dyDescent="0.25">
@@ -46680,9 +47602,9 @@
         <f>'Bowtie v1.0 reorg'!A364</f>
         <v>362</v>
       </c>
-      <c r="B363">
+      <c r="B363" t="str">
         <f>'Bowtie v1.0 reorg'!E364</f>
-        <v>0</v>
+        <v>status-pause-sm</v>
       </c>
       <c r="C363" t="str">
         <f>'Bowtie v1.0 reorg'!C364</f>
@@ -46692,37 +47614,37 @@
         <f>'Bowtie v1.0 reorg'!D364</f>
         <v>60009</v>
       </c>
-      <c r="E363" t="str">
+      <c r="E363">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F364),"",'Bowtie v1.0 reorg'!F364)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G364),"",'Bowtie v1.0 reorg'!G364)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I364),"",'Bowtie v1.0 reorg'!I364)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J364),"",'Bowtie v1.0 reorg'!J364)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H364),"",'Bowtie v1.0 reorg'!H364)</f>
-        <v/>
+        <v>status pause</v>
       </c>
       <c r="J363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K364),"",'Bowtie v1.0 reorg'!K364)</f>
-        <v/>
-      </c>
-      <c r="K363" t="e">
+        <v>This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot.</v>
+      </c>
+      <c r="K363" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L363" t="e">
+        <v>{'id':362,'name':'status-pause-sm','unicode':'EA69','decimal':60009,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','pause'],'usage':'This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot.'}</v>
+      </c>
+      <c r="L363" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":362,"name":"status-pause-sm","unicode":"EA69","decimal":60009,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","pause"],"usage":"This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot."}</v>
       </c>
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.25">
@@ -46730,9 +47652,9 @@
         <f>'Bowtie v1.0 reorg'!A365</f>
         <v>363</v>
       </c>
-      <c r="B364">
+      <c r="B364" t="str">
         <f>'Bowtie v1.0 reorg'!E365</f>
-        <v>0</v>
+        <v>status-waiting-fill-sm</v>
       </c>
       <c r="C364" t="str">
         <f>'Bowtie v1.0 reorg'!C365</f>
@@ -46742,37 +47664,37 @@
         <f>'Bowtie v1.0 reorg'!D365</f>
         <v>60010</v>
       </c>
-      <c r="E364" t="str">
+      <c r="E364">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F365),"",'Bowtie v1.0 reorg'!F365)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G365),"",'Bowtie v1.0 reorg'!G365)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I365),"",'Bowtie v1.0 reorg'!I365)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J365),"",'Bowtie v1.0 reorg'!J365)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H365),"",'Bowtie v1.0 reorg'!H365)</f>
-        <v/>
+        <v>status waiting clock time pending queue</v>
       </c>
       <c r="J364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K365),"",'Bowtie v1.0 reorg'!K365)</f>
-        <v/>
-      </c>
-      <c r="K364" t="e">
+        <v>This is a smaller version of bowtie-status-waiting-fill. It is used for stacking with bowtie-dot.</v>
+      </c>
+      <c r="K364" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L364" t="e">
+        <v>{'id':363,'name':'status-waiting-fill-sm','unicode':'EA6A','decimal':60010,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','waiting','clock','time','pending','queue'],'usage':'This is a smaller version of bowtie-status-waiting-fill. It is used for stacking with bowtie-dot.'}</v>
+      </c>
+      <c r="L364" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":363,"name":"status-waiting-fill-sm","unicode":"EA6A","decimal":60010,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","waiting","clock","time","pending","queue"],"usage":"This is a smaller version of bowtie-status-waiting-fill. It is used for stacking with bowtie-dot."}</v>
       </c>
     </row>
     <row r="365" spans="1:12" x14ac:dyDescent="0.25">
@@ -46780,9 +47702,9 @@
         <f>'Bowtie v1.0 reorg'!A366</f>
         <v>364</v>
       </c>
-      <c r="B365">
+      <c r="B365" t="str">
         <f>'Bowtie v1.0 reorg'!E366</f>
-        <v>0</v>
+        <v>status-no-fill-sm</v>
       </c>
       <c r="C365" t="str">
         <f>'Bowtie v1.0 reorg'!C366</f>
@@ -46792,37 +47714,37 @@
         <f>'Bowtie v1.0 reorg'!D366</f>
         <v>60011</v>
       </c>
-      <c r="E365" t="str">
+      <c r="E365">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F366),"",'Bowtie v1.0 reorg'!F366)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G366),"",'Bowtie v1.0 reorg'!G366)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I366),"",'Bowtie v1.0 reorg'!I366)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J366),"",'Bowtie v1.0 reorg'!J366)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H366),"",'Bowtie v1.0 reorg'!H366)</f>
-        <v/>
+        <v>status no block mute unavailable</v>
       </c>
       <c r="J365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K366),"",'Bowtie v1.0 reorg'!K366)</f>
-        <v/>
-      </c>
-      <c r="K365" t="e">
+        <v>This is a smaller version of bowtie-status-no-fill. It is used for stacking with bowtie-dot.</v>
+      </c>
+      <c r="K365" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L365" t="e">
+        <v>{'id':364,'name':'status-no-fill-sm','unicode':'EA6B','decimal':60011,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','no','block','mute','unavailable'],'usage':'This is a smaller version of bowtie-status-no-fill. It is used for stacking with bowtie-dot.'}</v>
+      </c>
+      <c r="L365" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":364,"name":"status-no-fill-sm","unicode":"EA6B","decimal":60011,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","no","block","mute","unavailable"],"usage":"This is a smaller version of bowtie-status-no-fill. It is used for stacking with bowtie-dot."}</v>
       </c>
     </row>
     <row r="366" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added assessment group icon for compliance hub
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="692">
   <si>
     <t>name</t>
   </si>
@@ -2084,6 +2084,18 @@
   </si>
   <si>
     <t>This is a smaller version of bowtie-status-no-fill. It is used for stacking with bowtie-dot.</t>
+  </si>
+  <si>
+    <t>assessment-group</t>
+  </si>
+  <si>
+    <t>assessment group compliance</t>
+  </si>
+  <si>
+    <t>Compliance</t>
+  </si>
+  <si>
+    <t>Used in treeview in Compliance hub to represent assessment type node.</t>
   </si>
 </sst>
 </file>
@@ -16062,6 +16074,44 @@
         <a:xfrm>
           <a:off x="1114425" y="146637375"/>
           <a:ext cx="190527" cy="181000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>366</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409606</xdr:colOff>
+      <xdr:row>366</xdr:row>
+      <xdr:rowOff>361979</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="367" name="Picture 366"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId365"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="147056475"/>
+          <a:ext cx="219106" cy="209579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16340,7 +16390,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A358" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N364" sqref="N364"/>
+      <selection pane="bottomLeft" activeCell="E368" sqref="E368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28946,9 +28996,30 @@
       <c r="D367" s="13">
         <v>60012</v>
       </c>
+      <c r="E367" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="F367" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G367" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H367" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="I367" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J367" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="K367" s="2" t="s">
+        <v>691</v>
+      </c>
       <c r="L367" t="str">
         <f t="shared" si="11"/>
-        <v>uEA6C-.svg</v>
+        <v>uEA6C-assessment-group.svg</v>
       </c>
     </row>
     <row r="368" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -29503,7 +29574,7 @@
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="B365" sqref="B365"/>
+      <selection activeCell="U373" sqref="U373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47752,9 +47823,9 @@
         <f>'Bowtie v1.0 reorg'!A367</f>
         <v>365</v>
       </c>
-      <c r="B366">
+      <c r="B366" t="str">
         <f>'Bowtie v1.0 reorg'!E367</f>
-        <v>0</v>
+        <v>assessment-group</v>
       </c>
       <c r="C366" t="str">
         <f>'Bowtie v1.0 reorg'!C367</f>
@@ -47764,37 +47835,37 @@
         <f>'Bowtie v1.0 reorg'!D367</f>
         <v>60012</v>
       </c>
-      <c r="E366" t="str">
+      <c r="E366">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F367),"",'Bowtie v1.0 reorg'!F367)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F366" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G367),"",'Bowtie v1.0 reorg'!G367)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G366" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I367),"",'Bowtie v1.0 reorg'!I367)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H366" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J367),"",'Bowtie v1.0 reorg'!J367)</f>
-        <v/>
+        <v>Compliance</v>
       </c>
       <c r="I366" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H367),"",'Bowtie v1.0 reorg'!H367)</f>
-        <v/>
+        <v>assessment group compliance</v>
       </c>
       <c r="J366" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K367),"",'Bowtie v1.0 reorg'!K367)</f>
-        <v/>
-      </c>
-      <c r="K366" t="e">
+        <v>Used in treeview in Compliance hub to represent assessment type node.</v>
+      </c>
+      <c r="K366" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L366" t="e">
+        <v>{'id':365,'name':'assessment-group','unicode':'EA6C','decimal':60012,'version':'1.1','style':'bold','subset':'VSTS','group':'Compliance','keywords':['assessment','group','compliance'],'usage':'Used in treeview in Compliance hub to represent assessment type node.'}</v>
+      </c>
+      <c r="L366" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":365,"name":"assessment-group","unicode":"EA6C","decimal":60012,"version":"1.1","style":"bold","subset":"VSTS","group":"Compliance","keywords":["assessment","group","compliance"],"usage":"Used in treeview in Compliance hub to represent assessment type node."}</v>
       </c>
     </row>
     <row r="367" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
moved some drafts to final
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="701">
   <si>
     <t>name</t>
   </si>
@@ -2096,6 +2096,33 @@
   </si>
   <si>
     <t>Used in treeview in Compliance hub to represent assessment type node.</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>table database matrix</t>
+  </si>
+  <si>
+    <t>Used for database table, matrix or views that look like a data table.</t>
+  </si>
+  <si>
+    <t>timeline-delivery</t>
+  </si>
+  <si>
+    <t>timeline-progress</t>
+  </si>
+  <si>
+    <t>timeline delivery schedule kanban card</t>
+  </si>
+  <si>
+    <t>timeline progress date row line bar</t>
+  </si>
+  <si>
+    <t>Used to indicate delivery card style backlog timeline view.</t>
+  </si>
+  <si>
+    <t>Used to indicate progress bar style backlog timeline view.</t>
   </si>
 </sst>
 </file>
@@ -16112,6 +16139,120 @@
         <a:xfrm>
           <a:off x="1133475" y="147056475"/>
           <a:ext cx="219106" cy="209579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390557</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>295304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="356" name="Picture 355"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId366"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="147389850"/>
+          <a:ext cx="228632" cy="209579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>368</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361975</xdr:colOff>
+      <xdr:row>368</xdr:row>
+      <xdr:rowOff>304825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="368" name="Picture 367"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId367"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1123950" y="147828000"/>
+          <a:ext cx="181000" cy="181000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>369</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400075</xdr:colOff>
+      <xdr:row>369</xdr:row>
+      <xdr:rowOff>342931</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="369" name="Picture 368"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId368"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1162050" y="148228050"/>
+          <a:ext cx="181000" cy="219106"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16389,7 +16530,7 @@
   <dimension ref="A1:AL410"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A358" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A367" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E368" sqref="E368"/>
     </sheetView>
   </sheetViews>
@@ -29033,9 +29174,30 @@
       <c r="D368" s="13">
         <v>60013</v>
       </c>
+      <c r="E368" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="F368" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G368" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H368" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="I368" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J368" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="K368" s="2" t="s">
+        <v>694</v>
+      </c>
       <c r="L368" t="str">
         <f t="shared" si="11"/>
-        <v>uEA6D-.svg</v>
+        <v>uEA6D-table.svg</v>
       </c>
     </row>
     <row r="369" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -29049,9 +29211,30 @@
       <c r="D369" s="13">
         <v>60014</v>
       </c>
+      <c r="E369" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="F369" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G369" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H369" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="I369" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J369" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="K369" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="L369" t="str">
         <f t="shared" si="11"/>
-        <v>uEA6E-.svg</v>
+        <v>uEA6E-timeline-delivery.svg</v>
       </c>
     </row>
     <row r="370" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -29065,9 +29248,30 @@
       <c r="D370" s="13">
         <v>60015</v>
       </c>
+      <c r="E370" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="F370" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G370" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H370" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="I370" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J370" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="K370" s="2" t="s">
+        <v>700</v>
+      </c>
       <c r="L370" t="str">
         <f t="shared" si="11"/>
-        <v>uEA6F-.svg</v>
+        <v>uEA6F-timeline-progress.svg</v>
       </c>
     </row>
     <row r="371" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -29574,7 +29778,7 @@
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="U373" sqref="U373"/>
+      <selection activeCell="B370" sqref="B370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47873,9 +48077,9 @@
         <f>'Bowtie v1.0 reorg'!A368</f>
         <v>366</v>
       </c>
-      <c r="B367">
+      <c r="B367" t="str">
         <f>'Bowtie v1.0 reorg'!E368</f>
-        <v>0</v>
+        <v>table</v>
       </c>
       <c r="C367" t="str">
         <f>'Bowtie v1.0 reorg'!C368</f>
@@ -47885,37 +48089,37 @@
         <f>'Bowtie v1.0 reorg'!D368</f>
         <v>60013</v>
       </c>
-      <c r="E367" t="str">
+      <c r="E367">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F368),"",'Bowtie v1.0 reorg'!F368)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F367" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G368),"",'Bowtie v1.0 reorg'!G368)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G367" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I368),"",'Bowtie v1.0 reorg'!I368)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H367" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J368),"",'Bowtie v1.0 reorg'!J368)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I367" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H368),"",'Bowtie v1.0 reorg'!H368)</f>
-        <v/>
+        <v>table database matrix</v>
       </c>
       <c r="J367" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K368),"",'Bowtie v1.0 reorg'!K368)</f>
-        <v/>
-      </c>
-      <c r="K367" t="e">
+        <v>Used for database table, matrix or views that look like a data table.</v>
+      </c>
+      <c r="K367" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L367" t="e">
+        <v>{'id':366,'name':'table','unicode':'EA6D','decimal':60013,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['table','database','matrix'],'usage':'Used for database table, matrix or views that look like a data table.'}</v>
+      </c>
+      <c r="L367" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":366,"name":"table","unicode":"EA6D","decimal":60013,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["table","database","matrix"],"usage":"Used for database table, matrix or views that look like a data table."}</v>
       </c>
     </row>
     <row r="368" spans="1:12" x14ac:dyDescent="0.25">
@@ -47923,9 +48127,9 @@
         <f>'Bowtie v1.0 reorg'!A369</f>
         <v>367</v>
       </c>
-      <c r="B368">
+      <c r="B368" t="str">
         <f>'Bowtie v1.0 reorg'!E369</f>
-        <v>0</v>
+        <v>timeline-delivery</v>
       </c>
       <c r="C368" t="str">
         <f>'Bowtie v1.0 reorg'!C369</f>
@@ -47935,37 +48139,37 @@
         <f>'Bowtie v1.0 reorg'!D369</f>
         <v>60014</v>
       </c>
-      <c r="E368" t="str">
+      <c r="E368">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F369),"",'Bowtie v1.0 reorg'!F369)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F368" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G369),"",'Bowtie v1.0 reorg'!G369)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G368" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I369),"",'Bowtie v1.0 reorg'!I369)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H368" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J369),"",'Bowtie v1.0 reorg'!J369)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="I368" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H369),"",'Bowtie v1.0 reorg'!H369)</f>
-        <v/>
+        <v>timeline delivery schedule kanban card</v>
       </c>
       <c r="J368" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K369),"",'Bowtie v1.0 reorg'!K369)</f>
-        <v/>
-      </c>
-      <c r="K368" t="e">
+        <v>Used to indicate delivery card style backlog timeline view.</v>
+      </c>
+      <c r="K368" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L368" t="e">
+        <v>{'id':367,'name':'timeline-delivery','unicode':'EA6E','decimal':60014,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['timeline','delivery','schedule','kanban','card'],'usage':'Used to indicate delivery card style backlog timeline view.'}</v>
+      </c>
+      <c r="L368" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":367,"name":"timeline-delivery","unicode":"EA6E","decimal":60014,"version":"1.1","style":"bold","subset":"VSTS","group":"Work","keywords":["timeline","delivery","schedule","kanban","card"],"usage":"Used to indicate delivery card style backlog timeline view."}</v>
       </c>
     </row>
     <row r="369" spans="1:12" x14ac:dyDescent="0.25">
@@ -47973,9 +48177,9 @@
         <f>'Bowtie v1.0 reorg'!A370</f>
         <v>368</v>
       </c>
-      <c r="B369">
+      <c r="B369" t="str">
         <f>'Bowtie v1.0 reorg'!E370</f>
-        <v>0</v>
+        <v>timeline-progress</v>
       </c>
       <c r="C369" t="str">
         <f>'Bowtie v1.0 reorg'!C370</f>
@@ -47985,37 +48189,37 @@
         <f>'Bowtie v1.0 reorg'!D370</f>
         <v>60015</v>
       </c>
-      <c r="E369" t="str">
+      <c r="E369">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F370),"",'Bowtie v1.0 reorg'!F370)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F369" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G370),"",'Bowtie v1.0 reorg'!G370)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G369" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I370),"",'Bowtie v1.0 reorg'!I370)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H369" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J370),"",'Bowtie v1.0 reorg'!J370)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="I369" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H370),"",'Bowtie v1.0 reorg'!H370)</f>
-        <v/>
+        <v>timeline progress date row line bar</v>
       </c>
       <c r="J369" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K370),"",'Bowtie v1.0 reorg'!K370)</f>
-        <v/>
-      </c>
-      <c r="K369" t="e">
+        <v>Used to indicate progress bar style backlog timeline view.</v>
+      </c>
+      <c r="K369" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L369" t="e">
+        <v>{'id':368,'name':'timeline-progress','unicode':'EA6F','decimal':60015,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['timeline','progress','date','row','line','bar'],'usage':'Used to indicate progress bar style backlog timeline view.'}</v>
+      </c>
+      <c r="L369" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":368,"name":"timeline-progress","unicode":"EA6F","decimal":60015,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["timeline","progress","date","row","line","bar"],"usage":"Used to indicate progress bar style backlog timeline view."}</v>
       </c>
     </row>
     <row r="370" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added split icon for work item context menu
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="800">
   <si>
     <t>name</t>
   </si>
@@ -2411,6 +2411,15 @@
   </si>
   <si>
     <t>Used for templating preprocessor file type like .jade, .haml, etc.</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <t>split arrow</t>
+  </si>
+  <si>
+    <t>Used for splitting work item.</t>
   </si>
 </sst>
 </file>
@@ -18033,9 +18042,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL468"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A399" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C402" sqref="C402"/>
+      <selection pane="bottomLeft" activeCell="L403" sqref="L403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32735,7 +32744,7 @@
       <c r="K402" s="2" t="s">
         <v>796</v>
       </c>
-      <c r="L402" t="str">
+      <c r="L402" s="15" t="str">
         <f t="shared" si="13"/>
         <v>uEA8F-file-type-template.svg</v>
       </c>
@@ -32751,9 +32760,30 @@
       <c r="D403" s="16">
         <v>60048</v>
       </c>
+      <c r="E403" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="F403" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G403" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H403" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="I403" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J403" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="K403" s="2" t="s">
+        <v>799</v>
+      </c>
       <c r="L403" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>uEA90-.svg</v>
+        <v>uEA90-split.svg</v>
       </c>
     </row>
     <row r="404" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32766,6 +32796,15 @@
       </c>
       <c r="D404" s="13">
         <v>60049</v>
+      </c>
+      <c r="F404" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G404" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I404" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="L404" s="15" t="str">
         <f t="shared" si="13"/>
@@ -33637,8 +33676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView topLeftCell="A382" workbookViewId="0">
-      <selection activeCell="F405" sqref="F405"/>
+    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
+      <selection activeCell="G392" sqref="G392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53527,11 +53566,11 @@
         <v>Used for resource file (.resx) node in code explorer tree view.</v>
       </c>
       <c r="K398" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="K398:K408" si="16">IF(NOT(ISBLANK(A398)),CONCATENATE("{'",$A$1,"':",A398,",'",$B$1,"':'",B398,"',","'",$C$1,"':'",C398,"','",$D$1,"':",D398,",'",$E$1,"':'",FIXED(E398,1),"','",$F$1,"':'",F398,"','",$G$1,"':'",G398,"','",$H$1,"':'",H398,"','",$I$1,"':['",SUBSTITUTE(I398," ","','"),"'],'",$J$1,"':'",J398,"'}"))</f>
         <v>{'id':397,'name':'file-stack','unicode':'EA8C','decimal':60044,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','stack','group','resx','resource'],'usage':'Used for resource file (.resx) node in code explorer tree view.'}</v>
       </c>
       <c r="L398" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="L398:L408" si="17">SUBSTITUTE(K398,"'","""")</f>
         <v>{"id":397,"name":"file-stack","unicode":"EA8C","decimal":60044,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","stack","group","resx","resource"],"usage":"Used for resource file (.resx) node in code explorer tree view."}</v>
       </c>
     </row>
@@ -53577,11 +53616,11 @@
         <v>Generic script file</v>
       </c>
       <c r="K399" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>{'id':398,'name':'script','unicode':'EA8D','decimal':60045,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['script','scroll'],'usage':'Generic script file'}</v>
       </c>
       <c r="L399" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>{"id":398,"name":"script","unicode":"EA8D","decimal":60045,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["script","scroll"],"usage":"Generic script file"}</v>
       </c>
     </row>
@@ -53627,11 +53666,11 @@
         <v>Generic executable file such as .bat, .exe</v>
       </c>
       <c r="K400" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>{'id':399,'name':'default-executable','unicode':'EA8E','decimal':60046,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['default','executable','gear','process'],'usage':'Generic executable file such as .bat, .exe'}</v>
       </c>
       <c r="L400" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>{"id":399,"name":"default-executable","unicode":"EA8E","decimal":60046,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["default","executable","gear","process"],"usage":"Generic executable file such as .bat, .exe"}</v>
       </c>
     </row>
@@ -53677,11 +53716,11 @@
         <v>Used for templating preprocessor file type like .jade, .haml, etc.</v>
       </c>
       <c r="K401" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>{'id':400,'name':'file-type-template','unicode':'EA8F','decimal':60047,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','template','preprocessor','dotted','line'],'usage':'Used for templating preprocessor file type like .jade, .haml, etc.'}</v>
       </c>
       <c r="L401" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>{"id":400,"name":"file-type-template","unicode":"EA8F","decimal":60047,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","template","preprocessor","dotted","line"],"usage":"Used for templating preprocessor file type like .jade, .haml, etc."}</v>
       </c>
     </row>
@@ -53690,9 +53729,9 @@
         <f>'Bowtie v1.0 reorg'!A403</f>
         <v>401</v>
       </c>
-      <c r="B402">
+      <c r="B402" t="str">
         <f>'Bowtie v1.0 reorg'!E403</f>
-        <v>0</v>
+        <v>split</v>
       </c>
       <c r="C402" t="str">
         <f>'Bowtie v1.0 reorg'!C403</f>
@@ -53702,37 +53741,37 @@
         <f>'Bowtie v1.0 reorg'!D403</f>
         <v>60048</v>
       </c>
-      <c r="E402" t="str">
+      <c r="E402">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F403),"",'Bowtie v1.0 reorg'!F403)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F402" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G403),"",'Bowtie v1.0 reorg'!G403)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G402" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I403),"",'Bowtie v1.0 reorg'!I403)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H402" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J403),"",'Bowtie v1.0 reorg'!J403)</f>
-        <v/>
+        <v>Arrow</v>
       </c>
       <c r="I402" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H403),"",'Bowtie v1.0 reorg'!H403)</f>
-        <v/>
+        <v>split arrow</v>
       </c>
       <c r="J402" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K403),"",'Bowtie v1.0 reorg'!K403)</f>
-        <v/>
-      </c>
-      <c r="K402" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L402" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>Used for splitting work item.</v>
+      </c>
+      <c r="K402" t="str">
+        <f t="shared" si="16"/>
+        <v>{'id':401,'name':'split','unicode':'EA90','decimal':60048,'version':'1.1','style':'light','subset':'VSTS','group':'Arrow','keywords':['split','arrow'],'usage':'Used for splitting work item.'}</v>
+      </c>
+      <c r="L402" t="str">
+        <f t="shared" si="17"/>
+        <v>{"id":401,"name":"split","unicode":"EA90","decimal":60048,"version":"1.1","style":"light","subset":"VSTS","group":"Arrow","keywords":["split","arrow"],"usage":"Used for splitting work item."}</v>
       </c>
     </row>
     <row r="403" spans="1:12" x14ac:dyDescent="0.25">
@@ -53752,17 +53791,17 @@
         <f>'Bowtie v1.0 reorg'!D404</f>
         <v>60049</v>
       </c>
-      <c r="E403" t="str">
+      <c r="E403">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F404),"",'Bowtie v1.0 reorg'!F404)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F403" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G404),"",'Bowtie v1.0 reorg'!G404)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G403" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I404),"",'Bowtie v1.0 reorg'!I404)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H403" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J404),"",'Bowtie v1.0 reorg'!J404)</f>
@@ -53776,13 +53815,13 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K404),"",'Bowtie v1.0 reorg'!K404)</f>
         <v/>
       </c>
-      <c r="K403" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L403" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="K403" t="str">
+        <f t="shared" si="16"/>
+        <v>{'id':402,'name':'0','unicode':'EA91','decimal':60049,'version':'1.1','style':'light','subset':'VSTS','group':'','keywords':[''],'usage':''}</v>
+      </c>
+      <c r="L403" t="str">
+        <f t="shared" si="17"/>
+        <v>{"id":402,"name":"0","unicode":"EA91","decimal":60049,"version":"1.1","style":"light","subset":"VSTS","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="404" spans="1:12" x14ac:dyDescent="0.25">
@@ -53827,11 +53866,11 @@
         <v/>
       </c>
       <c r="K404" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
       <c r="L404" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -53877,11 +53916,11 @@
         <v/>
       </c>
       <c r="K405" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
       <c r="L405" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -53927,11 +53966,11 @@
         <v/>
       </c>
       <c r="K406" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
       <c r="L406" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -53977,11 +54016,11 @@
         <v/>
       </c>
       <c r="K407" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
       <c r="L407" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -54027,11 +54066,11 @@
         <v/>
       </c>
       <c r="K408" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
       <c r="L408" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56277,11 +56316,11 @@
         <v/>
       </c>
       <c r="K453" t="e">
-        <f t="shared" ref="K453:K466" si="16">IF(NOT(ISBLANK(A453)),CONCATENATE("{'",$A$1,"':",A453,",'",$B$1,"':'",B453,"',","'",$C$1,"':'",C453,"','",$D$1,"':",D453,",'",$E$1,"':'",FIXED(E453,1),"','",$F$1,"':'",F453,"','",$G$1,"':'",G453,"','",$H$1,"':'",H453,"','",$I$1,"':['",SUBSTITUTE(I453," ","','"),"'],'",$J$1,"':'",J453,"'}"))</f>
+        <f t="shared" ref="K453:K466" si="18">IF(NOT(ISBLANK(A453)),CONCATENATE("{'",$A$1,"':",A453,",'",$B$1,"':'",B453,"',","'",$C$1,"':'",C453,"','",$D$1,"':",D453,",'",$E$1,"':'",FIXED(E453,1),"','",$F$1,"':'",F453,"','",$G$1,"':'",G453,"','",$H$1,"':'",H453,"','",$I$1,"':['",SUBSTITUTE(I453," ","','"),"'],'",$J$1,"':'",J453,"'}"))</f>
         <v>#VALUE!</v>
       </c>
       <c r="L453" t="e">
-        <f t="shared" ref="L453:L466" si="17">SUBSTITUTE(K453,"'","""")</f>
+        <f t="shared" ref="L453:L466" si="19">SUBSTITUTE(K453,"'","""")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56327,11 +56366,11 @@
         <v/>
       </c>
       <c r="K454" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L454" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56377,11 +56416,11 @@
         <v/>
       </c>
       <c r="K455" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L455" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56427,11 +56466,11 @@
         <v/>
       </c>
       <c r="K456" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L456" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56477,11 +56516,11 @@
         <v/>
       </c>
       <c r="K457" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L457" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56527,11 +56566,11 @@
         <v/>
       </c>
       <c r="K458" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L458" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56577,11 +56616,11 @@
         <v/>
       </c>
       <c r="K459" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L459" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56627,11 +56666,11 @@
         <v/>
       </c>
       <c r="K460" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L460" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56677,11 +56716,11 @@
         <v/>
       </c>
       <c r="K461" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L461" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56727,11 +56766,11 @@
         <v/>
       </c>
       <c r="K462" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L462" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56777,11 +56816,11 @@
         <v/>
       </c>
       <c r="K463" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L463" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56827,11 +56866,11 @@
         <v/>
       </c>
       <c r="K464" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L464" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56877,11 +56916,11 @@
         <v/>
       </c>
       <c r="K465" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L465" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56927,11 +56966,11 @@
         <v/>
       </c>
       <c r="K466" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L466" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -56977,11 +57016,11 @@
         <v/>
       </c>
       <c r="K467" t="e">
-        <f t="shared" ref="K467:K470" si="18">IF(NOT(ISBLANK(A467)),CONCATENATE("{'",$A$1,"':",A467,",'",$B$1,"':'",B467,"',","'",$C$1,"':'",C467,"','",$D$1,"':",D467,",'",$E$1,"':'",FIXED(E467,1),"','",$F$1,"':'",F467,"','",$G$1,"':'",G467,"','",$H$1,"':'",H467,"','",$I$1,"':['",SUBSTITUTE(I467," ","','"),"'],'",$J$1,"':'",J467,"'}"))</f>
+        <f t="shared" ref="K467:K470" si="20">IF(NOT(ISBLANK(A467)),CONCATENATE("{'",$A$1,"':",A467,",'",$B$1,"':'",B467,"',","'",$C$1,"':'",C467,"','",$D$1,"':",D467,",'",$E$1,"':'",FIXED(E467,1),"','",$F$1,"':'",F467,"','",$G$1,"':'",G467,"','",$H$1,"':'",H467,"','",$I$1,"':['",SUBSTITUTE(I467," ","','"),"'],'",$J$1,"':'",J467,"'}"))</f>
         <v>#VALUE!</v>
       </c>
       <c r="L467" t="e">
-        <f t="shared" ref="L467:L470" si="19">SUBSTITUTE(K467,"'","""")</f>
+        <f t="shared" ref="L467:L470" si="21">SUBSTITUTE(K467,"'","""")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -57027,11 +57066,11 @@
         <v/>
       </c>
       <c r="K468" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="L468" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -57077,11 +57116,11 @@
         <v/>
       </c>
       <c r="K469" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="L469" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -57127,11 +57166,11 @@
         <v/>
       </c>
       <c r="K470" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="L470" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added shield icons for vc view of branches
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="806">
   <si>
     <t>name</t>
   </si>
@@ -2429,6 +2429,15 @@
   </si>
   <si>
     <t>Used for capturing user actions in the form of an image action log, in TCM Web Runner.</t>
+  </si>
+  <si>
+    <t>shield</t>
+  </si>
+  <si>
+    <t>shield-fill</t>
+  </si>
+  <si>
+    <t>Used in version control view of branches.</t>
   </si>
 </sst>
 </file>
@@ -17851,6 +17860,82 @@
         <a:xfrm>
           <a:off x="1152525" y="161401125"/>
           <a:ext cx="190527" cy="181000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>404</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390557</xdr:colOff>
+      <xdr:row>404</xdr:row>
+      <xdr:rowOff>352458</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="375" name="Picture 374"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId403"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="162220275"/>
+          <a:ext cx="228632" cy="238158"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>405</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419128</xdr:colOff>
+      <xdr:row>405</xdr:row>
+      <xdr:rowOff>342928</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="376" name="Picture 375"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId404"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1162050" y="162648900"/>
+          <a:ext cx="200053" cy="200053"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18128,8 +18213,8 @@
   <dimension ref="A1:AL468"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A399" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C403" sqref="C403"/>
+      <pane ySplit="2" topLeftCell="A402" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C406" sqref="C406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32919,9 +33004,30 @@
       <c r="D405" s="16">
         <v>60050</v>
       </c>
+      <c r="E405" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="F405" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G405" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H405" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="I405" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J405" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="K405" s="2" t="s">
+        <v>805</v>
+      </c>
       <c r="L405" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>uEA92-.svg</v>
+        <v>uEA92-shield.svg</v>
       </c>
     </row>
     <row r="406" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32935,9 +33041,30 @@
       <c r="D406" s="16">
         <v>60051</v>
       </c>
+      <c r="E406" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="F406" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G406" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H406" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="I406" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J406" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="K406" s="2" t="s">
+        <v>805</v>
+      </c>
       <c r="L406" s="15" t="str">
         <f t="shared" si="13"/>
-        <v>uEA93-.svg</v>
+        <v>uEA93-shield-fill.svg</v>
       </c>
     </row>
     <row r="407" spans="1:38" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -33774,7 +33901,7 @@
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView topLeftCell="A382" workbookViewId="0">
-      <selection activeCell="L403" sqref="L403"/>
+      <selection activeCell="I408" sqref="I408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53926,9 +54053,9 @@
         <f>'Bowtie v1.0 reorg'!A405</f>
         <v>403</v>
       </c>
-      <c r="B404">
+      <c r="B404" t="str">
         <f>'Bowtie v1.0 reorg'!E405</f>
-        <v>0</v>
+        <v>shield</v>
       </c>
       <c r="C404" t="str">
         <f>'Bowtie v1.0 reorg'!C405</f>
@@ -53938,37 +54065,37 @@
         <f>'Bowtie v1.0 reorg'!D405</f>
         <v>60050</v>
       </c>
-      <c r="E404" t="str">
+      <c r="E404">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F405),"",'Bowtie v1.0 reorg'!F405)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F404" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G405),"",'Bowtie v1.0 reorg'!G405)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G404" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I405),"",'Bowtie v1.0 reorg'!I405)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H404" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J405),"",'Bowtie v1.0 reorg'!J405)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I404" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H405),"",'Bowtie v1.0 reorg'!H405)</f>
-        <v/>
+        <v>shield</v>
       </c>
       <c r="J404" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K405),"",'Bowtie v1.0 reorg'!K405)</f>
-        <v/>
-      </c>
-      <c r="K404" t="e">
+        <v>Used in version control view of branches.</v>
+      </c>
+      <c r="K404" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L404" t="e">
+        <v>{'id':403,'name':'shield','unicode':'EA92','decimal':60050,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['shield'],'usage':'Used in version control view of branches.'}</v>
+      </c>
+      <c r="L404" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":403,"name":"shield","unicode":"EA92","decimal":60050,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["shield"],"usage":"Used in version control view of branches."}</v>
       </c>
     </row>
     <row r="405" spans="1:12" x14ac:dyDescent="0.25">
@@ -53976,9 +54103,9 @@
         <f>'Bowtie v1.0 reorg'!A406</f>
         <v>404</v>
       </c>
-      <c r="B405">
+      <c r="B405" t="str">
         <f>'Bowtie v1.0 reorg'!E406</f>
-        <v>0</v>
+        <v>shield-fill</v>
       </c>
       <c r="C405" t="str">
         <f>'Bowtie v1.0 reorg'!C406</f>
@@ -53988,37 +54115,37 @@
         <f>'Bowtie v1.0 reorg'!D406</f>
         <v>60051</v>
       </c>
-      <c r="E405" t="str">
+      <c r="E405">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F406),"",'Bowtie v1.0 reorg'!F406)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F405" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G406),"",'Bowtie v1.0 reorg'!G406)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G405" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I406),"",'Bowtie v1.0 reorg'!I406)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H405" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J406),"",'Bowtie v1.0 reorg'!J406)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I405" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H406),"",'Bowtie v1.0 reorg'!H406)</f>
-        <v/>
+        <v>shield</v>
       </c>
       <c r="J405" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K406),"",'Bowtie v1.0 reorg'!K406)</f>
-        <v/>
-      </c>
-      <c r="K405" t="e">
+        <v>Used in version control view of branches.</v>
+      </c>
+      <c r="K405" t="str">
         <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L405" t="e">
+        <v>{'id':404,'name':'shield-fill','unicode':'EA93','decimal':60051,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['shield'],'usage':'Used in version control view of branches.'}</v>
+      </c>
+      <c r="L405" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>{"id":404,"name":"shield-fill","unicode":"EA93","decimal":60051,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["shield"],"usage":"Used in version control view of branches."}</v>
       </c>
     </row>
     <row r="406" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added package feed icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -10,7 +10,7 @@
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId1"/>
     <sheet name="json" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="829">
   <si>
     <t>name</t>
   </si>
@@ -2477,12 +2477,42 @@
   </si>
   <si>
     <t>Add new team project.</t>
+  </si>
+  <si>
+    <t>package-feed-remote</t>
+  </si>
+  <si>
+    <t>package-feed-mix</t>
+  </si>
+  <si>
+    <t>package-feed-local</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds.</t>
+  </si>
+  <si>
+    <t>Used in Package hub treeview to represent package feed is a reference to remote repo.</t>
+  </si>
+  <si>
+    <t>Used in Package hub treeview to represent package feed is a local folder.</t>
+  </si>
+  <si>
+    <t>package feed mix box square</t>
+  </si>
+  <si>
+    <t>package feed local box square</t>
+  </si>
+  <si>
+    <t>package feed remote signal reference wave virtual box square</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -18120,6 +18150,120 @@
         <a:xfrm>
           <a:off x="1152525" y="164191950"/>
           <a:ext cx="200053" cy="200053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>412</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342929</xdr:colOff>
+      <xdr:row>412</xdr:row>
+      <xdr:rowOff>314354</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="409" name="Picture 408"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId408"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1076325" y="165411150"/>
+          <a:ext cx="209579" cy="209579"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>411</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381028</xdr:colOff>
+      <xdr:row>411</xdr:row>
+      <xdr:rowOff>314353</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="411" name="Picture 410"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId409"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1123950" y="165020625"/>
+          <a:ext cx="200053" cy="200053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>410</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361975</xdr:colOff>
+      <xdr:row>410</xdr:row>
+      <xdr:rowOff>285781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="412" name="Picture 411"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId410"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1123950" y="164572950"/>
+          <a:ext cx="181000" cy="219106"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18430,9 +18574,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A405" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C409" sqref="C409"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A406" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C411" sqref="C411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32424,9 +32568,30 @@
       <c r="D411">
         <v>60056</v>
       </c>
+      <c r="E411" t="s">
+        <v>820</v>
+      </c>
+      <c r="F411">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G411" t="s">
+        <v>17</v>
+      </c>
+      <c r="H411" t="s">
+        <v>826</v>
+      </c>
+      <c r="I411" t="s">
+        <v>15</v>
+      </c>
+      <c r="J411" t="s">
+        <v>822</v>
+      </c>
+      <c r="K411" t="s">
+        <v>823</v>
+      </c>
       <c r="L411" t="str">
         <f t="shared" si="13"/>
-        <v>uEA98-.svg</v>
+        <v>uEA98-package-feed-mix.svg</v>
       </c>
     </row>
     <row r="412" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32440,9 +32605,30 @@
       <c r="D412">
         <v>60057</v>
       </c>
+      <c r="E412" t="s">
+        <v>819</v>
+      </c>
+      <c r="F412">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G412" t="s">
+        <v>17</v>
+      </c>
+      <c r="H412" t="s">
+        <v>828</v>
+      </c>
+      <c r="I412" t="s">
+        <v>15</v>
+      </c>
+      <c r="J412" t="s">
+        <v>822</v>
+      </c>
+      <c r="K412" t="s">
+        <v>824</v>
+      </c>
       <c r="L412" t="str">
         <f t="shared" si="13"/>
-        <v>uEA99-.svg</v>
+        <v>uEA99-package-feed-remote.svg</v>
       </c>
     </row>
     <row r="413" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32456,9 +32642,30 @@
       <c r="D413">
         <v>60058</v>
       </c>
+      <c r="E413" t="s">
+        <v>821</v>
+      </c>
+      <c r="F413">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G413" t="s">
+        <v>17</v>
+      </c>
+      <c r="H413" t="s">
+        <v>827</v>
+      </c>
+      <c r="I413" t="s">
+        <v>15</v>
+      </c>
+      <c r="J413" t="s">
+        <v>822</v>
+      </c>
+      <c r="K413" t="s">
+        <v>825</v>
+      </c>
       <c r="L413" t="str">
         <f t="shared" si="13"/>
-        <v>uEA9A-.svg</v>
+        <v>uEA9A-package-feed-local.svg</v>
       </c>
     </row>
     <row r="414" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -33247,7 +33454,7 @@
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="F400" sqref="F400"/>
+      <selection activeCell="F405" sqref="F405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53699,9 +53906,9 @@
         <f>'Bowtie v1.0 reorg'!A411</f>
         <v>409</v>
       </c>
-      <c r="B410">
+      <c r="B410" t="str">
         <f>'Bowtie v1.0 reorg'!E411</f>
-        <v>0</v>
+        <v>package-feed-mix</v>
       </c>
       <c r="C410" t="str">
         <f>'Bowtie v1.0 reorg'!C411</f>
@@ -53711,37 +53918,37 @@
         <f>'Bowtie v1.0 reorg'!D411</f>
         <v>60056</v>
       </c>
-      <c r="E410" t="str">
+      <c r="E410">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F411),"",'Bowtie v1.0 reorg'!F411)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F410" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G411),"",'Bowtie v1.0 reorg'!G411)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G410" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I411),"",'Bowtie v1.0 reorg'!I411)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H410" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J411),"",'Bowtie v1.0 reorg'!J411)</f>
-        <v/>
+        <v>Package</v>
       </c>
       <c r="I410" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H411),"",'Bowtie v1.0 reorg'!H411)</f>
-        <v/>
+        <v>package feed mix box square</v>
       </c>
       <c r="J410" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K411),"",'Bowtie v1.0 reorg'!K411)</f>
-        <v/>
-      </c>
-      <c r="K410" t="e">
+        <v>Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds.</v>
+      </c>
+      <c r="K410" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L410" t="e">
+        <v>{'id':409,'name':'package-feed-mix','unicode':'EA98','decimal':60056,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','mix','box','square'],'usage':'Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds.'}</v>
+      </c>
+      <c r="L410" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":409,"name":"package-feed-mix","unicode":"EA98","decimal":60056,"version":"1.1","style":"light","subset":"VSTS","group":"Package","keywords":["package","feed","mix","box","square"],"usage":"Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds."}</v>
       </c>
     </row>
     <row r="411" spans="1:12" x14ac:dyDescent="0.25">
@@ -53749,9 +53956,9 @@
         <f>'Bowtie v1.0 reorg'!A412</f>
         <v>410</v>
       </c>
-      <c r="B411">
+      <c r="B411" t="str">
         <f>'Bowtie v1.0 reorg'!E412</f>
-        <v>0</v>
+        <v>package-feed-remote</v>
       </c>
       <c r="C411" t="str">
         <f>'Bowtie v1.0 reorg'!C412</f>
@@ -53761,37 +53968,37 @@
         <f>'Bowtie v1.0 reorg'!D412</f>
         <v>60057</v>
       </c>
-      <c r="E411" t="str">
+      <c r="E411">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F412),"",'Bowtie v1.0 reorg'!F412)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F411" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G412),"",'Bowtie v1.0 reorg'!G412)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G411" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I412),"",'Bowtie v1.0 reorg'!I412)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H411" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J412),"",'Bowtie v1.0 reorg'!J412)</f>
-        <v/>
+        <v>Package</v>
       </c>
       <c r="I411" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H412),"",'Bowtie v1.0 reorg'!H412)</f>
-        <v/>
+        <v>package feed remote signal reference wave virtual box square</v>
       </c>
       <c r="J411" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K412),"",'Bowtie v1.0 reorg'!K412)</f>
-        <v/>
-      </c>
-      <c r="K411" t="e">
+        <v>Used in Package hub treeview to represent package feed is a reference to remote repo.</v>
+      </c>
+      <c r="K411" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L411" t="e">
+        <v>{'id':410,'name':'package-feed-remote','unicode':'EA99','decimal':60057,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','remote','signal','reference','wave','virtual','box','square'],'usage':'Used in Package hub treeview to represent package feed is a reference to remote repo.'}</v>
+      </c>
+      <c r="L411" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":410,"name":"package-feed-remote","unicode":"EA99","decimal":60057,"version":"1.1","style":"light","subset":"VSTS","group":"Package","keywords":["package","feed","remote","signal","reference","wave","virtual","box","square"],"usage":"Used in Package hub treeview to represent package feed is a reference to remote repo."}</v>
       </c>
     </row>
     <row r="412" spans="1:12" x14ac:dyDescent="0.25">
@@ -53799,9 +54006,9 @@
         <f>'Bowtie v1.0 reorg'!A413</f>
         <v>411</v>
       </c>
-      <c r="B412">
+      <c r="B412" t="str">
         <f>'Bowtie v1.0 reorg'!E413</f>
-        <v>0</v>
+        <v>package-feed-local</v>
       </c>
       <c r="C412" t="str">
         <f>'Bowtie v1.0 reorg'!C413</f>
@@ -53811,37 +54018,37 @@
         <f>'Bowtie v1.0 reorg'!D413</f>
         <v>60058</v>
       </c>
-      <c r="E412" t="str">
+      <c r="E412">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F413),"",'Bowtie v1.0 reorg'!F413)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F412" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G413),"",'Bowtie v1.0 reorg'!G413)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G412" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I413),"",'Bowtie v1.0 reorg'!I413)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H412" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J413),"",'Bowtie v1.0 reorg'!J413)</f>
-        <v/>
+        <v>Package</v>
       </c>
       <c r="I412" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H413),"",'Bowtie v1.0 reorg'!H413)</f>
-        <v/>
+        <v>package feed local box square</v>
       </c>
       <c r="J412" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K413),"",'Bowtie v1.0 reorg'!K413)</f>
-        <v/>
-      </c>
-      <c r="K412" t="e">
+        <v>Used in Package hub treeview to represent package feed is a local folder.</v>
+      </c>
+      <c r="K412" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L412" t="e">
+        <v>{'id':411,'name':'package-feed-local','unicode':'EA9A','decimal':60058,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','local','box','square'],'usage':'Used in Package hub treeview to represent package feed is a local folder.'}</v>
+      </c>
+      <c r="L412" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":411,"name":"package-feed-local","unicode":"EA9A","decimal":60058,"version":"1.1","style":"light","subset":"VSTS","group":"Package","keywords":["package","feed","local","box","square"],"usage":"Used in Package hub treeview to represent package feed is a local folder."}</v>
       </c>
     </row>
     <row r="413" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added work item bar outline version
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -10,7 +10,7 @@
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId1"/>
     <sheet name="json" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="832">
   <si>
     <t>name</t>
   </si>
@@ -2507,12 +2507,21 @@
   </si>
   <si>
     <t>package feed remote signal reference wave virtual box square</t>
+  </si>
+  <si>
+    <t>work-item-bar-outline</t>
+  </si>
+  <si>
+    <t>work item bar</t>
+  </si>
+  <si>
+    <t>Used in Work hub backlog tree view to represent work items.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -18264,6 +18273,44 @@
         <a:xfrm>
           <a:off x="1123950" y="164572950"/>
           <a:ext cx="181000" cy="219106"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>413</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342925</xdr:colOff>
+      <xdr:row>413</xdr:row>
+      <xdr:rowOff>314352</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="413" name="Picture 412"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId411"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="165830250"/>
+          <a:ext cx="181000" cy="190527"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18576,7 +18623,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A406" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C411" sqref="C411"/>
+      <selection pane="bottomLeft" activeCell="E414" sqref="E414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32679,9 +32726,30 @@
       <c r="D414">
         <v>60059</v>
       </c>
+      <c r="E414" t="s">
+        <v>829</v>
+      </c>
+      <c r="F414">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G414" t="s">
+        <v>17</v>
+      </c>
+      <c r="H414" t="s">
+        <v>830</v>
+      </c>
+      <c r="I414" t="s">
+        <v>15</v>
+      </c>
+      <c r="J414" t="s">
+        <v>602</v>
+      </c>
+      <c r="K414" t="s">
+        <v>831</v>
+      </c>
       <c r="L414" t="str">
         <f t="shared" si="13"/>
-        <v>uEA9B-.svg</v>
+        <v>uEA9B-work-item-bar-outline.svg</v>
       </c>
     </row>
     <row r="415" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -33454,7 +33522,7 @@
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="F405" sqref="F405"/>
+      <selection activeCell="J407" sqref="J407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54056,9 +54124,9 @@
         <f>'Bowtie v1.0 reorg'!A414</f>
         <v>412</v>
       </c>
-      <c r="B413">
+      <c r="B413" t="str">
         <f>'Bowtie v1.0 reorg'!E414</f>
-        <v>0</v>
+        <v>work-item-bar-outline</v>
       </c>
       <c r="C413" t="str">
         <f>'Bowtie v1.0 reorg'!C414</f>
@@ -54068,37 +54136,37 @@
         <f>'Bowtie v1.0 reorg'!D414</f>
         <v>60059</v>
       </c>
-      <c r="E413" t="str">
+      <c r="E413">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F414),"",'Bowtie v1.0 reorg'!F414)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F413" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G414),"",'Bowtie v1.0 reorg'!G414)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G413" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I414),"",'Bowtie v1.0 reorg'!I414)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H413" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J414),"",'Bowtie v1.0 reorg'!J414)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="I413" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H414),"",'Bowtie v1.0 reorg'!H414)</f>
-        <v/>
+        <v>work item bar</v>
       </c>
       <c r="J413" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K414),"",'Bowtie v1.0 reorg'!K414)</f>
-        <v/>
-      </c>
-      <c r="K413" t="e">
+        <v>Used in Work hub backlog tree view to represent work items.</v>
+      </c>
+      <c r="K413" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L413" t="e">
+        <v>{'id':412,'name':'work-item-bar-outline','unicode':'EA9B','decimal':60059,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['work','item','bar'],'usage':'Used in Work hub backlog tree view to represent work items.'}</v>
+      </c>
+      <c r="L413" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":412,"name":"work-item-bar-outline","unicode":"EA9B","decimal":60059,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["work","item","bar"],"usage":"Used in Work hub backlog tree view to represent work items."}</v>
       </c>
     </row>
     <row r="414" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added sort-asc and sort-desc
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="837">
   <si>
     <t>name</t>
   </si>
@@ -2516,6 +2516,21 @@
   </si>
   <si>
     <t>Used in Work hub backlog tree view to represent work items.</t>
+  </si>
+  <si>
+    <t>sort-asc</t>
+  </si>
+  <si>
+    <t>sort-desc</t>
+  </si>
+  <si>
+    <t>sort alphabetically ascending arrow down letter</t>
+  </si>
+  <si>
+    <t>sort alphabetically descending arrow down letter</t>
+  </si>
+  <si>
+    <t>Used in ListView control sorting funcionality.</t>
   </si>
 </sst>
 </file>
@@ -18622,8 +18637,8 @@
   <dimension ref="A1:AL532"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A406" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E414" sqref="E414"/>
+      <pane ySplit="2" topLeftCell="A409" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H413" sqref="H413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32763,9 +32778,30 @@
       <c r="D415">
         <v>60060</v>
       </c>
+      <c r="E415" t="s">
+        <v>832</v>
+      </c>
+      <c r="F415">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G415" t="s">
+        <v>17</v>
+      </c>
+      <c r="H415" t="s">
+        <v>834</v>
+      </c>
+      <c r="I415" t="s">
+        <v>15</v>
+      </c>
+      <c r="J415" t="s">
+        <v>598</v>
+      </c>
+      <c r="K415" t="s">
+        <v>836</v>
+      </c>
       <c r="L415" t="str">
         <f t="shared" si="13"/>
-        <v>uEA9C-.svg</v>
+        <v>uEA9C-sort-asc.svg</v>
       </c>
     </row>
     <row r="416" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32779,9 +32815,30 @@
       <c r="D416">
         <v>60061</v>
       </c>
+      <c r="E416" t="s">
+        <v>833</v>
+      </c>
+      <c r="F416">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G416" t="s">
+        <v>17</v>
+      </c>
+      <c r="H416" t="s">
+        <v>835</v>
+      </c>
+      <c r="I416" t="s">
+        <v>15</v>
+      </c>
+      <c r="J416" t="s">
+        <v>598</v>
+      </c>
+      <c r="K416" t="s">
+        <v>836</v>
+      </c>
       <c r="L416" t="str">
         <f t="shared" si="13"/>
-        <v>uEA9D-.svg</v>
+        <v>uEA9D-sort-desc.svg</v>
       </c>
     </row>
     <row r="417" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -54174,9 +54231,9 @@
         <f>'Bowtie v1.0 reorg'!A415</f>
         <v>413</v>
       </c>
-      <c r="B414">
+      <c r="B414" t="str">
         <f>'Bowtie v1.0 reorg'!E415</f>
-        <v>0</v>
+        <v>sort-asc</v>
       </c>
       <c r="C414" t="str">
         <f>'Bowtie v1.0 reorg'!C415</f>
@@ -54186,37 +54243,37 @@
         <f>'Bowtie v1.0 reorg'!D415</f>
         <v>60060</v>
       </c>
-      <c r="E414" t="str">
+      <c r="E414">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F415),"",'Bowtie v1.0 reorg'!F415)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F414" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G415),"",'Bowtie v1.0 reorg'!G415)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G414" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I415),"",'Bowtie v1.0 reorg'!I415)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H414" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J415),"",'Bowtie v1.0 reorg'!J415)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I414" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H415),"",'Bowtie v1.0 reorg'!H415)</f>
-        <v/>
+        <v>sort alphabetically ascending arrow down letter</v>
       </c>
       <c r="J414" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K415),"",'Bowtie v1.0 reorg'!K415)</f>
-        <v/>
-      </c>
-      <c r="K414" t="e">
+        <v>Used in ListView control sorting funcionality.</v>
+      </c>
+      <c r="K414" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L414" t="e">
+        <v>{'id':413,'name':'sort-asc','unicode':'EA9C','decimal':60060,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['sort','alphabetically','ascending','arrow','down','letter'],'usage':'Used in ListView control sorting funcionality.'}</v>
+      </c>
+      <c r="L414" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":413,"name":"sort-asc","unicode":"EA9C","decimal":60060,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["sort","alphabetically","ascending","arrow","down","letter"],"usage":"Used in ListView control sorting funcionality."}</v>
       </c>
     </row>
     <row r="415" spans="1:12" x14ac:dyDescent="0.25">
@@ -54224,9 +54281,9 @@
         <f>'Bowtie v1.0 reorg'!A416</f>
         <v>414</v>
       </c>
-      <c r="B415">
+      <c r="B415" t="str">
         <f>'Bowtie v1.0 reorg'!E416</f>
-        <v>0</v>
+        <v>sort-desc</v>
       </c>
       <c r="C415" t="str">
         <f>'Bowtie v1.0 reorg'!C416</f>
@@ -54236,37 +54293,37 @@
         <f>'Bowtie v1.0 reorg'!D416</f>
         <v>60061</v>
       </c>
-      <c r="E415" t="str">
+      <c r="E415">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F416),"",'Bowtie v1.0 reorg'!F416)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F415" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G416),"",'Bowtie v1.0 reorg'!G416)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G415" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I416),"",'Bowtie v1.0 reorg'!I416)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H415" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J416),"",'Bowtie v1.0 reorg'!J416)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I415" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H416),"",'Bowtie v1.0 reorg'!H416)</f>
-        <v/>
+        <v>sort alphabetically descending arrow down letter</v>
       </c>
       <c r="J415" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K416),"",'Bowtie v1.0 reorg'!K416)</f>
-        <v/>
-      </c>
-      <c r="K415" t="e">
+        <v>Used in ListView control sorting funcionality.</v>
+      </c>
+      <c r="K415" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L415" t="e">
+        <v>{'id':414,'name':'sort-desc','unicode':'EA9D','decimal':60061,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['sort','alphabetically','descending','arrow','down','letter'],'usage':'Used in ListView control sorting funcionality.'}</v>
+      </c>
+      <c r="L415" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":414,"name":"sort-desc","unicode":"EA9D","decimal":60061,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["sort","alphabetically","descending","arrow","down","letter"],"usage":"Used in ListView control sorting funcionality."}</v>
       </c>
     </row>
     <row r="416" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added some new icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="850">
   <si>
     <t>name</t>
   </si>
@@ -2531,6 +2531,45 @@
   </si>
   <si>
     <t>Used in ListView control sorting funcionality.</t>
+  </si>
+  <si>
+    <t>plug-disconnected</t>
+  </si>
+  <si>
+    <t>plug-connected</t>
+  </si>
+  <si>
+    <t>plug-disconnected-fill</t>
+  </si>
+  <si>
+    <t>plug-connected-fill</t>
+  </si>
+  <si>
+    <t>plug disconnected unplug offline</t>
+  </si>
+  <si>
+    <t>plug connected plugged online</t>
+  </si>
+  <si>
+    <t>Indicate connection status.</t>
+  </si>
+  <si>
+    <t>sync-user</t>
+  </si>
+  <si>
+    <t>sync update user</t>
+  </si>
+  <si>
+    <t>Used in Backlog capacity editor for adding missing team members.</t>
+  </si>
+  <si>
+    <t>clear-filter</t>
+  </si>
+  <si>
+    <t>clear remove delete cancel filter funnel</t>
+  </si>
+  <si>
+    <t>Used in Code hub to clear applied filters.</t>
   </si>
 </sst>
 </file>
@@ -18326,6 +18365,310 @@
         <a:xfrm>
           <a:off x="1104900" y="165830250"/>
           <a:ext cx="181000" cy="190527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>414</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409606</xdr:colOff>
+      <xdr:row>414</xdr:row>
+      <xdr:rowOff>314361</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="414" name="Picture 413"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId412"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="166163625"/>
+          <a:ext cx="219106" cy="257211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>415</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419135</xdr:colOff>
+      <xdr:row>415</xdr:row>
+      <xdr:rowOff>314361</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="415" name="Picture 414"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId413"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="166563675"/>
+          <a:ext cx="247685" cy="257211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>416</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419131</xdr:colOff>
+      <xdr:row>416</xdr:row>
+      <xdr:rowOff>304833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="416" name="Picture 415"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId414"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="166973250"/>
+          <a:ext cx="219106" cy="238158"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>417</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352450</xdr:colOff>
+      <xdr:row>417</xdr:row>
+      <xdr:rowOff>314358</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="417" name="Picture 416"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId415"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="167382825"/>
+          <a:ext cx="181000" cy="238158"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>418</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361978</xdr:colOff>
+      <xdr:row>418</xdr:row>
+      <xdr:rowOff>333407</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="418" name="Picture 417"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId416"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="167811450"/>
+          <a:ext cx="200053" cy="228632"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>419</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381031</xdr:colOff>
+      <xdr:row>419</xdr:row>
+      <xdr:rowOff>295306</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="419" name="Picture 418"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId417"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="168182925"/>
+          <a:ext cx="219106" cy="219106"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>420</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>371503</xdr:colOff>
+      <xdr:row>420</xdr:row>
+      <xdr:rowOff>371510</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="420" name="Picture 419"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId418"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="168630600"/>
+          <a:ext cx="200053" cy="247685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>421</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381027</xdr:colOff>
+      <xdr:row>421</xdr:row>
+      <xdr:rowOff>333410</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="421" name="Picture 420"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId419"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="168992550"/>
+          <a:ext cx="190527" cy="247685"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -18636,9 +18979,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A409" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H413" sqref="H413"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A418" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E422" sqref="E422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32852,9 +33195,30 @@
       <c r="D417">
         <v>60062</v>
       </c>
+      <c r="E417" t="s">
+        <v>837</v>
+      </c>
+      <c r="F417">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G417" t="s">
+        <v>17</v>
+      </c>
+      <c r="H417" t="s">
+        <v>841</v>
+      </c>
+      <c r="I417" t="s">
+        <v>15</v>
+      </c>
+      <c r="J417" t="s">
+        <v>598</v>
+      </c>
+      <c r="K417" t="s">
+        <v>843</v>
+      </c>
       <c r="L417" t="str">
         <f t="shared" si="13"/>
-        <v>uEA9E-.svg</v>
+        <v>uEA9E-plug-disconnected.svg</v>
       </c>
     </row>
     <row r="418" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32868,9 +33232,30 @@
       <c r="D418">
         <v>60063</v>
       </c>
+      <c r="E418" t="s">
+        <v>838</v>
+      </c>
+      <c r="F418">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G418" t="s">
+        <v>17</v>
+      </c>
+      <c r="H418" t="s">
+        <v>842</v>
+      </c>
+      <c r="I418" t="s">
+        <v>15</v>
+      </c>
+      <c r="J418" t="s">
+        <v>598</v>
+      </c>
+      <c r="K418" t="s">
+        <v>843</v>
+      </c>
       <c r="L418" t="str">
         <f t="shared" si="13"/>
-        <v>uEA9F-.svg</v>
+        <v>uEA9F-plug-connected.svg</v>
       </c>
     </row>
     <row r="419" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32884,9 +33269,30 @@
       <c r="D419">
         <v>60064</v>
       </c>
+      <c r="E419" t="s">
+        <v>839</v>
+      </c>
+      <c r="F419">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G419" t="s">
+        <v>16</v>
+      </c>
+      <c r="H419" t="s">
+        <v>841</v>
+      </c>
+      <c r="I419" t="s">
+        <v>15</v>
+      </c>
+      <c r="J419" t="s">
+        <v>598</v>
+      </c>
+      <c r="K419" t="s">
+        <v>843</v>
+      </c>
       <c r="L419" t="str">
         <f t="shared" si="13"/>
-        <v>uEAA0-.svg</v>
+        <v>uEAA0-plug-disconnected-fill.svg</v>
       </c>
     </row>
     <row r="420" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32900,9 +33306,30 @@
       <c r="D420">
         <v>60065</v>
       </c>
+      <c r="E420" t="s">
+        <v>840</v>
+      </c>
+      <c r="F420">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G420" t="s">
+        <v>16</v>
+      </c>
+      <c r="H420" t="s">
+        <v>842</v>
+      </c>
+      <c r="I420" t="s">
+        <v>15</v>
+      </c>
+      <c r="J420" t="s">
+        <v>598</v>
+      </c>
+      <c r="K420" t="s">
+        <v>843</v>
+      </c>
       <c r="L420" t="str">
         <f t="shared" si="13"/>
-        <v>uEAA1-.svg</v>
+        <v>uEAA1-plug-connected-fill.svg</v>
       </c>
     </row>
     <row r="421" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32916,9 +33343,30 @@
       <c r="D421">
         <v>60066</v>
       </c>
+      <c r="E421" t="s">
+        <v>844</v>
+      </c>
+      <c r="F421">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G421" t="s">
+        <v>17</v>
+      </c>
+      <c r="H421" t="s">
+        <v>845</v>
+      </c>
+      <c r="I421" t="s">
+        <v>15</v>
+      </c>
+      <c r="J421" t="s">
+        <v>602</v>
+      </c>
+      <c r="K421" t="s">
+        <v>846</v>
+      </c>
       <c r="L421" t="str">
         <f t="shared" si="13"/>
-        <v>uEAA2-.svg</v>
+        <v>uEAA2-sync-user.svg</v>
       </c>
     </row>
     <row r="422" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32932,9 +33380,30 @@
       <c r="D422">
         <v>60067</v>
       </c>
+      <c r="E422" t="s">
+        <v>847</v>
+      </c>
+      <c r="F422">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G422" t="s">
+        <v>17</v>
+      </c>
+      <c r="H422" t="s">
+        <v>848</v>
+      </c>
+      <c r="I422" t="s">
+        <v>15</v>
+      </c>
+      <c r="J422" t="s">
+        <v>701</v>
+      </c>
+      <c r="K422" t="s">
+        <v>849</v>
+      </c>
       <c r="L422" t="str">
         <f t="shared" si="13"/>
-        <v>uEAA3-.svg</v>
+        <v>uEAA3-clear-filter.svg</v>
       </c>
     </row>
     <row r="423" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -33579,7 +34048,7 @@
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="J407" sqref="J407"/>
+      <selection activeCell="O412" sqref="O412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54331,9 +54800,9 @@
         <f>'Bowtie v1.0 reorg'!A417</f>
         <v>415</v>
       </c>
-      <c r="B416">
+      <c r="B416" t="str">
         <f>'Bowtie v1.0 reorg'!E417</f>
-        <v>0</v>
+        <v>plug-disconnected</v>
       </c>
       <c r="C416" t="str">
         <f>'Bowtie v1.0 reorg'!C417</f>
@@ -54343,37 +54812,37 @@
         <f>'Bowtie v1.0 reorg'!D417</f>
         <v>60062</v>
       </c>
-      <c r="E416" t="str">
+      <c r="E416">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F417),"",'Bowtie v1.0 reorg'!F417)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F416" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G417),"",'Bowtie v1.0 reorg'!G417)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G416" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I417),"",'Bowtie v1.0 reorg'!I417)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H416" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J417),"",'Bowtie v1.0 reorg'!J417)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I416" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H417),"",'Bowtie v1.0 reorg'!H417)</f>
-        <v/>
+        <v>plug disconnected unplug offline</v>
       </c>
       <c r="J416" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K417),"",'Bowtie v1.0 reorg'!K417)</f>
-        <v/>
-      </c>
-      <c r="K416" t="e">
+        <v>Indicate connection status.</v>
+      </c>
+      <c r="K416" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L416" t="e">
+        <v>{'id':415,'name':'plug-disconnected','unicode':'EA9E','decimal':60062,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['plug','disconnected','unplug','offline'],'usage':'Indicate connection status.'}</v>
+      </c>
+      <c r="L416" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":415,"name":"plug-disconnected","unicode":"EA9E","decimal":60062,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["plug","disconnected","unplug","offline"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
     <row r="417" spans="1:12" x14ac:dyDescent="0.25">
@@ -54381,9 +54850,9 @@
         <f>'Bowtie v1.0 reorg'!A418</f>
         <v>416</v>
       </c>
-      <c r="B417">
+      <c r="B417" t="str">
         <f>'Bowtie v1.0 reorg'!E418</f>
-        <v>0</v>
+        <v>plug-connected</v>
       </c>
       <c r="C417" t="str">
         <f>'Bowtie v1.0 reorg'!C418</f>
@@ -54393,37 +54862,37 @@
         <f>'Bowtie v1.0 reorg'!D418</f>
         <v>60063</v>
       </c>
-      <c r="E417" t="str">
+      <c r="E417">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F418),"",'Bowtie v1.0 reorg'!F418)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F417" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G418),"",'Bowtie v1.0 reorg'!G418)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G417" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I418),"",'Bowtie v1.0 reorg'!I418)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H417" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J418),"",'Bowtie v1.0 reorg'!J418)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I417" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H418),"",'Bowtie v1.0 reorg'!H418)</f>
-        <v/>
+        <v>plug connected plugged online</v>
       </c>
       <c r="J417" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K418),"",'Bowtie v1.0 reorg'!K418)</f>
-        <v/>
-      </c>
-      <c r="K417" t="e">
+        <v>Indicate connection status.</v>
+      </c>
+      <c r="K417" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L417" t="e">
+        <v>{'id':416,'name':'plug-connected','unicode':'EA9F','decimal':60063,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['plug','connected','plugged','online'],'usage':'Indicate connection status.'}</v>
+      </c>
+      <c r="L417" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":416,"name":"plug-connected","unicode":"EA9F","decimal":60063,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["plug","connected","plugged","online"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
     <row r="418" spans="1:12" x14ac:dyDescent="0.25">
@@ -54431,9 +54900,9 @@
         <f>'Bowtie v1.0 reorg'!A419</f>
         <v>417</v>
       </c>
-      <c r="B418">
+      <c r="B418" t="str">
         <f>'Bowtie v1.0 reorg'!E419</f>
-        <v>0</v>
+        <v>plug-disconnected-fill</v>
       </c>
       <c r="C418" t="str">
         <f>'Bowtie v1.0 reorg'!C419</f>
@@ -54443,37 +54912,37 @@
         <f>'Bowtie v1.0 reorg'!D419</f>
         <v>60064</v>
       </c>
-      <c r="E418" t="str">
+      <c r="E418">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F419),"",'Bowtie v1.0 reorg'!F419)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F418" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G419),"",'Bowtie v1.0 reorg'!G419)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G418" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I419),"",'Bowtie v1.0 reorg'!I419)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H418" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J419),"",'Bowtie v1.0 reorg'!J419)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I418" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H419),"",'Bowtie v1.0 reorg'!H419)</f>
-        <v/>
+        <v>plug disconnected unplug offline</v>
       </c>
       <c r="J418" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K419),"",'Bowtie v1.0 reorg'!K419)</f>
-        <v/>
-      </c>
-      <c r="K418" t="e">
+        <v>Indicate connection status.</v>
+      </c>
+      <c r="K418" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L418" t="e">
+        <v>{'id':417,'name':'plug-disconnected-fill','unicode':'EAA0','decimal':60064,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['plug','disconnected','unplug','offline'],'usage':'Indicate connection status.'}</v>
+      </c>
+      <c r="L418" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":417,"name":"plug-disconnected-fill","unicode":"EAA0","decimal":60064,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["plug","disconnected","unplug","offline"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
     <row r="419" spans="1:12" x14ac:dyDescent="0.25">
@@ -54481,9 +54950,9 @@
         <f>'Bowtie v1.0 reorg'!A420</f>
         <v>418</v>
       </c>
-      <c r="B419">
+      <c r="B419" t="str">
         <f>'Bowtie v1.0 reorg'!E420</f>
-        <v>0</v>
+        <v>plug-connected-fill</v>
       </c>
       <c r="C419" t="str">
         <f>'Bowtie v1.0 reorg'!C420</f>
@@ -54493,37 +54962,37 @@
         <f>'Bowtie v1.0 reorg'!D420</f>
         <v>60065</v>
       </c>
-      <c r="E419" t="str">
+      <c r="E419">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F420),"",'Bowtie v1.0 reorg'!F420)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F419" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G420),"",'Bowtie v1.0 reorg'!G420)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G419" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I420),"",'Bowtie v1.0 reorg'!I420)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H419" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J420),"",'Bowtie v1.0 reorg'!J420)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I419" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H420),"",'Bowtie v1.0 reorg'!H420)</f>
-        <v/>
+        <v>plug connected plugged online</v>
       </c>
       <c r="J419" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K420),"",'Bowtie v1.0 reorg'!K420)</f>
-        <v/>
-      </c>
-      <c r="K419" t="e">
+        <v>Indicate connection status.</v>
+      </c>
+      <c r="K419" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L419" t="e">
+        <v>{'id':418,'name':'plug-connected-fill','unicode':'EAA1','decimal':60065,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['plug','connected','plugged','online'],'usage':'Indicate connection status.'}</v>
+      </c>
+      <c r="L419" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":418,"name":"plug-connected-fill","unicode":"EAA1","decimal":60065,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["plug","connected","plugged","online"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
     <row r="420" spans="1:12" x14ac:dyDescent="0.25">
@@ -54531,9 +55000,9 @@
         <f>'Bowtie v1.0 reorg'!A421</f>
         <v>419</v>
       </c>
-      <c r="B420">
+      <c r="B420" t="str">
         <f>'Bowtie v1.0 reorg'!E421</f>
-        <v>0</v>
+        <v>sync-user</v>
       </c>
       <c r="C420" t="str">
         <f>'Bowtie v1.0 reorg'!C421</f>
@@ -54543,37 +55012,37 @@
         <f>'Bowtie v1.0 reorg'!D421</f>
         <v>60066</v>
       </c>
-      <c r="E420" t="str">
+      <c r="E420">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F421),"",'Bowtie v1.0 reorg'!F421)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F420" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G421),"",'Bowtie v1.0 reorg'!G421)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G420" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I421),"",'Bowtie v1.0 reorg'!I421)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H420" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J421),"",'Bowtie v1.0 reorg'!J421)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="I420" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H421),"",'Bowtie v1.0 reorg'!H421)</f>
-        <v/>
+        <v>sync update user</v>
       </c>
       <c r="J420" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K421),"",'Bowtie v1.0 reorg'!K421)</f>
-        <v/>
-      </c>
-      <c r="K420" t="e">
+        <v>Used in Backlog capacity editor for adding missing team members.</v>
+      </c>
+      <c r="K420" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L420" t="e">
+        <v>{'id':419,'name':'sync-user','unicode':'EAA2','decimal':60066,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['sync','update','user'],'usage':'Used in Backlog capacity editor for adding missing team members.'}</v>
+      </c>
+      <c r="L420" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":419,"name":"sync-user","unicode":"EAA2","decimal":60066,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["sync","update","user"],"usage":"Used in Backlog capacity editor for adding missing team members."}</v>
       </c>
     </row>
     <row r="421" spans="1:12" x14ac:dyDescent="0.25">
@@ -54581,9 +55050,9 @@
         <f>'Bowtie v1.0 reorg'!A422</f>
         <v>420</v>
       </c>
-      <c r="B421">
+      <c r="B421" t="str">
         <f>'Bowtie v1.0 reorg'!E422</f>
-        <v>0</v>
+        <v>clear-filter</v>
       </c>
       <c r="C421" t="str">
         <f>'Bowtie v1.0 reorg'!C422</f>
@@ -54593,37 +55062,37 @@
         <f>'Bowtie v1.0 reorg'!D422</f>
         <v>60067</v>
       </c>
-      <c r="E421" t="str">
+      <c r="E421">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F422),"",'Bowtie v1.0 reorg'!F422)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F421" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G422),"",'Bowtie v1.0 reorg'!G422)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G421" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I422),"",'Bowtie v1.0 reorg'!I422)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H421" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J422),"",'Bowtie v1.0 reorg'!J422)</f>
-        <v/>
+        <v>Code</v>
       </c>
       <c r="I421" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H422),"",'Bowtie v1.0 reorg'!H422)</f>
-        <v/>
+        <v>clear remove delete cancel filter funnel</v>
       </c>
       <c r="J421" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K422),"",'Bowtie v1.0 reorg'!K422)</f>
-        <v/>
-      </c>
-      <c r="K421" t="e">
+        <v>Used in Code hub to clear applied filters.</v>
+      </c>
+      <c r="K421" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L421" t="e">
+        <v>{'id':420,'name':'clear-filter','unicode':'EAA3','decimal':60067,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['clear','remove','delete','cancel','filter','funnel'],'usage':'Used in Code hub to clear applied filters.'}</v>
+      </c>
+      <c r="L421" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":420,"name":"clear-filter","unicode":"EAA3","decimal":60067,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["clear","remove","delete","cancel","filter","funnel"],"usage":"Used in Code hub to clear applied filters."}</v>
       </c>
     </row>
     <row r="422" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added new icons; added tasks for exporting some common format pngs
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="858">
   <si>
     <t>name</t>
   </si>
@@ -2570,6 +2570,30 @@
   </si>
   <si>
     <t>Used in Code hub to clear applied filters.</t>
+  </si>
+  <si>
+    <t>watch-eye-off</t>
+  </si>
+  <si>
+    <t>watch eye follow off slash</t>
+  </si>
+  <si>
+    <t>Used for turning off follow on an work item.</t>
+  </si>
+  <si>
+    <t>shopping-cart</t>
+  </si>
+  <si>
+    <t>shopping-cart-fill</t>
+  </si>
+  <si>
+    <t>shop cart buy purchase store</t>
+  </si>
+  <si>
+    <t>VSCOM</t>
+  </si>
+  <si>
+    <t>Use this version when shopping cart needs two states: empty and filled</t>
   </si>
 </sst>
 </file>
@@ -18979,9 +19003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A418" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E422" sqref="E422"/>
+      <selection pane="bottomLeft" activeCell="H431" sqref="H431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -33417,9 +33441,30 @@
       <c r="D423">
         <v>60068</v>
       </c>
+      <c r="E423" t="s">
+        <v>850</v>
+      </c>
+      <c r="F423">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G423" t="s">
+        <v>17</v>
+      </c>
+      <c r="H423" t="s">
+        <v>851</v>
+      </c>
+      <c r="I423" t="s">
+        <v>15</v>
+      </c>
+      <c r="J423" t="s">
+        <v>602</v>
+      </c>
+      <c r="K423" t="s">
+        <v>852</v>
+      </c>
       <c r="L423" t="str">
         <f t="shared" si="13"/>
-        <v>uEAA4-.svg</v>
+        <v>uEAA4-watch-eye-off.svg</v>
       </c>
     </row>
     <row r="424" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -33433,9 +33478,30 @@
       <c r="D424">
         <v>60069</v>
       </c>
+      <c r="E424" t="s">
+        <v>853</v>
+      </c>
+      <c r="F424">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G424" t="s">
+        <v>17</v>
+      </c>
+      <c r="H424" t="s">
+        <v>855</v>
+      </c>
+      <c r="I424" t="s">
+        <v>856</v>
+      </c>
+      <c r="J424" t="s">
+        <v>598</v>
+      </c>
+      <c r="K424" t="s">
+        <v>857</v>
+      </c>
       <c r="L424" t="str">
         <f t="shared" si="13"/>
-        <v>uEAA5-.svg</v>
+        <v>uEAA5-shopping-cart.svg</v>
       </c>
     </row>
     <row r="425" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -33449,9 +33515,30 @@
       <c r="D425">
         <v>60070</v>
       </c>
+      <c r="E425" t="s">
+        <v>854</v>
+      </c>
+      <c r="F425">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G425" t="s">
+        <v>17</v>
+      </c>
+      <c r="H425" t="s">
+        <v>855</v>
+      </c>
+      <c r="I425" t="s">
+        <v>856</v>
+      </c>
+      <c r="J425" t="s">
+        <v>598</v>
+      </c>
+      <c r="K425" t="s">
+        <v>857</v>
+      </c>
       <c r="L425" t="str">
         <f t="shared" si="13"/>
-        <v>uEAA6-.svg</v>
+        <v>uEAA6-shopping-cart-fill.svg</v>
       </c>
     </row>
     <row r="426" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -34047,8 +34134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="O412" sqref="O412"/>
+    <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
+      <selection activeCell="L424" sqref="L423:L424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55100,9 +55187,9 @@
         <f>'Bowtie v1.0 reorg'!A423</f>
         <v>421</v>
       </c>
-      <c r="B422">
+      <c r="B422" t="str">
         <f>'Bowtie v1.0 reorg'!E423</f>
-        <v>0</v>
+        <v>watch-eye-off</v>
       </c>
       <c r="C422" t="str">
         <f>'Bowtie v1.0 reorg'!C423</f>
@@ -55112,37 +55199,37 @@
         <f>'Bowtie v1.0 reorg'!D423</f>
         <v>60068</v>
       </c>
-      <c r="E422" t="str">
+      <c r="E422">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F423),"",'Bowtie v1.0 reorg'!F423)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F422" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G423),"",'Bowtie v1.0 reorg'!G423)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G422" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I423),"",'Bowtie v1.0 reorg'!I423)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H422" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J423),"",'Bowtie v1.0 reorg'!J423)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="I422" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H423),"",'Bowtie v1.0 reorg'!H423)</f>
-        <v/>
+        <v>watch eye follow off slash</v>
       </c>
       <c r="J422" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K423),"",'Bowtie v1.0 reorg'!K423)</f>
-        <v/>
-      </c>
-      <c r="K422" t="e">
+        <v>Used for turning off follow on an work item.</v>
+      </c>
+      <c r="K422" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L422" t="e">
+        <v>{'id':421,'name':'watch-eye-off','unicode':'EAA4','decimal':60068,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['watch','eye','follow','off','slash'],'usage':'Used for turning off follow on an work item.'}</v>
+      </c>
+      <c r="L422" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":421,"name":"watch-eye-off","unicode":"EAA4","decimal":60068,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["watch","eye","follow","off","slash"],"usage":"Used for turning off follow on an work item."}</v>
       </c>
     </row>
     <row r="423" spans="1:12" x14ac:dyDescent="0.25">
@@ -55150,9 +55237,9 @@
         <f>'Bowtie v1.0 reorg'!A424</f>
         <v>422</v>
       </c>
-      <c r="B423">
+      <c r="B423" t="str">
         <f>'Bowtie v1.0 reorg'!E424</f>
-        <v>0</v>
+        <v>shopping-cart</v>
       </c>
       <c r="C423" t="str">
         <f>'Bowtie v1.0 reorg'!C424</f>
@@ -55162,37 +55249,37 @@
         <f>'Bowtie v1.0 reorg'!D424</f>
         <v>60069</v>
       </c>
-      <c r="E423" t="str">
+      <c r="E423">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F424),"",'Bowtie v1.0 reorg'!F424)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F423" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G424),"",'Bowtie v1.0 reorg'!G424)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G423" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I424),"",'Bowtie v1.0 reorg'!I424)</f>
-        <v/>
+        <v>VSCOM</v>
       </c>
       <c r="H423" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J424),"",'Bowtie v1.0 reorg'!J424)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I423" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H424),"",'Bowtie v1.0 reorg'!H424)</f>
-        <v/>
+        <v>shop cart buy purchase store</v>
       </c>
       <c r="J423" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K424),"",'Bowtie v1.0 reorg'!K424)</f>
-        <v/>
-      </c>
-      <c r="K423" t="e">
+        <v>Use this version when shopping cart needs two states: empty and filled</v>
+      </c>
+      <c r="K423" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L423" t="e">
+        <v>{'id':422,'name':'shopping-cart','unicode':'EAA5','decimal':60069,'version':'1.1','style':'light','subset':'VSCOM','group':'Common','keywords':['shop','cart','buy','purchase','store'],'usage':'Use this version when shopping cart needs two states: empty and filled'}</v>
+      </c>
+      <c r="L423" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":422,"name":"shopping-cart","unicode":"EAA5","decimal":60069,"version":"1.1","style":"light","subset":"VSCOM","group":"Common","keywords":["shop","cart","buy","purchase","store"],"usage":"Use this version when shopping cart needs two states: empty and filled"}</v>
       </c>
     </row>
     <row r="424" spans="1:12" x14ac:dyDescent="0.25">
@@ -55200,9 +55287,9 @@
         <f>'Bowtie v1.0 reorg'!A425</f>
         <v>423</v>
       </c>
-      <c r="B424">
+      <c r="B424" t="str">
         <f>'Bowtie v1.0 reorg'!E425</f>
-        <v>0</v>
+        <v>shopping-cart-fill</v>
       </c>
       <c r="C424" t="str">
         <f>'Bowtie v1.0 reorg'!C425</f>
@@ -55212,37 +55299,37 @@
         <f>'Bowtie v1.0 reorg'!D425</f>
         <v>60070</v>
       </c>
-      <c r="E424" t="str">
+      <c r="E424">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F425),"",'Bowtie v1.0 reorg'!F425)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F424" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G425),"",'Bowtie v1.0 reorg'!G425)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G424" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I425),"",'Bowtie v1.0 reorg'!I425)</f>
-        <v/>
+        <v>VSCOM</v>
       </c>
       <c r="H424" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J425),"",'Bowtie v1.0 reorg'!J425)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I424" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H425),"",'Bowtie v1.0 reorg'!H425)</f>
-        <v/>
+        <v>shop cart buy purchase store</v>
       </c>
       <c r="J424" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K425),"",'Bowtie v1.0 reorg'!K425)</f>
-        <v/>
-      </c>
-      <c r="K424" t="e">
+        <v>Use this version when shopping cart needs two states: empty and filled</v>
+      </c>
+      <c r="K424" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L424" t="e">
+        <v>{'id':423,'name':'shopping-cart-fill','unicode':'EAA6','decimal':60070,'version':'1.1','style':'light','subset':'VSCOM','group':'Common','keywords':['shop','cart','buy','purchase','store'],'usage':'Use this version when shopping cart needs two states: empty and filled'}</v>
+      </c>
+      <c r="L424" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":423,"name":"shopping-cart-fill","unicode":"EAA6","decimal":60070,"version":"1.1","style":"light","subset":"VSCOM","group":"Common","keywords":["shop","cart","buy","purchase","store"],"usage":"Use this version when shopping cart needs two states: empty and filled"}</v>
       </c>
     </row>
     <row r="425" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added new icon engineering-group
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720" activeTab="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="896">
   <si>
     <t>name</t>
   </si>
@@ -2696,6 +2696,18 @@
   </si>
   <si>
     <t>Used in Release hub for task group.</t>
+  </si>
+  <si>
+    <t>Used in Build &amp; Release hub to represent a group of task.</t>
+  </si>
+  <si>
+    <t>engineering-group</t>
+  </si>
+  <si>
+    <t>engineering group loop organization chart schema</t>
+  </si>
+  <si>
+    <t>Used in Compliance hub for Engineering Group node dropdown.</t>
   </si>
 </sst>
 </file>
@@ -22153,9 +22165,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A431" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I437" sqref="I437"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A434" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E438" sqref="E438"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37109,9 +37121,30 @@
       <c r="D437">
         <v>60082</v>
       </c>
+      <c r="E437" t="s">
+        <v>889</v>
+      </c>
+      <c r="F437">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G437" t="s">
+        <v>17</v>
+      </c>
+      <c r="H437" t="s">
+        <v>890</v>
+      </c>
+      <c r="I437" t="s">
+        <v>15</v>
+      </c>
+      <c r="J437" t="s">
+        <v>597</v>
+      </c>
+      <c r="K437" t="s">
+        <v>892</v>
+      </c>
       <c r="L437" t="str">
         <f t="shared" si="13"/>
-        <v>uEAB2-.svg</v>
+        <v>uEAB2-task-group.svg</v>
       </c>
     </row>
     <row r="438" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37125,9 +37158,30 @@
       <c r="D438">
         <v>60083</v>
       </c>
+      <c r="E438" t="s">
+        <v>893</v>
+      </c>
+      <c r="F438">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G438" t="s">
+        <v>16</v>
+      </c>
+      <c r="H438" t="s">
+        <v>894</v>
+      </c>
+      <c r="I438" t="s">
+        <v>15</v>
+      </c>
+      <c r="J438" t="s">
+        <v>688</v>
+      </c>
+      <c r="K438" t="s">
+        <v>895</v>
+      </c>
       <c r="L438" t="str">
         <f t="shared" si="13"/>
-        <v>uEAB3-.svg</v>
+        <v>uEAB3-engineering-group.svg</v>
       </c>
     </row>
     <row r="439" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37530,8 +37584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
-      <selection activeCell="L436" sqref="L436"/>
+    <sheetView tabSelected="1" topLeftCell="A424" workbookViewId="0">
+      <selection activeCell="F431" sqref="F431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59326,9 +59380,9 @@
         <f>'Bowtie v1.0 reorg'!A438</f>
         <v>436</v>
       </c>
-      <c r="B437">
+      <c r="B437" t="str">
         <f>'Bowtie v1.0 reorg'!E438</f>
-        <v>0</v>
+        <v>engineering-group</v>
       </c>
       <c r="C437" t="str">
         <f>'Bowtie v1.0 reorg'!C438</f>
@@ -59338,37 +59392,37 @@
         <f>'Bowtie v1.0 reorg'!D438</f>
         <v>60083</v>
       </c>
-      <c r="E437" t="str">
+      <c r="E437">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F438),"",'Bowtie v1.0 reorg'!F438)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F437" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G438),"",'Bowtie v1.0 reorg'!G438)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G437" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I438),"",'Bowtie v1.0 reorg'!I438)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H437" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J438),"",'Bowtie v1.0 reorg'!J438)</f>
-        <v/>
+        <v>Compliance</v>
       </c>
       <c r="I437" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H438),"",'Bowtie v1.0 reorg'!H438)</f>
-        <v/>
+        <v>engineering group loop organization chart schema</v>
       </c>
       <c r="J437" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K438),"",'Bowtie v1.0 reorg'!K438)</f>
-        <v/>
-      </c>
-      <c r="K437" t="e">
+        <v>Used in Compliance hub for Engineering Group node dropdown.</v>
+      </c>
+      <c r="K437" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L437" t="e">
+        <v>{'id':436,'name':'engineering-group','unicode':'EAB3','decimal':60083,'version':'1.1','style':'bold','subset':'VSTS','group':'Compliance','keywords':['engineering','group','loop','organization','chart','schema'],'usage':'Used in Compliance hub for Engineering Group node dropdown.'}</v>
+      </c>
+      <c r="L437" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":436,"name":"engineering-group","unicode":"EAB3","decimal":60083,"version":"1.1","style":"bold","subset":"VSTS","group":"Compliance","keywords":["engineering","group","loop","organization","chart","schema"],"usage":"Used in Compliance hub for Engineering Group node dropdown."}</v>
       </c>
     </row>
     <row r="438" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed output png default color to #222222; added new icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="902">
   <si>
     <t>name</t>
   </si>
@@ -2708,6 +2708,24 @@
   </si>
   <si>
     <t>Used in Compliance hub for Engineering Group node dropdown.</t>
+  </si>
+  <si>
+    <t>briefcase</t>
+  </si>
+  <si>
+    <t>briefcase project container</t>
+  </si>
+  <si>
+    <t>Used for team project.</t>
+  </si>
+  <si>
+    <t>variable-group</t>
+  </si>
+  <si>
+    <t>variable group parameter x letter brackets</t>
+  </si>
+  <si>
+    <t>Variable group is a group of configuration variables which can be used in deployments across build and release.</t>
   </si>
 </sst>
 </file>
@@ -22166,8 +22184,8 @@
   <dimension ref="A1:AL532"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A434" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E438" sqref="E438"/>
+      <pane ySplit="2" topLeftCell="A435" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F440" sqref="F440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37195,9 +37213,30 @@
       <c r="D439">
         <v>60084</v>
       </c>
+      <c r="E439" t="s">
+        <v>896</v>
+      </c>
+      <c r="F439">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G439" t="s">
+        <v>17</v>
+      </c>
+      <c r="H439" t="s">
+        <v>897</v>
+      </c>
+      <c r="I439" t="s">
+        <v>15</v>
+      </c>
+      <c r="J439" t="s">
+        <v>598</v>
+      </c>
+      <c r="K439" t="s">
+        <v>898</v>
+      </c>
       <c r="L439" t="str">
         <f t="shared" si="13"/>
-        <v>uEAB4-.svg</v>
+        <v>uEAB4-briefcase.svg</v>
       </c>
     </row>
     <row r="440" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37206,11 +37245,35 @@
       </c>
       <c r="C440" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EAB5</v>
+      </c>
+      <c r="D440">
+        <v>60085</v>
+      </c>
+      <c r="E440" t="s">
+        <v>899</v>
+      </c>
+      <c r="F440">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G440" t="s">
+        <v>17</v>
+      </c>
+      <c r="H440" t="s">
+        <v>900</v>
+      </c>
+      <c r="I440" t="s">
+        <v>15</v>
+      </c>
+      <c r="J440" t="s">
+        <v>582</v>
+      </c>
+      <c r="K440" t="s">
+        <v>901</v>
       </c>
       <c r="L440" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEAB5-variable-group.svg</v>
       </c>
     </row>
     <row r="441" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37219,11 +37282,14 @@
       </c>
       <c r="C441" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EAB6</v>
+      </c>
+      <c r="D441">
+        <v>60086</v>
       </c>
       <c r="L441" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEAB6-.svg</v>
       </c>
     </row>
     <row r="442" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37232,11 +37298,14 @@
       </c>
       <c r="C442" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EAB7</v>
+      </c>
+      <c r="D442">
+        <v>60087</v>
       </c>
       <c r="L442" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEAB7-.svg</v>
       </c>
     </row>
     <row r="443" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37245,11 +37314,14 @@
       </c>
       <c r="C443" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EAB8</v>
+      </c>
+      <c r="D443">
+        <v>60088</v>
       </c>
       <c r="L443" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEAB8-.svg</v>
       </c>
     </row>
     <row r="444" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37258,11 +37330,14 @@
       </c>
       <c r="C444" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EAB9</v>
+      </c>
+      <c r="D444">
+        <v>60089</v>
       </c>
       <c r="L444" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEAB9-.svg</v>
       </c>
     </row>
     <row r="445" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37271,11 +37346,14 @@
       </c>
       <c r="C445" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EABA</v>
+      </c>
+      <c r="D445">
+        <v>60090</v>
       </c>
       <c r="L445" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEABA-.svg</v>
       </c>
     </row>
     <row r="446" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37284,11 +37362,14 @@
       </c>
       <c r="C446" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EABB</v>
+      </c>
+      <c r="D446">
+        <v>60091</v>
       </c>
       <c r="L446" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEABB-.svg</v>
       </c>
     </row>
     <row r="447" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37297,11 +37378,14 @@
       </c>
       <c r="C447" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EABC</v>
+      </c>
+      <c r="D447">
+        <v>60092</v>
       </c>
       <c r="L447" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEABC-.svg</v>
       </c>
     </row>
     <row r="448" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37310,11 +37394,14 @@
       </c>
       <c r="C448" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EABD</v>
+      </c>
+      <c r="D448">
+        <v>60093</v>
       </c>
       <c r="L448" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEABD-.svg</v>
       </c>
     </row>
     <row r="449" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37323,11 +37410,14 @@
       </c>
       <c r="C449" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EABE</v>
+      </c>
+      <c r="D449">
+        <v>60094</v>
       </c>
       <c r="L449" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEABE-.svg</v>
       </c>
     </row>
     <row r="450" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37336,11 +37426,14 @@
       </c>
       <c r="C450" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>EABF</v>
+      </c>
+      <c r="D450">
+        <v>60095</v>
       </c>
       <c r="L450" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEABF-.svg</v>
       </c>
     </row>
     <row r="451" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37349,11 +37442,14 @@
       </c>
       <c r="C451" t="str">
         <f t="shared" ref="C451:C454" si="15">DEC2HEX(D451)</f>
-        <v>0</v>
+        <v>EAC0</v>
+      </c>
+      <c r="D451">
+        <v>60096</v>
       </c>
       <c r="L451" t="str">
         <f t="shared" si="13"/>
-        <v>u0-.svg</v>
+        <v>uEAC0-.svg</v>
       </c>
     </row>
     <row r="452" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37362,11 +37458,14 @@
       </c>
       <c r="C452" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EAC1</v>
+      </c>
+      <c r="D452">
+        <v>60097</v>
       </c>
       <c r="L452" t="str">
-        <f t="shared" ref="L452:L464" si="16">CONCATENATE("u",C452,"-",E452,".svg")</f>
-        <v>u0-.svg</v>
+        <f t="shared" ref="L452:L466" si="16">CONCATENATE("u",C452,"-",E452,".svg")</f>
+        <v>uEAC1-.svg</v>
       </c>
     </row>
     <row r="453" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37375,11 +37474,14 @@
       </c>
       <c r="C453" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EAC2</v>
+      </c>
+      <c r="D453">
+        <v>60098</v>
       </c>
       <c r="L453" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEAC2-.svg</v>
       </c>
     </row>
     <row r="454" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37388,17 +37490,23 @@
       </c>
       <c r="C454" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EAC3</v>
+      </c>
+      <c r="D454">
+        <v>60099</v>
       </c>
       <c r="L454" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEAC3-.svg</v>
       </c>
     </row>
     <row r="455" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>453</v>
       </c>
+      <c r="D455">
+        <v>60100</v>
+      </c>
       <c r="L455" t="str">
         <f t="shared" si="16"/>
         <v>u-.svg</v>
@@ -37408,6 +37516,9 @@
       <c r="A456">
         <v>454</v>
       </c>
+      <c r="D456">
+        <v>60101</v>
+      </c>
       <c r="L456" t="str">
         <f t="shared" si="16"/>
         <v>u-.svg</v>
@@ -37417,6 +37528,9 @@
       <c r="A457">
         <v>455</v>
       </c>
+      <c r="D457">
+        <v>60102</v>
+      </c>
       <c r="L457" t="str">
         <f t="shared" si="16"/>
         <v>u-.svg</v>
@@ -37426,6 +37540,9 @@
       <c r="A458">
         <v>456</v>
       </c>
+      <c r="D458">
+        <v>60103</v>
+      </c>
       <c r="L458" t="str">
         <f t="shared" si="16"/>
         <v>u-.svg</v>
@@ -37485,38 +37602,46 @@
         <v>u-.svg</v>
       </c>
     </row>
-    <row r="465" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>463</v>
       </c>
-    </row>
-    <row r="466" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L465" t="str">
+        <f t="shared" si="16"/>
+        <v>u-.svg</v>
+      </c>
+    </row>
+    <row r="466" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>464</v>
       </c>
-    </row>
-    <row r="467" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L466" t="str">
+        <f t="shared" si="16"/>
+        <v>u-.svg</v>
+      </c>
+    </row>
+    <row r="467" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>465</v>
       </c>
     </row>
-    <row r="468" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>466</v>
       </c>
     </row>
-    <row r="469" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" spans="1:1" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="481" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="482" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="483" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37584,8 +37709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A424" workbookViewId="0">
-      <selection activeCell="F431" sqref="F431"/>
+    <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
+      <selection activeCell="H440" sqref="H440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59430,9 +59555,9 @@
         <f>'Bowtie v1.0 reorg'!A439</f>
         <v>437</v>
       </c>
-      <c r="B438">
+      <c r="B438" t="str">
         <f>'Bowtie v1.0 reorg'!E439</f>
-        <v>0</v>
+        <v>briefcase</v>
       </c>
       <c r="C438" t="str">
         <f>'Bowtie v1.0 reorg'!C439</f>
@@ -59442,37 +59567,37 @@
         <f>'Bowtie v1.0 reorg'!D439</f>
         <v>60084</v>
       </c>
-      <c r="E438" t="str">
+      <c r="E438">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F439),"",'Bowtie v1.0 reorg'!F439)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F438" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G439),"",'Bowtie v1.0 reorg'!G439)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G438" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I439),"",'Bowtie v1.0 reorg'!I439)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H438" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J439),"",'Bowtie v1.0 reorg'!J439)</f>
-        <v/>
+        <v>Common</v>
       </c>
       <c r="I438" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H439),"",'Bowtie v1.0 reorg'!H439)</f>
-        <v/>
+        <v>briefcase project container</v>
       </c>
       <c r="J438" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K439),"",'Bowtie v1.0 reorg'!K439)</f>
-        <v/>
-      </c>
-      <c r="K438" t="e">
+        <v>Used for team project.</v>
+      </c>
+      <c r="K438" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L438" t="e">
+        <v>{'id':437,'name':'briefcase','unicode':'EAB4','decimal':60084,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['briefcase','project','container'],'usage':'Used for team project.'}</v>
+      </c>
+      <c r="L438" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":437,"name":"briefcase","unicode":"EAB4","decimal":60084,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["briefcase","project","container"],"usage":"Used for team project."}</v>
       </c>
     </row>
     <row r="439" spans="1:12" x14ac:dyDescent="0.25">
@@ -59480,49 +59605,49 @@
         <f>'Bowtie v1.0 reorg'!A440</f>
         <v>438</v>
       </c>
-      <c r="B439">
+      <c r="B439" t="str">
         <f>'Bowtie v1.0 reorg'!E440</f>
-        <v>0</v>
+        <v>variable-group</v>
       </c>
       <c r="C439" t="str">
         <f>'Bowtie v1.0 reorg'!C440</f>
-        <v>0</v>
+        <v>EAB5</v>
       </c>
       <c r="D439">
         <f>'Bowtie v1.0 reorg'!D440</f>
-        <v>0</v>
-      </c>
-      <c r="E439" t="str">
+        <v>60085</v>
+      </c>
+      <c r="E439">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F440),"",'Bowtie v1.0 reorg'!F440)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F439" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G440),"",'Bowtie v1.0 reorg'!G440)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G439" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I440),"",'Bowtie v1.0 reorg'!I440)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H439" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J440),"",'Bowtie v1.0 reorg'!J440)</f>
-        <v/>
+        <v>Test</v>
       </c>
       <c r="I439" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H440),"",'Bowtie v1.0 reorg'!H440)</f>
-        <v/>
+        <v>variable group parameter x letter brackets</v>
       </c>
       <c r="J439" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K440),"",'Bowtie v1.0 reorg'!K440)</f>
-        <v/>
-      </c>
-      <c r="K439" t="e">
+        <v>Variable group is a group of configuration variables which can be used in deployments across build and release.</v>
+      </c>
+      <c r="K439" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L439" t="e">
+        <v>{'id':438,'name':'variable-group','unicode':'EAB5','decimal':60085,'version':'1.1','style':'light','subset':'VSTS','group':'Test','keywords':['variable','group','parameter','x','letter','brackets'],'usage':'Variable group is a group of configuration variables which can be used in deployments across build and release.'}</v>
+      </c>
+      <c r="L439" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":438,"name":"variable-group","unicode":"EAB5","decimal":60085,"version":"1.1","style":"light","subset":"VSTS","group":"Test","keywords":["variable","group","parameter","x","letter","brackets"],"usage":"Variable group is a group of configuration variables which can be used in deployments across build and release."}</v>
       </c>
     </row>
     <row r="440" spans="1:12" x14ac:dyDescent="0.25">
@@ -59536,11 +59661,11 @@
       </c>
       <c r="C440" t="str">
         <f>'Bowtie v1.0 reorg'!C441</f>
-        <v>0</v>
+        <v>EAB6</v>
       </c>
       <c r="D440">
         <f>'Bowtie v1.0 reorg'!D441</f>
-        <v>0</v>
+        <v>60086</v>
       </c>
       <c r="E440" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F441),"",'Bowtie v1.0 reorg'!F441)</f>
@@ -59586,11 +59711,11 @@
       </c>
       <c r="C441" t="str">
         <f>'Bowtie v1.0 reorg'!C442</f>
-        <v>0</v>
+        <v>EAB7</v>
       </c>
       <c r="D441">
         <f>'Bowtie v1.0 reorg'!D442</f>
-        <v>0</v>
+        <v>60087</v>
       </c>
       <c r="E441" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F442),"",'Bowtie v1.0 reorg'!F442)</f>
@@ -59636,11 +59761,11 @@
       </c>
       <c r="C442" t="str">
         <f>'Bowtie v1.0 reorg'!C443</f>
-        <v>0</v>
+        <v>EAB8</v>
       </c>
       <c r="D442">
         <f>'Bowtie v1.0 reorg'!D443</f>
-        <v>0</v>
+        <v>60088</v>
       </c>
       <c r="E442" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F443),"",'Bowtie v1.0 reorg'!F443)</f>
@@ -59686,11 +59811,11 @@
       </c>
       <c r="C443" t="str">
         <f>'Bowtie v1.0 reorg'!C444</f>
-        <v>0</v>
+        <v>EAB9</v>
       </c>
       <c r="D443">
         <f>'Bowtie v1.0 reorg'!D444</f>
-        <v>0</v>
+        <v>60089</v>
       </c>
       <c r="E443" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F444),"",'Bowtie v1.0 reorg'!F444)</f>
@@ -59736,11 +59861,11 @@
       </c>
       <c r="C444" t="str">
         <f>'Bowtie v1.0 reorg'!C445</f>
-        <v>0</v>
+        <v>EABA</v>
       </c>
       <c r="D444">
         <f>'Bowtie v1.0 reorg'!D445</f>
-        <v>0</v>
+        <v>60090</v>
       </c>
       <c r="E444" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F445),"",'Bowtie v1.0 reorg'!F445)</f>
@@ -59786,11 +59911,11 @@
       </c>
       <c r="C445" t="str">
         <f>'Bowtie v1.0 reorg'!C446</f>
-        <v>0</v>
+        <v>EABB</v>
       </c>
       <c r="D445">
         <f>'Bowtie v1.0 reorg'!D446</f>
-        <v>0</v>
+        <v>60091</v>
       </c>
       <c r="E445" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F446),"",'Bowtie v1.0 reorg'!F446)</f>
@@ -59836,11 +59961,11 @@
       </c>
       <c r="C446" t="str">
         <f>'Bowtie v1.0 reorg'!C447</f>
-        <v>0</v>
+        <v>EABC</v>
       </c>
       <c r="D446">
         <f>'Bowtie v1.0 reorg'!D447</f>
-        <v>0</v>
+        <v>60092</v>
       </c>
       <c r="E446" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F447),"",'Bowtie v1.0 reorg'!F447)</f>
@@ -59886,11 +60011,11 @@
       </c>
       <c r="C447" t="str">
         <f>'Bowtie v1.0 reorg'!C448</f>
-        <v>0</v>
+        <v>EABD</v>
       </c>
       <c r="D447">
         <f>'Bowtie v1.0 reorg'!D448</f>
-        <v>0</v>
+        <v>60093</v>
       </c>
       <c r="E447" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F448),"",'Bowtie v1.0 reorg'!F448)</f>
@@ -59936,11 +60061,11 @@
       </c>
       <c r="C448" t="str">
         <f>'Bowtie v1.0 reorg'!C449</f>
-        <v>0</v>
+        <v>EABE</v>
       </c>
       <c r="D448">
         <f>'Bowtie v1.0 reorg'!D449</f>
-        <v>0</v>
+        <v>60094</v>
       </c>
       <c r="E448" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F449),"",'Bowtie v1.0 reorg'!F449)</f>
@@ -59986,11 +60111,11 @@
       </c>
       <c r="C449" t="str">
         <f>'Bowtie v1.0 reorg'!C450</f>
-        <v>0</v>
+        <v>EABF</v>
       </c>
       <c r="D449">
         <f>'Bowtie v1.0 reorg'!D450</f>
-        <v>0</v>
+        <v>60095</v>
       </c>
       <c r="E449" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F450),"",'Bowtie v1.0 reorg'!F450)</f>
@@ -60036,11 +60161,11 @@
       </c>
       <c r="C450" t="str">
         <f>'Bowtie v1.0 reorg'!C451</f>
-        <v>0</v>
+        <v>EAC0</v>
       </c>
       <c r="D450">
         <f>'Bowtie v1.0 reorg'!D451</f>
-        <v>0</v>
+        <v>60096</v>
       </c>
       <c r="E450" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F451),"",'Bowtie v1.0 reorg'!F451)</f>
@@ -60086,11 +60211,11 @@
       </c>
       <c r="C451" t="str">
         <f>'Bowtie v1.0 reorg'!C452</f>
-        <v>0</v>
+        <v>EAC1</v>
       </c>
       <c r="D451">
         <f>'Bowtie v1.0 reorg'!D452</f>
-        <v>0</v>
+        <v>60097</v>
       </c>
       <c r="E451" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F452),"",'Bowtie v1.0 reorg'!F452)</f>
@@ -60136,11 +60261,11 @@
       </c>
       <c r="C452" t="str">
         <f>'Bowtie v1.0 reorg'!C453</f>
-        <v>0</v>
+        <v>EAC2</v>
       </c>
       <c r="D452">
         <f>'Bowtie v1.0 reorg'!D453</f>
-        <v>0</v>
+        <v>60098</v>
       </c>
       <c r="E452" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F453),"",'Bowtie v1.0 reorg'!F453)</f>
@@ -60186,11 +60311,11 @@
       </c>
       <c r="C453" t="str">
         <f>'Bowtie v1.0 reorg'!C454</f>
-        <v>0</v>
+        <v>EAC3</v>
       </c>
       <c r="D453">
         <f>'Bowtie v1.0 reorg'!D454</f>
-        <v>0</v>
+        <v>60099</v>
       </c>
       <c r="E453" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F454),"",'Bowtie v1.0 reorg'!F454)</f>
@@ -60217,7 +60342,7 @@
         <v/>
       </c>
       <c r="K453" t="e">
-        <f t="shared" ref="K453:K466" si="18">IF(NOT(ISBLANK(A453)),CONCATENATE("{'",$A$1,"':",A453,",'",$B$1,"':'",B453,"',","'",$C$1,"':'",C453,"','",$D$1,"':",D453,",'",$E$1,"':'",FIXED(E453,1),"','",$F$1,"':'",F453,"','",$G$1,"':'",G453,"','",$H$1,"':'",H453,"','",$I$1,"':['",SUBSTITUTE(I453," ","','"),"'],'",$J$1,"':'",J453,"'}"))</f>
+        <f t="shared" ref="K453:K470" si="18">IF(NOT(ISBLANK(A453)),CONCATENATE("{'",$A$1,"':",A453,",'",$B$1,"':'",B453,"',","'",$C$1,"':'",C453,"','",$D$1,"':",D453,",'",$E$1,"':'",FIXED(E453,1),"','",$F$1,"':'",F453,"','",$G$1,"':'",G453,"','",$H$1,"':'",H453,"','",$I$1,"':['",SUBSTITUTE(I453," ","','"),"'],'",$J$1,"':'",J453,"'}"))</f>
         <v>#VALUE!</v>
       </c>
       <c r="L453" t="e">
@@ -60240,7 +60365,7 @@
       </c>
       <c r="D454">
         <f>'Bowtie v1.0 reorg'!D455</f>
-        <v>0</v>
+        <v>60100</v>
       </c>
       <c r="E454" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F455),"",'Bowtie v1.0 reorg'!F455)</f>
@@ -60290,7 +60415,7 @@
       </c>
       <c r="D455">
         <f>'Bowtie v1.0 reorg'!D456</f>
-        <v>0</v>
+        <v>60101</v>
       </c>
       <c r="E455" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F456),"",'Bowtie v1.0 reorg'!F456)</f>
@@ -60340,7 +60465,7 @@
       </c>
       <c r="D456">
         <f>'Bowtie v1.0 reorg'!D457</f>
-        <v>0</v>
+        <v>60102</v>
       </c>
       <c r="E456" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F457),"",'Bowtie v1.0 reorg'!F457)</f>
@@ -60390,7 +60515,7 @@
       </c>
       <c r="D457">
         <f>'Bowtie v1.0 reorg'!D458</f>
-        <v>0</v>
+        <v>60103</v>
       </c>
       <c r="E457" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F458),"",'Bowtie v1.0 reorg'!F458)</f>
@@ -60917,11 +61042,11 @@
         <v/>
       </c>
       <c r="K467" t="e">
-        <f t="shared" ref="K467:K470" si="20">IF(NOT(ISBLANK(A467)),CONCATENATE("{'",$A$1,"':",A467,",'",$B$1,"':'",B467,"',","'",$C$1,"':'",C467,"','",$D$1,"':",D467,",'",$E$1,"':'",FIXED(E467,1),"','",$F$1,"':'",F467,"','",$G$1,"':'",G467,"','",$H$1,"':'",H467,"','",$I$1,"':['",SUBSTITUTE(I467," ","','"),"'],'",$J$1,"':'",J467,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
       <c r="L467" t="e">
-        <f t="shared" ref="L467:L470" si="21">SUBSTITUTE(K467,"'","""")</f>
+        <f t="shared" ref="L467:L470" si="20">SUBSTITUTE(K467,"'","""")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60967,11 +61092,11 @@
         <v/>
       </c>
       <c r="K468" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L468" t="e">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L468" t="e">
-        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -61017,11 +61142,11 @@
         <v/>
       </c>
       <c r="K469" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L469" t="e">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L469" t="e">
-        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -61067,11 +61192,11 @@
         <v/>
       </c>
       <c r="K470" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L470" t="e">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L470" t="e">
-        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed sm status icons used for stacking. we'll use full size for stacking.
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2193" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2131" uniqueCount="880">
   <si>
     <t>name</t>
   </si>
@@ -1985,99 +1985,6 @@
   </si>
   <si>
     <t>Used for stacking icons as background.</t>
-  </si>
-  <si>
-    <t>status-success-sm</t>
-  </si>
-  <si>
-    <t>status-warning-sm</t>
-  </si>
-  <si>
-    <t>status-info-sm</t>
-  </si>
-  <si>
-    <t>status-failure-sm</t>
-  </si>
-  <si>
-    <t>status-error-sm</t>
-  </si>
-  <si>
-    <t>status-run-sm</t>
-  </si>
-  <si>
-    <t>status-help-sm</t>
-  </si>
-  <si>
-    <t>status-stop-sm</t>
-  </si>
-  <si>
-    <t>status-pause-sm</t>
-  </si>
-  <si>
-    <t>This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot.</t>
-  </si>
-  <si>
-    <t>This is a smaller version of bowtie-status-warning. It is used for stacking with bowtie-triangle.</t>
-  </si>
-  <si>
-    <t>This is a smaller version of bowtie-status-info. It is used for stacking with bowtie-dot.</t>
-  </si>
-  <si>
-    <t>This is a smaller version of bowtie-status-failure. It is used for stacking with bowtie-dot.</t>
-  </si>
-  <si>
-    <t>This is a smaller version of bowtie-status-error. It is used for stacking with bowtie-dot.</t>
-  </si>
-  <si>
-    <t>This is a smaller version of bowtie-status-run. It is used for stacking with bowtie-dot.</t>
-  </si>
-  <si>
-    <t>This is a smaller version of bowtie-status-help. It is used for stacking with bowtie-dot.</t>
-  </si>
-  <si>
-    <t>This is a smaller version of bowtie-status-stop. It is used for stacking with bowtie-dot.</t>
-  </si>
-  <si>
-    <t>status success complete ok pass positive good checkmark</t>
-  </si>
-  <si>
-    <t>status warning problem attention exclaimation</t>
-  </si>
-  <si>
-    <t>status information letter i</t>
-  </si>
-  <si>
-    <t>status failure negative critical problem fatal error</t>
-  </si>
-  <si>
-    <t>status run play execute in progress triangle</t>
-  </si>
-  <si>
-    <t>status help question</t>
-  </si>
-  <si>
-    <t>status stop square</t>
-  </si>
-  <si>
-    <t>status pause</t>
-  </si>
-  <si>
-    <t>status waiting clock time pending queue</t>
-  </si>
-  <si>
-    <t>status no block mute unavailable</t>
-  </si>
-  <si>
-    <t>status-waiting-fill-sm</t>
-  </si>
-  <si>
-    <t>This is a smaller version of bowtie-status-waiting-fill. It is used for stacking with bowtie-dot.</t>
-  </si>
-  <si>
-    <t>status-no-fill-sm</t>
-  </si>
-  <si>
-    <t>This is a smaller version of bowtie-status-no-fill. It is used for stacking with bowtie-dot.</t>
   </si>
   <si>
     <t>assessment-group</t>
@@ -18259,490 +18166,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>355</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>323877</xdr:colOff>
-      <xdr:row>355</xdr:row>
-      <xdr:rowOff>314352</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="355" name="Picture 354">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000063010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId350"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1076325" y="142627350"/>
-          <a:ext cx="190527" cy="190527"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>356</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>409607</xdr:colOff>
-      <xdr:row>356</xdr:row>
-      <xdr:rowOff>333404</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="357" name="Picture 356">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000065010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId351"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1123950" y="143027400"/>
-          <a:ext cx="228632" cy="209579"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>357</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>381027</xdr:colOff>
-      <xdr:row>357</xdr:row>
-      <xdr:rowOff>314350</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="358" name="Picture 357">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000066010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId352"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1133475" y="143436975"/>
-          <a:ext cx="190527" cy="181000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>358</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>371504</xdr:colOff>
-      <xdr:row>358</xdr:row>
-      <xdr:rowOff>323879</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="359" name="Picture 358">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000067010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId353"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1104900" y="143817975"/>
-          <a:ext cx="209579" cy="209579"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>359</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>381029</xdr:colOff>
-      <xdr:row>359</xdr:row>
-      <xdr:rowOff>333404</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="360" name="Picture 359">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000068010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId354"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1114425" y="144227550"/>
-          <a:ext cx="209579" cy="209579"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>360</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>381031</xdr:colOff>
-      <xdr:row>360</xdr:row>
-      <xdr:rowOff>352461</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="361" name="Picture 360">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000069010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId355"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1104900" y="144599025"/>
-          <a:ext cx="219106" cy="257211"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>361</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>361982</xdr:colOff>
-      <xdr:row>361</xdr:row>
-      <xdr:rowOff>342935</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="362" name="Picture 361">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId356"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1076325" y="144999075"/>
-          <a:ext cx="228632" cy="247685"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>362</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>352452</xdr:colOff>
-      <xdr:row>362</xdr:row>
-      <xdr:rowOff>304827</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="363" name="Picture 362">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006B010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId357"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1104900" y="145418175"/>
-          <a:ext cx="190527" cy="190527"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>363</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>419135</xdr:colOff>
-      <xdr:row>363</xdr:row>
-      <xdr:rowOff>314358</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="364" name="Picture 363">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId358"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1114425" y="145780125"/>
-          <a:ext cx="247685" cy="238158"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>364</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>361981</xdr:colOff>
-      <xdr:row>364</xdr:row>
-      <xdr:rowOff>361982</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="365" name="Picture 364">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId359"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1085850" y="146237325"/>
-          <a:ext cx="219106" cy="228632"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>365</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>361977</xdr:colOff>
-      <xdr:row>365</xdr:row>
-      <xdr:rowOff>314350</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="366" name="Picture 365">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E010000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId360"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1114425" y="146637375"/>
-          <a:ext cx="190527" cy="181000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>366</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -18767,7 +18190,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId361"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId350"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -18811,7 +18234,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId362"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId351"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -18855,7 +18278,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId363"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId352"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -18899,7 +18322,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId364"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId353"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -18943,7 +18366,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId365"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId354"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -18987,7 +18410,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId366"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId355"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19031,7 +18454,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId367"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId356"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19075,7 +18498,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId368"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId357"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19119,7 +18542,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId369"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId358"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19163,7 +18586,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId370"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId359"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19207,7 +18630,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId371"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId360"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19251,7 +18674,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId372"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId361"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19295,7 +18718,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId373"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId362"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19339,7 +18762,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId374"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId363"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19383,7 +18806,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId375"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId364"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19427,7 +18850,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId376"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId365"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19471,7 +18894,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId377"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId366"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19515,7 +18938,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId378"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId367"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19559,7 +18982,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId379"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId368"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19603,7 +19026,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId380"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId369"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19647,7 +19070,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId381"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId370"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19691,7 +19114,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId381"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId370"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19735,7 +19158,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId382"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId371"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19779,7 +19202,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId383"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId372"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19823,7 +19246,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId384"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId373"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19867,7 +19290,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId385"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId374"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19911,7 +19334,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId386"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId375"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19955,7 +19378,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId387"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId376"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -19999,7 +19422,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId388"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId377"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20043,7 +19466,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId389"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId378"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20087,7 +19510,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId390"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId379"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20131,7 +19554,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId391"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId380"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20175,7 +19598,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId392"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId381"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20219,7 +19642,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId393"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId382"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20263,7 +19686,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId394"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId383"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20307,7 +19730,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId395"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId384"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20351,7 +19774,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId396"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId385"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20395,7 +19818,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId397"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId386"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20439,7 +19862,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId398"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId387"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20483,7 +19906,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId399"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId388"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20527,7 +19950,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId400"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId389"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20571,7 +19994,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId401"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId390"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20615,7 +20038,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId402"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId391"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20659,7 +20082,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId403"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId392"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20703,7 +20126,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId404"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId393"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20747,7 +20170,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId405"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId394"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20791,7 +20214,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId406"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId395"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20835,7 +20258,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId407"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId396"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20879,7 +20302,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId408"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId397"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20923,7 +20346,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId409"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId398"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -20967,7 +20390,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId410"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId399"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21011,7 +20434,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId411"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId400"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21055,7 +20478,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId412"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId401"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21099,7 +20522,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId413"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId402"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21143,7 +20566,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId414"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId403"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21187,7 +20610,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId415"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId404"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21212,8 +20635,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>943006</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>31</xdr:colOff>
       <xdr:row>89</xdr:row>
       <xdr:rowOff>390556</xdr:rowOff>
     </xdr:to>
@@ -21231,7 +20654,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId416"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId405"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21275,7 +20698,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId416"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId405"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21319,7 +20742,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId417"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId406"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21363,7 +20786,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId418"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId407"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21407,7 +20830,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId419"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId408"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21451,7 +20874,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId420"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId409"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21495,7 +20918,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId421"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId410"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21539,7 +20962,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId422"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId411"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21583,7 +21006,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId423"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId412"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21627,7 +21050,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId424"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId413"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21671,7 +21094,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId425"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId414"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21715,7 +21138,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId426"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId415"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21759,7 +21182,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId427"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId416"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21803,7 +21226,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId428"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId417"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21847,7 +21270,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId429"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId418"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21891,7 +21314,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId430"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId419"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21935,7 +21358,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId431"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId420"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -21979,7 +21402,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId432"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId421"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -22023,7 +21446,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId433"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId422"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -22067,7 +21490,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId434"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId423"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -22111,7 +21534,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId435"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId424"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -22155,7 +21578,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId436"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId425"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -22199,7 +21622,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId437"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId426"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -22518,25 +21941,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A439" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K444" sqref="K444"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="2"/>
-    <col min="3" max="3" width="13.375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="26.25" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="13.42578125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="16" style="3" customWidth="1"/>
     <col min="7" max="7" width="24" style="2" customWidth="1"/>
-    <col min="8" max="8" width="29.875" style="2" customWidth="1"/>
-    <col min="9" max="10" width="14.25" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" style="2" customWidth="1"/>
+    <col min="9" max="10" width="14.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="28" style="2" customWidth="1"/>
     <col min="12" max="38" width="9" customWidth="1"/>
-    <col min="39" max="16384" width="9.125" style="2"/>
+    <col min="39" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -27653,7 +27076,7 @@
         <v>16</v>
       </c>
       <c r="H140" t="s">
-        <v>805</v>
+        <v>774</v>
       </c>
       <c r="I140" t="s">
         <v>15</v>
@@ -27662,7 +27085,7 @@
         <v>598</v>
       </c>
       <c r="K140" t="s">
-        <v>806</v>
+        <v>775</v>
       </c>
       <c r="L140" t="str">
         <f t="shared" si="5"/>
@@ -34466,413 +33889,17 @@
         <v>uEA60-brand-vsts.svg</v>
       </c>
     </row>
-    <row r="356" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A356">
-        <v>354</v>
-      </c>
-      <c r="C356" t="str">
-        <f t="shared" si="10"/>
-        <v>EA61</v>
-      </c>
-      <c r="D356">
-        <v>60001</v>
-      </c>
-      <c r="E356" t="s">
-        <v>655</v>
-      </c>
-      <c r="F356">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G356" t="s">
-        <v>16</v>
-      </c>
-      <c r="H356" t="s">
-        <v>672</v>
-      </c>
-      <c r="I356" t="s">
-        <v>15</v>
-      </c>
-      <c r="J356" t="s">
-        <v>607</v>
-      </c>
-      <c r="K356" t="s">
-        <v>664</v>
-      </c>
-      <c r="L356" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA61-status-success-sm.svg</v>
-      </c>
-    </row>
-    <row r="357" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A357">
-        <v>355</v>
-      </c>
-      <c r="C357" t="str">
-        <f t="shared" si="10"/>
-        <v>EA62</v>
-      </c>
-      <c r="D357">
-        <v>60002</v>
-      </c>
-      <c r="E357" t="s">
-        <v>656</v>
-      </c>
-      <c r="F357">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G357" t="s">
-        <v>16</v>
-      </c>
-      <c r="H357" t="s">
-        <v>673</v>
-      </c>
-      <c r="I357" t="s">
-        <v>15</v>
-      </c>
-      <c r="J357" t="s">
-        <v>607</v>
-      </c>
-      <c r="K357" t="s">
-        <v>665</v>
-      </c>
-      <c r="L357" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA62-status-warning-sm.svg</v>
-      </c>
-    </row>
-    <row r="358" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A358">
-        <v>356</v>
-      </c>
-      <c r="C358" t="str">
-        <f t="shared" si="10"/>
-        <v>EA63</v>
-      </c>
-      <c r="D358">
-        <v>60003</v>
-      </c>
-      <c r="E358" t="s">
-        <v>657</v>
-      </c>
-      <c r="F358">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G358" t="s">
-        <v>16</v>
-      </c>
-      <c r="H358" t="s">
-        <v>674</v>
-      </c>
-      <c r="I358" t="s">
-        <v>15</v>
-      </c>
-      <c r="J358" t="s">
-        <v>607</v>
-      </c>
-      <c r="K358" t="s">
-        <v>666</v>
-      </c>
-      <c r="L358" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA63-status-info-sm.svg</v>
-      </c>
-    </row>
-    <row r="359" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A359">
-        <v>357</v>
-      </c>
-      <c r="C359" t="str">
-        <f t="shared" si="10"/>
-        <v>EA64</v>
-      </c>
-      <c r="D359">
-        <v>60004</v>
-      </c>
-      <c r="E359" t="s">
-        <v>658</v>
-      </c>
-      <c r="F359">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G359" t="s">
-        <v>16</v>
-      </c>
-      <c r="H359" t="s">
-        <v>675</v>
-      </c>
-      <c r="I359" t="s">
-        <v>15</v>
-      </c>
-      <c r="J359" t="s">
-        <v>607</v>
-      </c>
-      <c r="K359" t="s">
-        <v>667</v>
-      </c>
-      <c r="L359" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA64-status-failure-sm.svg</v>
-      </c>
-    </row>
-    <row r="360" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A360">
-        <v>358</v>
-      </c>
-      <c r="C360" t="str">
-        <f t="shared" si="10"/>
-        <v>EA65</v>
-      </c>
-      <c r="D360">
-        <v>60005</v>
-      </c>
-      <c r="E360" t="s">
-        <v>659</v>
-      </c>
-      <c r="F360">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G360" t="s">
-        <v>16</v>
-      </c>
-      <c r="H360" t="s">
-        <v>172</v>
-      </c>
-      <c r="I360" t="s">
-        <v>15</v>
-      </c>
-      <c r="J360" t="s">
-        <v>607</v>
-      </c>
-      <c r="K360" t="s">
-        <v>668</v>
-      </c>
-      <c r="L360" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA65-status-error-sm.svg</v>
-      </c>
-    </row>
-    <row r="361" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A361">
-        <v>359</v>
-      </c>
-      <c r="C361" t="str">
-        <f t="shared" si="10"/>
-        <v>EA66</v>
-      </c>
-      <c r="D361">
-        <v>60006</v>
-      </c>
-      <c r="E361" t="s">
-        <v>660</v>
-      </c>
-      <c r="F361">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G361" t="s">
-        <v>16</v>
-      </c>
-      <c r="H361" t="s">
-        <v>676</v>
-      </c>
-      <c r="I361" t="s">
-        <v>15</v>
-      </c>
-      <c r="J361" t="s">
-        <v>607</v>
-      </c>
-      <c r="K361" t="s">
-        <v>669</v>
-      </c>
-      <c r="L361" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA66-status-run-sm.svg</v>
-      </c>
-    </row>
-    <row r="362" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A362">
-        <v>360</v>
-      </c>
-      <c r="C362" t="str">
-        <f t="shared" si="10"/>
-        <v>EA67</v>
-      </c>
-      <c r="D362">
-        <v>60007</v>
-      </c>
-      <c r="E362" t="s">
-        <v>661</v>
-      </c>
-      <c r="F362">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G362" t="s">
-        <v>16</v>
-      </c>
-      <c r="H362" t="s">
-        <v>677</v>
-      </c>
-      <c r="I362" t="s">
-        <v>15</v>
-      </c>
-      <c r="J362" t="s">
-        <v>607</v>
-      </c>
-      <c r="K362" t="s">
-        <v>670</v>
-      </c>
-      <c r="L362" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA67-status-help-sm.svg</v>
-      </c>
-    </row>
-    <row r="363" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A363">
-        <v>361</v>
-      </c>
-      <c r="C363" t="str">
-        <f t="shared" si="10"/>
-        <v>EA68</v>
-      </c>
-      <c r="D363">
-        <v>60008</v>
-      </c>
-      <c r="E363" t="s">
-        <v>662</v>
-      </c>
-      <c r="F363">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G363" t="s">
-        <v>16</v>
-      </c>
-      <c r="H363" t="s">
-        <v>678</v>
-      </c>
-      <c r="I363" t="s">
-        <v>15</v>
-      </c>
-      <c r="J363" t="s">
-        <v>607</v>
-      </c>
-      <c r="K363" t="s">
-        <v>671</v>
-      </c>
-      <c r="L363" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA68-status-stop-sm.svg</v>
-      </c>
-    </row>
-    <row r="364" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A364">
-        <v>362</v>
-      </c>
-      <c r="C364" t="str">
-        <f t="shared" si="10"/>
-        <v>EA69</v>
-      </c>
-      <c r="D364">
-        <v>60009</v>
-      </c>
-      <c r="E364" t="s">
-        <v>663</v>
-      </c>
-      <c r="F364">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G364" t="s">
-        <v>16</v>
-      </c>
-      <c r="H364" t="s">
-        <v>679</v>
-      </c>
-      <c r="I364" t="s">
-        <v>15</v>
-      </c>
-      <c r="J364" t="s">
-        <v>607</v>
-      </c>
-      <c r="K364" t="s">
-        <v>664</v>
-      </c>
-      <c r="L364" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA69-status-pause-sm.svg</v>
-      </c>
-    </row>
-    <row r="365" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A365">
-        <v>363</v>
-      </c>
-      <c r="C365" t="str">
-        <f t="shared" si="10"/>
-        <v>EA6A</v>
-      </c>
-      <c r="D365">
-        <v>60010</v>
-      </c>
-      <c r="E365" t="s">
-        <v>682</v>
-      </c>
-      <c r="F365">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G365" t="s">
-        <v>16</v>
-      </c>
-      <c r="H365" t="s">
-        <v>680</v>
-      </c>
-      <c r="I365" t="s">
-        <v>15</v>
-      </c>
-      <c r="J365" t="s">
-        <v>607</v>
-      </c>
-      <c r="K365" t="s">
-        <v>683</v>
-      </c>
-      <c r="L365" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA6A-status-waiting-fill-sm.svg</v>
-      </c>
-    </row>
-    <row r="366" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A366">
-        <v>364</v>
-      </c>
-      <c r="C366" t="str">
-        <f t="shared" si="10"/>
-        <v>EA6B</v>
-      </c>
-      <c r="D366">
-        <v>60011</v>
-      </c>
-      <c r="E366" t="s">
-        <v>684</v>
-      </c>
-      <c r="F366">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G366" t="s">
-        <v>16</v>
-      </c>
-      <c r="H366" t="s">
-        <v>681</v>
-      </c>
-      <c r="I366" t="s">
-        <v>15</v>
-      </c>
-      <c r="J366" t="s">
-        <v>607</v>
-      </c>
-      <c r="K366" t="s">
-        <v>685</v>
-      </c>
-      <c r="L366" t="str">
-        <f t="shared" si="11"/>
-        <v>uEA6B-status-no-fill-sm.svg</v>
-      </c>
-    </row>
+    <row r="356" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="367" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>365</v>
@@ -34885,7 +33912,7 @@
         <v>60012</v>
       </c>
       <c r="E367" t="s">
-        <v>686</v>
+        <v>655</v>
       </c>
       <c r="F367">
         <v>1.1000000000000001</v>
@@ -34894,16 +33921,16 @@
         <v>16</v>
       </c>
       <c r="H367" t="s">
-        <v>687</v>
+        <v>656</v>
       </c>
       <c r="I367" t="s">
         <v>15</v>
       </c>
       <c r="J367" t="s">
-        <v>688</v>
+        <v>657</v>
       </c>
       <c r="K367" t="s">
-        <v>689</v>
+        <v>658</v>
       </c>
       <c r="L367" t="str">
         <f t="shared" si="11"/>
@@ -34922,7 +33949,7 @@
         <v>60013</v>
       </c>
       <c r="E368" t="s">
-        <v>690</v>
+        <v>659</v>
       </c>
       <c r="F368">
         <v>1.1000000000000001</v>
@@ -34931,7 +33958,7 @@
         <v>16</v>
       </c>
       <c r="H368" t="s">
-        <v>691</v>
+        <v>660</v>
       </c>
       <c r="I368" t="s">
         <v>15</v>
@@ -34940,7 +33967,7 @@
         <v>598</v>
       </c>
       <c r="K368" t="s">
-        <v>692</v>
+        <v>661</v>
       </c>
       <c r="L368" t="str">
         <f t="shared" si="11"/>
@@ -34959,7 +33986,7 @@
         <v>60014</v>
       </c>
       <c r="E369" t="s">
-        <v>693</v>
+        <v>662</v>
       </c>
       <c r="F369">
         <v>1.1000000000000001</v>
@@ -34968,7 +33995,7 @@
         <v>16</v>
       </c>
       <c r="H369" t="s">
-        <v>695</v>
+        <v>664</v>
       </c>
       <c r="I369" t="s">
         <v>15</v>
@@ -34977,7 +34004,7 @@
         <v>602</v>
       </c>
       <c r="K369" t="s">
-        <v>697</v>
+        <v>666</v>
       </c>
       <c r="L369" t="str">
         <f t="shared" si="11"/>
@@ -34996,7 +34023,7 @@
         <v>60015</v>
       </c>
       <c r="E370" t="s">
-        <v>694</v>
+        <v>663</v>
       </c>
       <c r="F370">
         <v>1.1000000000000001</v>
@@ -35005,7 +34032,7 @@
         <v>17</v>
       </c>
       <c r="H370" t="s">
-        <v>696</v>
+        <v>665</v>
       </c>
       <c r="I370" t="s">
         <v>15</v>
@@ -35014,7 +34041,7 @@
         <v>602</v>
       </c>
       <c r="K370" t="s">
-        <v>698</v>
+        <v>667</v>
       </c>
       <c r="L370" t="str">
         <f t="shared" si="11"/>
@@ -35033,7 +34060,7 @@
         <v>60016</v>
       </c>
       <c r="E371" t="s">
-        <v>703</v>
+        <v>672</v>
       </c>
       <c r="F371">
         <v>1.1000000000000001</v>
@@ -35042,16 +34069,16 @@
         <v>17</v>
       </c>
       <c r="H371" t="s">
-        <v>704</v>
+        <v>673</v>
       </c>
       <c r="I371" t="s">
         <v>15</v>
       </c>
       <c r="J371" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K371" t="s">
-        <v>705</v>
+        <v>674</v>
       </c>
       <c r="L371" t="str">
         <f>CONCATENATE("u",C371,"-",E372,".svg")</f>
@@ -35070,7 +34097,7 @@
         <v>60017</v>
       </c>
       <c r="E372" t="s">
-        <v>699</v>
+        <v>668</v>
       </c>
       <c r="F372">
         <v>1.1000000000000001</v>
@@ -35079,16 +34106,16 @@
         <v>17</v>
       </c>
       <c r="H372" t="s">
-        <v>700</v>
+        <v>669</v>
       </c>
       <c r="I372" t="s">
         <v>15</v>
       </c>
       <c r="J372" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K372" t="s">
-        <v>702</v>
+        <v>671</v>
       </c>
       <c r="L372" t="str">
         <f t="shared" si="11"/>
@@ -35107,7 +34134,7 @@
         <v>60018</v>
       </c>
       <c r="E373" t="s">
-        <v>706</v>
+        <v>675</v>
       </c>
       <c r="F373">
         <v>1.1000000000000001</v>
@@ -35116,16 +34143,16 @@
         <v>17</v>
       </c>
       <c r="H373" t="s">
-        <v>707</v>
+        <v>676</v>
       </c>
       <c r="I373" t="s">
         <v>15</v>
       </c>
       <c r="J373" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K373" t="s">
-        <v>708</v>
+        <v>677</v>
       </c>
       <c r="L373" t="str">
         <f t="shared" si="11"/>
@@ -35144,7 +34171,7 @@
         <v>60019</v>
       </c>
       <c r="E374" t="s">
-        <v>709</v>
+        <v>678</v>
       </c>
       <c r="F374">
         <v>1.1000000000000001</v>
@@ -35153,16 +34180,16 @@
         <v>17</v>
       </c>
       <c r="H374" t="s">
-        <v>710</v>
+        <v>679</v>
       </c>
       <c r="I374" t="s">
         <v>15</v>
       </c>
       <c r="J374" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K374" t="s">
-        <v>711</v>
+        <v>680</v>
       </c>
       <c r="L374" t="str">
         <f t="shared" si="11"/>
@@ -35181,7 +34208,7 @@
         <v>60020</v>
       </c>
       <c r="E375" t="s">
-        <v>712</v>
+        <v>681</v>
       </c>
       <c r="F375">
         <v>1.1000000000000001</v>
@@ -35190,16 +34217,16 @@
         <v>17</v>
       </c>
       <c r="H375" t="s">
-        <v>713</v>
+        <v>682</v>
       </c>
       <c r="I375" t="s">
         <v>15</v>
       </c>
       <c r="J375" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K375" t="s">
-        <v>714</v>
+        <v>683</v>
       </c>
       <c r="L375" t="str">
         <f t="shared" si="11"/>
@@ -35218,7 +34245,7 @@
         <v>60021</v>
       </c>
       <c r="E376" t="s">
-        <v>715</v>
+        <v>684</v>
       </c>
       <c r="F376">
         <v>1.1000000000000001</v>
@@ -35227,16 +34254,16 @@
         <v>17</v>
       </c>
       <c r="H376" t="s">
-        <v>716</v>
+        <v>685</v>
       </c>
       <c r="I376" t="s">
         <v>15</v>
       </c>
       <c r="J376" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K376" t="s">
-        <v>717</v>
+        <v>686</v>
       </c>
       <c r="L376" t="str">
         <f t="shared" si="11"/>
@@ -35255,7 +34282,7 @@
         <v>60022</v>
       </c>
       <c r="E377" t="s">
-        <v>718</v>
+        <v>687</v>
       </c>
       <c r="F377">
         <v>1.1000000000000001</v>
@@ -35264,16 +34291,16 @@
         <v>17</v>
       </c>
       <c r="H377" t="s">
-        <v>719</v>
+        <v>688</v>
       </c>
       <c r="I377" t="s">
         <v>15</v>
       </c>
       <c r="J377" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K377" t="s">
-        <v>720</v>
+        <v>689</v>
       </c>
       <c r="L377" t="str">
         <f t="shared" si="11"/>
@@ -35292,7 +34319,7 @@
         <v>60023</v>
       </c>
       <c r="E378" t="s">
-        <v>721</v>
+        <v>690</v>
       </c>
       <c r="F378">
         <v>1.1000000000000001</v>
@@ -35301,16 +34328,16 @@
         <v>17</v>
       </c>
       <c r="H378" t="s">
-        <v>722</v>
+        <v>691</v>
       </c>
       <c r="I378" t="s">
         <v>15</v>
       </c>
       <c r="J378" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K378" t="s">
-        <v>723</v>
+        <v>692</v>
       </c>
       <c r="L378" t="str">
         <f t="shared" si="11"/>
@@ -35329,7 +34356,7 @@
         <v>60024</v>
       </c>
       <c r="E379" t="s">
-        <v>724</v>
+        <v>693</v>
       </c>
       <c r="F379">
         <v>1.1000000000000001</v>
@@ -35338,16 +34365,16 @@
         <v>17</v>
       </c>
       <c r="H379" t="s">
-        <v>725</v>
+        <v>694</v>
       </c>
       <c r="I379" t="s">
         <v>15</v>
       </c>
       <c r="J379" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K379" t="s">
-        <v>726</v>
+        <v>695</v>
       </c>
       <c r="L379" t="str">
         <f t="shared" si="11"/>
@@ -35366,7 +34393,7 @@
         <v>60025</v>
       </c>
       <c r="E380" t="s">
-        <v>727</v>
+        <v>696</v>
       </c>
       <c r="F380">
         <v>1.1000000000000001</v>
@@ -35375,16 +34402,16 @@
         <v>17</v>
       </c>
       <c r="H380" t="s">
-        <v>728</v>
+        <v>697</v>
       </c>
       <c r="I380" t="s">
         <v>15</v>
       </c>
       <c r="J380" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K380" t="s">
-        <v>729</v>
+        <v>698</v>
       </c>
       <c r="L380" t="str">
         <f t="shared" si="11"/>
@@ -35403,7 +34430,7 @@
         <v>60026</v>
       </c>
       <c r="E381" t="s">
-        <v>730</v>
+        <v>699</v>
       </c>
       <c r="F381">
         <v>1.1000000000000001</v>
@@ -35412,16 +34439,16 @@
         <v>17</v>
       </c>
       <c r="H381" t="s">
-        <v>731</v>
+        <v>700</v>
       </c>
       <c r="I381" t="s">
         <v>15</v>
       </c>
       <c r="J381" t="s">
+        <v>670</v>
+      </c>
+      <c r="K381" t="s">
         <v>701</v>
-      </c>
-      <c r="K381" t="s">
-        <v>732</v>
       </c>
       <c r="L381" t="str">
         <f t="shared" si="11"/>
@@ -35440,7 +34467,7 @@
         <v>60027</v>
       </c>
       <c r="E382" t="s">
-        <v>733</v>
+        <v>702</v>
       </c>
       <c r="F382">
         <v>1.1000000000000001</v>
@@ -35449,16 +34476,16 @@
         <v>17</v>
       </c>
       <c r="H382" t="s">
-        <v>734</v>
+        <v>703</v>
       </c>
       <c r="I382" t="s">
         <v>15</v>
       </c>
       <c r="J382" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K382" t="s">
-        <v>735</v>
+        <v>704</v>
       </c>
       <c r="L382" t="str">
         <f t="shared" si="11"/>
@@ -35477,7 +34504,7 @@
         <v>60028</v>
       </c>
       <c r="E383" t="s">
-        <v>736</v>
+        <v>705</v>
       </c>
       <c r="F383">
         <v>1.1000000000000001</v>
@@ -35486,16 +34513,16 @@
         <v>17</v>
       </c>
       <c r="H383" t="s">
-        <v>737</v>
+        <v>706</v>
       </c>
       <c r="I383" t="s">
         <v>15</v>
       </c>
       <c r="J383" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K383" t="s">
-        <v>738</v>
+        <v>707</v>
       </c>
       <c r="L383" t="str">
         <f t="shared" si="11"/>
@@ -35514,7 +34541,7 @@
         <v>60029</v>
       </c>
       <c r="E384" t="s">
-        <v>739</v>
+        <v>708</v>
       </c>
       <c r="F384">
         <v>1.1000000000000001</v>
@@ -35523,16 +34550,16 @@
         <v>17</v>
       </c>
       <c r="H384" t="s">
-        <v>740</v>
+        <v>709</v>
       </c>
       <c r="I384" t="s">
         <v>15</v>
       </c>
       <c r="J384" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K384" t="s">
-        <v>741</v>
+        <v>710</v>
       </c>
       <c r="L384" t="str">
         <f t="shared" si="11"/>
@@ -35551,7 +34578,7 @@
         <v>60030</v>
       </c>
       <c r="E385" t="s">
-        <v>742</v>
+        <v>711</v>
       </c>
       <c r="F385">
         <v>1.1000000000000001</v>
@@ -35560,16 +34587,16 @@
         <v>17</v>
       </c>
       <c r="H385" t="s">
-        <v>743</v>
+        <v>712</v>
       </c>
       <c r="I385" t="s">
         <v>15</v>
       </c>
       <c r="J385" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K385" t="s">
-        <v>744</v>
+        <v>713</v>
       </c>
       <c r="L385" t="str">
         <f t="shared" si="11"/>
@@ -35588,7 +34615,7 @@
         <v>60031</v>
       </c>
       <c r="E386" t="s">
-        <v>745</v>
+        <v>714</v>
       </c>
       <c r="F386">
         <v>1.1000000000000001</v>
@@ -35597,16 +34624,16 @@
         <v>17</v>
       </c>
       <c r="H386" t="s">
-        <v>746</v>
+        <v>715</v>
       </c>
       <c r="I386" t="s">
         <v>15</v>
       </c>
       <c r="J386" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K386" t="s">
-        <v>747</v>
+        <v>716</v>
       </c>
       <c r="L386" t="str">
         <f t="shared" si="11"/>
@@ -35625,7 +34652,7 @@
         <v>60032</v>
       </c>
       <c r="E387" t="s">
-        <v>748</v>
+        <v>717</v>
       </c>
       <c r="F387">
         <v>1.1000000000000001</v>
@@ -35634,16 +34661,16 @@
         <v>17</v>
       </c>
       <c r="H387" t="s">
-        <v>749</v>
+        <v>718</v>
       </c>
       <c r="I387" t="s">
         <v>15</v>
       </c>
       <c r="J387" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K387" t="s">
-        <v>750</v>
+        <v>719</v>
       </c>
       <c r="L387" t="str">
         <f t="shared" si="11"/>
@@ -35662,7 +34689,7 @@
         <v>60033</v>
       </c>
       <c r="E388" t="s">
-        <v>751</v>
+        <v>720</v>
       </c>
       <c r="F388">
         <v>1.1000000000000001</v>
@@ -35671,16 +34698,16 @@
         <v>17</v>
       </c>
       <c r="H388" t="s">
-        <v>752</v>
+        <v>721</v>
       </c>
       <c r="I388" t="s">
         <v>15</v>
       </c>
       <c r="J388" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K388" t="s">
-        <v>753</v>
+        <v>722</v>
       </c>
       <c r="L388" t="str">
         <f t="shared" ref="L388:L451" si="13">CONCATENATE("u",C388,"-",E388,".svg")</f>
@@ -35699,7 +34726,7 @@
         <v>60034</v>
       </c>
       <c r="E389" t="s">
-        <v>754</v>
+        <v>723</v>
       </c>
       <c r="F389">
         <v>1.1000000000000001</v>
@@ -35708,16 +34735,16 @@
         <v>17</v>
       </c>
       <c r="H389" t="s">
-        <v>755</v>
+        <v>724</v>
       </c>
       <c r="I389" t="s">
         <v>15</v>
       </c>
       <c r="J389" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K389" t="s">
-        <v>756</v>
+        <v>725</v>
       </c>
       <c r="L389" t="str">
         <f t="shared" si="13"/>
@@ -35736,7 +34763,7 @@
         <v>60035</v>
       </c>
       <c r="E390" t="s">
-        <v>757</v>
+        <v>726</v>
       </c>
       <c r="F390">
         <v>1.1000000000000001</v>
@@ -35745,16 +34772,16 @@
         <v>17</v>
       </c>
       <c r="H390" t="s">
-        <v>758</v>
+        <v>727</v>
       </c>
       <c r="I390" t="s">
         <v>15</v>
       </c>
       <c r="J390" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K390" t="s">
-        <v>759</v>
+        <v>728</v>
       </c>
       <c r="L390" t="str">
         <f t="shared" si="13"/>
@@ -35773,7 +34800,7 @@
         <v>60036</v>
       </c>
       <c r="E391" t="s">
-        <v>760</v>
+        <v>729</v>
       </c>
       <c r="F391">
         <v>1.1000000000000001</v>
@@ -35782,16 +34809,16 @@
         <v>17</v>
       </c>
       <c r="H391" t="s">
-        <v>761</v>
+        <v>730</v>
       </c>
       <c r="I391" t="s">
         <v>15</v>
       </c>
       <c r="J391" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K391" t="s">
-        <v>762</v>
+        <v>731</v>
       </c>
       <c r="L391" t="str">
         <f t="shared" si="13"/>
@@ -35810,7 +34837,7 @@
         <v>60037</v>
       </c>
       <c r="E392" t="s">
-        <v>763</v>
+        <v>732</v>
       </c>
       <c r="F392">
         <v>1.1000000000000001</v>
@@ -35819,16 +34846,16 @@
         <v>17</v>
       </c>
       <c r="H392" t="s">
-        <v>764</v>
+        <v>733</v>
       </c>
       <c r="I392" t="s">
         <v>15</v>
       </c>
       <c r="J392" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K392" t="s">
-        <v>765</v>
+        <v>734</v>
       </c>
       <c r="L392" t="str">
         <f t="shared" si="13"/>
@@ -35847,7 +34874,7 @@
         <v>60038</v>
       </c>
       <c r="E393" t="s">
-        <v>766</v>
+        <v>735</v>
       </c>
       <c r="F393">
         <v>1.1000000000000001</v>
@@ -35856,16 +34883,16 @@
         <v>17</v>
       </c>
       <c r="H393" t="s">
-        <v>767</v>
+        <v>736</v>
       </c>
       <c r="I393" t="s">
         <v>15</v>
       </c>
       <c r="J393" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K393" t="s">
-        <v>768</v>
+        <v>737</v>
       </c>
       <c r="L393" t="str">
         <f t="shared" si="13"/>
@@ -35884,7 +34911,7 @@
         <v>60039</v>
       </c>
       <c r="E394" t="s">
-        <v>769</v>
+        <v>738</v>
       </c>
       <c r="F394">
         <v>1.1000000000000001</v>
@@ -35893,16 +34920,16 @@
         <v>17</v>
       </c>
       <c r="H394" t="s">
-        <v>770</v>
+        <v>739</v>
       </c>
       <c r="I394" t="s">
         <v>15</v>
       </c>
       <c r="J394" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K394" t="s">
-        <v>771</v>
+        <v>740</v>
       </c>
       <c r="L394" t="str">
         <f t="shared" si="13"/>
@@ -35921,7 +34948,7 @@
         <v>60040</v>
       </c>
       <c r="E395" t="s">
-        <v>772</v>
+        <v>741</v>
       </c>
       <c r="F395">
         <v>1.1000000000000001</v>
@@ -35930,16 +34957,16 @@
         <v>17</v>
       </c>
       <c r="H395" t="s">
-        <v>773</v>
+        <v>742</v>
       </c>
       <c r="I395" t="s">
         <v>15</v>
       </c>
       <c r="J395" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K395" t="s">
-        <v>774</v>
+        <v>743</v>
       </c>
       <c r="L395" t="str">
         <f t="shared" si="13"/>
@@ -35958,7 +34985,7 @@
         <v>60041</v>
       </c>
       <c r="E396" t="s">
-        <v>775</v>
+        <v>744</v>
       </c>
       <c r="F396">
         <v>1.1000000000000001</v>
@@ -35967,16 +34994,16 @@
         <v>17</v>
       </c>
       <c r="H396" t="s">
-        <v>776</v>
+        <v>745</v>
       </c>
       <c r="I396" t="s">
         <v>15</v>
       </c>
       <c r="J396" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K396" t="s">
-        <v>777</v>
+        <v>746</v>
       </c>
       <c r="L396" t="str">
         <f t="shared" si="13"/>
@@ -35995,7 +35022,7 @@
         <v>60042</v>
       </c>
       <c r="E397" t="s">
-        <v>778</v>
+        <v>747</v>
       </c>
       <c r="F397">
         <v>1.1000000000000001</v>
@@ -36004,16 +35031,16 @@
         <v>17</v>
       </c>
       <c r="H397" t="s">
-        <v>779</v>
+        <v>748</v>
       </c>
       <c r="I397" t="s">
         <v>15</v>
       </c>
       <c r="J397" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K397" t="s">
-        <v>780</v>
+        <v>749</v>
       </c>
       <c r="L397" t="str">
         <f t="shared" si="13"/>
@@ -36032,7 +35059,7 @@
         <v>60043</v>
       </c>
       <c r="E398" t="s">
-        <v>781</v>
+        <v>750</v>
       </c>
       <c r="F398">
         <v>1.1000000000000001</v>
@@ -36041,16 +35068,16 @@
         <v>17</v>
       </c>
       <c r="H398" t="s">
-        <v>782</v>
+        <v>751</v>
       </c>
       <c r="I398" t="s">
         <v>15</v>
       </c>
       <c r="J398" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K398" t="s">
-        <v>783</v>
+        <v>752</v>
       </c>
       <c r="L398" t="str">
         <f t="shared" si="13"/>
@@ -36069,7 +35096,7 @@
         <v>60044</v>
       </c>
       <c r="E399" t="s">
-        <v>784</v>
+        <v>753</v>
       </c>
       <c r="F399">
         <v>1.1000000000000001</v>
@@ -36078,16 +35105,16 @@
         <v>17</v>
       </c>
       <c r="H399" t="s">
-        <v>785</v>
+        <v>754</v>
       </c>
       <c r="I399" t="s">
         <v>15</v>
       </c>
       <c r="J399" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K399" t="s">
-        <v>786</v>
+        <v>755</v>
       </c>
       <c r="L399" t="str">
         <f t="shared" si="13"/>
@@ -36106,7 +35133,7 @@
         <v>60045</v>
       </c>
       <c r="E400" t="s">
-        <v>787</v>
+        <v>756</v>
       </c>
       <c r="F400">
         <v>1.1000000000000001</v>
@@ -36115,7 +35142,7 @@
         <v>17</v>
       </c>
       <c r="H400" t="s">
-        <v>788</v>
+        <v>757</v>
       </c>
       <c r="I400" t="s">
         <v>15</v>
@@ -36124,7 +35151,7 @@
         <v>598</v>
       </c>
       <c r="K400" t="s">
-        <v>789</v>
+        <v>758</v>
       </c>
       <c r="L400" t="str">
         <f t="shared" si="13"/>
@@ -36143,7 +35170,7 @@
         <v>60046</v>
       </c>
       <c r="E401" t="s">
-        <v>790</v>
+        <v>759</v>
       </c>
       <c r="F401">
         <v>1.1000000000000001</v>
@@ -36152,7 +35179,7 @@
         <v>17</v>
       </c>
       <c r="H401" t="s">
-        <v>791</v>
+        <v>760</v>
       </c>
       <c r="I401" t="s">
         <v>15</v>
@@ -36161,7 +35188,7 @@
         <v>598</v>
       </c>
       <c r="K401" t="s">
-        <v>792</v>
+        <v>761</v>
       </c>
       <c r="L401" t="str">
         <f t="shared" si="13"/>
@@ -36180,7 +35207,7 @@
         <v>60047</v>
       </c>
       <c r="E402" t="s">
-        <v>793</v>
+        <v>762</v>
       </c>
       <c r="F402">
         <v>1.1000000000000001</v>
@@ -36189,16 +35216,16 @@
         <v>17</v>
       </c>
       <c r="H402" t="s">
-        <v>794</v>
+        <v>763</v>
       </c>
       <c r="I402" t="s">
         <v>15</v>
       </c>
       <c r="J402" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K402" t="s">
-        <v>795</v>
+        <v>764</v>
       </c>
       <c r="L402" t="str">
         <f t="shared" si="13"/>
@@ -36217,7 +35244,7 @@
         <v>60048</v>
       </c>
       <c r="E403" t="s">
-        <v>796</v>
+        <v>765</v>
       </c>
       <c r="F403">
         <v>1.1000000000000001</v>
@@ -36226,7 +35253,7 @@
         <v>17</v>
       </c>
       <c r="H403" t="s">
-        <v>797</v>
+        <v>766</v>
       </c>
       <c r="I403" t="s">
         <v>15</v>
@@ -36235,7 +35262,7 @@
         <v>603</v>
       </c>
       <c r="K403" t="s">
-        <v>798</v>
+        <v>767</v>
       </c>
       <c r="L403" t="str">
         <f t="shared" si="13"/>
@@ -36254,7 +35281,7 @@
         <v>60049</v>
       </c>
       <c r="E404" t="s">
-        <v>799</v>
+        <v>768</v>
       </c>
       <c r="F404">
         <v>1.1000000000000001</v>
@@ -36263,7 +35290,7 @@
         <v>17</v>
       </c>
       <c r="H404" t="s">
-        <v>800</v>
+        <v>769</v>
       </c>
       <c r="I404" t="s">
         <v>15</v>
@@ -36272,7 +35299,7 @@
         <v>582</v>
       </c>
       <c r="K404" t="s">
-        <v>801</v>
+        <v>770</v>
       </c>
       <c r="L404" t="str">
         <f t="shared" si="13"/>
@@ -36291,7 +35318,7 @@
         <v>60050</v>
       </c>
       <c r="E405" t="s">
-        <v>802</v>
+        <v>771</v>
       </c>
       <c r="F405">
         <v>1.1000000000000001</v>
@@ -36300,7 +35327,7 @@
         <v>17</v>
       </c>
       <c r="H405" t="s">
-        <v>802</v>
+        <v>771</v>
       </c>
       <c r="I405" t="s">
         <v>15</v>
@@ -36309,7 +35336,7 @@
         <v>598</v>
       </c>
       <c r="K405" t="s">
-        <v>804</v>
+        <v>773</v>
       </c>
       <c r="L405" t="str">
         <f t="shared" si="13"/>
@@ -36328,7 +35355,7 @@
         <v>60051</v>
       </c>
       <c r="E406" t="s">
-        <v>803</v>
+        <v>772</v>
       </c>
       <c r="F406">
         <v>1.1000000000000001</v>
@@ -36337,7 +35364,7 @@
         <v>16</v>
       </c>
       <c r="H406" t="s">
-        <v>802</v>
+        <v>771</v>
       </c>
       <c r="I406" t="s">
         <v>15</v>
@@ -36346,7 +35373,7 @@
         <v>598</v>
       </c>
       <c r="K406" t="s">
-        <v>804</v>
+        <v>773</v>
       </c>
       <c r="L406" t="str">
         <f t="shared" si="13"/>
@@ -36365,7 +35392,7 @@
         <v>60052</v>
       </c>
       <c r="E407" t="s">
-        <v>807</v>
+        <v>776</v>
       </c>
       <c r="F407">
         <v>1.1000000000000001</v>
@@ -36374,7 +35401,7 @@
         <v>17</v>
       </c>
       <c r="H407" t="s">
-        <v>808</v>
+        <v>777</v>
       </c>
       <c r="I407" t="s">
         <v>15</v>
@@ -36383,7 +35410,7 @@
         <v>608</v>
       </c>
       <c r="K407" t="s">
-        <v>809</v>
+        <v>778</v>
       </c>
       <c r="L407" t="str">
         <f t="shared" si="13"/>
@@ -36402,7 +35429,7 @@
         <v>60053</v>
       </c>
       <c r="E408" t="s">
-        <v>810</v>
+        <v>779</v>
       </c>
       <c r="F408">
         <v>1.1000000000000001</v>
@@ -36411,7 +35438,7 @@
         <v>16</v>
       </c>
       <c r="H408" t="s">
-        <v>811</v>
+        <v>780</v>
       </c>
       <c r="I408" t="s">
         <v>15</v>
@@ -36420,7 +35447,7 @@
         <v>607</v>
       </c>
       <c r="K408" t="s">
-        <v>812</v>
+        <v>781</v>
       </c>
       <c r="L408" t="str">
         <f t="shared" si="13"/>
@@ -36439,7 +35466,7 @@
         <v>60054</v>
       </c>
       <c r="E409" t="s">
-        <v>813</v>
+        <v>782</v>
       </c>
       <c r="F409">
         <v>1.1000000000000001</v>
@@ -36448,7 +35475,7 @@
         <v>17</v>
       </c>
       <c r="H409" t="s">
-        <v>814</v>
+        <v>783</v>
       </c>
       <c r="I409" t="s">
         <v>15</v>
@@ -36457,7 +35484,7 @@
         <v>603</v>
       </c>
       <c r="K409" t="s">
-        <v>815</v>
+        <v>784</v>
       </c>
       <c r="L409" t="str">
         <f t="shared" si="13"/>
@@ -36476,7 +35503,7 @@
         <v>60055</v>
       </c>
       <c r="E410" t="s">
-        <v>816</v>
+        <v>785</v>
       </c>
       <c r="F410">
         <v>1.1000000000000001</v>
@@ -36485,7 +35512,7 @@
         <v>17</v>
       </c>
       <c r="H410" t="s">
-        <v>817</v>
+        <v>786</v>
       </c>
       <c r="I410" t="s">
         <v>15</v>
@@ -36494,7 +35521,7 @@
         <v>598</v>
       </c>
       <c r="K410" t="s">
-        <v>818</v>
+        <v>787</v>
       </c>
       <c r="L410" t="str">
         <f t="shared" si="13"/>
@@ -36513,7 +35540,7 @@
         <v>60056</v>
       </c>
       <c r="E411" t="s">
-        <v>820</v>
+        <v>789</v>
       </c>
       <c r="F411">
         <v>1.1000000000000001</v>
@@ -36522,16 +35549,16 @@
         <v>17</v>
       </c>
       <c r="H411" t="s">
-        <v>826</v>
+        <v>795</v>
       </c>
       <c r="I411" t="s">
         <v>15</v>
       </c>
       <c r="J411" t="s">
-        <v>822</v>
+        <v>791</v>
       </c>
       <c r="K411" t="s">
-        <v>823</v>
+        <v>792</v>
       </c>
       <c r="L411" t="str">
         <f t="shared" si="13"/>
@@ -36550,7 +35577,7 @@
         <v>60057</v>
       </c>
       <c r="E412" t="s">
-        <v>819</v>
+        <v>788</v>
       </c>
       <c r="F412">
         <v>1.1000000000000001</v>
@@ -36559,16 +35586,16 @@
         <v>17</v>
       </c>
       <c r="H412" t="s">
-        <v>828</v>
+        <v>797</v>
       </c>
       <c r="I412" t="s">
         <v>15</v>
       </c>
       <c r="J412" t="s">
-        <v>822</v>
+        <v>791</v>
       </c>
       <c r="K412" t="s">
-        <v>824</v>
+        <v>793</v>
       </c>
       <c r="L412" t="str">
         <f t="shared" si="13"/>
@@ -36587,7 +35614,7 @@
         <v>60058</v>
       </c>
       <c r="E413" t="s">
-        <v>821</v>
+        <v>790</v>
       </c>
       <c r="F413">
         <v>1.1000000000000001</v>
@@ -36596,16 +35623,16 @@
         <v>17</v>
       </c>
       <c r="H413" t="s">
-        <v>827</v>
+        <v>796</v>
       </c>
       <c r="I413" t="s">
         <v>15</v>
       </c>
       <c r="J413" t="s">
-        <v>822</v>
+        <v>791</v>
       </c>
       <c r="K413" t="s">
-        <v>825</v>
+        <v>794</v>
       </c>
       <c r="L413" t="str">
         <f t="shared" si="13"/>
@@ -36624,7 +35651,7 @@
         <v>60059</v>
       </c>
       <c r="E414" t="s">
-        <v>829</v>
+        <v>798</v>
       </c>
       <c r="F414">
         <v>1.1000000000000001</v>
@@ -36633,7 +35660,7 @@
         <v>17</v>
       </c>
       <c r="H414" t="s">
-        <v>830</v>
+        <v>799</v>
       </c>
       <c r="I414" t="s">
         <v>15</v>
@@ -36642,7 +35669,7 @@
         <v>602</v>
       </c>
       <c r="K414" t="s">
-        <v>831</v>
+        <v>800</v>
       </c>
       <c r="L414" t="str">
         <f t="shared" si="13"/>
@@ -36661,7 +35688,7 @@
         <v>60060</v>
       </c>
       <c r="E415" t="s">
-        <v>832</v>
+        <v>801</v>
       </c>
       <c r="F415">
         <v>1.1000000000000001</v>
@@ -36670,7 +35697,7 @@
         <v>17</v>
       </c>
       <c r="H415" t="s">
-        <v>834</v>
+        <v>803</v>
       </c>
       <c r="I415" t="s">
         <v>15</v>
@@ -36679,7 +35706,7 @@
         <v>598</v>
       </c>
       <c r="K415" t="s">
-        <v>836</v>
+        <v>805</v>
       </c>
       <c r="L415" t="str">
         <f t="shared" si="13"/>
@@ -36698,7 +35725,7 @@
         <v>60061</v>
       </c>
       <c r="E416" t="s">
-        <v>833</v>
+        <v>802</v>
       </c>
       <c r="F416">
         <v>1.1000000000000001</v>
@@ -36707,7 +35734,7 @@
         <v>17</v>
       </c>
       <c r="H416" t="s">
-        <v>835</v>
+        <v>804</v>
       </c>
       <c r="I416" t="s">
         <v>15</v>
@@ -36716,7 +35743,7 @@
         <v>598</v>
       </c>
       <c r="K416" t="s">
-        <v>836</v>
+        <v>805</v>
       </c>
       <c r="L416" t="str">
         <f t="shared" si="13"/>
@@ -36735,7 +35762,7 @@
         <v>60062</v>
       </c>
       <c r="E417" t="s">
-        <v>837</v>
+        <v>806</v>
       </c>
       <c r="F417">
         <v>1.1000000000000001</v>
@@ -36744,7 +35771,7 @@
         <v>17</v>
       </c>
       <c r="H417" t="s">
-        <v>841</v>
+        <v>810</v>
       </c>
       <c r="I417" t="s">
         <v>15</v>
@@ -36753,7 +35780,7 @@
         <v>598</v>
       </c>
       <c r="K417" t="s">
-        <v>843</v>
+        <v>812</v>
       </c>
       <c r="L417" t="str">
         <f t="shared" si="13"/>
@@ -36772,7 +35799,7 @@
         <v>60063</v>
       </c>
       <c r="E418" t="s">
-        <v>838</v>
+        <v>807</v>
       </c>
       <c r="F418">
         <v>1.1000000000000001</v>
@@ -36781,7 +35808,7 @@
         <v>17</v>
       </c>
       <c r="H418" t="s">
-        <v>842</v>
+        <v>811</v>
       </c>
       <c r="I418" t="s">
         <v>15</v>
@@ -36790,7 +35817,7 @@
         <v>598</v>
       </c>
       <c r="K418" t="s">
-        <v>843</v>
+        <v>812</v>
       </c>
       <c r="L418" t="str">
         <f t="shared" si="13"/>
@@ -36809,7 +35836,7 @@
         <v>60064</v>
       </c>
       <c r="E419" t="s">
-        <v>839</v>
+        <v>808</v>
       </c>
       <c r="F419">
         <v>1.1000000000000001</v>
@@ -36818,7 +35845,7 @@
         <v>16</v>
       </c>
       <c r="H419" t="s">
-        <v>841</v>
+        <v>810</v>
       </c>
       <c r="I419" t="s">
         <v>15</v>
@@ -36827,7 +35854,7 @@
         <v>598</v>
       </c>
       <c r="K419" t="s">
-        <v>843</v>
+        <v>812</v>
       </c>
       <c r="L419" t="str">
         <f t="shared" si="13"/>
@@ -36846,7 +35873,7 @@
         <v>60065</v>
       </c>
       <c r="E420" t="s">
-        <v>840</v>
+        <v>809</v>
       </c>
       <c r="F420">
         <v>1.1000000000000001</v>
@@ -36855,7 +35882,7 @@
         <v>16</v>
       </c>
       <c r="H420" t="s">
-        <v>842</v>
+        <v>811</v>
       </c>
       <c r="I420" t="s">
         <v>15</v>
@@ -36864,7 +35891,7 @@
         <v>598</v>
       </c>
       <c r="K420" t="s">
-        <v>843</v>
+        <v>812</v>
       </c>
       <c r="L420" t="str">
         <f t="shared" si="13"/>
@@ -36883,7 +35910,7 @@
         <v>60066</v>
       </c>
       <c r="E421" t="s">
-        <v>844</v>
+        <v>813</v>
       </c>
       <c r="F421">
         <v>1.1000000000000001</v>
@@ -36892,7 +35919,7 @@
         <v>17</v>
       </c>
       <c r="H421" t="s">
-        <v>845</v>
+        <v>814</v>
       </c>
       <c r="I421" t="s">
         <v>15</v>
@@ -36901,7 +35928,7 @@
         <v>602</v>
       </c>
       <c r="K421" t="s">
-        <v>846</v>
+        <v>815</v>
       </c>
       <c r="L421" t="str">
         <f t="shared" si="13"/>
@@ -36920,7 +35947,7 @@
         <v>60067</v>
       </c>
       <c r="E422" t="s">
-        <v>847</v>
+        <v>816</v>
       </c>
       <c r="F422">
         <v>1.1000000000000001</v>
@@ -36929,16 +35956,16 @@
         <v>17</v>
       </c>
       <c r="H422" t="s">
-        <v>848</v>
+        <v>817</v>
       </c>
       <c r="I422" t="s">
         <v>15</v>
       </c>
       <c r="J422" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K422" t="s">
-        <v>849</v>
+        <v>818</v>
       </c>
       <c r="L422" t="str">
         <f t="shared" si="13"/>
@@ -36957,7 +35984,7 @@
         <v>60068</v>
       </c>
       <c r="E423" t="s">
-        <v>850</v>
+        <v>819</v>
       </c>
       <c r="F423">
         <v>1.1000000000000001</v>
@@ -36966,7 +35993,7 @@
         <v>17</v>
       </c>
       <c r="H423" t="s">
-        <v>851</v>
+        <v>820</v>
       </c>
       <c r="I423" t="s">
         <v>15</v>
@@ -36975,7 +36002,7 @@
         <v>602</v>
       </c>
       <c r="K423" t="s">
-        <v>852</v>
+        <v>821</v>
       </c>
       <c r="L423" t="str">
         <f t="shared" si="13"/>
@@ -36994,7 +36021,7 @@
         <v>60069</v>
       </c>
       <c r="E424" t="s">
-        <v>853</v>
+        <v>822</v>
       </c>
       <c r="F424">
         <v>1.1000000000000001</v>
@@ -37003,16 +36030,16 @@
         <v>17</v>
       </c>
       <c r="H424" t="s">
-        <v>855</v>
+        <v>824</v>
       </c>
       <c r="I424" t="s">
-        <v>856</v>
+        <v>825</v>
       </c>
       <c r="J424" t="s">
         <v>598</v>
       </c>
       <c r="K424" t="s">
-        <v>857</v>
+        <v>826</v>
       </c>
       <c r="L424" t="str">
         <f t="shared" si="13"/>
@@ -37031,7 +36058,7 @@
         <v>60070</v>
       </c>
       <c r="E425" t="s">
-        <v>854</v>
+        <v>823</v>
       </c>
       <c r="F425">
         <v>1.1000000000000001</v>
@@ -37040,16 +36067,16 @@
         <v>17</v>
       </c>
       <c r="H425" t="s">
-        <v>855</v>
+        <v>824</v>
       </c>
       <c r="I425" t="s">
-        <v>856</v>
+        <v>825</v>
       </c>
       <c r="J425" t="s">
         <v>598</v>
       </c>
       <c r="K425" t="s">
-        <v>857</v>
+        <v>826</v>
       </c>
       <c r="L425" t="str">
         <f t="shared" si="13"/>
@@ -37068,7 +36095,7 @@
         <v>60071</v>
       </c>
       <c r="E426" t="s">
-        <v>861</v>
+        <v>830</v>
       </c>
       <c r="F426">
         <v>1.1000000000000001</v>
@@ -37077,7 +36104,7 @@
         <v>17</v>
       </c>
       <c r="H426" t="s">
-        <v>862</v>
+        <v>831</v>
       </c>
       <c r="I426" t="s">
         <v>15</v>
@@ -37086,7 +36113,7 @@
         <v>598</v>
       </c>
       <c r="K426" t="s">
-        <v>863</v>
+        <v>832</v>
       </c>
       <c r="L426" t="str">
         <f t="shared" si="13"/>
@@ -37105,7 +36132,7 @@
         <v>60072</v>
       </c>
       <c r="E427" t="s">
-        <v>859</v>
+        <v>828</v>
       </c>
       <c r="F427">
         <v>1.1000000000000001</v>
@@ -37114,7 +36141,7 @@
         <v>17</v>
       </c>
       <c r="H427" t="s">
-        <v>860</v>
+        <v>829</v>
       </c>
       <c r="I427" t="s">
         <v>15</v>
@@ -37123,7 +36150,7 @@
         <v>602</v>
       </c>
       <c r="K427" t="s">
-        <v>858</v>
+        <v>827</v>
       </c>
       <c r="L427" t="str">
         <f t="shared" si="13"/>
@@ -37142,7 +36169,7 @@
         <v>60073</v>
       </c>
       <c r="E428" t="s">
-        <v>864</v>
+        <v>833</v>
       </c>
       <c r="F428">
         <v>1.1000000000000001</v>
@@ -37151,7 +36178,7 @@
         <v>17</v>
       </c>
       <c r="H428" t="s">
-        <v>865</v>
+        <v>834</v>
       </c>
       <c r="I428" t="s">
         <v>15</v>
@@ -37160,7 +36187,7 @@
         <v>598</v>
       </c>
       <c r="K428" t="s">
-        <v>866</v>
+        <v>835</v>
       </c>
       <c r="L428" t="str">
         <f t="shared" si="13"/>
@@ -37179,7 +36206,7 @@
         <v>60074</v>
       </c>
       <c r="E429" t="s">
-        <v>867</v>
+        <v>836</v>
       </c>
       <c r="F429">
         <v>1.1000000000000001</v>
@@ -37188,7 +36215,7 @@
         <v>16</v>
       </c>
       <c r="H429" t="s">
-        <v>865</v>
+        <v>834</v>
       </c>
       <c r="I429" t="s">
         <v>15</v>
@@ -37197,7 +36224,7 @@
         <v>598</v>
       </c>
       <c r="K429" t="s">
-        <v>866</v>
+        <v>835</v>
       </c>
       <c r="L429" t="str">
         <f t="shared" si="13"/>
@@ -37216,7 +36243,7 @@
         <v>60075</v>
       </c>
       <c r="E430" t="s">
-        <v>868</v>
+        <v>837</v>
       </c>
       <c r="F430">
         <v>1.1000000000000001</v>
@@ -37225,7 +36252,7 @@
         <v>16</v>
       </c>
       <c r="H430" t="s">
-        <v>869</v>
+        <v>838</v>
       </c>
       <c r="I430" t="s">
         <v>15</v>
@@ -37234,7 +36261,7 @@
         <v>602</v>
       </c>
       <c r="K430" t="s">
-        <v>877</v>
+        <v>846</v>
       </c>
       <c r="L430" t="str">
         <f t="shared" si="13"/>
@@ -37253,7 +36280,7 @@
         <v>60076</v>
       </c>
       <c r="E431" t="s">
-        <v>870</v>
+        <v>839</v>
       </c>
       <c r="F431">
         <v>1.1000000000000001</v>
@@ -37262,7 +36289,7 @@
         <v>16</v>
       </c>
       <c r="H431" t="s">
-        <v>871</v>
+        <v>840</v>
       </c>
       <c r="I431" t="s">
         <v>15</v>
@@ -37271,7 +36298,7 @@
         <v>602</v>
       </c>
       <c r="K431" t="s">
-        <v>872</v>
+        <v>841</v>
       </c>
       <c r="L431" t="str">
         <f t="shared" si="13"/>
@@ -37290,7 +36317,7 @@
         <v>60077</v>
       </c>
       <c r="E432" t="s">
-        <v>873</v>
+        <v>842</v>
       </c>
       <c r="F432">
         <v>1.1000000000000001</v>
@@ -37299,7 +36326,7 @@
         <v>17</v>
       </c>
       <c r="H432" t="s">
-        <v>874</v>
+        <v>843</v>
       </c>
       <c r="I432" t="s">
         <v>15</v>
@@ -37308,7 +36335,7 @@
         <v>602</v>
       </c>
       <c r="K432" t="s">
-        <v>878</v>
+        <v>847</v>
       </c>
       <c r="L432" t="str">
         <f t="shared" si="13"/>
@@ -37327,7 +36354,7 @@
         <v>60078</v>
       </c>
       <c r="E433" t="s">
-        <v>875</v>
+        <v>844</v>
       </c>
       <c r="F433">
         <v>1.1000000000000001</v>
@@ -37336,7 +36363,7 @@
         <v>16</v>
       </c>
       <c r="H433" t="s">
-        <v>876</v>
+        <v>845</v>
       </c>
       <c r="I433" t="s">
         <v>15</v>
@@ -37345,7 +36372,7 @@
         <v>602</v>
       </c>
       <c r="K433" t="s">
-        <v>879</v>
+        <v>848</v>
       </c>
       <c r="L433" t="str">
         <f t="shared" si="13"/>
@@ -37364,7 +36391,7 @@
         <v>60079</v>
       </c>
       <c r="E434" t="s">
-        <v>880</v>
+        <v>849</v>
       </c>
       <c r="F434">
         <v>1.1000000000000001</v>
@@ -37373,7 +36400,7 @@
         <v>17</v>
       </c>
       <c r="H434" t="s">
-        <v>881</v>
+        <v>850</v>
       </c>
       <c r="I434" t="s">
         <v>15</v>
@@ -37382,7 +36409,7 @@
         <v>602</v>
       </c>
       <c r="K434" t="s">
-        <v>882</v>
+        <v>851</v>
       </c>
       <c r="L434" t="str">
         <f t="shared" si="13"/>
@@ -37401,7 +36428,7 @@
         <v>60080</v>
       </c>
       <c r="E435" t="s">
-        <v>883</v>
+        <v>852</v>
       </c>
       <c r="F435">
         <v>1.1000000000000001</v>
@@ -37410,7 +36437,7 @@
         <v>17</v>
       </c>
       <c r="H435" t="s">
-        <v>884</v>
+        <v>853</v>
       </c>
       <c r="I435" t="s">
         <v>15</v>
@@ -37419,7 +36446,7 @@
         <v>602</v>
       </c>
       <c r="K435" t="s">
-        <v>885</v>
+        <v>854</v>
       </c>
       <c r="L435" t="str">
         <f t="shared" si="13"/>
@@ -37438,7 +36465,7 @@
         <v>60081</v>
       </c>
       <c r="E436" t="s">
-        <v>886</v>
+        <v>855</v>
       </c>
       <c r="F436">
         <v>1.1000000000000001</v>
@@ -37447,7 +36474,7 @@
         <v>16</v>
       </c>
       <c r="H436" t="s">
-        <v>887</v>
+        <v>856</v>
       </c>
       <c r="I436" t="s">
         <v>15</v>
@@ -37456,7 +36483,7 @@
         <v>582</v>
       </c>
       <c r="K436" t="s">
-        <v>888</v>
+        <v>857</v>
       </c>
       <c r="L436" t="str">
         <f t="shared" si="13"/>
@@ -37475,7 +36502,7 @@
         <v>60082</v>
       </c>
       <c r="E437" t="s">
-        <v>889</v>
+        <v>858</v>
       </c>
       <c r="F437">
         <v>1.1000000000000001</v>
@@ -37484,7 +36511,7 @@
         <v>17</v>
       </c>
       <c r="H437" t="s">
-        <v>890</v>
+        <v>859</v>
       </c>
       <c r="I437" t="s">
         <v>15</v>
@@ -37493,7 +36520,7 @@
         <v>597</v>
       </c>
       <c r="K437" t="s">
-        <v>892</v>
+        <v>861</v>
       </c>
       <c r="L437" t="str">
         <f t="shared" si="13"/>
@@ -37512,7 +36539,7 @@
         <v>60083</v>
       </c>
       <c r="E438" t="s">
-        <v>893</v>
+        <v>862</v>
       </c>
       <c r="F438">
         <v>1.1000000000000001</v>
@@ -37521,16 +36548,16 @@
         <v>16</v>
       </c>
       <c r="H438" t="s">
-        <v>894</v>
+        <v>863</v>
       </c>
       <c r="I438" t="s">
         <v>15</v>
       </c>
       <c r="J438" t="s">
-        <v>688</v>
+        <v>657</v>
       </c>
       <c r="K438" t="s">
-        <v>895</v>
+        <v>864</v>
       </c>
       <c r="L438" t="str">
         <f t="shared" si="13"/>
@@ -37549,7 +36576,7 @@
         <v>60084</v>
       </c>
       <c r="E439" t="s">
-        <v>896</v>
+        <v>865</v>
       </c>
       <c r="F439">
         <v>1.1000000000000001</v>
@@ -37558,7 +36585,7 @@
         <v>17</v>
       </c>
       <c r="H439" t="s">
-        <v>897</v>
+        <v>866</v>
       </c>
       <c r="I439" t="s">
         <v>15</v>
@@ -37567,7 +36594,7 @@
         <v>598</v>
       </c>
       <c r="K439" t="s">
-        <v>898</v>
+        <v>867</v>
       </c>
       <c r="L439" t="str">
         <f t="shared" si="13"/>
@@ -37586,7 +36613,7 @@
         <v>60085</v>
       </c>
       <c r="E440" t="s">
-        <v>899</v>
+        <v>868</v>
       </c>
       <c r="F440">
         <v>1.1000000000000001</v>
@@ -37595,7 +36622,7 @@
         <v>17</v>
       </c>
       <c r="H440" t="s">
-        <v>900</v>
+        <v>869</v>
       </c>
       <c r="I440" t="s">
         <v>15</v>
@@ -37604,7 +36631,7 @@
         <v>582</v>
       </c>
       <c r="K440" t="s">
-        <v>901</v>
+        <v>870</v>
       </c>
       <c r="L440" t="str">
         <f t="shared" si="13"/>
@@ -37623,7 +36650,7 @@
         <v>60086</v>
       </c>
       <c r="E441" t="s">
-        <v>904</v>
+        <v>873</v>
       </c>
       <c r="F441">
         <v>1.1000000000000001</v>
@@ -37632,16 +36659,16 @@
         <v>17</v>
       </c>
       <c r="H441" t="s">
-        <v>902</v>
+        <v>871</v>
       </c>
       <c r="I441" t="s">
         <v>15</v>
       </c>
       <c r="J441" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="K441" t="s">
-        <v>903</v>
+        <v>872</v>
       </c>
       <c r="L441" t="str">
         <f t="shared" si="13"/>
@@ -37660,7 +36687,7 @@
         <v>60087</v>
       </c>
       <c r="E442" t="s">
-        <v>905</v>
+        <v>874</v>
       </c>
       <c r="F442">
         <v>1.1000000000000001</v>
@@ -37669,16 +36696,16 @@
         <v>17</v>
       </c>
       <c r="H442" t="s">
-        <v>907</v>
+        <v>876</v>
       </c>
       <c r="I442" t="s">
         <v>15</v>
       </c>
       <c r="J442" t="s">
-        <v>688</v>
+        <v>657</v>
       </c>
       <c r="K442" t="s">
-        <v>909</v>
+        <v>878</v>
       </c>
       <c r="L442" t="str">
         <f t="shared" si="13"/>
@@ -37697,7 +36724,7 @@
         <v>60088</v>
       </c>
       <c r="E443" t="s">
-        <v>906</v>
+        <v>875</v>
       </c>
       <c r="F443">
         <v>1.1000000000000001</v>
@@ -37706,16 +36733,16 @@
         <v>17</v>
       </c>
       <c r="H443" t="s">
-        <v>908</v>
+        <v>877</v>
       </c>
       <c r="I443" t="s">
         <v>15</v>
       </c>
       <c r="J443" t="s">
-        <v>688</v>
+        <v>657</v>
       </c>
       <c r="K443" t="s">
-        <v>910</v>
+        <v>879</v>
       </c>
       <c r="L443" t="str">
         <f t="shared" si="13"/>
@@ -38107,17 +37134,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="H440" sqref="H440"/>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="I355" sqref="I355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.875" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="14"/>
-    <col min="8" max="8" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="14"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="16.875" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -38826,9 +37853,8 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F16),"",'Bowtie v1.0 reorg'!F16)</f>
         <v>1</v>
       </c>
-      <c r="F15" t="str">
-        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G16),"",'Bowtie v1.0 reorg'!G16)</f>
-        <v/>
+      <c r="F15" t="s">
+        <v>17</v>
       </c>
       <c r="G15" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I16),"",'Bowtie v1.0 reorg'!I16)</f>
@@ -38848,11 +37874,11 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="2"/>
-        <v>{'id':14,'name':'switch','unicode':'E90D','decimal':59661,'version':'1.0','style':'','subset':'VSTS','group':'Arrow','keywords':['arrow','switch','exchange','left','right'],'usage':''}</v>
+        <v>{'id':14,'name':'switch','unicode':'E90D','decimal':59661,'version':'1.0','style':'light','subset':'VSTS','group':'Arrow','keywords':['arrow','switch','exchange','left','right'],'usage':''}</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="3"/>
-        <v>{"id":14,"name":"switch","unicode":"E90D","decimal":59661,"version":"1.0","style":"","subset":"VSTS","group":"Arrow","keywords":["arrow","switch","exchange","left","right"],"usage":""}</v>
+        <v>{"id":14,"name":"switch","unicode":"E90D","decimal":59661,"version":"1.0","style":"light","subset":"VSTS","group":"Arrow","keywords":["arrow","switch","exchange","left","right"],"usage":""}</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -38876,9 +37902,8 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F17),"",'Bowtie v1.0 reorg'!F17)</f>
         <v>1</v>
       </c>
-      <c r="F16" t="str">
-        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G17),"",'Bowtie v1.0 reorg'!G17)</f>
-        <v/>
+      <c r="F16" t="s">
+        <v>17</v>
       </c>
       <c r="G16" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I17),"",'Bowtie v1.0 reorg'!I17)</f>
@@ -38898,11 +37923,11 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="2"/>
-        <v>{'id':15,'name':'synchronize','unicode':'E90E','decimal':59662,'version':'1.0','style':'','subset':'VSTS','group':'Arrow','keywords':['arrow','synchronize','sync','update','upload','download'],'usage':'Used for synchronizing and data exchange, different from refresh'}</v>
+        <v>{'id':15,'name':'synchronize','unicode':'E90E','decimal':59662,'version':'1.0','style':'light','subset':'VSTS','group':'Arrow','keywords':['arrow','synchronize','sync','update','upload','download'],'usage':'Used for synchronizing and data exchange, different from refresh'}</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="3"/>
-        <v>{"id":15,"name":"synchronize","unicode":"E90E","decimal":59662,"version":"1.0","style":"","subset":"VSTS","group":"Arrow","keywords":["arrow","synchronize","sync","update","upload","download"],"usage":"Used for synchronizing and data exchange, different from refresh"}</v>
+        <v>{"id":15,"name":"synchronize","unicode":"E90E","decimal":59662,"version":"1.0","style":"light","subset":"VSTS","group":"Arrow","keywords":["arrow","synchronize","sync","update","upload","download"],"usage":"Used for synchronizing and data exchange, different from refresh"}</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -38926,9 +37951,8 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F18),"",'Bowtie v1.0 reorg'!F18)</f>
         <v>1</v>
       </c>
-      <c r="F17" t="str">
-        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G18),"",'Bowtie v1.0 reorg'!G18)</f>
-        <v/>
+      <c r="F17" t="s">
+        <v>17</v>
       </c>
       <c r="G17" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I18),"",'Bowtie v1.0 reorg'!I18)</f>
@@ -38948,11 +37972,11 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="2"/>
-        <v>{'id':16,'name':'transfer-download','unicode':'E90F','decimal':59663,'version':'1.0','style':'','subset':'VSTS','group':'Arrow','keywords':['download','bottom','arrow','down'],'usage':'Used for download or go to bottom'}</v>
+        <v>{'id':16,'name':'transfer-download','unicode':'E90F','decimal':59663,'version':'1.0','style':'light','subset':'VSTS','group':'Arrow','keywords':['download','bottom','arrow','down'],'usage':'Used for download or go to bottom'}</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="3"/>
-        <v>{"id":16,"name":"transfer-download","unicode":"E90F","decimal":59663,"version":"1.0","style":"","subset":"VSTS","group":"Arrow","keywords":["download","bottom","arrow","down"],"usage":"Used for download or go to bottom"}</v>
+        <v>{"id":16,"name":"transfer-download","unicode":"E90F","decimal":59663,"version":"1.0","style":"light","subset":"VSTS","group":"Arrow","keywords":["download","bottom","arrow","down"],"usage":"Used for download or go to bottom"}</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -38976,9 +38000,8 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F19),"",'Bowtie v1.0 reorg'!F19)</f>
         <v>1</v>
       </c>
-      <c r="F18" t="str">
-        <f>IF(ISBLANK('Bowtie v1.0 reorg'!G19),"",'Bowtie v1.0 reorg'!G19)</f>
-        <v/>
+      <c r="F18" t="s">
+        <v>17</v>
       </c>
       <c r="G18" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I19),"",'Bowtie v1.0 reorg'!I19)</f>
@@ -38998,11 +38021,11 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="2"/>
-        <v>{'id':17,'name':'transfer-upload','unicode':'E910','decimal':59664,'version':'1.0','style':'','subset':'VSTS','group':'Arrow','keywords':['upload','top','arrow','up'],'usage':'Used for upload or go to top'}</v>
+        <v>{'id':17,'name':'transfer-upload','unicode':'E910','decimal':59664,'version':'1.0','style':'light','subset':'VSTS','group':'Arrow','keywords':['upload','top','arrow','up'],'usage':'Used for upload or go to top'}</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="3"/>
-        <v>{"id":17,"name":"transfer-upload","unicode":"E910","decimal":59664,"version":"1.0","style":"","subset":"VSTS","group":"Arrow","keywords":["upload","top","arrow","up"],"usage":"Used for upload or go to top"}</v>
+        <v>{"id":17,"name":"transfer-upload","unicode":"E910","decimal":59664,"version":"1.0","style":"light","subset":"VSTS","group":"Arrow","keywords":["upload","top","arrow","up"],"usage":"Used for upload or go to top"}</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -55808,551 +54831,551 @@
     <row r="355" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A355">
         <f>'Bowtie v1.0 reorg'!A356</f>
-        <v>354</v>
-      </c>
-      <c r="B355" t="str">
+        <v>0</v>
+      </c>
+      <c r="B355">
         <f>'Bowtie v1.0 reorg'!E356</f>
-        <v>status-success-sm</v>
-      </c>
-      <c r="C355" t="str">
+        <v>0</v>
+      </c>
+      <c r="C355">
         <f>'Bowtie v1.0 reorg'!C356</f>
-        <v>EA61</v>
+        <v>0</v>
       </c>
       <c r="D355">
         <f>'Bowtie v1.0 reorg'!D356</f>
-        <v>60001</v>
-      </c>
-      <c r="E355">
+        <v>0</v>
+      </c>
+      <c r="E355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F356),"",'Bowtie v1.0 reorg'!F356)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G356),"",'Bowtie v1.0 reorg'!G356)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I356),"",'Bowtie v1.0 reorg'!I356)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J356),"",'Bowtie v1.0 reorg'!J356)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H356),"",'Bowtie v1.0 reorg'!H356)</f>
-        <v>status success complete ok pass positive good checkmark</v>
+        <v/>
       </c>
       <c r="J355" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K356),"",'Bowtie v1.0 reorg'!K356)</f>
-        <v>This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot.</v>
-      </c>
-      <c r="K355" t="str">
+        <v/>
+      </c>
+      <c r="K355" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':354,'name':'status-success-sm','unicode':'EA61','decimal':60001,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','success','complete','ok','pass','positive','good','checkmark'],'usage':'This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot.'}</v>
-      </c>
-      <c r="L355" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L355" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":354,"name":"status-success-sm","unicode":"EA61","decimal":60001,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","success","complete","ok","pass","positive","good","checkmark"],"usage":"This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="356" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A356">
         <f>'Bowtie v1.0 reorg'!A357</f>
-        <v>355</v>
-      </c>
-      <c r="B356" t="str">
+        <v>0</v>
+      </c>
+      <c r="B356">
         <f>'Bowtie v1.0 reorg'!E357</f>
-        <v>status-warning-sm</v>
-      </c>
-      <c r="C356" t="str">
+        <v>0</v>
+      </c>
+      <c r="C356">
         <f>'Bowtie v1.0 reorg'!C357</f>
-        <v>EA62</v>
+        <v>0</v>
       </c>
       <c r="D356">
         <f>'Bowtie v1.0 reorg'!D357</f>
-        <v>60002</v>
-      </c>
-      <c r="E356">
+        <v>0</v>
+      </c>
+      <c r="E356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F357),"",'Bowtie v1.0 reorg'!F357)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G357),"",'Bowtie v1.0 reorg'!G357)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I357),"",'Bowtie v1.0 reorg'!I357)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J357),"",'Bowtie v1.0 reorg'!J357)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H357),"",'Bowtie v1.0 reorg'!H357)</f>
-        <v>status warning problem attention exclaimation</v>
+        <v/>
       </c>
       <c r="J356" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K357),"",'Bowtie v1.0 reorg'!K357)</f>
-        <v>This is a smaller version of bowtie-status-warning. It is used for stacking with bowtie-triangle.</v>
-      </c>
-      <c r="K356" t="str">
+        <v/>
+      </c>
+      <c r="K356" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':355,'name':'status-warning-sm','unicode':'EA62','decimal':60002,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','warning','problem','attention','exclaimation'],'usage':'This is a smaller version of bowtie-status-warning. It is used for stacking with bowtie-triangle.'}</v>
-      </c>
-      <c r="L356" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L356" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":355,"name":"status-warning-sm","unicode":"EA62","decimal":60002,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","warning","problem","attention","exclaimation"],"usage":"This is a smaller version of bowtie-status-warning. It is used for stacking with bowtie-triangle."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357">
         <f>'Bowtie v1.0 reorg'!A358</f>
-        <v>356</v>
-      </c>
-      <c r="B357" t="str">
+        <v>0</v>
+      </c>
+      <c r="B357">
         <f>'Bowtie v1.0 reorg'!E358</f>
-        <v>status-info-sm</v>
-      </c>
-      <c r="C357" t="str">
+        <v>0</v>
+      </c>
+      <c r="C357">
         <f>'Bowtie v1.0 reorg'!C358</f>
-        <v>EA63</v>
+        <v>0</v>
       </c>
       <c r="D357">
         <f>'Bowtie v1.0 reorg'!D358</f>
-        <v>60003</v>
-      </c>
-      <c r="E357">
+        <v>0</v>
+      </c>
+      <c r="E357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F358),"",'Bowtie v1.0 reorg'!F358)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G358),"",'Bowtie v1.0 reorg'!G358)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I358),"",'Bowtie v1.0 reorg'!I358)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J358),"",'Bowtie v1.0 reorg'!J358)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H358),"",'Bowtie v1.0 reorg'!H358)</f>
-        <v>status information letter i</v>
+        <v/>
       </c>
       <c r="J357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K358),"",'Bowtie v1.0 reorg'!K358)</f>
-        <v>This is a smaller version of bowtie-status-info. It is used for stacking with bowtie-dot.</v>
-      </c>
-      <c r="K357" t="str">
+        <v/>
+      </c>
+      <c r="K357" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':356,'name':'status-info-sm','unicode':'EA63','decimal':60003,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','information','letter','i'],'usage':'This is a smaller version of bowtie-status-info. It is used for stacking with bowtie-dot.'}</v>
-      </c>
-      <c r="L357" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L357" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":356,"name":"status-info-sm","unicode":"EA63","decimal":60003,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","information","letter","i"],"usage":"This is a smaller version of bowtie-status-info. It is used for stacking with bowtie-dot."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="358" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A358">
         <f>'Bowtie v1.0 reorg'!A359</f>
-        <v>357</v>
-      </c>
-      <c r="B358" t="str">
+        <v>0</v>
+      </c>
+      <c r="B358">
         <f>'Bowtie v1.0 reorg'!E359</f>
-        <v>status-failure-sm</v>
-      </c>
-      <c r="C358" t="str">
+        <v>0</v>
+      </c>
+      <c r="C358">
         <f>'Bowtie v1.0 reorg'!C359</f>
-        <v>EA64</v>
+        <v>0</v>
       </c>
       <c r="D358">
         <f>'Bowtie v1.0 reorg'!D359</f>
-        <v>60004</v>
-      </c>
-      <c r="E358">
+        <v>0</v>
+      </c>
+      <c r="E358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F359),"",'Bowtie v1.0 reorg'!F359)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G359),"",'Bowtie v1.0 reorg'!G359)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I359),"",'Bowtie v1.0 reorg'!I359)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J359),"",'Bowtie v1.0 reorg'!J359)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H359),"",'Bowtie v1.0 reorg'!H359)</f>
-        <v>status failure negative critical problem fatal error</v>
+        <v/>
       </c>
       <c r="J358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K359),"",'Bowtie v1.0 reorg'!K359)</f>
-        <v>This is a smaller version of bowtie-status-failure. It is used for stacking with bowtie-dot.</v>
-      </c>
-      <c r="K358" t="str">
+        <v/>
+      </c>
+      <c r="K358" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':357,'name':'status-failure-sm','unicode':'EA64','decimal':60004,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','failure','negative','critical','problem','fatal','error'],'usage':'This is a smaller version of bowtie-status-failure. It is used for stacking with bowtie-dot.'}</v>
-      </c>
-      <c r="L358" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L358" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":357,"name":"status-failure-sm","unicode":"EA64","decimal":60004,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","failure","negative","critical","problem","fatal","error"],"usage":"This is a smaller version of bowtie-status-failure. It is used for stacking with bowtie-dot."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="359" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A359">
         <f>'Bowtie v1.0 reorg'!A360</f>
-        <v>358</v>
-      </c>
-      <c r="B359" t="str">
+        <v>0</v>
+      </c>
+      <c r="B359">
         <f>'Bowtie v1.0 reorg'!E360</f>
-        <v>status-error-sm</v>
-      </c>
-      <c r="C359" t="str">
+        <v>0</v>
+      </c>
+      <c r="C359">
         <f>'Bowtie v1.0 reorg'!C360</f>
-        <v>EA65</v>
+        <v>0</v>
       </c>
       <c r="D359">
         <f>'Bowtie v1.0 reorg'!D360</f>
-        <v>60005</v>
-      </c>
-      <c r="E359">
+        <v>0</v>
+      </c>
+      <c r="E359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F360),"",'Bowtie v1.0 reorg'!F360)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G360),"",'Bowtie v1.0 reorg'!G360)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I360),"",'Bowtie v1.0 reorg'!I360)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J360),"",'Bowtie v1.0 reorg'!J360)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H360),"",'Bowtie v1.0 reorg'!H360)</f>
-        <v>status error alert invalid problem circle exclaimation</v>
+        <v/>
       </c>
       <c r="J359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K360),"",'Bowtie v1.0 reorg'!K360)</f>
-        <v>This is a smaller version of bowtie-status-error. It is used for stacking with bowtie-dot.</v>
-      </c>
-      <c r="K359" t="str">
+        <v/>
+      </c>
+      <c r="K359" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':358,'name':'status-error-sm','unicode':'EA65','decimal':60005,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','error','alert','invalid','problem','circle','exclaimation'],'usage':'This is a smaller version of bowtie-status-error. It is used for stacking with bowtie-dot.'}</v>
-      </c>
-      <c r="L359" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L359" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":358,"name":"status-error-sm","unicode":"EA65","decimal":60005,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","error","alert","invalid","problem","circle","exclaimation"],"usage":"This is a smaller version of bowtie-status-error. It is used for stacking with bowtie-dot."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="360" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A360">
         <f>'Bowtie v1.0 reorg'!A361</f>
-        <v>359</v>
-      </c>
-      <c r="B360" t="str">
+        <v>0</v>
+      </c>
+      <c r="B360">
         <f>'Bowtie v1.0 reorg'!E361</f>
-        <v>status-run-sm</v>
-      </c>
-      <c r="C360" t="str">
+        <v>0</v>
+      </c>
+      <c r="C360">
         <f>'Bowtie v1.0 reorg'!C361</f>
-        <v>EA66</v>
+        <v>0</v>
       </c>
       <c r="D360">
         <f>'Bowtie v1.0 reorg'!D361</f>
-        <v>60006</v>
-      </c>
-      <c r="E360">
+        <v>0</v>
+      </c>
+      <c r="E360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F361),"",'Bowtie v1.0 reorg'!F361)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G361),"",'Bowtie v1.0 reorg'!G361)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I361),"",'Bowtie v1.0 reorg'!I361)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J361),"",'Bowtie v1.0 reorg'!J361)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H361),"",'Bowtie v1.0 reorg'!H361)</f>
-        <v>status run play execute in progress triangle</v>
+        <v/>
       </c>
       <c r="J360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K361),"",'Bowtie v1.0 reorg'!K361)</f>
-        <v>This is a smaller version of bowtie-status-run. It is used for stacking with bowtie-dot.</v>
-      </c>
-      <c r="K360" t="str">
+        <v/>
+      </c>
+      <c r="K360" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':359,'name':'status-run-sm','unicode':'EA66','decimal':60006,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','run','play','execute','in','progress','triangle'],'usage':'This is a smaller version of bowtie-status-run. It is used for stacking with bowtie-dot.'}</v>
-      </c>
-      <c r="L360" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L360" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":359,"name":"status-run-sm","unicode":"EA66","decimal":60006,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","run","play","execute","in","progress","triangle"],"usage":"This is a smaller version of bowtie-status-run. It is used for stacking with bowtie-dot."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="361" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A361">
         <f>'Bowtie v1.0 reorg'!A362</f>
-        <v>360</v>
-      </c>
-      <c r="B361" t="str">
+        <v>0</v>
+      </c>
+      <c r="B361">
         <f>'Bowtie v1.0 reorg'!E362</f>
-        <v>status-help-sm</v>
-      </c>
-      <c r="C361" t="str">
+        <v>0</v>
+      </c>
+      <c r="C361">
         <f>'Bowtie v1.0 reorg'!C362</f>
-        <v>EA67</v>
+        <v>0</v>
       </c>
       <c r="D361">
         <f>'Bowtie v1.0 reorg'!D362</f>
-        <v>60007</v>
-      </c>
-      <c r="E361">
+        <v>0</v>
+      </c>
+      <c r="E361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F362),"",'Bowtie v1.0 reorg'!F362)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G362),"",'Bowtie v1.0 reorg'!G362)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I362),"",'Bowtie v1.0 reorg'!I362)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J362),"",'Bowtie v1.0 reorg'!J362)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H362),"",'Bowtie v1.0 reorg'!H362)</f>
-        <v>status help question</v>
+        <v/>
       </c>
       <c r="J361" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K362),"",'Bowtie v1.0 reorg'!K362)</f>
-        <v>This is a smaller version of bowtie-status-help. It is used for stacking with bowtie-dot.</v>
-      </c>
-      <c r="K361" t="str">
+        <v/>
+      </c>
+      <c r="K361" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':360,'name':'status-help-sm','unicode':'EA67','decimal':60007,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','help','question'],'usage':'This is a smaller version of bowtie-status-help. It is used for stacking with bowtie-dot.'}</v>
-      </c>
-      <c r="L361" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L361" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":360,"name":"status-help-sm","unicode":"EA67","decimal":60007,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","help","question"],"usage":"This is a smaller version of bowtie-status-help. It is used for stacking with bowtie-dot."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="362" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A362">
         <f>'Bowtie v1.0 reorg'!A363</f>
-        <v>361</v>
-      </c>
-      <c r="B362" t="str">
+        <v>0</v>
+      </c>
+      <c r="B362">
         <f>'Bowtie v1.0 reorg'!E363</f>
-        <v>status-stop-sm</v>
-      </c>
-      <c r="C362" t="str">
+        <v>0</v>
+      </c>
+      <c r="C362">
         <f>'Bowtie v1.0 reorg'!C363</f>
-        <v>EA68</v>
+        <v>0</v>
       </c>
       <c r="D362">
         <f>'Bowtie v1.0 reorg'!D363</f>
-        <v>60008</v>
-      </c>
-      <c r="E362">
+        <v>0</v>
+      </c>
+      <c r="E362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F363),"",'Bowtie v1.0 reorg'!F363)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G363),"",'Bowtie v1.0 reorg'!G363)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I363),"",'Bowtie v1.0 reorg'!I363)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J363),"",'Bowtie v1.0 reorg'!J363)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H363),"",'Bowtie v1.0 reorg'!H363)</f>
-        <v>status stop square</v>
+        <v/>
       </c>
       <c r="J362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K363),"",'Bowtie v1.0 reorg'!K363)</f>
-        <v>This is a smaller version of bowtie-status-stop. It is used for stacking with bowtie-dot.</v>
-      </c>
-      <c r="K362" t="str">
+        <v/>
+      </c>
+      <c r="K362" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':361,'name':'status-stop-sm','unicode':'EA68','decimal':60008,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','stop','square'],'usage':'This is a smaller version of bowtie-status-stop. It is used for stacking with bowtie-dot.'}</v>
-      </c>
-      <c r="L362" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L362" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":361,"name":"status-stop-sm","unicode":"EA68","decimal":60008,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","stop","square"],"usage":"This is a smaller version of bowtie-status-stop. It is used for stacking with bowtie-dot."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="363" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A363">
         <f>'Bowtie v1.0 reorg'!A364</f>
-        <v>362</v>
-      </c>
-      <c r="B363" t="str">
+        <v>0</v>
+      </c>
+      <c r="B363">
         <f>'Bowtie v1.0 reorg'!E364</f>
-        <v>status-pause-sm</v>
-      </c>
-      <c r="C363" t="str">
+        <v>0</v>
+      </c>
+      <c r="C363">
         <f>'Bowtie v1.0 reorg'!C364</f>
-        <v>EA69</v>
+        <v>0</v>
       </c>
       <c r="D363">
         <f>'Bowtie v1.0 reorg'!D364</f>
-        <v>60009</v>
-      </c>
-      <c r="E363">
+        <v>0</v>
+      </c>
+      <c r="E363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F364),"",'Bowtie v1.0 reorg'!F364)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G364),"",'Bowtie v1.0 reorg'!G364)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I364),"",'Bowtie v1.0 reorg'!I364)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J364),"",'Bowtie v1.0 reorg'!J364)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H364),"",'Bowtie v1.0 reorg'!H364)</f>
-        <v>status pause</v>
+        <v/>
       </c>
       <c r="J363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K364),"",'Bowtie v1.0 reorg'!K364)</f>
-        <v>This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot.</v>
-      </c>
-      <c r="K363" t="str">
+        <v/>
+      </c>
+      <c r="K363" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':362,'name':'status-pause-sm','unicode':'EA69','decimal':60009,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','pause'],'usage':'This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot.'}</v>
-      </c>
-      <c r="L363" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L363" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":362,"name":"status-pause-sm","unicode":"EA69","decimal":60009,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","pause"],"usage":"This is a smaller version of bowtie-status-success. It is used for stacking with bowtie-dot."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A364">
         <f>'Bowtie v1.0 reorg'!A365</f>
-        <v>363</v>
-      </c>
-      <c r="B364" t="str">
+        <v>0</v>
+      </c>
+      <c r="B364">
         <f>'Bowtie v1.0 reorg'!E365</f>
-        <v>status-waiting-fill-sm</v>
-      </c>
-      <c r="C364" t="str">
+        <v>0</v>
+      </c>
+      <c r="C364">
         <f>'Bowtie v1.0 reorg'!C365</f>
-        <v>EA6A</v>
+        <v>0</v>
       </c>
       <c r="D364">
         <f>'Bowtie v1.0 reorg'!D365</f>
-        <v>60010</v>
-      </c>
-      <c r="E364">
+        <v>0</v>
+      </c>
+      <c r="E364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F365),"",'Bowtie v1.0 reorg'!F365)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G365),"",'Bowtie v1.0 reorg'!G365)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I365),"",'Bowtie v1.0 reorg'!I365)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J365),"",'Bowtie v1.0 reorg'!J365)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H365),"",'Bowtie v1.0 reorg'!H365)</f>
-        <v>status waiting clock time pending queue</v>
+        <v/>
       </c>
       <c r="J364" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K365),"",'Bowtie v1.0 reorg'!K365)</f>
-        <v>This is a smaller version of bowtie-status-waiting-fill. It is used for stacking with bowtie-dot.</v>
-      </c>
-      <c r="K364" t="str">
+        <v/>
+      </c>
+      <c r="K364" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':363,'name':'status-waiting-fill-sm','unicode':'EA6A','decimal':60010,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','waiting','clock','time','pending','queue'],'usage':'This is a smaller version of bowtie-status-waiting-fill. It is used for stacking with bowtie-dot.'}</v>
-      </c>
-      <c r="L364" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L364" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":363,"name":"status-waiting-fill-sm","unicode":"EA6A","decimal":60010,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","waiting","clock","time","pending","queue"],"usage":"This is a smaller version of bowtie-status-waiting-fill. It is used for stacking with bowtie-dot."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="365" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A365">
         <f>'Bowtie v1.0 reorg'!A366</f>
-        <v>364</v>
-      </c>
-      <c r="B365" t="str">
+        <v>0</v>
+      </c>
+      <c r="B365">
         <f>'Bowtie v1.0 reorg'!E366</f>
-        <v>status-no-fill-sm</v>
-      </c>
-      <c r="C365" t="str">
+        <v>0</v>
+      </c>
+      <c r="C365">
         <f>'Bowtie v1.0 reorg'!C366</f>
-        <v>EA6B</v>
+        <v>0</v>
       </c>
       <c r="D365">
         <f>'Bowtie v1.0 reorg'!D366</f>
-        <v>60011</v>
-      </c>
-      <c r="E365">
+        <v>0</v>
+      </c>
+      <c r="E365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F366),"",'Bowtie v1.0 reorg'!F366)</f>
-        <v>1.1000000000000001</v>
+        <v/>
       </c>
       <c r="F365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G366),"",'Bowtie v1.0 reorg'!G366)</f>
-        <v>bold</v>
+        <v/>
       </c>
       <c r="G365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I366),"",'Bowtie v1.0 reorg'!I366)</f>
-        <v>VSTS</v>
+        <v/>
       </c>
       <c r="H365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J366),"",'Bowtie v1.0 reorg'!J366)</f>
-        <v>Status</v>
+        <v/>
       </c>
       <c r="I365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H366),"",'Bowtie v1.0 reorg'!H366)</f>
-        <v>status no block mute unavailable</v>
+        <v/>
       </c>
       <c r="J365" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K366),"",'Bowtie v1.0 reorg'!K366)</f>
-        <v>This is a smaller version of bowtie-status-no-fill. It is used for stacking with bowtie-dot.</v>
-      </c>
-      <c r="K365" t="str">
+        <v/>
+      </c>
+      <c r="K365" t="e">
         <f t="shared" si="12"/>
-        <v>{'id':364,'name':'status-no-fill-sm','unicode':'EA6B','decimal':60011,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['status','no','block','mute','unavailable'],'usage':'This is a smaller version of bowtie-status-no-fill. It is used for stacking with bowtie-dot.'}</v>
-      </c>
-      <c r="L365" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L365" t="e">
         <f t="shared" si="13"/>
-        <v>{"id":364,"name":"status-no-fill-sm","unicode":"EA6B","decimal":60011,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["status","no","block","mute","unavailable"],"usage":"This is a smaller version of bowtie-status-no-fill. It is used for stacking with bowtie-dot."}</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="366" spans="1:12" x14ac:dyDescent="0.25">
@@ -59861,7 +58884,7 @@
         <v>435</v>
       </c>
       <c r="B436" t="s">
-        <v>889</v>
+        <v>858</v>
       </c>
       <c r="C436" t="str">
         <f>'Bowtie v1.0 reorg'!C437</f>
@@ -59884,10 +58907,10 @@
         <v>597</v>
       </c>
       <c r="I436" t="s">
-        <v>890</v>
+        <v>859</v>
       </c>
       <c r="J436" t="s">
-        <v>891</v>
+        <v>860</v>
       </c>
       <c r="K436" t="str">
         <f t="shared" si="14"/>

</xml_diff>

<commit_message>
added new icon search-in-branch
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="889">
   <si>
     <t>name</t>
   </si>
@@ -2678,6 +2678,15 @@
   </si>
   <si>
     <t>package collection group registry box repository</t>
+  </si>
+  <si>
+    <t>search-in-branch</t>
+  </si>
+  <si>
+    <t>search branch version control magnifying glass</t>
+  </si>
+  <si>
+    <t>Search within a branch.</t>
   </si>
 </sst>
 </file>
@@ -21959,9 +21968,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A354" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H358" sqref="H358"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A353" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E358" sqref="E358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -33991,6 +34000,31 @@
       </c>
       <c r="D358">
         <v>60003</v>
+      </c>
+      <c r="E358" t="s">
+        <v>886</v>
+      </c>
+      <c r="F358">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G358" t="s">
+        <v>17</v>
+      </c>
+      <c r="H358" t="s">
+        <v>887</v>
+      </c>
+      <c r="I358" t="s">
+        <v>15</v>
+      </c>
+      <c r="J358" t="s">
+        <v>670</v>
+      </c>
+      <c r="K358" t="s">
+        <v>888</v>
+      </c>
+      <c r="L358" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA63-search-in-branch.svg</v>
       </c>
     </row>
     <row r="359" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37324,7 +37358,7 @@
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="L352" sqref="L1:L1048576"/>
+      <selection activeCell="L357" sqref="L357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55122,9 +55156,9 @@
         <f>'Bowtie v1.0 reorg'!A358</f>
         <v>356</v>
       </c>
-      <c r="B357">
+      <c r="B357" t="str">
         <f>'Bowtie v1.0 reorg'!E358</f>
-        <v>0</v>
+        <v>search-in-branch</v>
       </c>
       <c r="C357" t="str">
         <f>'Bowtie v1.0 reorg'!C358</f>
@@ -55134,37 +55168,37 @@
         <f>'Bowtie v1.0 reorg'!D358</f>
         <v>60003</v>
       </c>
-      <c r="E357" t="str">
+      <c r="E357">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F358),"",'Bowtie v1.0 reorg'!F358)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G358),"",'Bowtie v1.0 reorg'!G358)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I358),"",'Bowtie v1.0 reorg'!I358)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J358),"",'Bowtie v1.0 reorg'!J358)</f>
-        <v/>
+        <v>Code</v>
       </c>
       <c r="I357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H358),"",'Bowtie v1.0 reorg'!H358)</f>
-        <v/>
+        <v>search branch version control magnifying glass</v>
       </c>
       <c r="J357" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K358),"",'Bowtie v1.0 reorg'!K358)</f>
-        <v/>
-      </c>
-      <c r="K357" t="e">
+        <v>Search within a branch.</v>
+      </c>
+      <c r="K357" t="str">
         <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L357" t="e">
+        <v>{'id':356,'name':'search-in-branch','unicode':'EA63','decimal':60003,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['search','branch','version','control','magnifying','glass'],'usage':'Search within a branch.'}</v>
+      </c>
+      <c r="L357" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+        <v>{"id":356,"name":"search-in-branch","unicode":"EA63","decimal":60003,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["search","branch","version","control","magnifying","glass"],"usage":"Search within a branch."}</v>
       </c>
     </row>
     <row r="358" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added the status-xxx-sm glyphs back to temporarily fix the broken references. will work with the outdated feature to update reference to use full size status icons for stacking
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17531"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720" activeTab="1"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="901">
   <si>
     <t>name</t>
   </si>
@@ -2687,6 +2687,42 @@
   </si>
   <si>
     <t>Search within a branch.</t>
+  </si>
+  <si>
+    <t>status-success-sm</t>
+  </si>
+  <si>
+    <t>status-warning-sm</t>
+  </si>
+  <si>
+    <t>status-info-sm</t>
+  </si>
+  <si>
+    <t>status-failure-sm</t>
+  </si>
+  <si>
+    <t>status-error-sm</t>
+  </si>
+  <si>
+    <t>status-run-sm</t>
+  </si>
+  <si>
+    <t>status-help-sm</t>
+  </si>
+  <si>
+    <t>status-stop-sm</t>
+  </si>
+  <si>
+    <t>status-pause-sm</t>
+  </si>
+  <si>
+    <t>status-waiting-fill-sm</t>
+  </si>
+  <si>
+    <t>status-no-fill-sm</t>
+  </si>
+  <si>
+    <t>Temporary solution for badging.</t>
   </si>
 </sst>
 </file>
@@ -21968,9 +22004,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A353" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E358" sqref="E358"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K444" sqref="K444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -36983,9 +37019,21 @@
       <c r="D444">
         <v>60089</v>
       </c>
+      <c r="E444" t="s">
+        <v>889</v>
+      </c>
+      <c r="F444">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G444" t="s">
+        <v>16</v>
+      </c>
+      <c r="K444" t="s">
+        <v>900</v>
+      </c>
       <c r="L444" t="str">
         <f t="shared" si="13"/>
-        <v>uEAB9-.svg</v>
+        <v>uEAB9-status-success-sm.svg</v>
       </c>
     </row>
     <row r="445" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -36999,9 +37047,21 @@
       <c r="D445">
         <v>60090</v>
       </c>
+      <c r="E445" t="s">
+        <v>890</v>
+      </c>
+      <c r="F445">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G445" t="s">
+        <v>16</v>
+      </c>
+      <c r="K445" t="s">
+        <v>900</v>
+      </c>
       <c r="L445" t="str">
         <f t="shared" si="13"/>
-        <v>uEABA-.svg</v>
+        <v>uEABA-status-warning-sm.svg</v>
       </c>
     </row>
     <row r="446" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37015,9 +37075,21 @@
       <c r="D446">
         <v>60091</v>
       </c>
+      <c r="E446" t="s">
+        <v>891</v>
+      </c>
+      <c r="F446">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G446" t="s">
+        <v>16</v>
+      </c>
+      <c r="K446" t="s">
+        <v>900</v>
+      </c>
       <c r="L446" t="str">
         <f t="shared" si="13"/>
-        <v>uEABB-.svg</v>
+        <v>uEABB-status-info-sm.svg</v>
       </c>
     </row>
     <row r="447" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37031,9 +37103,21 @@
       <c r="D447">
         <v>60092</v>
       </c>
+      <c r="E447" t="s">
+        <v>892</v>
+      </c>
+      <c r="F447">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G447" t="s">
+        <v>16</v>
+      </c>
+      <c r="K447" t="s">
+        <v>900</v>
+      </c>
       <c r="L447" t="str">
         <f t="shared" si="13"/>
-        <v>uEABC-.svg</v>
+        <v>uEABC-status-failure-sm.svg</v>
       </c>
     </row>
     <row r="448" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37047,9 +37131,21 @@
       <c r="D448">
         <v>60093</v>
       </c>
+      <c r="E448" t="s">
+        <v>893</v>
+      </c>
+      <c r="F448">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G448" t="s">
+        <v>16</v>
+      </c>
+      <c r="K448" t="s">
+        <v>900</v>
+      </c>
       <c r="L448" t="str">
         <f t="shared" si="13"/>
-        <v>uEABD-.svg</v>
+        <v>uEABD-status-error-sm.svg</v>
       </c>
     </row>
     <row r="449" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37063,9 +37159,21 @@
       <c r="D449">
         <v>60094</v>
       </c>
+      <c r="E449" t="s">
+        <v>894</v>
+      </c>
+      <c r="F449">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G449" t="s">
+        <v>16</v>
+      </c>
+      <c r="K449" t="s">
+        <v>900</v>
+      </c>
       <c r="L449" t="str">
         <f t="shared" si="13"/>
-        <v>uEABE-.svg</v>
+        <v>uEABE-status-run-sm.svg</v>
       </c>
     </row>
     <row r="450" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37079,9 +37187,21 @@
       <c r="D450">
         <v>60095</v>
       </c>
+      <c r="E450" t="s">
+        <v>895</v>
+      </c>
+      <c r="F450">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G450" t="s">
+        <v>16</v>
+      </c>
+      <c r="K450" t="s">
+        <v>900</v>
+      </c>
       <c r="L450" t="str">
         <f t="shared" si="13"/>
-        <v>uEABF-.svg</v>
+        <v>uEABF-status-help-sm.svg</v>
       </c>
     </row>
     <row r="451" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37089,15 +37209,27 @@
         <v>449</v>
       </c>
       <c r="C451" t="str">
-        <f t="shared" ref="C451:C454" si="15">DEC2HEX(D451)</f>
+        <f t="shared" ref="C451:C468" si="15">DEC2HEX(D451)</f>
         <v>EAC0</v>
       </c>
       <c r="D451">
         <v>60096</v>
       </c>
+      <c r="E451" t="s">
+        <v>896</v>
+      </c>
+      <c r="F451">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G451" t="s">
+        <v>16</v>
+      </c>
+      <c r="K451" t="s">
+        <v>900</v>
+      </c>
       <c r="L451" t="str">
         <f t="shared" si="13"/>
-        <v>uEAC0-.svg</v>
+        <v>uEAC0-status-stop-sm.svg</v>
       </c>
     </row>
     <row r="452" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37111,9 +37243,21 @@
       <c r="D452">
         <v>60097</v>
       </c>
+      <c r="E452" t="s">
+        <v>897</v>
+      </c>
+      <c r="F452">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G452" t="s">
+        <v>16</v>
+      </c>
+      <c r="K452" t="s">
+        <v>900</v>
+      </c>
       <c r="L452" t="str">
         <f t="shared" ref="L452:L466" si="16">CONCATENATE("u",C452,"-",E452,".svg")</f>
-        <v>uEAC1-.svg</v>
+        <v>uEAC1-status-pause-sm.svg</v>
       </c>
     </row>
     <row r="453" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37127,9 +37271,21 @@
       <c r="D453">
         <v>60098</v>
       </c>
+      <c r="E453" t="s">
+        <v>898</v>
+      </c>
+      <c r="F453">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G453" t="s">
+        <v>16</v>
+      </c>
+      <c r="K453" t="s">
+        <v>900</v>
+      </c>
       <c r="L453" t="str">
         <f t="shared" si="16"/>
-        <v>uEAC2-.svg</v>
+        <v>uEAC2-status-waiting-fill-sm.svg</v>
       </c>
     </row>
     <row r="454" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37143,139 +37299,219 @@
       <c r="D454">
         <v>60099</v>
       </c>
+      <c r="E454" t="s">
+        <v>899</v>
+      </c>
+      <c r="F454">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G454" t="s">
+        <v>16</v>
+      </c>
+      <c r="K454" t="s">
+        <v>900</v>
+      </c>
       <c r="L454" t="str">
         <f t="shared" si="16"/>
-        <v>uEAC3-.svg</v>
+        <v>uEAC3-status-no-fill-sm.svg</v>
       </c>
     </row>
     <row r="455" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>453</v>
       </c>
+      <c r="C455" t="str">
+        <f t="shared" si="15"/>
+        <v>EAC4</v>
+      </c>
       <c r="D455">
         <v>60100</v>
       </c>
+      <c r="F455">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="L455" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>uEAC4-.svg</v>
       </c>
     </row>
     <row r="456" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>454</v>
       </c>
+      <c r="C456" t="str">
+        <f t="shared" si="15"/>
+        <v>EAC5</v>
+      </c>
       <c r="D456">
         <v>60101</v>
       </c>
+      <c r="F456">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="L456" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>uEAC5-.svg</v>
       </c>
     </row>
     <row r="457" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>455</v>
       </c>
+      <c r="C457" t="str">
+        <f t="shared" si="15"/>
+        <v>EAC6</v>
+      </c>
       <c r="D457">
         <v>60102</v>
       </c>
+      <c r="F457">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="L457" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>uEAC6-.svg</v>
       </c>
     </row>
     <row r="458" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>456</v>
       </c>
+      <c r="C458" t="str">
+        <f t="shared" si="15"/>
+        <v>EAC7</v>
+      </c>
       <c r="D458">
         <v>60103</v>
       </c>
+      <c r="F458">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="L458" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>uEAC7-.svg</v>
       </c>
     </row>
     <row r="459" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>457</v>
       </c>
+      <c r="C459" t="str">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="L459" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>u0-.svg</v>
       </c>
     </row>
     <row r="460" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>458</v>
       </c>
+      <c r="C460" t="str">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="L460" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>u0-.svg</v>
       </c>
     </row>
     <row r="461" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>459</v>
       </c>
+      <c r="C461" t="str">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="L461" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>u0-.svg</v>
       </c>
     </row>
     <row r="462" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>460</v>
       </c>
+      <c r="C462" t="str">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="L462" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>u0-.svg</v>
       </c>
     </row>
     <row r="463" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>461</v>
       </c>
+      <c r="C463" t="str">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="L463" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>u0-.svg</v>
       </c>
     </row>
     <row r="464" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>462</v>
       </c>
+      <c r="C464" t="str">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="L464" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>u0-.svg</v>
       </c>
     </row>
     <row r="465" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>463</v>
       </c>
+      <c r="C465" t="str">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="L465" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>u0-.svg</v>
       </c>
     </row>
     <row r="466" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>464</v>
       </c>
+      <c r="C466" t="str">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
       <c r="L466" t="str">
         <f t="shared" si="16"/>
-        <v>u-.svg</v>
+        <v>u0-.svg</v>
       </c>
     </row>
     <row r="467" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>465</v>
       </c>
+      <c r="C467" t="str">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="468" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>466</v>
+      </c>
+      <c r="C468" t="str">
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
     </row>
     <row r="469" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37357,8 +37593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="L357" sqref="L357"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L453" sqref="L2:L453"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56793,11 +57029,11 @@
         <v>Used for Sass stylesheet (.sass, .scss) file node in code explorer tree view.</v>
       </c>
       <c r="K389" t="str">
-        <f t="shared" ref="K389:K452" si="14">IF(NOT(ISBLANK(A389)),CONCATENATE("{'",$A$1,"':",A389,",'",$B$1,"':'",B389,"',","'",$C$1,"':'",C389,"','",$D$1,"':",D389,",'",$E$1,"':'",FIXED(E389,1),"','",$F$1,"':'",F389,"','",$G$1,"':'",G389,"','",$H$1,"':'",H389,"','",$I$1,"':['",SUBSTITUTE(I389," ","','"),"'],'",$J$1,"':'",J389,"'}"))</f>
+        <f>IF(NOT(ISBLANK(A389)),CONCATENATE("{'",$A$1,"':",A389,",'",$B$1,"':'",B389,"',","'",$C$1,"':'",C389,"','",$D$1,"':",D389,",'",$E$1,"':'",FIXED(E389,1),"','",$F$1,"':'",F389,"','",$G$1,"':'",G389,"','",$H$1,"':'",H389,"','",$I$1,"':['",SUBSTITUTE(I389," ","','"),"'],'",$J$1,"':'",J389,"'}"))</f>
         <v>{'id':388,'name':'file-type-sass','unicode':'EA83','decimal':60035,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','css','sass','scss','stylesheet'],'usage':'Used for Sass stylesheet (.sass, .scss) file node in code explorer tree view.'}</v>
       </c>
       <c r="L389" t="str">
-        <f t="shared" ref="L389:L452" si="15">SUBSTITUTE(K389,"'","""")</f>
+        <f t="shared" ref="L389:L452" si="14">SUBSTITUTE(K389,"'","""")</f>
         <v>{"id":388,"name":"file-type-sass","unicode":"EA83","decimal":60035,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","css","sass","scss","stylesheet"],"usage":"Used for Sass stylesheet (.sass, .scss) file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -56843,11 +57079,11 @@
         <v>Used for Less stylesheet (.less) file node in code explorer tree view.</v>
       </c>
       <c r="K390" t="str">
+        <f>IF(NOT(ISBLANK(A390)),CONCATENATE("{'",$A$1,"':",A390,",'",$B$1,"':'",B390,"',","'",$C$1,"':'",C390,"','",$D$1,"':",D390,",'",$E$1,"':'",FIXED(E390,1),"','",$F$1,"':'",F390,"','",$G$1,"':'",G390,"','",$H$1,"':'",H390,"','",$I$1,"':['",SUBSTITUTE(I390," ","','"),"'],'",$J$1,"':'",J390,"'}"))</f>
+        <v>{'id':389,'name':'file-type-less','unicode':'EA84','decimal':60036,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','css','less','stylesheet'],'usage':'Used for Less stylesheet (.less) file node in code explorer tree view.'}</v>
+      </c>
+      <c r="L390" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':389,'name':'file-type-less','unicode':'EA84','decimal':60036,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','css','less','stylesheet'],'usage':'Used for Less stylesheet (.less) file node in code explorer tree view.'}</v>
-      </c>
-      <c r="L390" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":389,"name":"file-type-less","unicode":"EA84","decimal":60036,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","css","less","stylesheet"],"usage":"Used for Less stylesheet (.less) file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -56893,11 +57129,11 @@
         <v>Used for .json file node in code explorer tree view.</v>
       </c>
       <c r="K391" t="str">
+        <f>IF(NOT(ISBLANK(A391)),CONCATENATE("{'",$A$1,"':",A391,",'",$B$1,"':'",B391,"',","'",$C$1,"':'",C391,"','",$D$1,"':",D391,",'",$E$1,"':'",FIXED(E391,1),"','",$F$1,"':'",F391,"','",$G$1,"':'",G391,"','",$H$1,"':'",H391,"','",$I$1,"':['",SUBSTITUTE(I391," ","','"),"'],'",$J$1,"':'",J391,"'}"))</f>
+        <v>{'id':390,'name':'file-type-json','unicode':'EA85','decimal':60037,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','json'],'usage':'Used for .json file node in code explorer tree view.'}</v>
+      </c>
+      <c r="L391" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':390,'name':'file-type-json','unicode':'EA85','decimal':60037,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','json'],'usage':'Used for .json file node in code explorer tree view.'}</v>
-      </c>
-      <c r="L391" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":390,"name":"file-type-json","unicode":"EA85","decimal":60037,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","json"],"usage":"Used for .json file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -56943,11 +57179,11 @@
         <v>Used for .xml file node in code explorer tree view.</v>
       </c>
       <c r="K392" t="str">
+        <f>IF(NOT(ISBLANK(A392)),CONCATENATE("{'",$A$1,"':",A392,",'",$B$1,"':'",B392,"',","'",$C$1,"':'",C392,"','",$D$1,"':",D392,",'",$E$1,"':'",FIXED(E392,1),"','",$F$1,"':'",F392,"','",$G$1,"':'",G392,"','",$H$1,"':'",H392,"','",$I$1,"':['",SUBSTITUTE(I392," ","','"),"'],'",$J$1,"':'",J392,"'}"))</f>
+        <v>{'id':391,'name':'file-type-xml','unicode':'EA86','decimal':60038,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','xml','markup'],'usage':'Used for .xml file node in code explorer tree view.'}</v>
+      </c>
+      <c r="L392" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':391,'name':'file-type-xml','unicode':'EA86','decimal':60038,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','xml','markup'],'usage':'Used for .xml file node in code explorer tree view.'}</v>
-      </c>
-      <c r="L392" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":391,"name":"file-type-xml","unicode":"EA86","decimal":60038,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","xml","markup"],"usage":"Used for .xml file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -56993,11 +57229,11 @@
         <v>Used for .md, .markdown file node in code explorer tree view.</v>
       </c>
       <c r="K393" t="str">
+        <f>IF(NOT(ISBLANK(A393)),CONCATENATE("{'",$A$1,"':",A393,",'",$B$1,"':'",B393,"',","'",$C$1,"':'",C393,"','",$D$1,"':",D393,",'",$E$1,"':'",FIXED(E393,1),"','",$F$1,"':'",F393,"','",$G$1,"':'",G393,"','",$H$1,"':'",H393,"','",$I$1,"':['",SUBSTITUTE(I393," ","','"),"'],'",$J$1,"':'",J393,"'}"))</f>
+        <v>{'id':392,'name':'file-type-md','unicode':'EA87','decimal':60039,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','md','markdown'],'usage':'Used for .md, .markdown file node in code explorer tree view.'}</v>
+      </c>
+      <c r="L393" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':392,'name':'file-type-md','unicode':'EA87','decimal':60039,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','md','markdown'],'usage':'Used for .md, .markdown file node in code explorer tree view.'}</v>
-      </c>
-      <c r="L393" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":392,"name":"file-type-md","unicode":"EA87","decimal":60039,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","md","markdown"],"usage":"Used for .md, .markdown file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57043,11 +57279,11 @@
         <v>Used for PowerShell (.ps1) file node in code explorer tree view.</v>
       </c>
       <c r="K394" t="str">
+        <f>IF(NOT(ISBLANK(A394)),CONCATENATE("{'",$A$1,"':",A394,",'",$B$1,"':'",B394,"',","'",$C$1,"':'",C394,"','",$D$1,"':",D394,",'",$E$1,"':'",FIXED(E394,1),"','",$F$1,"':'",F394,"','",$G$1,"':'",G394,"','",$H$1,"':'",H394,"','",$I$1,"':['",SUBSTITUTE(I394," ","','"),"'],'",$J$1,"':'",J394,"'}"))</f>
+        <v>{'id':393,'name':'file-type-powershell','unicode':'EA88','decimal':60040,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','powershell','ps1'],'usage':'Used for PowerShell (.ps1) file node in code explorer tree view.'}</v>
+      </c>
+      <c r="L394" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':393,'name':'file-type-powershell','unicode':'EA88','decimal':60040,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','powershell','ps1'],'usage':'Used for PowerShell (.ps1) file node in code explorer tree view.'}</v>
-      </c>
-      <c r="L394" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":393,"name":"file-type-powershell","unicode":"EA88","decimal":60040,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","powershell","ps1"],"usage":"Used for PowerShell (.ps1) file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57093,11 +57329,11 @@
         <v>Used for .cmd file node in code explorer tree view.</v>
       </c>
       <c r="K395" t="str">
+        <f>IF(NOT(ISBLANK(A395)),CONCATENATE("{'",$A$1,"':",A395,",'",$B$1,"':'",B395,"',","'",$C$1,"':'",C395,"','",$D$1,"':",D395,",'",$E$1,"':'",FIXED(E395,1),"','",$F$1,"':'",F395,"','",$G$1,"':'",G395,"','",$H$1,"':'",H395,"','",$I$1,"':['",SUBSTITUTE(I395," ","','"),"'],'",$J$1,"':'",J395,"'}"))</f>
+        <v>{'id':394,'name':'file-type-cmd','unicode':'EA89','decimal':60041,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','cmd'],'usage':'Used for .cmd file node in code explorer tree view.'}</v>
+      </c>
+      <c r="L395" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':394,'name':'file-type-cmd','unicode':'EA89','decimal':60041,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','cmd'],'usage':'Used for .cmd file node in code explorer tree view.'}</v>
-      </c>
-      <c r="L395" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":394,"name":"file-type-cmd","unicode":"EA89","decimal":60041,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","cmd"],"usage":"Used for .cmd file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57143,11 +57379,11 @@
         <v>Used for .java file node in code explorer tree view.</v>
       </c>
       <c r="K396" t="str">
+        <f>IF(NOT(ISBLANK(A396)),CONCATENATE("{'",$A$1,"':",A396,",'",$B$1,"':'",B396,"',","'",$C$1,"':'",C396,"','",$D$1,"':",D396,",'",$E$1,"':'",FIXED(E396,1),"','",$F$1,"':'",F396,"','",$G$1,"':'",G396,"','",$H$1,"':'",H396,"','",$I$1,"':['",SUBSTITUTE(I396," ","','"),"'],'",$J$1,"':'",J396,"'}"))</f>
+        <v>{'id':395,'name':'file-type-java','unicode':'EA8A','decimal':60042,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','java'],'usage':'Used for .java file node in code explorer tree view.'}</v>
+      </c>
+      <c r="L396" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':395,'name':'file-type-java','unicode':'EA8A','decimal':60042,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','java'],'usage':'Used for .java file node in code explorer tree view.'}</v>
-      </c>
-      <c r="L396" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":395,"name":"file-type-java","unicode":"EA8A","decimal":60042,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","java"],"usage":"Used for .java file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57193,11 +57429,11 @@
         <v>Used for .sql file node in code explorer tree view.</v>
       </c>
       <c r="K397" t="str">
+        <f>IF(NOT(ISBLANK(A397)),CONCATENATE("{'",$A$1,"':",A397,",'",$B$1,"':'",B397,"',","'",$C$1,"':'",C397,"','",$D$1,"':",D397,",'",$E$1,"':'",FIXED(E397,1),"','",$F$1,"':'",F397,"','",$G$1,"':'",G397,"','",$H$1,"':'",H397,"','",$I$1,"':['",SUBSTITUTE(I397," ","','"),"'],'",$J$1,"':'",J397,"'}"))</f>
+        <v>{'id':396,'name':'file-type-sql','unicode':'EA8B','decimal':60043,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','sql'],'usage':'Used for .sql file node in code explorer tree view.'}</v>
+      </c>
+      <c r="L397" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':396,'name':'file-type-sql','unicode':'EA8B','decimal':60043,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','sql'],'usage':'Used for .sql file node in code explorer tree view.'}</v>
-      </c>
-      <c r="L397" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":396,"name":"file-type-sql","unicode":"EA8B","decimal":60043,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","sql"],"usage":"Used for .sql file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57243,11 +57479,11 @@
         <v>Used for resource file (.resx) node in code explorer tree view.</v>
       </c>
       <c r="K398" t="str">
-        <f t="shared" ref="K398:K408" si="16">IF(NOT(ISBLANK(A398)),CONCATENATE("{'",$A$1,"':",A398,",'",$B$1,"':'",B398,"',","'",$C$1,"':'",C398,"','",$D$1,"':",D398,",'",$E$1,"':'",FIXED(E398,1),"','",$F$1,"':'",F398,"','",$G$1,"':'",G398,"','",$H$1,"':'",H398,"','",$I$1,"':['",SUBSTITUTE(I398," ","','"),"'],'",$J$1,"':'",J398,"'}"))</f>
+        <f t="shared" ref="K398:K408" si="15">IF(NOT(ISBLANK(A398)),CONCATENATE("{'",$A$1,"':",A398,",'",$B$1,"':'",B398,"',","'",$C$1,"':'",C398,"','",$D$1,"':",D398,",'",$E$1,"':'",FIXED(E398,1),"','",$F$1,"':'",F398,"','",$G$1,"':'",G398,"','",$H$1,"':'",H398,"','",$I$1,"':['",SUBSTITUTE(I398," ","','"),"'],'",$J$1,"':'",J398,"'}"))</f>
         <v>{'id':397,'name':'file-stack','unicode':'EA8C','decimal':60044,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','stack','group','resx','resource'],'usage':'Used for resource file (.resx) node in code explorer tree view.'}</v>
       </c>
       <c r="L398" t="str">
-        <f t="shared" ref="L398:L408" si="17">SUBSTITUTE(K398,"'","""")</f>
+        <f t="shared" ref="L398:L408" si="16">SUBSTITUTE(K398,"'","""")</f>
         <v>{"id":397,"name":"file-stack","unicode":"EA8C","decimal":60044,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","stack","group","resx","resource"],"usage":"Used for resource file (.resx) node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57293,11 +57529,11 @@
         <v>Generic script file</v>
       </c>
       <c r="K399" t="str">
+        <f t="shared" si="15"/>
+        <v>{'id':398,'name':'script','unicode':'EA8D','decimal':60045,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['script','scroll'],'usage':'Generic script file'}</v>
+      </c>
+      <c r="L399" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':398,'name':'script','unicode':'EA8D','decimal':60045,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['script','scroll'],'usage':'Generic script file'}</v>
-      </c>
-      <c r="L399" t="str">
-        <f t="shared" si="17"/>
         <v>{"id":398,"name":"script","unicode":"EA8D","decimal":60045,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["script","scroll"],"usage":"Generic script file"}</v>
       </c>
     </row>
@@ -57343,11 +57579,11 @@
         <v>Generic executable file such as .bat, .exe</v>
       </c>
       <c r="K400" t="str">
+        <f t="shared" si="15"/>
+        <v>{'id':399,'name':'default-executable','unicode':'EA8E','decimal':60046,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['default','executable','gear','process'],'usage':'Generic executable file such as .bat, .exe'}</v>
+      </c>
+      <c r="L400" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':399,'name':'default-executable','unicode':'EA8E','decimal':60046,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['default','executable','gear','process'],'usage':'Generic executable file such as .bat, .exe'}</v>
-      </c>
-      <c r="L400" t="str">
-        <f t="shared" si="17"/>
         <v>{"id":399,"name":"default-executable","unicode":"EA8E","decimal":60046,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["default","executable","gear","process"],"usage":"Generic executable file such as .bat, .exe"}</v>
       </c>
     </row>
@@ -57393,11 +57629,11 @@
         <v>Used for templating preprocessor file type like .jade, .haml, etc.</v>
       </c>
       <c r="K401" t="str">
+        <f t="shared" si="15"/>
+        <v>{'id':400,'name':'file-type-template','unicode':'EA8F','decimal':60047,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','template','preprocessor','dotted','line'],'usage':'Used for templating preprocessor file type like .jade, .haml, etc.'}</v>
+      </c>
+      <c r="L401" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':400,'name':'file-type-template','unicode':'EA8F','decimal':60047,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','template','preprocessor','dotted','line'],'usage':'Used for templating preprocessor file type like .jade, .haml, etc.'}</v>
-      </c>
-      <c r="L401" t="str">
-        <f t="shared" si="17"/>
         <v>{"id":400,"name":"file-type-template","unicode":"EA8F","decimal":60047,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","template","preprocessor","dotted","line"],"usage":"Used for templating preprocessor file type like .jade, .haml, etc."}</v>
       </c>
     </row>
@@ -57443,11 +57679,11 @@
         <v>Used for splitting work item.</v>
       </c>
       <c r="K402" t="str">
+        <f t="shared" si="15"/>
+        <v>{'id':401,'name':'split','unicode':'EA90','decimal':60048,'version':'1.1','style':'light','subset':'VSTS','group':'Arrow','keywords':['split','arrow'],'usage':'Used for splitting work item.'}</v>
+      </c>
+      <c r="L402" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':401,'name':'split','unicode':'EA90','decimal':60048,'version':'1.1','style':'light','subset':'VSTS','group':'Arrow','keywords':['split','arrow'],'usage':'Used for splitting work item.'}</v>
-      </c>
-      <c r="L402" t="str">
-        <f t="shared" si="17"/>
         <v>{"id":401,"name":"split","unicode":"EA90","decimal":60048,"version":"1.1","style":"light","subset":"VSTS","group":"Arrow","keywords":["split","arrow"],"usage":"Used for splitting work item."}</v>
       </c>
     </row>
@@ -57493,11 +57729,11 @@
         <v>Used for capturing user actions in the form of an image action log, in TCM Web Runner.</v>
       </c>
       <c r="K403" t="str">
+        <f t="shared" si="15"/>
+        <v>{'id':402,'name':'image-action-log','unicode':'EA91','decimal':60049,'version':'1.1','style':'light','subset':'VSTS','group':'Test','keywords':['image','picture','action','crosshair','target'],'usage':'Used for capturing user actions in the form of an image action log, in TCM Web Runner.'}</v>
+      </c>
+      <c r="L403" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':402,'name':'image-action-log','unicode':'EA91','decimal':60049,'version':'1.1','style':'light','subset':'VSTS','group':'Test','keywords':['image','picture','action','crosshair','target'],'usage':'Used for capturing user actions in the form of an image action log, in TCM Web Runner.'}</v>
-      </c>
-      <c r="L403" t="str">
-        <f t="shared" si="17"/>
         <v>{"id":402,"name":"image-action-log","unicode":"EA91","decimal":60049,"version":"1.1","style":"light","subset":"VSTS","group":"Test","keywords":["image","picture","action","crosshair","target"],"usage":"Used for capturing user actions in the form of an image action log, in TCM Web Runner."}</v>
       </c>
     </row>
@@ -57543,11 +57779,11 @@
         <v>Used in version control view of branches.</v>
       </c>
       <c r="K404" t="str">
+        <f t="shared" si="15"/>
+        <v>{'id':403,'name':'shield','unicode':'EA92','decimal':60050,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['shield'],'usage':'Used in version control view of branches.'}</v>
+      </c>
+      <c r="L404" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':403,'name':'shield','unicode':'EA92','decimal':60050,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['shield'],'usage':'Used in version control view of branches.'}</v>
-      </c>
-      <c r="L404" t="str">
-        <f t="shared" si="17"/>
         <v>{"id":403,"name":"shield","unicode":"EA92","decimal":60050,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["shield"],"usage":"Used in version control view of branches."}</v>
       </c>
     </row>
@@ -57593,11 +57829,11 @@
         <v>Used in version control view of branches.</v>
       </c>
       <c r="K405" t="str">
+        <f t="shared" si="15"/>
+        <v>{'id':404,'name':'shield-fill','unicode':'EA93','decimal':60051,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['shield'],'usage':'Used in version control view of branches.'}</v>
+      </c>
+      <c r="L405" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':404,'name':'shield-fill','unicode':'EA93','decimal':60051,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['shield'],'usage':'Used in version control view of branches.'}</v>
-      </c>
-      <c r="L405" t="str">
-        <f t="shared" si="17"/>
         <v>{"id":404,"name":"shield-fill","unicode":"EA93","decimal":60051,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["shield"],"usage":"Used in version control view of branches."}</v>
       </c>
     </row>
@@ -57643,11 +57879,11 @@
         <v>Used in VC view for git fork. Name is tfvc just because the other VC icons are like that.</v>
       </c>
       <c r="K406" t="str">
+        <f t="shared" si="15"/>
+        <v>{'id':405,'name':'tfvc-fork','unicode':'EA94','decimal':60052,'version':'1.1','style':'light','subset':'VSTS','group':'Version Control','keywords':['fork'],'usage':'Used in VC view for git fork. Name is tfvc just because the other VC icons are like that.'}</v>
+      </c>
+      <c r="L406" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':405,'name':'tfvc-fork','unicode':'EA94','decimal':60052,'version':'1.1','style':'light','subset':'VSTS','group':'Version Control','keywords':['fork'],'usage':'Used in VC view for git fork. Name is tfvc just because the other VC icons are like that.'}</v>
-      </c>
-      <c r="L406" t="str">
-        <f t="shared" si="17"/>
         <v>{"id":405,"name":"tfvc-fork","unicode":"EA94","decimal":60052,"version":"1.1","style":"light","subset":"VSTS","group":"Version Control","keywords":["fork"],"usage":"Used in VC view for git fork. Name is tfvc just because the other VC icons are like that."}</v>
       </c>
     </row>
@@ -57693,11 +57929,11 @@
         <v>Used in build view to indicate build is running in progress.</v>
       </c>
       <c r="K407" t="str">
+        <f t="shared" si="15"/>
+        <v>{'id':406,'name':'status-run-box','unicode':'EA95','decimal':60053,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['run','in','progress'],'usage':'Used in build view to indicate build is running in progress.'}</v>
+      </c>
+      <c r="L407" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':406,'name':'status-run-box','unicode':'EA95','decimal':60053,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['run','in','progress'],'usage':'Used in build view to indicate build is running in progress.'}</v>
-      </c>
-      <c r="L407" t="str">
-        <f t="shared" si="17"/>
         <v>{"id":406,"name":"status-run-box","unicode":"EA95","decimal":60053,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["run","in","progress"],"usage":"Used in build view to indicate build is running in progress."}</v>
       </c>
     </row>
@@ -57743,11 +57979,11 @@
         <v>Import</v>
       </c>
       <c r="K408" t="str">
+        <f t="shared" si="15"/>
+        <v>{'id':407,'name':'arrow-import','unicode':'EA96','decimal':60054,'version':'1.1','style':'light','subset':'VSTS','group':'Arrow','keywords':['arrow','import'],'usage':'Import'}</v>
+      </c>
+      <c r="L408" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':407,'name':'arrow-import','unicode':'EA96','decimal':60054,'version':'1.1','style':'light','subset':'VSTS','group':'Arrow','keywords':['arrow','import'],'usage':'Import'}</v>
-      </c>
-      <c r="L408" t="str">
-        <f t="shared" si="17"/>
         <v>{"id":407,"name":"arrow-import","unicode":"EA96","decimal":60054,"version":"1.1","style":"light","subset":"VSTS","group":"Arrow","keywords":["arrow","import"],"usage":"Import"}</v>
       </c>
     </row>
@@ -57793,11 +58029,11 @@
         <v>Add new team project.</v>
       </c>
       <c r="K409" t="str">
+        <f>IF(NOT(ISBLANK(A409)),CONCATENATE("{'",$A$1,"':",A409,",'",$B$1,"':'",B409,"',","'",$C$1,"':'",C409,"','",$D$1,"':",D409,",'",$E$1,"':'",FIXED(E409,1),"','",$F$1,"':'",F409,"','",$G$1,"':'",G409,"','",$H$1,"':'",H409,"','",$I$1,"':['",SUBSTITUTE(I409," ","','"),"'],'",$J$1,"':'",J409,"'}"))</f>
+        <v>{'id':408,'name':'new-team-project','unicode':'EA97','decimal':60055,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['new','add','project','folder','plus','chevron'],'usage':'Add new team project.'}</v>
+      </c>
+      <c r="L409" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':408,'name':'new-team-project','unicode':'EA97','decimal':60055,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['new','add','project','folder','plus','chevron'],'usage':'Add new team project.'}</v>
-      </c>
-      <c r="L409" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":408,"name":"new-team-project","unicode":"EA97","decimal":60055,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["new","add","project","folder","plus","chevron"],"usage":"Add new team project."}</v>
       </c>
     </row>
@@ -57843,11 +58079,11 @@
         <v>Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds.</v>
       </c>
       <c r="K410" t="str">
+        <f>IF(NOT(ISBLANK(A410)),CONCATENATE("{'",$A$1,"':",A410,",'",$B$1,"':'",B410,"',","'",$C$1,"':'",C410,"','",$D$1,"':",D410,",'",$E$1,"':'",FIXED(E410,1),"','",$F$1,"':'",F410,"','",$G$1,"':'",G410,"','",$H$1,"':'",H410,"','",$I$1,"':['",SUBSTITUTE(I410," ","','"),"'],'",$J$1,"':'",J410,"'}"))</f>
+        <v>{'id':409,'name':'package-feed-mix','unicode':'EA98','decimal':60056,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','mix','box','square'],'usage':'Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds.'}</v>
+      </c>
+      <c r="L410" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':409,'name':'package-feed-mix','unicode':'EA98','decimal':60056,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','mix','box','square'],'usage':'Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds.'}</v>
-      </c>
-      <c r="L410" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":409,"name":"package-feed-mix","unicode":"EA98","decimal":60056,"version":"1.1","style":"light","subset":"VSTS","group":"Package","keywords":["package","feed","mix","box","square"],"usage":"Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds."}</v>
       </c>
     </row>
@@ -57893,11 +58129,11 @@
         <v>Used in Package hub treeview to represent package feed is a reference to remote repo.</v>
       </c>
       <c r="K411" t="str">
+        <f>IF(NOT(ISBLANK(A411)),CONCATENATE("{'",$A$1,"':",A411,",'",$B$1,"':'",B411,"',","'",$C$1,"':'",C411,"','",$D$1,"':",D411,",'",$E$1,"':'",FIXED(E411,1),"','",$F$1,"':'",F411,"','",$G$1,"':'",G411,"','",$H$1,"':'",H411,"','",$I$1,"':['",SUBSTITUTE(I411," ","','"),"'],'",$J$1,"':'",J411,"'}"))</f>
+        <v>{'id':410,'name':'package-feed-remote','unicode':'EA99','decimal':60057,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','remote','signal','reference','wave','virtual','box','square'],'usage':'Used in Package hub treeview to represent package feed is a reference to remote repo.'}</v>
+      </c>
+      <c r="L411" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':410,'name':'package-feed-remote','unicode':'EA99','decimal':60057,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','remote','signal','reference','wave','virtual','box','square'],'usage':'Used in Package hub treeview to represent package feed is a reference to remote repo.'}</v>
-      </c>
-      <c r="L411" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":410,"name":"package-feed-remote","unicode":"EA99","decimal":60057,"version":"1.1","style":"light","subset":"VSTS","group":"Package","keywords":["package","feed","remote","signal","reference","wave","virtual","box","square"],"usage":"Used in Package hub treeview to represent package feed is a reference to remote repo."}</v>
       </c>
     </row>
@@ -57943,11 +58179,11 @@
         <v>Used in Package hub treeview to represent package feed is a local folder.</v>
       </c>
       <c r="K412" t="str">
+        <f>IF(NOT(ISBLANK(A412)),CONCATENATE("{'",$A$1,"':",A412,",'",$B$1,"':'",B412,"',","'",$C$1,"':'",C412,"','",$D$1,"':",D412,",'",$E$1,"':'",FIXED(E412,1),"','",$F$1,"':'",F412,"','",$G$1,"':'",G412,"','",$H$1,"':'",H412,"','",$I$1,"':['",SUBSTITUTE(I412," ","','"),"'],'",$J$1,"':'",J412,"'}"))</f>
+        <v>{'id':411,'name':'package-feed-local','unicode':'EA9A','decimal':60058,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','local','box','square'],'usage':'Used in Package hub treeview to represent package feed is a local folder.'}</v>
+      </c>
+      <c r="L412" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':411,'name':'package-feed-local','unicode':'EA9A','decimal':60058,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','local','box','square'],'usage':'Used in Package hub treeview to represent package feed is a local folder.'}</v>
-      </c>
-      <c r="L412" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":411,"name":"package-feed-local","unicode":"EA9A","decimal":60058,"version":"1.1","style":"light","subset":"VSTS","group":"Package","keywords":["package","feed","local","box","square"],"usage":"Used in Package hub treeview to represent package feed is a local folder."}</v>
       </c>
     </row>
@@ -57993,11 +58229,11 @@
         <v>Used in Work hub backlog tree view to represent work items.</v>
       </c>
       <c r="K413" t="str">
+        <f>IF(NOT(ISBLANK(A413)),CONCATENATE("{'",$A$1,"':",A413,",'",$B$1,"':'",B413,"',","'",$C$1,"':'",C413,"','",$D$1,"':",D413,",'",$E$1,"':'",FIXED(E413,1),"','",$F$1,"':'",F413,"','",$G$1,"':'",G413,"','",$H$1,"':'",H413,"','",$I$1,"':['",SUBSTITUTE(I413," ","','"),"'],'",$J$1,"':'",J413,"'}"))</f>
+        <v>{'id':412,'name':'work-item-bar-outline','unicode':'EA9B','decimal':60059,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['work','item','bar'],'usage':'Used in Work hub backlog tree view to represent work items.'}</v>
+      </c>
+      <c r="L413" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':412,'name':'work-item-bar-outline','unicode':'EA9B','decimal':60059,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['work','item','bar'],'usage':'Used in Work hub backlog tree view to represent work items.'}</v>
-      </c>
-      <c r="L413" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":412,"name":"work-item-bar-outline","unicode":"EA9B","decimal":60059,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["work","item","bar"],"usage":"Used in Work hub backlog tree view to represent work items."}</v>
       </c>
     </row>
@@ -58043,11 +58279,11 @@
         <v>Used in ListView control sorting funcionality.</v>
       </c>
       <c r="K414" t="str">
+        <f>IF(NOT(ISBLANK(A414)),CONCATENATE("{'",$A$1,"':",A414,",'",$B$1,"':'",B414,"',","'",$C$1,"':'",C414,"','",$D$1,"':",D414,",'",$E$1,"':'",FIXED(E414,1),"','",$F$1,"':'",F414,"','",$G$1,"':'",G414,"','",$H$1,"':'",H414,"','",$I$1,"':['",SUBSTITUTE(I414," ","','"),"'],'",$J$1,"':'",J414,"'}"))</f>
+        <v>{'id':413,'name':'sort-asc','unicode':'EA9C','decimal':60060,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['sort','alphabetically','ascending','arrow','down','letter'],'usage':'Used in ListView control sorting funcionality.'}</v>
+      </c>
+      <c r="L414" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':413,'name':'sort-asc','unicode':'EA9C','decimal':60060,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['sort','alphabetically','ascending','arrow','down','letter'],'usage':'Used in ListView control sorting funcionality.'}</v>
-      </c>
-      <c r="L414" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":413,"name":"sort-asc","unicode":"EA9C","decimal":60060,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["sort","alphabetically","ascending","arrow","down","letter"],"usage":"Used in ListView control sorting funcionality."}</v>
       </c>
     </row>
@@ -58093,11 +58329,11 @@
         <v>Used in ListView control sorting funcionality.</v>
       </c>
       <c r="K415" t="str">
+        <f>IF(NOT(ISBLANK(A415)),CONCATENATE("{'",$A$1,"':",A415,",'",$B$1,"':'",B415,"',","'",$C$1,"':'",C415,"','",$D$1,"':",D415,",'",$E$1,"':'",FIXED(E415,1),"','",$F$1,"':'",F415,"','",$G$1,"':'",G415,"','",$H$1,"':'",H415,"','",$I$1,"':['",SUBSTITUTE(I415," ","','"),"'],'",$J$1,"':'",J415,"'}"))</f>
+        <v>{'id':414,'name':'sort-desc','unicode':'EA9D','decimal':60061,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['sort','alphabetically','descending','arrow','down','letter'],'usage':'Used in ListView control sorting funcionality.'}</v>
+      </c>
+      <c r="L415" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':414,'name':'sort-desc','unicode':'EA9D','decimal':60061,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['sort','alphabetically','descending','arrow','down','letter'],'usage':'Used in ListView control sorting funcionality.'}</v>
-      </c>
-      <c r="L415" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":414,"name":"sort-desc","unicode":"EA9D","decimal":60061,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["sort","alphabetically","descending","arrow","down","letter"],"usage":"Used in ListView control sorting funcionality."}</v>
       </c>
     </row>
@@ -58143,11 +58379,11 @@
         <v>Indicate connection status.</v>
       </c>
       <c r="K416" t="str">
+        <f>IF(NOT(ISBLANK(A416)),CONCATENATE("{'",$A$1,"':",A416,",'",$B$1,"':'",B416,"',","'",$C$1,"':'",C416,"','",$D$1,"':",D416,",'",$E$1,"':'",FIXED(E416,1),"','",$F$1,"':'",F416,"','",$G$1,"':'",G416,"','",$H$1,"':'",H416,"','",$I$1,"':['",SUBSTITUTE(I416," ","','"),"'],'",$J$1,"':'",J416,"'}"))</f>
+        <v>{'id':415,'name':'plug-disconnected','unicode':'EA9E','decimal':60062,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['plug','disconnected','unplug','offline'],'usage':'Indicate connection status.'}</v>
+      </c>
+      <c r="L416" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':415,'name':'plug-disconnected','unicode':'EA9E','decimal':60062,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['plug','disconnected','unplug','offline'],'usage':'Indicate connection status.'}</v>
-      </c>
-      <c r="L416" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":415,"name":"plug-disconnected","unicode":"EA9E","decimal":60062,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["plug","disconnected","unplug","offline"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
@@ -58193,11 +58429,11 @@
         <v>Indicate connection status.</v>
       </c>
       <c r="K417" t="str">
+        <f>IF(NOT(ISBLANK(A417)),CONCATENATE("{'",$A$1,"':",A417,",'",$B$1,"':'",B417,"',","'",$C$1,"':'",C417,"','",$D$1,"':",D417,",'",$E$1,"':'",FIXED(E417,1),"','",$F$1,"':'",F417,"','",$G$1,"':'",G417,"','",$H$1,"':'",H417,"','",$I$1,"':['",SUBSTITUTE(I417," ","','"),"'],'",$J$1,"':'",J417,"'}"))</f>
+        <v>{'id':416,'name':'plug-connected','unicode':'EA9F','decimal':60063,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['plug','connected','plugged','online'],'usage':'Indicate connection status.'}</v>
+      </c>
+      <c r="L417" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':416,'name':'plug-connected','unicode':'EA9F','decimal':60063,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['plug','connected','plugged','online'],'usage':'Indicate connection status.'}</v>
-      </c>
-      <c r="L417" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":416,"name":"plug-connected","unicode":"EA9F","decimal":60063,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["plug","connected","plugged","online"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
@@ -58243,11 +58479,11 @@
         <v>Indicate connection status.</v>
       </c>
       <c r="K418" t="str">
+        <f>IF(NOT(ISBLANK(A418)),CONCATENATE("{'",$A$1,"':",A418,",'",$B$1,"':'",B418,"',","'",$C$1,"':'",C418,"','",$D$1,"':",D418,",'",$E$1,"':'",FIXED(E418,1),"','",$F$1,"':'",F418,"','",$G$1,"':'",G418,"','",$H$1,"':'",H418,"','",$I$1,"':['",SUBSTITUTE(I418," ","','"),"'],'",$J$1,"':'",J418,"'}"))</f>
+        <v>{'id':417,'name':'plug-disconnected-fill','unicode':'EAA0','decimal':60064,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['plug','disconnected','unplug','offline'],'usage':'Indicate connection status.'}</v>
+      </c>
+      <c r="L418" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':417,'name':'plug-disconnected-fill','unicode':'EAA0','decimal':60064,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['plug','disconnected','unplug','offline'],'usage':'Indicate connection status.'}</v>
-      </c>
-      <c r="L418" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":417,"name":"plug-disconnected-fill","unicode":"EAA0","decimal":60064,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["plug","disconnected","unplug","offline"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
@@ -58293,11 +58529,11 @@
         <v>Indicate connection status.</v>
       </c>
       <c r="K419" t="str">
+        <f>IF(NOT(ISBLANK(A419)),CONCATENATE("{'",$A$1,"':",A419,",'",$B$1,"':'",B419,"',","'",$C$1,"':'",C419,"','",$D$1,"':",D419,",'",$E$1,"':'",FIXED(E419,1),"','",$F$1,"':'",F419,"','",$G$1,"':'",G419,"','",$H$1,"':'",H419,"','",$I$1,"':['",SUBSTITUTE(I419," ","','"),"'],'",$J$1,"':'",J419,"'}"))</f>
+        <v>{'id':418,'name':'plug-connected-fill','unicode':'EAA1','decimal':60065,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['plug','connected','plugged','online'],'usage':'Indicate connection status.'}</v>
+      </c>
+      <c r="L419" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':418,'name':'plug-connected-fill','unicode':'EAA1','decimal':60065,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['plug','connected','plugged','online'],'usage':'Indicate connection status.'}</v>
-      </c>
-      <c r="L419" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":418,"name":"plug-connected-fill","unicode":"EAA1","decimal":60065,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["plug","connected","plugged","online"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
@@ -58343,11 +58579,11 @@
         <v>Used in Backlog capacity editor for adding missing team members.</v>
       </c>
       <c r="K420" t="str">
+        <f>IF(NOT(ISBLANK(A420)),CONCATENATE("{'",$A$1,"':",A420,",'",$B$1,"':'",B420,"',","'",$C$1,"':'",C420,"','",$D$1,"':",D420,",'",$E$1,"':'",FIXED(E420,1),"','",$F$1,"':'",F420,"','",$G$1,"':'",G420,"','",$H$1,"':'",H420,"','",$I$1,"':['",SUBSTITUTE(I420," ","','"),"'],'",$J$1,"':'",J420,"'}"))</f>
+        <v>{'id':419,'name':'sync-user','unicode':'EAA2','decimal':60066,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['sync','update','user'],'usage':'Used in Backlog capacity editor for adding missing team members.'}</v>
+      </c>
+      <c r="L420" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':419,'name':'sync-user','unicode':'EAA2','decimal':60066,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['sync','update','user'],'usage':'Used in Backlog capacity editor for adding missing team members.'}</v>
-      </c>
-      <c r="L420" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":419,"name":"sync-user","unicode":"EAA2","decimal":60066,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["sync","update","user"],"usage":"Used in Backlog capacity editor for adding missing team members."}</v>
       </c>
     </row>
@@ -58393,11 +58629,11 @@
         <v>Used in Code hub to clear applied filters.</v>
       </c>
       <c r="K421" t="str">
+        <f>IF(NOT(ISBLANK(A421)),CONCATENATE("{'",$A$1,"':",A421,",'",$B$1,"':'",B421,"',","'",$C$1,"':'",C421,"','",$D$1,"':",D421,",'",$E$1,"':'",FIXED(E421,1),"','",$F$1,"':'",F421,"','",$G$1,"':'",G421,"','",$H$1,"':'",H421,"','",$I$1,"':['",SUBSTITUTE(I421," ","','"),"'],'",$J$1,"':'",J421,"'}"))</f>
+        <v>{'id':420,'name':'clear-filter','unicode':'EAA3','decimal':60067,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['clear','remove','delete','cancel','filter','funnel'],'usage':'Used in Code hub to clear applied filters.'}</v>
+      </c>
+      <c r="L421" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':420,'name':'clear-filter','unicode':'EAA3','decimal':60067,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['clear','remove','delete','cancel','filter','funnel'],'usage':'Used in Code hub to clear applied filters.'}</v>
-      </c>
-      <c r="L421" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":420,"name":"clear-filter","unicode":"EAA3","decimal":60067,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["clear","remove","delete","cancel","filter","funnel"],"usage":"Used in Code hub to clear applied filters."}</v>
       </c>
     </row>
@@ -58443,11 +58679,11 @@
         <v>Used for turning off follow on an work item.</v>
       </c>
       <c r="K422" t="str">
+        <f>IF(NOT(ISBLANK(A422)),CONCATENATE("{'",$A$1,"':",A422,",'",$B$1,"':'",B422,"',","'",$C$1,"':'",C422,"','",$D$1,"':",D422,",'",$E$1,"':'",FIXED(E422,1),"','",$F$1,"':'",F422,"','",$G$1,"':'",G422,"','",$H$1,"':'",H422,"','",$I$1,"':['",SUBSTITUTE(I422," ","','"),"'],'",$J$1,"':'",J422,"'}"))</f>
+        <v>{'id':421,'name':'watch-eye-off','unicode':'EAA4','decimal':60068,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['watch','eye','follow','off','slash'],'usage':'Used for turning off follow on an work item.'}</v>
+      </c>
+      <c r="L422" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':421,'name':'watch-eye-off','unicode':'EAA4','decimal':60068,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['watch','eye','follow','off','slash'],'usage':'Used for turning off follow on an work item.'}</v>
-      </c>
-      <c r="L422" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":421,"name":"watch-eye-off","unicode":"EAA4","decimal":60068,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["watch","eye","follow","off","slash"],"usage":"Used for turning off follow on an work item."}</v>
       </c>
     </row>
@@ -58493,11 +58729,11 @@
         <v>Use this version when shopping cart needs two states: empty and filled</v>
       </c>
       <c r="K423" t="str">
+        <f>IF(NOT(ISBLANK(A423)),CONCATENATE("{'",$A$1,"':",A423,",'",$B$1,"':'",B423,"',","'",$C$1,"':'",C423,"','",$D$1,"':",D423,",'",$E$1,"':'",FIXED(E423,1),"','",$F$1,"':'",F423,"','",$G$1,"':'",G423,"','",$H$1,"':'",H423,"','",$I$1,"':['",SUBSTITUTE(I423," ","','"),"'],'",$J$1,"':'",J423,"'}"))</f>
+        <v>{'id':422,'name':'shopping-cart','unicode':'EAA5','decimal':60069,'version':'1.1','style':'light','subset':'VSCOM','group':'Common','keywords':['shop','cart','buy','purchase','store'],'usage':'Use this version when shopping cart needs two states: empty and filled'}</v>
+      </c>
+      <c r="L423" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':422,'name':'shopping-cart','unicode':'EAA5','decimal':60069,'version':'1.1','style':'light','subset':'VSCOM','group':'Common','keywords':['shop','cart','buy','purchase','store'],'usage':'Use this version when shopping cart needs two states: empty and filled'}</v>
-      </c>
-      <c r="L423" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":422,"name":"shopping-cart","unicode":"EAA5","decimal":60069,"version":"1.1","style":"light","subset":"VSCOM","group":"Common","keywords":["shop","cart","buy","purchase","store"],"usage":"Use this version when shopping cart needs two states: empty and filled"}</v>
       </c>
     </row>
@@ -58543,11 +58779,11 @@
         <v>Use this version when shopping cart needs two states: empty and filled</v>
       </c>
       <c r="K424" t="str">
+        <f>IF(NOT(ISBLANK(A424)),CONCATENATE("{'",$A$1,"':",A424,",'",$B$1,"':'",B424,"',","'",$C$1,"':'",C424,"','",$D$1,"':",D424,",'",$E$1,"':'",FIXED(E424,1),"','",$F$1,"':'",F424,"','",$G$1,"':'",G424,"','",$H$1,"':'",H424,"','",$I$1,"':['",SUBSTITUTE(I424," ","','"),"'],'",$J$1,"':'",J424,"'}"))</f>
+        <v>{'id':423,'name':'shopping-cart-fill','unicode':'EAA6','decimal':60070,'version':'1.1','style':'light','subset':'VSCOM','group':'Common','keywords':['shop','cart','buy','purchase','store'],'usage':'Use this version when shopping cart needs two states: empty and filled'}</v>
+      </c>
+      <c r="L424" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':423,'name':'shopping-cart-fill','unicode':'EAA6','decimal':60070,'version':'1.1','style':'light','subset':'VSCOM','group':'Common','keywords':['shop','cart','buy','purchase','store'],'usage':'Use this version when shopping cart needs two states: empty and filled'}</v>
-      </c>
-      <c r="L424" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":423,"name":"shopping-cart-fill","unicode":"EAA6","decimal":60070,"version":"1.1","style":"light","subset":"VSCOM","group":"Common","keywords":["shop","cart","buy","purchase","store"],"usage":"Use this version when shopping cart needs two states: empty and filled"}</v>
       </c>
     </row>
@@ -58593,11 +58829,11 @@
         <v>The common control panel.</v>
       </c>
       <c r="K425" t="str">
+        <f>IF(NOT(ISBLANK(A425)),CONCATENATE("{'",$A$1,"':",A425,",'",$B$1,"':'",B425,"',","'",$C$1,"':'",C425,"','",$D$1,"':",D425,",'",$E$1,"':'",FIXED(E425,1),"','",$F$1,"':'",F425,"','",$G$1,"':'",G425,"','",$H$1,"':'",H425,"','",$I$1,"':['",SUBSTITUTE(I425," ","','"),"'],'",$J$1,"':'",J425,"'}"))</f>
+        <v>{'id':424,'name':'control-panel','unicode':'EAA7','decimal':60071,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['control','panel','settings','configuration','slide','adjust'],'usage':'The common control panel.'}</v>
+      </c>
+      <c r="L425" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':424,'name':'control-panel','unicode':'EAA7','decimal':60071,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['control','panel','settings','configuration','slide','adjust'],'usage':'The common control panel.'}</v>
-      </c>
-      <c r="L425" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":424,"name":"control-panel","unicode":"EAA7","decimal":60071,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["control","panel","settings","configuration","slide","adjust"],"usage":"The common control panel."}</v>
       </c>
     </row>
@@ -58643,11 +58879,11 @@
         <v>Used in capacity view to add missing team member.</v>
       </c>
       <c r="K426" t="str">
+        <f>IF(NOT(ISBLANK(A426)),CONCATENATE("{'",$A$1,"':",A426,",'",$B$1,"':'",B426,"',","'",$C$1,"':'",C426,"','",$D$1,"':",D426,",'",$E$1,"':'",FIXED(E426,1),"','",$F$1,"':'",F426,"','",$G$1,"':'",G426,"','",$H$1,"':'",H426,"','",$I$1,"':['",SUBSTITUTE(I426," ","','"),"'],'",$J$1,"':'",J426,"'}"))</f>
+        <v>{'id':425,'name':'add-team','unicode':'EAA8','decimal':60072,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['add','team','user','member'],'usage':'Used in capacity view to add missing team member.'}</v>
+      </c>
+      <c r="L426" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':425,'name':'add-team','unicode':'EAA8','decimal':60072,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['add','team','user','member'],'usage':'Used in capacity view to add missing team member.'}</v>
-      </c>
-      <c r="L426" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":425,"name":"add-team","unicode":"EAA8","decimal":60072,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["add","team","user","member"],"usage":"Used in capacity view to add missing team member."}</v>
       </c>
     </row>
@@ -58693,11 +58929,11 @@
         <v>Used for unpin command. Do not use for not-pinned/pinned toggle.</v>
       </c>
       <c r="K427" t="str">
+        <f>IF(NOT(ISBLANK(A427)),CONCATENATE("{'",$A$1,"':",A427,",'",$B$1,"':'",B427,"',","'",$C$1,"':'",C427,"','",$D$1,"':",D427,",'",$E$1,"':'",FIXED(E427,1),"','",$F$1,"':'",F427,"','",$G$1,"':'",G427,"','",$H$1,"':'",H427,"','",$I$1,"':['",SUBSTITUTE(I427," ","','"),"'],'",$J$1,"':'",J427,"'}"))</f>
+        <v>{'id':426,'name':'unpin','unicode':'EAA9','decimal':60073,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['pin','unpin','remove'],'usage':'Used for unpin command. Do not use for not-pinned/pinned toggle.'}</v>
+      </c>
+      <c r="L427" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':426,'name':'unpin','unicode':'EAA9','decimal':60073,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['pin','unpin','remove'],'usage':'Used for unpin command. Do not use for not-pinned/pinned toggle.'}</v>
-      </c>
-      <c r="L427" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":426,"name":"unpin","unicode":"EAA9","decimal":60073,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["pin","unpin","remove"],"usage":"Used for unpin command. Do not use for not-pinned/pinned toggle."}</v>
       </c>
     </row>
@@ -58743,11 +58979,11 @@
         <v>Used for unpin command. Do not use for not-pinned/pinned toggle.</v>
       </c>
       <c r="K428" t="str">
+        <f>IF(NOT(ISBLANK(A428)),CONCATENATE("{'",$A$1,"':",A428,",'",$B$1,"':'",B428,"',","'",$C$1,"':'",C428,"','",$D$1,"':",D428,",'",$E$1,"':'",FIXED(E428,1),"','",$F$1,"':'",F428,"','",$G$1,"':'",G428,"','",$H$1,"':'",H428,"','",$I$1,"':['",SUBSTITUTE(I428," ","','"),"'],'",$J$1,"':'",J428,"'}"))</f>
+        <v>{'id':427,'name':'unpin-fill','unicode':'EAAA','decimal':60074,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['pin','unpin','remove'],'usage':'Used for unpin command. Do not use for not-pinned/pinned toggle.'}</v>
+      </c>
+      <c r="L428" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':427,'name':'unpin-fill','unicode':'EAAA','decimal':60074,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['pin','unpin','remove'],'usage':'Used for unpin command. Do not use for not-pinned/pinned toggle.'}</v>
-      </c>
-      <c r="L428" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":427,"name":"unpin-fill","unicode":"EAAA","decimal":60074,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["pin","unpin","remove"],"usage":"Used for unpin command. Do not use for not-pinned/pinned toggle."}</v>
       </c>
     </row>
@@ -58793,11 +59029,11 @@
         <v>Used on Backlogs tab.</v>
       </c>
       <c r="K429" t="str">
+        <f>IF(NOT(ISBLANK(A429)),CONCATENATE("{'",$A$1,"':",A429,",'",$B$1,"':'",B429,"',","'",$C$1,"':'",C429,"','",$D$1,"':",D429,",'",$E$1,"':'",FIXED(E429,1),"','",$F$1,"':'",F429,"','",$G$1,"':'",G429,"','",$H$1,"':'",H429,"','",$I$1,"':['",SUBSTITUTE(I429," ","','"),"'],'",$J$1,"':'",J429,"'}"))</f>
+        <v>{'id':428,'name':'backlog','unicode':'EAAB','decimal':60075,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['backlog','board','kanban','card'],'usage':'Used on Backlogs tab.'}</v>
+      </c>
+      <c r="L429" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':428,'name':'backlog','unicode':'EAAB','decimal':60075,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['backlog','board','kanban','card'],'usage':'Used on Backlogs tab.'}</v>
-      </c>
-      <c r="L429" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":428,"name":"backlog","unicode":"EAAB","decimal":60075,"version":"1.1","style":"bold","subset":"VSTS","group":"Work","keywords":["backlog","board","kanban","card"],"usage":"Used on Backlogs tab."}</v>
       </c>
     </row>
@@ -58843,11 +59079,11 @@
         <v>Common list view, often used together with grid view.</v>
       </c>
       <c r="K430" t="str">
+        <f>IF(NOT(ISBLANK(A430)),CONCATENATE("{'",$A$1,"':",A430,",'",$B$1,"':'",B430,"',","'",$C$1,"':'",C430,"','",$D$1,"':",D430,",'",$E$1,"':'",FIXED(E430,1),"','",$F$1,"':'",F430,"','",$G$1,"':'",G430,"','",$H$1,"':'",H430,"','",$I$1,"':['",SUBSTITUTE(I430," ","','"),"'],'",$J$1,"':'",J430,"'}"))</f>
+        <v>{'id':429,'name':'backlog-view-list','unicode':'EAAC','decimal':60076,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['view','list'],'usage':'Common list view, often used together with grid view.'}</v>
+      </c>
+      <c r="L430" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':429,'name':'backlog-view-list','unicode':'EAAC','decimal':60076,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['view','list'],'usage':'Common list view, often used together with grid view.'}</v>
-      </c>
-      <c r="L430" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":429,"name":"backlog-view-list","unicode":"EAAC","decimal":60076,"version":"1.1","style":"bold","subset":"VSTS","group":"Work","keywords":["view","list"],"usage":"Common list view, often used together with grid view."}</v>
       </c>
     </row>
@@ -58893,11 +59129,11 @@
         <v>Used on Plans tab.</v>
       </c>
       <c r="K431" t="str">
+        <f>IF(NOT(ISBLANK(A431)),CONCATENATE("{'",$A$1,"':",A431,",'",$B$1,"':'",B431,"',","'",$C$1,"':'",C431,"','",$D$1,"':",D431,",'",$E$1,"':'",FIXED(E431,1),"','",$F$1,"':'",F431,"','",$G$1,"':'",G431,"','",$H$1,"':'",H431,"','",$I$1,"':['",SUBSTITUTE(I431," ","','"),"'],'",$J$1,"':'",J431,"'}"))</f>
+        <v>{'id':430,'name':'plan','unicode':'EAAD','decimal':60077,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['plan','schedule','timeline'],'usage':'Used on Plans tab.'}</v>
+      </c>
+      <c r="L431" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':430,'name':'plan','unicode':'EAAD','decimal':60077,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['plan','schedule','timeline'],'usage':'Used on Plans tab.'}</v>
-      </c>
-      <c r="L431" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":430,"name":"plan","unicode":"EAAD","decimal":60077,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["plan","schedule","timeline"],"usage":"Used on Plans tab."}</v>
       </c>
     </row>
@@ -58943,11 +59179,11 @@
         <v>Used on Queries tab.</v>
       </c>
       <c r="K432" t="str">
+        <f>IF(NOT(ISBLANK(A432)),CONCATENATE("{'",$A$1,"':",A432,",'",$B$1,"':'",B432,"',","'",$C$1,"':'",C432,"','",$D$1,"':",D432,",'",$E$1,"':'",FIXED(E432,1),"','",$F$1,"':'",F432,"','",$G$1,"':'",G432,"','",$H$1,"':'",H432,"','",$I$1,"':['",SUBSTITUTE(I432," ","','"),"'],'",$J$1,"':'",J432,"'}"))</f>
+        <v>{'id':431,'name':'query-list','unicode':'EAAE','decimal':60078,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['query','list'],'usage':'Used on Queries tab.'}</v>
+      </c>
+      <c r="L432" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':431,'name':'query-list','unicode':'EAAE','decimal':60078,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['query','list'],'usage':'Used on Queries tab.'}</v>
-      </c>
-      <c r="L432" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":431,"name":"query-list","unicode":"EAAE","decimal":60078,"version":"1.1","style":"bold","subset":"VSTS","group":"Work","keywords":["query","list"],"usage":"Used on Queries tab."}</v>
       </c>
     </row>
@@ -58993,11 +59229,11 @@
         <v>Used to indicate matix style backlog timeline view.</v>
       </c>
       <c r="K433" t="str">
+        <f>IF(NOT(ISBLANK(A433)),CONCATENATE("{'",$A$1,"':",A433,",'",$B$1,"':'",B433,"',","'",$C$1,"':'",C433,"','",$D$1,"':",D433,",'",$E$1,"':'",FIXED(E433,1),"','",$F$1,"':'",F433,"','",$G$1,"':'",G433,"','",$H$1,"':'",H433,"','",$I$1,"':['",SUBSTITUTE(I433," ","','"),"'],'",$J$1,"':'",J433,"'}"))</f>
+        <v>{'id':432,'name':'timeline-matrix','unicode':'EAAF','decimal':60079,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['timeline','delivery','schedule','matrix'],'usage':'Used to indicate matix style backlog timeline view.'}</v>
+      </c>
+      <c r="L433" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':432,'name':'timeline-matrix','unicode':'EAAF','decimal':60079,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['timeline','delivery','schedule','matrix'],'usage':'Used to indicate matix style backlog timeline view.'}</v>
-      </c>
-      <c r="L433" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":432,"name":"timeline-matrix","unicode":"EAAF","decimal":60079,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["timeline","delivery","schedule","matrix"],"usage":"Used to indicate matix style backlog timeline view."}</v>
       </c>
     </row>
@@ -59043,11 +59279,11 @@
         <v>Used in Work hub Query page for team favorite queries.</v>
       </c>
       <c r="K434" t="str">
+        <f>IF(NOT(ISBLANK(A434)),CONCATENATE("{'",$A$1,"':",A434,",'",$B$1,"':'",B434,"',","'",$C$1,"':'",C434,"','",$D$1,"':",D434,",'",$E$1,"':'",FIXED(E434,1),"','",$F$1,"':'",F434,"','",$G$1,"':'",G434,"','",$H$1,"':'",H434,"','",$I$1,"':['",SUBSTITUTE(I434," ","','"),"'],'",$J$1,"':'",J434,"'}"))</f>
+        <v>{'id':433,'name':'team-favorite','unicode':'EAB0','decimal':60080,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['team','favorite','user','people','star'],'usage':'Used in Work hub Query page for team favorite queries.'}</v>
+      </c>
+      <c r="L434" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':433,'name':'team-favorite','unicode':'EAB0','decimal':60080,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['team','favorite','user','people','star'],'usage':'Used in Work hub Query page for team favorite queries.'}</v>
-      </c>
-      <c r="L434" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":433,"name":"team-favorite","unicode":"EAB0","decimal":60080,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["team","favorite","user","people","star"],"usage":"Used in Work hub Query page for team favorite queries."}</v>
       </c>
     </row>
@@ -59093,11 +59329,11 @@
         <v>Test impact.</v>
       </c>
       <c r="K435" t="str">
+        <f>IF(NOT(ISBLANK(A435)),CONCATENATE("{'",$A$1,"':",A435,",'",$B$1,"':'",B435,"',","'",$C$1,"':'",C435,"','",$D$1,"':",D435,",'",$E$1,"':'",FIXED(E435,1),"','",$F$1,"':'",F435,"','",$G$1,"':'",G435,"','",$H$1,"':'",H435,"','",$I$1,"':['",SUBSTITUTE(I435," ","','"),"'],'",$J$1,"':'",J435,"'}"))</f>
+        <v>{'id':434,'name':'test-impact-fill','unicode':'EAB1','decimal':60081,'version':'1.1','style':'bold','subset':'VSTS','group':'Test','keywords':['test','impact','beaker','flask','hammer'],'usage':'Test impact.'}</v>
+      </c>
+      <c r="L435" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':434,'name':'test-impact-fill','unicode':'EAB1','decimal':60081,'version':'1.1','style':'bold','subset':'VSTS','group':'Test','keywords':['test','impact','beaker','flask','hammer'],'usage':'Test impact.'}</v>
-      </c>
-      <c r="L435" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":434,"name":"test-impact-fill","unicode":"EAB1","decimal":60081,"version":"1.1","style":"bold","subset":"VSTS","group":"Test","keywords":["test","impact","beaker","flask","hammer"],"usage":"Test impact."}</v>
       </c>
     </row>
@@ -59106,8 +59342,9 @@
         <f>'Bowtie v1.0 reorg'!A437</f>
         <v>435</v>
       </c>
-      <c r="B436" t="s">
-        <v>858</v>
+      <c r="B436" t="str">
+        <f>'Bowtie v1.0 reorg'!E437</f>
+        <v>task-group</v>
       </c>
       <c r="C436" t="str">
         <f>'Bowtie v1.0 reorg'!C437</f>
@@ -59136,11 +59373,11 @@
         <v>860</v>
       </c>
       <c r="K436" t="str">
+        <f>IF(NOT(ISBLANK(A436)),CONCATENATE("{'",$A$1,"':",A436,",'",$B$1,"':'",B436,"',","'",$C$1,"':'",C436,"','",$D$1,"':",D436,",'",$E$1,"':'",FIXED(E436,1),"','",$F$1,"':'",F436,"','",$G$1,"':'",G436,"','",$H$1,"':'",H436,"','",$I$1,"':['",SUBSTITUTE(I436," ","','"),"'],'",$J$1,"':'",J436,"'}"))</f>
+        <v>{'id':435,'name':'task-group','unicode':'EAB2','decimal':60082,'version':'1.1','style':'light','subset':'VSTS','group':'Build','keywords':['task','group','list'],'usage':'Used in Release hub for task group.'}</v>
+      </c>
+      <c r="L436" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':435,'name':'task-group','unicode':'EAB2','decimal':60082,'version':'1.1','style':'light','subset':'VSTS','group':'Build','keywords':['task','group','list'],'usage':'Used in Release hub for task group.'}</v>
-      </c>
-      <c r="L436" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":435,"name":"task-group","unicode":"EAB2","decimal":60082,"version":"1.1","style":"light","subset":"VSTS","group":"Build","keywords":["task","group","list"],"usage":"Used in Release hub for task group."}</v>
       </c>
     </row>
@@ -59186,11 +59423,11 @@
         <v>Used in Compliance hub for Engineering Group node dropdown.</v>
       </c>
       <c r="K437" t="str">
+        <f>IF(NOT(ISBLANK(A437)),CONCATENATE("{'",$A$1,"':",A437,",'",$B$1,"':'",B437,"',","'",$C$1,"':'",C437,"','",$D$1,"':",D437,",'",$E$1,"':'",FIXED(E437,1),"','",$F$1,"':'",F437,"','",$G$1,"':'",G437,"','",$H$1,"':'",H437,"','",$I$1,"':['",SUBSTITUTE(I437," ","','"),"'],'",$J$1,"':'",J437,"'}"))</f>
+        <v>{'id':436,'name':'engineering-group','unicode':'EAB3','decimal':60083,'version':'1.1','style':'bold','subset':'VSTS','group':'Compliance','keywords':['engineering','group','loop','organization','chart','schema'],'usage':'Used in Compliance hub for Engineering Group node dropdown.'}</v>
+      </c>
+      <c r="L437" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':436,'name':'engineering-group','unicode':'EAB3','decimal':60083,'version':'1.1','style':'bold','subset':'VSTS','group':'Compliance','keywords':['engineering','group','loop','organization','chart','schema'],'usage':'Used in Compliance hub for Engineering Group node dropdown.'}</v>
-      </c>
-      <c r="L437" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":436,"name":"engineering-group","unicode":"EAB3","decimal":60083,"version":"1.1","style":"bold","subset":"VSTS","group":"Compliance","keywords":["engineering","group","loop","organization","chart","schema"],"usage":"Used in Compliance hub for Engineering Group node dropdown."}</v>
       </c>
     </row>
@@ -59236,11 +59473,11 @@
         <v>Used for team project.</v>
       </c>
       <c r="K438" t="str">
+        <f>IF(NOT(ISBLANK(A438)),CONCATENATE("{'",$A$1,"':",A438,",'",$B$1,"':'",B438,"',","'",$C$1,"':'",C438,"','",$D$1,"':",D438,",'",$E$1,"':'",FIXED(E438,1),"','",$F$1,"':'",F438,"','",$G$1,"':'",G438,"','",$H$1,"':'",H438,"','",$I$1,"':['",SUBSTITUTE(I438," ","','"),"'],'",$J$1,"':'",J438,"'}"))</f>
+        <v>{'id':437,'name':'briefcase','unicode':'EAB4','decimal':60084,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['briefcase','project','container'],'usage':'Used for team project.'}</v>
+      </c>
+      <c r="L438" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':437,'name':'briefcase','unicode':'EAB4','decimal':60084,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['briefcase','project','container'],'usage':'Used for team project.'}</v>
-      </c>
-      <c r="L438" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":437,"name":"briefcase","unicode":"EAB4","decimal":60084,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["briefcase","project","container"],"usage":"Used for team project."}</v>
       </c>
     </row>
@@ -59286,11 +59523,11 @@
         <v>Variable group is a group of configuration variables which can be used in deployments across build and release.</v>
       </c>
       <c r="K439" t="str">
+        <f>IF(NOT(ISBLANK(A439)),CONCATENATE("{'",$A$1,"':",A439,",'",$B$1,"':'",B439,"',","'",$C$1,"':'",C439,"','",$D$1,"':",D439,",'",$E$1,"':'",FIXED(E439,1),"','",$F$1,"':'",F439,"','",$G$1,"':'",G439,"','",$H$1,"':'",H439,"','",$I$1,"':['",SUBSTITUTE(I439," ","','"),"'],'",$J$1,"':'",J439,"'}"))</f>
+        <v>{'id':438,'name':'variable-group','unicode':'EAB5','decimal':60085,'version':'1.1','style':'light','subset':'VSTS','group':'Test','keywords':['variable','group','parameter','x','letter','brackets'],'usage':'Variable group is a group of configuration variables which can be used in deployments across build and release.'}</v>
+      </c>
+      <c r="L439" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':438,'name':'variable-group','unicode':'EAB5','decimal':60085,'version':'1.1','style':'light','subset':'VSTS','group':'Test','keywords':['variable','group','parameter','x','letter','brackets'],'usage':'Variable group is a group of configuration variables which can be used in deployments across build and release.'}</v>
-      </c>
-      <c r="L439" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":438,"name":"variable-group","unicode":"EAB5","decimal":60085,"version":"1.1","style":"light","subset":"VSTS","group":"Test","keywords":["variable","group","parameter","x","letter","brackets"],"usage":"Variable group is a group of configuration variables which can be used in deployments across build and release."}</v>
       </c>
     </row>
@@ -59336,11 +59573,11 @@
         <v>To show full history of a file.</v>
       </c>
       <c r="K440" t="str">
+        <f>IF(NOT(ISBLANK(A440)),CONCATENATE("{'",$A$1,"':",A440,",'",$B$1,"':'",B440,"',","'",$C$1,"':'",C440,"','",$D$1,"':",D440,",'",$E$1,"':'",FIXED(E440,1),"','",$F$1,"':'",F440,"','",$G$1,"':'",G440,"','",$H$1,"':'",H440,"','",$I$1,"':['",SUBSTITUTE(I440," ","','"),"'],'",$J$1,"':'",J440,"'}"))</f>
+        <v>{'id':439,'name':'full-history','unicode':'EAB6','decimal':60086,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['history','list','full','all','clock','arrow','time'],'usage':'To show full history of a file.'}</v>
+      </c>
+      <c r="L440" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':439,'name':'full-history','unicode':'EAB6','decimal':60086,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['history','list','full','all','clock','arrow','time'],'usage':'To show full history of a file.'}</v>
-      </c>
-      <c r="L440" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":439,"name":"full-history","unicode":"EAB6","decimal":60086,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["history","list","full","all","clock","arrow","time"],"usage":"To show full history of a file."}</v>
       </c>
     </row>
@@ -59386,11 +59623,11 @@
         <v>Used in Compliance hub for Baseline parent node in treeview.</v>
       </c>
       <c r="K441" t="str">
+        <f>IF(NOT(ISBLANK(A441)),CONCATENATE("{'",$A$1,"':",A441,",'",$B$1,"':'",B441,"',","'",$C$1,"':'",C441,"','",$D$1,"':",D441,",'",$E$1,"':'",FIXED(E441,1),"','",$F$1,"':'",F441,"','",$G$1,"':'",G441,"','",$H$1,"':'",H441,"','",$I$1,"':['",SUBSTITUTE(I441," ","','"),"'],'",$J$1,"':'",J441,"'}"))</f>
+        <v>{'id':440,'name':'scope-template','unicode':'EAB7','decimal':60087,'version':'1.1','style':'light','subset':'VSTS','group':'Compliance','keywords':['scope','template','baseline','compliance','document'],'usage':'Used in Compliance hub for Baseline parent node in treeview.'}</v>
+      </c>
+      <c r="L441" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':440,'name':'scope-template','unicode':'EAB7','decimal':60087,'version':'1.1','style':'light','subset':'VSTS','group':'Compliance','keywords':['scope','template','baseline','compliance','document'],'usage':'Used in Compliance hub for Baseline parent node in treeview.'}</v>
-      </c>
-      <c r="L441" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":440,"name":"scope-template","unicode":"EAB7","decimal":60087,"version":"1.1","style":"light","subset":"VSTS","group":"Compliance","keywords":["scope","template","baseline","compliance","document"],"usage":"Used in Compliance hub for Baseline parent node in treeview."}</v>
       </c>
     </row>
@@ -59436,11 +59673,11 @@
         <v>Used in Compliance hub for Baseline child node in treeview.</v>
       </c>
       <c r="K442" t="str">
+        <f>IF(NOT(ISBLANK(A442)),CONCATENATE("{'",$A$1,"':",A442,",'",$B$1,"':'",B442,"',","'",$C$1,"':'",C442,"','",$D$1,"':",D442,",'",$E$1,"':'",FIXED(E442,1),"','",$F$1,"':'",F442,"','",$G$1,"':'",G442,"','",$H$1,"':'",H442,"','",$I$1,"':['",SUBSTITUTE(I442," ","','"),"'],'",$J$1,"':'",J442,"'}"))</f>
+        <v>{'id':441,'name':'assessment-group-template','unicode':'EAB8','decimal':60088,'version':'1.1','style':'light','subset':'VSTS','group':'Compliance','keywords':['assessment','group','compliance','template','document'],'usage':'Used in Compliance hub for Baseline child node in treeview.'}</v>
+      </c>
+      <c r="L442" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':441,'name':'assessment-group-template','unicode':'EAB8','decimal':60088,'version':'1.1','style':'light','subset':'VSTS','group':'Compliance','keywords':['assessment','group','compliance','template','document'],'usage':'Used in Compliance hub for Baseline child node in treeview.'}</v>
-      </c>
-      <c r="L442" t="str">
-        <f t="shared" si="15"/>
         <v>{"id":441,"name":"assessment-group-template","unicode":"EAB8","decimal":60088,"version":"1.1","style":"light","subset":"VSTS","group":"Compliance","keywords":["assessment","group","compliance","template","document"],"usage":"Used in Compliance hub for Baseline child node in treeview."}</v>
       </c>
     </row>
@@ -59449,9 +59686,9 @@
         <f>'Bowtie v1.0 reorg'!A444</f>
         <v>442</v>
       </c>
-      <c r="B443">
+      <c r="B443" t="str">
         <f>'Bowtie v1.0 reorg'!E444</f>
-        <v>0</v>
+        <v>status-success-sm</v>
       </c>
       <c r="C443" t="str">
         <f>'Bowtie v1.0 reorg'!C444</f>
@@ -59461,13 +59698,13 @@
         <f>'Bowtie v1.0 reorg'!D444</f>
         <v>60089</v>
       </c>
-      <c r="E443" t="str">
+      <c r="E443">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F444),"",'Bowtie v1.0 reorg'!F444)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F443" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G444),"",'Bowtie v1.0 reorg'!G444)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G443" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I444),"",'Bowtie v1.0 reorg'!I444)</f>
@@ -59483,15 +59720,15 @@
       </c>
       <c r="J443" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K444),"",'Bowtie v1.0 reorg'!K444)</f>
-        <v/>
-      </c>
-      <c r="K443" t="e">
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K443" t="str">
+        <f>IF(NOT(ISBLANK(A443)),CONCATENATE("{'",$A$1,"':",A443,",'",$B$1,"':'",'Bowtie v1.0 reorg'!E444,"',","'",$C$1,"':'",C443,"','",$D$1,"':",D443,",'",$E$1,"':'",FIXED(E443,1),"','",$F$1,"':'",F443,"','",$G$1,"':'",G443,"','",$H$1,"':'",H443,"','",$I$1,"':['",SUBSTITUTE(I443," ","','"),"'],'",$J$1,"':'",J443,"'}"))</f>
+        <v>{'id':442,'name':'status-success-sm','unicode':'EAB9','decimal':60089,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L443" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L443" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":442,"name":"status-success-sm","unicode":"EAB9","decimal":60089,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="444" spans="1:12" x14ac:dyDescent="0.25">
@@ -59499,9 +59736,9 @@
         <f>'Bowtie v1.0 reorg'!A445</f>
         <v>443</v>
       </c>
-      <c r="B444">
+      <c r="B444" t="str">
         <f>'Bowtie v1.0 reorg'!E445</f>
-        <v>0</v>
+        <v>status-warning-sm</v>
       </c>
       <c r="C444" t="str">
         <f>'Bowtie v1.0 reorg'!C445</f>
@@ -59511,13 +59748,13 @@
         <f>'Bowtie v1.0 reorg'!D445</f>
         <v>60090</v>
       </c>
-      <c r="E444" t="str">
+      <c r="E444">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F445),"",'Bowtie v1.0 reorg'!F445)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F444" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G445),"",'Bowtie v1.0 reorg'!G445)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G444" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I445),"",'Bowtie v1.0 reorg'!I445)</f>
@@ -59533,15 +59770,15 @@
       </c>
       <c r="J444" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K445),"",'Bowtie v1.0 reorg'!K445)</f>
-        <v/>
-      </c>
-      <c r="K444" t="e">
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K444" t="str">
+        <f>IF(NOT(ISBLANK(A444)),CONCATENATE("{'",$A$1,"':",A444,",'",$B$1,"':'",'Bowtie v1.0 reorg'!E445,"',","'",$C$1,"':'",C444,"','",$D$1,"':",D444,",'",$E$1,"':'",FIXED(E444,1),"','",$F$1,"':'",F444,"','",$G$1,"':'",G444,"','",$H$1,"':'",H444,"','",$I$1,"':['",SUBSTITUTE(I444," ","','"),"'],'",$J$1,"':'",J444,"'}"))</f>
+        <v>{'id':443,'name':'status-warning-sm','unicode':'EABA','decimal':60090,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L444" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L444" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":443,"name":"status-warning-sm","unicode":"EABA","decimal":60090,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="445" spans="1:12" x14ac:dyDescent="0.25">
@@ -59549,9 +59786,9 @@
         <f>'Bowtie v1.0 reorg'!A446</f>
         <v>444</v>
       </c>
-      <c r="B445">
+      <c r="B445" t="str">
         <f>'Bowtie v1.0 reorg'!E446</f>
-        <v>0</v>
+        <v>status-info-sm</v>
       </c>
       <c r="C445" t="str">
         <f>'Bowtie v1.0 reorg'!C446</f>
@@ -59561,13 +59798,13 @@
         <f>'Bowtie v1.0 reorg'!D446</f>
         <v>60091</v>
       </c>
-      <c r="E445" t="str">
+      <c r="E445">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F446),"",'Bowtie v1.0 reorg'!F446)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F445" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G446),"",'Bowtie v1.0 reorg'!G446)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G445" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I446),"",'Bowtie v1.0 reorg'!I446)</f>
@@ -59583,15 +59820,15 @@
       </c>
       <c r="J445" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K446),"",'Bowtie v1.0 reorg'!K446)</f>
-        <v/>
-      </c>
-      <c r="K445" t="e">
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K445" t="str">
+        <f>IF(NOT(ISBLANK(A445)),CONCATENATE("{'",$A$1,"':",A445,",'",$B$1,"':'",'Bowtie v1.0 reorg'!E446,"',","'",$C$1,"':'",C445,"','",$D$1,"':",D445,",'",$E$1,"':'",FIXED(E445,1),"','",$F$1,"':'",F445,"','",$G$1,"':'",G445,"','",$H$1,"':'",H445,"','",$I$1,"':['",SUBSTITUTE(I445," ","','"),"'],'",$J$1,"':'",J445,"'}"))</f>
+        <v>{'id':444,'name':'status-info-sm','unicode':'EABB','decimal':60091,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L445" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L445" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":444,"name":"status-info-sm","unicode":"EABB","decimal":60091,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.25">
@@ -59599,9 +59836,9 @@
         <f>'Bowtie v1.0 reorg'!A447</f>
         <v>445</v>
       </c>
-      <c r="B446">
+      <c r="B446" t="str">
         <f>'Bowtie v1.0 reorg'!E447</f>
-        <v>0</v>
+        <v>status-failure-sm</v>
       </c>
       <c r="C446" t="str">
         <f>'Bowtie v1.0 reorg'!C447</f>
@@ -59611,13 +59848,13 @@
         <f>'Bowtie v1.0 reorg'!D447</f>
         <v>60092</v>
       </c>
-      <c r="E446" t="str">
+      <c r="E446">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F447),"",'Bowtie v1.0 reorg'!F447)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F446" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G447),"",'Bowtie v1.0 reorg'!G447)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G446" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I447),"",'Bowtie v1.0 reorg'!I447)</f>
@@ -59633,15 +59870,15 @@
       </c>
       <c r="J446" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K447),"",'Bowtie v1.0 reorg'!K447)</f>
-        <v/>
-      </c>
-      <c r="K446" t="e">
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K446" t="str">
+        <f>IF(NOT(ISBLANK(A446)),CONCATENATE("{'",$A$1,"':",A446,",'",$B$1,"':'",'Bowtie v1.0 reorg'!E447,"',","'",$C$1,"':'",C446,"','",$D$1,"':",D446,",'",$E$1,"':'",FIXED(E446,1),"','",$F$1,"':'",F446,"','",$G$1,"':'",G446,"','",$H$1,"':'",H446,"','",$I$1,"':['",SUBSTITUTE(I446," ","','"),"'],'",$J$1,"':'",J446,"'}"))</f>
+        <v>{'id':445,'name':'status-failure-sm','unicode':'EABC','decimal':60092,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L446" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L446" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":445,"name":"status-failure-sm","unicode":"EABC","decimal":60092,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="447" spans="1:12" x14ac:dyDescent="0.25">
@@ -59649,9 +59886,9 @@
         <f>'Bowtie v1.0 reorg'!A448</f>
         <v>446</v>
       </c>
-      <c r="B447">
+      <c r="B447" t="str">
         <f>'Bowtie v1.0 reorg'!E448</f>
-        <v>0</v>
+        <v>status-error-sm</v>
       </c>
       <c r="C447" t="str">
         <f>'Bowtie v1.0 reorg'!C448</f>
@@ -59661,13 +59898,13 @@
         <f>'Bowtie v1.0 reorg'!D448</f>
         <v>60093</v>
       </c>
-      <c r="E447" t="str">
+      <c r="E447">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F448),"",'Bowtie v1.0 reorg'!F448)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F447" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G448),"",'Bowtie v1.0 reorg'!G448)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G447" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I448),"",'Bowtie v1.0 reorg'!I448)</f>
@@ -59683,15 +59920,15 @@
       </c>
       <c r="J447" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K448),"",'Bowtie v1.0 reorg'!K448)</f>
-        <v/>
-      </c>
-      <c r="K447" t="e">
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K447" t="str">
+        <f>IF(NOT(ISBLANK(A447)),CONCATENATE("{'",$A$1,"':",A447,",'",$B$1,"':'",'Bowtie v1.0 reorg'!E448,"',","'",$C$1,"':'",C447,"','",$D$1,"':",D447,",'",$E$1,"':'",FIXED(E447,1),"','",$F$1,"':'",F447,"','",$G$1,"':'",G447,"','",$H$1,"':'",H447,"','",$I$1,"':['",SUBSTITUTE(I447," ","','"),"'],'",$J$1,"':'",J447,"'}"))</f>
+        <v>{'id':446,'name':'status-error-sm','unicode':'EABD','decimal':60093,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L447" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L447" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":446,"name":"status-error-sm","unicode":"EABD","decimal":60093,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="448" spans="1:12" x14ac:dyDescent="0.25">
@@ -59699,9 +59936,9 @@
         <f>'Bowtie v1.0 reorg'!A449</f>
         <v>447</v>
       </c>
-      <c r="B448">
+      <c r="B448" t="str">
         <f>'Bowtie v1.0 reorg'!E449</f>
-        <v>0</v>
+        <v>status-run-sm</v>
       </c>
       <c r="C448" t="str">
         <f>'Bowtie v1.0 reorg'!C449</f>
@@ -59711,13 +59948,13 @@
         <f>'Bowtie v1.0 reorg'!D449</f>
         <v>60094</v>
       </c>
-      <c r="E448" t="str">
+      <c r="E448">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F449),"",'Bowtie v1.0 reorg'!F449)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F448" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G449),"",'Bowtie v1.0 reorg'!G449)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G448" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I449),"",'Bowtie v1.0 reorg'!I449)</f>
@@ -59733,15 +59970,15 @@
       </c>
       <c r="J448" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K449),"",'Bowtie v1.0 reorg'!K449)</f>
-        <v/>
-      </c>
-      <c r="K448" t="e">
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K448" t="str">
+        <f>IF(NOT(ISBLANK(A448)),CONCATENATE("{'",$A$1,"':",A448,",'",$B$1,"':'",'Bowtie v1.0 reorg'!E449,"',","'",$C$1,"':'",C448,"','",$D$1,"':",D448,",'",$E$1,"':'",FIXED(E448,1),"','",$F$1,"':'",F448,"','",$G$1,"':'",G448,"','",$H$1,"':'",H448,"','",$I$1,"':['",SUBSTITUTE(I448," ","','"),"'],'",$J$1,"':'",J448,"'}"))</f>
+        <v>{'id':447,'name':'status-run-sm','unicode':'EABE','decimal':60094,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L448" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L448" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":447,"name":"status-run-sm","unicode":"EABE","decimal":60094,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="449" spans="1:12" x14ac:dyDescent="0.25">
@@ -59749,9 +59986,9 @@
         <f>'Bowtie v1.0 reorg'!A450</f>
         <v>448</v>
       </c>
-      <c r="B449">
+      <c r="B449" t="str">
         <f>'Bowtie v1.0 reorg'!E450</f>
-        <v>0</v>
+        <v>status-help-sm</v>
       </c>
       <c r="C449" t="str">
         <f>'Bowtie v1.0 reorg'!C450</f>
@@ -59761,13 +59998,13 @@
         <f>'Bowtie v1.0 reorg'!D450</f>
         <v>60095</v>
       </c>
-      <c r="E449" t="str">
+      <c r="E449">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F450),"",'Bowtie v1.0 reorg'!F450)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F449" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G450),"",'Bowtie v1.0 reorg'!G450)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G449" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I450),"",'Bowtie v1.0 reorg'!I450)</f>
@@ -59783,15 +60020,15 @@
       </c>
       <c r="J449" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K450),"",'Bowtie v1.0 reorg'!K450)</f>
-        <v/>
-      </c>
-      <c r="K449" t="e">
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K449" t="str">
+        <f>IF(NOT(ISBLANK(A449)),CONCATENATE("{'",$A$1,"':",A449,",'",$B$1,"':'",'Bowtie v1.0 reorg'!E450,"',","'",$C$1,"':'",C449,"','",$D$1,"':",D449,",'",$E$1,"':'",FIXED(E449,1),"','",$F$1,"':'",F449,"','",$G$1,"':'",G449,"','",$H$1,"':'",H449,"','",$I$1,"':['",SUBSTITUTE(I449," ","','"),"'],'",$J$1,"':'",J449,"'}"))</f>
+        <v>{'id':448,'name':'status-help-sm','unicode':'EABF','decimal':60095,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L449" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L449" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":448,"name":"status-help-sm","unicode":"EABF","decimal":60095,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="450" spans="1:12" x14ac:dyDescent="0.25">
@@ -59799,9 +60036,9 @@
         <f>'Bowtie v1.0 reorg'!A451</f>
         <v>449</v>
       </c>
-      <c r="B450">
+      <c r="B450" t="str">
         <f>'Bowtie v1.0 reorg'!E451</f>
-        <v>0</v>
+        <v>status-stop-sm</v>
       </c>
       <c r="C450" t="str">
         <f>'Bowtie v1.0 reorg'!C451</f>
@@ -59811,13 +60048,13 @@
         <f>'Bowtie v1.0 reorg'!D451</f>
         <v>60096</v>
       </c>
-      <c r="E450" t="str">
+      <c r="E450">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F451),"",'Bowtie v1.0 reorg'!F451)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F450" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G451),"",'Bowtie v1.0 reorg'!G451)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G450" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I451),"",'Bowtie v1.0 reorg'!I451)</f>
@@ -59833,15 +60070,15 @@
       </c>
       <c r="J450" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K451),"",'Bowtie v1.0 reorg'!K451)</f>
-        <v/>
-      </c>
-      <c r="K450" t="e">
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K450" t="str">
+        <f>IF(NOT(ISBLANK(A450)),CONCATENATE("{'",$A$1,"':",A450,",'",$B$1,"':'",'Bowtie v1.0 reorg'!E451,"',","'",$C$1,"':'",C450,"','",$D$1,"':",D450,",'",$E$1,"':'",FIXED(E450,1),"','",$F$1,"':'",F450,"','",$G$1,"':'",G450,"','",$H$1,"':'",H450,"','",$I$1,"':['",SUBSTITUTE(I450," ","','"),"'],'",$J$1,"':'",J450,"'}"))</f>
+        <v>{'id':449,'name':'status-stop-sm','unicode':'EAC0','decimal':60096,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L450" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L450" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":449,"name":"status-stop-sm","unicode":"EAC0","decimal":60096,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="451" spans="1:12" x14ac:dyDescent="0.25">
@@ -59849,9 +60086,9 @@
         <f>'Bowtie v1.0 reorg'!A452</f>
         <v>450</v>
       </c>
-      <c r="B451">
+      <c r="B451" t="str">
         <f>'Bowtie v1.0 reorg'!E452</f>
-        <v>0</v>
+        <v>status-pause-sm</v>
       </c>
       <c r="C451" t="str">
         <f>'Bowtie v1.0 reorg'!C452</f>
@@ -59861,13 +60098,13 @@
         <f>'Bowtie v1.0 reorg'!D452</f>
         <v>60097</v>
       </c>
-      <c r="E451" t="str">
+      <c r="E451">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F452),"",'Bowtie v1.0 reorg'!F452)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F451" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G452),"",'Bowtie v1.0 reorg'!G452)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G451" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I452),"",'Bowtie v1.0 reorg'!I452)</f>
@@ -59883,15 +60120,15 @@
       </c>
       <c r="J451" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K452),"",'Bowtie v1.0 reorg'!K452)</f>
-        <v/>
-      </c>
-      <c r="K451" t="e">
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K451" t="str">
+        <f>IF(NOT(ISBLANK(A451)),CONCATENATE("{'",$A$1,"':",A451,",'",$B$1,"':'",'Bowtie v1.0 reorg'!E452,"',","'",$C$1,"':'",C451,"','",$D$1,"':",D451,",'",$E$1,"':'",FIXED(E451,1),"','",$F$1,"':'",F451,"','",$G$1,"':'",G451,"','",$H$1,"':'",H451,"','",$I$1,"':['",SUBSTITUTE(I451," ","','"),"'],'",$J$1,"':'",J451,"'}"))</f>
+        <v>{'id':450,'name':'status-pause-sm','unicode':'EAC1','decimal':60097,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L451" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L451" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":450,"name":"status-pause-sm","unicode":"EAC1","decimal":60097,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="452" spans="1:12" x14ac:dyDescent="0.25">
@@ -59899,9 +60136,9 @@
         <f>'Bowtie v1.0 reorg'!A453</f>
         <v>451</v>
       </c>
-      <c r="B452">
+      <c r="B452" t="str">
         <f>'Bowtie v1.0 reorg'!E453</f>
-        <v>0</v>
+        <v>status-waiting-fill-sm</v>
       </c>
       <c r="C452" t="str">
         <f>'Bowtie v1.0 reorg'!C453</f>
@@ -59911,13 +60148,13 @@
         <f>'Bowtie v1.0 reorg'!D453</f>
         <v>60098</v>
       </c>
-      <c r="E452" t="str">
+      <c r="E452">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F453),"",'Bowtie v1.0 reorg'!F453)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F452" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G453),"",'Bowtie v1.0 reorg'!G453)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G452" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I453),"",'Bowtie v1.0 reorg'!I453)</f>
@@ -59933,15 +60170,15 @@
       </c>
       <c r="J452" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K453),"",'Bowtie v1.0 reorg'!K453)</f>
-        <v/>
-      </c>
-      <c r="K452" t="e">
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K452" t="str">
+        <f>IF(NOT(ISBLANK(A452)),CONCATENATE("{'",$A$1,"':",A452,",'",$B$1,"':'",'Bowtie v1.0 reorg'!E453,"',","'",$C$1,"':'",C452,"','",$D$1,"':",D452,",'",$E$1,"':'",FIXED(E452,1),"','",$F$1,"':'",F452,"','",$G$1,"':'",G452,"','",$H$1,"':'",H452,"','",$I$1,"':['",SUBSTITUTE(I452," ","','"),"'],'",$J$1,"':'",J452,"'}"))</f>
+        <v>{'id':451,'name':'status-waiting-fill-sm','unicode':'EAC2','decimal':60098,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L452" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L452" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+        <v>{"id":451,"name":"status-waiting-fill-sm","unicode":"EAC2","decimal":60098,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="453" spans="1:12" x14ac:dyDescent="0.25">
@@ -59949,9 +60186,9 @@
         <f>'Bowtie v1.0 reorg'!A454</f>
         <v>452</v>
       </c>
-      <c r="B453">
+      <c r="B453" t="str">
         <f>'Bowtie v1.0 reorg'!E454</f>
-        <v>0</v>
+        <v>status-no-fill-sm</v>
       </c>
       <c r="C453" t="str">
         <f>'Bowtie v1.0 reorg'!C454</f>
@@ -59961,13 +60198,13 @@
         <f>'Bowtie v1.0 reorg'!D454</f>
         <v>60099</v>
       </c>
-      <c r="E453" t="str">
+      <c r="E453">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F454),"",'Bowtie v1.0 reorg'!F454)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F453" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G454),"",'Bowtie v1.0 reorg'!G454)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G453" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I454),"",'Bowtie v1.0 reorg'!I454)</f>
@@ -59983,15 +60220,15 @@
       </c>
       <c r="J453" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K454),"",'Bowtie v1.0 reorg'!K454)</f>
-        <v/>
-      </c>
-      <c r="K453" t="e">
-        <f t="shared" ref="K453:K470" si="18">IF(NOT(ISBLANK(A453)),CONCATENATE("{'",$A$1,"':",A453,",'",$B$1,"':'",B453,"',","'",$C$1,"':'",C453,"','",$D$1,"':",D453,",'",$E$1,"':'",FIXED(E453,1),"','",$F$1,"':'",F453,"','",$G$1,"':'",G453,"','",$H$1,"':'",H453,"','",$I$1,"':['",SUBSTITUTE(I453," ","','"),"'],'",$J$1,"':'",J453,"'}"))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L453" t="e">
-        <f t="shared" ref="L453:L466" si="19">SUBSTITUTE(K453,"'","""")</f>
-        <v>#VALUE!</v>
+        <v>Temporary solution for badging.</v>
+      </c>
+      <c r="K453" t="str">
+        <f t="shared" ref="K453:K470" si="17">IF(NOT(ISBLANK(A453)),CONCATENATE("{'",$A$1,"':",A453,",'",$B$1,"':'",B453,"',","'",$C$1,"':'",C453,"','",$D$1,"':",D453,",'",$E$1,"':'",FIXED(E453,1),"','",$F$1,"':'",F453,"','",$G$1,"':'",G453,"','",$H$1,"':'",H453,"','",$I$1,"':['",SUBSTITUTE(I453," ","','"),"'],'",$J$1,"':'",J453,"'}"))</f>
+        <v>{'id':452,'name':'status-no-fill-sm','unicode':'EAC3','decimal':60099,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
+      </c>
+      <c r="L453" t="str">
+        <f t="shared" ref="L453:L466" si="18">SUBSTITUTE(K453,"'","""")</f>
+        <v>{"id":452,"name":"status-no-fill-sm","unicode":"EAC3","decimal":60099,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
     <row r="454" spans="1:12" x14ac:dyDescent="0.25">
@@ -60003,17 +60240,17 @@
         <f>'Bowtie v1.0 reorg'!E455</f>
         <v>0</v>
       </c>
-      <c r="C454">
+      <c r="C454" t="str">
         <f>'Bowtie v1.0 reorg'!C455</f>
-        <v>0</v>
+        <v>EAC4</v>
       </c>
       <c r="D454">
         <f>'Bowtie v1.0 reorg'!D455</f>
         <v>60100</v>
       </c>
-      <c r="E454" t="str">
+      <c r="E454">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F455),"",'Bowtie v1.0 reorg'!F455)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F454" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G455),"",'Bowtie v1.0 reorg'!G455)</f>
@@ -60035,13 +60272,13 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K455),"",'Bowtie v1.0 reorg'!K455)</f>
         <v/>
       </c>
-      <c r="K454" t="e">
+      <c r="K454" t="str">
+        <f t="shared" si="17"/>
+        <v>{'id':453,'name':'0','unicode':'EAC4','decimal':60100,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+      </c>
+      <c r="L454" t="str">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L454" t="e">
-        <f t="shared" si="19"/>
-        <v>#VALUE!</v>
+        <v>{"id":453,"name":"0","unicode":"EAC4","decimal":60100,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="455" spans="1:12" x14ac:dyDescent="0.25">
@@ -60053,17 +60290,17 @@
         <f>'Bowtie v1.0 reorg'!E456</f>
         <v>0</v>
       </c>
-      <c r="C455">
+      <c r="C455" t="str">
         <f>'Bowtie v1.0 reorg'!C456</f>
-        <v>0</v>
+        <v>EAC5</v>
       </c>
       <c r="D455">
         <f>'Bowtie v1.0 reorg'!D456</f>
         <v>60101</v>
       </c>
-      <c r="E455" t="str">
+      <c r="E455">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F456),"",'Bowtie v1.0 reorg'!F456)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F455" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G456),"",'Bowtie v1.0 reorg'!G456)</f>
@@ -60085,13 +60322,13 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K456),"",'Bowtie v1.0 reorg'!K456)</f>
         <v/>
       </c>
-      <c r="K455" t="e">
+      <c r="K455" t="str">
+        <f t="shared" si="17"/>
+        <v>{'id':454,'name':'0','unicode':'EAC5','decimal':60101,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+      </c>
+      <c r="L455" t="str">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L455" t="e">
-        <f t="shared" si="19"/>
-        <v>#VALUE!</v>
+        <v>{"id":454,"name":"0","unicode":"EAC5","decimal":60101,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="456" spans="1:12" x14ac:dyDescent="0.25">
@@ -60103,17 +60340,17 @@
         <f>'Bowtie v1.0 reorg'!E457</f>
         <v>0</v>
       </c>
-      <c r="C456">
+      <c r="C456" t="str">
         <f>'Bowtie v1.0 reorg'!C457</f>
-        <v>0</v>
+        <v>EAC6</v>
       </c>
       <c r="D456">
         <f>'Bowtie v1.0 reorg'!D457</f>
         <v>60102</v>
       </c>
-      <c r="E456" t="str">
+      <c r="E456">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F457),"",'Bowtie v1.0 reorg'!F457)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F456" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G457),"",'Bowtie v1.0 reorg'!G457)</f>
@@ -60135,13 +60372,13 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K457),"",'Bowtie v1.0 reorg'!K457)</f>
         <v/>
       </c>
-      <c r="K456" t="e">
+      <c r="K456" t="str">
+        <f t="shared" si="17"/>
+        <v>{'id':455,'name':'0','unicode':'EAC6','decimal':60102,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+      </c>
+      <c r="L456" t="str">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L456" t="e">
-        <f t="shared" si="19"/>
-        <v>#VALUE!</v>
+        <v>{"id":455,"name":"0","unicode":"EAC6","decimal":60102,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="457" spans="1:12" x14ac:dyDescent="0.25">
@@ -60153,17 +60390,17 @@
         <f>'Bowtie v1.0 reorg'!E458</f>
         <v>0</v>
       </c>
-      <c r="C457">
+      <c r="C457" t="str">
         <f>'Bowtie v1.0 reorg'!C458</f>
-        <v>0</v>
+        <v>EAC7</v>
       </c>
       <c r="D457">
         <f>'Bowtie v1.0 reorg'!D458</f>
         <v>60103</v>
       </c>
-      <c r="E457" t="str">
+      <c r="E457">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F458),"",'Bowtie v1.0 reorg'!F458)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F457" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G458),"",'Bowtie v1.0 reorg'!G458)</f>
@@ -60185,13 +60422,13 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K458),"",'Bowtie v1.0 reorg'!K458)</f>
         <v/>
       </c>
-      <c r="K457" t="e">
+      <c r="K457" t="str">
+        <f t="shared" si="17"/>
+        <v>{'id':456,'name':'0','unicode':'EAC7','decimal':60103,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+      </c>
+      <c r="L457" t="str">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L457" t="e">
-        <f t="shared" si="19"/>
-        <v>#VALUE!</v>
+        <v>{"id":456,"name":"0","unicode":"EAC7","decimal":60103,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="458" spans="1:12" x14ac:dyDescent="0.25">
@@ -60203,7 +60440,7 @@
         <f>'Bowtie v1.0 reorg'!E459</f>
         <v>0</v>
       </c>
-      <c r="C458">
+      <c r="C458" t="str">
         <f>'Bowtie v1.0 reorg'!C459</f>
         <v>0</v>
       </c>
@@ -60236,11 +60473,11 @@
         <v/>
       </c>
       <c r="K458" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L458" t="e">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L458" t="e">
-        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60253,7 +60490,7 @@
         <f>'Bowtie v1.0 reorg'!E460</f>
         <v>0</v>
       </c>
-      <c r="C459">
+      <c r="C459" t="str">
         <f>'Bowtie v1.0 reorg'!C460</f>
         <v>0</v>
       </c>
@@ -60286,11 +60523,11 @@
         <v/>
       </c>
       <c r="K459" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L459" t="e">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L459" t="e">
-        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60303,7 +60540,7 @@
         <f>'Bowtie v1.0 reorg'!E461</f>
         <v>0</v>
       </c>
-      <c r="C460">
+      <c r="C460" t="str">
         <f>'Bowtie v1.0 reorg'!C461</f>
         <v>0</v>
       </c>
@@ -60336,11 +60573,11 @@
         <v/>
       </c>
       <c r="K460" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L460" t="e">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L460" t="e">
-        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60353,7 +60590,7 @@
         <f>'Bowtie v1.0 reorg'!E462</f>
         <v>0</v>
       </c>
-      <c r="C461">
+      <c r="C461" t="str">
         <f>'Bowtie v1.0 reorg'!C462</f>
         <v>0</v>
       </c>
@@ -60386,11 +60623,11 @@
         <v/>
       </c>
       <c r="K461" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L461" t="e">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L461" t="e">
-        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60403,7 +60640,7 @@
         <f>'Bowtie v1.0 reorg'!E463</f>
         <v>0</v>
       </c>
-      <c r="C462">
+      <c r="C462" t="str">
         <f>'Bowtie v1.0 reorg'!C463</f>
         <v>0</v>
       </c>
@@ -60436,11 +60673,11 @@
         <v/>
       </c>
       <c r="K462" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L462" t="e">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L462" t="e">
-        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60453,7 +60690,7 @@
         <f>'Bowtie v1.0 reorg'!E464</f>
         <v>0</v>
       </c>
-      <c r="C463">
+      <c r="C463" t="str">
         <f>'Bowtie v1.0 reorg'!C464</f>
         <v>0</v>
       </c>
@@ -60486,11 +60723,11 @@
         <v/>
       </c>
       <c r="K463" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L463" t="e">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L463" t="e">
-        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60503,7 +60740,7 @@
         <f>'Bowtie v1.0 reorg'!E465</f>
         <v>0</v>
       </c>
-      <c r="C464">
+      <c r="C464" t="str">
         <f>'Bowtie v1.0 reorg'!C465</f>
         <v>0</v>
       </c>
@@ -60536,11 +60773,11 @@
         <v/>
       </c>
       <c r="K464" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L464" t="e">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L464" t="e">
-        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60553,7 +60790,7 @@
         <f>'Bowtie v1.0 reorg'!E466</f>
         <v>0</v>
       </c>
-      <c r="C465">
+      <c r="C465" t="str">
         <f>'Bowtie v1.0 reorg'!C466</f>
         <v>0</v>
       </c>
@@ -60586,11 +60823,11 @@
         <v/>
       </c>
       <c r="K465" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L465" t="e">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L465" t="e">
-        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60603,7 +60840,7 @@
         <f>'Bowtie v1.0 reorg'!E467</f>
         <v>0</v>
       </c>
-      <c r="C466">
+      <c r="C466" t="str">
         <f>'Bowtie v1.0 reorg'!C467</f>
         <v>0</v>
       </c>
@@ -60636,11 +60873,11 @@
         <v/>
       </c>
       <c r="K466" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L466" t="e">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L466" t="e">
-        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60653,7 +60890,7 @@
         <f>'Bowtie v1.0 reorg'!E468</f>
         <v>0</v>
       </c>
-      <c r="C467">
+      <c r="C467" t="str">
         <f>'Bowtie v1.0 reorg'!C468</f>
         <v>0</v>
       </c>
@@ -60686,11 +60923,11 @@
         <v/>
       </c>
       <c r="K467" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
       <c r="L467" t="e">
-        <f t="shared" ref="L467:L470" si="20">SUBSTITUTE(K467,"'","""")</f>
+        <f t="shared" ref="L467:L470" si="19">SUBSTITUTE(K467,"'","""")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60736,11 +60973,11 @@
         <v/>
       </c>
       <c r="K468" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
       <c r="L468" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60786,11 +61023,11 @@
         <v/>
       </c>
       <c r="K469" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
       <c r="L469" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60836,11 +61073,11 @@
         <v/>
       </c>
       <c r="K470" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
       <c r="L470" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added some file type icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="910">
   <si>
     <t>name</t>
   </si>
@@ -2723,6 +2723,33 @@
   </si>
   <si>
     <t>Temporary solution for badging.</t>
+  </si>
+  <si>
+    <t>file-type-settings</t>
+  </si>
+  <si>
+    <t>file settings configuration system gears document</t>
+  </si>
+  <si>
+    <t>Used for *.dll file type</t>
+  </si>
+  <si>
+    <t>file-type-pdb</t>
+  </si>
+  <si>
+    <t>file pdb document dot</t>
+  </si>
+  <si>
+    <t>Used for *.pdb file type</t>
+  </si>
+  <si>
+    <t>file-type-zip</t>
+  </si>
+  <si>
+    <t>file zip compressed package</t>
+  </si>
+  <si>
+    <t>Used for compressed file types such as zip, tar, tarz, etc.</t>
   </si>
 </sst>
 </file>
@@ -22004,9 +22031,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K444" sqref="K444"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A357" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G357" sqref="G357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34074,6 +34101,31 @@
       <c r="D359">
         <v>60004</v>
       </c>
+      <c r="E359" t="s">
+        <v>901</v>
+      </c>
+      <c r="F359">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G359" t="s">
+        <v>16</v>
+      </c>
+      <c r="H359" t="s">
+        <v>902</v>
+      </c>
+      <c r="I359" t="s">
+        <v>15</v>
+      </c>
+      <c r="J359" t="s">
+        <v>670</v>
+      </c>
+      <c r="K359" t="s">
+        <v>903</v>
+      </c>
+      <c r="L359" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA64-file-type-settings.svg</v>
+      </c>
     </row>
     <row r="360" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360">
@@ -34086,6 +34138,31 @@
       <c r="D360">
         <v>60005</v>
       </c>
+      <c r="E360" t="s">
+        <v>904</v>
+      </c>
+      <c r="F360">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G360" t="s">
+        <v>16</v>
+      </c>
+      <c r="H360" t="s">
+        <v>905</v>
+      </c>
+      <c r="I360" t="s">
+        <v>15</v>
+      </c>
+      <c r="J360" t="s">
+        <v>670</v>
+      </c>
+      <c r="K360" t="s">
+        <v>906</v>
+      </c>
+      <c r="L360" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA65-file-type-pdb.svg</v>
+      </c>
     </row>
     <row r="361" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361">
@@ -34097,6 +34174,31 @@
       </c>
       <c r="D361">
         <v>60006</v>
+      </c>
+      <c r="E361" t="s">
+        <v>907</v>
+      </c>
+      <c r="F361">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G361" t="s">
+        <v>16</v>
+      </c>
+      <c r="H361" t="s">
+        <v>908</v>
+      </c>
+      <c r="I361" t="s">
+        <v>15</v>
+      </c>
+      <c r="J361" t="s">
+        <v>670</v>
+      </c>
+      <c r="K361" t="s">
+        <v>909</v>
+      </c>
+      <c r="L361" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA66-file-type-zip.svg</v>
       </c>
     </row>
     <row r="362" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37593,8 +37695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L453" sqref="L2:L453"/>
+    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
+      <selection activeCell="H454" sqref="H454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55442,9 +55544,9 @@
         <f>'Bowtie v1.0 reorg'!A359</f>
         <v>357</v>
       </c>
-      <c r="B358">
+      <c r="B358" t="str">
         <f>'Bowtie v1.0 reorg'!E359</f>
-        <v>0</v>
+        <v>file-type-settings</v>
       </c>
       <c r="C358" t="str">
         <f>'Bowtie v1.0 reorg'!C359</f>
@@ -55454,37 +55556,37 @@
         <f>'Bowtie v1.0 reorg'!D359</f>
         <v>60004</v>
       </c>
-      <c r="E358" t="str">
+      <c r="E358">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F359),"",'Bowtie v1.0 reorg'!F359)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G359),"",'Bowtie v1.0 reorg'!G359)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I359),"",'Bowtie v1.0 reorg'!I359)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J359),"",'Bowtie v1.0 reorg'!J359)</f>
-        <v/>
+        <v>Code</v>
       </c>
       <c r="I358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H359),"",'Bowtie v1.0 reorg'!H359)</f>
-        <v/>
+        <v>file settings configuration system gears document</v>
       </c>
       <c r="J358" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K359),"",'Bowtie v1.0 reorg'!K359)</f>
-        <v/>
-      </c>
-      <c r="K358" t="e">
+        <v>Used for *.dll file type</v>
+      </c>
+      <c r="K358" t="str">
         <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L358" t="e">
+        <v>{'id':357,'name':'file-type-settings','unicode':'EA64','decimal':60004,'version':'1.1','style':'bold','subset':'VSTS','group':'Code','keywords':['file','settings','configuration','system','gears','document'],'usage':'Used for *.dll file type'}</v>
+      </c>
+      <c r="L358" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+        <v>{"id":357,"name":"file-type-settings","unicode":"EA64","decimal":60004,"version":"1.1","style":"bold","subset":"VSTS","group":"Code","keywords":["file","settings","configuration","system","gears","document"],"usage":"Used for *.dll file type"}</v>
       </c>
     </row>
     <row r="359" spans="1:12" x14ac:dyDescent="0.25">
@@ -55492,9 +55594,9 @@
         <f>'Bowtie v1.0 reorg'!A360</f>
         <v>358</v>
       </c>
-      <c r="B359">
+      <c r="B359" t="str">
         <f>'Bowtie v1.0 reorg'!E360</f>
-        <v>0</v>
+        <v>file-type-pdb</v>
       </c>
       <c r="C359" t="str">
         <f>'Bowtie v1.0 reorg'!C360</f>
@@ -55504,37 +55606,37 @@
         <f>'Bowtie v1.0 reorg'!D360</f>
         <v>60005</v>
       </c>
-      <c r="E359" t="str">
+      <c r="E359">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F360),"",'Bowtie v1.0 reorg'!F360)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G360),"",'Bowtie v1.0 reorg'!G360)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I360),"",'Bowtie v1.0 reorg'!I360)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J360),"",'Bowtie v1.0 reorg'!J360)</f>
-        <v/>
+        <v>Code</v>
       </c>
       <c r="I359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H360),"",'Bowtie v1.0 reorg'!H360)</f>
-        <v/>
+        <v>file pdb document dot</v>
       </c>
       <c r="J359" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K360),"",'Bowtie v1.0 reorg'!K360)</f>
-        <v/>
-      </c>
-      <c r="K359" t="e">
+        <v>Used for *.pdb file type</v>
+      </c>
+      <c r="K359" t="str">
         <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L359" t="e">
+        <v>{'id':358,'name':'file-type-pdb','unicode':'EA65','decimal':60005,'version':'1.1','style':'bold','subset':'VSTS','group':'Code','keywords':['file','pdb','document','dot'],'usage':'Used for *.pdb file type'}</v>
+      </c>
+      <c r="L359" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+        <v>{"id":358,"name":"file-type-pdb","unicode":"EA65","decimal":60005,"version":"1.1","style":"bold","subset":"VSTS","group":"Code","keywords":["file","pdb","document","dot"],"usage":"Used for *.pdb file type"}</v>
       </c>
     </row>
     <row r="360" spans="1:12" x14ac:dyDescent="0.25">
@@ -55542,9 +55644,9 @@
         <f>'Bowtie v1.0 reorg'!A361</f>
         <v>359</v>
       </c>
-      <c r="B360">
+      <c r="B360" t="str">
         <f>'Bowtie v1.0 reorg'!E361</f>
-        <v>0</v>
+        <v>file-type-zip</v>
       </c>
       <c r="C360" t="str">
         <f>'Bowtie v1.0 reorg'!C361</f>
@@ -55554,37 +55656,37 @@
         <f>'Bowtie v1.0 reorg'!D361</f>
         <v>60006</v>
       </c>
-      <c r="E360" t="str">
+      <c r="E360">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F361),"",'Bowtie v1.0 reorg'!F361)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G361),"",'Bowtie v1.0 reorg'!G361)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I361),"",'Bowtie v1.0 reorg'!I361)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J361),"",'Bowtie v1.0 reorg'!J361)</f>
-        <v/>
+        <v>Code</v>
       </c>
       <c r="I360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H361),"",'Bowtie v1.0 reorg'!H361)</f>
-        <v/>
+        <v>file zip compressed package</v>
       </c>
       <c r="J360" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K361),"",'Bowtie v1.0 reorg'!K361)</f>
-        <v/>
-      </c>
-      <c r="K360" t="e">
+        <v>Used for compressed file types such as zip, tar, tarz, etc.</v>
+      </c>
+      <c r="K360" t="str">
         <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L360" t="e">
+        <v>{'id':359,'name':'file-type-zip','unicode':'EA66','decimal':60006,'version':'1.1','style':'bold','subset':'VSTS','group':'Code','keywords':['file','zip','compressed','package'],'usage':'Used for compressed file types such as zip, tar, tarz, etc.'}</v>
+      </c>
+      <c r="L360" t="str">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
+        <v>{"id":359,"name":"file-type-zip","unicode":"EA66","decimal":60006,"version":"1.1","style":"bold","subset":"VSTS","group":"Code","keywords":["file","zip","compressed","package"],"usage":"Used for compressed file types such as zip, tar, tarz, etc."}</v>
       </c>
     </row>
     <row r="361" spans="1:12" x14ac:dyDescent="0.25">
@@ -57029,11 +57131,11 @@
         <v>Used for Sass stylesheet (.sass, .scss) file node in code explorer tree view.</v>
       </c>
       <c r="K389" t="str">
-        <f>IF(NOT(ISBLANK(A389)),CONCATENATE("{'",$A$1,"':",A389,",'",$B$1,"':'",B389,"',","'",$C$1,"':'",C389,"','",$D$1,"':",D389,",'",$E$1,"':'",FIXED(E389,1),"','",$F$1,"':'",F389,"','",$G$1,"':'",G389,"','",$H$1,"':'",H389,"','",$I$1,"':['",SUBSTITUTE(I389," ","','"),"'],'",$J$1,"':'",J389,"'}"))</f>
+        <f t="shared" ref="K389:K397" si="14">IF(NOT(ISBLANK(A389)),CONCATENATE("{'",$A$1,"':",A389,",'",$B$1,"':'",B389,"',","'",$C$1,"':'",C389,"','",$D$1,"':",D389,",'",$E$1,"':'",FIXED(E389,1),"','",$F$1,"':'",F389,"','",$G$1,"':'",G389,"','",$H$1,"':'",H389,"','",$I$1,"':['",SUBSTITUTE(I389," ","','"),"'],'",$J$1,"':'",J389,"'}"))</f>
         <v>{'id':388,'name':'file-type-sass','unicode':'EA83','decimal':60035,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','css','sass','scss','stylesheet'],'usage':'Used for Sass stylesheet (.sass, .scss) file node in code explorer tree view.'}</v>
       </c>
       <c r="L389" t="str">
-        <f t="shared" ref="L389:L452" si="14">SUBSTITUTE(K389,"'","""")</f>
+        <f t="shared" ref="L389:L452" si="15">SUBSTITUTE(K389,"'","""")</f>
         <v>{"id":388,"name":"file-type-sass","unicode":"EA83","decimal":60035,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","css","sass","scss","stylesheet"],"usage":"Used for Sass stylesheet (.sass, .scss) file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57079,11 +57181,11 @@
         <v>Used for Less stylesheet (.less) file node in code explorer tree view.</v>
       </c>
       <c r="K390" t="str">
-        <f>IF(NOT(ISBLANK(A390)),CONCATENATE("{'",$A$1,"':",A390,",'",$B$1,"':'",B390,"',","'",$C$1,"':'",C390,"','",$D$1,"':",D390,",'",$E$1,"':'",FIXED(E390,1),"','",$F$1,"':'",F390,"','",$G$1,"':'",G390,"','",$H$1,"':'",H390,"','",$I$1,"':['",SUBSTITUTE(I390," ","','"),"'],'",$J$1,"':'",J390,"'}"))</f>
+        <f t="shared" si="14"/>
         <v>{'id':389,'name':'file-type-less','unicode':'EA84','decimal':60036,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','css','less','stylesheet'],'usage':'Used for Less stylesheet (.less) file node in code explorer tree view.'}</v>
       </c>
       <c r="L390" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":389,"name":"file-type-less","unicode":"EA84","decimal":60036,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","css","less","stylesheet"],"usage":"Used for Less stylesheet (.less) file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57129,11 +57231,11 @@
         <v>Used for .json file node in code explorer tree view.</v>
       </c>
       <c r="K391" t="str">
-        <f>IF(NOT(ISBLANK(A391)),CONCATENATE("{'",$A$1,"':",A391,",'",$B$1,"':'",B391,"',","'",$C$1,"':'",C391,"','",$D$1,"':",D391,",'",$E$1,"':'",FIXED(E391,1),"','",$F$1,"':'",F391,"','",$G$1,"':'",G391,"','",$H$1,"':'",H391,"','",$I$1,"':['",SUBSTITUTE(I391," ","','"),"'],'",$J$1,"':'",J391,"'}"))</f>
+        <f t="shared" si="14"/>
         <v>{'id':390,'name':'file-type-json','unicode':'EA85','decimal':60037,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','json'],'usage':'Used for .json file node in code explorer tree view.'}</v>
       </c>
       <c r="L391" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":390,"name":"file-type-json","unicode":"EA85","decimal":60037,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","json"],"usage":"Used for .json file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57179,11 +57281,11 @@
         <v>Used for .xml file node in code explorer tree view.</v>
       </c>
       <c r="K392" t="str">
-        <f>IF(NOT(ISBLANK(A392)),CONCATENATE("{'",$A$1,"':",A392,",'",$B$1,"':'",B392,"',","'",$C$1,"':'",C392,"','",$D$1,"':",D392,",'",$E$1,"':'",FIXED(E392,1),"','",$F$1,"':'",F392,"','",$G$1,"':'",G392,"','",$H$1,"':'",H392,"','",$I$1,"':['",SUBSTITUTE(I392," ","','"),"'],'",$J$1,"':'",J392,"'}"))</f>
+        <f t="shared" si="14"/>
         <v>{'id':391,'name':'file-type-xml','unicode':'EA86','decimal':60038,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','xml','markup'],'usage':'Used for .xml file node in code explorer tree view.'}</v>
       </c>
       <c r="L392" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":391,"name":"file-type-xml","unicode":"EA86","decimal":60038,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","xml","markup"],"usage":"Used for .xml file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57229,11 +57331,11 @@
         <v>Used for .md, .markdown file node in code explorer tree view.</v>
       </c>
       <c r="K393" t="str">
-        <f>IF(NOT(ISBLANK(A393)),CONCATENATE("{'",$A$1,"':",A393,",'",$B$1,"':'",B393,"',","'",$C$1,"':'",C393,"','",$D$1,"':",D393,",'",$E$1,"':'",FIXED(E393,1),"','",$F$1,"':'",F393,"','",$G$1,"':'",G393,"','",$H$1,"':'",H393,"','",$I$1,"':['",SUBSTITUTE(I393," ","','"),"'],'",$J$1,"':'",J393,"'}"))</f>
+        <f t="shared" si="14"/>
         <v>{'id':392,'name':'file-type-md','unicode':'EA87','decimal':60039,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','md','markdown'],'usage':'Used for .md, .markdown file node in code explorer tree view.'}</v>
       </c>
       <c r="L393" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":392,"name":"file-type-md","unicode":"EA87","decimal":60039,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","md","markdown"],"usage":"Used for .md, .markdown file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57279,11 +57381,11 @@
         <v>Used for PowerShell (.ps1) file node in code explorer tree view.</v>
       </c>
       <c r="K394" t="str">
-        <f>IF(NOT(ISBLANK(A394)),CONCATENATE("{'",$A$1,"':",A394,",'",$B$1,"':'",B394,"',","'",$C$1,"':'",C394,"','",$D$1,"':",D394,",'",$E$1,"':'",FIXED(E394,1),"','",$F$1,"':'",F394,"','",$G$1,"':'",G394,"','",$H$1,"':'",H394,"','",$I$1,"':['",SUBSTITUTE(I394," ","','"),"'],'",$J$1,"':'",J394,"'}"))</f>
+        <f t="shared" si="14"/>
         <v>{'id':393,'name':'file-type-powershell','unicode':'EA88','decimal':60040,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','powershell','ps1'],'usage':'Used for PowerShell (.ps1) file node in code explorer tree view.'}</v>
       </c>
       <c r="L394" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":393,"name":"file-type-powershell","unicode":"EA88","decimal":60040,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","powershell","ps1"],"usage":"Used for PowerShell (.ps1) file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57329,11 +57431,11 @@
         <v>Used for .cmd file node in code explorer tree view.</v>
       </c>
       <c r="K395" t="str">
-        <f>IF(NOT(ISBLANK(A395)),CONCATENATE("{'",$A$1,"':",A395,",'",$B$1,"':'",B395,"',","'",$C$1,"':'",C395,"','",$D$1,"':",D395,",'",$E$1,"':'",FIXED(E395,1),"','",$F$1,"':'",F395,"','",$G$1,"':'",G395,"','",$H$1,"':'",H395,"','",$I$1,"':['",SUBSTITUTE(I395," ","','"),"'],'",$J$1,"':'",J395,"'}"))</f>
+        <f t="shared" si="14"/>
         <v>{'id':394,'name':'file-type-cmd','unicode':'EA89','decimal':60041,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','cmd'],'usage':'Used for .cmd file node in code explorer tree view.'}</v>
       </c>
       <c r="L395" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":394,"name":"file-type-cmd","unicode":"EA89","decimal":60041,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","cmd"],"usage":"Used for .cmd file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57379,11 +57481,11 @@
         <v>Used for .java file node in code explorer tree view.</v>
       </c>
       <c r="K396" t="str">
-        <f>IF(NOT(ISBLANK(A396)),CONCATENATE("{'",$A$1,"':",A396,",'",$B$1,"':'",B396,"',","'",$C$1,"':'",C396,"','",$D$1,"':",D396,",'",$E$1,"':'",FIXED(E396,1),"','",$F$1,"':'",F396,"','",$G$1,"':'",G396,"','",$H$1,"':'",H396,"','",$I$1,"':['",SUBSTITUTE(I396," ","','"),"'],'",$J$1,"':'",J396,"'}"))</f>
+        <f t="shared" si="14"/>
         <v>{'id':395,'name':'file-type-java','unicode':'EA8A','decimal':60042,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','java'],'usage':'Used for .java file node in code explorer tree view.'}</v>
       </c>
       <c r="L396" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":395,"name":"file-type-java","unicode":"EA8A","decimal":60042,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","java"],"usage":"Used for .java file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57429,11 +57531,11 @@
         <v>Used for .sql file node in code explorer tree view.</v>
       </c>
       <c r="K397" t="str">
-        <f>IF(NOT(ISBLANK(A397)),CONCATENATE("{'",$A$1,"':",A397,",'",$B$1,"':'",B397,"',","'",$C$1,"':'",C397,"','",$D$1,"':",D397,",'",$E$1,"':'",FIXED(E397,1),"','",$F$1,"':'",F397,"','",$G$1,"':'",G397,"','",$H$1,"':'",H397,"','",$I$1,"':['",SUBSTITUTE(I397," ","','"),"'],'",$J$1,"':'",J397,"'}"))</f>
+        <f t="shared" si="14"/>
         <v>{'id':396,'name':'file-type-sql','unicode':'EA8B','decimal':60043,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','sql'],'usage':'Used for .sql file node in code explorer tree view.'}</v>
       </c>
       <c r="L397" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":396,"name":"file-type-sql","unicode":"EA8B","decimal":60043,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","sql"],"usage":"Used for .sql file node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57479,11 +57581,11 @@
         <v>Used for resource file (.resx) node in code explorer tree view.</v>
       </c>
       <c r="K398" t="str">
-        <f t="shared" ref="K398:K408" si="15">IF(NOT(ISBLANK(A398)),CONCATENATE("{'",$A$1,"':",A398,",'",$B$1,"':'",B398,"',","'",$C$1,"':'",C398,"','",$D$1,"':",D398,",'",$E$1,"':'",FIXED(E398,1),"','",$F$1,"':'",F398,"','",$G$1,"':'",G398,"','",$H$1,"':'",H398,"','",$I$1,"':['",SUBSTITUTE(I398," ","','"),"'],'",$J$1,"':'",J398,"'}"))</f>
+        <f t="shared" ref="K398:K408" si="16">IF(NOT(ISBLANK(A398)),CONCATENATE("{'",$A$1,"':",A398,",'",$B$1,"':'",B398,"',","'",$C$1,"':'",C398,"','",$D$1,"':",D398,",'",$E$1,"':'",FIXED(E398,1),"','",$F$1,"':'",F398,"','",$G$1,"':'",G398,"','",$H$1,"':'",H398,"','",$I$1,"':['",SUBSTITUTE(I398," ","','"),"'],'",$J$1,"':'",J398,"'}"))</f>
         <v>{'id':397,'name':'file-stack','unicode':'EA8C','decimal':60044,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','stack','group','resx','resource'],'usage':'Used for resource file (.resx) node in code explorer tree view.'}</v>
       </c>
       <c r="L398" t="str">
-        <f t="shared" ref="L398:L408" si="16">SUBSTITUTE(K398,"'","""")</f>
+        <f t="shared" ref="L398:L408" si="17">SUBSTITUTE(K398,"'","""")</f>
         <v>{"id":397,"name":"file-stack","unicode":"EA8C","decimal":60044,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","stack","group","resx","resource"],"usage":"Used for resource file (.resx) node in code explorer tree view."}</v>
       </c>
     </row>
@@ -57529,11 +57631,11 @@
         <v>Generic script file</v>
       </c>
       <c r="K399" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{'id':398,'name':'script','unicode':'EA8D','decimal':60045,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['script','scroll'],'usage':'Generic script file'}</v>
       </c>
       <c r="L399" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{"id":398,"name":"script","unicode":"EA8D","decimal":60045,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["script","scroll"],"usage":"Generic script file"}</v>
       </c>
     </row>
@@ -57579,11 +57681,11 @@
         <v>Generic executable file such as .bat, .exe</v>
       </c>
       <c r="K400" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{'id':399,'name':'default-executable','unicode':'EA8E','decimal':60046,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['default','executable','gear','process'],'usage':'Generic executable file such as .bat, .exe'}</v>
       </c>
       <c r="L400" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{"id":399,"name":"default-executable","unicode":"EA8E","decimal":60046,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["default","executable","gear","process"],"usage":"Generic executable file such as .bat, .exe"}</v>
       </c>
     </row>
@@ -57629,11 +57731,11 @@
         <v>Used for templating preprocessor file type like .jade, .haml, etc.</v>
       </c>
       <c r="K401" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{'id':400,'name':'file-type-template','unicode':'EA8F','decimal':60047,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['file','template','preprocessor','dotted','line'],'usage':'Used for templating preprocessor file type like .jade, .haml, etc.'}</v>
       </c>
       <c r="L401" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{"id":400,"name":"file-type-template","unicode":"EA8F","decimal":60047,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["file","template","preprocessor","dotted","line"],"usage":"Used for templating preprocessor file type like .jade, .haml, etc."}</v>
       </c>
     </row>
@@ -57679,11 +57781,11 @@
         <v>Used for splitting work item.</v>
       </c>
       <c r="K402" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{'id':401,'name':'split','unicode':'EA90','decimal':60048,'version':'1.1','style':'light','subset':'VSTS','group':'Arrow','keywords':['split','arrow'],'usage':'Used for splitting work item.'}</v>
       </c>
       <c r="L402" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{"id":401,"name":"split","unicode":"EA90","decimal":60048,"version":"1.1","style":"light","subset":"VSTS","group":"Arrow","keywords":["split","arrow"],"usage":"Used for splitting work item."}</v>
       </c>
     </row>
@@ -57729,11 +57831,11 @@
         <v>Used for capturing user actions in the form of an image action log, in TCM Web Runner.</v>
       </c>
       <c r="K403" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{'id':402,'name':'image-action-log','unicode':'EA91','decimal':60049,'version':'1.1','style':'light','subset':'VSTS','group':'Test','keywords':['image','picture','action','crosshair','target'],'usage':'Used for capturing user actions in the form of an image action log, in TCM Web Runner.'}</v>
       </c>
       <c r="L403" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{"id":402,"name":"image-action-log","unicode":"EA91","decimal":60049,"version":"1.1","style":"light","subset":"VSTS","group":"Test","keywords":["image","picture","action","crosshair","target"],"usage":"Used for capturing user actions in the form of an image action log, in TCM Web Runner."}</v>
       </c>
     </row>
@@ -57779,11 +57881,11 @@
         <v>Used in version control view of branches.</v>
       </c>
       <c r="K404" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{'id':403,'name':'shield','unicode':'EA92','decimal':60050,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['shield'],'usage':'Used in version control view of branches.'}</v>
       </c>
       <c r="L404" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{"id":403,"name":"shield","unicode":"EA92","decimal":60050,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["shield"],"usage":"Used in version control view of branches."}</v>
       </c>
     </row>
@@ -57829,11 +57931,11 @@
         <v>Used in version control view of branches.</v>
       </c>
       <c r="K405" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{'id':404,'name':'shield-fill','unicode':'EA93','decimal':60051,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['shield'],'usage':'Used in version control view of branches.'}</v>
       </c>
       <c r="L405" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{"id":404,"name":"shield-fill","unicode":"EA93","decimal":60051,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["shield"],"usage":"Used in version control view of branches."}</v>
       </c>
     </row>
@@ -57879,11 +57981,11 @@
         <v>Used in VC view for git fork. Name is tfvc just because the other VC icons are like that.</v>
       </c>
       <c r="K406" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{'id':405,'name':'tfvc-fork','unicode':'EA94','decimal':60052,'version':'1.1','style':'light','subset':'VSTS','group':'Version Control','keywords':['fork'],'usage':'Used in VC view for git fork. Name is tfvc just because the other VC icons are like that.'}</v>
       </c>
       <c r="L406" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{"id":405,"name":"tfvc-fork","unicode":"EA94","decimal":60052,"version":"1.1","style":"light","subset":"VSTS","group":"Version Control","keywords":["fork"],"usage":"Used in VC view for git fork. Name is tfvc just because the other VC icons are like that."}</v>
       </c>
     </row>
@@ -57929,11 +58031,11 @@
         <v>Used in build view to indicate build is running in progress.</v>
       </c>
       <c r="K407" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{'id':406,'name':'status-run-box','unicode':'EA95','decimal':60053,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['run','in','progress'],'usage':'Used in build view to indicate build is running in progress.'}</v>
       </c>
       <c r="L407" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{"id":406,"name":"status-run-box","unicode":"EA95","decimal":60053,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["run","in","progress"],"usage":"Used in build view to indicate build is running in progress."}</v>
       </c>
     </row>
@@ -57979,11 +58081,11 @@
         <v>Import</v>
       </c>
       <c r="K408" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>{'id':407,'name':'arrow-import','unicode':'EA96','decimal':60054,'version':'1.1','style':'light','subset':'VSTS','group':'Arrow','keywords':['arrow','import'],'usage':'Import'}</v>
       </c>
       <c r="L408" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>{"id":407,"name":"arrow-import","unicode":"EA96","decimal":60054,"version":"1.1","style":"light","subset":"VSTS","group":"Arrow","keywords":["arrow","import"],"usage":"Import"}</v>
       </c>
     </row>
@@ -58029,11 +58131,11 @@
         <v>Add new team project.</v>
       </c>
       <c r="K409" t="str">
-        <f>IF(NOT(ISBLANK(A409)),CONCATENATE("{'",$A$1,"':",A409,",'",$B$1,"':'",B409,"',","'",$C$1,"':'",C409,"','",$D$1,"':",D409,",'",$E$1,"':'",FIXED(E409,1),"','",$F$1,"':'",F409,"','",$G$1,"':'",G409,"','",$H$1,"':'",H409,"','",$I$1,"':['",SUBSTITUTE(I409," ","','"),"'],'",$J$1,"':'",J409,"'}"))</f>
+        <f t="shared" ref="K409:K442" si="18">IF(NOT(ISBLANK(A409)),CONCATENATE("{'",$A$1,"':",A409,",'",$B$1,"':'",B409,"',","'",$C$1,"':'",C409,"','",$D$1,"':",D409,",'",$E$1,"':'",FIXED(E409,1),"','",$F$1,"':'",F409,"','",$G$1,"':'",G409,"','",$H$1,"':'",H409,"','",$I$1,"':['",SUBSTITUTE(I409," ","','"),"'],'",$J$1,"':'",J409,"'}"))</f>
         <v>{'id':408,'name':'new-team-project','unicode':'EA97','decimal':60055,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['new','add','project','folder','plus','chevron'],'usage':'Add new team project.'}</v>
       </c>
       <c r="L409" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":408,"name":"new-team-project","unicode":"EA97","decimal":60055,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["new","add","project","folder","plus","chevron"],"usage":"Add new team project."}</v>
       </c>
     </row>
@@ -58079,11 +58181,11 @@
         <v>Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds.</v>
       </c>
       <c r="K410" t="str">
-        <f>IF(NOT(ISBLANK(A410)),CONCATENATE("{'",$A$1,"':",A410,",'",$B$1,"':'",B410,"',","'",$C$1,"':'",C410,"','",$D$1,"':",D410,",'",$E$1,"':'",FIXED(E410,1),"','",$F$1,"':'",F410,"','",$G$1,"':'",G410,"','",$H$1,"':'",H410,"','",$I$1,"':['",SUBSTITUTE(I410," ","','"),"'],'",$J$1,"':'",J410,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':409,'name':'package-feed-mix','unicode':'EA98','decimal':60056,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','mix','box','square'],'usage':'Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds.'}</v>
       </c>
       <c r="L410" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":409,"name":"package-feed-mix","unicode":"EA98","decimal":60056,"version":"1.1","style":"light","subset":"VSTS","group":"Package","keywords":["package","feed","mix","box","square"],"usage":"Used in Package hub treeview to represent aggregated package feed that includes both remote and local feeds."}</v>
       </c>
     </row>
@@ -58129,11 +58231,11 @@
         <v>Used in Package hub treeview to represent package feed is a reference to remote repo.</v>
       </c>
       <c r="K411" t="str">
-        <f>IF(NOT(ISBLANK(A411)),CONCATENATE("{'",$A$1,"':",A411,",'",$B$1,"':'",B411,"',","'",$C$1,"':'",C411,"','",$D$1,"':",D411,",'",$E$1,"':'",FIXED(E411,1),"','",$F$1,"':'",F411,"','",$G$1,"':'",G411,"','",$H$1,"':'",H411,"','",$I$1,"':['",SUBSTITUTE(I411," ","','"),"'],'",$J$1,"':'",J411,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':410,'name':'package-feed-remote','unicode':'EA99','decimal':60057,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','remote','signal','reference','wave','virtual','box','square'],'usage':'Used in Package hub treeview to represent package feed is a reference to remote repo.'}</v>
       </c>
       <c r="L411" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":410,"name":"package-feed-remote","unicode":"EA99","decimal":60057,"version":"1.1","style":"light","subset":"VSTS","group":"Package","keywords":["package","feed","remote","signal","reference","wave","virtual","box","square"],"usage":"Used in Package hub treeview to represent package feed is a reference to remote repo."}</v>
       </c>
     </row>
@@ -58179,11 +58281,11 @@
         <v>Used in Package hub treeview to represent package feed is a local folder.</v>
       </c>
       <c r="K412" t="str">
-        <f>IF(NOT(ISBLANK(A412)),CONCATENATE("{'",$A$1,"':",A412,",'",$B$1,"':'",B412,"',","'",$C$1,"':'",C412,"','",$D$1,"':",D412,",'",$E$1,"':'",FIXED(E412,1),"','",$F$1,"':'",F412,"','",$G$1,"':'",G412,"','",$H$1,"':'",H412,"','",$I$1,"':['",SUBSTITUTE(I412," ","','"),"'],'",$J$1,"':'",J412,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':411,'name':'package-feed-local','unicode':'EA9A','decimal':60058,'version':'1.1','style':'light','subset':'VSTS','group':'Package','keywords':['package','feed','local','box','square'],'usage':'Used in Package hub treeview to represent package feed is a local folder.'}</v>
       </c>
       <c r="L412" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":411,"name":"package-feed-local","unicode":"EA9A","decimal":60058,"version":"1.1","style":"light","subset":"VSTS","group":"Package","keywords":["package","feed","local","box","square"],"usage":"Used in Package hub treeview to represent package feed is a local folder."}</v>
       </c>
     </row>
@@ -58229,11 +58331,11 @@
         <v>Used in Work hub backlog tree view to represent work items.</v>
       </c>
       <c r="K413" t="str">
-        <f>IF(NOT(ISBLANK(A413)),CONCATENATE("{'",$A$1,"':",A413,",'",$B$1,"':'",B413,"',","'",$C$1,"':'",C413,"','",$D$1,"':",D413,",'",$E$1,"':'",FIXED(E413,1),"','",$F$1,"':'",F413,"','",$G$1,"':'",G413,"','",$H$1,"':'",H413,"','",$I$1,"':['",SUBSTITUTE(I413," ","','"),"'],'",$J$1,"':'",J413,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':412,'name':'work-item-bar-outline','unicode':'EA9B','decimal':60059,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['work','item','bar'],'usage':'Used in Work hub backlog tree view to represent work items.'}</v>
       </c>
       <c r="L413" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":412,"name":"work-item-bar-outline","unicode":"EA9B","decimal":60059,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["work","item","bar"],"usage":"Used in Work hub backlog tree view to represent work items."}</v>
       </c>
     </row>
@@ -58279,11 +58381,11 @@
         <v>Used in ListView control sorting funcionality.</v>
       </c>
       <c r="K414" t="str">
-        <f>IF(NOT(ISBLANK(A414)),CONCATENATE("{'",$A$1,"':",A414,",'",$B$1,"':'",B414,"',","'",$C$1,"':'",C414,"','",$D$1,"':",D414,",'",$E$1,"':'",FIXED(E414,1),"','",$F$1,"':'",F414,"','",$G$1,"':'",G414,"','",$H$1,"':'",H414,"','",$I$1,"':['",SUBSTITUTE(I414," ","','"),"'],'",$J$1,"':'",J414,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':413,'name':'sort-asc','unicode':'EA9C','decimal':60060,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['sort','alphabetically','ascending','arrow','down','letter'],'usage':'Used in ListView control sorting funcionality.'}</v>
       </c>
       <c r="L414" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":413,"name":"sort-asc","unicode":"EA9C","decimal":60060,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["sort","alphabetically","ascending","arrow","down","letter"],"usage":"Used in ListView control sorting funcionality."}</v>
       </c>
     </row>
@@ -58329,11 +58431,11 @@
         <v>Used in ListView control sorting funcionality.</v>
       </c>
       <c r="K415" t="str">
-        <f>IF(NOT(ISBLANK(A415)),CONCATENATE("{'",$A$1,"':",A415,",'",$B$1,"':'",B415,"',","'",$C$1,"':'",C415,"','",$D$1,"':",D415,",'",$E$1,"':'",FIXED(E415,1),"','",$F$1,"':'",F415,"','",$G$1,"':'",G415,"','",$H$1,"':'",H415,"','",$I$1,"':['",SUBSTITUTE(I415," ","','"),"'],'",$J$1,"':'",J415,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':414,'name':'sort-desc','unicode':'EA9D','decimal':60061,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['sort','alphabetically','descending','arrow','down','letter'],'usage':'Used in ListView control sorting funcionality.'}</v>
       </c>
       <c r="L415" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":414,"name":"sort-desc","unicode":"EA9D","decimal":60061,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["sort","alphabetically","descending","arrow","down","letter"],"usage":"Used in ListView control sorting funcionality."}</v>
       </c>
     </row>
@@ -58379,11 +58481,11 @@
         <v>Indicate connection status.</v>
       </c>
       <c r="K416" t="str">
-        <f>IF(NOT(ISBLANK(A416)),CONCATENATE("{'",$A$1,"':",A416,",'",$B$1,"':'",B416,"',","'",$C$1,"':'",C416,"','",$D$1,"':",D416,",'",$E$1,"':'",FIXED(E416,1),"','",$F$1,"':'",F416,"','",$G$1,"':'",G416,"','",$H$1,"':'",H416,"','",$I$1,"':['",SUBSTITUTE(I416," ","','"),"'],'",$J$1,"':'",J416,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':415,'name':'plug-disconnected','unicode':'EA9E','decimal':60062,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['plug','disconnected','unplug','offline'],'usage':'Indicate connection status.'}</v>
       </c>
       <c r="L416" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":415,"name":"plug-disconnected","unicode":"EA9E","decimal":60062,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["plug","disconnected","unplug","offline"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
@@ -58429,11 +58531,11 @@
         <v>Indicate connection status.</v>
       </c>
       <c r="K417" t="str">
-        <f>IF(NOT(ISBLANK(A417)),CONCATENATE("{'",$A$1,"':",A417,",'",$B$1,"':'",B417,"',","'",$C$1,"':'",C417,"','",$D$1,"':",D417,",'",$E$1,"':'",FIXED(E417,1),"','",$F$1,"':'",F417,"','",$G$1,"':'",G417,"','",$H$1,"':'",H417,"','",$I$1,"':['",SUBSTITUTE(I417," ","','"),"'],'",$J$1,"':'",J417,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':416,'name':'plug-connected','unicode':'EA9F','decimal':60063,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['plug','connected','plugged','online'],'usage':'Indicate connection status.'}</v>
       </c>
       <c r="L417" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":416,"name":"plug-connected","unicode":"EA9F","decimal":60063,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["plug","connected","plugged","online"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
@@ -58479,11 +58581,11 @@
         <v>Indicate connection status.</v>
       </c>
       <c r="K418" t="str">
-        <f>IF(NOT(ISBLANK(A418)),CONCATENATE("{'",$A$1,"':",A418,",'",$B$1,"':'",B418,"',","'",$C$1,"':'",C418,"','",$D$1,"':",D418,",'",$E$1,"':'",FIXED(E418,1),"','",$F$1,"':'",F418,"','",$G$1,"':'",G418,"','",$H$1,"':'",H418,"','",$I$1,"':['",SUBSTITUTE(I418," ","','"),"'],'",$J$1,"':'",J418,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':417,'name':'plug-disconnected-fill','unicode':'EAA0','decimal':60064,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['plug','disconnected','unplug','offline'],'usage':'Indicate connection status.'}</v>
       </c>
       <c r="L418" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":417,"name":"plug-disconnected-fill","unicode":"EAA0","decimal":60064,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["plug","disconnected","unplug","offline"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
@@ -58529,11 +58631,11 @@
         <v>Indicate connection status.</v>
       </c>
       <c r="K419" t="str">
-        <f>IF(NOT(ISBLANK(A419)),CONCATENATE("{'",$A$1,"':",A419,",'",$B$1,"':'",B419,"',","'",$C$1,"':'",C419,"','",$D$1,"':",D419,",'",$E$1,"':'",FIXED(E419,1),"','",$F$1,"':'",F419,"','",$G$1,"':'",G419,"','",$H$1,"':'",H419,"','",$I$1,"':['",SUBSTITUTE(I419," ","','"),"'],'",$J$1,"':'",J419,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':418,'name':'plug-connected-fill','unicode':'EAA1','decimal':60065,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['plug','connected','plugged','online'],'usage':'Indicate connection status.'}</v>
       </c>
       <c r="L419" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":418,"name":"plug-connected-fill","unicode":"EAA1","decimal":60065,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["plug","connected","plugged","online"],"usage":"Indicate connection status."}</v>
       </c>
     </row>
@@ -58579,11 +58681,11 @@
         <v>Used in Backlog capacity editor for adding missing team members.</v>
       </c>
       <c r="K420" t="str">
-        <f>IF(NOT(ISBLANK(A420)),CONCATENATE("{'",$A$1,"':",A420,",'",$B$1,"':'",B420,"',","'",$C$1,"':'",C420,"','",$D$1,"':",D420,",'",$E$1,"':'",FIXED(E420,1),"','",$F$1,"':'",F420,"','",$G$1,"':'",G420,"','",$H$1,"':'",H420,"','",$I$1,"':['",SUBSTITUTE(I420," ","','"),"'],'",$J$1,"':'",J420,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':419,'name':'sync-user','unicode':'EAA2','decimal':60066,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['sync','update','user'],'usage':'Used in Backlog capacity editor for adding missing team members.'}</v>
       </c>
       <c r="L420" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":419,"name":"sync-user","unicode":"EAA2","decimal":60066,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["sync","update","user"],"usage":"Used in Backlog capacity editor for adding missing team members."}</v>
       </c>
     </row>
@@ -58629,11 +58731,11 @@
         <v>Used in Code hub to clear applied filters.</v>
       </c>
       <c r="K421" t="str">
-        <f>IF(NOT(ISBLANK(A421)),CONCATENATE("{'",$A$1,"':",A421,",'",$B$1,"':'",B421,"',","'",$C$1,"':'",C421,"','",$D$1,"':",D421,",'",$E$1,"':'",FIXED(E421,1),"','",$F$1,"':'",F421,"','",$G$1,"':'",G421,"','",$H$1,"':'",H421,"','",$I$1,"':['",SUBSTITUTE(I421," ","','"),"'],'",$J$1,"':'",J421,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':420,'name':'clear-filter','unicode':'EAA3','decimal':60067,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['clear','remove','delete','cancel','filter','funnel'],'usage':'Used in Code hub to clear applied filters.'}</v>
       </c>
       <c r="L421" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":420,"name":"clear-filter","unicode":"EAA3","decimal":60067,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["clear","remove","delete","cancel","filter","funnel"],"usage":"Used in Code hub to clear applied filters."}</v>
       </c>
     </row>
@@ -58679,11 +58781,11 @@
         <v>Used for turning off follow on an work item.</v>
       </c>
       <c r="K422" t="str">
-        <f>IF(NOT(ISBLANK(A422)),CONCATENATE("{'",$A$1,"':",A422,",'",$B$1,"':'",B422,"',","'",$C$1,"':'",C422,"','",$D$1,"':",D422,",'",$E$1,"':'",FIXED(E422,1),"','",$F$1,"':'",F422,"','",$G$1,"':'",G422,"','",$H$1,"':'",H422,"','",$I$1,"':['",SUBSTITUTE(I422," ","','"),"'],'",$J$1,"':'",J422,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':421,'name':'watch-eye-off','unicode':'EAA4','decimal':60068,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['watch','eye','follow','off','slash'],'usage':'Used for turning off follow on an work item.'}</v>
       </c>
       <c r="L422" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":421,"name":"watch-eye-off","unicode":"EAA4","decimal":60068,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["watch","eye","follow","off","slash"],"usage":"Used for turning off follow on an work item."}</v>
       </c>
     </row>
@@ -58729,11 +58831,11 @@
         <v>Use this version when shopping cart needs two states: empty and filled</v>
       </c>
       <c r="K423" t="str">
-        <f>IF(NOT(ISBLANK(A423)),CONCATENATE("{'",$A$1,"':",A423,",'",$B$1,"':'",B423,"',","'",$C$1,"':'",C423,"','",$D$1,"':",D423,",'",$E$1,"':'",FIXED(E423,1),"','",$F$1,"':'",F423,"','",$G$1,"':'",G423,"','",$H$1,"':'",H423,"','",$I$1,"':['",SUBSTITUTE(I423," ","','"),"'],'",$J$1,"':'",J423,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':422,'name':'shopping-cart','unicode':'EAA5','decimal':60069,'version':'1.1','style':'light','subset':'VSCOM','group':'Common','keywords':['shop','cart','buy','purchase','store'],'usage':'Use this version when shopping cart needs two states: empty and filled'}</v>
       </c>
       <c r="L423" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":422,"name":"shopping-cart","unicode":"EAA5","decimal":60069,"version":"1.1","style":"light","subset":"VSCOM","group":"Common","keywords":["shop","cart","buy","purchase","store"],"usage":"Use this version when shopping cart needs two states: empty and filled"}</v>
       </c>
     </row>
@@ -58779,11 +58881,11 @@
         <v>Use this version when shopping cart needs two states: empty and filled</v>
       </c>
       <c r="K424" t="str">
-        <f>IF(NOT(ISBLANK(A424)),CONCATENATE("{'",$A$1,"':",A424,",'",$B$1,"':'",B424,"',","'",$C$1,"':'",C424,"','",$D$1,"':",D424,",'",$E$1,"':'",FIXED(E424,1),"','",$F$1,"':'",F424,"','",$G$1,"':'",G424,"','",$H$1,"':'",H424,"','",$I$1,"':['",SUBSTITUTE(I424," ","','"),"'],'",$J$1,"':'",J424,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':423,'name':'shopping-cart-fill','unicode':'EAA6','decimal':60070,'version':'1.1','style':'light','subset':'VSCOM','group':'Common','keywords':['shop','cart','buy','purchase','store'],'usage':'Use this version when shopping cart needs two states: empty and filled'}</v>
       </c>
       <c r="L424" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":423,"name":"shopping-cart-fill","unicode":"EAA6","decimal":60070,"version":"1.1","style":"light","subset":"VSCOM","group":"Common","keywords":["shop","cart","buy","purchase","store"],"usage":"Use this version when shopping cart needs two states: empty and filled"}</v>
       </c>
     </row>
@@ -58829,11 +58931,11 @@
         <v>The common control panel.</v>
       </c>
       <c r="K425" t="str">
-        <f>IF(NOT(ISBLANK(A425)),CONCATENATE("{'",$A$1,"':",A425,",'",$B$1,"':'",B425,"',","'",$C$1,"':'",C425,"','",$D$1,"':",D425,",'",$E$1,"':'",FIXED(E425,1),"','",$F$1,"':'",F425,"','",$G$1,"':'",G425,"','",$H$1,"':'",H425,"','",$I$1,"':['",SUBSTITUTE(I425," ","','"),"'],'",$J$1,"':'",J425,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':424,'name':'control-panel','unicode':'EAA7','decimal':60071,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['control','panel','settings','configuration','slide','adjust'],'usage':'The common control panel.'}</v>
       </c>
       <c r="L425" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":424,"name":"control-panel","unicode":"EAA7","decimal":60071,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["control","panel","settings","configuration","slide","adjust"],"usage":"The common control panel."}</v>
       </c>
     </row>
@@ -58879,11 +58981,11 @@
         <v>Used in capacity view to add missing team member.</v>
       </c>
       <c r="K426" t="str">
-        <f>IF(NOT(ISBLANK(A426)),CONCATENATE("{'",$A$1,"':",A426,",'",$B$1,"':'",B426,"',","'",$C$1,"':'",C426,"','",$D$1,"':",D426,",'",$E$1,"':'",FIXED(E426,1),"','",$F$1,"':'",F426,"','",$G$1,"':'",G426,"','",$H$1,"':'",H426,"','",$I$1,"':['",SUBSTITUTE(I426," ","','"),"'],'",$J$1,"':'",J426,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':425,'name':'add-team','unicode':'EAA8','decimal':60072,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['add','team','user','member'],'usage':'Used in capacity view to add missing team member.'}</v>
       </c>
       <c r="L426" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":425,"name":"add-team","unicode":"EAA8","decimal":60072,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["add","team","user","member"],"usage":"Used in capacity view to add missing team member."}</v>
       </c>
     </row>
@@ -58929,11 +59031,11 @@
         <v>Used for unpin command. Do not use for not-pinned/pinned toggle.</v>
       </c>
       <c r="K427" t="str">
-        <f>IF(NOT(ISBLANK(A427)),CONCATENATE("{'",$A$1,"':",A427,",'",$B$1,"':'",B427,"',","'",$C$1,"':'",C427,"','",$D$1,"':",D427,",'",$E$1,"':'",FIXED(E427,1),"','",$F$1,"':'",F427,"','",$G$1,"':'",G427,"','",$H$1,"':'",H427,"','",$I$1,"':['",SUBSTITUTE(I427," ","','"),"'],'",$J$1,"':'",J427,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':426,'name':'unpin','unicode':'EAA9','decimal':60073,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['pin','unpin','remove'],'usage':'Used for unpin command. Do not use for not-pinned/pinned toggle.'}</v>
       </c>
       <c r="L427" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":426,"name":"unpin","unicode":"EAA9","decimal":60073,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["pin","unpin","remove"],"usage":"Used for unpin command. Do not use for not-pinned/pinned toggle."}</v>
       </c>
     </row>
@@ -58979,11 +59081,11 @@
         <v>Used for unpin command. Do not use for not-pinned/pinned toggle.</v>
       </c>
       <c r="K428" t="str">
-        <f>IF(NOT(ISBLANK(A428)),CONCATENATE("{'",$A$1,"':",A428,",'",$B$1,"':'",B428,"',","'",$C$1,"':'",C428,"','",$D$1,"':",D428,",'",$E$1,"':'",FIXED(E428,1),"','",$F$1,"':'",F428,"','",$G$1,"':'",G428,"','",$H$1,"':'",H428,"','",$I$1,"':['",SUBSTITUTE(I428," ","','"),"'],'",$J$1,"':'",J428,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':427,'name':'unpin-fill','unicode':'EAAA','decimal':60074,'version':'1.1','style':'bold','subset':'VSTS','group':'Common','keywords':['pin','unpin','remove'],'usage':'Used for unpin command. Do not use for not-pinned/pinned toggle.'}</v>
       </c>
       <c r="L428" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":427,"name":"unpin-fill","unicode":"EAAA","decimal":60074,"version":"1.1","style":"bold","subset":"VSTS","group":"Common","keywords":["pin","unpin","remove"],"usage":"Used for unpin command. Do not use for not-pinned/pinned toggle."}</v>
       </c>
     </row>
@@ -59029,11 +59131,11 @@
         <v>Used on Backlogs tab.</v>
       </c>
       <c r="K429" t="str">
-        <f>IF(NOT(ISBLANK(A429)),CONCATENATE("{'",$A$1,"':",A429,",'",$B$1,"':'",B429,"',","'",$C$1,"':'",C429,"','",$D$1,"':",D429,",'",$E$1,"':'",FIXED(E429,1),"','",$F$1,"':'",F429,"','",$G$1,"':'",G429,"','",$H$1,"':'",H429,"','",$I$1,"':['",SUBSTITUTE(I429," ","','"),"'],'",$J$1,"':'",J429,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':428,'name':'backlog','unicode':'EAAB','decimal':60075,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['backlog','board','kanban','card'],'usage':'Used on Backlogs tab.'}</v>
       </c>
       <c r="L429" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":428,"name":"backlog","unicode":"EAAB","decimal":60075,"version":"1.1","style":"bold","subset":"VSTS","group":"Work","keywords":["backlog","board","kanban","card"],"usage":"Used on Backlogs tab."}</v>
       </c>
     </row>
@@ -59079,11 +59181,11 @@
         <v>Common list view, often used together with grid view.</v>
       </c>
       <c r="K430" t="str">
-        <f>IF(NOT(ISBLANK(A430)),CONCATENATE("{'",$A$1,"':",A430,",'",$B$1,"':'",B430,"',","'",$C$1,"':'",C430,"','",$D$1,"':",D430,",'",$E$1,"':'",FIXED(E430,1),"','",$F$1,"':'",F430,"','",$G$1,"':'",G430,"','",$H$1,"':'",H430,"','",$I$1,"':['",SUBSTITUTE(I430," ","','"),"'],'",$J$1,"':'",J430,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':429,'name':'backlog-view-list','unicode':'EAAC','decimal':60076,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['view','list'],'usage':'Common list view, often used together with grid view.'}</v>
       </c>
       <c r="L430" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":429,"name":"backlog-view-list","unicode":"EAAC","decimal":60076,"version":"1.1","style":"bold","subset":"VSTS","group":"Work","keywords":["view","list"],"usage":"Common list view, often used together with grid view."}</v>
       </c>
     </row>
@@ -59129,11 +59231,11 @@
         <v>Used on Plans tab.</v>
       </c>
       <c r="K431" t="str">
-        <f>IF(NOT(ISBLANK(A431)),CONCATENATE("{'",$A$1,"':",A431,",'",$B$1,"':'",B431,"',","'",$C$1,"':'",C431,"','",$D$1,"':",D431,",'",$E$1,"':'",FIXED(E431,1),"','",$F$1,"':'",F431,"','",$G$1,"':'",G431,"','",$H$1,"':'",H431,"','",$I$1,"':['",SUBSTITUTE(I431," ","','"),"'],'",$J$1,"':'",J431,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':430,'name':'plan','unicode':'EAAD','decimal':60077,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['plan','schedule','timeline'],'usage':'Used on Plans tab.'}</v>
       </c>
       <c r="L431" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":430,"name":"plan","unicode":"EAAD","decimal":60077,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["plan","schedule","timeline"],"usage":"Used on Plans tab."}</v>
       </c>
     </row>
@@ -59179,11 +59281,11 @@
         <v>Used on Queries tab.</v>
       </c>
       <c r="K432" t="str">
-        <f>IF(NOT(ISBLANK(A432)),CONCATENATE("{'",$A$1,"':",A432,",'",$B$1,"':'",B432,"',","'",$C$1,"':'",C432,"','",$D$1,"':",D432,",'",$E$1,"':'",FIXED(E432,1),"','",$F$1,"':'",F432,"','",$G$1,"':'",G432,"','",$H$1,"':'",H432,"','",$I$1,"':['",SUBSTITUTE(I432," ","','"),"'],'",$J$1,"':'",J432,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':431,'name':'query-list','unicode':'EAAE','decimal':60078,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['query','list'],'usage':'Used on Queries tab.'}</v>
       </c>
       <c r="L432" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":431,"name":"query-list","unicode":"EAAE","decimal":60078,"version":"1.1","style":"bold","subset":"VSTS","group":"Work","keywords":["query","list"],"usage":"Used on Queries tab."}</v>
       </c>
     </row>
@@ -59229,11 +59331,11 @@
         <v>Used to indicate matix style backlog timeline view.</v>
       </c>
       <c r="K433" t="str">
-        <f>IF(NOT(ISBLANK(A433)),CONCATENATE("{'",$A$1,"':",A433,",'",$B$1,"':'",B433,"',","'",$C$1,"':'",C433,"','",$D$1,"':",D433,",'",$E$1,"':'",FIXED(E433,1),"','",$F$1,"':'",F433,"','",$G$1,"':'",G433,"','",$H$1,"':'",H433,"','",$I$1,"':['",SUBSTITUTE(I433," ","','"),"'],'",$J$1,"':'",J433,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':432,'name':'timeline-matrix','unicode':'EAAF','decimal':60079,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['timeline','delivery','schedule','matrix'],'usage':'Used to indicate matix style backlog timeline view.'}</v>
       </c>
       <c r="L433" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":432,"name":"timeline-matrix","unicode":"EAAF","decimal":60079,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["timeline","delivery","schedule","matrix"],"usage":"Used to indicate matix style backlog timeline view."}</v>
       </c>
     </row>
@@ -59279,11 +59381,11 @@
         <v>Used in Work hub Query page for team favorite queries.</v>
       </c>
       <c r="K434" t="str">
-        <f>IF(NOT(ISBLANK(A434)),CONCATENATE("{'",$A$1,"':",A434,",'",$B$1,"':'",B434,"',","'",$C$1,"':'",C434,"','",$D$1,"':",D434,",'",$E$1,"':'",FIXED(E434,1),"','",$F$1,"':'",F434,"','",$G$1,"':'",G434,"','",$H$1,"':'",H434,"','",$I$1,"':['",SUBSTITUTE(I434," ","','"),"'],'",$J$1,"':'",J434,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':433,'name':'team-favorite','unicode':'EAB0','decimal':60080,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['team','favorite','user','people','star'],'usage':'Used in Work hub Query page for team favorite queries.'}</v>
       </c>
       <c r="L434" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":433,"name":"team-favorite","unicode":"EAB0","decimal":60080,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["team","favorite","user","people","star"],"usage":"Used in Work hub Query page for team favorite queries."}</v>
       </c>
     </row>
@@ -59329,11 +59431,11 @@
         <v>Test impact.</v>
       </c>
       <c r="K435" t="str">
-        <f>IF(NOT(ISBLANK(A435)),CONCATENATE("{'",$A$1,"':",A435,",'",$B$1,"':'",B435,"',","'",$C$1,"':'",C435,"','",$D$1,"':",D435,",'",$E$1,"':'",FIXED(E435,1),"','",$F$1,"':'",F435,"','",$G$1,"':'",G435,"','",$H$1,"':'",H435,"','",$I$1,"':['",SUBSTITUTE(I435," ","','"),"'],'",$J$1,"':'",J435,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':434,'name':'test-impact-fill','unicode':'EAB1','decimal':60081,'version':'1.1','style':'bold','subset':'VSTS','group':'Test','keywords':['test','impact','beaker','flask','hammer'],'usage':'Test impact.'}</v>
       </c>
       <c r="L435" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":434,"name":"test-impact-fill","unicode":"EAB1","decimal":60081,"version":"1.1","style":"bold","subset":"VSTS","group":"Test","keywords":["test","impact","beaker","flask","hammer"],"usage":"Test impact."}</v>
       </c>
     </row>
@@ -59373,11 +59475,11 @@
         <v>860</v>
       </c>
       <c r="K436" t="str">
-        <f>IF(NOT(ISBLANK(A436)),CONCATENATE("{'",$A$1,"':",A436,",'",$B$1,"':'",B436,"',","'",$C$1,"':'",C436,"','",$D$1,"':",D436,",'",$E$1,"':'",FIXED(E436,1),"','",$F$1,"':'",F436,"','",$G$1,"':'",G436,"','",$H$1,"':'",H436,"','",$I$1,"':['",SUBSTITUTE(I436," ","','"),"'],'",$J$1,"':'",J436,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':435,'name':'task-group','unicode':'EAB2','decimal':60082,'version':'1.1','style':'light','subset':'VSTS','group':'Build','keywords':['task','group','list'],'usage':'Used in Release hub for task group.'}</v>
       </c>
       <c r="L436" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":435,"name":"task-group","unicode":"EAB2","decimal":60082,"version":"1.1","style":"light","subset":"VSTS","group":"Build","keywords":["task","group","list"],"usage":"Used in Release hub for task group."}</v>
       </c>
     </row>
@@ -59423,11 +59525,11 @@
         <v>Used in Compliance hub for Engineering Group node dropdown.</v>
       </c>
       <c r="K437" t="str">
-        <f>IF(NOT(ISBLANK(A437)),CONCATENATE("{'",$A$1,"':",A437,",'",$B$1,"':'",B437,"',","'",$C$1,"':'",C437,"','",$D$1,"':",D437,",'",$E$1,"':'",FIXED(E437,1),"','",$F$1,"':'",F437,"','",$G$1,"':'",G437,"','",$H$1,"':'",H437,"','",$I$1,"':['",SUBSTITUTE(I437," ","','"),"'],'",$J$1,"':'",J437,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':436,'name':'engineering-group','unicode':'EAB3','decimal':60083,'version':'1.1','style':'bold','subset':'VSTS','group':'Compliance','keywords':['engineering','group','loop','organization','chart','schema'],'usage':'Used in Compliance hub for Engineering Group node dropdown.'}</v>
       </c>
       <c r="L437" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":436,"name":"engineering-group","unicode":"EAB3","decimal":60083,"version":"1.1","style":"bold","subset":"VSTS","group":"Compliance","keywords":["engineering","group","loop","organization","chart","schema"],"usage":"Used in Compliance hub for Engineering Group node dropdown."}</v>
       </c>
     </row>
@@ -59473,11 +59575,11 @@
         <v>Used for team project.</v>
       </c>
       <c r="K438" t="str">
-        <f>IF(NOT(ISBLANK(A438)),CONCATENATE("{'",$A$1,"':",A438,",'",$B$1,"':'",B438,"',","'",$C$1,"':'",C438,"','",$D$1,"':",D438,",'",$E$1,"':'",FIXED(E438,1),"','",$F$1,"':'",F438,"','",$G$1,"':'",G438,"','",$H$1,"':'",H438,"','",$I$1,"':['",SUBSTITUTE(I438," ","','"),"'],'",$J$1,"':'",J438,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':437,'name':'briefcase','unicode':'EAB4','decimal':60084,'version':'1.1','style':'light','subset':'VSTS','group':'Common','keywords':['briefcase','project','container'],'usage':'Used for team project.'}</v>
       </c>
       <c r="L438" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":437,"name":"briefcase","unicode":"EAB4","decimal":60084,"version":"1.1","style":"light","subset":"VSTS","group":"Common","keywords":["briefcase","project","container"],"usage":"Used for team project."}</v>
       </c>
     </row>
@@ -59523,11 +59625,11 @@
         <v>Variable group is a group of configuration variables which can be used in deployments across build and release.</v>
       </c>
       <c r="K439" t="str">
-        <f>IF(NOT(ISBLANK(A439)),CONCATENATE("{'",$A$1,"':",A439,",'",$B$1,"':'",B439,"',","'",$C$1,"':'",C439,"','",$D$1,"':",D439,",'",$E$1,"':'",FIXED(E439,1),"','",$F$1,"':'",F439,"','",$G$1,"':'",G439,"','",$H$1,"':'",H439,"','",$I$1,"':['",SUBSTITUTE(I439," ","','"),"'],'",$J$1,"':'",J439,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':438,'name':'variable-group','unicode':'EAB5','decimal':60085,'version':'1.1','style':'light','subset':'VSTS','group':'Test','keywords':['variable','group','parameter','x','letter','brackets'],'usage':'Variable group is a group of configuration variables which can be used in deployments across build and release.'}</v>
       </c>
       <c r="L439" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":438,"name":"variable-group","unicode":"EAB5","decimal":60085,"version":"1.1","style":"light","subset":"VSTS","group":"Test","keywords":["variable","group","parameter","x","letter","brackets"],"usage":"Variable group is a group of configuration variables which can be used in deployments across build and release."}</v>
       </c>
     </row>
@@ -59573,11 +59675,11 @@
         <v>To show full history of a file.</v>
       </c>
       <c r="K440" t="str">
-        <f>IF(NOT(ISBLANK(A440)),CONCATENATE("{'",$A$1,"':",A440,",'",$B$1,"':'",B440,"',","'",$C$1,"':'",C440,"','",$D$1,"':",D440,",'",$E$1,"':'",FIXED(E440,1),"','",$F$1,"':'",F440,"','",$G$1,"':'",G440,"','",$H$1,"':'",H440,"','",$I$1,"':['",SUBSTITUTE(I440," ","','"),"'],'",$J$1,"':'",J440,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':439,'name':'full-history','unicode':'EAB6','decimal':60086,'version':'1.1','style':'light','subset':'VSTS','group':'Code','keywords':['history','list','full','all','clock','arrow','time'],'usage':'To show full history of a file.'}</v>
       </c>
       <c r="L440" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":439,"name":"full-history","unicode":"EAB6","decimal":60086,"version":"1.1","style":"light","subset":"VSTS","group":"Code","keywords":["history","list","full","all","clock","arrow","time"],"usage":"To show full history of a file."}</v>
       </c>
     </row>
@@ -59623,11 +59725,11 @@
         <v>Used in Compliance hub for Baseline parent node in treeview.</v>
       </c>
       <c r="K441" t="str">
-        <f>IF(NOT(ISBLANK(A441)),CONCATENATE("{'",$A$1,"':",A441,",'",$B$1,"':'",B441,"',","'",$C$1,"':'",C441,"','",$D$1,"':",D441,",'",$E$1,"':'",FIXED(E441,1),"','",$F$1,"':'",F441,"','",$G$1,"':'",G441,"','",$H$1,"':'",H441,"','",$I$1,"':['",SUBSTITUTE(I441," ","','"),"'],'",$J$1,"':'",J441,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':440,'name':'scope-template','unicode':'EAB7','decimal':60087,'version':'1.1','style':'light','subset':'VSTS','group':'Compliance','keywords':['scope','template','baseline','compliance','document'],'usage':'Used in Compliance hub for Baseline parent node in treeview.'}</v>
       </c>
       <c r="L441" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":440,"name":"scope-template","unicode":"EAB7","decimal":60087,"version":"1.1","style":"light","subset":"VSTS","group":"Compliance","keywords":["scope","template","baseline","compliance","document"],"usage":"Used in Compliance hub for Baseline parent node in treeview."}</v>
       </c>
     </row>
@@ -59673,11 +59775,11 @@
         <v>Used in Compliance hub for Baseline child node in treeview.</v>
       </c>
       <c r="K442" t="str">
-        <f>IF(NOT(ISBLANK(A442)),CONCATENATE("{'",$A$1,"':",A442,",'",$B$1,"':'",B442,"',","'",$C$1,"':'",C442,"','",$D$1,"':",D442,",'",$E$1,"':'",FIXED(E442,1),"','",$F$1,"':'",F442,"','",$G$1,"':'",G442,"','",$H$1,"':'",H442,"','",$I$1,"':['",SUBSTITUTE(I442," ","','"),"'],'",$J$1,"':'",J442,"'}"))</f>
+        <f t="shared" si="18"/>
         <v>{'id':441,'name':'assessment-group-template','unicode':'EAB8','decimal':60088,'version':'1.1','style':'light','subset':'VSTS','group':'Compliance','keywords':['assessment','group','compliance','template','document'],'usage':'Used in Compliance hub for Baseline child node in treeview.'}</v>
       </c>
       <c r="L442" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":441,"name":"assessment-group-template","unicode":"EAB8","decimal":60088,"version":"1.1","style":"light","subset":"VSTS","group":"Compliance","keywords":["assessment","group","compliance","template","document"],"usage":"Used in Compliance hub for Baseline child node in treeview."}</v>
       </c>
     </row>
@@ -59727,7 +59829,7 @@
         <v>{'id':442,'name':'status-success-sm','unicode':'EAB9','decimal':60089,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L443" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":442,"name":"status-success-sm","unicode":"EAB9","decimal":60089,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -59777,7 +59879,7 @@
         <v>{'id':443,'name':'status-warning-sm','unicode':'EABA','decimal':60090,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L444" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":443,"name":"status-warning-sm","unicode":"EABA","decimal":60090,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -59827,7 +59929,7 @@
         <v>{'id':444,'name':'status-info-sm','unicode':'EABB','decimal':60091,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L445" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":444,"name":"status-info-sm","unicode":"EABB","decimal":60091,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -59877,7 +59979,7 @@
         <v>{'id':445,'name':'status-failure-sm','unicode':'EABC','decimal':60092,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L446" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":445,"name":"status-failure-sm","unicode":"EABC","decimal":60092,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -59927,7 +60029,7 @@
         <v>{'id':446,'name':'status-error-sm','unicode':'EABD','decimal':60093,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L447" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":446,"name":"status-error-sm","unicode":"EABD","decimal":60093,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -59977,7 +60079,7 @@
         <v>{'id':447,'name':'status-run-sm','unicode':'EABE','decimal':60094,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L448" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":447,"name":"status-run-sm","unicode":"EABE","decimal":60094,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -60027,7 +60129,7 @@
         <v>{'id':448,'name':'status-help-sm','unicode':'EABF','decimal':60095,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L449" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":448,"name":"status-help-sm","unicode":"EABF","decimal":60095,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -60077,7 +60179,7 @@
         <v>{'id':449,'name':'status-stop-sm','unicode':'EAC0','decimal':60096,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L450" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":449,"name":"status-stop-sm","unicode":"EAC0","decimal":60096,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -60127,7 +60229,7 @@
         <v>{'id':450,'name':'status-pause-sm','unicode':'EAC1','decimal':60097,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L451" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":450,"name":"status-pause-sm","unicode":"EAC1","decimal":60097,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -60177,7 +60279,7 @@
         <v>{'id':451,'name':'status-waiting-fill-sm','unicode':'EAC2','decimal':60098,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L452" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>{"id":451,"name":"status-waiting-fill-sm","unicode":"EAC2","decimal":60098,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -60223,11 +60325,11 @@
         <v>Temporary solution for badging.</v>
       </c>
       <c r="K453" t="str">
-        <f t="shared" ref="K453:K470" si="17">IF(NOT(ISBLANK(A453)),CONCATENATE("{'",$A$1,"':",A453,",'",$B$1,"':'",B453,"',","'",$C$1,"':'",C453,"','",$D$1,"':",D453,",'",$E$1,"':'",FIXED(E453,1),"','",$F$1,"':'",F453,"','",$G$1,"':'",G453,"','",$H$1,"':'",H453,"','",$I$1,"':['",SUBSTITUTE(I453," ","','"),"'],'",$J$1,"':'",J453,"'}"))</f>
+        <f t="shared" ref="K453:K470" si="19">IF(NOT(ISBLANK(A453)),CONCATENATE("{'",$A$1,"':",A453,",'",$B$1,"':'",B453,"',","'",$C$1,"':'",C453,"','",$D$1,"':",D453,",'",$E$1,"':'",FIXED(E453,1),"','",$F$1,"':'",F453,"','",$G$1,"':'",G453,"','",$H$1,"':'",H453,"','",$I$1,"':['",SUBSTITUTE(I453," ","','"),"'],'",$J$1,"':'",J453,"'}"))</f>
         <v>{'id':452,'name':'status-no-fill-sm','unicode':'EAC3','decimal':60099,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':'Temporary solution for badging.'}</v>
       </c>
       <c r="L453" t="str">
-        <f t="shared" ref="L453:L466" si="18">SUBSTITUTE(K453,"'","""")</f>
+        <f t="shared" ref="L453:L466" si="20">SUBSTITUTE(K453,"'","""")</f>
         <v>{"id":452,"name":"status-no-fill-sm","unicode":"EAC3","decimal":60099,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":"Temporary solution for badging."}</v>
       </c>
     </row>
@@ -60273,11 +60375,11 @@
         <v/>
       </c>
       <c r="K454" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>{'id':453,'name':'0','unicode':'EAC4','decimal':60100,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L454" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>{"id":453,"name":"0","unicode":"EAC4","decimal":60100,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
@@ -60323,11 +60425,11 @@
         <v/>
       </c>
       <c r="K455" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>{'id':454,'name':'0','unicode':'EAC5','decimal':60101,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L455" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>{"id":454,"name":"0","unicode":"EAC5","decimal":60101,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
@@ -60373,11 +60475,11 @@
         <v/>
       </c>
       <c r="K456" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>{'id':455,'name':'0','unicode':'EAC6','decimal':60102,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L456" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>{"id":455,"name":"0","unicode":"EAC6","decimal":60102,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
@@ -60423,11 +60525,11 @@
         <v/>
       </c>
       <c r="K457" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>{'id':456,'name':'0','unicode':'EAC7','decimal':60103,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L457" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>{"id":456,"name":"0","unicode":"EAC7","decimal":60103,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
@@ -60473,11 +60575,11 @@
         <v/>
       </c>
       <c r="K458" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L458" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60523,11 +60625,11 @@
         <v/>
       </c>
       <c r="K459" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L459" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60573,11 +60675,11 @@
         <v/>
       </c>
       <c r="K460" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L460" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60623,11 +60725,11 @@
         <v/>
       </c>
       <c r="K461" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L461" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60673,11 +60775,11 @@
         <v/>
       </c>
       <c r="K462" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L462" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60723,11 +60825,11 @@
         <v/>
       </c>
       <c r="K463" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L463" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60773,11 +60875,11 @@
         <v/>
       </c>
       <c r="K464" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L464" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60823,11 +60925,11 @@
         <v/>
       </c>
       <c r="K465" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L465" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60873,11 +60975,11 @@
         <v/>
       </c>
       <c r="K466" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L466" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60923,11 +61025,11 @@
         <v/>
       </c>
       <c r="K467" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L467" t="e">
-        <f t="shared" ref="L467:L470" si="19">SUBSTITUTE(K467,"'","""")</f>
+        <f t="shared" ref="L467:L470" si="21">SUBSTITUTE(K467,"'","""")</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -60973,11 +61075,11 @@
         <v/>
       </c>
       <c r="K468" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L468" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -61023,11 +61125,11 @@
         <v/>
       </c>
       <c r="K469" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L469" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -61073,11 +61175,11 @@
         <v/>
       </c>
       <c r="K470" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="L470" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added user intervention icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2217" uniqueCount="919">
   <si>
     <t>name</t>
   </si>
@@ -2759,6 +2759,24 @@
   </si>
   <si>
     <t>Used as link type indicating there is bug created from build result.</t>
+  </si>
+  <si>
+    <t>user-pause</t>
+  </si>
+  <si>
+    <t>user-pending</t>
+  </si>
+  <si>
+    <t>user pending time clock halt</t>
+  </si>
+  <si>
+    <t>user pause manual intervention halt</t>
+  </si>
+  <si>
+    <t>Used for deployment HALT status when manual intervention is needed.</t>
+  </si>
+  <si>
+    <t>Used for deployment HALT status when user approval is needed.</t>
   </si>
 </sst>
 </file>
@@ -22041,8 +22059,8 @@
   <dimension ref="A1:AL532"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A442" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E455" sqref="E455"/>
+      <pane ySplit="2" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C364" sqref="C364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -34258,6 +34276,31 @@
       <c r="D363">
         <v>60008</v>
       </c>
+      <c r="E363" t="s">
+        <v>913</v>
+      </c>
+      <c r="F363">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G363" t="s">
+        <v>17</v>
+      </c>
+      <c r="H363" t="s">
+        <v>916</v>
+      </c>
+      <c r="I363" t="s">
+        <v>15</v>
+      </c>
+      <c r="J363" t="s">
+        <v>670</v>
+      </c>
+      <c r="K363" t="s">
+        <v>917</v>
+      </c>
+      <c r="L363" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA68-user-pause.svg</v>
+      </c>
     </row>
     <row r="364" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A364">
@@ -34269,6 +34312,31 @@
       </c>
       <c r="D364">
         <v>60009</v>
+      </c>
+      <c r="E364" t="s">
+        <v>914</v>
+      </c>
+      <c r="F364">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G364" t="s">
+        <v>17</v>
+      </c>
+      <c r="H364" t="s">
+        <v>915</v>
+      </c>
+      <c r="I364" t="s">
+        <v>15</v>
+      </c>
+      <c r="J364" t="s">
+        <v>670</v>
+      </c>
+      <c r="K364" t="s">
+        <v>918</v>
+      </c>
+      <c r="L364" t="str">
+        <f t="shared" si="11"/>
+        <v>uEA69-user-pending.svg</v>
       </c>
     </row>
     <row r="365" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -37730,8 +37798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="B450" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -55779,9 +55847,9 @@
         <f>'Bowtie v1.0 reorg'!A363</f>
         <v>361</v>
       </c>
-      <c r="B362">
+      <c r="B362" t="str">
         <f>'Bowtie v1.0 reorg'!E363</f>
-        <v>0</v>
+        <v>user-pause</v>
       </c>
       <c r="C362" t="str">
         <f>'Bowtie v1.0 reorg'!C363</f>
@@ -55791,29 +55859,29 @@
         <f>'Bowtie v1.0 reorg'!D363</f>
         <v>60008</v>
       </c>
-      <c r="E362" t="str">
+      <c r="E362">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F363),"",'Bowtie v1.0 reorg'!F363)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G363),"",'Bowtie v1.0 reorg'!G363)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I363),"",'Bowtie v1.0 reorg'!I363)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J363),"",'Bowtie v1.0 reorg'!J363)</f>
-        <v/>
+        <v>Code</v>
       </c>
       <c r="I362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H363),"",'Bowtie v1.0 reorg'!H363)</f>
-        <v/>
+        <v>user pause manual intervention halt</v>
       </c>
       <c r="J362" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K363),"",'Bowtie v1.0 reorg'!K363)</f>
-        <v/>
+        <v>Used for deployment HALT status when manual intervention is needed.</v>
       </c>
     </row>
     <row r="363" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -55821,9 +55889,9 @@
         <f>'Bowtie v1.0 reorg'!A364</f>
         <v>362</v>
       </c>
-      <c r="B363">
+      <c r="B363" t="str">
         <f>'Bowtie v1.0 reorg'!E364</f>
-        <v>0</v>
+        <v>user-pending</v>
       </c>
       <c r="C363" t="str">
         <f>'Bowtie v1.0 reorg'!C364</f>
@@ -55833,29 +55901,29 @@
         <f>'Bowtie v1.0 reorg'!D364</f>
         <v>60009</v>
       </c>
-      <c r="E363" t="str">
+      <c r="E363">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F364),"",'Bowtie v1.0 reorg'!F364)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G364),"",'Bowtie v1.0 reorg'!G364)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I364),"",'Bowtie v1.0 reorg'!I364)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J364),"",'Bowtie v1.0 reorg'!J364)</f>
-        <v/>
+        <v>Code</v>
       </c>
       <c r="I363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H364),"",'Bowtie v1.0 reorg'!H364)</f>
-        <v/>
+        <v>user pending time clock halt</v>
       </c>
       <c r="J363" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K364),"",'Bowtie v1.0 reorg'!K364)</f>
-        <v/>
+        <v>Used for deployment HALT status when user approval is needed.</v>
       </c>
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Replaced construction icon with giftbox-open
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -2779,13 +2779,13 @@
     <t>Used to indicate the build definition is a draft.</t>
   </si>
   <si>
-    <t>construction</t>
-  </si>
-  <si>
-    <t>under construction work in progress</t>
-  </si>
-  <si>
-    <t>Used to represent preview features under construction.</t>
+    <t>giftbox-open</t>
+  </si>
+  <si>
+    <t>giftbox open new feature magic preview</t>
+  </si>
+  <si>
+    <t>Used to represent preview features.</t>
   </si>
 </sst>
 </file>
@@ -22069,7 +22069,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A443" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L447" sqref="L447"/>
+      <selection pane="bottomLeft" activeCell="K447" sqref="K447"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37379,7 +37379,7 @@
       </c>
       <c r="L446" t="str">
         <f t="shared" si="13"/>
-        <v>uEABB-construction.svg</v>
+        <v>uEABB-giftbox-open.svg</v>
       </c>
     </row>
     <row r="447" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -59999,7 +59999,7 @@
       </c>
       <c r="B445" t="str">
         <f>'Bowtie v1.0 reorg'!E446</f>
-        <v>construction</v>
+        <v>giftbox-open</v>
       </c>
       <c r="C445" t="str">
         <f>'Bowtie v1.0 reorg'!C446</f>
@@ -60023,15 +60023,15 @@
       </c>
       <c r="I445" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H446),"",'Bowtie v1.0 reorg'!H446)</f>
-        <v>under construction work in progress</v>
+        <v>giftbox open new feature magic preview</v>
       </c>
       <c r="K445" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':444,'name':'construction','unicode':'EABB','decimal':60091,'version':'1.1','style':'','subset':'VSTS','group':'Common','keywords':['under','construction','work','in','progress'],'usage':''}</v>
+        <v>{'id':444,'name':'giftbox-open','unicode':'EABB','decimal':60091,'version':'1.1','style':'','subset':'VSTS','group':'Common','keywords':['giftbox','open','new','feature','magic','preview'],'usage':''}</v>
       </c>
       <c r="L445" t="str">
         <f t="shared" si="15"/>
-        <v>{"id":444,"name":"construction","unicode":"EABB","decimal":60091,"version":"1.1","style":"","subset":"VSTS","group":"Common","keywords":["under","construction","work","in","progress"],"usage":""}</v>
+        <v>{"id":444,"name":"giftbox-open","unicode":"EABB","decimal":60091,"version":"1.1","style":"","subset":"VSTS","group":"Common","keywords":["giftbox","open","new","feature","magic","preview"],"usage":""}</v>
       </c>
     </row>
     <row r="446" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added metadata for notification icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17668"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bowtie v1.0 reorg" sheetId="2" r:id="rId1"/>
@@ -22067,9 +22067,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A443" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K447" sqref="K447"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A446" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F447" sqref="F447"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37812,8 +37812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView topLeftCell="A434" workbookViewId="0">
-      <selection activeCell="B445" sqref="B445"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
work item type icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17668"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720" activeTab="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2214" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="940">
   <si>
     <t>name</t>
   </si>
@@ -2786,6 +2786,60 @@
   </si>
   <si>
     <t>Used to represent preview features.</t>
+  </si>
+  <si>
+    <t>symbol-bug</t>
+  </si>
+  <si>
+    <t>symbol-epic</t>
+  </si>
+  <si>
+    <t>symbol-feature</t>
+  </si>
+  <si>
+    <t>symbol-task</t>
+  </si>
+  <si>
+    <t>symbol-roadmap</t>
+  </si>
+  <si>
+    <t>symbol-impediment</t>
+  </si>
+  <si>
+    <t>symbol-ask</t>
+  </si>
+  <si>
+    <t>symbol-risk</t>
+  </si>
+  <si>
+    <t>symbol-review</t>
+  </si>
+  <si>
+    <t>symbol-unparented</t>
+  </si>
+  <si>
+    <t>symbol-custom</t>
+  </si>
+  <si>
+    <t>test-plan</t>
+  </si>
+  <si>
+    <t>test-suite</t>
+  </si>
+  <si>
+    <t>test-step</t>
+  </si>
+  <si>
+    <t>test-parameter</t>
+  </si>
+  <si>
+    <t>bug spider insect beetle</t>
+  </si>
+  <si>
+    <t>Work item type indicator.</t>
+  </si>
+  <si>
+    <t>symbol-book</t>
   </si>
 </sst>
 </file>
@@ -22067,9 +22121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A446" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F447" sqref="F447"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A450" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C452" sqref="C452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37393,12 +37447,30 @@
       <c r="D447">
         <v>60092</v>
       </c>
+      <c r="E447" t="s">
+        <v>922</v>
+      </c>
       <c r="F447">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G447" t="s">
+        <v>16</v>
+      </c>
+      <c r="H447" t="s">
+        <v>937</v>
+      </c>
+      <c r="I447" t="s">
+        <v>15</v>
+      </c>
+      <c r="J447" t="s">
+        <v>602</v>
+      </c>
+      <c r="K447" t="s">
+        <v>938</v>
+      </c>
       <c r="L447" t="str">
         <f t="shared" si="13"/>
-        <v>uEABC-.svg</v>
+        <v>uEABC-symbol-bug.svg</v>
       </c>
     </row>
     <row r="448" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37412,12 +37484,18 @@
       <c r="D448">
         <v>60093</v>
       </c>
+      <c r="E448" t="s">
+        <v>923</v>
+      </c>
       <c r="F448">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G448" t="s">
+        <v>16</v>
+      </c>
       <c r="L448" t="str">
         <f t="shared" si="13"/>
-        <v>uEABD-.svg</v>
+        <v>uEABD-symbol-epic.svg</v>
       </c>
     </row>
     <row r="449" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37431,12 +37509,18 @@
       <c r="D449">
         <v>60094</v>
       </c>
+      <c r="E449" t="s">
+        <v>924</v>
+      </c>
       <c r="F449">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G449" t="s">
+        <v>16</v>
+      </c>
       <c r="L449" t="str">
         <f t="shared" si="13"/>
-        <v>uEABE-.svg</v>
+        <v>uEABE-symbol-feature.svg</v>
       </c>
     </row>
     <row r="450" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37450,12 +37534,18 @@
       <c r="D450">
         <v>60095</v>
       </c>
+      <c r="E450" t="s">
+        <v>925</v>
+      </c>
       <c r="F450">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G450" t="s">
+        <v>16</v>
+      </c>
       <c r="L450" t="str">
         <f t="shared" si="13"/>
-        <v>uEABF-.svg</v>
+        <v>uEABF-symbol-task.svg</v>
       </c>
     </row>
     <row r="451" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37469,12 +37559,18 @@
       <c r="D451">
         <v>60096</v>
       </c>
+      <c r="E451" t="s">
+        <v>926</v>
+      </c>
       <c r="F451">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G451" t="s">
+        <v>16</v>
+      </c>
       <c r="L451" t="str">
         <f t="shared" si="13"/>
-        <v>uEAC0-.svg</v>
+        <v>uEAC0-symbol-roadmap.svg</v>
       </c>
     </row>
     <row r="452" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37488,12 +37584,18 @@
       <c r="D452">
         <v>60097</v>
       </c>
+      <c r="E452" t="s">
+        <v>927</v>
+      </c>
       <c r="F452">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G452" t="s">
+        <v>16</v>
+      </c>
       <c r="L452" t="str">
-        <f t="shared" ref="L452:L466" si="16">CONCATENATE("u",C452,"-",E452,".svg")</f>
-        <v>uEAC1-.svg</v>
+        <f t="shared" ref="L452:L467" si="16">CONCATENATE("u",C452,"-",E452,".svg")</f>
+        <v>uEAC1-symbol-impediment.svg</v>
       </c>
     </row>
     <row r="453" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37507,12 +37609,18 @@
       <c r="D453">
         <v>60098</v>
       </c>
+      <c r="E453" t="s">
+        <v>928</v>
+      </c>
       <c r="F453">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G453" t="s">
+        <v>16</v>
+      </c>
       <c r="L453" t="str">
         <f t="shared" si="16"/>
-        <v>uEAC2-.svg</v>
+        <v>uEAC2-symbol-ask.svg</v>
       </c>
     </row>
     <row r="454" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37526,12 +37634,18 @@
       <c r="D454">
         <v>60099</v>
       </c>
+      <c r="E454" t="s">
+        <v>929</v>
+      </c>
       <c r="F454">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G454" t="s">
+        <v>16</v>
+      </c>
       <c r="L454" t="str">
         <f t="shared" si="16"/>
-        <v>uEAC3-.svg</v>
+        <v>uEAC3-symbol-risk.svg</v>
       </c>
     </row>
     <row r="455" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37545,13 +37659,18 @@
       <c r="D455">
         <v>60100</v>
       </c>
-      <c r="E455" s="2"/>
+      <c r="E455" s="2" t="s">
+        <v>930</v>
+      </c>
       <c r="F455">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G455" t="s">
+        <v>16</v>
+      </c>
       <c r="L455" t="str">
         <f t="shared" si="16"/>
-        <v>uEAC4-.svg</v>
+        <v>uEAC4-symbol-review.svg</v>
       </c>
     </row>
     <row r="456" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37565,12 +37684,18 @@
       <c r="D456">
         <v>60101</v>
       </c>
+      <c r="E456" t="s">
+        <v>931</v>
+      </c>
       <c r="F456">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G456" t="s">
+        <v>16</v>
+      </c>
       <c r="L456" t="str">
         <f t="shared" si="16"/>
-        <v>uEAC5-.svg</v>
+        <v>uEAC5-symbol-unparented.svg</v>
       </c>
     </row>
     <row r="457" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37584,12 +37709,18 @@
       <c r="D457">
         <v>60102</v>
       </c>
+      <c r="E457" t="s">
+        <v>932</v>
+      </c>
       <c r="F457">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G457" t="s">
+        <v>16</v>
+      </c>
       <c r="L457" t="str">
         <f t="shared" si="16"/>
-        <v>uEAC6-.svg</v>
+        <v>uEAC6-symbol-custom.svg</v>
       </c>
     </row>
     <row r="458" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37603,12 +37734,18 @@
       <c r="D458">
         <v>60103</v>
       </c>
+      <c r="E458" t="s">
+        <v>933</v>
+      </c>
       <c r="F458">
         <v>1.1000000000000001</v>
       </c>
+      <c r="G458" t="s">
+        <v>16</v>
+      </c>
       <c r="L458" t="str">
         <f t="shared" si="16"/>
-        <v>uEAC7-.svg</v>
+        <v>uEAC7-test-plan.svg</v>
       </c>
     </row>
     <row r="459" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37617,11 +37754,23 @@
       </c>
       <c r="C459" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EAC8</v>
+      </c>
+      <c r="D459">
+        <v>60104</v>
+      </c>
+      <c r="E459" t="s">
+        <v>934</v>
+      </c>
+      <c r="F459">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G459" t="s">
+        <v>16</v>
       </c>
       <c r="L459" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEAC8-test-suite.svg</v>
       </c>
     </row>
     <row r="460" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37630,11 +37779,23 @@
       </c>
       <c r="C460" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EAC9</v>
+      </c>
+      <c r="D460">
+        <v>60105</v>
+      </c>
+      <c r="E460" t="s">
+        <v>935</v>
+      </c>
+      <c r="F460">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G460" t="s">
+        <v>16</v>
       </c>
       <c r="L460" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEAC9-test-step.svg</v>
       </c>
     </row>
     <row r="461" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37643,11 +37804,23 @@
       </c>
       <c r="C461" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EACA</v>
+      </c>
+      <c r="D461">
+        <v>60106</v>
+      </c>
+      <c r="E461" t="s">
+        <v>936</v>
+      </c>
+      <c r="F461">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G461" t="s">
+        <v>16</v>
       </c>
       <c r="L461" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEACA-test-parameter.svg</v>
       </c>
     </row>
     <row r="462" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37656,11 +37829,23 @@
       </c>
       <c r="C462" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EACB</v>
+      </c>
+      <c r="D462">
+        <v>60107</v>
+      </c>
+      <c r="E462" t="s">
+        <v>939</v>
+      </c>
+      <c r="F462">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G462" t="s">
+        <v>16</v>
       </c>
       <c r="L462" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEACB-symbol-book.svg</v>
       </c>
     </row>
     <row r="463" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37722,6 +37907,10 @@
       <c r="C467" t="str">
         <f t="shared" si="15"/>
         <v>0</v>
+      </c>
+      <c r="L467" t="str">
+        <f t="shared" si="16"/>
+        <v>u0-.svg</v>
       </c>
     </row>
     <row r="468" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37813,7 +38002,7 @@
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60039,9 +60228,9 @@
         <f>'Bowtie v1.0 reorg'!A447</f>
         <v>445</v>
       </c>
-      <c r="B446">
+      <c r="B446" t="str">
         <f>'Bowtie v1.0 reorg'!E447</f>
-        <v>0</v>
+        <v>symbol-bug</v>
       </c>
       <c r="C446" t="str">
         <f>'Bowtie v1.0 reorg'!C447</f>
@@ -60057,23 +60246,23 @@
       </c>
       <c r="G446" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I447),"",'Bowtie v1.0 reorg'!I447)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H446" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J447),"",'Bowtie v1.0 reorg'!J447)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="I446" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H447),"",'Bowtie v1.0 reorg'!H447)</f>
-        <v/>
+        <v>bug spider insect beetle</v>
       </c>
       <c r="K446" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':445,'name':'0','unicode':'EABC','decimal':60092,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':445,'name':'symbol-bug','unicode':'EABC','decimal':60092,'version':'1.1','style':'','subset':'VSTS','group':'Work','keywords':['bug','spider','insect','beetle'],'usage':''}</v>
       </c>
       <c r="L446" t="str">
         <f t="shared" si="15"/>
-        <v>{"id":445,"name":"0","unicode":"EABC","decimal":60092,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":445,"name":"symbol-bug","unicode":"EABC","decimal":60092,"version":"1.1","style":"","subset":"VSTS","group":"Work","keywords":["bug","spider","insect","beetle"],"usage":""}</v>
       </c>
     </row>
     <row r="447" spans="1:12" x14ac:dyDescent="0.25">
@@ -60081,9 +60270,9 @@
         <f>'Bowtie v1.0 reorg'!A448</f>
         <v>446</v>
       </c>
-      <c r="B447">
+      <c r="B447" t="str">
         <f>'Bowtie v1.0 reorg'!E448</f>
-        <v>0</v>
+        <v>symbol-epic</v>
       </c>
       <c r="C447" t="str">
         <f>'Bowtie v1.0 reorg'!C448</f>
@@ -60111,11 +60300,11 @@
       </c>
       <c r="K447" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':446,'name':'0','unicode':'EABD','decimal':60093,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':446,'name':'symbol-epic','unicode':'EABD','decimal':60093,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L447" t="str">
         <f t="shared" si="15"/>
-        <v>{"id":446,"name":"0","unicode":"EABD","decimal":60093,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":446,"name":"symbol-epic","unicode":"EABD","decimal":60093,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="448" spans="1:12" x14ac:dyDescent="0.25">
@@ -60123,9 +60312,9 @@
         <f>'Bowtie v1.0 reorg'!A449</f>
         <v>447</v>
       </c>
-      <c r="B448">
+      <c r="B448" t="str">
         <f>'Bowtie v1.0 reorg'!E449</f>
-        <v>0</v>
+        <v>symbol-feature</v>
       </c>
       <c r="C448" t="str">
         <f>'Bowtie v1.0 reorg'!C449</f>
@@ -60153,11 +60342,11 @@
       </c>
       <c r="K448" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':447,'name':'0','unicode':'EABE','decimal':60094,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':447,'name':'symbol-feature','unicode':'EABE','decimal':60094,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L448" t="str">
         <f t="shared" si="15"/>
-        <v>{"id":447,"name":"0","unicode":"EABE","decimal":60094,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":447,"name":"symbol-feature","unicode":"EABE","decimal":60094,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="449" spans="1:12" x14ac:dyDescent="0.25">
@@ -60165,9 +60354,9 @@
         <f>'Bowtie v1.0 reorg'!A450</f>
         <v>448</v>
       </c>
-      <c r="B449">
+      <c r="B449" t="str">
         <f>'Bowtie v1.0 reorg'!E450</f>
-        <v>0</v>
+        <v>symbol-task</v>
       </c>
       <c r="C449" t="str">
         <f>'Bowtie v1.0 reorg'!C450</f>
@@ -60195,11 +60384,11 @@
       </c>
       <c r="K449" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':448,'name':'0','unicode':'EABF','decimal':60095,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':448,'name':'symbol-task','unicode':'EABF','decimal':60095,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L449" t="str">
         <f t="shared" si="15"/>
-        <v>{"id":448,"name":"0","unicode":"EABF","decimal":60095,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":448,"name":"symbol-task","unicode":"EABF","decimal":60095,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="450" spans="1:12" x14ac:dyDescent="0.25">
@@ -60207,9 +60396,9 @@
         <f>'Bowtie v1.0 reorg'!A451</f>
         <v>449</v>
       </c>
-      <c r="B450">
+      <c r="B450" t="str">
         <f>'Bowtie v1.0 reorg'!E451</f>
-        <v>0</v>
+        <v>symbol-roadmap</v>
       </c>
       <c r="C450" t="str">
         <f>'Bowtie v1.0 reorg'!C451</f>
@@ -60237,11 +60426,11 @@
       </c>
       <c r="K450" t="str">
         <f t="shared" si="14"/>
-        <v>{'id':449,'name':'0','unicode':'EAC0','decimal':60096,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':449,'name':'symbol-roadmap','unicode':'EAC0','decimal':60096,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L450" t="str">
         <f t="shared" si="15"/>
-        <v>{"id":449,"name":"0","unicode":"EAC0","decimal":60096,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":449,"name":"symbol-roadmap","unicode":"EAC0","decimal":60096,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="451" spans="1:12" x14ac:dyDescent="0.25">
@@ -60249,6 +60438,10 @@
         <f>'Bowtie v1.0 reorg'!A452</f>
         <v>450</v>
       </c>
+      <c r="B451" t="str">
+        <f>'Bowtie v1.0 reorg'!E452</f>
+        <v>symbol-impediment</v>
+      </c>
       <c r="C451" t="str">
         <f>'Bowtie v1.0 reorg'!C452</f>
         <v>EAC1</v>
@@ -60275,11 +60468,11 @@
       </c>
       <c r="K451" t="str">
         <f t="shared" ref="K451:K452" si="16">IF(NOT(ISBLANK(A451)),CONCATENATE("{'",$A$1,"':",A451,",'",$B$1,"':'",B451,"',","'",$C$1,"':'",C451,"','",$D$1,"':",D451,",'",$E$1,"':'",FIXED(E451,1),"','",$F$1,"':'",F451,"','",$G$1,"':'",G451,"','",$H$1,"':'",H451,"','",$I$1,"':['",SUBSTITUTE(I451," ","','"),"'],'",$J$1,"':'",J451,"'}"))</f>
-        <v>{'id':450,'name':'','unicode':'EAC1','decimal':60097,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':450,'name':'symbol-impediment','unicode':'EAC1','decimal':60097,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L451" t="str">
         <f t="shared" ref="L451" si="17">SUBSTITUTE(K451,"'","""")</f>
-        <v>{"id":450,"name":"","unicode":"EAC1","decimal":60097,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":450,"name":"symbol-impediment","unicode":"EAC1","decimal":60097,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="452" spans="1:12" x14ac:dyDescent="0.25">
@@ -60287,6 +60480,10 @@
         <f>'Bowtie v1.0 reorg'!A453</f>
         <v>451</v>
       </c>
+      <c r="B452" t="str">
+        <f>'Bowtie v1.0 reorg'!E453</f>
+        <v>symbol-ask</v>
+      </c>
       <c r="C452" t="str">
         <f>'Bowtie v1.0 reorg'!C453</f>
         <v>EAC2</v>
@@ -60313,11 +60510,11 @@
       </c>
       <c r="K452" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':451,'name':'','unicode':'EAC2','decimal':60098,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':451,'name':'symbol-ask','unicode':'EAC2','decimal':60098,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L452" t="str">
         <f t="shared" ref="L452:L458" si="18">SUBSTITUTE(K452,"'","""")</f>
-        <v>{"id":451,"name":"","unicode":"EAC2","decimal":60098,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":451,"name":"symbol-ask","unicode":"EAC2","decimal":60098,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="453" spans="1:12" x14ac:dyDescent="0.25">
@@ -60325,6 +60522,10 @@
         <f>'Bowtie v1.0 reorg'!A454</f>
         <v>452</v>
       </c>
+      <c r="B453" t="str">
+        <f>'Bowtie v1.0 reorg'!E454</f>
+        <v>symbol-risk</v>
+      </c>
       <c r="C453" t="str">
         <f>'Bowtie v1.0 reorg'!C454</f>
         <v>EAC3</v>
@@ -60351,11 +60552,11 @@
       </c>
       <c r="K453" t="str">
         <f t="shared" ref="K453:K470" si="19">IF(NOT(ISBLANK(A453)),CONCATENATE("{'",$A$1,"':",A453,",'",$B$1,"':'",B453,"',","'",$C$1,"':'",C453,"','",$D$1,"':",D453,",'",$E$1,"':'",FIXED(E453,1),"','",$F$1,"':'",F453,"','",$G$1,"':'",G453,"','",$H$1,"':'",H453,"','",$I$1,"':['",SUBSTITUTE(I453," ","','"),"'],'",$J$1,"':'",J453,"'}"))</f>
-        <v>{'id':452,'name':'','unicode':'EAC3','decimal':60099,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':452,'name':'symbol-risk','unicode':'EAC3','decimal':60099,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L453" t="str">
         <f t="shared" si="18"/>
-        <v>{"id":452,"name":"","unicode":"EAC3","decimal":60099,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":452,"name":"symbol-risk","unicode":"EAC3","decimal":60099,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="454" spans="1:12" x14ac:dyDescent="0.25">
@@ -60363,6 +60564,10 @@
         <f>'Bowtie v1.0 reorg'!A455</f>
         <v>453</v>
       </c>
+      <c r="B454" t="str">
+        <f>'Bowtie v1.0 reorg'!E455</f>
+        <v>symbol-review</v>
+      </c>
       <c r="C454" t="str">
         <f>'Bowtie v1.0 reorg'!C455</f>
         <v>EAC4</v>
@@ -60377,7 +60582,7 @@
       </c>
       <c r="F454" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G455),"",'Bowtie v1.0 reorg'!G455)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G454" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I455),"",'Bowtie v1.0 reorg'!I455)</f>
@@ -60397,11 +60602,11 @@
       </c>
       <c r="K454" t="str">
         <f t="shared" si="19"/>
-        <v>{'id':453,'name':'','unicode':'EAC4','decimal':60100,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':453,'name':'symbol-review','unicode':'EAC4','decimal':60100,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L454" t="str">
         <f t="shared" si="18"/>
-        <v>{"id":453,"name":"","unicode":"EAC4","decimal":60100,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":453,"name":"symbol-review","unicode":"EAC4","decimal":60100,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="455" spans="1:12" x14ac:dyDescent="0.25">
@@ -60409,9 +60614,9 @@
         <f>'Bowtie v1.0 reorg'!A456</f>
         <v>454</v>
       </c>
-      <c r="B455">
+      <c r="B455" t="str">
         <f>'Bowtie v1.0 reorg'!E456</f>
-        <v>0</v>
+        <v>symbol-unparented</v>
       </c>
       <c r="C455" t="str">
         <f>'Bowtie v1.0 reorg'!C456</f>
@@ -60427,7 +60632,7 @@
       </c>
       <c r="F455" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G456),"",'Bowtie v1.0 reorg'!G456)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G455" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I456),"",'Bowtie v1.0 reorg'!I456)</f>
@@ -60447,11 +60652,11 @@
       </c>
       <c r="K455" t="str">
         <f t="shared" si="19"/>
-        <v>{'id':454,'name':'0','unicode':'EAC5','decimal':60101,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':454,'name':'symbol-unparented','unicode':'EAC5','decimal':60101,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L455" t="str">
         <f t="shared" si="18"/>
-        <v>{"id":454,"name":"0","unicode":"EAC5","decimal":60101,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":454,"name":"symbol-unparented","unicode":"EAC5","decimal":60101,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="456" spans="1:12" x14ac:dyDescent="0.25">
@@ -60459,9 +60664,9 @@
         <f>'Bowtie v1.0 reorg'!A457</f>
         <v>455</v>
       </c>
-      <c r="B456">
+      <c r="B456" t="str">
         <f>'Bowtie v1.0 reorg'!E457</f>
-        <v>0</v>
+        <v>symbol-custom</v>
       </c>
       <c r="C456" t="str">
         <f>'Bowtie v1.0 reorg'!C457</f>
@@ -60477,7 +60682,7 @@
       </c>
       <c r="F456" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G457),"",'Bowtie v1.0 reorg'!G457)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G456" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I457),"",'Bowtie v1.0 reorg'!I457)</f>
@@ -60497,11 +60702,11 @@
       </c>
       <c r="K456" t="str">
         <f t="shared" si="19"/>
-        <v>{'id':455,'name':'0','unicode':'EAC6','decimal':60102,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':455,'name':'symbol-custom','unicode':'EAC6','decimal':60102,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L456" t="str">
         <f t="shared" si="18"/>
-        <v>{"id":455,"name":"0","unicode":"EAC6","decimal":60102,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":455,"name":"symbol-custom","unicode":"EAC6","decimal":60102,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="457" spans="1:12" x14ac:dyDescent="0.25">
@@ -60509,9 +60714,9 @@
         <f>'Bowtie v1.0 reorg'!A458</f>
         <v>456</v>
       </c>
-      <c r="B457">
+      <c r="B457" t="str">
         <f>'Bowtie v1.0 reorg'!E458</f>
-        <v>0</v>
+        <v>test-plan</v>
       </c>
       <c r="C457" t="str">
         <f>'Bowtie v1.0 reorg'!C458</f>
@@ -60527,7 +60732,7 @@
       </c>
       <c r="F457" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G458),"",'Bowtie v1.0 reorg'!G458)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G457" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I458),"",'Bowtie v1.0 reorg'!I458)</f>
@@ -60547,11 +60752,11 @@
       </c>
       <c r="K457" t="str">
         <f t="shared" si="19"/>
-        <v>{'id':456,'name':'0','unicode':'EAC7','decimal':60103,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':456,'name':'test-plan','unicode':'EAC7','decimal':60103,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':''}</v>
       </c>
       <c r="L457" t="str">
         <f t="shared" si="18"/>
-        <v>{"id":456,"name":"0","unicode":"EAC7","decimal":60103,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":456,"name":"test-plan","unicode":"EAC7","decimal":60103,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="458" spans="1:12" x14ac:dyDescent="0.25">
@@ -60559,25 +60764,25 @@
         <f>'Bowtie v1.0 reorg'!A459</f>
         <v>457</v>
       </c>
-      <c r="B458">
+      <c r="B458" t="str">
         <f>'Bowtie v1.0 reorg'!E459</f>
-        <v>0</v>
+        <v>test-suite</v>
       </c>
       <c r="C458" t="str">
         <f>'Bowtie v1.0 reorg'!C459</f>
-        <v>0</v>
+        <v>EAC8</v>
       </c>
       <c r="D458">
         <f>'Bowtie v1.0 reorg'!D459</f>
-        <v>0</v>
-      </c>
-      <c r="E458" t="str">
+        <v>60104</v>
+      </c>
+      <c r="E458">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F459),"",'Bowtie v1.0 reorg'!F459)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F458" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G459),"",'Bowtie v1.0 reorg'!G459)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G458" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I459),"",'Bowtie v1.0 reorg'!I459)</f>
@@ -60595,13 +60800,13 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K459),"",'Bowtie v1.0 reorg'!K459)</f>
         <v/>
       </c>
-      <c r="K458" t="e">
+      <c r="K458" t="str">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L458" t="e">
+        <v>{'id':457,'name':'test-suite','unicode':'EAC8','decimal':60104,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':''}</v>
+      </c>
+      <c r="L458" t="str">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
+        <v>{"id":457,"name":"test-suite","unicode":"EAC8","decimal":60104,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="459" spans="1:12" x14ac:dyDescent="0.25">
@@ -60609,25 +60814,25 @@
         <f>'Bowtie v1.0 reorg'!A460</f>
         <v>458</v>
       </c>
-      <c r="B459">
+      <c r="B459" t="str">
         <f>'Bowtie v1.0 reorg'!E460</f>
-        <v>0</v>
+        <v>test-step</v>
       </c>
       <c r="C459" t="str">
         <f>'Bowtie v1.0 reorg'!C460</f>
-        <v>0</v>
+        <v>EAC9</v>
       </c>
       <c r="D459">
         <f>'Bowtie v1.0 reorg'!D460</f>
-        <v>0</v>
-      </c>
-      <c r="E459" t="str">
+        <v>60105</v>
+      </c>
+      <c r="E459">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F460),"",'Bowtie v1.0 reorg'!F460)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F459" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G460),"",'Bowtie v1.0 reorg'!G460)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G459" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I460),"",'Bowtie v1.0 reorg'!I460)</f>
@@ -60645,13 +60850,13 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K460),"",'Bowtie v1.0 reorg'!K460)</f>
         <v/>
       </c>
-      <c r="K459" t="e">
+      <c r="K459" t="str">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L459" t="e">
+        <v>{'id':458,'name':'test-step','unicode':'EAC9','decimal':60105,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':''}</v>
+      </c>
+      <c r="L459" t="str">
         <f t="shared" ref="L459:L466" si="20">SUBSTITUTE(K459,"'","""")</f>
-        <v>#VALUE!</v>
+        <v>{"id":458,"name":"test-step","unicode":"EAC9","decimal":60105,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="460" spans="1:12" x14ac:dyDescent="0.25">
@@ -60659,25 +60864,25 @@
         <f>'Bowtie v1.0 reorg'!A461</f>
         <v>459</v>
       </c>
-      <c r="B460">
+      <c r="B460" t="str">
         <f>'Bowtie v1.0 reorg'!E461</f>
-        <v>0</v>
+        <v>test-parameter</v>
       </c>
       <c r="C460" t="str">
         <f>'Bowtie v1.0 reorg'!C461</f>
-        <v>0</v>
+        <v>EACA</v>
       </c>
       <c r="D460">
         <f>'Bowtie v1.0 reorg'!D461</f>
-        <v>0</v>
-      </c>
-      <c r="E460" t="str">
+        <v>60106</v>
+      </c>
+      <c r="E460">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F461),"",'Bowtie v1.0 reorg'!F461)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F460" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G461),"",'Bowtie v1.0 reorg'!G461)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G460" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I461),"",'Bowtie v1.0 reorg'!I461)</f>
@@ -60695,13 +60900,13 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K461),"",'Bowtie v1.0 reorg'!K461)</f>
         <v/>
       </c>
-      <c r="K460" t="e">
+      <c r="K460" t="str">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L460" t="e">
+        <v>{'id':459,'name':'test-parameter','unicode':'EACA','decimal':60106,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':''}</v>
+      </c>
+      <c r="L460" t="str">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
+        <v>{"id":459,"name":"test-parameter","unicode":"EACA","decimal":60106,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="461" spans="1:12" x14ac:dyDescent="0.25">
@@ -60709,25 +60914,25 @@
         <f>'Bowtie v1.0 reorg'!A462</f>
         <v>460</v>
       </c>
-      <c r="B461">
+      <c r="B461" t="str">
         <f>'Bowtie v1.0 reorg'!E462</f>
-        <v>0</v>
+        <v>symbol-book</v>
       </c>
       <c r="C461" t="str">
         <f>'Bowtie v1.0 reorg'!C462</f>
-        <v>0</v>
+        <v>EACB</v>
       </c>
       <c r="D461">
         <f>'Bowtie v1.0 reorg'!D462</f>
-        <v>0</v>
-      </c>
-      <c r="E461" t="str">
+        <v>60107</v>
+      </c>
+      <c r="E461">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F462),"",'Bowtie v1.0 reorg'!F462)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F461" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G462),"",'Bowtie v1.0 reorg'!G462)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G461" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I462),"",'Bowtie v1.0 reorg'!I462)</f>
@@ -60745,13 +60950,13 @@
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K462),"",'Bowtie v1.0 reorg'!K462)</f>
         <v/>
       </c>
-      <c r="K461" t="e">
+      <c r="K461" t="str">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L461" t="e">
+        <v>{'id':460,'name':'symbol-book','unicode':'EACB','decimal':60107,'version':'1.1','style':'bold','subset':'','group':'','keywords':[''],'usage':''}</v>
+      </c>
+      <c r="L461" t="str">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
+        <v>{"id":460,"name":"symbol-book","unicode":"EACB","decimal":60107,"version":"1.1","style":"bold","subset":"","group":"","keywords":[""],"usage":""}</v>
       </c>
     </row>
     <row r="462" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New VSTS product icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17668"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720" activeTab="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2214" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2220" uniqueCount="926">
   <si>
     <t>name</t>
   </si>
@@ -2786,6 +2786,18 @@
   </si>
   <si>
     <t>Used to represent preview features.</t>
+  </si>
+  <si>
+    <t>brand-vsts-alt-1</t>
+  </si>
+  <si>
+    <t>brand-vsts-alt-2</t>
+  </si>
+  <si>
+    <t>brand vsts rtw</t>
+  </si>
+  <si>
+    <t>brand vsts rc preview</t>
   </si>
 </sst>
 </file>
@@ -22067,9 +22079,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A446" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F447" sqref="F447"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A460" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C464" sqref="C464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37617,11 +37629,14 @@
       </c>
       <c r="C459" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EAC8</v>
+      </c>
+      <c r="D459">
+        <v>60104</v>
       </c>
       <c r="L459" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEAC8-.svg</v>
       </c>
     </row>
     <row r="460" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37630,11 +37645,14 @@
       </c>
       <c r="C460" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EAC9</v>
+      </c>
+      <c r="D460">
+        <v>60105</v>
       </c>
       <c r="L460" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEAC9-.svg</v>
       </c>
     </row>
     <row r="461" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37643,11 +37661,14 @@
       </c>
       <c r="C461" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EACA</v>
+      </c>
+      <c r="D461">
+        <v>60106</v>
       </c>
       <c r="L461" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEACA-.svg</v>
       </c>
     </row>
     <row r="462" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37656,11 +37677,14 @@
       </c>
       <c r="C462" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EACB</v>
+      </c>
+      <c r="D462">
+        <v>60107</v>
       </c>
       <c r="L462" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEACB-.svg</v>
       </c>
     </row>
     <row r="463" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37669,11 +37693,26 @@
       </c>
       <c r="C463" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EACC</v>
+      </c>
+      <c r="D463">
+        <v>60108</v>
+      </c>
+      <c r="E463" t="s">
+        <v>922</v>
+      </c>
+      <c r="F463">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G463" t="s">
+        <v>16</v>
+      </c>
+      <c r="H463" t="s">
+        <v>924</v>
       </c>
       <c r="L463" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEACC-brand-vsts-alt-1.svg</v>
       </c>
     </row>
     <row r="464" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37682,11 +37721,26 @@
       </c>
       <c r="C464" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EACD</v>
+      </c>
+      <c r="D464">
+        <v>60109</v>
+      </c>
+      <c r="E464" t="s">
+        <v>923</v>
+      </c>
+      <c r="F464">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G464" t="s">
+        <v>16</v>
+      </c>
+      <c r="H464" t="s">
+        <v>925</v>
       </c>
       <c r="L464" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEACD-brand-vsts-alt-2.svg</v>
       </c>
     </row>
     <row r="465" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37695,11 +37749,14 @@
       </c>
       <c r="C465" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EACE</v>
+      </c>
+      <c r="D465">
+        <v>60110</v>
       </c>
       <c r="L465" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEACE-.svg</v>
       </c>
     </row>
     <row r="466" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37813,7 +37870,7 @@
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60565,11 +60622,11 @@
       </c>
       <c r="C458" t="str">
         <f>'Bowtie v1.0 reorg'!C459</f>
-        <v>0</v>
+        <v>EAC8</v>
       </c>
       <c r="D458">
         <f>'Bowtie v1.0 reorg'!D459</f>
-        <v>0</v>
+        <v>60104</v>
       </c>
       <c r="E458" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F459),"",'Bowtie v1.0 reorg'!F459)</f>
@@ -60615,11 +60672,11 @@
       </c>
       <c r="C459" t="str">
         <f>'Bowtie v1.0 reorg'!C460</f>
-        <v>0</v>
+        <v>EAC9</v>
       </c>
       <c r="D459">
         <f>'Bowtie v1.0 reorg'!D460</f>
-        <v>0</v>
+        <v>60105</v>
       </c>
       <c r="E459" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F460),"",'Bowtie v1.0 reorg'!F460)</f>
@@ -60665,11 +60722,11 @@
       </c>
       <c r="C460" t="str">
         <f>'Bowtie v1.0 reorg'!C461</f>
-        <v>0</v>
+        <v>EACA</v>
       </c>
       <c r="D460">
         <f>'Bowtie v1.0 reorg'!D461</f>
-        <v>0</v>
+        <v>60106</v>
       </c>
       <c r="E460" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F461),"",'Bowtie v1.0 reorg'!F461)</f>
@@ -60715,11 +60772,11 @@
       </c>
       <c r="C461" t="str">
         <f>'Bowtie v1.0 reorg'!C462</f>
-        <v>0</v>
+        <v>EACB</v>
       </c>
       <c r="D461">
         <f>'Bowtie v1.0 reorg'!D462</f>
-        <v>0</v>
+        <v>60107</v>
       </c>
       <c r="E461" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F462),"",'Bowtie v1.0 reorg'!F462)</f>
@@ -60759,25 +60816,25 @@
         <f>'Bowtie v1.0 reorg'!A463</f>
         <v>461</v>
       </c>
-      <c r="B462">
+      <c r="B462" t="str">
         <f>'Bowtie v1.0 reorg'!E463</f>
-        <v>0</v>
+        <v>brand-vsts-alt-1</v>
       </c>
       <c r="C462" t="str">
         <f>'Bowtie v1.0 reorg'!C463</f>
-        <v>0</v>
+        <v>EACC</v>
       </c>
       <c r="D462">
         <f>'Bowtie v1.0 reorg'!D463</f>
-        <v>0</v>
-      </c>
-      <c r="E462" t="str">
+        <v>60108</v>
+      </c>
+      <c r="E462">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F463),"",'Bowtie v1.0 reorg'!F463)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F462" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G463),"",'Bowtie v1.0 reorg'!G463)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G462" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I463),"",'Bowtie v1.0 reorg'!I463)</f>
@@ -60789,19 +60846,19 @@
       </c>
       <c r="I462" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H463),"",'Bowtie v1.0 reorg'!H463)</f>
-        <v/>
+        <v>brand vsts rtw</v>
       </c>
       <c r="J462" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K463),"",'Bowtie v1.0 reorg'!K463)</f>
         <v/>
       </c>
-      <c r="K462" t="e">
+      <c r="K462" t="str">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L462" t="e">
+        <v>{'id':461,'name':'brand-vsts-alt-1','unicode':'EACC','decimal':60108,'version':'1.1','style':'bold','subset':'','group':'','keywords':['brand','vsts','rtw'],'usage':''}</v>
+      </c>
+      <c r="L462" t="str">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
+        <v>{"id":461,"name":"brand-vsts-alt-1","unicode":"EACC","decimal":60108,"version":"1.1","style":"bold","subset":"","group":"","keywords":["brand","vsts","rtw"],"usage":""}</v>
       </c>
     </row>
     <row r="463" spans="1:12" x14ac:dyDescent="0.25">
@@ -60809,25 +60866,25 @@
         <f>'Bowtie v1.0 reorg'!A464</f>
         <v>462</v>
       </c>
-      <c r="B463">
+      <c r="B463" t="str">
         <f>'Bowtie v1.0 reorg'!E464</f>
-        <v>0</v>
+        <v>brand-vsts-alt-2</v>
       </c>
       <c r="C463" t="str">
         <f>'Bowtie v1.0 reorg'!C464</f>
-        <v>0</v>
+        <v>EACD</v>
       </c>
       <c r="D463">
         <f>'Bowtie v1.0 reorg'!D464</f>
-        <v>0</v>
-      </c>
-      <c r="E463" t="str">
+        <v>60109</v>
+      </c>
+      <c r="E463">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F464),"",'Bowtie v1.0 reorg'!F464)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F463" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G464),"",'Bowtie v1.0 reorg'!G464)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G463" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I464),"",'Bowtie v1.0 reorg'!I464)</f>
@@ -60839,19 +60896,19 @@
       </c>
       <c r="I463" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H464),"",'Bowtie v1.0 reorg'!H464)</f>
-        <v/>
+        <v>brand vsts rc preview</v>
       </c>
       <c r="J463" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K464),"",'Bowtie v1.0 reorg'!K464)</f>
         <v/>
       </c>
-      <c r="K463" t="e">
+      <c r="K463" t="str">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L463" t="e">
+        <v>{'id':462,'name':'brand-vsts-alt-2','unicode':'EACD','decimal':60109,'version':'1.1','style':'bold','subset':'','group':'','keywords':['brand','vsts','rc','preview'],'usage':''}</v>
+      </c>
+      <c r="L463" t="str">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
+        <v>{"id":462,"name":"brand-vsts-alt-2","unicode":"EACD","decimal":60109,"version":"1.1","style":"bold","subset":"","group":"","keywords":["brand","vsts","rc","preview"],"usage":""}</v>
       </c>
     </row>
     <row r="464" spans="1:12" x14ac:dyDescent="0.25">
@@ -60865,11 +60922,11 @@
       </c>
       <c r="C464" t="str">
         <f>'Bowtie v1.0 reorg'!C465</f>
-        <v>0</v>
+        <v>EACE</v>
       </c>
       <c r="D464">
         <f>'Bowtie v1.0 reorg'!D465</f>
-        <v>0</v>
+        <v>60110</v>
       </c>
       <c r="E464" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F465),"",'Bowtie v1.0 reorg'!F465)</f>

</xml_diff>

<commit_message>
map icon for I'm here
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2220" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="930">
   <si>
     <t>name</t>
   </si>
@@ -2798,6 +2798,18 @@
   </si>
   <si>
     <t>brand vsts rc preview</t>
+  </si>
+  <si>
+    <t>map-pin</t>
+  </si>
+  <si>
+    <t>map-pin-fill</t>
+  </si>
+  <si>
+    <t>map pin mark location</t>
+  </si>
+  <si>
+    <t>Used in work item topology diagram to indicate the current position.</t>
   </si>
 </sst>
 </file>
@@ -22080,8 +22092,8 @@
   <dimension ref="A1:AL532"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A460" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C464" sqref="C464"/>
+      <pane ySplit="2" topLeftCell="A463" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C466" sqref="C466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37754,9 +37766,27 @@
       <c r="D465">
         <v>60110</v>
       </c>
+      <c r="E465" t="s">
+        <v>926</v>
+      </c>
+      <c r="F465">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G465" t="s">
+        <v>17</v>
+      </c>
+      <c r="H465" t="s">
+        <v>928</v>
+      </c>
+      <c r="I465" t="s">
+        <v>602</v>
+      </c>
+      <c r="K465" t="s">
+        <v>929</v>
+      </c>
       <c r="L465" t="str">
         <f t="shared" si="16"/>
-        <v>uEACE-.svg</v>
+        <v>uEACE-map-pin.svg</v>
       </c>
     </row>
     <row r="466" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37765,11 +37795,32 @@
       </c>
       <c r="C466" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>EACF</v>
+      </c>
+      <c r="D466">
+        <v>60111</v>
+      </c>
+      <c r="E466" t="s">
+        <v>927</v>
+      </c>
+      <c r="F466">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G466" t="s">
+        <v>16</v>
+      </c>
+      <c r="H466" t="s">
+        <v>928</v>
+      </c>
+      <c r="I466" t="s">
+        <v>602</v>
+      </c>
+      <c r="K466" t="s">
+        <v>929</v>
       </c>
       <c r="L466" t="str">
         <f t="shared" si="16"/>
-        <v>u0-.svg</v>
+        <v>uEACF-map-pin-fill.svg</v>
       </c>
     </row>
     <row r="467" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37869,8 +37920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
+      <selection activeCell="L465" sqref="L464:L465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60916,9 +60967,9 @@
         <f>'Bowtie v1.0 reorg'!A465</f>
         <v>463</v>
       </c>
-      <c r="B464">
+      <c r="B464" t="str">
         <f>'Bowtie v1.0 reorg'!E465</f>
-        <v>0</v>
+        <v>map-pin</v>
       </c>
       <c r="C464" t="str">
         <f>'Bowtie v1.0 reorg'!C465</f>
@@ -60928,17 +60979,17 @@
         <f>'Bowtie v1.0 reorg'!D465</f>
         <v>60110</v>
       </c>
-      <c r="E464" t="str">
+      <c r="E464">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F465),"",'Bowtie v1.0 reorg'!F465)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F464" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G465),"",'Bowtie v1.0 reorg'!G465)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G464" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I465),"",'Bowtie v1.0 reorg'!I465)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="H464" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J465),"",'Bowtie v1.0 reorg'!J465)</f>
@@ -60946,19 +60997,19 @@
       </c>
       <c r="I464" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H465),"",'Bowtie v1.0 reorg'!H465)</f>
-        <v/>
+        <v>map pin mark location</v>
       </c>
       <c r="J464" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K465),"",'Bowtie v1.0 reorg'!K465)</f>
-        <v/>
-      </c>
-      <c r="K464" t="e">
+        <v>Used in work item topology diagram to indicate the current position.</v>
+      </c>
+      <c r="K464" t="str">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L464" t="e">
+        <v>{'id':463,'name':'map-pin','unicode':'EACE','decimal':60110,'version':'1.1','style':'light','subset':'Work','group':'','keywords':['map','pin','mark','location'],'usage':'Used in work item topology diagram to indicate the current position.'}</v>
+      </c>
+      <c r="L464" t="str">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
+        <v>{"id":463,"name":"map-pin","unicode":"EACE","decimal":60110,"version":"1.1","style":"light","subset":"Work","group":"","keywords":["map","pin","mark","location"],"usage":"Used in work item topology diagram to indicate the current position."}</v>
       </c>
     </row>
     <row r="465" spans="1:12" x14ac:dyDescent="0.25">
@@ -60966,29 +61017,29 @@
         <f>'Bowtie v1.0 reorg'!A466</f>
         <v>464</v>
       </c>
-      <c r="B465">
+      <c r="B465" t="str">
         <f>'Bowtie v1.0 reorg'!E466</f>
-        <v>0</v>
+        <v>map-pin-fill</v>
       </c>
       <c r="C465" t="str">
         <f>'Bowtie v1.0 reorg'!C466</f>
-        <v>0</v>
+        <v>EACF</v>
       </c>
       <c r="D465">
         <f>'Bowtie v1.0 reorg'!D466</f>
-        <v>0</v>
-      </c>
-      <c r="E465" t="str">
+        <v>60111</v>
+      </c>
+      <c r="E465">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!F466),"",'Bowtie v1.0 reorg'!F466)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F465" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G466),"",'Bowtie v1.0 reorg'!G466)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G465" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I466),"",'Bowtie v1.0 reorg'!I466)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="H465" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J466),"",'Bowtie v1.0 reorg'!J466)</f>
@@ -60996,19 +61047,19 @@
       </c>
       <c r="I465" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H466),"",'Bowtie v1.0 reorg'!H466)</f>
-        <v/>
+        <v>map pin mark location</v>
       </c>
       <c r="J465" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K466),"",'Bowtie v1.0 reorg'!K466)</f>
-        <v/>
-      </c>
-      <c r="K465" t="e">
+        <v>Used in work item topology diagram to indicate the current position.</v>
+      </c>
+      <c r="K465" t="str">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L465" t="e">
+        <v>{'id':464,'name':'map-pin-fill','unicode':'EACF','decimal':60111,'version':'1.1','style':'bold','subset':'Work','group':'','keywords':['map','pin','mark','location'],'usage':'Used in work item topology diagram to indicate the current position.'}</v>
+      </c>
+      <c r="L465" t="str">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
+        <v>{"id":464,"name":"map-pin-fill","unicode":"EACF","decimal":60111,"version":"1.1","style":"bold","subset":"Work","group":"","keywords":["map","pin","mark","location"],"usage":"Used in work item topology diagram to indicate the current position."}</v>
       </c>
     </row>
     <row r="466" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added map destination icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2331" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="970">
   <si>
     <t>name</t>
   </si>
@@ -2918,6 +2918,18 @@
   </si>
   <si>
     <t>symbol-flame</t>
+  </si>
+  <si>
+    <t>map-destination</t>
+  </si>
+  <si>
+    <t>map destination circle</t>
+  </si>
+  <si>
+    <t>Used in work item topology diagram to indicate the destination.</t>
+  </si>
+  <si>
+    <t>map-destination-fill</t>
   </si>
 </sst>
 </file>
@@ -22199,9 +22211,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H458" sqref="H458"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E469" sqref="E469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -38302,13 +38314,30 @@
       <c r="D468">
         <v>60113</v>
       </c>
+      <c r="E468" t="s">
+        <v>966</v>
+      </c>
       <c r="F468">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I468" s="2"/>
+      <c r="G468" t="s">
+        <v>17</v>
+      </c>
+      <c r="H468" t="s">
+        <v>967</v>
+      </c>
+      <c r="I468" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J468" t="s">
+        <v>602</v>
+      </c>
+      <c r="K468" t="s">
+        <v>968</v>
+      </c>
       <c r="L468" t="str">
         <f t="shared" si="18"/>
-        <v>uEAD1-.svg</v>
+        <v>uEAD1-map-destination.svg</v>
       </c>
     </row>
     <row r="469" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -38322,13 +38351,30 @@
       <c r="D469">
         <v>60114</v>
       </c>
+      <c r="E469" t="s">
+        <v>969</v>
+      </c>
       <c r="F469">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I469" s="2"/>
+      <c r="G469" t="s">
+        <v>16</v>
+      </c>
+      <c r="H469" t="s">
+        <v>967</v>
+      </c>
+      <c r="I469" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J469" t="s">
+        <v>602</v>
+      </c>
+      <c r="K469" t="s">
+        <v>968</v>
+      </c>
       <c r="L469" t="str">
         <f t="shared" si="18"/>
-        <v>uEAD2-.svg</v>
+        <v>uEAD2-map-destination-fill.svg</v>
       </c>
     </row>
     <row r="470" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -38474,8 +38520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A449" workbookViewId="0">
-      <selection activeCell="B461" sqref="B461"/>
+    <sheetView tabSelected="1" topLeftCell="A461" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61777,9 +61823,9 @@
         <f>'Bowtie v1.0 reorg'!A468</f>
         <v>466</v>
       </c>
-      <c r="B467">
+      <c r="B467" t="str">
         <f>'Bowtie v1.0 reorg'!E468</f>
-        <v>0</v>
+        <v>map-destination</v>
       </c>
       <c r="C467" t="str">
         <f>'Bowtie v1.0 reorg'!C468</f>
@@ -61795,31 +61841,31 @@
       </c>
       <c r="F467" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G468),"",'Bowtie v1.0 reorg'!G468)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G467" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I468),"",'Bowtie v1.0 reorg'!I468)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H467" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J468),"",'Bowtie v1.0 reorg'!J468)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="I467" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H468),"",'Bowtie v1.0 reorg'!H468)</f>
-        <v/>
+        <v>map destination circle</v>
       </c>
       <c r="J467" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K468),"",'Bowtie v1.0 reorg'!K468)</f>
-        <v/>
+        <v>Used in work item topology diagram to indicate the destination.</v>
       </c>
       <c r="K467" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':466,'name':'0','unicode':'EAD1','decimal':60113,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':466,'name':'map-destination','unicode':'EAD1','decimal':60113,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['map','destination','circle'],'usage':'Used in work item topology diagram to indicate the destination.'}</v>
       </c>
       <c r="L467" t="str">
         <f t="shared" si="17"/>
-        <v>{"id":466,"name":"0","unicode":"EAD1","decimal":60113,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":466,"name":"map-destination","unicode":"EAD1","decimal":60113,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["map","destination","circle"],"usage":"Used in work item topology diagram to indicate the destination."}</v>
       </c>
     </row>
     <row r="468" spans="1:12" x14ac:dyDescent="0.25">
@@ -61827,9 +61873,9 @@
         <f>'Bowtie v1.0 reorg'!A469</f>
         <v>467</v>
       </c>
-      <c r="B468">
+      <c r="B468" t="str">
         <f>'Bowtie v1.0 reorg'!E469</f>
-        <v>0</v>
+        <v>map-destination-fill</v>
       </c>
       <c r="C468" t="str">
         <f>'Bowtie v1.0 reorg'!C469</f>
@@ -61845,31 +61891,31 @@
       </c>
       <c r="F468" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!G469),"",'Bowtie v1.0 reorg'!G469)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G468" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!I469),"",'Bowtie v1.0 reorg'!I469)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H468" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!J469),"",'Bowtie v1.0 reorg'!J469)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="I468" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!H469),"",'Bowtie v1.0 reorg'!H469)</f>
-        <v/>
+        <v>map destination circle</v>
       </c>
       <c r="J468" t="str">
         <f>IF(ISBLANK('Bowtie v1.0 reorg'!K469),"",'Bowtie v1.0 reorg'!K469)</f>
-        <v/>
+        <v>Used in work item topology diagram to indicate the destination.</v>
       </c>
       <c r="K468" t="str">
         <f t="shared" si="16"/>
-        <v>{'id':467,'name':'0','unicode':'EAD2','decimal':60114,'version':'1.1','style':'','subset':'','group':'','keywords':[''],'usage':''}</v>
+        <v>{'id':467,'name':'map-destination-fill','unicode':'EAD2','decimal':60114,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['map','destination','circle'],'usage':'Used in work item topology diagram to indicate the destination.'}</v>
       </c>
       <c r="L468" t="str">
         <f t="shared" si="17"/>
-        <v>{"id":467,"name":"0","unicode":"EAD2","decimal":60114,"version":"1.1","style":"","subset":"","group":"","keywords":[""],"usage":""}</v>
+        <v>{"id":467,"name":"map-destination-fill","unicode":"EAD2","decimal":60114,"version":"1.1","style":"bold","subset":"VSTS","group":"Work","keywords":["map","destination","circle"],"usage":"Used in work item topology diagram to indicate the destination."}</v>
       </c>
     </row>
     <row r="469" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added azure key vault icon
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bowtie" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2602" uniqueCount="1080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2608" uniqueCount="1083">
   <si>
     <t>name</t>
   </si>
@@ -3260,6 +3260,15 @@
   </si>
   <si>
     <t>stopwatch duration time clock</t>
+  </si>
+  <si>
+    <t>azure-key-vault</t>
+  </si>
+  <si>
+    <t>azure key vault</t>
+  </si>
+  <si>
+    <t>Azure Key Vault.</t>
   </si>
 </sst>
 </file>
@@ -22541,9 +22550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL532"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A501" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C511" sqref="C511"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A510" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G514" sqref="G514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -38456,7 +38465,7 @@
         <v>461</v>
       </c>
       <c r="C463" t="str">
-        <f t="shared" ref="C463:C512" si="17">DEC2HEX(D463)</f>
+        <f t="shared" ref="C463:C513" si="17">DEC2HEX(D463)</f>
         <v>EACC</v>
       </c>
       <c r="D463">
@@ -38484,7 +38493,7 @@
         <v>930</v>
       </c>
       <c r="L463" t="str">
-        <f t="shared" ref="L463:L512" si="18">CONCATENATE("u",C463,"-",E463,".svg")</f>
+        <f t="shared" ref="L463:L513" si="18">CONCATENATE("u",C463,"-",E463,".svg")</f>
         <v>uEACC-brand-vsts-alt-1.svg</v>
       </c>
     </row>
@@ -40301,22 +40310,58 @@
         <v>uEAFD-stopwatch.svg</v>
       </c>
     </row>
-    <row r="513" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A513">
+        <v>511</v>
+      </c>
+      <c r="C513" t="str">
+        <f t="shared" si="17"/>
+        <v>EAFE</v>
+      </c>
+      <c r="D513">
+        <v>60158</v>
+      </c>
+      <c r="E513" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F513">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G513" t="s">
+        <v>16</v>
+      </c>
+      <c r="H513" t="s">
+        <v>1081</v>
+      </c>
+      <c r="I513" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J513" t="s">
+        <v>610</v>
+      </c>
+      <c r="K513" t="s">
+        <v>1082</v>
+      </c>
+      <c r="L513" t="str">
+        <f t="shared" si="18"/>
+        <v>uEAFE-azure-key-vault.svg</v>
+      </c>
+    </row>
+    <row r="514" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" spans="1:12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="529" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="530" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="531" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -40336,8 +40381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L559"/>
   <sheetViews>
-    <sheetView topLeftCell="A505" workbookViewId="0">
-      <selection activeCell="L511" sqref="L511"/>
+    <sheetView tabSelected="1" topLeftCell="A505" workbookViewId="0">
+      <selection activeCell="H515" sqref="H515"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65887,51 +65932,51 @@
     <row r="512" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A512">
         <f>bowtie!A513</f>
-        <v>0</v>
-      </c>
-      <c r="B512">
+        <v>511</v>
+      </c>
+      <c r="B512" t="str">
         <f>bowtie!E513</f>
-        <v>0</v>
-      </c>
-      <c r="C512">
+        <v>azure-key-vault</v>
+      </c>
+      <c r="C512" t="str">
         <f>bowtie!C513</f>
-        <v>0</v>
+        <v>EAFE</v>
       </c>
       <c r="D512">
         <f>bowtie!D513</f>
-        <v>0</v>
-      </c>
-      <c r="E512" t="str">
+        <v>60158</v>
+      </c>
+      <c r="E512">
         <f>IF(ISBLANK(bowtie!F513),"",bowtie!F513)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F512" t="str">
         <f>IF(ISBLANK(bowtie!G513),"",bowtie!G513)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G512" t="str">
         <f>IF(ISBLANK(bowtie!I513),"",bowtie!I513)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H512" t="str">
         <f>IF(ISBLANK(bowtie!J513),"",bowtie!J513)</f>
-        <v/>
+        <v>Brand</v>
       </c>
       <c r="I512" t="str">
         <f>IF(ISBLANK(bowtie!H513),"",bowtie!H513)</f>
-        <v/>
+        <v>azure key vault</v>
       </c>
       <c r="J512" t="str">
         <f>IF(ISBLANK(bowtie!K513),"",bowtie!K513)</f>
-        <v/>
-      </c>
-      <c r="K512" t="e">
+        <v>Azure Key Vault.</v>
+      </c>
+      <c r="K512" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L512" t="e">
+        <v>{'id':511,'name':'azure-key-vault','unicode':'EAFE','decimal':60158,'version':'1.1','style':'bold','subset':'VSTS','group':'Brand','keywords':['azure','key','vault'],'usage':'Azure Key Vault.'}</v>
+      </c>
+      <c r="L512" t="str">
         <f t="shared" si="23"/>
-        <v>#VALUE!</v>
+        <v>{"id":511,"name":"azure-key-vault","unicode":"EAFE","decimal":60158,"version":"1.1","style":"bold","subset":"VSTS","group":"Brand","keywords":["azure","key","vault"],"usage":"Azure Key Vault."}</v>
       </c>
     </row>
     <row r="513" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added test outcome icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2620" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2632" uniqueCount="1095">
   <si>
     <t>name</t>
   </si>
@@ -3287,6 +3287,24 @@
   </si>
   <si>
     <t>Used to represent the user does not have permission to a file.</t>
+  </si>
+  <si>
+    <t>not-executed</t>
+  </si>
+  <si>
+    <t>not execute run play triangle block no</t>
+  </si>
+  <si>
+    <t>Used in Test hub for not executed test outcome.</t>
+  </si>
+  <si>
+    <t>not-impacted</t>
+  </si>
+  <si>
+    <t>not impact hammer block no</t>
+  </si>
+  <si>
+    <t>Used in Test hub for not impacted test outcome.</t>
   </si>
 </sst>
 </file>
@@ -22579,8 +22597,8 @@
   <dimension ref="A1:AL532"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A511" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M513" sqref="M513"/>
+      <pane ySplit="2" topLeftCell="A513" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O517" sqref="O517"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -38493,7 +38511,7 @@
         <v>461</v>
       </c>
       <c r="C463" t="str">
-        <f t="shared" ref="C463:C515" si="17">DEC2HEX(D463)</f>
+        <f t="shared" ref="C463:C516" si="17">DEC2HEX(D463)</f>
         <v>EACC</v>
       </c>
       <c r="D463">
@@ -38521,7 +38539,7 @@
         <v>930</v>
       </c>
       <c r="L463" t="str">
-        <f t="shared" ref="L463:L515" si="18">CONCATENATE("u",C463,"-",E463,".svg")</f>
+        <f t="shared" ref="L463:L517" si="18">CONCATENATE("u",C463,"-",E463,".svg")</f>
         <v>uEACC-brand-vsts-alt-1.svg</v>
       </c>
     </row>
@@ -40452,8 +40470,81 @@
         <v>20170518</v>
       </c>
     </row>
-    <row r="516" spans="1:14" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="517" spans="1:14" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="516" spans="1:14" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A516">
+        <v>514</v>
+      </c>
+      <c r="C516" t="str">
+        <f t="shared" si="17"/>
+        <v>EB01</v>
+      </c>
+      <c r="D516">
+        <v>60161</v>
+      </c>
+      <c r="E516" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F516">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G516" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H516" t="s">
+        <v>1090</v>
+      </c>
+      <c r="I516" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J516" s="15" t="s">
+        <v>607</v>
+      </c>
+      <c r="K516" t="s">
+        <v>1091</v>
+      </c>
+      <c r="L516" t="str">
+        <f t="shared" si="18"/>
+        <v>uEB01-not-executed.svg</v>
+      </c>
+    </row>
+    <row r="517" spans="1:14" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A517" s="15">
+        <v>515</v>
+      </c>
+      <c r="B517" s="15"/>
+      <c r="C517" s="15" t="str">
+        <f t="shared" ref="C517" si="20">DEC2HEX(D517)</f>
+        <v>EB02</v>
+      </c>
+      <c r="D517" s="15">
+        <v>60162</v>
+      </c>
+      <c r="E517" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F517">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G517" t="s">
+        <v>16</v>
+      </c>
+      <c r="H517" t="s">
+        <v>1093</v>
+      </c>
+      <c r="I517" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J517" s="15" t="s">
+        <v>607</v>
+      </c>
+      <c r="K517" t="s">
+        <v>1094</v>
+      </c>
+      <c r="L517" t="str">
+        <f t="shared" si="18"/>
+        <v>uEB02-not-impacted.svg</v>
+      </c>
+    </row>
     <row r="518" spans="1:14" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="519" spans="1:14" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="520" spans="1:14" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -66185,101 +66276,101 @@
     <row r="515" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A515">
         <f>bowtie!A516</f>
-        <v>0</v>
-      </c>
-      <c r="B515">
+        <v>514</v>
+      </c>
+      <c r="B515" t="str">
         <f>bowtie!E516</f>
-        <v>0</v>
-      </c>
-      <c r="C515">
+        <v>not-executed</v>
+      </c>
+      <c r="C515" t="str">
         <f>bowtie!C516</f>
-        <v>0</v>
+        <v>EB01</v>
       </c>
       <c r="D515">
         <f>bowtie!D516</f>
-        <v>0</v>
-      </c>
-      <c r="E515" t="str">
+        <v>60161</v>
+      </c>
+      <c r="E515">
         <f>IF(ISBLANK(bowtie!F516),"",bowtie!F516)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F515" t="str">
         <f>IF(ISBLANK(bowtie!G516),"",bowtie!G516)</f>
-        <v/>
+        <v>light</v>
       </c>
       <c r="G515" t="str">
         <f>IF(ISBLANK(bowtie!I516),"",bowtie!I516)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H515" t="str">
         <f>IF(ISBLANK(bowtie!J516),"",bowtie!J516)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I515" t="str">
         <f>IF(ISBLANK(bowtie!H516),"",bowtie!H516)</f>
-        <v/>
+        <v>not execute run play triangle block no</v>
       </c>
       <c r="J515" t="str">
         <f>IF(ISBLANK(bowtie!K516),"",bowtie!K516)</f>
-        <v/>
-      </c>
-      <c r="K515" t="e">
+        <v>Used in Test hub for not executed test outcome.</v>
+      </c>
+      <c r="K515" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L515" t="e">
+        <v>{'id':514,'name':'not-executed','unicode':'EB01','decimal':60161,'version':'1.1','style':'light','subset':'VSTS','group':'Status','keywords':['not','execute','run','play','triangle','block','no'],'usage':'Used in Test hub for not executed test outcome.'}</v>
+      </c>
+      <c r="L515" t="str">
         <f t="shared" si="23"/>
-        <v>#VALUE!</v>
+        <v>{"id":514,"name":"not-executed","unicode":"EB01","decimal":60161,"version":"1.1","style":"light","subset":"VSTS","group":"Status","keywords":["not","execute","run","play","triangle","block","no"],"usage":"Used in Test hub for not executed test outcome."}</v>
       </c>
     </row>
     <row r="516" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A516">
         <f>bowtie!A517</f>
-        <v>0</v>
-      </c>
-      <c r="B516">
+        <v>515</v>
+      </c>
+      <c r="B516" t="str">
         <f>bowtie!E517</f>
-        <v>0</v>
-      </c>
-      <c r="C516">
+        <v>not-impacted</v>
+      </c>
+      <c r="C516" t="str">
         <f>bowtie!C517</f>
-        <v>0</v>
+        <v>EB02</v>
       </c>
       <c r="D516">
         <f>bowtie!D517</f>
-        <v>0</v>
-      </c>
-      <c r="E516" t="str">
+        <v>60162</v>
+      </c>
+      <c r="E516">
         <f>IF(ISBLANK(bowtie!F517),"",bowtie!F517)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F516" t="str">
         <f>IF(ISBLANK(bowtie!G517),"",bowtie!G517)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G516" t="str">
         <f>IF(ISBLANK(bowtie!I517),"",bowtie!I517)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H516" t="str">
         <f>IF(ISBLANK(bowtie!J517),"",bowtie!J517)</f>
-        <v/>
+        <v>Status</v>
       </c>
       <c r="I516" t="str">
         <f>IF(ISBLANK(bowtie!H517),"",bowtie!H517)</f>
-        <v/>
+        <v>not impact hammer block no</v>
       </c>
       <c r="J516" t="str">
         <f>IF(ISBLANK(bowtie!K517),"",bowtie!K517)</f>
-        <v/>
-      </c>
-      <c r="K516" t="e">
+        <v>Used in Test hub for not impacted test outcome.</v>
+      </c>
+      <c r="K516" t="str">
         <f t="shared" si="22"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L516" t="e">
+        <v>{'id':515,'name':'not-impacted','unicode':'EB02','decimal':60162,'version':'1.1','style':'bold','subset':'VSTS','group':'Status','keywords':['not','impact','hammer','block','no'],'usage':'Used in Test hub for not impacted test outcome.'}</v>
+      </c>
+      <c r="L516" t="str">
         <f t="shared" si="23"/>
-        <v>#VALUE!</v>
+        <v>{"id":515,"name":"not-impacted","unicode":"EB02","decimal":60162,"version":"1.1","style":"bold","subset":"VSTS","group":"Status","keywords":["not","impact","hammer","block","no"],"usage":"Used in Test hub for not impacted test outcome."}</v>
       </c>
     </row>
     <row r="517" spans="1:12" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Added two more work item type icon
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5259" uniqueCount="2535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5277" uniqueCount="2539">
   <si>
     <t>name</t>
   </si>
@@ -7630,6 +7630,18 @@
   </si>
   <si>
     <t>Used in Build &amp; Relase hub for selecting build source.</t>
+  </si>
+  <si>
+    <t>symbol-issue</t>
+  </si>
+  <si>
+    <t>symbol-defect</t>
+  </si>
+  <si>
+    <t>symbol work item issue task exclamation</t>
+  </si>
+  <si>
+    <t>symbol work item defect lightbulb crack broken</t>
   </si>
 </sst>
 </file>
@@ -8131,7 +8143,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P525" sqref="P3:P525"/>
+      <selection pane="bottomLeft" activeCell="P527" sqref="P3:P527"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -34827,7 +34839,7 @@
         <v>1040</v>
       </c>
       <c r="L500" t="str">
-        <f t="shared" ref="L500:L525" si="26">CONCATENATE("u",E500,"-",D500,".svg")</f>
+        <f t="shared" ref="L500:L527" si="26">CONCATENATE("u",E500,"-",D500,".svg")</f>
         <v>uEAF1-search-and-apps.svg</v>
       </c>
       <c r="M500" s="17" t="s">
@@ -35959,7 +35971,7 @@
         <v>2525</v>
       </c>
       <c r="E522" s="19" t="str">
-        <f t="shared" ref="E522:E525" si="30">DEC2HEX(B522)</f>
+        <f t="shared" ref="E522:E527" si="30">DEC2HEX(B522)</f>
         <v>EB07</v>
       </c>
       <c r="F522" s="19">
@@ -36148,8 +36160,106 @@
         <v>{"decimal":"60170","namebowtie":"brand-jenkins","namemdl2":"null","codebowtie":"EB0A","codemdl2":"null"}</v>
       </c>
     </row>
-    <row r="526" spans="1:16" customFormat="1" ht="32.1" customHeight="1"/>
-    <row r="527" spans="1:16" customFormat="1" ht="32.1" customHeight="1"/>
+    <row r="526" spans="1:16" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A526" s="19">
+        <v>524</v>
+      </c>
+      <c r="B526" s="19">
+        <v>60171</v>
+      </c>
+      <c r="D526" s="19" t="s">
+        <v>2535</v>
+      </c>
+      <c r="E526" s="19" t="str">
+        <f t="shared" si="30"/>
+        <v>EB0B</v>
+      </c>
+      <c r="F526" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G526" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H526" t="s">
+        <v>2537</v>
+      </c>
+      <c r="I526" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J526" s="19" t="s">
+        <v>599</v>
+      </c>
+      <c r="K526" t="s">
+        <v>932</v>
+      </c>
+      <c r="L526" s="19" t="str">
+        <f t="shared" si="26"/>
+        <v>uEB0B-symbol-issue.svg</v>
+      </c>
+      <c r="M526" s="20" t="s">
+        <v>2515</v>
+      </c>
+      <c r="N526" s="19" t="s">
+        <v>2515</v>
+      </c>
+      <c r="O526" s="19" t="s">
+        <v>2515</v>
+      </c>
+      <c r="P526" s="19" t="str">
+        <f t="shared" ref="P526:P527" si="31">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",B526,"','namebowtie':'",D526,"','namemdl2':'",N526,"','codebowtie':'",E526,"','codemdl2':'",O526,"'}"),"'","""")</f>
+        <v>{"decimal":"60171","namebowtie":"symbol-issue","namemdl2":"null","codebowtie":"EB0B","codemdl2":"null"}</v>
+      </c>
+    </row>
+    <row r="527" spans="1:16" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A527" s="19">
+        <v>525</v>
+      </c>
+      <c r="B527" s="19">
+        <v>60172</v>
+      </c>
+      <c r="D527" s="19" t="s">
+        <v>2536</v>
+      </c>
+      <c r="E527" s="19" t="str">
+        <f t="shared" si="30"/>
+        <v>EB0C</v>
+      </c>
+      <c r="F527" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G527" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H527" t="s">
+        <v>2538</v>
+      </c>
+      <c r="I527" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J527" s="19" t="s">
+        <v>599</v>
+      </c>
+      <c r="K527" t="s">
+        <v>932</v>
+      </c>
+      <c r="L527" s="19" t="str">
+        <f t="shared" si="26"/>
+        <v>uEB0C-symbol-defect.svg</v>
+      </c>
+      <c r="M527" s="20" t="s">
+        <v>2515</v>
+      </c>
+      <c r="N527" s="19" t="s">
+        <v>2515</v>
+      </c>
+      <c r="O527" s="19" t="s">
+        <v>2515</v>
+      </c>
+      <c r="P527" s="19" t="str">
+        <f t="shared" si="31"/>
+        <v>{"decimal":"60172","namebowtie":"symbol-defect","namemdl2":"null","codebowtie":"EB0C","codemdl2":"null"}</v>
+      </c>
+    </row>
     <row r="528" spans="1:16" customFormat="1" ht="32.1" customHeight="1"/>
     <row r="529" customFormat="1" ht="32.1" customHeight="1"/>
     <row r="530" customFormat="1" ht="32.1" customHeight="1"/>
@@ -36171,7 +36281,7 @@
   <dimension ref="A1:L559"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L524" sqref="L2:L524"/>
+      <selection activeCell="L526" sqref="L2:L526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -61160,11 +61270,11 @@
         <v>An existing MDL2 icon. Used in VSTS when a work item is owned by another team and therefore you cannot reorder it.</v>
       </c>
       <c r="K500" t="str">
-        <f t="shared" ref="K500:K559" si="20">IF(NOT(ISBLANK(A500)),CONCATENATE("{'",$A$1,"':",A500,",'",$B$1,"':'",B500,"',","'",$C$1,"':'",C500,"','",$D$1,"':",D500,",'",$E$1,"':'",FIXED(E500,1),"','",$F$1,"':'",F500,"','",$G$1,"':'",G500,"','",$H$1,"':'",H500,"','",$I$1,"':['",SUBSTITUTE(I500," ","','"),"'],'",$J$1,"':'",J500,"'}"))</f>
+        <f t="shared" ref="K500:K507" si="20">IF(NOT(ISBLANK(A500)),CONCATENATE("{'",$A$1,"':",A500,",'",$B$1,"':'",B500,"',","'",$C$1,"':'",C500,"','",$D$1,"':",D500,",'",$E$1,"':'",FIXED(E500,1),"','",$F$1,"':'",F500,"','",$G$1,"':'",G500,"','",$H$1,"':'",H500,"','",$I$1,"':['",SUBSTITUTE(I500," ","','"),"'],'",$J$1,"':'",J500,"'}"))</f>
         <v>{'id':499,'name':'security-group','unicode':'EAF2','decimal':60146,'version':'1.1','style':'light','subset':'VSTS','group':'Work','keywords':['security','group','team','lock','ownership','user'],'usage':'An existing MDL2 icon. Used in VSTS when a work item is owned by another team and therefore you cannot reorder it.'}</v>
       </c>
       <c r="L500" t="str">
-        <f t="shared" ref="L500:L559" si="21">SUBSTITUTE(K500,"'","""")</f>
+        <f t="shared" ref="L500:L507" si="21">SUBSTITUTE(K500,"'","""")</f>
         <v>{"id":499,"name":"security-group","unicode":"EAF2","decimal":60146,"version":"1.1","style":"light","subset":"VSTS","group":"Work","keywords":["security","group","team","lock","ownership","user"],"usage":"An existing MDL2 icon. Used in VSTS when a work item is owned by another team and therefore you cannot reorder it."}</v>
       </c>
     </row>
@@ -61610,11 +61720,11 @@
         <v>Used in Build &amp; Release hub for Release definitions.</v>
       </c>
       <c r="K509" t="str">
-        <f t="shared" ref="K509:K536" si="24">IF(NOT(ISBLANK(A509)),CONCATENATE("{'",$A$1,"':",A509,",'",$B$1,"':'",B509,"',","'",$C$1,"':'",C509,"','",$D$1,"':",D509,",'",$E$1,"':'",FIXED(E509,1),"','",$F$1,"':'",F509,"','",$G$1,"':'",G509,"','",$H$1,"':'",H509,"','",$I$1,"':['",SUBSTITUTE(I509," ","','"),"'],'",$J$1,"':'",J509,"'}"))</f>
+        <f t="shared" ref="K509:K524" si="24">IF(NOT(ISBLANK(A509)),CONCATENATE("{'",$A$1,"':",A509,",'",$B$1,"':'",B509,"',","'",$C$1,"':'",C509,"','",$D$1,"':",D509,",'",$E$1,"':'",FIXED(E509,1),"','",$F$1,"':'",F509,"','",$G$1,"':'",G509,"','",$H$1,"':'",H509,"','",$I$1,"':['",SUBSTITUTE(I509," ","','"),"'],'",$J$1,"':'",J509,"'}"))</f>
         <v>{'id':508,'name':'rocket','unicode':'EAFB','decimal':60155,'version':'1.1','style':'light','subset':'VSTS','group':'Build','keywords':['rocket','launch','release'],'usage':'Used in Build &amp; Release hub for Release definitions.'}</v>
       </c>
       <c r="L509" t="str">
-        <f t="shared" ref="L509:L536" si="25">SUBSTITUTE(K509,"'","""")</f>
+        <f t="shared" ref="L509:L524" si="25">SUBSTITUTE(K509,"'","""")</f>
         <v>{"id":508,"name":"rocket","unicode":"EAFB","decimal":60155,"version":"1.1","style":"light","subset":"VSTS","group":"Build","keywords":["rocket","launch","release"],"usage":"Used in Build &amp; Release hub for Release definitions."}</v>
       </c>
     </row>
@@ -62371,101 +62481,101 @@
     <row r="525" spans="1:12">
       <c r="A525">
         <f>bowtie!A526</f>
-        <v>0</v>
-      </c>
-      <c r="B525">
+        <v>524</v>
+      </c>
+      <c r="B525" t="str">
         <f>bowtie!D526</f>
-        <v>0</v>
-      </c>
-      <c r="C525">
+        <v>symbol-issue</v>
+      </c>
+      <c r="C525" t="str">
         <f>bowtie!E526</f>
-        <v>0</v>
+        <v>EB0B</v>
       </c>
       <c r="D525">
         <f>bowtie!B526</f>
-        <v>0</v>
-      </c>
-      <c r="E525" t="str">
+        <v>60171</v>
+      </c>
+      <c r="E525">
         <f>IF(ISBLANK(bowtie!F526),"",bowtie!F526)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F525" t="str">
         <f>IF(ISBLANK(bowtie!G526),"",bowtie!G526)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G525" t="str">
         <f>IF(ISBLANK(bowtie!I526),"",bowtie!I526)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H525" t="str">
         <f>IF(ISBLANK(bowtie!J526),"",bowtie!J526)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="I525" t="str">
         <f>IF(ISBLANK(bowtie!H526),"",bowtie!H526)</f>
-        <v/>
+        <v>symbol work item issue task exclamation</v>
       </c>
       <c r="J525" t="str">
         <f>IF(ISBLANK(bowtie!K526),"",bowtie!K526)</f>
-        <v/>
-      </c>
-      <c r="K525" t="e">
+        <v>Work item type indicator.</v>
+      </c>
+      <c r="K525" t="str">
         <f t="shared" ref="K525:K559" si="26">IF(NOT(ISBLANK(A525)),CONCATENATE("{'",$A$1,"':",A525,",'",$B$1,"':'",B525,"',","'",$C$1,"':'",C525,"','",$D$1,"':",D525,",'",$E$1,"':'",FIXED(E525,1),"','",$F$1,"':'",F525,"','",$G$1,"':'",G525,"','",$H$1,"':'",H525,"','",$I$1,"':['",SUBSTITUTE(I525," ","','"),"'],'",$J$1,"':'",J525,"'}"))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L525" t="e">
+        <v>{'id':524,'name':'symbol-issue','unicode':'EB0B','decimal':60171,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['symbol','work','item','issue','task','exclamation'],'usage':'Work item type indicator.'}</v>
+      </c>
+      <c r="L525" t="str">
         <f t="shared" ref="L525:L559" si="27">SUBSTITUTE(K525,"'","""")</f>
-        <v>#VALUE!</v>
+        <v>{"id":524,"name":"symbol-issue","unicode":"EB0B","decimal":60171,"version":"1.1","style":"bold","subset":"VSTS","group":"Work","keywords":["symbol","work","item","issue","task","exclamation"],"usage":"Work item type indicator."}</v>
       </c>
     </row>
     <row r="526" spans="1:12">
       <c r="A526">
         <f>bowtie!A527</f>
-        <v>0</v>
-      </c>
-      <c r="B526">
+        <v>525</v>
+      </c>
+      <c r="B526" t="str">
         <f>bowtie!D527</f>
-        <v>0</v>
-      </c>
-      <c r="C526">
+        <v>symbol-defect</v>
+      </c>
+      <c r="C526" t="str">
         <f>bowtie!E527</f>
-        <v>0</v>
+        <v>EB0C</v>
       </c>
       <c r="D526">
         <f>bowtie!B527</f>
-        <v>0</v>
-      </c>
-      <c r="E526" t="str">
+        <v>60172</v>
+      </c>
+      <c r="E526">
         <f>IF(ISBLANK(bowtie!F527),"",bowtie!F527)</f>
-        <v/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F526" t="str">
         <f>IF(ISBLANK(bowtie!G527),"",bowtie!G527)</f>
-        <v/>
+        <v>bold</v>
       </c>
       <c r="G526" t="str">
         <f>IF(ISBLANK(bowtie!I527),"",bowtie!I527)</f>
-        <v/>
+        <v>VSTS</v>
       </c>
       <c r="H526" t="str">
         <f>IF(ISBLANK(bowtie!J527),"",bowtie!J527)</f>
-        <v/>
+        <v>Work</v>
       </c>
       <c r="I526" t="str">
         <f>IF(ISBLANK(bowtie!H527),"",bowtie!H527)</f>
-        <v/>
+        <v>symbol work item defect lightbulb crack broken</v>
       </c>
       <c r="J526" t="str">
         <f>IF(ISBLANK(bowtie!K527),"",bowtie!K527)</f>
-        <v/>
-      </c>
-      <c r="K526" t="e">
+        <v>Work item type indicator.</v>
+      </c>
+      <c r="K526" t="str">
         <f t="shared" si="26"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L526" t="e">
+        <v>{'id':525,'name':'symbol-defect','unicode':'EB0C','decimal':60172,'version':'1.1','style':'bold','subset':'VSTS','group':'Work','keywords':['symbol','work','item','defect','lightbulb','crack','broken'],'usage':'Work item type indicator.'}</v>
+      </c>
+      <c r="L526" t="str">
         <f t="shared" si="27"/>
-        <v>#VALUE!</v>
+        <v>{"id":525,"name":"symbol-defect","unicode":"EB0C","decimal":60172,"version":"1.1","style":"bold","subset":"VSTS","group":"Work","keywords":["symbol","work","item","defect","lightbulb","crack","broken"],"usage":"Work item type indicator."}</v>
       </c>
     </row>
     <row r="527" spans="1:12">

</xml_diff>

<commit_message>
Split gulp tasks into bite-size.
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -8114,9 +8114,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AH533"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A520" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J525" sqref="J525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -24343,7 +24343,7 @@
         <v>2499</v>
       </c>
       <c r="C349" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D349" t="str">
         <f t="shared" si="10"/>
@@ -24378,7 +24378,7 @@
       </c>
       <c r="N349" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>{"decimal":"59994","namebowtie":"locale-language","namemdl2":"WorldClock","codebowtie":"EA5A","codemdl2":"E918","stylevariation":"light","keywords":["web","globe","country","region","world","locale","language","letter","character"],"subset":"VSTS","group":"Profile","usagenotes":"Used for language preference on user profile page."}</v>
+        <v>{"decimal":"59994","namebowtie":"locale-timezone","namemdl2":"WorldClock","codebowtie":"EA5A","codemdl2":"E918","stylevariation":"light","keywords":["web","globe","country","region","world","locale","language","letter","character"],"subset":"VSTS","group":"Profile","usagenotes":"Used for language preference on user profile page."}</v>
       </c>
     </row>
     <row r="350" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
@@ -24389,7 +24389,7 @@
         <v>2499</v>
       </c>
       <c r="C350" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D350" t="str">
         <f t="shared" si="10"/>
@@ -24424,7 +24424,7 @@
       </c>
       <c r="N350" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>{"decimal":"59995","namebowtie":"locale-timezone","namemdl2":"LocaleLanguage","codebowtie":"EA5B","codemdl2":"F2B7","stylevariation":"light","keywords":["web","globe","country","region","world","timezone","time","clock"],"subset":"VSTS","group":"Profile","usagenotes":"Used for timezone preference on user profile page."}</v>
+        <v>{"decimal":"59995","namebowtie":"locale-language","namemdl2":"LocaleLanguage","codebowtie":"EA5B","codemdl2":"F2B7","stylevariation":"light","keywords":["web","globe","country","region","world","timezone","time","clock"],"subset":"VSTS","group":"Profile","usagenotes":"Used for timezone preference on user profile page."}</v>
       </c>
     </row>
     <row r="351" spans="1:14" customFormat="1" ht="32.1" customHeight="1">

</xml_diff>

<commit_message>
Added login icon for credentials
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cherrw\Dropbox\Code\vsfi\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwang\Dropbox\Code\vsfi\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5264" uniqueCount="2531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5273" uniqueCount="2534">
   <si>
     <t>keywords</t>
   </si>
@@ -7617,6 +7617,15 @@
   </si>
   <si>
     <t>{"decimal":"59648","namebowtie":"arrow-up","namemdl2":"Up","codebowtie":"E900","codemdl2":"E74A","stylevariation":"light","keywords":["arrow","up"],"subset":"VSTS","group":"Arrow","usagenotes":"Indicate direction, movement."}</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>login account credential user password lock security</t>
+  </si>
+  <si>
+    <t>Used in top nav Credentials command.</t>
   </si>
 </sst>
 </file>
@@ -8116,7 +8125,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A520" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J525" sqref="J525"/>
+      <selection pane="bottomLeft" activeCell="C528" sqref="C528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -32292,7 +32301,7 @@
         <v>2509</v>
       </c>
       <c r="D522" s="18" t="str">
-        <f t="shared" ref="D522:D527" si="17">DEC2HEX(A522)</f>
+        <f t="shared" ref="D522:D528" si="17">DEC2HEX(A522)</f>
         <v>EB07</v>
       </c>
       <c r="E522" s="18">
@@ -32542,7 +32551,49 @@
         <v>{"decimal":"60172","namebowtie":"symbol-defect","namemdl2":"null","codebowtie":"EB0C","codemdl2":"null","stylevariation":"bold","keywords":["symbol","work","item","defect","lightbulb","crack","broken"],"subset":"VSTS","group":"Work","usagenotes":"Work item type indicator."}</v>
       </c>
     </row>
-    <row r="528" spans="1:14" customFormat="1" ht="32.1" customHeight="1"/>
+    <row r="528" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A528" s="18">
+        <v>60173</v>
+      </c>
+      <c r="C528" s="18" t="s">
+        <v>2531</v>
+      </c>
+      <c r="D528" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>EB0D</v>
+      </c>
+      <c r="E528" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F528" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G528" s="18" t="s">
+        <v>2532</v>
+      </c>
+      <c r="H528" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I528" s="18" t="s">
+        <v>584</v>
+      </c>
+      <c r="J528" s="18" t="s">
+        <v>2533</v>
+      </c>
+      <c r="K528" s="19" t="s">
+        <v>2499</v>
+      </c>
+      <c r="L528" s="18" t="s">
+        <v>2499</v>
+      </c>
+      <c r="M528" s="18" t="s">
+        <v>2499</v>
+      </c>
+      <c r="N528" s="14" t="str">
+        <f t="shared" ref="N528" si="18">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A528,"','namebowtie':'",C528,"','namemdl2':'",L528,"','codebowtie':'",D528,"','codemdl2':'",M528,"','stylevariation':'",F528,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G528,"']")," ","','"),"'",""""),",'subset':'",H528,"','group':'",I528,"','usagenotes':'",J528,"'}"),"'","""")</f>
+        <v>{"decimal":"60173","namebowtie":"login","namemdl2":"null","codebowtie":"EB0D","codemdl2":"null","stylevariation":"light","keywords":["login","account","credential","user","password","lock","security"],"subset":"VSTS","group":"Common","usagenotes":"Used in top nav Credentials command."}</v>
+      </c>
+    </row>
     <row r="529" customFormat="1" ht="32.1" customHeight="1"/>
     <row r="530" customFormat="1" ht="32.1" customHeight="1"/>
     <row r="531" customFormat="1" ht="32.1" customHeight="1"/>

</xml_diff>

<commit_message>
Added mapping info for new icons added to Fabric MDL2
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="bowtie" sheetId="2" r:id="rId1"/>
     <sheet name="brands need clearance" sheetId="3" r:id="rId2"/>
-    <sheet name="20140804 request sent to Chieu" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bowtie!$A$2:$N$529</definedName>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5410" uniqueCount="2611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5326" uniqueCount="2624">
   <si>
     <t>keywords</t>
   </si>
@@ -7525,9 +7524,6 @@
     <t>null</t>
   </si>
   <si>
-    <t>backlog-board</t>
-  </si>
-  <si>
     <t>Used in Work hub for Board view.</t>
   </si>
   <si>
@@ -7753,12 +7749,6 @@
     <t>E919</t>
   </si>
   <si>
-    <t>E91A</t>
-  </si>
-  <si>
-    <t>E91B</t>
-  </si>
-  <si>
     <t>E91C</t>
   </si>
   <si>
@@ -7774,94 +7764,142 @@
     <t></t>
   </si>
   <si>
-    <t>Other notes</t>
-  </si>
-  <si>
-    <t>Need to match the hammer in "TestImpactSolid (F3AA)"</t>
-  </si>
-  <si>
-    <t>Need to match "Backlog (F2AC)"</t>
-  </si>
-  <si>
-    <t>Need to match "Build (F28F)"</t>
-  </si>
-  <si>
-    <t>Need to match other "Field" icons in (F2C1, F2C2, F2C3, F2C4)</t>
-  </si>
-  <si>
-    <t>1st party brand. Ok to add to MDL2.</t>
-  </si>
-  <si>
-    <t>Need to match "TaskSolid (F333)"</t>
-  </si>
-  <si>
-    <t>Need to match other solid icons because these are used for accessibility</t>
-  </si>
-  <si>
     <t>EB07</t>
   </si>
   <si>
     <t>EB0A</t>
   </si>
   <si>
-    <t>EB00</t>
-  </si>
-  <si>
-    <t>EB01</t>
-  </si>
-  <si>
-    <t>EB02</t>
-  </si>
-  <si>
-    <t>EB03</t>
-  </si>
-  <si>
-    <t>EB04</t>
-  </si>
-  <si>
-    <t>EB06</t>
-  </si>
-  <si>
-    <t>EB09</t>
-  </si>
-  <si>
-    <t>EB0B</t>
-  </si>
-  <si>
-    <t>EB0C</t>
-  </si>
-  <si>
-    <t>EB0D</t>
-  </si>
-  <si>
-    <t>EB0E</t>
-  </si>
-  <si>
-    <t>First party brand. OK to add to MDL2.</t>
-  </si>
-  <si>
-    <t>Microsoft Test Manager logo.</t>
-  </si>
-  <si>
-    <t>NuGet logo.</t>
-  </si>
-  <si>
-    <t>Team Foundation Version Control logo.</t>
-  </si>
-  <si>
-    <t>Feel free to adjust proportion. We just need an icon to indicate "user login credentials".</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
     <t>We've gotten permission before but I can't find the email thread.</t>
   </si>
   <si>
-    <t>Not sure if Full MDL2 already has an icon for "locked file" if so please just add to Fabric MDL2.</t>
-  </si>
-  <si>
-    <t>Need to match "Play (E768)"</t>
+    <t>board</t>
+  </si>
+  <si>
+    <t>F444</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>BacklogBoard</t>
+  </si>
+  <si>
+    <t>F43F</t>
+  </si>
+  <si>
+    <t>PageLock</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>F440</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>NotExecuted</t>
+  </si>
+  <si>
+    <t>F441</t>
+  </si>
+  <si>
+    <t>NotImpactedSolid</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>F442</t>
+  </si>
+  <si>
+    <t>FieldReadOnly</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>F443</t>
+  </si>
+  <si>
+    <t>FieldRequired</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>ExternalBuild</t>
+  </si>
+  <si>
+    <t>F445</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>ExternalTFVC</t>
+  </si>
+  <si>
+    <t>F446</t>
+  </si>
+  <si>
+    <t>F447</t>
+  </si>
+  <si>
+    <t>ExternalXAML</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>F448</t>
+  </si>
+  <si>
+    <t>IssueSolid</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>F449</t>
+  </si>
+  <si>
+    <t>DefectSolid</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>F44A</t>
+  </si>
+  <si>
+    <t>LadybugSolid</t>
+  </si>
+  <si>
+    <t>F427</t>
+  </si>
+  <si>
+    <t>IDBadge</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>EF74</t>
+  </si>
+  <si>
+    <t>GroupedList</t>
+  </si>
+  <si>
+    <t></t>
   </si>
 </sst>
 </file>
@@ -7871,7 +7909,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7934,17 +7972,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -8036,10 +8079,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -8061,17 +8100,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -8081,6 +8114,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -8403,9 +8442,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AH533"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D525" sqref="D525"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -8414,10 +8453,10 @@
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="26.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="16" style="3" customWidth="1"/>
-    <col min="6" max="6" width="24" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" style="2" customWidth="1"/>
-    <col min="8" max="9" width="14.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="14.28515625" style="2" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="28" style="2" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
     <col min="12" max="12" width="28.28515625" customWidth="1"/>
@@ -8488,16 +8527,16 @@
         <v>2496</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>2523</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>2524</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>2525</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>82</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>0</v>
@@ -8509,19 +8548,19 @@
         <v>168</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>2455</v>
       </c>
       <c r="L2" s="8" t="s">
+        <v>2525</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>2526</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>2527</v>
-      </c>
       <c r="N2" s="8" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="O2"/>
       <c r="P2"/>
@@ -8579,10 +8618,10 @@
       <c r="K3" s="16" t="s">
         <v>2454</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="19" t="s">
         <v>2452</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="19" t="s">
         <v>2453</v>
       </c>
       <c r="N3" s="14" t="str">
@@ -8591,7 +8630,7 @@
       </c>
       <c r="O3" s="14"/>
       <c r="P3" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="32.1" customHeight="1">
@@ -8629,10 +8668,10 @@
       <c r="K4" s="16" t="s">
         <v>2451</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="19" t="s">
         <v>2449</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="19" t="s">
         <v>2450</v>
       </c>
       <c r="N4" s="14" t="str">
@@ -8675,10 +8714,10 @@
       <c r="K5" s="16" t="s">
         <v>2448</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="19" t="s">
         <v>2446</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="19" t="s">
         <v>2447</v>
       </c>
       <c r="N5" s="14" t="str">
@@ -8721,10 +8760,10 @@
       <c r="K6" s="16" t="s">
         <v>2445</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="19" t="s">
         <v>2443</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="19" t="s">
         <v>2444</v>
       </c>
       <c r="N6" s="14" t="str">
@@ -9017,10 +9056,10 @@
       <c r="K12" s="16" t="s">
         <v>2427</v>
       </c>
-      <c r="L12" s="21" t="s">
+      <c r="L12" s="19" t="s">
         <v>2425</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="M12" s="19" t="s">
         <v>2426</v>
       </c>
       <c r="N12" s="14" t="str">
@@ -9063,10 +9102,10 @@
       <c r="K13" s="16" t="s">
         <v>2424</v>
       </c>
-      <c r="L13" s="21" t="s">
+      <c r="L13" s="19" t="s">
         <v>2422</v>
       </c>
-      <c r="M13" s="21" t="s">
+      <c r="M13" s="19" t="s">
         <v>2423</v>
       </c>
       <c r="N13" s="14" t="str">
@@ -9129,10 +9168,10 @@
       <c r="K14" s="16" t="s">
         <v>2421</v>
       </c>
-      <c r="L14" s="21" t="s">
+      <c r="L14" s="19" t="s">
         <v>2419</v>
       </c>
-      <c r="M14" s="21" t="s">
+      <c r="M14" s="19" t="s">
         <v>2420</v>
       </c>
       <c r="N14" s="14" t="str">
@@ -9175,10 +9214,10 @@
       <c r="K15" s="16" t="s">
         <v>2418</v>
       </c>
-      <c r="L15" s="21" t="s">
+      <c r="L15" s="19" t="s">
         <v>2416</v>
       </c>
-      <c r="M15" s="21" t="s">
+      <c r="M15" s="19" t="s">
         <v>2417</v>
       </c>
       <c r="N15" s="14" t="str">
@@ -9221,10 +9260,10 @@
       <c r="K16" s="16" t="s">
         <v>2415</v>
       </c>
-      <c r="L16" s="21" t="s">
+      <c r="L16" s="19" t="s">
         <v>2413</v>
       </c>
-      <c r="M16" s="21" t="s">
+      <c r="M16" s="19" t="s">
         <v>2414</v>
       </c>
       <c r="N16" s="14" t="str">
@@ -9267,10 +9306,10 @@
       <c r="K17" s="16" t="s">
         <v>2412</v>
       </c>
-      <c r="L17" s="21" t="s">
+      <c r="L17" s="19" t="s">
         <v>2410</v>
       </c>
-      <c r="M17" s="21" t="s">
+      <c r="M17" s="19" t="s">
         <v>2411</v>
       </c>
       <c r="N17" s="14" t="str">
@@ -9313,10 +9352,10 @@
       <c r="K18" s="16" t="s">
         <v>2409</v>
       </c>
-      <c r="L18" s="21" t="s">
+      <c r="L18" s="19" t="s">
         <v>2407</v>
       </c>
-      <c r="M18" s="21" t="s">
+      <c r="M18" s="19" t="s">
         <v>2408</v>
       </c>
       <c r="N18" s="14" t="str">
@@ -9359,10 +9398,10 @@
       <c r="K19" s="16" t="s">
         <v>2314</v>
       </c>
-      <c r="L19" s="21" t="s">
+      <c r="L19" s="19" t="s">
         <v>2312</v>
       </c>
-      <c r="M19" s="21" t="s">
+      <c r="M19" s="19" t="s">
         <v>2313</v>
       </c>
       <c r="N19" s="14" t="str">
@@ -9497,10 +9536,10 @@
       <c r="K22" s="16" t="s">
         <v>2400</v>
       </c>
-      <c r="L22" s="21" t="s">
+      <c r="L22" s="19" t="s">
         <v>2398</v>
       </c>
-      <c r="M22" s="21" t="s">
+      <c r="M22" s="19" t="s">
         <v>2399</v>
       </c>
       <c r="N22" s="14" t="str">
@@ -9543,10 +9582,10 @@
       <c r="K23" s="16" t="s">
         <v>2397</v>
       </c>
-      <c r="L23" s="21" t="s">
+      <c r="L23" s="19" t="s">
         <v>2395</v>
       </c>
-      <c r="M23" s="21" t="s">
+      <c r="M23" s="19" t="s">
         <v>2396</v>
       </c>
       <c r="N23" s="14" t="str">
@@ -9931,10 +9970,10 @@
       <c r="K31" s="16" t="s">
         <v>2497</v>
       </c>
-      <c r="L31" s="21" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M31" s="21" t="s">
+      <c r="L31" s="19" t="s">
+        <v>2497</v>
+      </c>
+      <c r="M31" s="19" t="s">
         <v>2497</v>
       </c>
       <c r="N31" s="14" t="str">
@@ -9977,10 +10016,10 @@
       <c r="K32" s="16" t="s">
         <v>2391</v>
       </c>
-      <c r="L32" s="21" t="s">
+      <c r="L32" s="19" t="s">
         <v>2389</v>
       </c>
-      <c r="M32" s="21" t="s">
+      <c r="M32" s="19" t="s">
         <v>2390</v>
       </c>
       <c r="N32" s="14" t="str">
@@ -10023,10 +10062,10 @@
       <c r="K33" s="16" t="s">
         <v>2394</v>
       </c>
-      <c r="L33" s="21" t="s">
+      <c r="L33" s="19" t="s">
         <v>2392</v>
       </c>
-      <c r="M33" s="21" t="s">
+      <c r="M33" s="19" t="s">
         <v>2393</v>
       </c>
       <c r="N33" s="14" t="str">
@@ -10115,10 +10154,10 @@
       <c r="K35" s="16" t="s">
         <v>2391</v>
       </c>
-      <c r="L35" s="21" t="s">
+      <c r="L35" s="19" t="s">
         <v>2389</v>
       </c>
-      <c r="M35" s="21" t="s">
+      <c r="M35" s="19" t="s">
         <v>2390</v>
       </c>
       <c r="N35" s="14" t="str">
@@ -10227,10 +10266,10 @@
       <c r="K37" s="16" t="s">
         <v>2388</v>
       </c>
-      <c r="L37" s="21" t="s">
+      <c r="L37" s="19" t="s">
         <v>2386</v>
       </c>
-      <c r="M37" s="21" t="s">
+      <c r="M37" s="19" t="s">
         <v>2387</v>
       </c>
       <c r="N37" s="14" t="str">
@@ -10273,10 +10312,10 @@
       <c r="K38" s="16" t="s">
         <v>2385</v>
       </c>
-      <c r="L38" s="21" t="s">
+      <c r="L38" s="19" t="s">
         <v>2383</v>
       </c>
-      <c r="M38" s="21" t="s">
+      <c r="M38" s="19" t="s">
         <v>2384</v>
       </c>
       <c r="N38" s="14" t="str">
@@ -10319,10 +10358,10 @@
       <c r="K39" s="16" t="s">
         <v>2382</v>
       </c>
-      <c r="L39" s="21" t="s">
+      <c r="L39" s="19" t="s">
         <v>2380</v>
       </c>
-      <c r="M39" s="21" t="s">
+      <c r="M39" s="19" t="s">
         <v>2381</v>
       </c>
       <c r="N39" s="14" t="str">
@@ -10365,10 +10404,10 @@
       <c r="K40" s="16" t="s">
         <v>2379</v>
       </c>
-      <c r="L40" s="21" t="s">
+      <c r="L40" s="19" t="s">
         <v>2377</v>
       </c>
-      <c r="M40" s="21" t="s">
+      <c r="M40" s="19" t="s">
         <v>2378</v>
       </c>
       <c r="N40" s="14" t="str">
@@ -10408,13 +10447,13 @@
       <c r="J41" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="K41" s="22" t="s">
+      <c r="K41" s="20" t="s">
         <v>2376</v>
       </c>
-      <c r="L41" s="21" t="s">
+      <c r="L41" s="19" t="s">
         <v>2374</v>
       </c>
-      <c r="M41" s="21" t="s">
+      <c r="M41" s="19" t="s">
         <v>2375</v>
       </c>
       <c r="N41" s="14" t="str">
@@ -10457,10 +10496,10 @@
       <c r="K42" s="16" t="s">
         <v>2373</v>
       </c>
-      <c r="L42" s="21" t="s">
+      <c r="L42" s="19" t="s">
         <v>2371</v>
       </c>
-      <c r="M42" s="21" t="s">
+      <c r="M42" s="19" t="s">
         <v>2372</v>
       </c>
       <c r="N42" s="14" t="str">
@@ -10503,10 +10542,10 @@
       <c r="K43" s="16" t="s">
         <v>2370</v>
       </c>
-      <c r="L43" s="21" t="s">
+      <c r="L43" s="19" t="s">
         <v>2368</v>
       </c>
-      <c r="M43" s="21" t="s">
+      <c r="M43" s="19" t="s">
         <v>2369</v>
       </c>
       <c r="N43" s="14" t="str">
@@ -10549,10 +10588,10 @@
       <c r="K44" s="16" t="s">
         <v>2367</v>
       </c>
-      <c r="L44" s="21" t="s">
+      <c r="L44" s="19" t="s">
         <v>2365</v>
       </c>
-      <c r="M44" s="21" t="s">
+      <c r="M44" s="19" t="s">
         <v>2366</v>
       </c>
       <c r="N44" s="14" t="str">
@@ -10595,10 +10634,10 @@
       <c r="K45" s="16" t="s">
         <v>2364</v>
       </c>
-      <c r="L45" s="21" t="s">
+      <c r="L45" s="19" t="s">
         <v>2362</v>
       </c>
-      <c r="M45" s="21" t="s">
+      <c r="M45" s="19" t="s">
         <v>2363</v>
       </c>
       <c r="N45" s="14" t="str">
@@ -10641,10 +10680,10 @@
       <c r="K46" s="16" t="s">
         <v>2361</v>
       </c>
-      <c r="L46" s="21" t="s">
+      <c r="L46" s="19" t="s">
         <v>2359</v>
       </c>
-      <c r="M46" s="21" t="s">
+      <c r="M46" s="19" t="s">
         <v>2360</v>
       </c>
       <c r="N46" s="14" t="str">
@@ -10657,7 +10696,7 @@
         <v>59692</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>261</v>
@@ -10687,10 +10726,10 @@
       <c r="K47" s="16" t="s">
         <v>2358</v>
       </c>
-      <c r="L47" s="21" t="s">
+      <c r="L47" s="19" t="s">
         <v>2356</v>
       </c>
-      <c r="M47" s="21" t="s">
+      <c r="M47" s="19" t="s">
         <v>2357</v>
       </c>
       <c r="N47" s="14" t="str">
@@ -10703,7 +10742,7 @@
         <v>59693</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>141</v>
@@ -10749,7 +10788,7 @@
         <v>59694</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>262</v>
@@ -10795,7 +10834,7 @@
         <v>59695</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>263</v>
@@ -10825,10 +10864,10 @@
       <c r="K50" s="16" t="s">
         <v>2349</v>
       </c>
-      <c r="L50" s="21" t="s">
+      <c r="L50" s="19" t="s">
         <v>2347</v>
       </c>
-      <c r="M50" s="21" t="s">
+      <c r="M50" s="19" t="s">
         <v>2348</v>
       </c>
       <c r="N50" s="14" t="str">
@@ -10871,10 +10910,10 @@
       <c r="K51" s="16" t="s">
         <v>2346</v>
       </c>
-      <c r="L51" s="21" t="s">
+      <c r="L51" s="19" t="s">
         <v>2344</v>
       </c>
-      <c r="M51" s="21" t="s">
+      <c r="M51" s="19" t="s">
         <v>2345</v>
       </c>
       <c r="N51" s="14" t="str">
@@ -10887,7 +10926,7 @@
         <v>59697</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>265</v>
@@ -10933,7 +10972,7 @@
         <v>59698</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>266</v>
@@ -10963,10 +11002,10 @@
       <c r="K53" s="16" t="s">
         <v>2340</v>
       </c>
-      <c r="L53" s="21" t="s">
+      <c r="L53" s="19" t="s">
         <v>2338</v>
       </c>
-      <c r="M53" s="21" t="s">
+      <c r="M53" s="19" t="s">
         <v>2339</v>
       </c>
       <c r="N53" s="14" t="str">
@@ -10979,7 +11018,7 @@
         <v>59699</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>267</v>
@@ -11025,7 +11064,7 @@
         <v>59700</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>268</v>
@@ -11058,7 +11097,7 @@
       <c r="L55" s="15" t="s">
         <v>2332</v>
       </c>
-      <c r="M55" s="21" t="s">
+      <c r="M55" s="19" t="s">
         <v>2333</v>
       </c>
       <c r="N55" s="14" t="str">
@@ -11071,7 +11110,7 @@
         <v>59701</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>269</v>
@@ -11101,10 +11140,10 @@
       <c r="K56" s="16" t="s">
         <v>2331</v>
       </c>
-      <c r="L56" s="21" t="s">
+      <c r="L56" s="19" t="s">
         <v>2329</v>
       </c>
-      <c r="M56" s="21" t="s">
+      <c r="M56" s="19" t="s">
         <v>2330</v>
       </c>
       <c r="N56" s="14" t="str">
@@ -11117,7 +11156,7 @@
         <v>59702</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>270</v>
@@ -11147,10 +11186,10 @@
       <c r="K57" s="16" t="s">
         <v>2328</v>
       </c>
-      <c r="L57" s="21" t="s">
+      <c r="L57" s="19" t="s">
         <v>2326</v>
       </c>
-      <c r="M57" s="21" t="s">
+      <c r="M57" s="19" t="s">
         <v>2327</v>
       </c>
       <c r="N57" s="14" t="str">
@@ -11163,7 +11202,7 @@
         <v>59703</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>271</v>
@@ -11193,10 +11232,10 @@
       <c r="K58" s="16" t="s">
         <v>2325</v>
       </c>
-      <c r="L58" s="21" t="s">
+      <c r="L58" s="19" t="s">
         <v>2323</v>
       </c>
-      <c r="M58" s="21" t="s">
+      <c r="M58" s="19" t="s">
         <v>2324</v>
       </c>
       <c r="N58" s="14" t="str">
@@ -11209,7 +11248,7 @@
         <v>59704</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>272</v>
@@ -11239,10 +11278,10 @@
       <c r="K59" s="16" t="s">
         <v>2322</v>
       </c>
-      <c r="L59" s="21" t="s">
+      <c r="L59" s="19" t="s">
         <v>2320</v>
       </c>
-      <c r="M59" s="21" t="s">
+      <c r="M59" s="19" t="s">
         <v>2321</v>
       </c>
       <c r="N59" s="14" t="str">
@@ -11255,7 +11294,7 @@
         <v>59705</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>32</v>
@@ -11285,10 +11324,10 @@
       <c r="K60" s="16" t="s">
         <v>2319</v>
       </c>
-      <c r="L60" s="21" t="s">
+      <c r="L60" s="19" t="s">
         <v>583</v>
       </c>
-      <c r="M60" s="21" t="s">
+      <c r="M60" s="19" t="s">
         <v>2318</v>
       </c>
       <c r="N60" s="14" t="str">
@@ -11301,7 +11340,7 @@
         <v>59706</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>273</v>
@@ -11331,10 +11370,10 @@
       <c r="K61" s="16" t="s">
         <v>2317</v>
       </c>
-      <c r="L61" s="21" t="s">
+      <c r="L61" s="19" t="s">
         <v>2315</v>
       </c>
-      <c r="M61" s="21" t="s">
+      <c r="M61" s="19" t="s">
         <v>2316</v>
       </c>
       <c r="N61" s="14" t="str">
@@ -11347,7 +11386,7 @@
         <v>59707</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>274</v>
@@ -11377,10 +11416,10 @@
       <c r="K62" s="16" t="s">
         <v>2314</v>
       </c>
-      <c r="L62" s="21" t="s">
+      <c r="L62" s="19" t="s">
         <v>2312</v>
       </c>
-      <c r="M62" s="21" t="s">
+      <c r="M62" s="19" t="s">
         <v>2313</v>
       </c>
       <c r="N62" s="14" t="str">
@@ -11393,7 +11432,7 @@
         <v>59708</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>275</v>
@@ -11426,7 +11465,7 @@
       <c r="L63" s="15" t="s">
         <v>2309</v>
       </c>
-      <c r="M63" s="21" t="s">
+      <c r="M63" s="19" t="s">
         <v>2310</v>
       </c>
       <c r="N63" s="14" t="str">
@@ -11439,7 +11478,7 @@
         <v>59709</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>276</v>
@@ -11469,10 +11508,10 @@
       <c r="K64" s="16" t="s">
         <v>2308</v>
       </c>
-      <c r="L64" s="21" t="s">
+      <c r="L64" s="19" t="s">
         <v>2306</v>
       </c>
-      <c r="M64" s="21" t="s">
+      <c r="M64" s="19" t="s">
         <v>2307</v>
       </c>
       <c r="N64" s="14" t="str">
@@ -11531,7 +11570,7 @@
         <v>59711</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>278</v>
@@ -11577,7 +11616,7 @@
         <v>59712</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>279</v>
@@ -11623,7 +11662,7 @@
         <v>59713</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>280</v>
@@ -11669,7 +11708,7 @@
         <v>59714</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>281</v>
@@ -11745,10 +11784,10 @@
       <c r="K70" s="16" t="s">
         <v>2299</v>
       </c>
-      <c r="L70" s="21" t="s">
+      <c r="L70" s="19" t="s">
         <v>2297</v>
       </c>
-      <c r="M70" s="21" t="s">
+      <c r="M70" s="19" t="s">
         <v>2298</v>
       </c>
       <c r="N70" s="14" t="str">
@@ -11761,7 +11800,7 @@
         <v>59716</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>283</v>
@@ -11903,10 +11942,10 @@
       <c r="K73" s="16" t="s">
         <v>2293</v>
       </c>
-      <c r="L73" s="21" t="s">
+      <c r="L73" s="19" t="s">
         <v>2291</v>
       </c>
-      <c r="M73" s="21" t="s">
+      <c r="M73" s="19" t="s">
         <v>2292</v>
       </c>
       <c r="N73" s="14" t="str">
@@ -11949,10 +11988,10 @@
       <c r="K74" s="16" t="s">
         <v>2290</v>
       </c>
-      <c r="L74" s="21" t="s">
+      <c r="L74" s="19" t="s">
         <v>2288</v>
       </c>
-      <c r="M74" s="21" t="s">
+      <c r="M74" s="19" t="s">
         <v>2289</v>
       </c>
       <c r="N74" s="14" t="str">
@@ -11995,10 +12034,10 @@
       <c r="K75" s="16" t="s">
         <v>2287</v>
       </c>
-      <c r="L75" s="21" t="s">
+      <c r="L75" s="19" t="s">
         <v>2285</v>
       </c>
-      <c r="M75" s="21" t="s">
+      <c r="M75" s="19" t="s">
         <v>2286</v>
       </c>
       <c r="N75" s="14" t="str">
@@ -12057,7 +12096,7 @@
         <v>59722</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>289</v>
@@ -12087,10 +12126,10 @@
       <c r="K77" s="16" t="s">
         <v>2284</v>
       </c>
-      <c r="L77" s="21" t="s">
+      <c r="L77" s="19" t="s">
         <v>2282</v>
       </c>
-      <c r="M77" s="21" t="s">
+      <c r="M77" s="19" t="s">
         <v>2283</v>
       </c>
       <c r="N77" s="14" t="str">
@@ -12179,10 +12218,10 @@
       <c r="K79" s="16" t="s">
         <v>2278</v>
       </c>
-      <c r="L79" s="21" t="s">
+      <c r="L79" s="19" t="s">
         <v>2276</v>
       </c>
-      <c r="M79" s="21" t="s">
+      <c r="M79" s="19" t="s">
         <v>2277</v>
       </c>
       <c r="N79" s="14" t="str">
@@ -12225,10 +12264,10 @@
       <c r="K80" s="16" t="s">
         <v>2275</v>
       </c>
-      <c r="L80" s="21" t="s">
+      <c r="L80" s="19" t="s">
         <v>2273</v>
       </c>
-      <c r="M80" s="21" t="s">
+      <c r="M80" s="19" t="s">
         <v>2274</v>
       </c>
       <c r="N80" s="14" t="str">
@@ -12271,10 +12310,10 @@
       <c r="K81" s="16" t="s">
         <v>2272</v>
       </c>
-      <c r="L81" s="21" t="s">
+      <c r="L81" s="19" t="s">
         <v>2270</v>
       </c>
-      <c r="M81" s="21" t="s">
+      <c r="M81" s="19" t="s">
         <v>2271</v>
       </c>
       <c r="N81" s="14" t="str">
@@ -12429,10 +12468,10 @@
       <c r="K84" s="16" t="s">
         <v>2269</v>
       </c>
-      <c r="L84" s="21" t="s">
+      <c r="L84" s="19" t="s">
         <v>2267</v>
       </c>
-      <c r="M84" s="21" t="s">
+      <c r="M84" s="19" t="s">
         <v>2268</v>
       </c>
       <c r="N84" s="14" t="str">
@@ -12475,10 +12514,10 @@
       <c r="K85" s="16" t="s">
         <v>1674</v>
       </c>
-      <c r="L85" s="21" t="s">
+      <c r="L85" s="19" t="s">
         <v>1672</v>
       </c>
-      <c r="M85" s="21" t="s">
+      <c r="M85" s="19" t="s">
         <v>1673</v>
       </c>
       <c r="N85" s="14" t="str">
@@ -12521,10 +12560,10 @@
       <c r="K86" s="16" t="s">
         <v>2266</v>
       </c>
-      <c r="L86" s="21" t="s">
+      <c r="L86" s="19" t="s">
         <v>2264</v>
       </c>
-      <c r="M86" s="21" t="s">
+      <c r="M86" s="19" t="s">
         <v>2265</v>
       </c>
       <c r="N86" s="14" t="str">
@@ -12567,10 +12606,10 @@
       <c r="K87" s="16" t="s">
         <v>2263</v>
       </c>
-      <c r="L87" s="21" t="s">
+      <c r="L87" s="19" t="s">
         <v>2261</v>
       </c>
-      <c r="M87" s="21" t="s">
+      <c r="M87" s="19" t="s">
         <v>2262</v>
       </c>
       <c r="N87" s="14" t="str">
@@ -12705,10 +12744,10 @@
       <c r="K90" s="16" t="s">
         <v>2254</v>
       </c>
-      <c r="L90" s="21" t="s">
+      <c r="L90" s="19" t="s">
         <v>2252</v>
       </c>
-      <c r="M90" s="21" t="s">
+      <c r="M90" s="19" t="s">
         <v>2253</v>
       </c>
       <c r="N90" s="14" t="str">
@@ -13093,10 +13132,10 @@
       <c r="K98" s="16" t="s">
         <v>2233</v>
       </c>
-      <c r="L98" s="21" t="s">
+      <c r="L98" s="19" t="s">
         <v>2231</v>
       </c>
-      <c r="M98" s="21" t="s">
+      <c r="M98" s="19" t="s">
         <v>2232</v>
       </c>
       <c r="N98" s="14" t="str">
@@ -13139,10 +13178,10 @@
       <c r="K99" s="16" t="s">
         <v>2230</v>
       </c>
-      <c r="L99" s="21" t="s">
+      <c r="L99" s="19" t="s">
         <v>2228</v>
       </c>
-      <c r="M99" s="21" t="s">
+      <c r="M99" s="19" t="s">
         <v>2229</v>
       </c>
       <c r="N99" s="14" t="str">
@@ -13185,10 +13224,10 @@
       <c r="K100" s="16" t="s">
         <v>2227</v>
       </c>
-      <c r="L100" s="21" t="s">
+      <c r="L100" s="19" t="s">
         <v>2225</v>
       </c>
-      <c r="M100" s="21" t="s">
+      <c r="M100" s="19" t="s">
         <v>2226</v>
       </c>
       <c r="N100" s="14" t="str">
@@ -13277,10 +13316,10 @@
       <c r="K102" s="16" t="s">
         <v>2221</v>
       </c>
-      <c r="L102" s="21" t="s">
+      <c r="L102" s="19" t="s">
         <v>2219</v>
       </c>
-      <c r="M102" s="21" t="s">
+      <c r="M102" s="19" t="s">
         <v>2220</v>
       </c>
       <c r="N102" s="14" t="str">
@@ -14355,10 +14394,10 @@
       <c r="K125" s="16" t="s">
         <v>2173</v>
       </c>
-      <c r="L125" s="21" t="s">
+      <c r="L125" s="19" t="s">
         <v>2171</v>
       </c>
-      <c r="M125" s="21" t="s">
+      <c r="M125" s="19" t="s">
         <v>2172</v>
       </c>
       <c r="N125" s="14" t="str">
@@ -14447,10 +14486,10 @@
       <c r="K127" s="16" t="s">
         <v>2167</v>
       </c>
-      <c r="L127" s="21" t="s">
+      <c r="L127" s="19" t="s">
         <v>2165</v>
       </c>
-      <c r="M127" s="21" t="s">
+      <c r="M127" s="19" t="s">
         <v>2166</v>
       </c>
       <c r="N127" s="14" t="str">
@@ -14493,10 +14532,10 @@
       <c r="K128" s="16" t="s">
         <v>2164</v>
       </c>
-      <c r="L128" s="21" t="s">
+      <c r="L128" s="19" t="s">
         <v>2162</v>
       </c>
-      <c r="M128" s="21" t="s">
+      <c r="M128" s="19" t="s">
         <v>2163</v>
       </c>
       <c r="N128" s="14" t="str">
@@ -14539,10 +14578,10 @@
       <c r="K129" s="16" t="s">
         <v>2161</v>
       </c>
-      <c r="L129" s="21" t="s">
+      <c r="L129" s="19" t="s">
         <v>2159</v>
       </c>
-      <c r="M129" s="21" t="s">
+      <c r="M129" s="19" t="s">
         <v>2160</v>
       </c>
       <c r="N129" s="14" t="str">
@@ -14585,10 +14624,10 @@
       <c r="K130" s="16" t="s">
         <v>2158</v>
       </c>
-      <c r="L130" s="21" t="s">
+      <c r="L130" s="19" t="s">
         <v>2156</v>
       </c>
-      <c r="M130" s="21" t="s">
+      <c r="M130" s="19" t="s">
         <v>2157</v>
       </c>
       <c r="N130" s="14" t="str">
@@ -14600,7 +14639,7 @@
       <c r="A131" s="13">
         <v>59776</v>
       </c>
-      <c r="B131" s="23" t="s">
+      <c r="B131" s="21" t="s">
         <v>2497</v>
       </c>
       <c r="C131" s="2" t="s">
@@ -14677,10 +14716,10 @@
       <c r="K132" s="16" t="s">
         <v>2155</v>
       </c>
-      <c r="L132" s="21" t="s">
+      <c r="L132" s="19" t="s">
         <v>2153</v>
       </c>
-      <c r="M132" s="21" t="s">
+      <c r="M132" s="19" t="s">
         <v>2154</v>
       </c>
       <c r="N132" s="14" t="str">
@@ -14910,8 +14949,8 @@
       <c r="L137" s="14" t="s">
         <v>2497</v>
       </c>
-      <c r="M137" s="21" t="s">
-        <v>2534</v>
+      <c r="M137" s="19" t="s">
+        <v>2533</v>
       </c>
       <c r="N137" s="14" t="str">
         <f t="shared" si="5"/>
@@ -14953,10 +14992,10 @@
       <c r="K138" s="16" t="s">
         <v>2139</v>
       </c>
-      <c r="L138" s="21" t="s">
+      <c r="L138" s="19" t="s">
         <v>2137</v>
       </c>
-      <c r="M138" s="21" t="s">
+      <c r="M138" s="19" t="s">
         <v>2138</v>
       </c>
       <c r="N138" s="14" t="str">
@@ -14997,13 +15036,13 @@
         <v>2497</v>
       </c>
       <c r="K139" s="16" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="L139" s="15" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="M139" s="14" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="N139" s="14" t="str">
         <f t="shared" si="5"/>
@@ -15091,10 +15130,10 @@
       <c r="K141" s="16" t="s">
         <v>2133</v>
       </c>
-      <c r="L141" s="21" t="s">
+      <c r="L141" s="19" t="s">
         <v>2131</v>
       </c>
-      <c r="M141" s="21" t="s">
+      <c r="M141" s="19" t="s">
         <v>2132</v>
       </c>
       <c r="N141" s="14" t="str">
@@ -15275,10 +15314,10 @@
       <c r="K145" s="16" t="s">
         <v>2121</v>
       </c>
-      <c r="L145" s="20" t="s">
+      <c r="L145" s="18" t="s">
         <v>2119</v>
       </c>
-      <c r="M145" s="20" t="s">
+      <c r="M145" s="18" t="s">
         <v>2120</v>
       </c>
       <c r="N145" s="14" t="str">
@@ -15367,10 +15406,10 @@
       <c r="K147" s="16" t="s">
         <v>2115</v>
       </c>
-      <c r="L147" s="21" t="s">
+      <c r="L147" s="19" t="s">
         <v>2113</v>
       </c>
-      <c r="M147" s="21" t="s">
+      <c r="M147" s="19" t="s">
         <v>2114</v>
       </c>
       <c r="N147" s="14" t="str">
@@ -15413,10 +15452,10 @@
       <c r="K148" s="16" t="s">
         <v>2112</v>
       </c>
-      <c r="L148" s="20" t="s">
+      <c r="L148" s="18" t="s">
         <v>2110</v>
       </c>
-      <c r="M148" s="21" t="s">
+      <c r="M148" s="19" t="s">
         <v>2111</v>
       </c>
       <c r="N148" s="14" t="str">
@@ -15459,10 +15498,10 @@
       <c r="K149" s="16" t="s">
         <v>2109</v>
       </c>
-      <c r="L149" s="21" t="s">
+      <c r="L149" s="19" t="s">
         <v>2107</v>
       </c>
-      <c r="M149" s="21" t="s">
+      <c r="M149" s="19" t="s">
         <v>2108</v>
       </c>
       <c r="N149" s="14" t="str">
@@ -15505,10 +15544,10 @@
       <c r="K150" s="16" t="s">
         <v>2106</v>
       </c>
-      <c r="L150" s="21" t="s">
+      <c r="L150" s="19" t="s">
         <v>2104</v>
       </c>
-      <c r="M150" s="21" t="s">
+      <c r="M150" s="19" t="s">
         <v>2105</v>
       </c>
       <c r="N150" s="14" t="str">
@@ -15643,10 +15682,10 @@
       <c r="K153" s="16" t="s">
         <v>2096</v>
       </c>
-      <c r="L153" s="21" t="s">
+      <c r="L153" s="19" t="s">
         <v>2095</v>
       </c>
-      <c r="M153" s="21" t="s">
+      <c r="M153" s="19" t="s">
         <v>2097</v>
       </c>
       <c r="N153" s="14" t="str">
@@ -15689,10 +15728,10 @@
       <c r="K154" s="16" t="s">
         <v>2096</v>
       </c>
-      <c r="L154" s="20" t="s">
+      <c r="L154" s="18" t="s">
         <v>2095</v>
       </c>
-      <c r="M154" s="21" t="s">
+      <c r="M154" s="19" t="s">
         <v>2097</v>
       </c>
       <c r="N154" s="14" t="str">
@@ -15735,10 +15774,10 @@
       <c r="K155" s="16" t="s">
         <v>2094</v>
       </c>
-      <c r="L155" s="21" t="s">
+      <c r="L155" s="19" t="s">
         <v>2092</v>
       </c>
-      <c r="M155" s="21" t="s">
+      <c r="M155" s="19" t="s">
         <v>2093</v>
       </c>
       <c r="N155" s="14" t="str">
@@ -15781,10 +15820,10 @@
       <c r="K156" s="16" t="s">
         <v>2091</v>
       </c>
-      <c r="L156" s="21" t="s">
+      <c r="L156" s="19" t="s">
         <v>2089</v>
       </c>
-      <c r="M156" s="21" t="s">
+      <c r="M156" s="19" t="s">
         <v>2090</v>
       </c>
       <c r="N156" s="14" t="str">
@@ -15827,10 +15866,10 @@
       <c r="K157" s="16" t="s">
         <v>2088</v>
       </c>
-      <c r="L157" s="21" t="s">
+      <c r="L157" s="19" t="s">
         <v>2086</v>
       </c>
-      <c r="M157" s="21" t="s">
+      <c r="M157" s="19" t="s">
         <v>2087</v>
       </c>
       <c r="N157" s="14" t="str">
@@ -15873,10 +15912,10 @@
       <c r="K158" s="16" t="s">
         <v>2085</v>
       </c>
-      <c r="L158" s="21" t="s">
+      <c r="L158" s="19" t="s">
         <v>2083</v>
       </c>
-      <c r="M158" s="21" t="s">
+      <c r="M158" s="19" t="s">
         <v>2084</v>
       </c>
       <c r="N158" s="14" t="str">
@@ -15919,10 +15958,10 @@
       <c r="K159" s="16" t="s">
         <v>2082</v>
       </c>
-      <c r="L159" s="21" t="s">
+      <c r="L159" s="19" t="s">
         <v>2080</v>
       </c>
-      <c r="M159" s="21" t="s">
+      <c r="M159" s="19" t="s">
         <v>2081</v>
       </c>
       <c r="N159" s="14" t="str">
@@ -15965,10 +16004,10 @@
       <c r="K160" s="16" t="s">
         <v>2079</v>
       </c>
-      <c r="L160" s="21" t="s">
+      <c r="L160" s="19" t="s">
         <v>2077</v>
       </c>
-      <c r="M160" s="21" t="s">
+      <c r="M160" s="19" t="s">
         <v>2078</v>
       </c>
       <c r="N160" s="14" t="str">
@@ -16057,10 +16096,10 @@
       <c r="K162" s="16" t="s">
         <v>2076</v>
       </c>
-      <c r="L162" s="21" t="s">
+      <c r="L162" s="19" t="s">
         <v>2074</v>
       </c>
-      <c r="M162" s="21" t="s">
+      <c r="M162" s="19" t="s">
         <v>2075</v>
       </c>
       <c r="N162" s="14" t="str">
@@ -16103,10 +16142,10 @@
       <c r="K163" s="16" t="s">
         <v>2073</v>
       </c>
-      <c r="L163" s="21" t="s">
+      <c r="L163" s="19" t="s">
         <v>2071</v>
       </c>
-      <c r="M163" s="21" t="s">
+      <c r="M163" s="19" t="s">
         <v>2072</v>
       </c>
       <c r="N163" s="14" t="str">
@@ -16149,10 +16188,10 @@
       <c r="K164" s="16" t="s">
         <v>2070</v>
       </c>
-      <c r="L164" s="21" t="s">
+      <c r="L164" s="19" t="s">
         <v>2068</v>
       </c>
-      <c r="M164" s="21" t="s">
+      <c r="M164" s="19" t="s">
         <v>2069</v>
       </c>
       <c r="N164" s="14" t="str">
@@ -17023,10 +17062,10 @@
       <c r="K183" s="16" t="s">
         <v>2013</v>
       </c>
-      <c r="L183" s="21" t="s">
+      <c r="L183" s="19" t="s">
         <v>2011</v>
       </c>
-      <c r="M183" s="21" t="s">
+      <c r="M183" s="19" t="s">
         <v>2012</v>
       </c>
       <c r="N183" s="14" t="str">
@@ -17115,10 +17154,10 @@
       <c r="K185" s="16" t="s">
         <v>2007</v>
       </c>
-      <c r="L185" s="21" t="s">
+      <c r="L185" s="19" t="s">
         <v>2005</v>
       </c>
-      <c r="M185" s="21" t="s">
+      <c r="M185" s="19" t="s">
         <v>2006</v>
       </c>
       <c r="N185" s="14" t="str">
@@ -17161,10 +17200,10 @@
       <c r="K186" s="16" t="s">
         <v>2004</v>
       </c>
-      <c r="L186" s="21" t="s">
+      <c r="L186" s="19" t="s">
         <v>2002</v>
       </c>
-      <c r="M186" s="21" t="s">
+      <c r="M186" s="19" t="s">
         <v>2003</v>
       </c>
       <c r="N186" s="14" t="str">
@@ -17207,10 +17246,10 @@
       <c r="K187" s="16" t="s">
         <v>2001</v>
       </c>
-      <c r="L187" s="21" t="s">
+      <c r="L187" s="19" t="s">
         <v>1999</v>
       </c>
-      <c r="M187" s="21" t="s">
+      <c r="M187" s="19" t="s">
         <v>2000</v>
       </c>
       <c r="N187" s="14" t="str">
@@ -17253,10 +17292,10 @@
       <c r="K188" s="16" t="s">
         <v>1998</v>
       </c>
-      <c r="L188" s="21" t="s">
+      <c r="L188" s="19" t="s">
         <v>1996</v>
       </c>
-      <c r="M188" s="21" t="s">
+      <c r="M188" s="19" t="s">
         <v>1997</v>
       </c>
       <c r="N188" s="14" t="str">
@@ -17437,10 +17476,10 @@
       <c r="K192" s="16" t="s">
         <v>1992</v>
       </c>
-      <c r="L192" s="21" t="s">
+      <c r="L192" s="19" t="s">
         <v>1990</v>
       </c>
-      <c r="M192" s="21" t="s">
+      <c r="M192" s="19" t="s">
         <v>1991</v>
       </c>
       <c r="N192" s="14" t="str">
@@ -17529,10 +17568,10 @@
       <c r="K194" s="16" t="s">
         <v>1989</v>
       </c>
-      <c r="L194" s="21" t="s">
+      <c r="L194" s="19" t="s">
         <v>1987</v>
       </c>
-      <c r="M194" s="21" t="s">
+      <c r="M194" s="19" t="s">
         <v>1988</v>
       </c>
       <c r="N194" s="14" t="str">
@@ -17575,10 +17614,10 @@
       <c r="K195" s="16" t="s">
         <v>1986</v>
       </c>
-      <c r="L195" s="21" t="s">
+      <c r="L195" s="19" t="s">
         <v>1984</v>
       </c>
-      <c r="M195" s="21" t="s">
+      <c r="M195" s="19" t="s">
         <v>1985</v>
       </c>
       <c r="N195" s="14" t="str">
@@ -17621,10 +17660,10 @@
       <c r="K196" s="16" t="s">
         <v>1983</v>
       </c>
-      <c r="L196" s="21" t="s">
+      <c r="L196" s="19" t="s">
         <v>1981</v>
       </c>
-      <c r="M196" s="21" t="s">
+      <c r="M196" s="19" t="s">
         <v>1982</v>
       </c>
       <c r="N196" s="14" t="str">
@@ -18449,10 +18488,10 @@
       <c r="K214" s="16" t="s">
         <v>1929</v>
       </c>
-      <c r="L214" s="21" t="s">
+      <c r="L214" s="19" t="s">
         <v>1927</v>
       </c>
-      <c r="M214" s="21" t="s">
+      <c r="M214" s="19" t="s">
         <v>1928</v>
       </c>
       <c r="N214" s="14" t="str">
@@ -18495,10 +18534,10 @@
       <c r="K215" s="16" t="s">
         <v>1926</v>
       </c>
-      <c r="L215" s="21" t="s">
+      <c r="L215" s="19" t="s">
         <v>1924</v>
       </c>
-      <c r="M215" s="21" t="s">
+      <c r="M215" s="19" t="s">
         <v>1925</v>
       </c>
       <c r="N215" s="14" t="str">
@@ -18541,10 +18580,10 @@
       <c r="K216" s="16" t="s">
         <v>1923</v>
       </c>
-      <c r="L216" s="21" t="s">
+      <c r="L216" s="19" t="s">
         <v>1921</v>
       </c>
-      <c r="M216" s="21" t="s">
+      <c r="M216" s="19" t="s">
         <v>1922</v>
       </c>
       <c r="N216" s="14" t="str">
@@ -18587,10 +18626,10 @@
       <c r="K217" s="16" t="s">
         <v>1920</v>
       </c>
-      <c r="L217" s="21" t="s">
+      <c r="L217" s="19" t="s">
         <v>1918</v>
       </c>
-      <c r="M217" s="21" t="s">
+      <c r="M217" s="19" t="s">
         <v>1919</v>
       </c>
       <c r="N217" s="14" t="str">
@@ -18679,10 +18718,10 @@
       <c r="K219" s="16" t="s">
         <v>1914</v>
       </c>
-      <c r="L219" s="21" t="s">
+      <c r="L219" s="19" t="s">
         <v>1912</v>
       </c>
-      <c r="M219" s="21" t="s">
+      <c r="M219" s="19" t="s">
         <v>1913</v>
       </c>
       <c r="N219" s="14" t="str">
@@ -18909,10 +18948,10 @@
       <c r="K224" s="16" t="s">
         <v>1899</v>
       </c>
-      <c r="L224" s="21" t="s">
+      <c r="L224" s="19" t="s">
         <v>1897</v>
       </c>
-      <c r="M224" s="21" t="s">
+      <c r="M224" s="19" t="s">
         <v>1898</v>
       </c>
       <c r="N224" s="14" t="str">
@@ -19384,7 +19423,7 @@
       <c r="A235">
         <v>59880</v>
       </c>
-      <c r="B235" s="23" t="s">
+      <c r="B235" s="21" t="s">
         <v>2497</v>
       </c>
       <c r="C235" t="s">
@@ -19921,10 +19960,10 @@
       <c r="K246" s="16" t="s">
         <v>1854</v>
       </c>
-      <c r="L246" s="21" t="s">
+      <c r="L246" s="19" t="s">
         <v>1852</v>
       </c>
-      <c r="M246" s="21" t="s">
+      <c r="M246" s="19" t="s">
         <v>1853</v>
       </c>
       <c r="N246" s="14" t="str">
@@ -19967,10 +20006,10 @@
       <c r="K247" s="16" t="s">
         <v>1854</v>
       </c>
-      <c r="L247" s="21" t="s">
+      <c r="L247" s="19" t="s">
         <v>1852</v>
       </c>
-      <c r="M247" s="21" t="s">
+      <c r="M247" s="19" t="s">
         <v>1853</v>
       </c>
       <c r="N247" s="14" t="str">
@@ -20013,10 +20052,10 @@
       <c r="K248" s="16" t="s">
         <v>1851</v>
       </c>
-      <c r="L248" s="21" t="s">
+      <c r="L248" s="19" t="s">
         <v>1849</v>
       </c>
-      <c r="M248" s="21" t="s">
+      <c r="M248" s="19" t="s">
         <v>1850</v>
       </c>
       <c r="N248" s="14" t="str">
@@ -20059,10 +20098,10 @@
       <c r="K249" s="16" t="s">
         <v>1851</v>
       </c>
-      <c r="L249" s="21" t="s">
+      <c r="L249" s="19" t="s">
         <v>1849</v>
       </c>
-      <c r="M249" s="21" t="s">
+      <c r="M249" s="19" t="s">
         <v>1850</v>
       </c>
       <c r="N249" s="14" t="str">
@@ -20519,10 +20558,10 @@
       <c r="K259" s="16" t="s">
         <v>1833</v>
       </c>
-      <c r="L259" s="21" t="s">
+      <c r="L259" s="19" t="s">
         <v>1831</v>
       </c>
-      <c r="M259" s="21" t="s">
+      <c r="M259" s="19" t="s">
         <v>1832</v>
       </c>
       <c r="N259" s="14" t="str">
@@ -20841,10 +20880,10 @@
       <c r="K266" s="16" t="s">
         <v>1815</v>
       </c>
-      <c r="L266" s="21" t="s">
+      <c r="L266" s="19" t="s">
         <v>1813</v>
       </c>
-      <c r="M266" s="21" t="s">
+      <c r="M266" s="19" t="s">
         <v>1814</v>
       </c>
       <c r="N266" s="14" t="str">
@@ -20933,10 +20972,10 @@
       <c r="K268" s="16" t="s">
         <v>1809</v>
       </c>
-      <c r="L268" s="21" t="s">
+      <c r="L268" s="19" t="s">
         <v>1807</v>
       </c>
-      <c r="M268" s="21" t="s">
+      <c r="M268" s="19" t="s">
         <v>1808</v>
       </c>
       <c r="N268" s="14" t="str">
@@ -20979,10 +21018,10 @@
       <c r="K269" s="16" t="s">
         <v>1806</v>
       </c>
-      <c r="L269" s="21" t="s">
+      <c r="L269" s="19" t="s">
         <v>1804</v>
       </c>
-      <c r="M269" s="21" t="s">
+      <c r="M269" s="19" t="s">
         <v>1805</v>
       </c>
       <c r="N269" s="14" t="str">
@@ -21347,10 +21386,10 @@
       <c r="K277" s="16" t="s">
         <v>1785</v>
       </c>
-      <c r="L277" s="21" t="s">
+      <c r="L277" s="19" t="s">
         <v>1783</v>
       </c>
-      <c r="M277" s="21" t="s">
+      <c r="M277" s="19" t="s">
         <v>1784</v>
       </c>
       <c r="N277" s="14" t="str">
@@ -21393,10 +21432,10 @@
       <c r="K278" s="16" t="s">
         <v>1782</v>
       </c>
-      <c r="L278" s="21" t="s">
+      <c r="L278" s="19" t="s">
         <v>1780</v>
       </c>
-      <c r="M278" s="21" t="s">
+      <c r="M278" s="19" t="s">
         <v>1781</v>
       </c>
       <c r="N278" s="14" t="str">
@@ -21439,10 +21478,10 @@
       <c r="K279" s="16" t="s">
         <v>1779</v>
       </c>
-      <c r="L279" s="21" t="s">
+      <c r="L279" s="19" t="s">
         <v>1777</v>
       </c>
-      <c r="M279" s="21" t="s">
+      <c r="M279" s="19" t="s">
         <v>1778</v>
       </c>
       <c r="N279" s="14" t="str">
@@ -21531,10 +21570,10 @@
       <c r="K281" s="16" t="s">
         <v>1773</v>
       </c>
-      <c r="L281" s="21" t="s">
+      <c r="L281" s="19" t="s">
         <v>1771</v>
       </c>
-      <c r="M281" s="21" t="s">
+      <c r="M281" s="19" t="s">
         <v>1772</v>
       </c>
       <c r="N281" s="14" t="str">
@@ -21577,10 +21616,10 @@
       <c r="K282" s="16" t="s">
         <v>1770</v>
       </c>
-      <c r="L282" s="21" t="s">
+      <c r="L282" s="19" t="s">
         <v>1768</v>
       </c>
-      <c r="M282" s="21" t="s">
+      <c r="M282" s="19" t="s">
         <v>1769</v>
       </c>
       <c r="N282" s="14" t="str">
@@ -21666,7 +21705,7 @@
       <c r="J284" t="s">
         <v>2497</v>
       </c>
-      <c r="K284" s="22" t="s">
+      <c r="K284" s="20" t="s">
         <v>1764</v>
       </c>
       <c r="L284" s="15" t="s">
@@ -21712,7 +21751,7 @@
       <c r="J285" t="s">
         <v>2497</v>
       </c>
-      <c r="K285" s="22" t="s">
+      <c r="K285" s="20" t="s">
         <v>1761</v>
       </c>
       <c r="L285" s="15" t="s">
@@ -21758,7 +21797,7 @@
       <c r="J286" t="s">
         <v>2497</v>
       </c>
-      <c r="K286" s="22" t="s">
+      <c r="K286" s="20" t="s">
         <v>1758</v>
       </c>
       <c r="L286" s="15" t="s">
@@ -21804,7 +21843,7 @@
       <c r="J287" t="s">
         <v>2497</v>
       </c>
-      <c r="K287" s="23" t="s">
+      <c r="K287" s="21" t="s">
         <v>2497</v>
       </c>
       <c r="L287" s="10" t="s">
@@ -21850,7 +21889,7 @@
       <c r="J288" t="s">
         <v>2497</v>
       </c>
-      <c r="K288" s="22" t="s">
+      <c r="K288" s="20" t="s">
         <v>1755</v>
       </c>
       <c r="L288" s="15" t="s">
@@ -21896,7 +21935,7 @@
       <c r="J289" t="s">
         <v>2497</v>
       </c>
-      <c r="K289" s="23" t="s">
+      <c r="K289" s="21" t="s">
         <v>2497</v>
       </c>
       <c r="L289" s="10" t="s">
@@ -21942,7 +21981,7 @@
       <c r="J290" t="s">
         <v>2497</v>
       </c>
-      <c r="K290" s="22" t="s">
+      <c r="K290" s="20" t="s">
         <v>1752</v>
       </c>
       <c r="L290" s="15" t="s">
@@ -21991,10 +22030,10 @@
       <c r="K291" s="16" t="s">
         <v>1749</v>
       </c>
-      <c r="L291" s="21" t="s">
+      <c r="L291" s="19" t="s">
         <v>1747</v>
       </c>
-      <c r="M291" s="21" t="s">
+      <c r="M291" s="19" t="s">
         <v>1748</v>
       </c>
       <c r="N291" s="14" t="str">
@@ -22129,10 +22168,10 @@
       <c r="K294" s="16" t="s">
         <v>1740</v>
       </c>
-      <c r="L294" s="21" t="s">
+      <c r="L294" s="19" t="s">
         <v>1738</v>
       </c>
-      <c r="M294" s="21" t="s">
+      <c r="M294" s="19" t="s">
         <v>1739</v>
       </c>
       <c r="N294" s="14" t="str">
@@ -22221,7 +22260,7 @@
       <c r="K296" s="16" t="s">
         <v>1734</v>
       </c>
-      <c r="L296" s="21" t="s">
+      <c r="L296" s="19" t="s">
         <v>1732</v>
       </c>
       <c r="M296" s="15" t="s">
@@ -22957,10 +22996,10 @@
       <c r="K312" s="16" t="s">
         <v>1701</v>
       </c>
-      <c r="L312" s="21" t="s">
+      <c r="L312" s="19" t="s">
         <v>1699</v>
       </c>
-      <c r="M312" s="21" t="s">
+      <c r="M312" s="19" t="s">
         <v>1700</v>
       </c>
       <c r="N312" s="14" t="str">
@@ -23368,7 +23407,7 @@
       <c r="J321" t="s">
         <v>2497</v>
       </c>
-      <c r="K321" s="22" t="s">
+      <c r="K321" s="20" t="s">
         <v>1674</v>
       </c>
       <c r="L321" s="14" t="s">
@@ -24153,10 +24192,10 @@
       <c r="K338" s="16" t="s">
         <v>1626</v>
       </c>
-      <c r="L338" s="21" t="s">
+      <c r="L338" s="19" t="s">
         <v>1624</v>
       </c>
-      <c r="M338" s="21" t="s">
+      <c r="M338" s="19" t="s">
         <v>1625</v>
       </c>
       <c r="N338" s="14" t="str">
@@ -24199,10 +24238,10 @@
       <c r="K339" s="16" t="s">
         <v>1623</v>
       </c>
-      <c r="L339" s="21" t="s">
+      <c r="L339" s="19" t="s">
         <v>1621</v>
       </c>
-      <c r="M339" s="21" t="s">
+      <c r="M339" s="19" t="s">
         <v>1622</v>
       </c>
       <c r="N339" s="14" t="str">
@@ -24475,10 +24514,10 @@
       <c r="K345" s="16" t="s">
         <v>1604</v>
       </c>
-      <c r="L345" s="21" t="s">
+      <c r="L345" s="19" t="s">
         <v>1602</v>
       </c>
-      <c r="M345" s="21" t="s">
+      <c r="M345" s="19" t="s">
         <v>1603</v>
       </c>
       <c r="N345" s="14" t="str">
@@ -24613,10 +24652,10 @@
       <c r="K348" s="16" t="s">
         <v>1595</v>
       </c>
-      <c r="L348" s="21" t="s">
+      <c r="L348" s="19" t="s">
         <v>1593</v>
       </c>
-      <c r="M348" s="21" t="s">
+      <c r="M348" s="19" t="s">
         <v>1594</v>
       </c>
       <c r="N348" s="14" t="str">
@@ -24659,10 +24698,10 @@
       <c r="K349" s="16" t="s">
         <v>1592</v>
       </c>
-      <c r="L349" s="21" t="s">
+      <c r="L349" s="19" t="s">
         <v>1590</v>
       </c>
-      <c r="M349" s="21" t="s">
+      <c r="M349" s="19" t="s">
         <v>1591</v>
       </c>
       <c r="N349" s="14" t="str">
@@ -24751,10 +24790,10 @@
       <c r="K351" s="16" t="s">
         <v>1586</v>
       </c>
-      <c r="L351" s="21" t="s">
+      <c r="L351" s="19" t="s">
         <v>1584</v>
       </c>
-      <c r="M351" s="21" t="s">
+      <c r="M351" s="19" t="s">
         <v>1585</v>
       </c>
       <c r="N351" s="14" t="str">
@@ -24797,10 +24836,10 @@
       <c r="K352" s="16" t="s">
         <v>1583</v>
       </c>
-      <c r="L352" s="21" t="s">
+      <c r="L352" s="19" t="s">
         <v>1581</v>
       </c>
-      <c r="M352" s="21" t="s">
+      <c r="M352" s="19" t="s">
         <v>1582</v>
       </c>
       <c r="N352" s="14" t="str">
@@ -24843,10 +24882,10 @@
       <c r="K353" s="16" t="s">
         <v>1580</v>
       </c>
-      <c r="L353" s="21" t="s">
+      <c r="L353" s="19" t="s">
         <v>1578</v>
       </c>
-      <c r="M353" s="21" t="s">
+      <c r="M353" s="19" t="s">
         <v>1579</v>
       </c>
       <c r="N353" s="14" t="str">
@@ -24889,10 +24928,10 @@
       <c r="K354" s="16" t="s">
         <v>1577</v>
       </c>
-      <c r="L354" s="21" t="s">
+      <c r="L354" s="19" t="s">
         <v>1575</v>
       </c>
-      <c r="M354" s="21" t="s">
+      <c r="M354" s="19" t="s">
         <v>1576</v>
       </c>
       <c r="N354" s="14" t="str">
@@ -24935,10 +24974,10 @@
       <c r="K355" s="16" t="s">
         <v>1574</v>
       </c>
-      <c r="L355" s="21" t="s">
+      <c r="L355" s="19" t="s">
         <v>1572</v>
       </c>
-      <c r="M355" s="21" t="s">
+      <c r="M355" s="19" t="s">
         <v>1573</v>
       </c>
       <c r="N355" s="14" t="str">
@@ -25533,10 +25572,10 @@
       <c r="K368" s="16" t="s">
         <v>1535</v>
       </c>
-      <c r="L368" s="21" t="s">
+      <c r="L368" s="19" t="s">
         <v>1533</v>
       </c>
-      <c r="M368" s="21" t="s">
+      <c r="M368" s="19" t="s">
         <v>1534</v>
       </c>
       <c r="N368" s="14" t="str">
@@ -25717,10 +25756,10 @@
       <c r="K372" s="16" t="s">
         <v>1523</v>
       </c>
-      <c r="L372" s="21" t="s">
+      <c r="L372" s="19" t="s">
         <v>1521</v>
       </c>
-      <c r="M372" s="21" t="s">
+      <c r="M372" s="19" t="s">
         <v>1522</v>
       </c>
       <c r="N372" s="14" t="str">
@@ -26959,10 +26998,10 @@
       <c r="K399" s="16" t="s">
         <v>1446</v>
       </c>
-      <c r="L399" s="21" t="s">
+      <c r="L399" s="19" t="s">
         <v>1444</v>
       </c>
-      <c r="M399" s="21" t="s">
+      <c r="M399" s="19" t="s">
         <v>1445</v>
       </c>
       <c r="N399" s="14" t="str">
@@ -27143,10 +27182,10 @@
       <c r="K403" s="16" t="s">
         <v>1434</v>
       </c>
-      <c r="L403" s="21" t="s">
+      <c r="L403" s="19" t="s">
         <v>1432</v>
       </c>
-      <c r="M403" s="21" t="s">
+      <c r="M403" s="19" t="s">
         <v>1433</v>
       </c>
       <c r="N403" s="14" t="str">
@@ -27480,7 +27519,7 @@
       <c r="A411">
         <v>60056</v>
       </c>
-      <c r="B411" s="23" t="s">
+      <c r="B411" s="21" t="s">
         <v>2497</v>
       </c>
       <c r="C411" t="s">
@@ -27526,7 +27565,7 @@
       <c r="A412">
         <v>60057</v>
       </c>
-      <c r="B412" s="23" t="s">
+      <c r="B412" s="21" t="s">
         <v>2497</v>
       </c>
       <c r="C412" t="s">
@@ -27572,7 +27611,7 @@
       <c r="A413">
         <v>60058</v>
       </c>
-      <c r="B413" s="23" t="s">
+      <c r="B413" s="21" t="s">
         <v>2497</v>
       </c>
       <c r="C413" t="s">
@@ -27695,10 +27734,10 @@
       <c r="K415" s="16" t="s">
         <v>1411</v>
       </c>
-      <c r="L415" s="21" t="s">
+      <c r="L415" s="19" t="s">
         <v>1409</v>
       </c>
-      <c r="M415" s="21" t="s">
+      <c r="M415" s="19" t="s">
         <v>1410</v>
       </c>
       <c r="N415" s="14" t="str">
@@ -27741,10 +27780,10 @@
       <c r="K416" s="16" t="s">
         <v>1408</v>
       </c>
-      <c r="L416" s="21" t="s">
+      <c r="L416" s="19" t="s">
         <v>1406</v>
       </c>
-      <c r="M416" s="21" t="s">
+      <c r="M416" s="19" t="s">
         <v>1407</v>
       </c>
       <c r="N416" s="14" t="str">
@@ -28017,10 +28056,10 @@
       <c r="K422" s="16" t="s">
         <v>1396</v>
       </c>
-      <c r="L422" s="21" t="s">
+      <c r="L422" s="19" t="s">
         <v>1394</v>
       </c>
-      <c r="M422" s="21" t="s">
+      <c r="M422" s="19" t="s">
         <v>1395</v>
       </c>
       <c r="N422" s="14" t="str">
@@ -28109,10 +28148,10 @@
       <c r="K424" s="16" t="s">
         <v>1390</v>
       </c>
-      <c r="L424" s="21" t="s">
+      <c r="L424" s="19" t="s">
         <v>1388</v>
       </c>
-      <c r="M424" s="21" t="s">
+      <c r="M424" s="19" t="s">
         <v>1389</v>
       </c>
       <c r="N424" s="14" t="str">
@@ -28201,10 +28240,10 @@
       <c r="K426" s="16" t="s">
         <v>1384</v>
       </c>
-      <c r="L426" s="21" t="s">
+      <c r="L426" s="19" t="s">
         <v>1382</v>
       </c>
-      <c r="M426" s="21" t="s">
+      <c r="M426" s="19" t="s">
         <v>1383</v>
       </c>
       <c r="N426" s="14" t="str">
@@ -28247,10 +28286,10 @@
       <c r="K427" s="16" t="s">
         <v>1381</v>
       </c>
-      <c r="L427" s="21" t="s">
+      <c r="L427" s="19" t="s">
         <v>1379</v>
       </c>
-      <c r="M427" s="21" t="s">
+      <c r="M427" s="19" t="s">
         <v>1380</v>
       </c>
       <c r="N427" s="14" t="str">
@@ -28429,17 +28468,17 @@
         <v>827</v>
       </c>
       <c r="K431" s="16" t="s">
-        <v>1372</v>
-      </c>
-      <c r="L431" s="15" t="s">
-        <v>1370</v>
-      </c>
-      <c r="M431" s="15" t="s">
-        <v>1371</v>
+        <v>2623</v>
+      </c>
+      <c r="L431" s="34" t="s">
+        <v>2622</v>
+      </c>
+      <c r="M431" s="33" t="s">
+        <v>2621</v>
       </c>
       <c r="N431" s="14" t="str">
         <f t="shared" si="13"/>
-        <v>{"decimal":"60076","namebowtie":"backlog-view-list","namemdl2":"GlobalNavButton","codebowtie":"EAAC","codemdl2":"E700","stylevariation":"bold","keywords":["view","list"],"subset":"VSTS","group":"Work","usagenotes":"Common list view, often used together with grid view."}</v>
+        <v>{"decimal":"60076","namebowtie":"backlog-view-list","namemdl2":"GroupedList","codebowtie":"EAAC","codemdl2":"EF74","stylevariation":"bold","keywords":["view","list"],"subset":"VSTS","group":"Work","usagenotes":"Common list view, often used together with grid view."}</v>
       </c>
     </row>
     <row r="432" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
@@ -28658,7 +28697,7 @@
       <c r="J436" t="s">
         <v>843</v>
       </c>
-      <c r="K436" s="22" t="s">
+      <c r="K436" s="20" t="s">
         <v>1357</v>
       </c>
       <c r="L436" s="15" t="s">
@@ -28799,10 +28838,10 @@
       <c r="K439" s="16" t="s">
         <v>1348</v>
       </c>
-      <c r="L439" s="21" t="s">
+      <c r="L439" s="19" t="s">
         <v>588</v>
       </c>
-      <c r="M439" s="21" t="s">
+      <c r="M439" s="19" t="s">
         <v>1347</v>
       </c>
       <c r="N439" s="14" t="str">
@@ -29029,10 +29068,10 @@
       <c r="K444" s="16" t="s">
         <v>1334</v>
       </c>
-      <c r="L444" s="21" t="s">
+      <c r="L444" s="19" t="s">
         <v>1332</v>
       </c>
-      <c r="M444" s="21" t="s">
+      <c r="M444" s="19" t="s">
         <v>1333</v>
       </c>
       <c r="N444" s="14" t="str">
@@ -29075,10 +29114,10 @@
       <c r="K445" s="16" t="s">
         <v>1331</v>
       </c>
-      <c r="L445" s="21" t="s">
+      <c r="L445" s="19" t="s">
         <v>1329</v>
       </c>
-      <c r="M445" s="21" t="s">
+      <c r="M445" s="19" t="s">
         <v>1330</v>
       </c>
       <c r="N445" s="14" t="str">
@@ -29121,10 +29160,10 @@
       <c r="K446" s="16" t="s">
         <v>1328</v>
       </c>
-      <c r="L446" s="21" t="s">
+      <c r="L446" s="19" t="s">
         <v>1326</v>
       </c>
-      <c r="M446" s="21" t="s">
+      <c r="M446" s="19" t="s">
         <v>1327</v>
       </c>
       <c r="N446" s="14" t="str">
@@ -29489,10 +29528,10 @@
       <c r="K454" s="16" t="s">
         <v>1304</v>
       </c>
-      <c r="L454" s="21" t="s">
+      <c r="L454" s="19" t="s">
         <v>1302</v>
       </c>
-      <c r="M454" s="21" t="s">
+      <c r="M454" s="19" t="s">
         <v>1303</v>
       </c>
       <c r="N454" s="14" t="str">
@@ -29716,7 +29755,7 @@
       <c r="J459" t="s">
         <v>921</v>
       </c>
-      <c r="K459" s="22" t="s">
+      <c r="K459" s="20" t="s">
         <v>1289</v>
       </c>
       <c r="L459" s="15" t="s">
@@ -29762,7 +29801,7 @@
       <c r="J460" t="s">
         <v>921</v>
       </c>
-      <c r="K460" s="22" t="s">
+      <c r="K460" s="20" t="s">
         <v>1286</v>
       </c>
       <c r="L460" s="15" t="s">
@@ -29808,7 +29847,7 @@
       <c r="J461" t="s">
         <v>921</v>
       </c>
-      <c r="K461" s="22" t="s">
+      <c r="K461" s="20" t="s">
         <v>1283</v>
       </c>
       <c r="L461" s="15" t="s">
@@ -29854,7 +29893,7 @@
       <c r="J462" t="s">
         <v>921</v>
       </c>
-      <c r="K462" s="22" t="s">
+      <c r="K462" s="20" t="s">
         <v>1280</v>
       </c>
       <c r="L462" s="15" t="s">
@@ -29873,7 +29912,7 @@
         <v>60108</v>
       </c>
       <c r="B463" s="17" t="s">
-        <v>2578</v>
+        <v>2575</v>
       </c>
       <c r="C463" t="s">
         <v>906</v>
@@ -29919,7 +29958,7 @@
         <v>60109</v>
       </c>
       <c r="B464" s="17" t="s">
-        <v>2579</v>
+        <v>2576</v>
       </c>
       <c r="C464" t="s">
         <v>907</v>
@@ -29995,10 +30034,10 @@
       <c r="K465" s="16" t="s">
         <v>1271</v>
       </c>
-      <c r="L465" s="21" t="s">
+      <c r="L465" s="19" t="s">
         <v>1269</v>
       </c>
-      <c r="M465" s="21" t="s">
+      <c r="M465" s="19" t="s">
         <v>1270</v>
       </c>
       <c r="N465" s="14" t="str">
@@ -30057,7 +30096,7 @@
         <v>60112</v>
       </c>
       <c r="B467" s="17" t="s">
-        <v>2580</v>
+        <v>2577</v>
       </c>
       <c r="C467" t="s">
         <v>914</v>
@@ -30317,10 +30356,10 @@
       <c r="K472" s="16" t="s">
         <v>1253</v>
       </c>
-      <c r="L472" s="21" t="s">
+      <c r="L472" s="19" t="s">
         <v>1251</v>
       </c>
-      <c r="M472" s="21" t="s">
+      <c r="M472" s="19" t="s">
         <v>1252</v>
       </c>
       <c r="N472" s="14" t="str">
@@ -32260,694 +32299,694 @@
         <v>{"decimal":"60159","namebowtie":"feedback","namemdl2":"Feedback","codebowtie":"EAFF","codemdl2":"ED15","stylevariation":"light","keywords":["feedback","user","voice","chat","bubble","suggestion"],"subset":"VSTS","group":"Common","usagenotes":"Used for feedback dropdown in navigation."}</v>
       </c>
     </row>
-    <row r="515" spans="1:14" s="18" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A515" s="18">
+    <row r="515" spans="1:14" s="29" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A515" s="29">
         <v>60160</v>
       </c>
-      <c r="B515" s="17" t="s">
+      <c r="B515" s="26" t="s">
         <v>1083</v>
       </c>
-      <c r="C515" s="18" t="s">
+      <c r="C515" s="29" t="s">
         <v>1072</v>
       </c>
-      <c r="D515" s="18" t="str">
+      <c r="D515" s="29" t="str">
         <f t="shared" ref="D515:D529" si="16">DEC2HEX(A515)</f>
         <v>EB00</v>
       </c>
-      <c r="E515" s="18">
+      <c r="E515" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F515" s="18" t="s">
+      <c r="F515" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G515" s="18" t="s">
+      <c r="G515" s="29" t="s">
         <v>1073</v>
       </c>
-      <c r="H515" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I515" s="18" t="s">
+      <c r="H515" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I515" s="29" t="s">
         <v>584</v>
       </c>
-      <c r="J515" s="18" t="s">
+      <c r="J515" s="29" t="s">
         <v>1074</v>
       </c>
-      <c r="K515" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L515" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M515" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N515" s="14" t="str">
-        <f t="shared" ref="N515:N578" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
-        <v>{"decimal":"60160","namebowtie":"file-lock","namemdl2":"null","codebowtie":"EB00","codemdl2":"null","stylevariation":"light","keywords":["file","document","lock","permission"],"subset":"VSTS","group":"Common","usagenotes":"Used to represent the user does not have permission to a file."}</v>
-      </c>
-    </row>
-    <row r="516" spans="1:14" s="18" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A516" s="18">
+      <c r="K515" s="16" t="s">
+        <v>2588</v>
+      </c>
+      <c r="L515" s="35" t="s">
+        <v>2587</v>
+      </c>
+      <c r="M515" s="35" t="s">
+        <v>2586</v>
+      </c>
+      <c r="N515" s="36" t="str">
+        <f t="shared" ref="N515:N529" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
+        <v>{"decimal":"60160","namebowtie":"file-lock","namemdl2":"PageLock","codebowtie":"EB00","codemdl2":"F43F","stylevariation":"light","keywords":["file","document","lock","permission"],"subset":"VSTS","group":"Common","usagenotes":"Used to represent the user does not have permission to a file."}</v>
+      </c>
+    </row>
+    <row r="516" spans="1:14" s="29" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A516" s="29">
         <v>60161</v>
       </c>
-      <c r="B516" s="17" t="s">
+      <c r="B516" s="26" t="s">
         <v>1082</v>
       </c>
-      <c r="C516" s="18" t="s">
+      <c r="C516" s="29" t="s">
         <v>1075</v>
       </c>
-      <c r="D516" s="18" t="str">
+      <c r="D516" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB01</v>
       </c>
-      <c r="E516" s="18">
+      <c r="E516" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F516" s="18" t="s">
+      <c r="F516" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G516" s="18" t="s">
+      <c r="G516" s="29" t="s">
         <v>1076</v>
       </c>
-      <c r="H516" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I516" s="18" t="s">
+      <c r="H516" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I516" s="29" t="s">
         <v>593</v>
       </c>
-      <c r="J516" s="18" t="s">
+      <c r="J516" s="29" t="s">
         <v>1077</v>
       </c>
-      <c r="K516" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L516" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M516" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N516" s="14" t="str">
+      <c r="K516" s="16" t="s">
+        <v>2590</v>
+      </c>
+      <c r="L516" s="35" t="s">
+        <v>2591</v>
+      </c>
+      <c r="M516" s="35" t="s">
+        <v>2589</v>
+      </c>
+      <c r="N516" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60161","namebowtie":"not-executed","namemdl2":"null","codebowtie":"EB01","codemdl2":"null","stylevariation":"light","keywords":["not","execute","run","play","triangle","block","no"],"subset":"VSTS","group":"Status","usagenotes":"Used in Test hub for not executed test outcome."}</v>
-      </c>
-    </row>
-    <row r="517" spans="1:14" s="18" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A517" s="18">
+        <v>{"decimal":"60161","namebowtie":"not-executed","namemdl2":"NotExecuted","codebowtie":"EB01","codemdl2":"F440","stylevariation":"light","keywords":["not","execute","run","play","triangle","block","no"],"subset":"VSTS","group":"Status","usagenotes":"Used in Test hub for not executed test outcome."}</v>
+      </c>
+    </row>
+    <row r="517" spans="1:14" s="29" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A517" s="29">
         <v>60162</v>
       </c>
-      <c r="B517" s="17" t="s">
+      <c r="B517" s="26" t="s">
         <v>1081</v>
       </c>
-      <c r="C517" s="18" t="s">
+      <c r="C517" s="29" t="s">
         <v>1078</v>
       </c>
-      <c r="D517" s="18" t="str">
+      <c r="D517" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB02</v>
       </c>
-      <c r="E517" s="18">
+      <c r="E517" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F517" s="18" t="s">
+      <c r="F517" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G517" s="18" t="s">
+      <c r="G517" s="29" t="s">
         <v>1079</v>
       </c>
-      <c r="H517" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I517" s="18" t="s">
+      <c r="H517" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I517" s="29" t="s">
         <v>593</v>
       </c>
-      <c r="J517" s="18" t="s">
+      <c r="J517" s="29" t="s">
         <v>1080</v>
       </c>
-      <c r="K517" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L517" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M517" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N517" s="14" t="str">
+      <c r="K517" s="16" t="s">
+        <v>2594</v>
+      </c>
+      <c r="L517" s="35" t="s">
+        <v>2593</v>
+      </c>
+      <c r="M517" s="35" t="s">
+        <v>2592</v>
+      </c>
+      <c r="N517" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60162","namebowtie":"not-impacted","namemdl2":"null","codebowtie":"EB02","codemdl2":"null","stylevariation":"bold","keywords":["not","impact","hammer","block","no"],"subset":"VSTS","group":"Status","usagenotes":"Used in Test hub for not impacted test outcome."}</v>
-      </c>
-    </row>
-    <row r="518" spans="1:14" s="18" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A518" s="18">
+        <v>{"decimal":"60162","namebowtie":"not-impacted","namemdl2":"NotImpactedSolid","codebowtie":"EB02","codemdl2":"F441","stylevariation":"bold","keywords":["not","impact","hammer","block","no"],"subset":"VSTS","group":"Status","usagenotes":"Used in Test hub for not impacted test outcome."}</v>
+      </c>
+    </row>
+    <row r="518" spans="1:14" s="29" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A518" s="29">
         <v>60163</v>
       </c>
-      <c r="B518" s="17" t="s">
-        <v>2538</v>
-      </c>
-      <c r="C518" s="18" t="s">
-        <v>2500</v>
-      </c>
-      <c r="D518" s="18" t="str">
+      <c r="B518" s="26" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C518" s="29" t="s">
+        <v>2499</v>
+      </c>
+      <c r="D518" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB03</v>
       </c>
-      <c r="E518" s="18">
+      <c r="E518" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F518" s="18" t="s">
+      <c r="F518" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G518" s="18" t="s">
-        <v>2502</v>
-      </c>
-      <c r="H518" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I518" s="18" t="s">
+      <c r="G518" s="29" t="s">
+        <v>2501</v>
+      </c>
+      <c r="H518" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I518" s="29" t="s">
         <v>588</v>
       </c>
-      <c r="J518" s="1" t="s">
-        <v>2504</v>
-      </c>
-      <c r="K518" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L518" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M518" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N518" s="14" t="str">
+      <c r="J518" s="28" t="s">
+        <v>2503</v>
+      </c>
+      <c r="K518" s="16" t="s">
+        <v>2597</v>
+      </c>
+      <c r="L518" s="35" t="s">
+        <v>2596</v>
+      </c>
+      <c r="M518" s="35" t="s">
+        <v>2595</v>
+      </c>
+      <c r="N518" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60163","namebowtie":"field-readonly","namemdl2":"null","codebowtie":"EB03","codemdl2":"null","stylevariation":"light","keywords":["field","lock","read","only"],"subset":"VSTS","group":"Work","usagenotes":"Used in rules editor to represent read-only field."}</v>
-      </c>
-    </row>
-    <row r="519" spans="1:14" s="18" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A519" s="18">
+        <v>{"decimal":"60163","namebowtie":"field-readonly","namemdl2":"FieldReadOnly","codebowtie":"EB03","codemdl2":"F442","stylevariation":"light","keywords":["field","lock","read","only"],"subset":"VSTS","group":"Work","usagenotes":"Used in rules editor to represent read-only field."}</v>
+      </c>
+    </row>
+    <row r="519" spans="1:14" s="29" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A519" s="29">
         <v>60164</v>
       </c>
-      <c r="B519" s="17" t="s">
-        <v>2539</v>
-      </c>
-      <c r="C519" s="18" t="s">
-        <v>2501</v>
-      </c>
-      <c r="D519" s="18" t="str">
+      <c r="B519" s="26" t="s">
+        <v>2538</v>
+      </c>
+      <c r="C519" s="29" t="s">
+        <v>2500</v>
+      </c>
+      <c r="D519" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB04</v>
       </c>
-      <c r="E519" s="18">
+      <c r="E519" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F519" s="18" t="s">
+      <c r="F519" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G519" s="18" t="s">
-        <v>2503</v>
-      </c>
-      <c r="H519" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I519" s="18" t="s">
+      <c r="G519" s="29" t="s">
+        <v>2502</v>
+      </c>
+      <c r="H519" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I519" s="29" t="s">
         <v>588</v>
       </c>
-      <c r="J519" s="1" t="s">
-        <v>2505</v>
-      </c>
-      <c r="K519" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L519" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M519" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N519" s="14" t="str">
+      <c r="J519" s="28" t="s">
+        <v>2504</v>
+      </c>
+      <c r="K519" s="16" t="s">
+        <v>2600</v>
+      </c>
+      <c r="L519" s="35" t="s">
+        <v>2599</v>
+      </c>
+      <c r="M519" s="35" t="s">
+        <v>2598</v>
+      </c>
+      <c r="N519" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60164","namebowtie":"field-required","namemdl2":"null","codebowtie":"EB04","codemdl2":"null","stylevariation":"light","keywords":["field","required","exclamation"],"subset":"VSTS","group":"Work","usagenotes":"Used in rules editor to represent required field."}</v>
-      </c>
-    </row>
-    <row r="520" spans="1:14" s="18" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A520" s="18">
+        <v>{"decimal":"60164","namebowtie":"field-required","namemdl2":"FieldRequired","codebowtie":"EB04","codemdl2":"F443","stylevariation":"light","keywords":["field","required","exclamation"],"subset":"VSTS","group":"Work","usagenotes":"Used in rules editor to represent required field."}</v>
+      </c>
+    </row>
+    <row r="520" spans="1:14" s="29" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A520" s="29">
         <v>60165</v>
       </c>
-      <c r="B520" s="17" t="s">
+      <c r="B520" s="26" t="s">
         <v>2379</v>
       </c>
-      <c r="C520" s="18" t="s">
-        <v>2498</v>
-      </c>
-      <c r="D520" s="18" t="str">
+      <c r="C520" s="29" t="s">
+        <v>2582</v>
+      </c>
+      <c r="D520" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB05</v>
       </c>
-      <c r="E520" s="18">
+      <c r="E520" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F520" s="18" t="s">
+      <c r="F520" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G520" s="18" t="s">
+      <c r="G520" s="29" t="s">
         <v>824</v>
       </c>
-      <c r="H520" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I520" s="18" t="s">
+      <c r="H520" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I520" s="29" t="s">
         <v>588</v>
       </c>
-      <c r="J520" s="18" t="s">
-        <v>2499</v>
-      </c>
-      <c r="K520" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L520" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M520" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N520" s="14" t="str">
+      <c r="J520" s="29" t="s">
+        <v>2498</v>
+      </c>
+      <c r="K520" s="16" t="s">
+        <v>2584</v>
+      </c>
+      <c r="L520" s="35" t="s">
+        <v>2585</v>
+      </c>
+      <c r="M520" s="35" t="s">
+        <v>2583</v>
+      </c>
+      <c r="N520" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60165","namebowtie":"backlog-board","namemdl2":"null","codebowtie":"EB05","codemdl2":"null","stylevariation":"light","keywords":["backlog","board","kanban","card"],"subset":"VSTS","group":"Work","usagenotes":"Used in Work hub for Board view."}</v>
-      </c>
-    </row>
-    <row r="521" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A521" s="18">
+        <v>{"decimal":"60165","namebowtie":"board","namemdl2":"BacklogBoard","codebowtie":"EB05","codemdl2":"F444","stylevariation":"light","keywords":["backlog","board","kanban","card"],"subset":"VSTS","group":"Work","usagenotes":"Used in Work hub for Board view."}</v>
+      </c>
+    </row>
+    <row r="521" spans="1:14" s="27" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A521" s="29">
         <v>60166</v>
       </c>
-      <c r="B521" s="17" t="s">
-        <v>2540</v>
-      </c>
-      <c r="C521" s="18" t="s">
-        <v>2506</v>
-      </c>
-      <c r="D521" s="18" t="str">
+      <c r="B521" s="26" t="s">
+        <v>2539</v>
+      </c>
+      <c r="C521" s="29" t="s">
+        <v>2505</v>
+      </c>
+      <c r="D521" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB06</v>
       </c>
-      <c r="E521" s="18">
+      <c r="E521" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F521" s="18" t="s">
+      <c r="F521" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G521" s="18" t="s">
-        <v>2511</v>
-      </c>
-      <c r="H521" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I521" s="18" t="s">
+      <c r="G521" s="29" t="s">
+        <v>2510</v>
+      </c>
+      <c r="H521" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I521" s="29" t="s">
         <v>583</v>
       </c>
-      <c r="J521" s="18" t="s">
-        <v>2516</v>
-      </c>
-      <c r="K521" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L521" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M521" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N521" s="14" t="str">
+      <c r="J521" s="29" t="s">
+        <v>2515</v>
+      </c>
+      <c r="K521" s="16" t="s">
+        <v>2603</v>
+      </c>
+      <c r="L521" s="35" t="s">
+        <v>2601</v>
+      </c>
+      <c r="M521" s="35" t="s">
+        <v>2602</v>
+      </c>
+      <c r="N521" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60166","namebowtie":"external-build","namemdl2":"null","codebowtie":"EB06","codemdl2":"null","stylevariation":"bold","keywords":["build","source","external"],"subset":"VSTS","group":"Build","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
-      </c>
-    </row>
-    <row r="522" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A522" s="18">
+        <v>{"decimal":"60166","namebowtie":"external-build","namemdl2":"ExternalBuild","codebowtie":"EB06","codemdl2":"F445","stylevariation":"bold","keywords":["build","source","external"],"subset":"VSTS","group":"Build","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
+      </c>
+    </row>
+    <row r="522" spans="1:14" s="27" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A522" s="29">
         <v>60167</v>
       </c>
-      <c r="B522" s="17" t="s">
-        <v>2541</v>
-      </c>
-      <c r="C522" s="18" t="s">
-        <v>2507</v>
-      </c>
-      <c r="D522" s="18" t="str">
+      <c r="B522" s="26" t="s">
+        <v>2540</v>
+      </c>
+      <c r="C522" s="29" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D522" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB07</v>
       </c>
-      <c r="E522" s="18">
+      <c r="E522" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F522" s="18" t="s">
+      <c r="F522" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G522" s="18" t="s">
-        <v>2512</v>
-      </c>
-      <c r="H522" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I522" s="18" t="s">
+      <c r="G522" s="29" t="s">
+        <v>2511</v>
+      </c>
+      <c r="H522" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I522" s="29" t="s">
         <v>596</v>
       </c>
-      <c r="J522" s="18" t="s">
-        <v>2516</v>
-      </c>
-      <c r="K522" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L522" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M522" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N522" s="14" t="str">
+      <c r="J522" s="29" t="s">
+        <v>2515</v>
+      </c>
+      <c r="K522" s="16" t="s">
+        <v>2497</v>
+      </c>
+      <c r="L522" s="35" t="s">
+        <v>2497</v>
+      </c>
+      <c r="M522" s="35" t="s">
+        <v>2497</v>
+      </c>
+      <c r="N522" s="36" t="str">
         <f t="shared" si="17"/>
         <v>{"decimal":"60167","namebowtie":"external-git","namemdl2":"null","codebowtie":"EB07","codemdl2":"null","stylevariation":"bold","keywords":["build","source","external","git"],"subset":"VSTS","group":"Brand","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
       </c>
     </row>
-    <row r="523" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A523" s="18">
+    <row r="523" spans="1:14" s="27" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A523" s="29">
         <v>60168</v>
       </c>
-      <c r="B523" s="17" t="s">
+      <c r="B523" s="26" t="s">
         <v>2197</v>
       </c>
-      <c r="C523" s="18" t="s">
-        <v>2508</v>
-      </c>
-      <c r="D523" s="18" t="str">
+      <c r="C523" s="29" t="s">
+        <v>2507</v>
+      </c>
+      <c r="D523" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB08</v>
       </c>
-      <c r="E523" s="18">
+      <c r="E523" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F523" s="18" t="s">
+      <c r="F523" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G523" s="18" t="s">
-        <v>2513</v>
-      </c>
-      <c r="H523" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I523" s="18" t="s">
+      <c r="G523" s="29" t="s">
+        <v>2512</v>
+      </c>
+      <c r="H523" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I523" s="29" t="s">
         <v>596</v>
       </c>
-      <c r="J523" s="18" t="s">
-        <v>2516</v>
-      </c>
-      <c r="K523" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L523" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M523" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N523" s="14" t="str">
+      <c r="J523" s="29" t="s">
+        <v>2515</v>
+      </c>
+      <c r="K523" s="16" t="s">
+        <v>2608</v>
+      </c>
+      <c r="L523" s="35" t="s">
+        <v>2604</v>
+      </c>
+      <c r="M523" s="35" t="s">
+        <v>2605</v>
+      </c>
+      <c r="N523" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60168","namebowtie":"external-tfvc","namemdl2":"null","codebowtie":"EB08","codemdl2":"null","stylevariation":"bold","keywords":["build","source","external","tfvc"],"subset":"VSTS","group":"Brand","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
-      </c>
-    </row>
-    <row r="524" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A524" s="18">
+        <v>{"decimal":"60168","namebowtie":"external-tfvc","namemdl2":"ExternalTFVC","codebowtie":"EB08","codemdl2":"F446","stylevariation":"bold","keywords":["build","source","external","tfvc"],"subset":"VSTS","group":"Brand","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
+      </c>
+    </row>
+    <row r="524" spans="1:14" s="27" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A524" s="29">
         <v>60169</v>
       </c>
-      <c r="B524" s="17" t="s">
-        <v>2542</v>
-      </c>
-      <c r="C524" s="18" t="s">
-        <v>2509</v>
-      </c>
-      <c r="D524" s="18" t="str">
+      <c r="B524" s="26" t="s">
+        <v>2541</v>
+      </c>
+      <c r="C524" s="29" t="s">
+        <v>2508</v>
+      </c>
+      <c r="D524" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB09</v>
       </c>
-      <c r="E524" s="18">
+      <c r="E524" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F524" s="18" t="s">
+      <c r="F524" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G524" s="18" t="s">
-        <v>2514</v>
-      </c>
-      <c r="H524" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I524" s="18" t="s">
+      <c r="G524" s="29" t="s">
+        <v>2513</v>
+      </c>
+      <c r="H524" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I524" s="29" t="s">
         <v>596</v>
       </c>
-      <c r="J524" s="18" t="s">
-        <v>2516</v>
-      </c>
-      <c r="K524" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L524" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M524" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N524" s="14" t="str">
+      <c r="J524" s="29" t="s">
+        <v>2515</v>
+      </c>
+      <c r="K524" s="16" t="s">
+        <v>2611</v>
+      </c>
+      <c r="L524" s="35" t="s">
+        <v>2607</v>
+      </c>
+      <c r="M524" s="35" t="s">
+        <v>2606</v>
+      </c>
+      <c r="N524" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60169","namebowtie":"external-xaml","namemdl2":"null","codebowtie":"EB09","codemdl2":"null","stylevariation":"bold","keywords":["build","source","external","xaml"],"subset":"VSTS","group":"Brand","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
-      </c>
-    </row>
-    <row r="525" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A525" s="18">
+        <v>{"decimal":"60169","namebowtie":"external-xaml","namemdl2":"ExternalXAML","codebowtie":"EB09","codemdl2":"F447","stylevariation":"bold","keywords":["build","source","external","xaml"],"subset":"VSTS","group":"Brand","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
+      </c>
+    </row>
+    <row r="525" spans="1:14" s="27" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A525" s="29">
         <v>60170</v>
       </c>
-      <c r="B525" s="17" t="s">
-        <v>2543</v>
-      </c>
-      <c r="C525" s="18" t="s">
-        <v>2510</v>
-      </c>
-      <c r="D525" s="18" t="str">
+      <c r="B525" s="26" t="s">
+        <v>2542</v>
+      </c>
+      <c r="C525" s="29" t="s">
+        <v>2509</v>
+      </c>
+      <c r="D525" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB0A</v>
       </c>
-      <c r="E525" s="18">
+      <c r="E525" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F525" s="18" t="s">
+      <c r="F525" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G525" s="18" t="s">
+      <c r="G525" s="29" t="s">
+        <v>2514</v>
+      </c>
+      <c r="H525" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I525" s="29" t="s">
+        <v>596</v>
+      </c>
+      <c r="J525" s="29" t="s">
         <v>2515</v>
       </c>
-      <c r="H525" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I525" s="18" t="s">
-        <v>596</v>
-      </c>
-      <c r="J525" s="18" t="s">
-        <v>2516</v>
-      </c>
-      <c r="K525" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L525" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M525" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N525" s="14" t="str">
+      <c r="K525" s="16" t="s">
+        <v>2497</v>
+      </c>
+      <c r="L525" s="35" t="s">
+        <v>2497</v>
+      </c>
+      <c r="M525" s="35" t="s">
+        <v>2497</v>
+      </c>
+      <c r="N525" s="36" t="str">
         <f t="shared" si="17"/>
         <v>{"decimal":"60170","namebowtie":"brand-jenkins","namemdl2":"null","codebowtie":"EB0A","codemdl2":"null","stylevariation":"bold","keywords":["build","source","external","jenkins","brand","logo"],"subset":"VSTS","group":"Brand","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
       </c>
     </row>
-    <row r="526" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A526" s="18">
+    <row r="526" spans="1:14" s="27" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A526" s="29">
         <v>60171</v>
       </c>
-      <c r="B526" s="17" t="s">
-        <v>2544</v>
-      </c>
-      <c r="C526" s="18" t="s">
-        <v>2517</v>
-      </c>
-      <c r="D526" s="18" t="str">
+      <c r="B526" s="26" t="s">
+        <v>2543</v>
+      </c>
+      <c r="C526" s="29" t="s">
+        <v>2516</v>
+      </c>
+      <c r="D526" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB0B</v>
       </c>
-      <c r="E526" s="18">
+      <c r="E526" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F526" s="18" t="s">
+      <c r="F526" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G526" t="s">
-        <v>2519</v>
-      </c>
-      <c r="H526" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I526" s="18" t="s">
+      <c r="G526" s="27" t="s">
+        <v>2518</v>
+      </c>
+      <c r="H526" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I526" s="29" t="s">
         <v>588</v>
       </c>
-      <c r="J526" t="s">
+      <c r="J526" s="27" t="s">
         <v>921</v>
       </c>
-      <c r="K526" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L526" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M526" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N526" s="14" t="str">
+      <c r="K526" s="16" t="s">
+        <v>2611</v>
+      </c>
+      <c r="L526" s="35" t="s">
+        <v>2610</v>
+      </c>
+      <c r="M526" s="35" t="s">
+        <v>2609</v>
+      </c>
+      <c r="N526" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60171","namebowtie":"symbol-issue","namemdl2":"null","codebowtie":"EB0B","codemdl2":"null","stylevariation":"bold","keywords":["symbol","work","item","issue","task","exclamation"],"subset":"VSTS","group":"Work","usagenotes":"Work item type indicator."}</v>
-      </c>
-    </row>
-    <row r="527" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A527" s="18">
+        <v>{"decimal":"60171","namebowtie":"symbol-issue","namemdl2":"IssueSolid","codebowtie":"EB0B","codemdl2":"F448","stylevariation":"bold","keywords":["symbol","work","item","issue","task","exclamation"],"subset":"VSTS","group":"Work","usagenotes":"Work item type indicator."}</v>
+      </c>
+    </row>
+    <row r="527" spans="1:14" s="27" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A527" s="29">
         <v>60172</v>
       </c>
-      <c r="B527" s="17" t="s">
-        <v>2545</v>
-      </c>
-      <c r="C527" s="18" t="s">
-        <v>2518</v>
-      </c>
-      <c r="D527" s="18" t="str">
+      <c r="B527" s="26" t="s">
+        <v>2544</v>
+      </c>
+      <c r="C527" s="29" t="s">
+        <v>2517</v>
+      </c>
+      <c r="D527" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB0C</v>
       </c>
-      <c r="E527" s="18">
+      <c r="E527" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F527" s="18" t="s">
+      <c r="F527" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G527" t="s">
-        <v>2520</v>
-      </c>
-      <c r="H527" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I527" s="18" t="s">
+      <c r="G527" s="27" t="s">
+        <v>2519</v>
+      </c>
+      <c r="H527" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I527" s="29" t="s">
         <v>588</v>
       </c>
-      <c r="J527" t="s">
+      <c r="J527" s="27" t="s">
         <v>921</v>
       </c>
-      <c r="K527" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L527" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M527" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N527" s="14" t="str">
+      <c r="K527" s="16" t="s">
+        <v>2614</v>
+      </c>
+      <c r="L527" s="35" t="s">
+        <v>2613</v>
+      </c>
+      <c r="M527" s="35" t="s">
+        <v>2612</v>
+      </c>
+      <c r="N527" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60172","namebowtie":"symbol-defect","namemdl2":"null","codebowtie":"EB0C","codemdl2":"null","stylevariation":"bold","keywords":["symbol","work","item","defect","lightbulb","crack","broken"],"subset":"VSTS","group":"Work","usagenotes":"Work item type indicator."}</v>
-      </c>
-    </row>
-    <row r="528" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A528" s="18">
+        <v>{"decimal":"60172","namebowtie":"symbol-defect","namemdl2":"DefectSolid","codebowtie":"EB0C","codemdl2":"F449","stylevariation":"bold","keywords":["symbol","work","item","defect","lightbulb","crack","broken"],"subset":"VSTS","group":"Work","usagenotes":"Work item type indicator."}</v>
+      </c>
+    </row>
+    <row r="528" spans="1:14" s="27" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A528" s="29">
         <v>60173</v>
       </c>
-      <c r="B528" s="17" t="s">
-        <v>2569</v>
-      </c>
-      <c r="C528" s="18" t="s">
-        <v>2529</v>
-      </c>
-      <c r="D528" s="18" t="str">
+      <c r="B528" s="26" t="s">
+        <v>2568</v>
+      </c>
+      <c r="C528" s="29" t="s">
+        <v>2528</v>
+      </c>
+      <c r="D528" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB0D</v>
       </c>
-      <c r="E528" s="18">
+      <c r="E528" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F528" s="18" t="s">
+      <c r="F528" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G528" s="18" t="s">
+      <c r="G528" s="29" t="s">
+        <v>2529</v>
+      </c>
+      <c r="H528" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I528" s="29" t="s">
+        <v>584</v>
+      </c>
+      <c r="J528" s="29" t="s">
         <v>2530</v>
       </c>
-      <c r="H528" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I528" s="18" t="s">
-        <v>584</v>
-      </c>
-      <c r="J528" s="18" t="s">
+      <c r="K528" s="16" t="s">
+        <v>2619</v>
+      </c>
+      <c r="L528" s="35" t="s">
+        <v>2618</v>
+      </c>
+      <c r="M528" s="35" t="s">
+        <v>2617</v>
+      </c>
+      <c r="N528" s="36" t="str">
+        <f t="shared" si="17"/>
+        <v>{"decimal":"60173","namebowtie":"login","namemdl2":"IDBadge","codebowtie":"EB0D","codemdl2":"F427","stylevariation":"light","keywords":["login","account","credential","user","password","lock","security"],"subset":"VSTS","group":"Common","usagenotes":"Used in top nav Credentials command."}</v>
+      </c>
+    </row>
+    <row r="529" spans="1:14" s="27" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A529" s="29">
+        <v>60174</v>
+      </c>
+      <c r="B529" s="26" t="s">
+        <v>2569</v>
+      </c>
+      <c r="C529" s="29" t="s">
         <v>2531</v>
       </c>
-      <c r="K528" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L528" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M528" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N528" s="14" t="str">
-        <f t="shared" si="17"/>
-        <v>{"decimal":"60173","namebowtie":"login","namemdl2":"null","codebowtie":"EB0D","codemdl2":"null","stylevariation":"light","keywords":["login","account","credential","user","password","lock","security"],"subset":"VSTS","group":"Common","usagenotes":"Used in top nav Credentials command."}</v>
-      </c>
-    </row>
-    <row r="529" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A529" s="18">
-        <v>60174</v>
-      </c>
-      <c r="B529" s="17" t="s">
-        <v>2570</v>
-      </c>
-      <c r="C529" s="18" t="s">
-        <v>2532</v>
-      </c>
-      <c r="D529" s="18" t="str">
+      <c r="D529" s="29" t="str">
         <f t="shared" si="16"/>
         <v>EB0E</v>
       </c>
-      <c r="E529" s="18">
+      <c r="E529" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F529" s="18" t="s">
+      <c r="F529" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G529" s="18" t="s">
-        <v>2533</v>
-      </c>
-      <c r="H529" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I529" s="18" t="s">
+      <c r="G529" s="29" t="s">
+        <v>2532</v>
+      </c>
+      <c r="H529" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I529" s="29" t="s">
         <v>588</v>
       </c>
-      <c r="J529" t="s">
+      <c r="J529" s="27" t="s">
         <v>921</v>
       </c>
-      <c r="K529" s="19" t="s">
-        <v>2497</v>
-      </c>
-      <c r="L529" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="M529" s="18" t="s">
-        <v>2497</v>
-      </c>
-      <c r="N529" s="14" t="str">
+      <c r="K529" s="16" t="s">
+        <v>2620</v>
+      </c>
+      <c r="L529" s="35" t="s">
+        <v>2616</v>
+      </c>
+      <c r="M529" s="35" t="s">
+        <v>2615</v>
+      </c>
+      <c r="N529" s="36" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60174","namebowtie":"symbol-ladybug","namemdl2":"null","codebowtie":"EB0E","codemdl2":"null","stylevariation":"bold","keywords":["symbol","work","item","ladybug","bug"],"subset":"VSTS","group":"Work","usagenotes":"Work item type indicator."}</v>
+        <v>{"decimal":"60174","namebowtie":"symbol-ladybug","namemdl2":"LadybugSolid","codebowtie":"EB0E","codemdl2":"F44A","stylevariation":"bold","keywords":["symbol","work","item","ladybug","bug"],"subset":"VSTS","group":"Work","usagenotes":"Work item type indicator."}</v>
       </c>
     </row>
     <row r="530" spans="1:14" customFormat="1" ht="32.1" customHeight="1"/>
@@ -32973,456 +33012,129 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" style="26" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="26" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" style="26" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="7.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="24" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>2496</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
+        <v>2523</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>2524</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>2525</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>2607</v>
+      <c r="D1" s="22" t="s">
+        <v>2580</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="32.1" customHeight="1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>2475</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="30" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="31" t="s">
+        <v>2570</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="32.1" customHeight="1">
+      <c r="A3" s="26" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="32.1" customHeight="1">
+      <c r="A4" s="26" t="s">
+        <v>2476</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="31" t="s">
         <v>2571</v>
       </c>
-      <c r="D2" s="26" t="s">
-        <v>2608</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="32.1" customHeight="1">
-      <c r="A3" s="28" t="s">
-        <v>1094</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>240</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>1093</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>2608</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="32.1" customHeight="1">
-      <c r="A4" s="28" t="s">
-        <v>2476</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="C4" s="35" t="s">
+    </row>
+    <row r="5" spans="1:8" ht="32.1" customHeight="1">
+      <c r="A5" s="26" t="s">
+        <v>2477</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" s="31" t="s">
         <v>2572</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="32.1" customHeight="1">
-      <c r="A5" s="28" t="s">
-        <v>2477</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>243</v>
-      </c>
-      <c r="C5" s="35" t="s">
+      <c r="D5" s="24" t="s">
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="32.1" customHeight="1">
+      <c r="A6" s="26" t="s">
+        <v>2480</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="C6" s="31" t="s">
         <v>2573</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>2608</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="32.1" customHeight="1">
-      <c r="A6" s="28" t="s">
-        <v>2480</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>246</v>
-      </c>
-      <c r="C6" s="35" t="s">
-        <v>2576</v>
-      </c>
     </row>
     <row r="7" spans="1:8" ht="32.1" customHeight="1">
-      <c r="A7" s="28" t="s">
-        <v>2580</v>
-      </c>
-      <c r="B7" s="34" t="s">
+      <c r="A7" s="26" t="s">
+        <v>2577</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>914</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>2577</v>
+      <c r="C7" s="24" t="s">
+        <v>2574</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="34.5">
-      <c r="A8" s="28" t="s">
-        <v>2541</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>2507</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>2589</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>2608</v>
-      </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="A8" s="26" t="s">
+        <v>2540</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>2506</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>2578</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>2581</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" ht="34.5">
-      <c r="A9" s="28" t="s">
-        <v>2543</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>2510</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>2590</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="9.140625" style="31"/>
-    <col min="4" max="4" width="32.7109375" style="31" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" style="31" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="31"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" s="32" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A1" s="30" t="s">
-        <v>2496</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>2524</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>2525</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>2523</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>2581</v>
-      </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-    </row>
-    <row r="2" spans="1:24" s="33" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A2" s="28" t="s">
-        <v>1083</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>1072</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>2591</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>2609</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" s="33" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A3" s="28" t="s">
-        <v>1082</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>1075</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>2592</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>1077</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>2610</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" s="33" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A4" s="28" t="s">
-        <v>1081</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>2593</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>1080</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>2582</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" s="33" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A5" s="28" t="s">
-        <v>2538</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>2500</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>2594</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>2504</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>2585</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" s="33" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A6" s="28" t="s">
-        <v>2539</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>2501</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>2595</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>2505</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>2585</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" s="33" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A7" s="28" t="s">
-        <v>2379</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>2498</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>2378</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>2499</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>2583</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="32.1" customHeight="1">
-      <c r="A8" s="28" t="s">
-        <v>2540</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>2506</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>2596</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>2516</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>2584</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="32.1" customHeight="1">
-      <c r="A9" s="28" t="s">
-        <v>2197</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>2508</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>2196</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>2516</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>2586</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="32.1" customHeight="1">
-      <c r="A10" s="28" t="s">
+      <c r="A9" s="26" t="s">
         <v>2542</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B9" s="25" t="s">
         <v>2509</v>
       </c>
-      <c r="C10" s="33" t="s">
-        <v>2597</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>2516</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="32.1" customHeight="1">
-      <c r="A11" s="28" t="s">
-        <v>2544</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>2517</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>2598</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>921</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>2587</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="32.1" customHeight="1">
-      <c r="A12" s="28" t="s">
-        <v>2545</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>2518</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>2599</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>921</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>2588</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" ht="32.1" customHeight="1">
-      <c r="A13" s="28" t="s">
-        <v>2569</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>2529</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>2600</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>2531</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>2606</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="32.1" customHeight="1">
-      <c r="A14" s="28" t="s">
-        <v>2570</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>2532</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>2601</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>921</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>2588</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="34.5">
-      <c r="A15" s="28" t="s">
-        <v>1592</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>242</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>1591</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>2603</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>2602</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="34.5">
-      <c r="A16" s="28" t="s">
-        <v>2478</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>2574</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>2604</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>2602</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="34.5">
-      <c r="A17" s="28" t="s">
-        <v>2479</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="C17" s="35" t="s">
-        <v>2575</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>2605</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>2602</v>
+      <c r="C9" s="25" t="s">
+        <v>2579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excluded generating that empty placeholder glyph
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -8496,8 +8496,8 @@
   <dimension ref="A1:AH533"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A521" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E527" sqref="E527"/>
+      <pane ySplit="2" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H531" sqref="H531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>

</xml_diff>

<commit_message>
Added paste option icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5330" uniqueCount="2635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5348" uniqueCount="2642">
   <si>
     <t>keywords</t>
   </si>
@@ -7933,6 +7933,27 @@
   </si>
   <si>
     <t>symbol work item type bug ladybug insect</t>
+  </si>
+  <si>
+    <t>paste-as-text</t>
+  </si>
+  <si>
+    <t>paste-as-html</t>
+  </si>
+  <si>
+    <t>paste clipboard text letter</t>
+  </si>
+  <si>
+    <t>paste clipboard code html brackets</t>
+  </si>
+  <si>
+    <t>Wiki</t>
+  </si>
+  <si>
+    <t>Used in Wiki editor toolbar for pasting as plain text.</t>
+  </si>
+  <si>
+    <t>Used in Wiki editor toolbar for pasting as HTML.</t>
   </si>
 </sst>
 </file>
@@ -8496,8 +8517,8 @@
   <dimension ref="A1:AH533"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A524" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H531" sqref="H531"/>
+      <pane ySplit="2" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G529" sqref="G529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -32363,7 +32384,7 @@
         <v>1070</v>
       </c>
       <c r="D515" s="29" t="str">
-        <f t="shared" ref="D515:D530" si="16">DEC2HEX(A515)</f>
+        <f t="shared" ref="D515:D532" si="16">DEC2HEX(A515)</f>
         <v>EB00</v>
       </c>
       <c r="E515" s="29">
@@ -32394,7 +32415,7 @@
         <v>2581</v>
       </c>
       <c r="N515" s="14" t="str">
-        <f t="shared" ref="N515:N530" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
+        <f t="shared" ref="N515:N532" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
         <v>{"decimal":"60160","namebowtie":"file-lock","namemdl2":"PageLock","codebowtie":"EB00","codemdl2":"F43F","stylevariation":"light","keywords":["file","document","lock","permission"],"subset":"VSTS","group":"Common","usagenotes":"Used to represent the user does not have permission to a file."}</v>
       </c>
     </row>
@@ -33022,10 +33043,7 @@
       <c r="M529" s="41" t="s">
         <v>2495</v>
       </c>
-      <c r="N529" s="42" t="str">
-        <f t="shared" si="17"/>
-        <v>{"decimal":"60174","namebowtie":"placeholder","namemdl2":"null","codebowtie":"null","codemdl2":"null","stylevariation":"","keywords":[""],"subset":"","group":"","usagenotes":"Empty codepoint due to deleted glyph."}</v>
-      </c>
+      <c r="N529" s="42"/>
     </row>
     <row r="530" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
       <c r="A530" s="29">
@@ -33070,8 +33088,92 @@
         <v>{"decimal":"60175","namebowtie":"brand-ivy","namemdl2":"null","codebowtie":"EB0F","codemdl2":"null","stylevariation":"bold","keywords":["brand","apache","ivy","package","feed"],"subset":"VSTS","group":"Package","usagenotes":"Used in Packages hub for Apache Ivy package feeds."}</v>
       </c>
     </row>
-    <row r="531" spans="1:14" customFormat="1" ht="32.1" customHeight="1"/>
-    <row r="532" spans="1:14" customFormat="1" ht="32.1" customHeight="1"/>
+    <row r="531" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A531" s="36">
+        <v>60176</v>
+      </c>
+      <c r="C531" s="29" t="s">
+        <v>2635</v>
+      </c>
+      <c r="D531" s="29" t="str">
+        <f t="shared" si="16"/>
+        <v>EB10</v>
+      </c>
+      <c r="E531" s="29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F531" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G531" s="29" t="s">
+        <v>2637</v>
+      </c>
+      <c r="H531" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I531" s="29" t="s">
+        <v>2639</v>
+      </c>
+      <c r="J531" s="27" t="s">
+        <v>2640</v>
+      </c>
+      <c r="K531" s="16" t="s">
+        <v>2495</v>
+      </c>
+      <c r="L531" s="16" t="s">
+        <v>2495</v>
+      </c>
+      <c r="M531" s="16" t="s">
+        <v>2495</v>
+      </c>
+      <c r="N531" s="14" t="str">
+        <f t="shared" si="17"/>
+        <v>{"decimal":"60176","namebowtie":"paste-as-text","namemdl2":"null","codebowtie":"EB10","codemdl2":"null","stylevariation":"light","keywords":["paste","clipboard","text","letter"],"subset":"VSTS","group":"Wiki","usagenotes":"Used in Wiki editor toolbar for pasting as plain text."}</v>
+      </c>
+    </row>
+    <row r="532" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A532" s="29">
+        <v>60177</v>
+      </c>
+      <c r="C532" s="29" t="s">
+        <v>2636</v>
+      </c>
+      <c r="D532" s="29" t="str">
+        <f t="shared" si="16"/>
+        <v>EB11</v>
+      </c>
+      <c r="E532" s="29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F532" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G532" s="29" t="s">
+        <v>2638</v>
+      </c>
+      <c r="H532" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I532" s="29" t="s">
+        <v>2639</v>
+      </c>
+      <c r="J532" s="27" t="s">
+        <v>2641</v>
+      </c>
+      <c r="K532" s="16" t="s">
+        <v>2495</v>
+      </c>
+      <c r="L532" s="16" t="s">
+        <v>2495</v>
+      </c>
+      <c r="M532" s="16" t="s">
+        <v>2495</v>
+      </c>
+      <c r="N532" s="14" t="str">
+        <f t="shared" si="17"/>
+        <v>{"decimal":"60177","namebowtie":"paste-as-html","namemdl2":"null","codebowtie":"EB11","codemdl2":"null","stylevariation":"light","keywords":["paste","clipboard","code","html","brackets"],"subset":"VSTS","group":"Wiki","usagenotes":"Used in Wiki editor toolbar for pasting as HTML."}</v>
+      </c>
+    </row>
     <row r="533" spans="1:14" customFormat="1" ht="32.1" customHeight="1"/>
   </sheetData>
   <sortState ref="A3:N529">

</xml_diff>

<commit_message>
Added toll icon for Gate in Release hub
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5369" uniqueCount="2649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5378" uniqueCount="2655">
   <si>
     <t>keywords</t>
   </si>
@@ -7975,6 +7975,24 @@
   </si>
   <si>
     <t>E7C6</t>
+  </si>
+  <si>
+    <t>toll</t>
+  </si>
+  <si>
+    <t>toll gate block guard traffic stop</t>
+  </si>
+  <si>
+    <t>Gate icon used in Release hub. A gate is a checklist before approving or rejecting a release.</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>F160</t>
+  </si>
+  <si>
+    <t>Toll</t>
   </si>
 </sst>
 </file>
@@ -8536,11 +8554,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AH534"/>
+  <dimension ref="A1:AH535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A534" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L539" sqref="L539"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A528" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G531" sqref="G531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -32406,7 +32424,7 @@
         <v>1067</v>
       </c>
       <c r="D515" s="29" t="str">
-        <f t="shared" ref="D515:D534" si="16">DEC2HEX(A515)</f>
+        <f t="shared" ref="D515:D535" si="16">DEC2HEX(A515)</f>
         <v>EB00</v>
       </c>
       <c r="E515" s="29">
@@ -32437,7 +32455,7 @@
         <v>2575</v>
       </c>
       <c r="N515" s="14" t="str">
-        <f t="shared" ref="N515:N534" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
+        <f t="shared" ref="N515:N535" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
         <v>{"decimal":"60160","namebowtie":"file-lock","namemdl2":"PageLock","codebowtie":"EB00","codemdl2":"F43F","stylevariation":"light","keywords":["file","document","lock","permission"],"subset":"VSTS","group":"Common","usagenotes":"Used to represent the user does not have permission to a file."}</v>
       </c>
     </row>
@@ -33294,6 +33312,49 @@
       <c r="N534" s="14" t="str">
         <f t="shared" si="17"/>
         <v>{"decimal":"60179","namebowtie":"brand-linux","namemdl2":"null","codebowtie":"EB13","codemdl2":"null","stylevariation":"bold","keywords":["linux","tux","penguin"],"subset":"VSTS","group":"Brand","usagenotes":"Linux logo. Used in Build queue picker."}</v>
+      </c>
+    </row>
+    <row r="535" spans="1:14" ht="32.1" customHeight="1">
+      <c r="A535" s="29">
+        <v>60180</v>
+      </c>
+      <c r="C535" s="2" t="s">
+        <v>2649</v>
+      </c>
+      <c r="D535" s="29" t="str">
+        <f t="shared" si="16"/>
+        <v>EB14</v>
+      </c>
+      <c r="E535" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F535" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G535" s="2" t="s">
+        <v>2650</v>
+      </c>
+      <c r="H535" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I535" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="J535" s="2" t="s">
+        <v>2651</v>
+      </c>
+      <c r="K535" s="16" t="s">
+        <v>2652</v>
+      </c>
+      <c r="L535" s="34" t="s">
+        <v>2654</v>
+      </c>
+      <c r="M535" s="33" t="s">
+        <v>2653</v>
+      </c>
+      <c r="N535" s="14" t="str">
+        <f t="shared" si="17"/>
+        <v>{"decimal":"60180","namebowtie":"toll","namemdl2":"Toll","codebowtie":"EB14","codemdl2":"F160","stylevariation":"light","keywords":["toll","gate","block","guard","traffic","stop"],"subset":"VSTS","group":"Build","usagenotes":"Gate icon used in Release hub. A gate is a checklist before approving or rejecting a release."}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added generic work item type icon
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5387" uniqueCount="2658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5396" uniqueCount="2661">
   <si>
     <t>keywords</t>
   </si>
@@ -8002,6 +8002,15 @@
   </si>
   <si>
     <t>Gradle logo. Used in Build hub.</t>
+  </si>
+  <si>
+    <t>symbol-work</t>
+  </si>
+  <si>
+    <t>symbol work item generic pencil</t>
+  </si>
+  <si>
+    <t>Default work item type indicator.</t>
   </si>
 </sst>
 </file>
@@ -8563,11 +8572,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AH536"/>
+  <dimension ref="A1:AH537"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A528" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N535" sqref="N535:N536"/>
+      <pane ySplit="2" topLeftCell="A534" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F536" sqref="F536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -32433,7 +32442,7 @@
         <v>1067</v>
       </c>
       <c r="D515" s="29" t="str">
-        <f t="shared" ref="D515:D536" si="16">DEC2HEX(A515)</f>
+        <f t="shared" ref="D515:D537" si="16">DEC2HEX(A515)</f>
         <v>EB00</v>
       </c>
       <c r="E515" s="29">
@@ -32464,7 +32473,7 @@
         <v>2575</v>
       </c>
       <c r="N515" s="14" t="str">
-        <f t="shared" ref="N515:N536" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
+        <f t="shared" ref="N515:N537" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
         <v>{"decimal":"60160","namebowtie":"file-lock","namemdl2":"PageLock","codebowtie":"EB00","codemdl2":"F43F","stylevariation":"light","keywords":["file","document","lock","permission"],"subset":"VSTS","group":"Common","usagenotes":"Used to represent the user does not have permission to a file."}</v>
       </c>
     </row>
@@ -33407,6 +33416,49 @@
       <c r="N536" s="14" t="str">
         <f t="shared" si="17"/>
         <v>{"decimal":"60181","namebowtie":"brand-gradle","namemdl2":"null","codebowtie":"EB15","codemdl2":"null","stylevariation":"bold","keywords":["brand","logo","gradle","elephant","build"],"subset":"VSTS","group":"Build","usagenotes":"Gradle logo. Used in Build hub."}</v>
+      </c>
+    </row>
+    <row r="537" spans="1:14" ht="32.1" customHeight="1">
+      <c r="A537" s="29">
+        <v>60182</v>
+      </c>
+      <c r="C537" s="2" t="s">
+        <v>2658</v>
+      </c>
+      <c r="D537" s="29" t="str">
+        <f t="shared" si="16"/>
+        <v>EB16</v>
+      </c>
+      <c r="E537" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F537" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G537" t="s">
+        <v>2659</v>
+      </c>
+      <c r="H537" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I537" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="J537" t="s">
+        <v>2660</v>
+      </c>
+      <c r="K537" s="16" t="s">
+        <v>2489</v>
+      </c>
+      <c r="L537" s="16" t="s">
+        <v>2489</v>
+      </c>
+      <c r="M537" s="16" t="s">
+        <v>2489</v>
+      </c>
+      <c r="N537" s="14" t="str">
+        <f t="shared" si="17"/>
+        <v>{"decimal":"60182","namebowtie":"symbol-work","namemdl2":"null","codebowtie":"EB16","codemdl2":"null","stylevariation":"bold","keywords":["symbol","work","item","generic","pencil"],"subset":"VSTS","group":"Work","usagenotes":"Default work item type indicator."}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Matched Bowtie full-screen icons to MDL2
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5396" uniqueCount="2661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5396" uniqueCount="2674">
   <si>
     <t>keywords</t>
   </si>
@@ -8007,10 +8007,49 @@
     <t>symbol-work</t>
   </si>
   <si>
-    <t>symbol work item generic pencil</t>
-  </si>
-  <si>
     <t>Default work item type indicator.</t>
+  </si>
+  <si>
+    <t>trigger lightning bolt event</t>
+  </si>
+  <si>
+    <t>trigger lightning bolt event auto gear cog</t>
+  </si>
+  <si>
+    <t>trigger lightning bolt event user manual</t>
+  </si>
+  <si>
+    <t>Used in Test hub for trigger.</t>
+  </si>
+  <si>
+    <t>Used in Test hub for auto trigger.</t>
+  </si>
+  <si>
+    <t>Used in Test hub for trigger that requires manual intervention.</t>
+  </si>
+  <si>
+    <t>symbol work item generic clipboard</t>
+  </si>
+  <si>
+    <t>work item clipboard checkmark task</t>
+  </si>
+  <si>
+    <t>work item bug exclamation bang clipboard</t>
+  </si>
+  <si>
+    <t>work item clipboard checkmark task move arrow</t>
+  </si>
+  <si>
+    <t>full screen arrow expand</t>
+  </si>
+  <si>
+    <t>full screen exit arrow collapse</t>
+  </si>
+  <si>
+    <t>Expand to full screen.</t>
+  </si>
+  <si>
+    <t>Exit full screen.</t>
   </si>
 </sst>
 </file>
@@ -8153,7 +8192,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8251,7 +8290,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -8572,11 +8610,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AH537"/>
+  <dimension ref="A1:AH538"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A534" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F536" sqref="F536"/>
+      <pane ySplit="2" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C212" sqref="C212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -18373,10 +18411,10 @@
         <v>1</v>
       </c>
       <c r="F209" t="s">
-        <v>2489</v>
+        <v>11</v>
       </c>
       <c r="G209" t="s">
-        <v>2489</v>
+        <v>2670</v>
       </c>
       <c r="H209" t="s">
         <v>9</v>
@@ -18385,7 +18423,7 @@
         <v>594</v>
       </c>
       <c r="J209" t="s">
-        <v>2489</v>
+        <v>2672</v>
       </c>
       <c r="K209" s="16" t="s">
         <v>1939</v>
@@ -18398,7 +18436,7 @@
       </c>
       <c r="N209" s="14" t="str">
         <f t="shared" si="7"/>
-        <v>{"decimal":"59854","namebowtie":"view-full-screen","namemdl2":"FullScreen","codebowtie":"E9CE","codemdl2":"E740","stylevariation":"null","keywords":["null"],"subset":"VSTS","group":"Control","usagenotes":"null"}</v>
+        <v>{"decimal":"59854","namebowtie":"view-full-screen","namemdl2":"FullScreen","codebowtie":"E9CE","codemdl2":"E740","stylevariation":"light","keywords":["full","screen","arrow","expand"],"subset":"VSTS","group":"Control","usagenotes":"Expand to full screen."}</v>
       </c>
     </row>
     <row r="210" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
@@ -18419,10 +18457,10 @@
         <v>1</v>
       </c>
       <c r="F210" t="s">
-        <v>2489</v>
+        <v>11</v>
       </c>
       <c r="G210" t="s">
-        <v>2489</v>
+        <v>2671</v>
       </c>
       <c r="H210" t="s">
         <v>9</v>
@@ -18431,7 +18469,7 @@
         <v>594</v>
       </c>
       <c r="J210" t="s">
-        <v>2489</v>
+        <v>2673</v>
       </c>
       <c r="K210" s="16" t="s">
         <v>1936</v>
@@ -18444,7 +18482,7 @@
       </c>
       <c r="N210" s="14" t="str">
         <f t="shared" si="7"/>
-        <v>{"decimal":"59855","namebowtie":"view-full-screen-exit","namemdl2":"BackToWindow","codebowtie":"E9CF","codemdl2":"E73F","stylevariation":"null","keywords":["null"],"subset":"VSTS","group":"Control","usagenotes":"null"}</v>
+        <v>{"decimal":"59855","namebowtie":"view-full-screen-exit","namemdl2":"BackToWindow","codebowtie":"E9CF","codemdl2":"E73F","stylevariation":"light","keywords":["full","screen","exit","arrow","collapse"],"subset":"VSTS","group":"Control","usagenotes":"Exit full screen."}</v>
       </c>
     </row>
     <row r="211" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
@@ -22148,7 +22186,7 @@
         <v>2489</v>
       </c>
       <c r="G291" t="s">
-        <v>2489</v>
+        <v>2660</v>
       </c>
       <c r="H291" t="s">
         <v>9</v>
@@ -22157,7 +22195,7 @@
         <v>567</v>
       </c>
       <c r="J291" t="s">
-        <v>2489</v>
+        <v>2663</v>
       </c>
       <c r="K291" s="16" t="s">
         <v>1744</v>
@@ -22170,7 +22208,7 @@
       </c>
       <c r="N291" s="14" t="str">
         <f t="shared" si="9"/>
-        <v>{"decimal":"59936","namebowtie":"trigger","namemdl2":"LightningBolt","codebowtie":"EA20","codemdl2":"E945","stylevariation":"null","keywords":["null"],"subset":"VSTS","group":"Test","usagenotes":"null"}</v>
+        <v>{"decimal":"59936","namebowtie":"trigger","namemdl2":"LightningBolt","codebowtie":"EA20","codemdl2":"E945","stylevariation":"null","keywords":["trigger","lightning","bolt","event"],"subset":"VSTS","group":"Test","usagenotes":"Used in Test hub for trigger."}</v>
       </c>
     </row>
     <row r="292" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
@@ -22194,7 +22232,7 @@
         <v>2489</v>
       </c>
       <c r="G292" t="s">
-        <v>2489</v>
+        <v>2661</v>
       </c>
       <c r="H292" t="s">
         <v>9</v>
@@ -22203,7 +22241,7 @@
         <v>567</v>
       </c>
       <c r="J292" t="s">
-        <v>2489</v>
+        <v>2664</v>
       </c>
       <c r="K292" s="16" t="s">
         <v>1741</v>
@@ -22216,7 +22254,7 @@
       </c>
       <c r="N292" s="14" t="str">
         <f t="shared" si="9"/>
-        <v>{"decimal":"59937","namebowtie":"trigger-auto","namemdl2":"TriggerAuto","codebowtie":"EA21","codemdl2":"F24A","stylevariation":"null","keywords":["null"],"subset":"VSTS","group":"Test","usagenotes":"null"}</v>
+        <v>{"decimal":"59937","namebowtie":"trigger-auto","namemdl2":"TriggerAuto","codebowtie":"EA21","codemdl2":"F24A","stylevariation":"null","keywords":["trigger","lightning","bolt","event","auto","gear","cog"],"subset":"VSTS","group":"Test","usagenotes":"Used in Test hub for auto trigger."}</v>
       </c>
     </row>
     <row r="293" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
@@ -22240,7 +22278,7 @@
         <v>2489</v>
       </c>
       <c r="G293" t="s">
-        <v>2489</v>
+        <v>2662</v>
       </c>
       <c r="H293" t="s">
         <v>9</v>
@@ -22249,7 +22287,7 @@
         <v>567</v>
       </c>
       <c r="J293" t="s">
-        <v>2489</v>
+        <v>2665</v>
       </c>
       <c r="K293" s="16" t="s">
         <v>1738</v>
@@ -22262,7 +22300,7 @@
       </c>
       <c r="N293" s="14" t="str">
         <f t="shared" si="9"/>
-        <v>{"decimal":"59938","namebowtie":"trigger-user","namemdl2":"TriggerUser","codebowtie":"EA22","codemdl2":"F24B","stylevariation":"null","keywords":["null"],"subset":"VSTS","group":"Test","usagenotes":"null"}</v>
+        <v>{"decimal":"59938","namebowtie":"trigger-user","namemdl2":"TriggerUser","codebowtie":"EA22","codemdl2":"F24B","stylevariation":"null","keywords":["trigger","lightning","bolt","event","user","manual"],"subset":"VSTS","group":"Test","usagenotes":"Used in Test hub for trigger that requires manual intervention."}</v>
       </c>
     </row>
     <row r="294" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
@@ -23712,7 +23750,7 @@
         <v>2489</v>
       </c>
       <c r="G325" t="s">
-        <v>2489</v>
+        <v>2667</v>
       </c>
       <c r="H325" t="s">
         <v>9</v>
@@ -23734,7 +23772,7 @@
       </c>
       <c r="N325" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>{"decimal":"59970","namebowtie":"work-item","namemdl2":"WorkItem","codebowtie":"EA42","codemdl2":"F314","stylevariation":"null","keywords":["null"],"subset":"VSTS","group":"Work","usagenotes":"null"}</v>
+        <v>{"decimal":"59970","namebowtie":"work-item","namemdl2":"WorkItem","codebowtie":"EA42","codemdl2":"F314","stylevariation":"null","keywords":["work","item","clipboard","checkmark","task"],"subset":"VSTS","group":"Work","usagenotes":"null"}</v>
       </c>
     </row>
     <row r="326" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
@@ -23758,7 +23796,7 @@
         <v>2489</v>
       </c>
       <c r="G326" t="s">
-        <v>2489</v>
+        <v>2668</v>
       </c>
       <c r="H326" t="s">
         <v>9</v>
@@ -23780,7 +23818,7 @@
       </c>
       <c r="N326" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>{"decimal":"59971","namebowtie":"work-item-bug","namemdl2":"WorkItemBug","codebowtie":"EA43","codemdl2":"F315","stylevariation":"null","keywords":["null"],"subset":"VSTS","group":"Work","usagenotes":"null"}</v>
+        <v>{"decimal":"59971","namebowtie":"work-item-bug","namemdl2":"WorkItemBug","codebowtie":"EA43","codemdl2":"F315","stylevariation":"null","keywords":["work","item","bug","exclamation","bang","clipboard"],"subset":"VSTS","group":"Work","usagenotes":"null"}</v>
       </c>
     </row>
     <row r="327" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
@@ -23804,7 +23842,7 @@
         <v>2489</v>
       </c>
       <c r="G327" t="s">
-        <v>2489</v>
+        <v>2669</v>
       </c>
       <c r="H327" t="s">
         <v>9</v>
@@ -23826,7 +23864,7 @@
       </c>
       <c r="N327" s="14" t="str">
         <f t="shared" si="11"/>
-        <v>{"decimal":"59972","namebowtie":"work-item-move","namemdl2":"Assign","codebowtie":"EA44","codemdl2":"E9D3","stylevariation":"null","keywords":["null"],"subset":"VSTS","group":"Work","usagenotes":"null"}</v>
+        <v>{"decimal":"59972","namebowtie":"work-item-move","namemdl2":"Assign","codebowtie":"EA44","codemdl2":"E9D3","stylevariation":"null","keywords":["work","item","clipboard","checkmark","task","move","arrow"],"subset":"VSTS","group":"Work","usagenotes":"null"}</v>
       </c>
     </row>
     <row r="328" spans="1:14" customFormat="1" ht="32.1" customHeight="1">
@@ -27504,7 +27542,7 @@
       <c r="M407" s="40" t="s">
         <v>1419</v>
       </c>
-      <c r="N407" s="40" t="str">
+      <c r="N407" s="14" t="str">
         <f t="shared" si="13"/>
         <v>{"decimal":"60052","namebowtie":"git-fork","namemdl2":"BranchFork2","codebowtie":"EA94","codemdl2":"F291","stylevariation":"light","keywords":["version","control","fork","git","diamond","brand"],"subset":"VSTS","group":"Version Control","usagenotes":"Used in Code hub for forked repos and the action of forking a repo."}</v>
       </c>
@@ -33112,7 +33150,7 @@
       <c r="M529" s="35" t="s">
         <v>2489</v>
       </c>
-      <c r="N529" s="41" t="str">
+      <c r="N529" s="14" t="str">
         <f t="shared" si="17"/>
         <v>{"decimal":"60174","namebowtie":"brand-vside","namemdl2":"null","codebowtie":"EB0E","codemdl2":"null","stylevariation":"bold","keywords":["brand","visual","studio","ide","infinity","logo"],"subset":"VSTS","group":"Brand","usagenotes":"Visual Studio IDE 2017 RTW brand icon."}</v>
       </c>
@@ -33436,7 +33474,7 @@
         <v>10</v>
       </c>
       <c r="G537" t="s">
-        <v>2659</v>
+        <v>2666</v>
       </c>
       <c r="H537" s="2" t="s">
         <v>9</v>
@@ -33445,7 +33483,7 @@
         <v>587</v>
       </c>
       <c r="J537" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
       <c r="K537" s="16" t="s">
         <v>2489</v>
@@ -33458,8 +33496,16 @@
       </c>
       <c r="N537" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60182","namebowtie":"symbol-work","namemdl2":"null","codebowtie":"EB16","codemdl2":"null","stylevariation":"bold","keywords":["symbol","work","item","generic","pencil"],"subset":"VSTS","group":"Work","usagenotes":"Default work item type indicator."}</v>
-      </c>
+        <v>{"decimal":"60182","namebowtie":"symbol-work","namemdl2":"null","codebowtie":"EB16","codemdl2":"null","stylevariation":"bold","keywords":["symbol","work","item","generic","clipboard"],"subset":"VSTS","group":"Work","usagenotes":"Default work item type indicator."}</v>
+      </c>
+    </row>
+    <row r="538" spans="1:14" ht="32.1" customHeight="1">
+      <c r="A538" s="29"/>
+      <c r="D538" s="29"/>
+      <c r="K538" s="16"/>
+      <c r="L538" s="16"/>
+      <c r="M538" s="16"/>
+      <c r="N538" s="14"/>
     </row>
   </sheetData>
   <sortState ref="A3:N529">

</xml_diff>

<commit_message>
Added file-type-yml icon, updated chart-stacked-area icon
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5399" uniqueCount="2679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5408" uniqueCount="2682">
   <si>
     <t>keywords</t>
   </si>
@@ -8064,6 +8064,15 @@
   </si>
   <si>
     <t>FileComment</t>
+  </si>
+  <si>
+    <t>file-type-yml</t>
+  </si>
+  <si>
+    <t>file type yml yaml document letter</t>
+  </si>
+  <si>
+    <t>Used for *.yml type files in Code hub file tree view.</t>
   </si>
 </sst>
 </file>
@@ -8073,7 +8082,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8153,6 +8162,16 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Bowtie"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Bowtie"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -8206,7 +8225,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8287,6 +8306,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -8607,11 +8633,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AH541"/>
+  <dimension ref="A1:AH542"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A534" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N535" sqref="N535"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -10677,7 +10703,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>47</v>
@@ -10702,7 +10728,7 @@
       </c>
       <c r="N42" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>{"decimal":"59687","namebowtie":"chart-stacked-area","namemdl2":"AreaChart","codebowtie":"E927","codemdl2":"E9D2","stylevariation":"bold","keywords":["chart","stack","area"],"subset":"VSTS","group":"Chart","usagenotes":"Stacked area chart type"}</v>
+        <v>{"decimal":"59687","namebowtie":"chart-stacked-area","namemdl2":"AreaChart","codebowtie":"E927","codemdl2":"E9D2","stylevariation":"light","keywords":["chart","stack","area"],"subset":"VSTS","group":"Chart","usagenotes":"Stacked area chart type"}</v>
       </c>
       <c r="O42" s="14"/>
     </row>
@@ -14922,7 +14948,7 @@
       <c r="A131" s="13">
         <v>59776</v>
       </c>
-      <c r="B131" s="21" t="s">
+      <c r="B131" s="34" t="s">
         <v>2488</v>
       </c>
       <c r="C131" s="2" t="s">
@@ -19810,7 +19836,7 @@
       <c r="A235">
         <v>59880</v>
       </c>
-      <c r="B235" s="21" t="s">
+      <c r="B235" s="34" t="s">
         <v>2488</v>
       </c>
       <c r="C235" t="s">
@@ -28083,7 +28109,7 @@
       <c r="A411">
         <v>60056</v>
       </c>
-      <c r="B411" s="21" t="s">
+      <c r="B411" s="34" t="s">
         <v>2488</v>
       </c>
       <c r="C411" t="s">
@@ -28130,7 +28156,7 @@
       <c r="A412">
         <v>60057</v>
       </c>
-      <c r="B412" s="21" t="s">
+      <c r="B412" s="34" t="s">
         <v>2488</v>
       </c>
       <c r="C412" t="s">
@@ -28177,7 +28203,7 @@
       <c r="A413">
         <v>60058</v>
       </c>
-      <c r="B413" s="21" t="s">
+      <c r="B413" s="34" t="s">
         <v>2488</v>
       </c>
       <c r="C413" t="s">
@@ -32978,7 +33004,7 @@
         <v>1067</v>
       </c>
       <c r="D515" s="25" t="str">
-        <f t="shared" ref="D515:D541" si="16">DEC2HEX(A515)</f>
+        <f t="shared" ref="D515:D542" si="16">DEC2HEX(A515)</f>
         <v>EB00</v>
       </c>
       <c r="E515" s="25">
@@ -33009,7 +33035,7 @@
         <v>2564</v>
       </c>
       <c r="N515" s="14" t="str">
-        <f t="shared" ref="N515:N541" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
+        <f t="shared" ref="N515:N542" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
         <v>{"decimal":"60160","namebowtie":"file-lock","namemdl2":"PageLock","codebowtie":"EB00","codemdl2":"F43F","stylevariation":"light","keywords":["file","document","lock","permission"],"subset":"VSTS","group":"Common","usagenotes":"Used to represent the user does not have permission to a file."}</v>
       </c>
       <c r="O515" s="14"/>
@@ -33687,6 +33713,7 @@
       <c r="A530" s="25">
         <v>60175</v>
       </c>
+      <c r="B530" s="35"/>
       <c r="C530" s="25" t="s">
         <v>2599</v>
       </c>
@@ -33731,6 +33758,7 @@
       <c r="A531" s="29">
         <v>60176</v>
       </c>
+      <c r="B531" s="35"/>
       <c r="C531" s="25" t="s">
         <v>2613</v>
       </c>
@@ -33775,6 +33803,7 @@
       <c r="A532" s="25">
         <v>60177</v>
       </c>
+      <c r="B532" s="35"/>
       <c r="C532" s="25" t="s">
         <v>2614</v>
       </c>
@@ -33819,6 +33848,7 @@
       <c r="A533" s="25">
         <v>60178</v>
       </c>
+      <c r="B533" s="35"/>
       <c r="C533" s="25" t="s">
         <v>2626</v>
       </c>
@@ -33863,6 +33893,7 @@
       <c r="A534" s="25">
         <v>60179</v>
       </c>
+      <c r="B534" s="36"/>
       <c r="C534" s="2" t="s">
         <v>2629</v>
       </c>
@@ -33907,6 +33938,7 @@
       <c r="A535" s="25">
         <v>60180</v>
       </c>
+      <c r="B535" s="36"/>
       <c r="C535" s="2" t="s">
         <v>2635</v>
       </c>
@@ -33951,6 +33983,7 @@
       <c r="A536" s="25">
         <v>60181</v>
       </c>
+      <c r="B536" s="36"/>
       <c r="C536" s="2" t="s">
         <v>2641</v>
       </c>
@@ -33995,6 +34028,7 @@
       <c r="A537" s="25">
         <v>60182</v>
       </c>
+      <c r="B537" s="36"/>
       <c r="C537" s="2" t="s">
         <v>2644</v>
       </c>
@@ -34039,6 +34073,7 @@
       <c r="A538" s="25">
         <v>60183</v>
       </c>
+      <c r="B538" s="36"/>
       <c r="C538" s="2" t="s">
         <v>2660</v>
       </c>
@@ -34083,6 +34118,7 @@
       <c r="A539" s="25">
         <v>60184</v>
       </c>
+      <c r="B539" s="36"/>
       <c r="C539" s="2" t="s">
         <v>2666</v>
       </c>
@@ -34127,6 +34163,7 @@
       <c r="A540" s="25">
         <v>60185</v>
       </c>
+      <c r="B540" s="36"/>
       <c r="C540" s="2" t="s">
         <v>2669</v>
       </c>
@@ -34171,6 +34208,7 @@
       <c r="A541" s="25">
         <v>60186</v>
       </c>
+      <c r="B541" s="36"/>
       <c r="C541" s="2" t="s">
         <v>2672</v>
       </c>
@@ -34210,6 +34248,49 @@
         <v>{"decimal":"60186","namebowtie":"desktop-screenshot","namemdl2":"null","codebowtie":"EB1A","codemdl2":"null","stylevariation":"light","keywords":["desktop","screenshot","camera","capture","monitor","screen"],"subset":"VSTS","group":"Test","usagenotes":"Used in Test extension for desktop screenshot."}</v>
       </c>
       <c r="O541" s="14"/>
+    </row>
+    <row r="542" spans="1:16" ht="32.1" customHeight="1">
+      <c r="A542" s="25">
+        <v>60187</v>
+      </c>
+      <c r="C542" s="2" t="s">
+        <v>2679</v>
+      </c>
+      <c r="D542" s="25" t="str">
+        <f t="shared" si="16"/>
+        <v>EB1B</v>
+      </c>
+      <c r="E542" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F542" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G542" s="2" t="s">
+        <v>2680</v>
+      </c>
+      <c r="H542" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I542" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="J542" s="2" t="s">
+        <v>2681</v>
+      </c>
+      <c r="K542" s="16" t="s">
+        <v>2488</v>
+      </c>
+      <c r="L542" s="16" t="s">
+        <v>2488</v>
+      </c>
+      <c r="M542" s="16" t="s">
+        <v>2488</v>
+      </c>
+      <c r="N542" s="14" t="str">
+        <f t="shared" si="17"/>
+        <v>{"decimal":"60187","namebowtie":"file-type-yml","namemdl2":"null","codebowtie":"EB1B","codemdl2":"null","stylevariation":"light","keywords":["file","type","yml","yaml","document","letter"],"subset":"VSTS","group":"Code","usagenotes":"Used for *.yml type files in Code hub file tree view."}</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A3:N529">

</xml_diff>

<commit_message>
Added unicode for some Fabric MDL2 icons
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5548" uniqueCount="2734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5548" uniqueCount="2746">
   <si>
     <t>keywords</t>
   </si>
@@ -8230,6 +8230,42 @@
   </si>
   <si>
     <t>FileYML</t>
+  </si>
+  <si>
+    <t>F5D0</t>
+  </si>
+  <si>
+    <t>F5D1</t>
+  </si>
+  <si>
+    <t>F5D2</t>
+  </si>
+  <si>
+    <t>F5D3</t>
+  </si>
+  <si>
+    <t>F5D4</t>
+  </si>
+  <si>
+    <t>F5D5</t>
+  </si>
+  <si>
+    <t>F5D6</t>
+  </si>
+  <si>
+    <t>F5DC</t>
+  </si>
+  <si>
+    <t>F5D7</t>
+  </si>
+  <si>
+    <t>F5D8</t>
+  </si>
+  <si>
+    <t>F5D9</t>
+  </si>
+  <si>
+    <t>F5DA</t>
   </si>
 </sst>
 </file>
@@ -8403,7 +8439,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8496,7 +8532,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -33888,11 +33923,11 @@
         <v>2722</v>
       </c>
       <c r="M529" s="25" t="s">
-        <v>2488</v>
+        <v>2734</v>
       </c>
       <c r="N529" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60174","namebowtie":"brand-vside","namemdl2":"VisualStudioIDELogo32","codebowtie":"EB0E","codemdl2":"null","stylevariation":"bold","keywords":["brand","visual","studio","ide","infinity","logo"],"subset":"VSTS","group":"Brand","usagenotes":"Visual Studio IDE 2017 RTW brand icon."}</v>
+        <v>{"decimal":"60174","namebowtie":"brand-vside","namemdl2":"VisualStudioIDELogo32","codebowtie":"EB0E","codemdl2":"F5D0","stylevariation":"bold","keywords":["brand","visual","studio","ide","infinity","logo"],"subset":"VSTS","group":"Brand","usagenotes":"Visual Studio IDE 2017 RTW brand icon."}</v>
       </c>
       <c r="O529" s="14"/>
       <c r="P529"/>
@@ -33936,11 +33971,11 @@
         <v>2723</v>
       </c>
       <c r="M530" s="25" t="s">
-        <v>2488</v>
+        <v>2735</v>
       </c>
       <c r="N530" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60175","namebowtie":"brand-ivy","namemdl2":"ApacheIvyLogo32","codebowtie":"EB0F","codemdl2":"null","stylevariation":"bold","keywords":["brand","apache","ivy","package","feed"],"subset":"VSTS","group":"Package","usagenotes":"Used in Packages hub for Apache Ivy package feeds."}</v>
+        <v>{"decimal":"60175","namebowtie":"brand-ivy","namemdl2":"ApacheIvyLogo32","codebowtie":"EB0F","codemdl2":"F5D1","stylevariation":"bold","keywords":["brand","apache","ivy","package","feed"],"subset":"VSTS","group":"Package","usagenotes":"Used in Packages hub for Apache Ivy package feeds."}</v>
       </c>
       <c r="O530" s="14"/>
     </row>
@@ -33983,11 +34018,11 @@
         <v>2727</v>
       </c>
       <c r="M531" s="25" t="s">
-        <v>2488</v>
+        <v>2739</v>
       </c>
       <c r="N531" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60176","namebowtie":"paste-as-text","namemdl2":"PasteAsText","codebowtie":"EB10","codemdl2":"null","stylevariation":"light","keywords":["paste","clipboard","text","letter"],"subset":"VSTS","group":"Wiki","usagenotes":"Used in Wiki editor toolbar for pasting as plain text."}</v>
+        <v>{"decimal":"60176","namebowtie":"paste-as-text","namemdl2":"PasteAsText","codebowtie":"EB10","codemdl2":"F5D5","stylevariation":"light","keywords":["paste","clipboard","text","letter"],"subset":"VSTS","group":"Wiki","usagenotes":"Used in Wiki editor toolbar for pasting as plain text."}</v>
       </c>
       <c r="O531" s="14"/>
     </row>
@@ -34030,11 +34065,11 @@
         <v>2728</v>
       </c>
       <c r="M532" s="25" t="s">
-        <v>2488</v>
+        <v>2740</v>
       </c>
       <c r="N532" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60177","namebowtie":"paste-as-html","namemdl2":"PasteAsCode","codebowtie":"EB11","codemdl2":"null","stylevariation":"light","keywords":["paste","clipboard","code","html","brackets"],"subset":"VSTS","group":"Wiki","usagenotes":"Used in Wiki editor toolbar for pasting as HTML."}</v>
+        <v>{"decimal":"60177","namebowtie":"paste-as-html","namemdl2":"PasteAsCode","codebowtie":"EB11","codemdl2":"F5D6","stylevariation":"light","keywords":["paste","clipboard","code","html","brackets"],"subset":"VSTS","group":"Wiki","usagenotes":"Used in Wiki editor toolbar for pasting as HTML."}</v>
       </c>
       <c r="O532" s="14"/>
     </row>
@@ -34077,11 +34112,11 @@
         <v>2724</v>
       </c>
       <c r="M533" s="25" t="s">
-        <v>2488</v>
+        <v>2736</v>
       </c>
       <c r="N533" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60178","namebowtie":"brand-bitbucket","namemdl2":"BitbucketLogo32","codebowtie":"EB12","codemdl2":"null","stylevariation":"bold","keywords":["bitbucket","version","control","git"],"subset":"VSTS","group":"Brand","usagenotes":"Bitbucket logo. Used in Build external source."}</v>
+        <v>{"decimal":"60178","namebowtie":"brand-bitbucket","namemdl2":"BitbucketLogo32","codebowtie":"EB12","codemdl2":"F5D2","stylevariation":"bold","keywords":["bitbucket","version","control","git"],"subset":"VSTS","group":"Brand","usagenotes":"Bitbucket logo. Used in Build external source."}</v>
       </c>
       <c r="O533" s="14"/>
     </row>
@@ -34124,11 +34159,11 @@
         <v>2725</v>
       </c>
       <c r="M534" s="25" t="s">
-        <v>2488</v>
+        <v>2737</v>
       </c>
       <c r="N534" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60179","namebowtie":"brand-linux","namemdl2":"LinuxLogo32","codebowtie":"EB13","codemdl2":"null","stylevariation":"bold","keywords":["linux","tux","penguin"],"subset":"VSTS","group":"Brand","usagenotes":"Linux logo. Used in Build queue picker."}</v>
+        <v>{"decimal":"60179","namebowtie":"brand-linux","namemdl2":"LinuxLogo32","codebowtie":"EB13","codemdl2":"F5D3","stylevariation":"bold","keywords":["linux","tux","penguin"],"subset":"VSTS","group":"Brand","usagenotes":"Linux logo. Used in Build queue picker."}</v>
       </c>
       <c r="O534" s="14"/>
     </row>
@@ -34218,11 +34253,11 @@
         <v>2726</v>
       </c>
       <c r="M536" s="25" t="s">
-        <v>2488</v>
+        <v>2738</v>
       </c>
       <c r="N536" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60181","namebowtie":"brand-gradle","namemdl2":"GradleLogo32","codebowtie":"EB15","codemdl2":"null","stylevariation":"bold","keywords":["brand","logo","gradle","elephant","build"],"subset":"VSTS","group":"Build","usagenotes":"Gradle logo. Used in Build hub."}</v>
+        <v>{"decimal":"60181","namebowtie":"brand-gradle","namemdl2":"GradleLogo32","codebowtie":"EB15","codemdl2":"F5D4","stylevariation":"bold","keywords":["brand","logo","gradle","elephant","build"],"subset":"VSTS","group":"Build","usagenotes":"Gradle logo. Used in Build hub."}</v>
       </c>
       <c r="O536" s="14"/>
     </row>
@@ -34265,11 +34300,11 @@
         <v>2729</v>
       </c>
       <c r="M537" s="25" t="s">
-        <v>2488</v>
+        <v>2741</v>
       </c>
       <c r="N537" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60182","namebowtie":"symbol-work","namemdl2":"ClipboardSolid","codebowtie":"EB16","codemdl2":"null","stylevariation":"bold","keywords":["symbol","work","item","generic","clipboard"],"subset":"VSTS","group":"Work","usagenotes":"Default work item type indicator."}</v>
+        <v>{"decimal":"60182","namebowtie":"symbol-work","namemdl2":"ClipboardSolid","codebowtie":"EB16","codemdl2":"F5DC","stylevariation":"bold","keywords":["symbol","work","item","generic","clipboard"],"subset":"VSTS","group":"Work","usagenotes":"Default work item type indicator."}</v>
       </c>
       <c r="O537" s="14"/>
     </row>
@@ -34312,11 +34347,11 @@
         <v>2730</v>
       </c>
       <c r="M538" s="25" t="s">
-        <v>2488</v>
+        <v>2742</v>
       </c>
       <c r="N538" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60183","namebowtie":"browser-tab","namemdl2":"BrowserTab","codebowtie":"EB17","codemdl2":"null","stylevariation":"light","keywords":["browser","tab"],"subset":"VSTS","group":"Test","usagenotes":"Used in Test extension for browser tab."}</v>
+        <v>{"decimal":"60183","namebowtie":"browser-tab","namemdl2":"BrowserTab","codebowtie":"EB17","codemdl2":"F5D7","stylevariation":"light","keywords":["browser","tab"],"subset":"VSTS","group":"Test","usagenotes":"Used in Test extension for browser tab."}</v>
       </c>
       <c r="O538" s="14"/>
     </row>
@@ -34406,11 +34441,11 @@
         <v>2731</v>
       </c>
       <c r="M540" s="25" t="s">
-        <v>2488</v>
+        <v>2743</v>
       </c>
       <c r="N540" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60185","namebowtie":"browser-tab-screenshot","namemdl2":"BrowserTabScreenshot","codebowtie":"EB19","codemdl2":"null","stylevariation":"light","keywords":["browser","tab","screenshot","camera","capture"],"subset":"VSTS","group":"Test","usagenotes":"Used in Test extension for browser tab screenshot."}</v>
+        <v>{"decimal":"60185","namebowtie":"browser-tab-screenshot","namemdl2":"BrowserTabScreenshot","codebowtie":"EB19","codemdl2":"F5D8","stylevariation":"light","keywords":["browser","tab","screenshot","camera","capture"],"subset":"VSTS","group":"Test","usagenotes":"Used in Test extension for browser tab screenshot."}</v>
       </c>
       <c r="O540" s="14"/>
     </row>
@@ -34453,11 +34488,11 @@
         <v>2732</v>
       </c>
       <c r="M541" s="25" t="s">
-        <v>2488</v>
+        <v>2744</v>
       </c>
       <c r="N541" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60186","namebowtie":"desktop-screenshot","namemdl2":"DesktopScreenshot","codebowtie":"EB1A","codemdl2":"null","stylevariation":"light","keywords":["desktop","screenshot","camera","capture","monitor","screen"],"subset":"VSTS","group":"Test","usagenotes":"Used in Test extension for desktop screenshot."}</v>
+        <v>{"decimal":"60186","namebowtie":"desktop-screenshot","namemdl2":"DesktopScreenshot","codebowtie":"EB1A","codemdl2":"F5D9","stylevariation":"light","keywords":["desktop","screenshot","camera","capture","monitor","screen"],"subset":"VSTS","group":"Test","usagenotes":"Used in Test extension for desktop screenshot."}</v>
       </c>
       <c r="O541" s="14"/>
     </row>
@@ -34500,11 +34535,11 @@
         <v>2733</v>
       </c>
       <c r="M542" s="25" t="s">
-        <v>2488</v>
+        <v>2745</v>
       </c>
       <c r="N542" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60187","namebowtie":"file-type-yml","namemdl2":"FileYML","codebowtie":"EB1B","codemdl2":"null","stylevariation":"light","keywords":["file","type","yml","yaml","document","letter"],"subset":"VSTS","group":"Code","usagenotes":"Used for *.yml type files in Code hub file tree view."}</v>
+        <v>{"decimal":"60187","namebowtie":"file-type-yml","namemdl2":"FileYML","codebowtie":"EB1B","codemdl2":"F5DA","stylevariation":"light","keywords":["file","type","yml","yaml","document","letter"],"subset":"VSTS","group":"Code","usagenotes":"Used for *.yml type files in Code hub file tree view."}</v>
       </c>
     </row>
     <row r="543" spans="1:16" ht="32.1" customHeight="1">
@@ -34591,7 +34626,7 @@
       <c r="M544" s="25" t="s">
         <v>2721</v>
       </c>
-      <c r="N544" s="40" t="str">
+      <c r="N544" s="14" t="str">
         <f t="shared" si="17"/>
         <v>{"decimal":"60189","namebowtie":"dom","namemdl2":"DOM","codebowtie":"EB1D","codemdl2":"EC8D","stylevariation":"light","keywords":["DOM"],"subset":"VSTS","group":"Keros","usagenotes":"Used in Keros to represent DOM."}</v>
       </c>

</xml_diff>

<commit_message>
Added new FabMDL2 icons; removed reference to other font formats in catalog
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="bowtie" sheetId="2" r:id="rId1"/>
-    <sheet name="20171110_MDL2 request" sheetId="3" r:id="rId2"/>
+    <sheet name="20180108_AddToFabric" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bowtie!$A$2:$N$529</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5557" uniqueCount="2749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5499" uniqueCount="2763">
   <si>
     <t>keywords</t>
   </si>
@@ -8118,18 +8118,6 @@
     <t></t>
   </si>
   <si>
-    <t>CELA</t>
-  </si>
-  <si>
-    <t>1st party brand</t>
-  </si>
-  <si>
-    <t>CELA approved.</t>
-  </si>
-  <si>
-    <t>Open source, doesn't need clearance.</t>
-  </si>
-  <si>
     <t>analytics-view</t>
   </si>
   <si>
@@ -8275,6 +8263,60 @@
   </si>
   <si>
     <t>Used in Code hub for Push.</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>AnalyticsView</t>
+  </si>
+  <si>
+    <t>F5F1</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>F665</t>
+  </si>
+  <si>
+    <t>ExternalGit</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>JenkinsLogo</t>
+  </si>
+  <si>
+    <t>F663</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>SVGLogo</t>
+  </si>
+  <si>
+    <t>F662</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>BranchPush</t>
+  </si>
+  <si>
+    <t>F664</t>
   </si>
 </sst>
 </file>
@@ -8284,7 +8326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8367,18 +8409,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="32"/>
-      <name val="Full MDL2 Assets"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Fabric MDL2 Assets"/>
       <family val="1"/>
     </font>
@@ -8400,6 +8430,11 @@
       <color theme="1"/>
       <name val="Fabric MDL2 Assets"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Bowtie"/>
     </font>
   </fonts>
   <fills count="6">
@@ -8448,7 +8483,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8513,34 +8548,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -8863,9 +8887,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AH545"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A531" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N545" sqref="N545"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L545" sqref="L545"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -8879,7 +8903,7 @@
     <col min="7" max="7" width="29.85546875" style="2" customWidth="1"/>
     <col min="8" max="9" width="14.28515625" style="2" customWidth="1"/>
     <col min="10" max="10" width="28" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9" style="33" customWidth="1"/>
+    <col min="11" max="11" width="9" style="28" customWidth="1"/>
     <col min="12" max="12" width="28.28515625" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="34" width="9" customWidth="1"/>
@@ -8915,7 +8939,7 @@
       <c r="J1" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="K1" s="33"/>
+      <c r="K1" s="28"/>
       <c r="L1"/>
       <c r="M1"/>
       <c r="N1"/>
@@ -8971,7 +8995,7 @@
       <c r="J2" s="8" t="s">
         <v>2513</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="29" t="s">
         <v>2446</v>
       </c>
       <c r="L2" s="8" t="s">
@@ -10898,7 +10922,7 @@
       <c r="J41" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="K41" s="35" t="s">
+      <c r="K41" s="30" t="s">
         <v>2367</v>
       </c>
       <c r="L41" s="19" t="s">
@@ -22395,7 +22419,7 @@
       <c r="J284" t="s">
         <v>2488</v>
       </c>
-      <c r="K284" s="35" t="s">
+      <c r="K284" s="30" t="s">
         <v>1759</v>
       </c>
       <c r="L284" s="15" t="s">
@@ -22442,7 +22466,7 @@
       <c r="J285" t="s">
         <v>2488</v>
       </c>
-      <c r="K285" s="35" t="s">
+      <c r="K285" s="30" t="s">
         <v>1756</v>
       </c>
       <c r="L285" s="15" t="s">
@@ -22489,7 +22513,7 @@
       <c r="J286" t="s">
         <v>2488</v>
       </c>
-      <c r="K286" s="35" t="s">
+      <c r="K286" s="30" t="s">
         <v>1753</v>
       </c>
       <c r="L286" s="15" t="s">
@@ -22536,7 +22560,7 @@
       <c r="J287" t="s">
         <v>2488</v>
       </c>
-      <c r="K287" s="36" t="s">
+      <c r="K287" s="31" t="s">
         <v>2488</v>
       </c>
       <c r="L287" s="10" t="s">
@@ -22583,7 +22607,7 @@
       <c r="J288" t="s">
         <v>2488</v>
       </c>
-      <c r="K288" s="35" t="s">
+      <c r="K288" s="30" t="s">
         <v>1750</v>
       </c>
       <c r="L288" s="15" t="s">
@@ -22630,7 +22654,7 @@
       <c r="J289" t="s">
         <v>2488</v>
       </c>
-      <c r="K289" s="36" t="s">
+      <c r="K289" s="31" t="s">
         <v>2488</v>
       </c>
       <c r="L289" s="10" t="s">
@@ -22677,7 +22701,7 @@
       <c r="J290" t="s">
         <v>2488</v>
       </c>
-      <c r="K290" s="35" t="s">
+      <c r="K290" s="30" t="s">
         <v>1747</v>
       </c>
       <c r="L290" s="15" t="s">
@@ -24134,7 +24158,7 @@
       <c r="J321" t="s">
         <v>2488</v>
       </c>
-      <c r="K321" s="35" t="s">
+      <c r="K321" s="30" t="s">
         <v>1669</v>
       </c>
       <c r="L321" s="14" t="s">
@@ -28149,7 +28173,7 @@
         <v>60052</v>
       </c>
       <c r="B407" s="17" t="s">
-        <v>2488</v>
+        <v>2748</v>
       </c>
       <c r="C407" s="26" t="s">
         <v>2620</v>
@@ -28176,7 +28200,7 @@
       <c r="J407" s="26" t="s">
         <v>2621</v>
       </c>
-      <c r="K407" s="37" t="s">
+      <c r="K407" s="32" t="s">
         <v>1420</v>
       </c>
       <c r="L407" s="27" t="s">
@@ -29540,7 +29564,7 @@
       <c r="J436" t="s">
         <v>839</v>
       </c>
-      <c r="K436" s="35" t="s">
+      <c r="K436" s="30" t="s">
         <v>1352</v>
       </c>
       <c r="L436" s="15" t="s">
@@ -30621,7 +30645,7 @@
       <c r="J459" t="s">
         <v>916</v>
       </c>
-      <c r="K459" s="35" t="s">
+      <c r="K459" s="30" t="s">
         <v>1284</v>
       </c>
       <c r="L459" s="15" t="s">
@@ -30668,7 +30692,7 @@
       <c r="J460" t="s">
         <v>916</v>
       </c>
-      <c r="K460" s="35" t="s">
+      <c r="K460" s="30" t="s">
         <v>1281</v>
       </c>
       <c r="L460" s="15" t="s">
@@ -30715,7 +30739,7 @@
       <c r="J461" t="s">
         <v>916</v>
       </c>
-      <c r="K461" s="35" t="s">
+      <c r="K461" s="30" t="s">
         <v>1278</v>
       </c>
       <c r="L461" s="15" t="s">
@@ -30762,7 +30786,7 @@
       <c r="J462" t="s">
         <v>916</v>
       </c>
-      <c r="K462" s="35" t="s">
+      <c r="K462" s="30" t="s">
         <v>1275</v>
       </c>
       <c r="L462" s="15" t="s">
@@ -30998,17 +31022,17 @@
         <v>913</v>
       </c>
       <c r="K467" s="16" t="s">
-        <v>2488</v>
+        <v>2757</v>
       </c>
       <c r="L467" s="14" t="s">
-        <v>2488</v>
+        <v>2758</v>
       </c>
       <c r="M467" s="14" t="s">
-        <v>2488</v>
+        <v>2759</v>
       </c>
       <c r="N467" s="14" t="str">
         <f t="shared" si="15"/>
-        <v>{"decimal":"60112","namebowtie":"brand-svn","namemdl2":"null","codebowtie":"EAD0","codemdl2":"null","stylevariation":"bold","keywords":["brand","svn","subversion","version","control"],"subset":"VSTS","group":"Brand","usagenotes":"Subversion logo."}</v>
+        <v>{"decimal":"60112","namebowtie":"brand-svn","namemdl2":"SVGLogo","codebowtie":"EAD0","codemdl2":"F662","stylevariation":"bold","keywords":["brand","svn","subversion","version","control"],"subset":"VSTS","group":"Brand","usagenotes":"Subversion logo."}</v>
       </c>
       <c r="O467" s="14"/>
     </row>
@@ -33590,17 +33614,17 @@
         <v>2506</v>
       </c>
       <c r="K522" s="16" t="s">
-        <v>2488</v>
+        <v>2751</v>
       </c>
       <c r="L522" s="25" t="s">
-        <v>2488</v>
+        <v>2753</v>
       </c>
       <c r="M522" s="25" t="s">
-        <v>2488</v>
+        <v>2752</v>
       </c>
       <c r="N522" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60167","namebowtie":"external-git","namemdl2":"null","codebowtie":"EB07","codemdl2":"null","stylevariation":"bold","keywords":["build","source","external","git"],"subset":"VSTS","group":"Brand","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
+        <v>{"decimal":"60167","namebowtie":"external-git","namemdl2":"ExternalGit","codebowtie":"EB07","codemdl2":"F665","stylevariation":"bold","keywords":["build","source","external","git"],"subset":"VSTS","group":"Brand","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
       </c>
       <c r="O522" s="14"/>
       <c r="P522"/>
@@ -33734,17 +33758,17 @@
         <v>2506</v>
       </c>
       <c r="K525" s="16" t="s">
-        <v>2488</v>
+        <v>2754</v>
       </c>
       <c r="L525" s="25" t="s">
-        <v>2488</v>
+        <v>2755</v>
       </c>
       <c r="M525" s="25" t="s">
-        <v>2488</v>
+        <v>2756</v>
       </c>
       <c r="N525" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60170","namebowtie":"brand-jenkins","namemdl2":"null","codebowtie":"EB0A","codemdl2":"null","stylevariation":"bold","keywords":["build","source","external","jenkins","brand","logo"],"subset":"VSTS","group":"Brand","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
+        <v>{"decimal":"60170","namebowtie":"brand-jenkins","namemdl2":"JenkinsLogo","codebowtie":"EB0A","codemdl2":"F663","stylevariation":"bold","keywords":["build","source","external","jenkins","brand","logo"],"subset":"VSTS","group":"Brand","usagenotes":"Used in Build &amp; Relase hub for selecting build source."}</v>
       </c>
       <c r="O525" s="14"/>
       <c r="P525"/>
@@ -33926,13 +33950,13 @@
         <v>2625</v>
       </c>
       <c r="K529" s="16" t="s">
-        <v>2704</v>
+        <v>2700</v>
       </c>
       <c r="L529" s="25" t="s">
-        <v>2722</v>
+        <v>2718</v>
       </c>
       <c r="M529" s="25" t="s">
-        <v>2734</v>
+        <v>2730</v>
       </c>
       <c r="N529" s="14" t="str">
         <f t="shared" si="17"/>
@@ -33974,13 +33998,13 @@
         <v>2601</v>
       </c>
       <c r="K530" s="16" t="s">
-        <v>2705</v>
+        <v>2701</v>
       </c>
       <c r="L530" s="25" t="s">
-        <v>2723</v>
+        <v>2719</v>
       </c>
       <c r="M530" s="25" t="s">
-        <v>2735</v>
+        <v>2731</v>
       </c>
       <c r="N530" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34021,13 +34045,13 @@
         <v>2618</v>
       </c>
       <c r="K531" s="16" t="s">
-        <v>2706</v>
+        <v>2702</v>
       </c>
       <c r="L531" s="25" t="s">
-        <v>2727</v>
+        <v>2723</v>
       </c>
       <c r="M531" s="25" t="s">
-        <v>2739</v>
+        <v>2735</v>
       </c>
       <c r="N531" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34068,13 +34092,13 @@
         <v>2619</v>
       </c>
       <c r="K532" s="16" t="s">
-        <v>2707</v>
+        <v>2703</v>
       </c>
       <c r="L532" s="25" t="s">
-        <v>2728</v>
+        <v>2724</v>
       </c>
       <c r="M532" s="25" t="s">
-        <v>2740</v>
+        <v>2736</v>
       </c>
       <c r="N532" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34115,13 +34139,13 @@
         <v>2628</v>
       </c>
       <c r="K533" s="16" t="s">
-        <v>2708</v>
+        <v>2704</v>
       </c>
       <c r="L533" s="25" t="s">
-        <v>2724</v>
+        <v>2720</v>
       </c>
       <c r="M533" s="25" t="s">
-        <v>2736</v>
+        <v>2732</v>
       </c>
       <c r="N533" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34162,13 +34186,13 @@
         <v>2631</v>
       </c>
       <c r="K534" s="16" t="s">
-        <v>2709</v>
+        <v>2705</v>
       </c>
       <c r="L534" s="25" t="s">
-        <v>2725</v>
+        <v>2721</v>
       </c>
       <c r="M534" s="25" t="s">
-        <v>2737</v>
+        <v>2733</v>
       </c>
       <c r="N534" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34208,7 +34232,7 @@
       <c r="J535" s="2" t="s">
         <v>2637</v>
       </c>
-      <c r="K535" s="28" t="s">
+      <c r="K535" s="16" t="s">
         <v>2638</v>
       </c>
       <c r="L535" s="25" t="s">
@@ -34256,13 +34280,13 @@
         <v>2643</v>
       </c>
       <c r="K536" s="16" t="s">
-        <v>2710</v>
+        <v>2706</v>
       </c>
       <c r="L536" s="25" t="s">
-        <v>2726</v>
+        <v>2722</v>
       </c>
       <c r="M536" s="25" t="s">
-        <v>2738</v>
+        <v>2734</v>
       </c>
       <c r="N536" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34302,14 +34326,14 @@
       <c r="J537" t="s">
         <v>2645</v>
       </c>
-      <c r="K537" s="38" t="s">
-        <v>2711</v>
+      <c r="K537" s="33" t="s">
+        <v>2707</v>
       </c>
       <c r="L537" s="25" t="s">
-        <v>2729</v>
+        <v>2725</v>
       </c>
       <c r="M537" s="25" t="s">
-        <v>2741</v>
+        <v>2737</v>
       </c>
       <c r="N537" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34350,13 +34374,13 @@
         <v>2662</v>
       </c>
       <c r="K538" s="16" t="s">
-        <v>2712</v>
+        <v>2708</v>
       </c>
       <c r="L538" s="25" t="s">
-        <v>2730</v>
+        <v>2726</v>
       </c>
       <c r="M538" s="25" t="s">
-        <v>2742</v>
+        <v>2738</v>
       </c>
       <c r="N538" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34444,13 +34468,13 @@
         <v>2671</v>
       </c>
       <c r="K540" s="16" t="s">
-        <v>2713</v>
+        <v>2709</v>
       </c>
       <c r="L540" s="25" t="s">
-        <v>2731</v>
+        <v>2727</v>
       </c>
       <c r="M540" s="25" t="s">
-        <v>2743</v>
+        <v>2739</v>
       </c>
       <c r="N540" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34491,13 +34515,13 @@
         <v>2674</v>
       </c>
       <c r="K541" s="16" t="s">
-        <v>2714</v>
+        <v>2710</v>
       </c>
       <c r="L541" s="25" t="s">
-        <v>2732</v>
+        <v>2728</v>
       </c>
       <c r="M541" s="25" t="s">
-        <v>2744</v>
+        <v>2740</v>
       </c>
       <c r="N541" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34538,13 +34562,13 @@
         <v>2681</v>
       </c>
       <c r="K542" s="16" t="s">
-        <v>2715</v>
+        <v>2711</v>
       </c>
       <c r="L542" s="25" t="s">
-        <v>2733</v>
+        <v>2729</v>
       </c>
       <c r="M542" s="25" t="s">
-        <v>2745</v>
+        <v>2741</v>
       </c>
       <c r="N542" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34559,7 +34583,7 @@
         <v>1789</v>
       </c>
       <c r="C543" s="2" t="s">
-        <v>2700</v>
+        <v>2696</v>
       </c>
       <c r="D543" s="22" t="str">
         <f t="shared" si="16"/>
@@ -34572,37 +34596,40 @@
         <v>11</v>
       </c>
       <c r="G543" s="2" t="s">
-        <v>2701</v>
+        <v>2697</v>
       </c>
       <c r="H543" s="2" t="s">
         <v>9</v>
       </c>
       <c r="I543" s="2" t="s">
-        <v>2702</v>
+        <v>2698</v>
       </c>
       <c r="J543" s="2" t="s">
-        <v>2703</v>
+        <v>2699</v>
       </c>
       <c r="K543" s="16" t="s">
-        <v>2488</v>
+        <v>2747</v>
       </c>
       <c r="L543" s="25" t="s">
-        <v>2488</v>
+        <v>2749</v>
       </c>
       <c r="M543" s="25" t="s">
-        <v>2488</v>
+        <v>2750</v>
       </c>
       <c r="N543" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60188","namebowtie":"analytics-view","namemdl2":"null","codebowtie":"EB1C","codemdl2":"null","stylevariation":"light","keywords":["analytics","view","table","bar","chart"],"subset":"VSTS","group":"Analytics","usagenotes":"Used in Analytics extension to indicate a view."}</v>
+        <v>{"decimal":"60188","namebowtie":"analytics-view","namemdl2":"AnalyticsView","codebowtie":"EB1C","codemdl2":"F5F1","stylevariation":"light","keywords":["analytics","view","table","bar","chart"],"subset":"VSTS","group":"Analytics","usagenotes":"Used in Analytics extension to indicate a view."}</v>
       </c>
     </row>
     <row r="544" spans="1:16" ht="32.1" customHeight="1">
       <c r="A544" s="22">
         <v>60189</v>
       </c>
+      <c r="B544" s="17" t="s">
+        <v>2745</v>
+      </c>
       <c r="C544" s="2" t="s">
-        <v>2717</v>
+        <v>2713</v>
       </c>
       <c r="D544" s="22" t="str">
         <f t="shared" si="16"/>
@@ -34615,25 +34642,25 @@
         <v>11</v>
       </c>
       <c r="G544" s="2" t="s">
-        <v>2718</v>
+        <v>2714</v>
       </c>
       <c r="H544" s="2" t="s">
         <v>9</v>
       </c>
       <c r="I544" s="2" t="s">
-        <v>2719</v>
+        <v>2715</v>
       </c>
       <c r="J544" s="2" t="s">
-        <v>2720</v>
-      </c>
-      <c r="K544" s="28" t="s">
         <v>2716</v>
       </c>
+      <c r="K544" s="16" t="s">
+        <v>2712</v>
+      </c>
       <c r="L544" s="25" t="s">
-        <v>2718</v>
+        <v>2714</v>
       </c>
       <c r="M544" s="25" t="s">
-        <v>2721</v>
+        <v>2717</v>
       </c>
       <c r="N544" s="14" t="str">
         <f t="shared" si="17"/>
@@ -34644,8 +34671,11 @@
       <c r="A545" s="22">
         <v>60190</v>
       </c>
+      <c r="B545" s="17" t="s">
+        <v>2746</v>
+      </c>
       <c r="C545" s="2" t="s">
-        <v>2746</v>
+        <v>2742</v>
       </c>
       <c r="D545" s="22" t="str">
         <f t="shared" si="16"/>
@@ -34658,7 +34688,7 @@
         <v>11</v>
       </c>
       <c r="G545" s="2" t="s">
-        <v>2747</v>
+        <v>2743</v>
       </c>
       <c r="H545" s="2" t="s">
         <v>9</v>
@@ -34667,20 +34697,20 @@
         <v>655</v>
       </c>
       <c r="J545" s="2" t="s">
-        <v>2748</v>
+        <v>2744</v>
       </c>
       <c r="K545" s="16" t="s">
-        <v>2488</v>
+        <v>2760</v>
       </c>
       <c r="L545" s="25" t="s">
-        <v>2488</v>
+        <v>2761</v>
       </c>
       <c r="M545" s="25" t="s">
-        <v>2488</v>
+        <v>2762</v>
       </c>
       <c r="N545" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60190","namebowtie":"tfvc-push","namemdl2":"null","codebowtie":"EB1E","codemdl2":"null","stylevariation":"light","keywords":["version","control","push","git"],"subset":"VSTS","group":"Code","usagenotes":"Used in Code hub for Push."}</v>
+        <v>{"decimal":"60190","namebowtie":"tfvc-push","namemdl2":"BranchPush","codebowtie":"EB1E","codemdl2":"F664","stylevariation":"light","keywords":["version","control","push","git"],"subset":"VSTS","group":"Code","usagenotes":"Used in Code hub for Push."}</v>
       </c>
     </row>
   </sheetData>
@@ -34694,706 +34724,242 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC17"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <cols>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="33"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s">
         <v>2487</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" t="s">
         <v>2514</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" t="s">
         <v>2515</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>2513</v>
       </c>
-      <c r="F1" s="34" t="s">
-        <v>2446</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>2516</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>2517</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>2696</v>
-      </c>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
-      <c r="Q1"/>
-      <c r="R1"/>
-      <c r="S1"/>
-      <c r="T1"/>
-      <c r="U1"/>
-      <c r="V1"/>
-      <c r="W1"/>
-      <c r="X1"/>
-      <c r="Y1"/>
-      <c r="Z1"/>
-      <c r="AA1"/>
-      <c r="AB1"/>
-    </row>
-    <row r="2" spans="1:29" s="20" customFormat="1" ht="32.1" customHeight="1">
+    </row>
+    <row r="2" spans="1:6" ht="32.1" customHeight="1">
       <c r="A2">
-        <v>60174</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>2682</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>2623</v>
-      </c>
-      <c r="D2" s="22" t="str">
-        <f t="shared" ref="D2:D17" si="0">DEC2HEX(A2)</f>
-        <v>EB0E</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>2625</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>2704</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>2697</v>
-      </c>
-      <c r="J2"/>
-    </row>
-    <row r="3" spans="1:29" ht="32.1" customHeight="1">
+        <v>59669</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>2466</v>
+      </c>
+      <c r="C2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D11" si="0">DEC2HEX(A2)</f>
+        <v>E915</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="32.1" customHeight="1">
       <c r="A3">
-        <v>60175</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>2683</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>2599</v>
-      </c>
-      <c r="D3" s="22" t="str">
+        <v>59670</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>EB0F</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>2601</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>2705</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>2698</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="32.1" customHeight="1">
+        <v>E916</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32.1" customHeight="1">
       <c r="A4">
-        <v>60176</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>2684</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>2613</v>
-      </c>
-      <c r="D4" s="22" t="str">
+        <v>59671</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>2467</v>
+      </c>
+      <c r="C4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>EB10</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>2618</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>2706</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I4" s="14"/>
-    </row>
-    <row r="5" spans="1:29" ht="32.1" customHeight="1">
+        <v>E917</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="32.1" customHeight="1">
       <c r="A5">
-        <v>60177</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>2685</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>2614</v>
-      </c>
-      <c r="D5" s="22" t="str">
+        <v>59673</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>2468</v>
+      </c>
+      <c r="C5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>EB11</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>2619</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>2707</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I5" s="14"/>
-    </row>
-    <row r="6" spans="1:29" ht="32.1" customHeight="1">
+        <v>E919</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2606</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32.1" customHeight="1">
       <c r="A6">
-        <v>60178</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>2686</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>2626</v>
-      </c>
-      <c r="D6" s="22" t="str">
+        <v>59679</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>2474</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>EB12</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>2628</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>2708</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>2698</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" s="2" customFormat="1" ht="32.1" customHeight="1">
+        <v>E91F</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="32.1" customHeight="1">
       <c r="A7">
-        <v>60179</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>2687</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>2629</v>
-      </c>
-      <c r="D7" s="22" t="str">
+        <v>60052</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>2748</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2620</v>
+      </c>
+      <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>EB13</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>2631</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>2709</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>2699</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
-    </row>
-    <row r="8" spans="1:29" s="2" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A8" s="32">
-        <v>60180</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>2688</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>2635</v>
-      </c>
-      <c r="D8" s="22" t="str">
+        <v>EA94</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2622</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="32.1" customHeight="1">
+      <c r="A8">
+        <v>60112</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>2559</v>
+      </c>
+      <c r="C8" t="s">
+        <v>910</v>
+      </c>
+      <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>EB14</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>2637</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>2638</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>2640</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>2639</v>
-      </c>
-      <c r="I8" s="14"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-      <c r="R8"/>
-      <c r="S8"/>
-      <c r="T8"/>
-      <c r="U8"/>
-      <c r="V8"/>
-      <c r="W8"/>
-      <c r="X8"/>
-      <c r="Y8"/>
-      <c r="Z8"/>
-      <c r="AA8"/>
-      <c r="AB8"/>
-    </row>
-    <row r="9" spans="1:29" s="2" customFormat="1" ht="32.1" customHeight="1">
+        <v>EAD0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>911</v>
+      </c>
+      <c r="F8" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="32.1" customHeight="1">
       <c r="A9">
-        <v>60181</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>2689</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>2641</v>
-      </c>
-      <c r="D9" s="22" t="str">
+        <v>60167</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>2528</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2497</v>
+      </c>
+      <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>EB15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>2643</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>2710</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>2698</v>
-      </c>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-    </row>
-    <row r="10" spans="1:29" s="2" customFormat="1" ht="32.1" customHeight="1">
+        <v>EB07</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2502</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="32.1" customHeight="1">
       <c r="A10">
-        <v>60182</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>2690</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>2644</v>
-      </c>
-      <c r="D10" s="22" t="str">
+        <v>60170</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>2530</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2500</v>
+      </c>
+      <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>EB16</v>
+        <v>EB0A</v>
       </c>
       <c r="E10" t="s">
-        <v>2645</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>2711</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
-      <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-      <c r="Z10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
-    </row>
-    <row r="11" spans="1:29" s="2" customFormat="1" ht="32.1" customHeight="1">
+        <v>2505</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="32.1" customHeight="1">
       <c r="A11">
-        <v>60183</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>2691</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>2660</v>
-      </c>
-      <c r="D11" s="22" t="str">
+        <v>60190</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>2746</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2742</v>
+      </c>
+      <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>EB17</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>2662</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>2712</v>
-      </c>
-      <c r="G11" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I11" s="14"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-      <c r="N11"/>
-      <c r="O11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
-      <c r="R11"/>
-      <c r="S11"/>
-      <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
-      <c r="Y11"/>
-      <c r="Z11"/>
-      <c r="AA11"/>
-      <c r="AB11"/>
-    </row>
-    <row r="12" spans="1:29" s="2" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A12" s="32">
-        <v>60184</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>2692</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2666</v>
-      </c>
-      <c r="D12" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>EB18</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>2668</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>2665</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>2663</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>2664</v>
-      </c>
-      <c r="I12" s="14"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-      <c r="R12"/>
-      <c r="S12"/>
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
-    </row>
-    <row r="13" spans="1:29" s="2" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A13">
-        <v>60185</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>2693</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>2669</v>
-      </c>
-      <c r="D13" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>EB19</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>2671</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>2713</v>
-      </c>
-      <c r="G13" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H13" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-      <c r="O13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
-      <c r="R13"/>
-      <c r="S13"/>
-      <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
-      <c r="Y13"/>
-      <c r="Z13"/>
-      <c r="AA13"/>
-      <c r="AB13"/>
-    </row>
-    <row r="14" spans="1:29" s="2" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A14">
-        <v>60186</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>2694</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>2672</v>
-      </c>
-      <c r="D14" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>EB1A</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>2674</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>2714</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="N14"/>
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
-      <c r="R14"/>
-      <c r="S14"/>
-      <c r="T14"/>
-      <c r="U14"/>
-      <c r="V14"/>
-      <c r="W14"/>
-      <c r="X14"/>
-      <c r="Y14"/>
-      <c r="Z14"/>
-      <c r="AA14"/>
-      <c r="AB14"/>
-    </row>
-    <row r="15" spans="1:29" s="2" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A15">
-        <v>60187</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>2695</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>2679</v>
-      </c>
-      <c r="D15" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>EB1B</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>2681</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>2715</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>2488</v>
-      </c>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-      <c r="R15"/>
-      <c r="S15"/>
-      <c r="T15"/>
-      <c r="U15"/>
-      <c r="V15"/>
-      <c r="W15"/>
-      <c r="X15"/>
-      <c r="Y15"/>
-      <c r="Z15"/>
-      <c r="AA15"/>
-      <c r="AB15"/>
-    </row>
-    <row r="16" spans="1:29" s="2" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A16" s="39">
-        <v>60188</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>1789</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>2700</v>
-      </c>
-      <c r="D16" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>EB1C</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>2703</v>
-      </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="14"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
-      <c r="Y16"/>
-      <c r="Z16"/>
-      <c r="AA16"/>
-      <c r="AB16"/>
-      <c r="AC16"/>
-    </row>
-    <row r="17" spans="1:7" ht="36">
-      <c r="A17" s="39">
-        <v>60189</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>2716</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>2717</v>
-      </c>
-      <c r="D17" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>EB1D</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>2718</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>2716</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>2718</v>
+        <v>EB1E</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2743</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added dictionary icons for Wiki
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwang\Dropbox\Code\vsfi\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsfi\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5499" uniqueCount="2763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5525" uniqueCount="2778">
   <si>
     <t>keywords</t>
   </si>
@@ -8317,6 +8317,51 @@
   </si>
   <si>
     <t>F664</t>
+  </si>
+  <si>
+    <t>dictionary</t>
+  </si>
+  <si>
+    <t>dictionary-add</t>
+  </si>
+  <si>
+    <t>dictionary-remove</t>
+  </si>
+  <si>
+    <t>dictionary book wiki</t>
+  </si>
+  <si>
+    <t>dictionary book wiki add plus</t>
+  </si>
+  <si>
+    <t>dictionary book wiki remove delete unlink cancel</t>
+  </si>
+  <si>
+    <t>Used in Wiki to represent a topic</t>
+  </si>
+  <si>
+    <t>Used in Wiki</t>
+  </si>
+  <si>
+    <t>Used in Wiki for unlinking repo.</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>Dictionary</t>
+  </si>
+  <si>
+    <t>E82D</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>DictionaryAdd</t>
+  </si>
+  <si>
+    <t>E82E</t>
   </si>
 </sst>
 </file>
@@ -8483,7 +8528,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8563,6 +8608,13 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8885,11 +8937,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AH545"/>
+  <dimension ref="A1:AH548"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L545" sqref="L545"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A527" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H534" sqref="H534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -33256,7 +33308,7 @@
         <v>1067</v>
       </c>
       <c r="D515" s="22" t="str">
-        <f t="shared" ref="D515:D545" si="16">DEC2HEX(A515)</f>
+        <f t="shared" ref="D515:D548" si="16">DEC2HEX(A515)</f>
         <v>EB00</v>
       </c>
       <c r="E515" s="22">
@@ -33287,7 +33339,7 @@
         <v>2564</v>
       </c>
       <c r="N515" s="14" t="str">
-        <f t="shared" ref="N515:N545" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
+        <f t="shared" ref="N515:N548" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
         <v>{"decimal":"60160","namebowtie":"file-lock","namemdl2":"PageLock","codebowtie":"EB00","codemdl2":"F43F","stylevariation":"light","keywords":["file","document","lock","permission"],"subset":"VSTS","group":"Common","usagenotes":"Used to represent the user does not have permission to a file."}</v>
       </c>
       <c r="O515" s="14"/>
@@ -34667,7 +34719,7 @@
         <v>{"decimal":"60189","namebowtie":"dom","namemdl2":"DOM","codebowtie":"EB1D","codemdl2":"EC8D","stylevariation":"light","keywords":["DOM"],"subset":"VSTS","group":"Keros","usagenotes":"Used in Keros to represent DOM."}</v>
       </c>
     </row>
-    <row r="545" spans="1:14" ht="32.1" customHeight="1">
+    <row r="545" spans="1:34" ht="32.1" customHeight="1">
       <c r="A545" s="22">
         <v>60190</v>
       </c>
@@ -34712,6 +34764,173 @@
         <f t="shared" si="17"/>
         <v>{"decimal":"60190","namebowtie":"tfvc-push","namemdl2":"BranchPush","codebowtie":"EB1E","codemdl2":"F664","stylevariation":"light","keywords":["version","control","push","git"],"subset":"VSTS","group":"Code","usagenotes":"Used in Code hub for Push."}</v>
       </c>
+    </row>
+    <row r="546" spans="1:34" ht="32.1" customHeight="1">
+      <c r="A546" s="22">
+        <v>60191</v>
+      </c>
+      <c r="C546" s="2" t="s">
+        <v>2763</v>
+      </c>
+      <c r="D546" s="22" t="str">
+        <f t="shared" si="16"/>
+        <v>EB1F</v>
+      </c>
+      <c r="E546" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F546" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G546" s="2" t="s">
+        <v>2766</v>
+      </c>
+      <c r="H546" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I546" s="2" t="s">
+        <v>2617</v>
+      </c>
+      <c r="J546" s="2" t="s">
+        <v>2769</v>
+      </c>
+      <c r="K546" s="16" t="s">
+        <v>2772</v>
+      </c>
+      <c r="L546" t="s">
+        <v>2773</v>
+      </c>
+      <c r="M546" t="s">
+        <v>2774</v>
+      </c>
+      <c r="N546" s="14" t="str">
+        <f t="shared" si="17"/>
+        <v>{"decimal":"60191","namebowtie":"dictionary","namemdl2":"Dictionary","codebowtie":"EB1F","codemdl2":"E82D","stylevariation":"light","keywords":["dictionary","book","wiki"],"subset":"VSTS","group":"Wiki","usagenotes":"Used in Wiki to represent a topic"}</v>
+      </c>
+    </row>
+    <row r="547" spans="1:34" s="1" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A547" s="35">
+        <v>60192</v>
+      </c>
+      <c r="C547" s="1" t="s">
+        <v>2764</v>
+      </c>
+      <c r="D547" s="35" t="str">
+        <f t="shared" si="16"/>
+        <v>EB20</v>
+      </c>
+      <c r="E547" s="36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F547" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G547" s="1" t="s">
+        <v>2767</v>
+      </c>
+      <c r="H547" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I547" s="1" t="s">
+        <v>2617</v>
+      </c>
+      <c r="J547" s="1" t="s">
+        <v>2770</v>
+      </c>
+      <c r="K547" s="16" t="s">
+        <v>2775</v>
+      </c>
+      <c r="L547" t="s">
+        <v>2776</v>
+      </c>
+      <c r="M547" s="35" t="s">
+        <v>2777</v>
+      </c>
+      <c r="N547" s="14" t="str">
+        <f t="shared" si="17"/>
+        <v>{"decimal":"60192","namebowtie":"dictionary-add","namemdl2":"DictionaryAdd","codebowtie":"EB20","codemdl2":"E82E","stylevariation":"light","keywords":["dictionary","book","wiki","add","plus"],"subset":"VSTS","group":"Wiki","usagenotes":"Used in Wiki"}</v>
+      </c>
+      <c r="O547" s="35"/>
+      <c r="P547" s="35"/>
+      <c r="Q547" s="35"/>
+      <c r="R547" s="35"/>
+      <c r="S547" s="35"/>
+      <c r="T547" s="35"/>
+      <c r="U547" s="35"/>
+      <c r="V547" s="35"/>
+      <c r="W547" s="35"/>
+      <c r="X547" s="35"/>
+      <c r="Y547" s="35"/>
+      <c r="Z547" s="35"/>
+      <c r="AA547" s="35"/>
+      <c r="AB547" s="35"/>
+      <c r="AC547" s="35"/>
+      <c r="AD547" s="35"/>
+      <c r="AE547" s="35"/>
+      <c r="AF547" s="35"/>
+      <c r="AG547" s="35"/>
+      <c r="AH547" s="35"/>
+    </row>
+    <row r="548" spans="1:34" s="1" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A548" s="35">
+        <v>60193</v>
+      </c>
+      <c r="C548" s="1" t="s">
+        <v>2765</v>
+      </c>
+      <c r="D548" s="35" t="str">
+        <f t="shared" si="16"/>
+        <v>EB21</v>
+      </c>
+      <c r="E548" s="36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F548" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G548" s="1" t="s">
+        <v>2768</v>
+      </c>
+      <c r="H548" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I548" s="1" t="s">
+        <v>2617</v>
+      </c>
+      <c r="J548" s="1" t="s">
+        <v>2771</v>
+      </c>
+      <c r="K548" s="37"/>
+      <c r="L548" s="35" t="s">
+        <v>2488</v>
+      </c>
+      <c r="M548" s="35" t="s">
+        <v>2488</v>
+      </c>
+      <c r="N548" s="14" t="str">
+        <f t="shared" si="17"/>
+        <v>{"decimal":"60193","namebowtie":"dictionary-remove","namemdl2":"null","codebowtie":"EB21","codemdl2":"null","stylevariation":"light","keywords":["dictionary","book","wiki","remove","delete","unlink","cancel"],"subset":"VSTS","group":"Wiki","usagenotes":"Used in Wiki for unlinking repo."}</v>
+      </c>
+      <c r="O548" s="35"/>
+      <c r="P548" s="35"/>
+      <c r="Q548" s="35"/>
+      <c r="R548" s="35"/>
+      <c r="S548" s="35"/>
+      <c r="T548" s="35"/>
+      <c r="U548" s="35"/>
+      <c r="V548" s="35"/>
+      <c r="W548" s="35"/>
+      <c r="X548" s="35"/>
+      <c r="Y548" s="35"/>
+      <c r="Z548" s="35"/>
+      <c r="AA548" s="35"/>
+      <c r="AB548" s="35"/>
+      <c r="AC548" s="35"/>
+      <c r="AD548" s="35"/>
+      <c r="AE548" s="35"/>
+      <c r="AF548" s="35"/>
+      <c r="AG548" s="35"/>
+      <c r="AH548" s="35"/>
     </row>
   </sheetData>
   <sortState ref="A3:N529">

</xml_diff>

<commit_message>
Aligned some code review icons with Fabric MDL2
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsfi\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cowang\Dropbox\Code\vsfi\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5525" uniqueCount="2778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5533" uniqueCount="2781">
   <si>
     <t>keywords</t>
   </si>
@@ -8362,6 +8362,15 @@
   </si>
   <si>
     <t>E82E</t>
+  </si>
+  <si>
+    <t>user-remove</t>
+  </si>
+  <si>
+    <t>user remove reject approval delete cancel</t>
+  </si>
+  <si>
+    <t>Used for approval rejected status.</t>
   </si>
 </sst>
 </file>
@@ -8937,11 +8946,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AH548"/>
+  <dimension ref="A1:AH549"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A527" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H534" sqref="H534"/>
+      <pane ySplit="2" topLeftCell="A542" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J549" sqref="J549"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -33308,7 +33317,7 @@
         <v>1067</v>
       </c>
       <c r="D515" s="22" t="str">
-        <f t="shared" ref="D515:D548" si="16">DEC2HEX(A515)</f>
+        <f t="shared" ref="D515:D549" si="16">DEC2HEX(A515)</f>
         <v>EB00</v>
       </c>
       <c r="E515" s="22">
@@ -33339,7 +33348,7 @@
         <v>2564</v>
       </c>
       <c r="N515" s="14" t="str">
-        <f t="shared" ref="N515:N548" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
+        <f t="shared" ref="N515:N549" si="17">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A515,"','namebowtie':'",C515,"','namemdl2':'",L515,"','codebowtie':'",D515,"','codemdl2':'",M515,"','stylevariation':'",F515,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G515,"']")," ","','"),"'",""""),",'subset':'",H515,"','group':'",I515,"','usagenotes':'",J515,"'}"),"'","""")</f>
         <v>{"decimal":"60160","namebowtie":"file-lock","namemdl2":"PageLock","codebowtie":"EB00","codemdl2":"F43F","stylevariation":"light","keywords":["file","document","lock","permission"],"subset":"VSTS","group":"Common","usagenotes":"Used to represent the user does not have permission to a file."}</v>
       </c>
       <c r="O515" s="14"/>
@@ -34931,6 +34940,46 @@
       <c r="AF548" s="35"/>
       <c r="AG548" s="35"/>
       <c r="AH548" s="35"/>
+    </row>
+    <row r="549" spans="1:34" ht="32.1" customHeight="1">
+      <c r="A549" s="22">
+        <v>60194</v>
+      </c>
+      <c r="C549" s="2" t="s">
+        <v>2778</v>
+      </c>
+      <c r="D549" s="22" t="str">
+        <f t="shared" si="16"/>
+        <v>EB22</v>
+      </c>
+      <c r="E549" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F549" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G549" s="2" t="s">
+        <v>2779</v>
+      </c>
+      <c r="H549" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I549" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="J549" s="2" t="s">
+        <v>2780</v>
+      </c>
+      <c r="L549" s="28" t="s">
+        <v>2488</v>
+      </c>
+      <c r="M549" s="28" t="s">
+        <v>2488</v>
+      </c>
+      <c r="N549" s="14" t="str">
+        <f t="shared" si="17"/>
+        <v>{"decimal":"60194","namebowtie":"user-remove","namemdl2":"null","codebowtie":"EB22","codemdl2":"null","stylevariation":"light","keywords":["user","remove","reject","approval","delete","cancel"],"subset":"VSTS","group":"Code","usagenotes":"Used for approval rejected status."}</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A3:N529">

</xml_diff>

<commit_message>
Added user-event icon for approver set status
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5533" uniqueCount="2781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5541" uniqueCount="2784">
   <si>
     <t>keywords</t>
   </si>
@@ -8371,6 +8371,15 @@
   </si>
   <si>
     <t>Used for approval rejected status.</t>
+  </si>
+  <si>
+    <t>user-event</t>
+  </si>
+  <si>
+    <t>Used for approval set status.</t>
+  </si>
+  <si>
+    <t>user event trigger lightning bolt</t>
   </si>
 </sst>
 </file>
@@ -8946,11 +8955,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AH549"/>
+  <dimension ref="A1:AH550"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A542" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J549" sqref="J549"/>
+      <pane ySplit="2" topLeftCell="A535" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D550" sqref="D550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -33317,7 +33326,7 @@
         <v>1067</v>
       </c>
       <c r="D515" s="22" t="str">
-        <f t="shared" ref="D515:D549" si="16">DEC2HEX(A515)</f>
+        <f t="shared" ref="D515:D550" si="16">DEC2HEX(A515)</f>
         <v>EB00</v>
       </c>
       <c r="E515" s="22">
@@ -34965,20 +34974,60 @@
         <v>9</v>
       </c>
       <c r="I549" s="2" t="s">
-        <v>655</v>
+        <v>582</v>
       </c>
       <c r="J549" s="2" t="s">
         <v>2780</v>
       </c>
-      <c r="L549" s="28" t="s">
-        <v>2488</v>
-      </c>
-      <c r="M549" s="28" t="s">
+      <c r="L549" t="s">
+        <v>2488</v>
+      </c>
+      <c r="M549" t="s">
         <v>2488</v>
       </c>
       <c r="N549" s="14" t="str">
         <f t="shared" si="17"/>
-        <v>{"decimal":"60194","namebowtie":"user-remove","namemdl2":"null","codebowtie":"EB22","codemdl2":"null","stylevariation":"light","keywords":["user","remove","reject","approval","delete","cancel"],"subset":"VSTS","group":"Code","usagenotes":"Used for approval rejected status."}</v>
+        <v>{"decimal":"60194","namebowtie":"user-remove","namemdl2":"null","codebowtie":"EB22","codemdl2":"null","stylevariation":"light","keywords":["user","remove","reject","approval","delete","cancel"],"subset":"VSTS","group":"Build","usagenotes":"Used for approval rejected status."}</v>
+      </c>
+    </row>
+    <row r="550" spans="1:34" ht="32.1" customHeight="1">
+      <c r="A550" s="22">
+        <v>60195</v>
+      </c>
+      <c r="C550" s="2" t="s">
+        <v>2781</v>
+      </c>
+      <c r="D550" s="22" t="str">
+        <f t="shared" si="16"/>
+        <v>EB23</v>
+      </c>
+      <c r="E550" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F550" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G550" s="2" t="s">
+        <v>2783</v>
+      </c>
+      <c r="H550" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I550" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="J550" s="2" t="s">
+        <v>2782</v>
+      </c>
+      <c r="L550" t="s">
+        <v>2488</v>
+      </c>
+      <c r="M550" t="s">
+        <v>2488</v>
+      </c>
+      <c r="N550" t="str">
+        <f t="shared" ref="N550" si="18">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A550,"','namebowtie':'",C550,"','namemdl2':'",L550,"','codebowtie':'",D550,"','codemdl2':'",M550,"','stylevariation':'",F550,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G550,"']")," ","','"),"'",""""),",'subset':'",H550,"','group':'",I550,"','usagenotes':'",J550,"'}"),"'","""")</f>
+        <v>{"decimal":"60195","namebowtie":"user-event","namemdl2":"null","codebowtie":"EB23","codemdl2":"null","stylevariation":"light","keywords":["user","event","trigger","lightning","bolt"],"subset":"VSTS","group":"Build","usagenotes":"Used for approval set status."}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added shield-verified-fill icon for VS Marketplace
</commit_message>
<xml_diff>
--- a/source/bowtie.xlsx
+++ b/source/bowtie.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cowang\Dropbox\Code\vsfi\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Code\vsfi\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DA1CFD-CFE8-49B0-B475-36E466AC9193}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bowtie" sheetId="2" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5541" uniqueCount="2784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5549" uniqueCount="2789">
   <si>
     <t>keywords</t>
   </si>
@@ -8380,12 +8381,27 @@
   </si>
   <si>
     <t>user event trigger lightning bolt</t>
+  </si>
+  <si>
+    <t>shield-verified-fill</t>
+  </si>
+  <si>
+    <t>shield verified check security</t>
+  </si>
+  <si>
+    <t>Maketplace</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Used in Marketplace for verified extension publisher.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -8640,9 +8656,9 @@
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Neutral 2" xfId="5"/>
+    <cellStyle name="Neutral 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8953,13 +8969,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AH550"/>
+  <dimension ref="A1:AH551"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A535" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D550" sqref="D550"/>
+      <pane ySplit="2" topLeftCell="A532" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N551" sqref="N551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.1" customHeight="1"/>
@@ -33326,7 +33342,7 @@
         <v>1067</v>
       </c>
       <c r="D515" s="22" t="str">
-        <f t="shared" ref="D515:D550" si="16">DEC2HEX(A515)</f>
+        <f t="shared" ref="D515:D551" si="16">DEC2HEX(A515)</f>
         <v>EB00</v>
       </c>
       <c r="E515" s="22">
@@ -35026,8 +35042,48 @@
         <v>2488</v>
       </c>
       <c r="N550" t="str">
-        <f t="shared" ref="N550" si="18">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A550,"','namebowtie':'",C550,"','namemdl2':'",L550,"','codebowtie':'",D550,"','codemdl2':'",M550,"','stylevariation':'",F550,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G550,"']")," ","','"),"'",""""),",'subset':'",H550,"','group':'",I550,"','usagenotes':'",J550,"'}"),"'","""")</f>
+        <f t="shared" ref="N550:N551" si="18">SUBSTITUTE(_xlfn.CONCAT("{'decimal':'",A550,"','namebowtie':'",C550,"','namemdl2':'",L550,"','codebowtie':'",D550,"','codemdl2':'",M550,"','stylevariation':'",F550,"','keywords':",SUBSTITUTE(SUBSTITUTE(_xlfn.CONCAT("['",G550,"']")," ","','"),"'",""""),",'subset':'",H550,"','group':'",I550,"','usagenotes':'",J550,"'}"),"'","""")</f>
         <v>{"decimal":"60195","namebowtie":"user-event","namemdl2":"null","codebowtie":"EB23","codemdl2":"null","stylevariation":"light","keywords":["user","event","trigger","lightning","bolt"],"subset":"VSTS","group":"Build","usagenotes":"Used for approval set status."}</v>
+      </c>
+    </row>
+    <row r="551" spans="1:34" ht="32.1" customHeight="1">
+      <c r="A551" s="22">
+        <v>60196</v>
+      </c>
+      <c r="C551" s="2" t="s">
+        <v>2784</v>
+      </c>
+      <c r="D551" s="22" t="str">
+        <f t="shared" si="16"/>
+        <v>EB24</v>
+      </c>
+      <c r="E551" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F551" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G551" s="2" t="s">
+        <v>2785</v>
+      </c>
+      <c r="H551" s="2" t="s">
+        <v>2786</v>
+      </c>
+      <c r="I551" s="2" t="s">
+        <v>2787</v>
+      </c>
+      <c r="J551" s="2" t="s">
+        <v>2788</v>
+      </c>
+      <c r="L551" t="s">
+        <v>2488</v>
+      </c>
+      <c r="M551" t="s">
+        <v>2488</v>
+      </c>
+      <c r="N551" t="str">
+        <f t="shared" si="18"/>
+        <v>{"decimal":"60196","namebowtie":"shield-verified-fill","namemdl2":"null","codebowtie":"EB24","codemdl2":"null","stylevariation":"bold","keywords":["shield","verified","check","security"],"subset":"Maketplace","group":"Web","usagenotes":"Used in Marketplace for verified extension publisher."}</v>
       </c>
     </row>
   </sheetData>
@@ -35040,7 +35096,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>